<commit_message>
Mise à jour de la traduction
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dossier Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6695F2B4-8698-43C0-A2CC-879D6263FFF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A88650-0744-4FA8-9E0B-63E2273CA277}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="14" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,10 @@
     <sheet name="Exporter Excel Personnalisé" sheetId="12" r:id="rId12"/>
     <sheet name="Autres" sheetId="13" r:id="rId13"/>
     <sheet name="Changer Configuration" sheetId="17" r:id="rId14"/>
-    <sheet name="FR_Properties" sheetId="14" r:id="rId15"/>
-    <sheet name="ES_Properties" sheetId="16" r:id="rId16"/>
-    <sheet name="Constants" sheetId="18" r:id="rId17"/>
+    <sheet name="A propos" sheetId="19" r:id="rId15"/>
+    <sheet name="FR_Properties" sheetId="14" r:id="rId16"/>
+    <sheet name="ES_Properties" sheetId="16" r:id="rId17"/>
+    <sheet name="Constants" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="567">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -241,9 +242,6 @@
     <t>Administra los materials</t>
   </si>
   <si>
-    <t>Repertorio de la biblioteca :</t>
-  </si>
-  <si>
     <t>Estado del análisis</t>
   </si>
   <si>
@@ -295,9 +293,6 @@
     <t>Numero</t>
   </si>
   <si>
-    <t xml:space="preserve">Repertorio analizado : </t>
-  </si>
-  <si>
     <t xml:space="preserve">Número de estructuras con errores : </t>
   </si>
   <si>
@@ -1715,6 +1710,45 @@
   </si>
   <si>
     <t>Configuración actual :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Directorio analizado : </t>
+  </si>
+  <si>
+    <t>Directorio de la biblioteca :</t>
+  </si>
+  <si>
+    <t>A propos</t>
+  </si>
+  <si>
+    <t>Acerca</t>
+  </si>
+  <si>
+    <t>#Message pour la fenêtre a propos</t>
+  </si>
+  <si>
+    <t>window.about.title</t>
+  </si>
+  <si>
+    <t>window.about.message.content</t>
+  </si>
+  <si>
+    <t>menu.about</t>
+  </si>
+  <si>
+    <t>menu.about.open</t>
+  </si>
+  <si>
+    <t>Ouvrir</t>
+  </si>
+  <si>
+    <t>Abrir</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;A propos de l'application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nom de l'application : &lt;/u&gt; Caerus&lt;br /&gt;&lt;u&gt;Version : &lt;/u&gt; 1.0.0&lt;br /&gt;&lt;u&gt;Editeur : &lt;/u&gt; Jeremy, Leda&lt;br /&gt;&lt;u&gt;Site web : &lt;/u&gt;https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Acerca de la application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nombre de la application :&lt;/u&gt; Caerus&lt;BR /&gt;&lt;u&gt;Versión :&lt;/u&gt; 1.0.0&lt;br /&gt;&lt;u&gt;Editor :&lt;/u&gt; Jeremy, Leda&lt;br/&gt;&lt;u&gt;Sitio web :&lt;/u&gt; https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</t>
   </si>
 </sst>
 </file>
@@ -22687,8 +22721,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08B73F6F-6897-453A-A261-1E8F78D02F2C}" name="Tableau1" displayName="Tableau1" ref="A1:D47" totalsRowShown="0" headerRowDxfId="36">
-  <autoFilter ref="A1:D47" xr:uid="{5A1C5E6C-13F0-43D6-93E5-7F1D2D7A93ED}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08B73F6F-6897-453A-A261-1E8F78D02F2C}" name="Tableau1" displayName="Tableau1" ref="A1:D49" totalsRowShown="0" headerRowDxfId="36">
+  <autoFilter ref="A1:D49" xr:uid="{5A1C5E6C-13F0-43D6-93E5-7F1D2D7A93ED}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{581AA08F-F8B9-4EB9-9270-F690B4699028}" name="Numero"/>
     <tableColumn id="2" xr3:uid="{86F9FD87-A94B-4F9B-BA16-3BEE622BE071}" name="Code"/>
@@ -22759,6 +22793,19 @@
     <tableColumn id="2" xr3:uid="{2BD08D0A-A06E-4823-A29F-229DAC1664B5}" name="Code"/>
     <tableColumn id="3" xr3:uid="{1106E753-C414-43B7-8028-DF7D2546A2D2}" name="Français"/>
     <tableColumn id="4" xr3:uid="{52E87CF4-50EE-426B-94A1-8281489E5B8E}" name="Español"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{54C75DA3-536A-47AA-84F8-D9CAFCFCCBCD}" name="Tableau161011" displayName="Tableau161011" ref="A1:D7" totalsRowShown="0">
+  <autoFilter ref="A1:D7" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{2EAF23AA-21BD-4ECF-A89A-1EE1FAB4FA7B}" name="Numero"/>
+    <tableColumn id="2" xr3:uid="{23137A6E-4186-404B-8C24-F3653D56A29E}" name="Code"/>
+    <tableColumn id="3" xr3:uid="{AD125158-21C5-4047-A063-80C29885C631}" name="Français"/>
+    <tableColumn id="4" xr3:uid="{F3A203CF-2262-4BDF-AA75-7DA21118D925}" name="Español"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -23165,10 +23212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF59B93E-40E9-44D6-98FA-7D0A802C1DCE}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23181,16 +23228,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -23241,7 +23288,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -23255,7 +23302,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -23269,7 +23316,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -23283,7 +23330,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -23297,7 +23344,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -23311,7 +23358,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -23325,13 +23372,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C14" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D14" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -23339,13 +23386,13 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C15" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D15" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -23353,7 +23400,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -23367,7 +23414,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -23381,7 +23428,7 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
@@ -23395,7 +23442,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>
@@ -23424,7 +23471,7 @@
         <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>555</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -23438,7 +23485,7 @@
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -23452,7 +23499,7 @@
         <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -23466,7 +23513,7 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -23480,7 +23527,7 @@
         <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -23494,7 +23541,7 @@
         <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>554</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -23508,7 +23555,7 @@
         <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -23519,10 +23566,10 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D29" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -23536,7 +23583,7 @@
         <v>52</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -23550,7 +23597,7 @@
         <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -23564,7 +23611,7 @@
         <v>35</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -23578,7 +23625,7 @@
         <v>37</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -23592,7 +23639,7 @@
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -23606,7 +23653,7 @@
         <v>41</v>
       </c>
       <c r="D35" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -23620,7 +23667,7 @@
         <v>43</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -23634,7 +23681,7 @@
         <v>45</v>
       </c>
       <c r="D37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -23648,7 +23695,7 @@
         <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -23662,7 +23709,7 @@
         <v>49</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -23670,13 +23717,13 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -23684,13 +23731,13 @@
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -23698,13 +23745,13 @@
         <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -23712,13 +23759,13 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D43" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -23726,13 +23773,13 @@
         <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D44" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -23740,13 +23787,13 @@
         <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D45" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -23754,13 +23801,41 @@
         <v>38</v>
       </c>
       <c r="B46" t="s">
+        <v>551</v>
+      </c>
+      <c r="C46" t="s">
+        <v>552</v>
+      </c>
+      <c r="D46" t="s">
         <v>553</v>
       </c>
-      <c r="C46" t="s">
-        <v>554</v>
-      </c>
-      <c r="D46" t="s">
-        <v>555</v>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>39</v>
+      </c>
+      <c r="B47" t="s">
+        <v>561</v>
+      </c>
+      <c r="C47" t="s">
+        <v>556</v>
+      </c>
+      <c r="D47" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>40</v>
+      </c>
+      <c r="B48" t="s">
+        <v>562</v>
+      </c>
+      <c r="C48" t="s">
+        <v>563</v>
+      </c>
+      <c r="D48" t="s">
+        <v>564</v>
       </c>
     </row>
   </sheetData>
@@ -23789,24 +23864,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -23814,13 +23889,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -23828,13 +23903,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -23842,13 +23917,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -23856,13 +23931,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -23870,13 +23945,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -23884,13 +23959,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D8" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -23898,13 +23973,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C9" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D9" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -23912,13 +23987,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D10" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -23926,13 +24001,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D11" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -23940,13 +24015,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C12" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -23954,13 +24029,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C13" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D13" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -23968,13 +24043,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C14" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D14" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -23982,13 +24057,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C15" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D15" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -24017,24 +24092,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -24042,13 +24117,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24056,13 +24131,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -24070,13 +24145,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -24084,13 +24159,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -24098,7 +24173,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Les fichiers suivants vont être générés : &lt;br/&gt;&lt;br/&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24114,13 +24189,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -24128,21 +24203,21 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C9" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D9" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D11" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -24150,13 +24225,13 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C12" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -24164,21 +24239,21 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C13" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D15" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -24186,13 +24261,13 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C16" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -24200,21 +24275,21 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C17" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D17" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D19" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -24222,13 +24297,13 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -24236,13 +24311,13 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C21" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D21" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -24269,24 +24344,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -24294,13 +24369,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C3" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D3" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24308,13 +24383,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D4" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -24322,13 +24397,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D5" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -24336,13 +24411,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -24350,7 +24425,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Le fichier suivant va être généré : &lt;br/&gt;&lt;br/&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24366,13 +24441,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C8" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D8" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -24380,13 +24455,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C9" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D9" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -24394,13 +24469,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D10" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -24408,13 +24483,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C11" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D11" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -24422,13 +24497,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -24436,13 +24511,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D13" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -24450,13 +24525,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C14" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D14" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -24464,13 +24539,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D15" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -24498,24 +24573,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -24523,13 +24598,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24537,21 +24612,21 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D4" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D6" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -24559,13 +24634,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C7" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D7" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -24573,13 +24648,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C8" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D8" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -24587,13 +24662,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C9" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D9" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -24601,21 +24676,21 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D12" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -24623,7 +24698,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Les fichiers suivants n'ont pas pu être déplacé, car ils existent déjà dans la bibliothéque : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24639,7 +24714,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Les fichiers suivants ont été déplacé : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24655,7 +24730,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Une erreur inconnu s'est produite : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24671,13 +24746,13 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C16" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D16" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -24685,21 +24760,21 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C17" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D17" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D19" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -24707,13 +24782,13 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C20" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D20" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -24721,13 +24796,13 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -24754,24 +24829,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -24779,13 +24854,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24793,13 +24868,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>528</v>
+      </c>
+      <c r="C4" t="s">
         <v>530</v>
       </c>
-      <c r="C4" t="s">
-        <v>532</v>
-      </c>
       <c r="D4" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -24807,13 +24882,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -24821,13 +24896,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D6" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="135" x14ac:dyDescent="0.25">
@@ -24835,7 +24910,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>CONCATENATE("&lt;html&gt;&lt;p&gt;La configuration de l'application Caerus repose sur un fichier qui permet de paramétrer entiérement la génération des interfaces et des analyses.&lt;br/&gt;","Vous pouvez modifier la configuration à utiliser dans cette interface, mais vous pouvez aussi ajouter, modifier ou supprimer des configurations en agissant dans le repertoire '%s'&lt;br/&gt;","Bientot des fenêtres graphique seront ajouter à l'application pour faciliter ses changements&lt;/p&gt;&lt;/html&gt;")</f>
@@ -24851,13 +24926,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C8" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D8" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -24865,13 +24940,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -24879,13 +24954,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -24915,11 +24990,100 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357A141E-D5BD-46DF-8EEC-B92516C123B1}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="53.85546875" customWidth="1"/>
+    <col min="3" max="4" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>558</v>
+      </c>
+      <c r="D2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>559</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>560</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904B2FA-CBC2-495A-A197-D0CDD47EB1AE}">
-  <dimension ref="A1:A369"/>
+  <dimension ref="A1:A391"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A369" sqref="A1:A369"/>
+    <sheetView showZeros="0" topLeftCell="A268" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A288" sqref="A1:A391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25200,13 +25364,13 @@
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>IF('Fenêtre principal'!B47&lt;&gt;"",CONCATENATE('Fenêtre principal'!B47,"=", 'Fenêtre principal'!C47),IF('Fenêtre principal'!C47&lt;&gt;"",'Fenêtre principal'!C47,""))</f>
-        <v/>
+        <v>menu.about=A propos</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>IF('Fenêtre principal'!B48&lt;&gt;"",CONCATENATE('Fenêtre principal'!B48,"=", 'Fenêtre principal'!C48),IF('Fenêtre principal'!C48&lt;&gt;"",'Fenêtre principal'!C48,""))</f>
-        <v/>
+        <v>menu.about.open=Ouvrir</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
@@ -25248,6 +25412,18 @@
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>IF('Fenêtre principal'!B55&lt;&gt;"",CONCATENATE('Fenêtre principal'!B55,"=", 'Fenêtre principal'!C55),IF('Fenêtre principal'!C55&lt;&gt;"",'Fenêtre principal'!C55,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="str">
+        <f>IF('Fenêtre principal'!B56&lt;&gt;"",CONCATENATE('Fenêtre principal'!B56,"=", 'Fenêtre principal'!C56),IF('Fenêtre principal'!C56&lt;&gt;"",'Fenêtre principal'!C56,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="str">
+        <f>IF('Fenêtre principal'!B57&lt;&gt;"",CONCATENATE('Fenêtre principal'!B57,"=", 'Fenêtre principal'!C57),IF('Fenêtre principal'!C57&lt;&gt;"",'Fenêtre principal'!C57,""))</f>
         <v/>
       </c>
     </row>
@@ -25695,6 +25871,42 @@
         <v/>
       </c>
     </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="str">
+        <f>IF('Fenêtre spécifique'!B32&lt;&gt;"",CONCATENATE('Fenêtre spécifique'!B32,"=", 'Fenêtre spécifique'!C32),IF('Fenêtre spécifique'!C32&lt;&gt;"",'Fenêtre spécifique'!C32,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="str">
+        <f>IF('Fenêtre spécifique'!B33&lt;&gt;"",CONCATENATE('Fenêtre spécifique'!B33,"=", 'Fenêtre spécifique'!C33),IF('Fenêtre spécifique'!C33&lt;&gt;"",'Fenêtre spécifique'!C33,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="str">
+        <f>IF('Fenêtre spécifique'!B34&lt;&gt;"",CONCATENATE('Fenêtre spécifique'!B34,"=", 'Fenêtre spécifique'!C34),IF('Fenêtre spécifique'!C34&lt;&gt;"",'Fenêtre spécifique'!C34,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="str">
+        <f>IF('Fenêtre spécifique'!B35&lt;&gt;"",CONCATENATE('Fenêtre spécifique'!B35,"=", 'Fenêtre spécifique'!C35),IF('Fenêtre spécifique'!C35&lt;&gt;"",'Fenêtre spécifique'!C35,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="str">
+        <f>IF('Fenêtre spécifique'!B36&lt;&gt;"",CONCATENATE('Fenêtre spécifique'!B36,"=", 'Fenêtre spécifique'!C36),IF('Fenêtre spécifique'!C36&lt;&gt;"",'Fenêtre spécifique'!C36,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="str">
+        <f>IF('Fenêtre spécifique'!B37&lt;&gt;"",CONCATENATE('Fenêtre spécifique'!B37,"=", 'Fenêtre spécifique'!C37),IF('Fenêtre spécifique'!C37&lt;&gt;"",'Fenêtre spécifique'!C37,""))</f>
+        <v/>
+      </c>
+    </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="str">
         <f>IF('Fenêtre Chargement document'!B2&lt;&gt;"",CONCATENATE('Fenêtre Chargement document'!B2,"=", 'Fenêtre Chargement document'!C2),IF('Fenêtre Chargement document'!C2&lt;&gt;"",'Fenêtre Chargement document'!C2,""))</f>
@@ -26751,339 +26963,477 @@
         <v/>
       </c>
     </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" t="str">
+        <f>IF(Autres!B2&lt;&gt;"",CONCATENATE(Autres!B2,"=", Autres!C2),IF(Autres!C2&lt;&gt;"",Autres!C2,""))</f>
+        <v>#Message reprise correction</v>
+      </c>
+    </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" t="str">
-        <f>IF(Autres!B2&lt;&gt;"",CONCATENATE(Autres!B2,"=", Autres!C2),IF(Autres!C2&lt;&gt;"",Autres!C2,""))</f>
-        <v>#Message reprise correction</v>
+        <f>IF(Autres!B3&lt;&gt;"",CONCATENATE(Autres!B3,"=", Autres!C3),IF(Autres!C3&lt;&gt;"",Autres!C3,""))</f>
+        <v>window.recovery.error.state.answer=Une analyse en cours de correction a été detecté.\nSouhaitez vous reprendre la correction en cours ?</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" t="str">
-        <f>IF(Autres!B3&lt;&gt;"",CONCATENATE(Autres!B3,"=", Autres!C3),IF(Autres!C3&lt;&gt;"",Autres!C3,""))</f>
-        <v>window.recovery.error.state.answer=Une analyse en cours de correction a été detecté.\nSouhaitez vous reprendre la correction en cours ?</v>
+        <f>IF(Autres!B4&lt;&gt;"",CONCATENATE(Autres!B4,"=", Autres!C4),IF(Autres!C4&lt;&gt;"",Autres!C4,""))</f>
+        <v>window.recovery.error.state.title=Reprendre</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" t="str">
-        <f>IF(Autres!B4&lt;&gt;"",CONCATENATE(Autres!B4,"=", Autres!C4),IF(Autres!C4&lt;&gt;"",Autres!C4,""))</f>
-        <v>window.recovery.error.state.title=Reprendre</v>
+        <f>IF(Autres!B5&lt;&gt;"",CONCATENATE(Autres!B5,"=", Autres!C5),IF(Autres!C5&lt;&gt;"",Autres!C5,""))</f>
+        <v/>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" t="str">
-        <f>IF(Autres!B5&lt;&gt;"",CONCATENATE(Autres!B5,"=", Autres!C5),IF(Autres!C5&lt;&gt;"",Autres!C5,""))</f>
-        <v/>
+        <f>IF(Autres!B6&lt;&gt;"",CONCATENATE(Autres!B6,"=", Autres!C6),IF(Autres!C6&lt;&gt;"",Autres!C6,""))</f>
+        <v>#Fenêtre d'information</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" t="str">
-        <f>IF(Autres!B6&lt;&gt;"",CONCATENATE(Autres!B6,"=", Autres!C6),IF(Autres!C6&lt;&gt;"",Autres!C6,""))</f>
-        <v>#Fenêtre d'information</v>
+        <f>IF(Autres!B7&lt;&gt;"",CONCATENATE(Autres!B7,"=", Autres!C7),IF(Autres!C7&lt;&gt;"",Autres!C7,""))</f>
+        <v>window.information.panel.label=Message d'information</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" t="str">
-        <f>IF(Autres!B7&lt;&gt;"",CONCATENATE(Autres!B7,"=", Autres!C7),IF(Autres!C7&lt;&gt;"",Autres!C7,""))</f>
-        <v>window.information.panel.label=Message d'information</v>
+        <f>IF(Autres!B8&lt;&gt;"",CONCATENATE(Autres!B8,"=", Autres!C8),IF(Autres!C8&lt;&gt;"",Autres!C8,""))</f>
+        <v>window.information.message.panel.label=Message</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" t="str">
-        <f>IF(Autres!B8&lt;&gt;"",CONCATENATE(Autres!B8,"=", Autres!C8),IF(Autres!C8&lt;&gt;"",Autres!C8,""))</f>
-        <v>window.information.message.panel.label=Message</v>
+        <f>IF(Autres!B9&lt;&gt;"",CONCATENATE(Autres!B9,"=", Autres!C9),IF(Autres!C9&lt;&gt;"",Autres!C9,""))</f>
+        <v>window.information.action.panel.label=Action utilisateur</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" t="str">
-        <f>IF(Autres!B9&lt;&gt;"",CONCATENATE(Autres!B9,"=", Autres!C9),IF(Autres!C9&lt;&gt;"",Autres!C9,""))</f>
-        <v>window.information.action.panel.label=Action utilisateur</v>
+        <f>IF(Autres!B10&lt;&gt;"",CONCATENATE(Autres!B10,"=", Autres!C10),IF(Autres!C10&lt;&gt;"",Autres!C10,""))</f>
+        <v>window.information.action.button.label=Fermer</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" t="str">
-        <f>IF(Autres!B10&lt;&gt;"",CONCATENATE(Autres!B10,"=", Autres!C10),IF(Autres!C10&lt;&gt;"",Autres!C10,""))</f>
-        <v>window.information.action.button.label=Fermer</v>
+        <f>IF(Autres!B11&lt;&gt;"",CONCATENATE(Autres!B11,"=", Autres!C11),IF(Autres!C11&lt;&gt;"",Autres!C11,""))</f>
+        <v/>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" t="str">
-        <f>IF(Autres!B11&lt;&gt;"",CONCATENATE(Autres!B11,"=", Autres!C11),IF(Autres!C11&lt;&gt;"",Autres!C11,""))</f>
-        <v/>
+        <f>IF(Autres!B12&lt;&gt;"",CONCATENATE(Autres!B12,"=", Autres!C12),IF(Autres!C12&lt;&gt;"",Autres!C12,""))</f>
+        <v>#Information pour le déplacement des fichiers</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" t="str">
-        <f>IF(Autres!B12&lt;&gt;"",CONCATENATE(Autres!B12,"=", Autres!C12),IF(Autres!C12&lt;&gt;"",Autres!C12,""))</f>
-        <v>#Information pour le déplacement des fichiers</v>
+        <f>IF(Autres!B13&lt;&gt;"",CONCATENATE(Autres!B13,"=", Autres!C13),IF(Autres!C13&lt;&gt;"",Autres!C13,""))</f>
+        <v>window.message.error.move.file.exists=&lt;html&gt;&lt;p&gt;Les fichiers suivants n'ont pas pu être déplacé, car ils existent déjà dans la bibliothéque : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" t="str">
-        <f>IF(Autres!B13&lt;&gt;"",CONCATENATE(Autres!B13,"=", Autres!C13),IF(Autres!C13&lt;&gt;"",Autres!C13,""))</f>
-        <v>window.message.error.move.file.exists=&lt;html&gt;&lt;p&gt;Les fichiers suivants n'ont pas pu être déplacé, car ils existent déjà dans la bibliothéque : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;</v>
+        <f>IF(Autres!B14&lt;&gt;"",CONCATENATE(Autres!B14,"=", Autres!C14),IF(Autres!C14&lt;&gt;"",Autres!C14,""))</f>
+        <v>window.message.result.move.file=&lt;html&gt;&lt;p&gt;Les fichiers suivants ont été déplacé : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" t="str">
-        <f>IF(Autres!B14&lt;&gt;"",CONCATENATE(Autres!B14,"=", Autres!C14),IF(Autres!C14&lt;&gt;"",Autres!C14,""))</f>
-        <v>window.message.result.move.file=&lt;html&gt;&lt;p&gt;Les fichiers suivants ont été déplacé : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;</v>
+        <f>IF(Autres!B15&lt;&gt;"",CONCATENATE(Autres!B15,"=", Autres!C15),IF(Autres!C15&lt;&gt;"",Autres!C15,""))</f>
+        <v>window.message.unknow.error=&lt;html&gt;&lt;p&gt;Une erreur inconnu s'est produite : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" t="str">
-        <f>IF(Autres!B15&lt;&gt;"",CONCATENATE(Autres!B15,"=", Autres!C15),IF(Autres!C15&lt;&gt;"",Autres!C15,""))</f>
-        <v>window.message.unknow.error=&lt;html&gt;&lt;p&gt;Une erreur inconnu s'est produite : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;</v>
+        <f>IF(Autres!B16&lt;&gt;"",CONCATENATE(Autres!B16,"=", Autres!C16),IF(Autres!C16&lt;&gt;"",Autres!C16,""))</f>
+        <v xml:space="preserve">window.message.from=Depuis : </v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" t="str">
-        <f>IF(Autres!B16&lt;&gt;"",CONCATENATE(Autres!B16,"=", Autres!C16),IF(Autres!C16&lt;&gt;"",Autres!C16,""))</f>
-        <v xml:space="preserve">window.message.from=Depuis : </v>
+        <f>IF(Autres!B17&lt;&gt;"",CONCATENATE(Autres!B17,"=", Autres!C17),IF(Autres!C17&lt;&gt;"",Autres!C17,""))</f>
+        <v xml:space="preserve">window.message.to=Vers : </v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" t="str">
-        <f>IF(Autres!B17&lt;&gt;"",CONCATENATE(Autres!B17,"=", Autres!C17),IF(Autres!C17&lt;&gt;"",Autres!C17,""))</f>
-        <v xml:space="preserve">window.message.to=Vers : </v>
+        <f>IF(Autres!B18&lt;&gt;"",CONCATENATE(Autres!B18,"=", Autres!C18),IF(Autres!C18&lt;&gt;"",Autres!C18,""))</f>
+        <v/>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" t="str">
-        <f>IF(Autres!B18&lt;&gt;"",CONCATENATE(Autres!B18,"=", Autres!C18),IF(Autres!C18&lt;&gt;"",Autres!C18,""))</f>
-        <v/>
+        <f>IF(Autres!B19&lt;&gt;"",CONCATENATE(Autres!B19,"=", Autres!C19),IF(Autres!C19&lt;&gt;"",Autres!C19,""))</f>
+        <v>#Message de prevention en cas de suppression</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" t="str">
-        <f>IF(Autres!B19&lt;&gt;"",CONCATENATE(Autres!B19,"=", Autres!C19),IF(Autres!C19&lt;&gt;"",Autres!C19,""))</f>
-        <v>#Message de prevention en cas de suppression</v>
+        <f>IF(Autres!B20&lt;&gt;"",CONCATENATE(Autres!B20,"=", Autres!C20),IF(Autres!C20&lt;&gt;"",Autres!C20,""))</f>
+        <v>window.manage.texts.delete.text.action.message.title=Message de prévention</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" t="str">
-        <f>IF(Autres!B20&lt;&gt;"",CONCATENATE(Autres!B20,"=", Autres!C20),IF(Autres!C20&lt;&gt;"",Autres!C20,""))</f>
-        <v>window.manage.texts.delete.text.action.message.title=Message de prévention</v>
+        <f>IF(Autres!B21&lt;&gt;"",CONCATENATE(Autres!B21,"=", Autres!C21),IF(Autres!C21&lt;&gt;"",Autres!C21,""))</f>
+        <v>window.manage.texts.delete.text.action.message.content=Vous allez supprimer un texte du corpus.\nCette action sera irréversible.\nVoulez vous continuer ?</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" t="str">
-        <f>IF(Autres!B21&lt;&gt;"",CONCATENATE(Autres!B21,"=", Autres!C21),IF(Autres!C21&lt;&gt;"",Autres!C21,""))</f>
-        <v>window.manage.texts.delete.text.action.message.content=Vous allez supprimer un texte du corpus.\nCette action sera irréversible.\nVoulez vous continuer ?</v>
+        <f>IF(Autres!B22&lt;&gt;"",CONCATENATE(Autres!B22,"=", Autres!C22),IF(Autres!C22&lt;&gt;"",Autres!C22,""))</f>
+        <v/>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" t="str">
-        <f>IF(Autres!B22&lt;&gt;"",CONCATENATE(Autres!B22,"=", Autres!C22),IF(Autres!C22&lt;&gt;"",Autres!C22,""))</f>
+        <f>IF(Autres!B23&lt;&gt;"",CONCATENATE(Autres!B23,"=", Autres!C23),IF(Autres!C23&lt;&gt;"",Autres!C23,""))</f>
         <v/>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" t="str">
-        <f>IF(Autres!B23&lt;&gt;"",CONCATENATE(Autres!B23,"=", Autres!C23),IF(Autres!C23&lt;&gt;"",Autres!C23,""))</f>
+        <f>IF(Autres!B24&lt;&gt;"",CONCATENATE(Autres!B24,"=", Autres!C24),IF(Autres!C24&lt;&gt;"",Autres!C24,""))</f>
         <v/>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" t="str">
-        <f>IF(Autres!B24&lt;&gt;"",CONCATENATE(Autres!B24,"=", Autres!C24),IF(Autres!C24&lt;&gt;"",Autres!C24,""))</f>
+        <f>IF(Autres!B25&lt;&gt;"",CONCATENATE(Autres!B25,"=", Autres!C25),IF(Autres!C25&lt;&gt;"",Autres!C25,""))</f>
         <v/>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" t="str">
-        <f>IF(Autres!B25&lt;&gt;"",CONCATENATE(Autres!B25,"=", Autres!C25),IF(Autres!C25&lt;&gt;"",Autres!C25,""))</f>
+        <f>IF(Autres!B26&lt;&gt;"",CONCATENATE(Autres!B26,"=", Autres!C26),IF(Autres!C26&lt;&gt;"",Autres!C26,""))</f>
         <v/>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" t="str">
-        <f>IF(Autres!B26&lt;&gt;"",CONCATENATE(Autres!B26,"=", Autres!C26),IF(Autres!C26&lt;&gt;"",Autres!C26,""))</f>
+        <f>IF(Autres!B27&lt;&gt;"",CONCATENATE(Autres!B27,"=", Autres!C27),IF(Autres!C27&lt;&gt;"",Autres!C27,""))</f>
         <v/>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" t="str">
-        <f>IF(Autres!B27&lt;&gt;"",CONCATENATE(Autres!B27,"=", Autres!C27),IF(Autres!C27&lt;&gt;"",Autres!C27,""))</f>
+        <f>IF(Autres!B28&lt;&gt;"",CONCATENATE(Autres!B28,"=", Autres!C28),IF(Autres!C28&lt;&gt;"",Autres!C28,""))</f>
         <v/>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" t="str">
-        <f>IF(Autres!B28&lt;&gt;"",CONCATENATE(Autres!B28,"=", Autres!C28),IF(Autres!C28&lt;&gt;"",Autres!C28,""))</f>
+        <f>IF(Autres!B29&lt;&gt;"",CONCATENATE(Autres!B29,"=", Autres!C29),IF(Autres!C29&lt;&gt;"",Autres!C29,""))</f>
         <v/>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" t="str">
-        <f>IF(Autres!B29&lt;&gt;"",CONCATENATE(Autres!B29,"=", Autres!C29),IF(Autres!C29&lt;&gt;"",Autres!C29,""))</f>
+        <f>IF(Autres!B30&lt;&gt;"",CONCATENATE(Autres!B30,"=", Autres!C30),IF(Autres!C30&lt;&gt;"",Autres!C30,""))</f>
         <v/>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" t="str">
-        <f>IF(Autres!B30&lt;&gt;"",CONCATENATE(Autres!B30,"=", Autres!C30),IF(Autres!C30&lt;&gt;"",Autres!C30,""))</f>
+        <f>IF(Autres!B31&lt;&gt;"",CONCATENATE(Autres!B31,"=", Autres!C31),IF(Autres!C31&lt;&gt;"",Autres!C31,""))</f>
         <v/>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" t="str">
-        <f>IF(Autres!B31&lt;&gt;"",CONCATENATE(Autres!B31,"=", Autres!C31),IF(Autres!C31&lt;&gt;"",Autres!C31,""))</f>
+        <f>IF(Autres!B32&lt;&gt;"",CONCATENATE(Autres!B32,"=", Autres!C32),IF(Autres!C32&lt;&gt;"",Autres!C32,""))</f>
         <v/>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" t="str">
-        <f>IF(Autres!B32&lt;&gt;"",CONCATENATE(Autres!B32,"=", Autres!C32),IF(Autres!C32&lt;&gt;"",Autres!C32,""))</f>
+        <f>IF(Autres!B33&lt;&gt;"",CONCATENATE(Autres!B33,"=", Autres!C33),IF(Autres!C33&lt;&gt;"",Autres!C33,""))</f>
         <v/>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" t="str">
-        <f>IF(Autres!B33&lt;&gt;"",CONCATENATE(Autres!B33,"=", Autres!C33),IF(Autres!C33&lt;&gt;"",Autres!C33,""))</f>
+        <f>IF(Autres!B34&lt;&gt;"",CONCATENATE(Autres!B34,"=", Autres!C34),IF(Autres!C34&lt;&gt;"",Autres!C34,""))</f>
         <v/>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" t="str">
-        <f>IF(Autres!B34&lt;&gt;"",CONCATENATE(Autres!B34,"=", Autres!C34),IF(Autres!C34&lt;&gt;"",Autres!C34,""))</f>
+        <f>IF(Autres!B35&lt;&gt;"",CONCATENATE(Autres!B35,"=", Autres!C35),IF(Autres!C35&lt;&gt;"",Autres!C35,""))</f>
         <v/>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" t="str">
-        <f>IF(Autres!B35&lt;&gt;"",CONCATENATE(Autres!B35,"=", Autres!C35),IF(Autres!C35&lt;&gt;"",Autres!C35,""))</f>
-        <v/>
+        <f>IF('Changer Configuration'!B2&lt;&gt;"",CONCATENATE('Changer Configuration'!B2,"=", 'Changer Configuration'!C2),IF('Changer Configuration'!C2&lt;&gt;"",'Changer Configuration'!C2,""))</f>
+        <v>#Message pour le changement de la configuration</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348" t="str">
-        <f>IF('Changer Configuration'!B2&lt;&gt;"",CONCATENATE('Changer Configuration'!B2,"=", 'Changer Configuration'!C2),IF('Changer Configuration'!C2&lt;&gt;"",'Changer Configuration'!C2,""))</f>
-        <v>#Message pour le changement de la configuration</v>
+        <f>IF('Changer Configuration'!B3&lt;&gt;"",CONCATENATE('Changer Configuration'!B3,"=", 'Changer Configuration'!C3),IF('Changer Configuration'!C3&lt;&gt;"",'Changer Configuration'!C3,""))</f>
+        <v>window.change.configuration.title=Configuration courante</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" t="str">
-        <f>IF('Changer Configuration'!B3&lt;&gt;"",CONCATENATE('Changer Configuration'!B3,"=", 'Changer Configuration'!C3),IF('Changer Configuration'!C3&lt;&gt;"",'Changer Configuration'!C3,""))</f>
-        <v>window.change.configuration.title=Configuration courante</v>
+        <f>IF('Changer Configuration'!B4&lt;&gt;"",CONCATENATE('Changer Configuration'!B4,"=", 'Changer Configuration'!C4),IF('Changer Configuration'!C4&lt;&gt;"",'Changer Configuration'!C4,""))</f>
+        <v>window.change.configuration.list.label=Configuration à utiliser :</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" t="str">
-        <f>IF('Changer Configuration'!B4&lt;&gt;"",CONCATENATE('Changer Configuration'!B4,"=", 'Changer Configuration'!C4),IF('Changer Configuration'!C4&lt;&gt;"",'Changer Configuration'!C4,""))</f>
-        <v>window.change.configuration.list.label=Configuration à utiliser :</v>
+        <f>IF('Changer Configuration'!B5&lt;&gt;"",CONCATENATE('Changer Configuration'!B5,"=", 'Changer Configuration'!C5),IF('Changer Configuration'!C5&lt;&gt;"",'Changer Configuration'!C5,""))</f>
+        <v>window.change.configuration.panel.title=Changement de la configuration</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" t="str">
-        <f>IF('Changer Configuration'!B5&lt;&gt;"",CONCATENATE('Changer Configuration'!B5,"=", 'Changer Configuration'!C5),IF('Changer Configuration'!C5&lt;&gt;"",'Changer Configuration'!C5,""))</f>
-        <v>window.change.configuration.panel.title=Changement de la configuration</v>
+        <f>IF('Changer Configuration'!B6&lt;&gt;"",CONCATENATE('Changer Configuration'!B6,"=", 'Changer Configuration'!C6),IF('Changer Configuration'!C6&lt;&gt;"",'Changer Configuration'!C6,""))</f>
+        <v>window.change.configuration.message.panel.title=Message d'information</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" t="str">
-        <f>IF('Changer Configuration'!B6&lt;&gt;"",CONCATENATE('Changer Configuration'!B6,"=", 'Changer Configuration'!C6),IF('Changer Configuration'!C6&lt;&gt;"",'Changer Configuration'!C6,""))</f>
-        <v>window.change.configuration.message.panel.title=Message d'information</v>
+        <f>IF('Changer Configuration'!B7&lt;&gt;"",CONCATENATE('Changer Configuration'!B7,"=", 'Changer Configuration'!C7),IF('Changer Configuration'!C7&lt;&gt;"",'Changer Configuration'!C7,""))</f>
+        <v>window.change.configuration.message.content=&lt;html&gt;&lt;p&gt;La configuration de l'application Caerus repose sur un fichier qui permet de paramétrer entiérement la génération des interfaces et des analyses.&lt;br/&gt;Vous pouvez modifier la configuration à utiliser dans cette interface, mais vous pouvez aussi ajouter, modifier ou supprimer des configurations en agissant dans le repertoire '%s'&lt;br/&gt;Bientot des fenêtres graphique seront ajouter à l'application pour faciliter ses changements&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" t="str">
-        <f>IF('Changer Configuration'!B7&lt;&gt;"",CONCATENATE('Changer Configuration'!B7,"=", 'Changer Configuration'!C7),IF('Changer Configuration'!C7&lt;&gt;"",'Changer Configuration'!C7,""))</f>
-        <v>window.change.configuration.message.content=&lt;html&gt;&lt;p&gt;La configuration de l'application Caerus repose sur un fichier qui permet de paramétrer entiérement la génération des interfaces et des analyses.&lt;br/&gt;Vous pouvez modifier la configuration à utiliser dans cette interface, mais vous pouvez aussi ajouter, modifier ou supprimer des configurations en agissant dans le repertoire '%s'&lt;br/&gt;Bientot des fenêtres graphique seront ajouter à l'application pour faciliter ses changements&lt;/p&gt;&lt;/html&gt;</v>
+        <f>IF('Changer Configuration'!B8&lt;&gt;"",CONCATENATE('Changer Configuration'!B8,"=", 'Changer Configuration'!C8),IF('Changer Configuration'!C8&lt;&gt;"",'Changer Configuration'!C8,""))</f>
+        <v>window.change.configuration.button.apply.and.close=Choisir cette configuration et fermer</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" t="str">
-        <f>IF('Changer Configuration'!B8&lt;&gt;"",CONCATENATE('Changer Configuration'!B8,"=", 'Changer Configuration'!C8),IF('Changer Configuration'!C8&lt;&gt;"",'Changer Configuration'!C8,""))</f>
-        <v>window.change.configuration.button.apply.and.close=Choisir cette configuration et fermer</v>
+        <f>IF('Changer Configuration'!B9&lt;&gt;"",CONCATENATE('Changer Configuration'!B9,"=", 'Changer Configuration'!C9),IF('Changer Configuration'!C9&lt;&gt;"",'Changer Configuration'!C9,""))</f>
+        <v>window.change.configuration.button.close=Fermer</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" t="str">
-        <f>IF('Changer Configuration'!B9&lt;&gt;"",CONCATENATE('Changer Configuration'!B9,"=", 'Changer Configuration'!C9),IF('Changer Configuration'!C9&lt;&gt;"",'Changer Configuration'!C9,""))</f>
-        <v>window.change.configuration.button.close=Fermer</v>
+        <f>IF('Changer Configuration'!B10&lt;&gt;"",CONCATENATE('Changer Configuration'!B10,"=", 'Changer Configuration'!C10),IF('Changer Configuration'!C10&lt;&gt;"",'Changer Configuration'!C10,""))</f>
+        <v>window.change.configuration.buttons.panel.title=Actions</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" t="str">
-        <f>IF('Changer Configuration'!B10&lt;&gt;"",CONCATENATE('Changer Configuration'!B10,"=", 'Changer Configuration'!C10),IF('Changer Configuration'!C10&lt;&gt;"",'Changer Configuration'!C10,""))</f>
-        <v>window.change.configuration.buttons.panel.title=Actions</v>
+        <f>IF('Changer Configuration'!B11&lt;&gt;"",CONCATENATE('Changer Configuration'!B11,"=", 'Changer Configuration'!C11),IF('Changer Configuration'!C11&lt;&gt;"",'Changer Configuration'!C11,""))</f>
+        <v/>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" t="str">
-        <f>IF('Changer Configuration'!B11&lt;&gt;"",CONCATENATE('Changer Configuration'!B11,"=", 'Changer Configuration'!C11),IF('Changer Configuration'!C11&lt;&gt;"",'Changer Configuration'!C11,""))</f>
+        <f>IF('Changer Configuration'!B12&lt;&gt;"",CONCATENATE('Changer Configuration'!B12,"=", 'Changer Configuration'!C12),IF('Changer Configuration'!C12&lt;&gt;"",'Changer Configuration'!C12,""))</f>
         <v/>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" t="str">
-        <f>IF('Changer Configuration'!B12&lt;&gt;"",CONCATENATE('Changer Configuration'!B12,"=", 'Changer Configuration'!C12),IF('Changer Configuration'!C12&lt;&gt;"",'Changer Configuration'!C12,""))</f>
+        <f>IF('Changer Configuration'!B13&lt;&gt;"",CONCATENATE('Changer Configuration'!B13,"=", 'Changer Configuration'!C13),IF('Changer Configuration'!C13&lt;&gt;"",'Changer Configuration'!C13,""))</f>
         <v/>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" t="str">
-        <f>IF('Changer Configuration'!B13&lt;&gt;"",CONCATENATE('Changer Configuration'!B13,"=", 'Changer Configuration'!C13),IF('Changer Configuration'!C13&lt;&gt;"",'Changer Configuration'!C13,""))</f>
+        <f>IF('Changer Configuration'!B14&lt;&gt;"",CONCATENATE('Changer Configuration'!B14,"=", 'Changer Configuration'!C14),IF('Changer Configuration'!C14&lt;&gt;"",'Changer Configuration'!C14,""))</f>
         <v/>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" t="str">
-        <f>IF('Changer Configuration'!B14&lt;&gt;"",CONCATENATE('Changer Configuration'!B14,"=", 'Changer Configuration'!C14),IF('Changer Configuration'!C14&lt;&gt;"",'Changer Configuration'!C14,""))</f>
+        <f>IF('Changer Configuration'!B15&lt;&gt;"",CONCATENATE('Changer Configuration'!B15,"=", 'Changer Configuration'!C15),IF('Changer Configuration'!C15&lt;&gt;"",'Changer Configuration'!C15,""))</f>
         <v/>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" t="str">
-        <f>IF('Changer Configuration'!B15&lt;&gt;"",CONCATENATE('Changer Configuration'!B15,"=", 'Changer Configuration'!C15),IF('Changer Configuration'!C15&lt;&gt;"",'Changer Configuration'!C15,""))</f>
+        <f>IF('Changer Configuration'!B16&lt;&gt;"",CONCATENATE('Changer Configuration'!B16,"=", 'Changer Configuration'!C16),IF('Changer Configuration'!C16&lt;&gt;"",'Changer Configuration'!C16,""))</f>
         <v/>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" t="str">
-        <f>IF('Changer Configuration'!B16&lt;&gt;"",CONCATENATE('Changer Configuration'!B16,"=", 'Changer Configuration'!C16),IF('Changer Configuration'!C16&lt;&gt;"",'Changer Configuration'!C16,""))</f>
+        <f>IF('Changer Configuration'!B17&lt;&gt;"",CONCATENATE('Changer Configuration'!B17,"=", 'Changer Configuration'!C17),IF('Changer Configuration'!C17&lt;&gt;"",'Changer Configuration'!C17,""))</f>
         <v/>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" t="str">
-        <f>IF('Changer Configuration'!B17&lt;&gt;"",CONCATENATE('Changer Configuration'!B17,"=", 'Changer Configuration'!C17),IF('Changer Configuration'!C17&lt;&gt;"",'Changer Configuration'!C17,""))</f>
+        <f>IF('Changer Configuration'!B18&lt;&gt;"",CONCATENATE('Changer Configuration'!B18,"=", 'Changer Configuration'!C18),IF('Changer Configuration'!C18&lt;&gt;"",'Changer Configuration'!C18,""))</f>
         <v/>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" t="str">
-        <f>IF('Changer Configuration'!B18&lt;&gt;"",CONCATENATE('Changer Configuration'!B18,"=", 'Changer Configuration'!C18),IF('Changer Configuration'!C18&lt;&gt;"",'Changer Configuration'!C18,""))</f>
+        <f>IF('Changer Configuration'!B19&lt;&gt;"",CONCATENATE('Changer Configuration'!B19,"=", 'Changer Configuration'!C19),IF('Changer Configuration'!C19&lt;&gt;"",'Changer Configuration'!C19,""))</f>
         <v/>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" t="str">
-        <f>IF('Changer Configuration'!B19&lt;&gt;"",CONCATENATE('Changer Configuration'!B19,"=", 'Changer Configuration'!C19),IF('Changer Configuration'!C19&lt;&gt;"",'Changer Configuration'!C19,""))</f>
+        <f>IF('Changer Configuration'!B20&lt;&gt;"",CONCATENATE('Changer Configuration'!B20,"=", 'Changer Configuration'!C20),IF('Changer Configuration'!C20&lt;&gt;"",'Changer Configuration'!C20,""))</f>
         <v/>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366" t="str">
-        <f>IF('Changer Configuration'!B20&lt;&gt;"",CONCATENATE('Changer Configuration'!B20,"=", 'Changer Configuration'!C20),IF('Changer Configuration'!C20&lt;&gt;"",'Changer Configuration'!C20,""))</f>
+        <f>IF('Changer Configuration'!B21&lt;&gt;"",CONCATENATE('Changer Configuration'!B21,"=", 'Changer Configuration'!C21),IF('Changer Configuration'!C21&lt;&gt;"",'Changer Configuration'!C21,""))</f>
         <v/>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" t="str">
-        <f>IF('Changer Configuration'!B21&lt;&gt;"",CONCATENATE('Changer Configuration'!B21,"=", 'Changer Configuration'!C21),IF('Changer Configuration'!C21&lt;&gt;"",'Changer Configuration'!C21,""))</f>
+        <f>IF('Changer Configuration'!B22&lt;&gt;"",CONCATENATE('Changer Configuration'!B22,"=", 'Changer Configuration'!C22),IF('Changer Configuration'!C22&lt;&gt;"",'Changer Configuration'!C22,""))</f>
         <v/>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" t="str">
-        <f>IF('Changer Configuration'!B22&lt;&gt;"",CONCATENATE('Changer Configuration'!B22,"=", 'Changer Configuration'!C22),IF('Changer Configuration'!C22&lt;&gt;"",'Changer Configuration'!C22,""))</f>
+        <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE('Changer Configuration'!B23,"=", 'Changer Configuration'!C23),IF('Changer Configuration'!C23&lt;&gt;"",'Changer Configuration'!C23,""))</f>
         <v/>
       </c>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A369" t="str">
-        <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE('Changer Configuration'!B23,"=", 'Changer Configuration'!C23),IF('Changer Configuration'!C23&lt;&gt;"",'Changer Configuration'!C23,""))</f>
+        <f>IF('A propos'!B2&lt;&gt;"",CONCATENATE('A propos'!B2,"=", 'A propos'!C2),IF('A propos'!C2&lt;&gt;"",'A propos'!C2,""))</f>
+        <v>#Message pour la fenêtre a propos</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" t="str">
+        <f>IF('A propos'!B3&lt;&gt;"",CONCATENATE('A propos'!B3,"=", 'A propos'!C3),IF('A propos'!C3&lt;&gt;"",'A propos'!C3,""))</f>
+        <v>window.about.title=A propos</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="str">
+        <f>IF('A propos'!B4&lt;&gt;"",CONCATENATE('A propos'!B4,"=", 'A propos'!C4),IF('A propos'!C4&lt;&gt;"",'A propos'!C4,""))</f>
+        <v>window.about.message.content=&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;A propos de l'application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nom de l'application : &lt;/u&gt; Caerus&lt;br /&gt;&lt;u&gt;Version : &lt;/u&gt; 1.0.0&lt;br /&gt;&lt;u&gt;Editeur : &lt;/u&gt; Jeremy, Leda&lt;br /&gt;&lt;u&gt;Site web : &lt;/u&gt;https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="str">
+        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE('A propos'!B5,"=", 'A propos'!C5),IF('A propos'!C5&lt;&gt;"",'A propos'!C5,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="str">
+        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE('A propos'!B6,"=", 'A propos'!C6),IF('A propos'!C6&lt;&gt;"",'A propos'!C6,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" t="str">
+        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE('A propos'!B7,"=", 'A propos'!C7),IF('A propos'!C7&lt;&gt;"",'A propos'!C7,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" t="str">
+        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE('A propos'!B8,"=", 'A propos'!C8),IF('A propos'!C8&lt;&gt;"",'A propos'!C8,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" t="str">
+        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE('A propos'!B9,"=", 'A propos'!C9),IF('A propos'!C9&lt;&gt;"",'A propos'!C9,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" t="str">
+        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE('A propos'!B10,"=", 'A propos'!C10),IF('A propos'!C10&lt;&gt;"",'A propos'!C10,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" t="str">
+        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE('A propos'!B11,"=", 'A propos'!C11),IF('A propos'!C11&lt;&gt;"",'A propos'!C11,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" t="str">
+        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE('A propos'!B12,"=", 'A propos'!C12),IF('A propos'!C12&lt;&gt;"",'A propos'!C12,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" t="str">
+        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE('A propos'!B13,"=", 'A propos'!C13),IF('A propos'!C13&lt;&gt;"",'A propos'!C13,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" t="str">
+        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE('A propos'!B14,"=", 'A propos'!C14),IF('A propos'!C14&lt;&gt;"",'A propos'!C14,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" t="str">
+        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE('A propos'!B15,"=", 'A propos'!C15),IF('A propos'!C15&lt;&gt;"",'A propos'!C15,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" t="str">
+        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE('A propos'!B16,"=", 'A propos'!C16),IF('A propos'!C16&lt;&gt;"",'A propos'!C16,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" t="str">
+        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!C17),IF('A propos'!C17&lt;&gt;"",'A propos'!C17,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" t="str">
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!C18),IF('A propos'!C18&lt;&gt;"",'A propos'!C18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" t="str">
+        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!C17),IF('A propos'!C17&lt;&gt;"",'A propos'!C17,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" t="str">
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!C18),IF('A propos'!C18&lt;&gt;"",'A propos'!C18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" t="str">
+        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!C19),IF('A propos'!C19&lt;&gt;"",'A propos'!C19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" t="str">
+        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE('A propos'!B20,"=", 'A propos'!C42),IF('A propos'!C20&lt;&gt;"",'A propos'!C20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" t="str">
+        <f>IF('A propos'!B21&lt;&gt;"",CONCATENATE('A propos'!B21,"=", 'A propos'!C43),IF('A propos'!C21&lt;&gt;"",'A propos'!C21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" t="str">
+        <f>IF('A propos'!B22&lt;&gt;"",CONCATENATE('A propos'!B22,"=", 'A propos'!C44),IF('A propos'!C22&lt;&gt;"",'A propos'!C22,""))</f>
         <v/>
       </c>
     </row>
@@ -27092,12 +27442,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
-  <dimension ref="A1:A369"/>
+  <dimension ref="A1:A390"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A328" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A343" sqref="A1:A369"/>
+    <sheetView showZeros="0" topLeftCell="A360" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A384" sqref="A1:A390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27228,7 +27578,7 @@
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF('Fenêtre principal'!B22&lt;&gt;"",CONCATENATE('Fenêtre principal'!B22,"=", 'Fenêtre principal'!D22),IF('Fenêtre principal'!D22&lt;&gt;"",'Fenêtre principal'!D22,""))</f>
-        <v>window.main.configuration.library.panel.state.label=Repertorio de la biblioteca :</v>
+        <v>window.main.configuration.library.panel.state.label=Directorio de la biblioteca :</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -27258,7 +27608,7 @@
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF('Fenêtre principal'!B27&lt;&gt;"",CONCATENATE('Fenêtre principal'!B27,"=", 'Fenêtre principal'!D27),IF('Fenêtre principal'!D27&lt;&gt;"",'Fenêtre principal'!D27,""))</f>
-        <v xml:space="preserve">window.main.analyze.panel.state.folder.label=Repertorio analizado : </v>
+        <v xml:space="preserve">window.main.analyze.panel.state.folder.label=Directorio analizado : </v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
@@ -27378,13 +27728,13 @@
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>IF('Fenêtre principal'!B47&lt;&gt;"",CONCATENATE('Fenêtre principal'!B47,"=", 'Fenêtre principal'!D47),IF('Fenêtre principal'!D47&lt;&gt;"",'Fenêtre principal'!D47,""))</f>
-        <v/>
+        <v>menu.about=Acerca</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>IF('Fenêtre principal'!B48&lt;&gt;"",CONCATENATE('Fenêtre principal'!B48,"=", 'Fenêtre principal'!D48),IF('Fenêtre principal'!D48&lt;&gt;"",'Fenêtre principal'!D48,""))</f>
-        <v/>
+        <v>menu.about.open=Abrir</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
@@ -29316,6 +29666,132 @@
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A369" t="str">
         <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE('Changer Configuration'!B23,"=", 'Changer Configuration'!C23),IF('Changer Configuration'!C23&lt;&gt;"",'Changer Configuration'!C23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" t="str">
+        <f>IF('A propos'!B2&lt;&gt;"",CONCATENATE('A propos'!B2,"=", 'A propos'!D2),IF('A propos'!D2&lt;&gt;"",'A propos'!D2,""))</f>
+        <v>#Mensaje para el cambio de configuración</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="str">
+        <f>IF('A propos'!B3&lt;&gt;"",CONCATENATE('A propos'!B3,"=", 'A propos'!D3),IF('A propos'!D3&lt;&gt;"",'A propos'!D3,""))</f>
+        <v>window.about.title=Acerca</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="str">
+        <f>IF('A propos'!B4&lt;&gt;"",CONCATENATE('A propos'!B4,"=", 'A propos'!D4),IF('A propos'!D4&lt;&gt;"",'A propos'!D4,""))</f>
+        <v>window.about.message.content=&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Acerca de la application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nombre de la application :&lt;/u&gt; Caerus&lt;BR /&gt;&lt;u&gt;Versión :&lt;/u&gt; 1.0.0&lt;br /&gt;&lt;u&gt;Editor :&lt;/u&gt; Jeremy, Leda&lt;br/&gt;&lt;u&gt;Sitio web :&lt;/u&gt; https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="str">
+        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE('A propos'!B5,"=", 'A propos'!D5),IF('A propos'!D5&lt;&gt;"",'A propos'!D5,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" t="str">
+        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE('A propos'!B6,"=", 'A propos'!D6),IF('A propos'!D6&lt;&gt;"",'A propos'!D6,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" t="str">
+        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE('A propos'!B7,"=", 'A propos'!D7),IF('A propos'!D7&lt;&gt;"",'A propos'!D7,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" t="str">
+        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE('A propos'!B8,"=", 'A propos'!D8),IF('A propos'!D8&lt;&gt;"",'A propos'!D8,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" t="str">
+        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE('A propos'!B9,"=", 'A propos'!D9),IF('A propos'!D9&lt;&gt;"",'A propos'!D9,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" t="str">
+        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE('A propos'!B10,"=", 'A propos'!D10),IF('A propos'!D10&lt;&gt;"",'A propos'!D10,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" t="str">
+        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE('A propos'!B11,"=", 'A propos'!D11),IF('A propos'!D11&lt;&gt;"",'A propos'!D11,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" t="str">
+        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE('A propos'!B12,"=", 'A propos'!D12),IF('A propos'!D12&lt;&gt;"",'A propos'!D12,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" t="str">
+        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE('A propos'!B13,"=", 'A propos'!D13),IF('A propos'!D13&lt;&gt;"",'A propos'!D13,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" t="str">
+        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE('A propos'!B14,"=", 'A propos'!D14),IF('A propos'!D14&lt;&gt;"",'A propos'!D14,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" t="str">
+        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE('A propos'!B15,"=", 'A propos'!D15),IF('A propos'!D15&lt;&gt;"",'A propos'!D15,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" t="str">
+        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE('A propos'!B16,"=", 'A propos'!D16),IF('A propos'!D16&lt;&gt;"",'A propos'!D16,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" t="str">
+        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!D17),IF('A propos'!D17&lt;&gt;"",'A propos'!D17,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" t="str">
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!D18),IF('A propos'!D18&lt;&gt;"",'A propos'!D18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" t="str">
+        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!D19),IF('A propos'!D19&lt;&gt;"",'A propos'!D19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" t="str">
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!D18),IF('A propos'!D18&lt;&gt;"",'A propos'!D18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" t="str">
+        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!D19),IF('A propos'!D19&lt;&gt;"",'A propos'!D19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" t="str">
+        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE('A propos'!B20,"=", 'A propos'!D20),IF('A propos'!D20&lt;&gt;"",'A propos'!D20,""))</f>
         <v/>
       </c>
     </row>
@@ -29324,12 +29800,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
-  <dimension ref="A1:A370"/>
+  <dimension ref="A1:A386"/>
   <sheetViews>
-    <sheetView topLeftCell="A336" workbookViewId="0">
-      <selection activeCell="A354" sqref="A354"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29610,13 +30086,13 @@
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>IF('Fenêtre principal'!B47&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Fenêtre principal'!B47),".","_"),"=""", 'Fenêtre principal'!B47,""";"),"")</f>
-        <v/>
+        <v>public static final String MENU_ABOUT="menu.about";</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>IF('Fenêtre principal'!B48&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Fenêtre principal'!B48),".","_"),"=""", 'Fenêtre principal'!B48,""";"),"")</f>
-        <v/>
+        <v>public static final String MENU_ABOUT_OPEN="menu.about.open";</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
@@ -31553,7 +32029,103 @@
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" t="str">
-        <f>IF('Changer Configuration'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B24),".","_"),"=""", 'Changer Configuration'!B24,""";"),"")</f>
+        <f>IF('A propos'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B2),".","_"),"=""", 'A propos'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="str">
+        <f>IF('A propos'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B3),".","_"),"=""", 'A propos'!B3,""";"),"")</f>
+        <v>public static final String WINDOW_ABOUT_TITLE="window.about.title";</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="str">
+        <f>IF('A propos'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B4),".","_"),"=""", 'A propos'!B4,""";"),"")</f>
+        <v>public static final String WINDOW_ABOUT_MESSAGE_CONTENT="window.about.message.content";</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="str">
+        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B5),".","_"),"=""", 'A propos'!B5,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" t="str">
+        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B6),".","_"),"=""", 'A propos'!B6,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" t="str">
+        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B7),".","_"),"=""", 'A propos'!B7,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" t="str">
+        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B8),".","_"),"=""", 'A propos'!B8,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" t="str">
+        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B9),".","_"),"=""", 'A propos'!B9,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" t="str">
+        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B10),".","_"),"=""", 'A propos'!B10,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" t="str">
+        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B11),".","_"),"=""", 'A propos'!B11,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" t="str">
+        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B12),".","_"),"=""", 'A propos'!B12,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" t="str">
+        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B13),".","_"),"=""", 'A propos'!B13,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" t="str">
+        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B14),".","_"),"=""", 'A propos'!B14,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" t="str">
+        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B15),".","_"),"=""", 'A propos'!B15,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" t="str">
+        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B16),".","_"),"=""", 'A propos'!B16,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" t="str">
+        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B17),".","_"),"=""", 'A propos'!B17,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" t="str">
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B18),".","_"),"=""", 'A propos'!B18,""";"),"")</f>
         <v/>
       </c>
     </row>
@@ -31577,26 +32149,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -31604,13 +32176,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -31618,13 +32190,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -31632,13 +32204,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -31646,13 +32218,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -31660,13 +32232,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -31674,13 +32246,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -31688,13 +32260,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -31702,13 +32274,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -31716,13 +32288,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -31749,26 +32321,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -31776,13 +32348,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -31790,13 +32362,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -31804,13 +32376,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -31818,13 +32390,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -31832,13 +32404,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -31847,10 +32419,10 @@
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="C9" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -31858,13 +32430,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D10" t="s">
         <v>153</v>
-      </c>
-      <c r="C10" t="s">
-        <v>154</v>
-      </c>
-      <c r="D10" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -31872,13 +32444,13 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -31886,21 +32458,21 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -31908,13 +32480,13 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -31922,13 +32494,13 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D16" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -31936,21 +32508,21 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
+        <v>180</v>
+      </c>
+      <c r="C17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D17" t="s">
         <v>182</v>
-      </c>
-      <c r="C17" t="s">
-        <v>183</v>
-      </c>
-      <c r="D17" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D19" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -31958,13 +32530,13 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -31972,13 +32544,13 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -32005,26 +32577,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32032,13 +32604,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32047,10 +32619,10 @@
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D5" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32058,13 +32630,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C6" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32073,10 +32645,10 @@
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="C8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D8" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32084,13 +32656,13 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32098,13 +32670,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32112,13 +32684,13 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32126,13 +32698,13 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32140,13 +32712,13 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32154,13 +32726,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32168,13 +32740,13 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32182,13 +32754,13 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32196,13 +32768,13 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D17" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32210,13 +32782,13 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32224,13 +32796,13 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
+        <v>214</v>
+      </c>
+      <c r="C19" t="s">
+        <v>215</v>
+      </c>
+      <c r="D19" t="s">
         <v>216</v>
-      </c>
-      <c r="C19" t="s">
-        <v>217</v>
-      </c>
-      <c r="D19" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32238,10 +32810,10 @@
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D21" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -32249,13 +32821,13 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C22" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D22" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="216.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -32263,7 +32835,7 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C23" s="1" t="str">
         <f>CONCATENATE("&lt;html&gt;&lt;p&gt;Ajouter :&lt;br/&gt;Pour ajouter une nouvelle donnée, il faut absolument remplir toutes les cases et cliquer sur"," Ajouter. Cela va permettre d'effectuer un ajout d'informations au texte en cours.&lt;br/&gt;Éditer :","&lt;br/&gt;Sélectionne exactement l'information de la colonne dans la file qui correspond, de cette manière on modifie l'information ","de cette case dans la ligne sélectionnée, sans créer une nouvelle file et donc des doublons.&lt;br/&gt;","Supprimer :&lt;br/&gt;suit le même fonctionnement de sélectionner la file entière que le bouton Ajouter, et donc, de la même manière,"," on doit faire attention car l'on efface une file complète (la ligne entière), et pas seulement la case de la colonne spécifique à la file sélectionné.&lt;/p&gt;&lt;/html&gt;")</f>
@@ -32279,13 +32851,13 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C24" t="s">
+        <v>223</v>
+      </c>
+      <c r="D24" t="s">
         <v>225</v>
-      </c>
-      <c r="D24" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -32293,7 +32865,7 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C25" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;ATTENTION : &lt;/u&gt;&lt;/b&gt;&lt;br/&gt;&lt;br/&gt;Des erreurs ont été detectés sur cette écran.&lt;br/&gt;Completer les tableaux ci-dessous pour rectifier les erreurs.&lt;br/&gt;Une fois les erreurs corrigés, ce message disparaitra.&lt;/p&gt;&lt;/html&gt;"</f>
@@ -32347,26 +32919,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -32374,13 +32946,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -32388,13 +32960,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -32402,13 +32974,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -32416,13 +32988,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -32430,13 +33002,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -32444,13 +33016,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -32458,13 +33030,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -32472,13 +33044,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -32486,13 +33058,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -32500,13 +33072,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -32514,13 +33086,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -32549,26 +33121,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -32576,13 +33148,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>263</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -32611,26 +33183,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -32638,13 +33210,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -32652,13 +33224,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -32666,13 +33238,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -32680,13 +33252,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -32694,13 +33266,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -32708,13 +33280,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32722,13 +33294,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -32736,13 +33308,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -32750,13 +33322,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -32764,13 +33336,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>498</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -32778,13 +33350,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -32811,26 +33383,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -32838,13 +33410,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -32852,13 +33424,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -32866,13 +33438,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -32880,13 +33452,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -32894,13 +33466,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -32935,24 +33507,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -32960,13 +33532,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -32974,13 +33546,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -32988,13 +33560,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -33002,13 +33574,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -33016,13 +33588,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -33030,13 +33602,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -33044,13 +33616,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -33058,13 +33630,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C10" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -33072,13 +33644,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -33086,13 +33658,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -33100,13 +33672,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D13" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -33114,13 +33686,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C14" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D14" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -33128,13 +33700,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C15" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D15" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -33142,13 +33714,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>325</v>
+      </c>
+      <c r="C16" t="s">
+        <v>326</v>
+      </c>
+      <c r="D16" t="s">
         <v>327</v>
-      </c>
-      <c r="C16" t="s">
-        <v>328</v>
-      </c>
-      <c r="D16" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -33156,13 +33728,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>504</v>
+      </c>
+      <c r="C17" t="s">
         <v>506</v>
       </c>
-      <c r="C17" t="s">
-        <v>508</v>
-      </c>
       <c r="D17" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="329.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -33170,7 +33742,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C18" s="1" t="str">
         <f>CONCATENATE("&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Filtrer :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Pour filtrer les textes cliquer sur Rechercher dans les textes, une fenêtre vous permettant de créer un nouveau filtre va s'ouvrir,","&lt;br /&gt;et vous devrez la fermer avoir de pouvoir faire toutes autres opérations","&lt;br /&gt;&lt;b&gt;&lt;u&gt;Edition corpus :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Après avoir cliquer sur un texte, lorsque vous éditez un corpus, vous pouvez ajouter un texte dans le corpus, &lt;br /&gt;","il sera nécessaire d'enregistrer les modifications pour que le texte soit écrit physiquement dans le fichier, &lt;br /&gt;sinon il sera perdu après la fermeture de l'application","&lt;br /&gt;&lt;b&gt;&lt;u&gt;Edition texte :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Après avoir cliquer sur un texte, cliquez sur le bouton éditer le texte pour éditer un texte&lt;br /&gt;","&lt;b&gt;&lt;u&gt;Supprimer texte :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Après avoir cliquer sur un texte, si vous désirez supprimer un texte, celui ci sera définitvement supprimer (même du fichier physique)&lt;/p&gt;&lt;/html&gt;")</f>

</xml_diff>

<commit_message>
Mise à jour de l'application (traduction)
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dossier Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A88650-0744-4FA8-9E0B-63E2273CA277}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425E0462-7A2B-4E6B-A446-F3828D367D04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="14" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -1721,9 +1721,6 @@
     <t>A propos</t>
   </si>
   <si>
-    <t>Acerca</t>
-  </si>
-  <si>
     <t>#Message pour la fenêtre a propos</t>
   </si>
   <si>
@@ -1749,6 +1746,9 @@
   </si>
   <si>
     <t>&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Acerca de la application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nombre de la application :&lt;/u&gt; Caerus&lt;BR /&gt;&lt;u&gt;Versión :&lt;/u&gt; 1.0.0&lt;br /&gt;&lt;u&gt;Editor :&lt;/u&gt; Jeremy, Leda&lt;br/&gt;&lt;u&gt;Sitio web :&lt;/u&gt; https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>Acerca de</t>
   </si>
 </sst>
 </file>
@@ -23214,8 +23214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF59B93E-40E9-44D6-98FA-7D0A802C1DCE}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23815,13 +23815,13 @@
         <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C47" t="s">
         <v>556</v>
       </c>
       <c r="D47" t="s">
-        <v>557</v>
+        <v>566</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -23829,13 +23829,13 @@
         <v>40</v>
       </c>
       <c r="B48" t="s">
+        <v>561</v>
+      </c>
+      <c r="C48" t="s">
         <v>562</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>563</v>
-      </c>
-      <c r="D48" t="s">
-        <v>564</v>
       </c>
     </row>
   </sheetData>
@@ -24993,8 +24993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357A141E-D5BD-46DF-8EEC-B92516C123B1}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25019,7 +25019,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D2" t="s">
         <v>535</v>
@@ -25030,13 +25030,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>556</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>557</v>
+        <v>566</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -25044,13 +25044,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>565</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -27447,7 +27447,7 @@
   <dimension ref="A1:A390"/>
   <sheetViews>
     <sheetView showZeros="0" topLeftCell="A360" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A384" sqref="A1:A390"/>
+      <selection activeCell="A379" sqref="A1:A390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27728,7 +27728,7 @@
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>IF('Fenêtre principal'!B47&lt;&gt;"",CONCATENATE('Fenêtre principal'!B47,"=", 'Fenêtre principal'!D47),IF('Fenêtre principal'!D47&lt;&gt;"",'Fenêtre principal'!D47,""))</f>
-        <v>menu.about=Acerca</v>
+        <v>menu.about=Acerca de</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
@@ -29678,7 +29678,7 @@
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" t="str">
         <f>IF('A propos'!B3&lt;&gt;"",CONCATENATE('A propos'!B3,"=", 'A propos'!D3),IF('A propos'!D3&lt;&gt;"",'A propos'!D3,""))</f>
-        <v>window.about.title=Acerca</v>
+        <v>window.about.title=Acerca de</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Relecture de la traduction et changement d'un label dans la config
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EEFCCB-FC57-4339-AF25-16DD78CC2039}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7894155-7101-46A4-B227-DC41ED3B8FA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="563">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -296,9 +296,6 @@
     <t>window.fixed.error.line.content.panel.line.error.label</t>
   </si>
   <si>
-    <t>Etiqueta errónea:</t>
-  </si>
-  <si>
     <t>window.fixed.error.line.content.panel.line.fixed.label</t>
   </si>
   <si>
@@ -395,9 +392,6 @@
     <t>window.create.text.name.label</t>
   </si>
   <si>
-    <t>Nom du document:</t>
-  </si>
-  <si>
     <t>window.create.text.content.panel.title</t>
   </si>
   <si>
@@ -410,9 +404,6 @@
     <t>Información del documento</t>
   </si>
   <si>
-    <t>Nombre del documento:</t>
-  </si>
-  <si>
     <t>window.create.text.title</t>
   </si>
   <si>
@@ -494,9 +485,6 @@
     <t>window.create.specific.context.panel.file.label</t>
   </si>
   <si>
-    <t>Nom du materiel:</t>
-  </si>
-  <si>
     <t>window.create.specific.details.panel.title</t>
   </si>
   <si>
@@ -539,9 +527,6 @@
     <t xml:space="preserve">Creación de las informaciones específicas </t>
   </si>
   <si>
-    <t>Nombre del material:</t>
-  </si>
-  <si>
     <t>Anterior</t>
   </si>
   <si>
@@ -1544,9 +1529,6 @@
     <t>Guardar las etiquetas corregidas</t>
   </si>
   <si>
-    <t xml:space="preserve">Ubicación del error: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Emplacement de l'erreur : </t>
   </si>
   <si>
@@ -1734,6 +1716,27 @@
   </si>
   <si>
     <t>Vous allez supprimer un texte du document.\nCette action sera irréversible.\nVoulez vous continuer ?</t>
+  </si>
+  <si>
+    <t>Nom du document</t>
+  </si>
+  <si>
+    <t>Nom du materiel :</t>
+  </si>
+  <si>
+    <t>Nombre del material :</t>
+  </si>
+  <si>
+    <t>Nom du document :</t>
+  </si>
+  <si>
+    <t>Nombre del documento :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubicación del error : </t>
+  </si>
+  <si>
+    <t>Etiqueta errónea :</t>
   </si>
 </sst>
 </file>
@@ -23430,7 +23433,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23503,7 +23506,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -23517,7 +23520,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -23531,13 +23534,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C10" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="D10" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -23545,13 +23548,13 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C11" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="D11" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -23559,7 +23562,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -23573,7 +23576,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -23587,13 +23590,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C14" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="D14" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -23601,13 +23604,13 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C15" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="D15" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -23615,7 +23618,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -23629,13 +23632,13 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C17" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="D17" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -23643,13 +23646,13 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C18" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="D18" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -23657,13 +23660,13 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C19" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D19" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -23683,10 +23686,10 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D22" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -23756,7 +23759,7 @@
         <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -23781,10 +23784,10 @@
         <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D29" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -23893,10 +23896,10 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="D37" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -23907,10 +23910,10 @@
         <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="D38" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -23921,10 +23924,10 @@
         <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="D39" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -23935,10 +23938,10 @@
         <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="D40" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -23949,10 +23952,10 @@
         <v>67</v>
       </c>
       <c r="C41" t="s">
+        <v>481</v>
+      </c>
+      <c r="D41" t="s">
         <v>486</v>
-      </c>
-      <c r="D41" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -23991,10 +23994,10 @@
         <v>74</v>
       </c>
       <c r="C44" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D44" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -24005,10 +24008,10 @@
         <v>75</v>
       </c>
       <c r="C45" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D45" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -24016,13 +24019,13 @@
         <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="C46" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="D46" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -24030,13 +24033,13 @@
         <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="C47" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D47" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -24044,13 +24047,13 @@
         <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="C48" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D48" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -24093,10 +24096,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D2" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -24104,13 +24107,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C3" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="D3" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24118,13 +24121,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C4" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="D4" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -24132,13 +24135,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C5" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -24146,13 +24149,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C6" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="D6" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -24160,13 +24163,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C7" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="D7" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -24174,13 +24177,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C8" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="D8" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -24188,13 +24191,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C9" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D9" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -24202,13 +24205,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C10" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="D10" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -24216,13 +24219,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C11" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="D11" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -24230,13 +24233,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C12" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D12" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -24244,13 +24247,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C13" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D13" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -24258,13 +24261,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C14" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="D14" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -24272,13 +24275,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C15" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D15" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -24321,10 +24324,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D2" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -24332,13 +24335,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C3" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="D3" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24346,13 +24349,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D4" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -24360,13 +24363,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D5" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -24374,13 +24377,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -24388,7 +24391,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Les fichiers suivants vont être générés : &lt;br/&gt;&lt;br/&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24404,13 +24407,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C8" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D8" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -24418,21 +24421,21 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C9" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="D9" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D11" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -24440,13 +24443,13 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C12" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="D12" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -24454,21 +24457,21 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C13" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="D13" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D15" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -24476,13 +24479,13 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C16" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="D16" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -24490,21 +24493,21 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C17" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D17" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D19" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -24512,13 +24515,13 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -24526,13 +24529,13 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C21" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D21" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
     </row>
   </sheetData>
@@ -24573,10 +24576,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D2" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -24584,13 +24587,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C3" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D3" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24598,13 +24601,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C4" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D4" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -24612,13 +24615,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="D5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -24626,13 +24629,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -24640,7 +24643,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Le fichier suivant va être généré : &lt;br/&gt;&lt;br/&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24656,13 +24659,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C8" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D8" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -24670,13 +24673,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C9" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D9" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -24684,13 +24687,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C10" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="D10" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -24698,13 +24701,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C11" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D11" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -24712,13 +24715,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C12" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D12" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -24726,13 +24729,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C13" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D13" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -24740,13 +24743,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C14" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D14" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -24754,13 +24757,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C15" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D15" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -24802,10 +24805,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D2" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -24813,13 +24816,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24827,21 +24830,21 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C4" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D4" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D6" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -24849,13 +24852,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C7" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D7" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -24863,13 +24866,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C8" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D8" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -24877,13 +24880,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C9" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D9" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -24891,21 +24894,21 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D12" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -24913,7 +24916,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Les fichiers suivants n'ont pas pu être déplacé, car ils y sont déjà dans la bibliothéque : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24929,7 +24932,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Les fichiers suivants ont été déplacé : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24945,7 +24948,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Une erreur inconnu s'est produite : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24961,13 +24964,13 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C16" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D16" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -24975,21 +24978,21 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C17" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D17" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="D19" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -24997,13 +25000,13 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C20" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="D20" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -25011,13 +25014,13 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -25058,10 +25061,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D2" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -25069,13 +25072,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>413</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -25083,13 +25086,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C4" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="D4" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -25097,13 +25100,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="C5" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D5" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -25111,13 +25114,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="C6" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D6" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -25125,7 +25128,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>CONCATENATE("&lt;html&gt;&lt;p&gt;La configuration de l’application Caerus est basée sur un fichier qui vous permet de configurer complètement l’interface en fonction des corpus textuels créés.&lt;br/&gt;","Vous pouvez modifier la configuration des corpus et les utiliser avec l'interface de Caerus, vous pouvez également ajouter , modifier ou supprimer les paramètres en agissant dans le répertoire '%s'&lt;br/&gt;","Des fenêtres graphiques seront bientôt ajoutées à l’application pour faciliter vos modifications&lt;/p&gt;&lt;/html&gt;")</f>
@@ -25141,13 +25144,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="C8" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D8" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -25155,13 +25158,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -25169,13 +25172,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -25234,10 +25237,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D2" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -25245,13 +25248,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -25259,13 +25262,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>430</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>440</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -25298,7 +25301,7 @@
   <dimension ref="A1:A391"/>
   <sheetViews>
     <sheetView showZeros="0" topLeftCell="A271" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A225" sqref="A1:A391"/>
+      <selection activeCell="A288" sqref="A1:A391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25819,7 +25822,7 @@
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f>IF('Correction Edit texte'!B12&lt;&gt;"",CONCATENATE('Correction Edit texte'!B12,"=", 'Correction Edit texte'!C12),IF('Correction Edit texte'!C12&lt;&gt;"",'Correction Edit texte'!C12,""))</f>
-        <v>window.create.text.name.label=Nom du document:</v>
+        <v>window.create.text.name.label=Nom du document :</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
@@ -25963,7 +25966,7 @@
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f>IF('Fenêtre spécifique'!B11&lt;&gt;"",CONCATENATE('Fenêtre spécifique'!B11,"=", 'Fenêtre spécifique'!C11),IF('Fenêtre spécifique'!C11&lt;&gt;"",'Fenêtre spécifique'!C11,""))</f>
-        <v>window.create.specific.context.panel.file.label=Nom du materiel:</v>
+        <v>window.create.specific.context.panel.file.label=Nom du materiel :</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
@@ -26347,7 +26350,7 @@
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="str">
         <f>IF('Fenetre Corpus'!B5&lt;&gt;"",CONCATENATE('Fenetre Corpus'!B5,"=", 'Fenetre Corpus'!C5),IF('Fenetre Corpus'!C5&lt;&gt;"",'Fenetre Corpus'!C5,""))</f>
-        <v>window.create.corpus.name.label=Nom du document:</v>
+        <v>window.create.corpus.name.label=Nom du document</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
@@ -27662,7 +27665,7 @@
   <dimension ref="A1:A390"/>
   <sheetViews>
     <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A1:A390"/>
+      <selection activeCell="A11" sqref="A1:A390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28027,7 +28030,7 @@
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f>IF('Fenêtre erreur ligne'!B5&lt;&gt;"",CONCATENATE('Fenêtre erreur ligne'!B5,"=", 'Fenêtre erreur ligne'!D5),IF('Fenêtre erreur ligne'!D5&lt;&gt;"",'Fenêtre erreur ligne'!D5,""))</f>
-        <v>window.fixed.error.line.content.panel.line.error.label=Etiqueta errónea:</v>
+        <v>window.fixed.error.line.content.panel.line.error.label=Etiqueta errónea :</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
@@ -28063,7 +28066,7 @@
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f>IF('Fenêtre erreur ligne'!B11&lt;&gt;"",CONCATENATE('Fenêtre erreur ligne'!B11,"=", 'Fenêtre erreur ligne'!D11),IF('Fenêtre erreur ligne'!D11&lt;&gt;"",'Fenêtre erreur ligne'!D11,""))</f>
-        <v xml:space="preserve">window.fixed.error.line.content.panel.line.file.label=Ubicación del error: </v>
+        <v xml:space="preserve">window.fixed.error.line.content.panel.line.file.label=Ubicación del error : </v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
@@ -28183,7 +28186,7 @@
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f>IF('Correction Edit texte'!B12&lt;&gt;"",CONCATENATE('Correction Edit texte'!B12,"=", 'Correction Edit texte'!D12),IF('Correction Edit texte'!D12&lt;&gt;"",'Correction Edit texte'!D12,""))</f>
-        <v>window.create.text.name.label=Nombre del documento:</v>
+        <v>window.create.text.name.label=Nombre del documento :</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
@@ -28327,7 +28330,7 @@
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f>IF('Fenêtre spécifique'!B11&lt;&gt;"",CONCATENATE('Fenêtre spécifique'!B11,"=", 'Fenêtre spécifique'!D11),IF('Fenêtre spécifique'!D11&lt;&gt;"",'Fenêtre spécifique'!D11,""))</f>
-        <v>window.create.specific.context.panel.file.label=Nombre del material:</v>
+        <v>window.create.specific.context.panel.file.label=Nombre del material :</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
@@ -32354,7 +32357,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32394,10 +32397,10 @@
         <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -32408,7 +32411,7 @@
         <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
         <v>80</v>
@@ -32422,10 +32425,10 @@
         <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>562</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -32433,13 +32436,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="D6" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -32447,13 +32450,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
         <v>84</v>
-      </c>
-      <c r="C7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -32461,13 +32464,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
         <v>86</v>
-      </c>
-      <c r="C8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -32475,13 +32478,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="D9" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -32489,13 +32492,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" t="s">
         <v>93</v>
-      </c>
-      <c r="C10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -32503,13 +32506,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="D11" t="s">
-        <v>498</v>
+        <v>561</v>
       </c>
     </row>
   </sheetData>
@@ -32525,8 +32528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56DE331-9367-41C8-8048-603F1BE40CC9}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32552,7 +32555,7 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>77</v>
@@ -32563,13 +32566,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="D3" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -32577,13 +32580,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
         <v>98</v>
       </c>
-      <c r="C4" t="s">
-        <v>99</v>
-      </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -32591,13 +32594,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="D5" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -32605,13 +32608,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
         <v>102</v>
       </c>
-      <c r="C6" t="s">
-        <v>103</v>
-      </c>
       <c r="D6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -32619,13 +32622,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" t="s">
         <v>104</v>
       </c>
-      <c r="C7" t="s">
-        <v>105</v>
-      </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -32634,10 +32637,10 @@
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="C9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -32645,13 +32648,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" t="s">
         <v>116</v>
-      </c>
-      <c r="C10" t="s">
-        <v>117</v>
-      </c>
-      <c r="D10" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -32659,13 +32662,13 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" t="s">
         <v>112</v>
       </c>
-      <c r="C11" t="s">
-        <v>113</v>
-      </c>
       <c r="D11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -32673,21 +32676,21 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>559</v>
       </c>
       <c r="D12" t="s">
-        <v>120</v>
+        <v>560</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -32695,13 +32698,13 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C15" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="D15" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -32709,13 +32712,13 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C16" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D16" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -32723,21 +32726,21 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D17" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D19" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -32745,13 +32748,13 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C20" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D20" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -32759,13 +32762,13 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D21" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -32781,8 +32784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A0CBF-D1EA-4398-BF25-4CB619502DB4}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32808,7 +32811,7 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>77</v>
@@ -32819,13 +32822,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32834,10 +32837,10 @@
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D5" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32845,13 +32848,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="C6" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D6" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32860,10 +32863,10 @@
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="C8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D8" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32871,13 +32874,13 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D9" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32885,13 +32888,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32899,13 +32902,13 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>557</v>
       </c>
       <c r="D11" t="s">
-        <v>163</v>
+        <v>558</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32913,13 +32916,13 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C12" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="D12" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32927,13 +32930,13 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D13" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32941,13 +32944,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D14" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32955,13 +32958,13 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C15" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D15" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32969,13 +32972,13 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C16" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D16" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32983,13 +32986,13 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C17" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D17" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32997,13 +33000,13 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D18" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33011,13 +33014,13 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C19" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D19" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33025,10 +33028,10 @@
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D21" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -33036,13 +33039,13 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C22" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D22" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="216.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -33050,7 +33053,7 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C23" s="1" t="str">
         <f>CONCATENATE("&lt;html&gt;&lt;p&gt;Ajouter :&lt;br/&gt;Pour ajouter des nouvelles données, c'est à dire une nouvelle file, il faut remplir toutes les cases vides et cliquer sur"," Ajouter. Cela va permettre d'effectuer un ajout de nouvelles informations au texte en cours.&lt;br/&gt;Éditer :","&lt;br/&gt;Sélectionne exactement l'information de la colonne dans la file qui correspond, de cette manière on modifie l'information ","de cette case dans la ligne sélectionnée, sans créer une nouvelle file et donc sans doublons.&lt;br/&gt;","Supprimer :&lt;br/&gt;fonctionne en sélectionnant la file entière et donc, on doit faire attention car l'on efface une file complète d'informations (la ligne entière), et pas seulement une case spécifique .&lt;/p&gt;&lt;/html&gt;")</f>
@@ -33066,13 +33069,13 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" t="s">
         <v>176</v>
-      </c>
-      <c r="C24" t="s">
-        <v>179</v>
-      </c>
-      <c r="D24" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -33080,7 +33083,7 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C25" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;ATTENTION : &lt;/u&gt;&lt;/b&gt;&lt;br/&gt;&lt;br/&gt;Des erreurs structurels ont été detectés.&lt;br/&gt;Completer les tableaux ci-dessous pour les rectifier.&lt;br/&gt;Une fois les erreurs corrigés ce message disparaitra.&lt;/p&gt;&lt;/html&gt;"</f>
@@ -33150,10 +33153,10 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -33161,13 +33164,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -33175,13 +33178,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -33189,13 +33192,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -33203,13 +33206,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -33217,13 +33220,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -33231,13 +33234,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -33245,13 +33248,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -33259,13 +33262,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -33273,13 +33276,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -33287,13 +33290,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -33301,13 +33304,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -33353,10 +33356,10 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -33364,13 +33367,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -33387,7 +33390,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33415,10 +33418,10 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -33426,13 +33429,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -33440,13 +33443,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -33454,13 +33457,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>115</v>
+        <v>556</v>
       </c>
       <c r="D5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -33468,13 +33471,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D6" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -33482,13 +33485,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -33496,13 +33499,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D8" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -33510,13 +33513,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="D9" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -33524,13 +33527,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D10" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -33538,13 +33541,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -33552,13 +33555,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -33566,13 +33569,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -33615,10 +33618,10 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -33626,13 +33629,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -33640,13 +33643,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -33654,13 +33657,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -33668,13 +33671,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -33682,13 +33685,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -33710,7 +33713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F59160BD-885A-4DEA-9FEE-62F72A09FE0A}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -33737,10 +33740,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D2" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -33748,13 +33751,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="D3" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -33762,13 +33765,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C4" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="D4" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -33776,13 +33779,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C5" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="D5" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -33790,13 +33793,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C6" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="D6" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -33804,13 +33807,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -33818,13 +33821,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -33832,13 +33835,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C9" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D9" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -33846,13 +33849,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C10" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="D10" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -33860,13 +33863,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C11" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="D11" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -33874,13 +33877,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C12" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="D12" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -33888,13 +33891,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C13" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="D13" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -33902,13 +33905,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C14" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="D14" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -33916,13 +33919,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C15" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="D15" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -33930,13 +33933,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C16" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="D16" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -33944,13 +33947,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="C17" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D17" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="329.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -33958,7 +33961,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C18" s="1" t="str">
         <f>CONCATENATE("&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Filtrer le contenu :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Cette fonction vous permet de créer des filtres pour effectuer des recherches dans la bibliothèque en fonction du contenu des documents","&lt;br /&gt;N'oubliez pas de fermer la fenêtre du filtre avant  de pouvoir continuer a faire toute autre opération","&lt;br /&gt;&lt;b&gt;&lt;u&gt;Consulter/Éditer le document :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Cette fonction vous permet de gérer manuellement le contenu de votre bibliothèque. Lorsque vous éditez un document, vous pouvez ajouter du matériel au document. &lt;br /&gt;"," Pensez à enregistrer les modifications pour que le nouveau matériel soit écrit physiquement dans le document .txt, &lt;br /&gt;sinon il sera perdu après la fermeture de l'application","&lt;br /&gt;&lt;b&gt;&lt;u&gt;Consulter/Éditer le matériel :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Cette option vous permet de modifier le texte du matériel et lui ajouter une structure additionnelle grâce aux informations spécifiques en CSV&lt;br /&gt;","&lt;b&gt;&lt;u&gt;Supprimer le matériel :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Après avoir sélectionné un texte, si vous voulez le supprimer , le texte peut être définitivement supprimé avec ce bouton (ATTENTION! vous ne pourrez pas annuler l’action)&lt;/p&gt;&lt;/html&gt;")</f>

</xml_diff>

<commit_message>
Revue des termes et correction choix export excel reference
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7894155-7101-46A4-B227-DC41ED3B8FA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{96846C89-B743-4FE8-B02A-9A5E7B98D02D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>Documents</t>
   </si>
   <si>
-    <t>Charger les documents</t>
-  </si>
-  <si>
     <t>Sortir</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>Documentos</t>
   </si>
   <si>
-    <t>Cargar los documentos .txt</t>
-  </si>
-  <si>
     <t>Salir</t>
   </si>
   <si>
@@ -785,9 +779,6 @@
     <t>window.manage.filters.global.panel.title</t>
   </si>
   <si>
-    <t>Gestion du filtrage des corpus</t>
-  </si>
-  <si>
     <t>window.manage.filters.panel.title</t>
   </si>
   <si>
@@ -830,9 +821,6 @@
     <t>Supprimer le filtre sélectionné</t>
   </si>
   <si>
-    <t>Gestión de filtrado de corpus</t>
-  </si>
-  <si>
     <t>Agregar filtro</t>
   </si>
   <si>
@@ -1403,9 +1391,6 @@
     <t>Consultar/Editar los materiales</t>
   </si>
   <si>
-    <t>Créer des matériels</t>
-  </si>
-  <si>
     <t>Crear materiales</t>
   </si>
   <si>
@@ -1439,9 +1424,6 @@
     <t>Configuración de la biblioteca: NO EXISTE AUN</t>
   </si>
   <si>
-    <t xml:space="preserve">Encabezados con etiquetas vacías : </t>
-  </si>
-  <si>
     <t xml:space="preserve">Materiales con etiquetas vacías : </t>
   </si>
   <si>
@@ -1454,18 +1436,6 @@
     <t>Nouvelle bibliothèque</t>
   </si>
   <si>
-    <t>Gestión de materiales</t>
-  </si>
-  <si>
-    <t>Gestion de matériels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cambiar la configuración </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Changer la configuration </t>
-  </si>
-  <si>
     <t>Guardar Excel personalizado</t>
   </si>
   <si>
@@ -1484,33 +1454,6 @@
     <t>Etiquetas no cumplimentadas</t>
   </si>
   <si>
-    <t xml:space="preserve">En-tête avec des balises vides : </t>
-  </si>
-  <si>
-    <t>Repertoire de ma bibliothèque :</t>
-  </si>
-  <si>
-    <t>Directorio de mi biblioteca :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Éditer les en-têtes </t>
-  </si>
-  <si>
-    <t>Editar etiquetas de materiales</t>
-  </si>
-  <si>
-    <t>Éditer balises des matériels</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bibliothèque Caerus "library"</t>
-  </si>
-  <si>
-    <t>Biblioteca Caerus "library"</t>
-  </si>
-  <si>
-    <t>Editar las cabeceras</t>
-  </si>
-  <si>
     <t xml:space="preserve">Correction des balises </t>
   </si>
   <si>
@@ -1640,12 +1583,6 @@
     <t>Tous les documents de la bibliothèque</t>
   </si>
   <si>
-    <t>La integralidad del contenido coincide con</t>
-  </si>
-  <si>
-    <t>L’intégralité du contenu coïncide avec</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aplicar en el apartado : </t>
   </si>
   <si>
@@ -1737,6 +1674,69 @@
   </si>
   <si>
     <t>Etiqueta errónea :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion du filtrage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestión de filtrado </t>
+  </si>
+  <si>
+    <t>Contenido integral</t>
+  </si>
+  <si>
+    <t>Contenu intégral</t>
+  </si>
+  <si>
+    <t>Editar materiales</t>
+  </si>
+  <si>
+    <t>Repertoire de la bibliothèque Caerus :</t>
+  </si>
+  <si>
+    <t>Directorio de la biblioteca Caerus :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biblioteca Caerus </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bibliothèque Caerus </t>
+  </si>
+  <si>
+    <t>Éditer matériels</t>
+  </si>
+  <si>
+    <t>Créer matériels</t>
+  </si>
+  <si>
+    <t>Cargar documentos .txt</t>
+  </si>
+  <si>
+    <t>Charger documents .txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cambiar configuración </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changer configuration </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documents avec des balises vides : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentos con etiquetas vacías : </t>
+  </si>
+  <si>
+    <t>Éditer les documents</t>
+  </si>
+  <si>
+    <t>Editar los documentos</t>
+  </si>
+  <si>
+    <t>Editar los materiales</t>
+  </si>
+  <si>
+    <t>Éditer les matériels</t>
   </si>
 </sst>
 </file>
@@ -4907,7 +4907,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11887200" y="4686300"/>
+          <a:off x="12430125" y="4686300"/>
           <a:ext cx="3676190" cy="5561905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -23433,7 +23433,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23446,16 +23446,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -23495,10 +23495,10 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -23506,13 +23506,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -23520,13 +23520,13 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>554</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>553</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -23534,13 +23534,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C10" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="D10" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -23548,13 +23548,13 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C11" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="D11" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -23562,13 +23562,13 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -23576,13 +23576,13 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -23590,13 +23590,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C14" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D14" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -23604,13 +23604,13 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C15" t="s">
-        <v>471</v>
+        <v>556</v>
       </c>
       <c r="D15" t="s">
-        <v>470</v>
+        <v>555</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -23618,13 +23618,13 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -23632,13 +23632,13 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C17" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="D17" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -23646,13 +23646,13 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C18" t="s">
-        <v>451</v>
+        <v>552</v>
       </c>
       <c r="D18" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -23660,13 +23660,13 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C19" t="s">
-        <v>469</v>
+        <v>551</v>
       </c>
       <c r="D19" t="s">
-        <v>468</v>
+        <v>546</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -23675,7 +23675,7 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -23683,13 +23683,13 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>479</v>
+        <v>547</v>
       </c>
       <c r="D22" t="s">
-        <v>480</v>
+        <v>548</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -23697,13 +23697,13 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
         <v>15</v>
       </c>
-      <c r="C23" t="s">
-        <v>16</v>
-      </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -23711,13 +23711,13 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -23725,13 +23725,13 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
         <v>18</v>
       </c>
-      <c r="C25" t="s">
-        <v>19</v>
-      </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -23739,13 +23739,13 @@
         <v>18</v>
       </c>
       <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
         <v>20</v>
       </c>
-      <c r="C26" t="s">
-        <v>21</v>
-      </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -23753,13 +23753,13 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -23767,13 +23767,13 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
         <v>23</v>
       </c>
-      <c r="C28" t="s">
-        <v>24</v>
-      </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -23781,13 +23781,13 @@
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D29" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -23795,13 +23795,13 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -23809,13 +23809,13 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
         <v>27</v>
       </c>
-      <c r="C31" t="s">
-        <v>28</v>
-      </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -23823,13 +23823,13 @@
         <v>24</v>
       </c>
       <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" t="s">
         <v>29</v>
       </c>
-      <c r="C32" t="s">
-        <v>30</v>
-      </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -23837,13 +23837,13 @@
         <v>25</v>
       </c>
       <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
         <v>31</v>
       </c>
-      <c r="C33" t="s">
-        <v>32</v>
-      </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -23851,13 +23851,13 @@
         <v>26</v>
       </c>
       <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
         <v>33</v>
       </c>
-      <c r="C34" t="s">
-        <v>34</v>
-      </c>
       <c r="D34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -23865,13 +23865,13 @@
         <v>27</v>
       </c>
       <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
         <v>35</v>
       </c>
-      <c r="C35" t="s">
-        <v>36</v>
-      </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -23879,13 +23879,13 @@
         <v>28</v>
       </c>
       <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
         <v>37</v>
       </c>
-      <c r="C36" t="s">
-        <v>38</v>
-      </c>
       <c r="D36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -23893,13 +23893,13 @@
         <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="D37" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -23907,13 +23907,13 @@
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="D38" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -23921,13 +23921,13 @@
         <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>483</v>
+        <v>562</v>
       </c>
       <c r="D39" t="s">
-        <v>482</v>
+        <v>561</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -23935,13 +23935,13 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>478</v>
+        <v>557</v>
       </c>
       <c r="D40" t="s">
-        <v>463</v>
+        <v>558</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -23949,13 +23949,13 @@
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C41" t="s">
-        <v>481</v>
+        <v>559</v>
       </c>
       <c r="D41" t="s">
-        <v>486</v>
+        <v>560</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -23963,13 +23963,13 @@
         <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C42" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -23977,13 +23977,13 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -23991,13 +23991,13 @@
         <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C44" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="D44" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -24005,13 +24005,13 @@
         <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C45" t="s">
-        <v>484</v>
+        <v>550</v>
       </c>
       <c r="D45" t="s">
-        <v>485</v>
+        <v>549</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -24019,13 +24019,13 @@
         <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C46" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D46" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -24033,13 +24033,13 @@
         <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C47" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D47" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -24047,13 +24047,13 @@
         <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C48" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D48" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -24070,8 +24070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{870B81E7-C827-40EF-A3A3-030244BFE705}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24082,24 +24082,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -24107,13 +24107,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C3" t="s">
-        <v>535</v>
+        <v>514</v>
       </c>
       <c r="D3" t="s">
-        <v>536</v>
+        <v>515</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24121,13 +24121,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C4" t="s">
-        <v>531</v>
+        <v>545</v>
       </c>
       <c r="D4" t="s">
-        <v>530</v>
+        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -24135,13 +24135,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C5" t="s">
-        <v>245</v>
+        <v>542</v>
       </c>
       <c r="D5" t="s">
-        <v>260</v>
+        <v>543</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -24149,13 +24149,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C6" t="s">
-        <v>526</v>
+        <v>507</v>
       </c>
       <c r="D6" t="s">
-        <v>527</v>
+        <v>508</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -24163,13 +24163,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C7" t="s">
-        <v>553</v>
+        <v>532</v>
       </c>
       <c r="D7" t="s">
-        <v>532</v>
+        <v>511</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -24177,13 +24177,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C8" t="s">
-        <v>533</v>
+        <v>512</v>
       </c>
       <c r="D8" t="s">
-        <v>534</v>
+        <v>513</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -24191,13 +24191,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C9" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D9" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -24205,13 +24205,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C10" t="s">
-        <v>517</v>
+        <v>498</v>
       </c>
       <c r="D10" t="s">
-        <v>510</v>
+        <v>491</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -24219,13 +24219,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C11" t="s">
-        <v>519</v>
+        <v>500</v>
       </c>
       <c r="D11" t="s">
-        <v>518</v>
+        <v>499</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -24233,13 +24233,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C12" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D12" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -24247,13 +24247,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C13" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D13" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -24261,13 +24261,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C14" t="s">
-        <v>529</v>
+        <v>510</v>
       </c>
       <c r="D14" t="s">
-        <v>528</v>
+        <v>509</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -24275,13 +24275,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C15" t="s">
+        <v>256</v>
+      </c>
+      <c r="D15" t="s">
         <v>258</v>
-      </c>
-      <c r="C15" t="s">
-        <v>259</v>
-      </c>
-      <c r="D15" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -24310,24 +24310,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -24335,13 +24335,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C3" t="s">
-        <v>543</v>
+        <v>522</v>
       </c>
       <c r="D3" t="s">
-        <v>544</v>
+        <v>523</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24349,13 +24349,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D4" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -24363,13 +24363,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D5" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -24377,13 +24377,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>545</v>
+        <v>524</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>546</v>
+        <v>525</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -24391,7 +24391,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Les fichiers suivants vont être générés : &lt;br/&gt;&lt;br/&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24407,13 +24407,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D8" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -24421,21 +24421,21 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C9" t="s">
-        <v>551</v>
+        <v>530</v>
       </c>
       <c r="D9" t="s">
-        <v>550</v>
+        <v>529</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D11" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -24443,13 +24443,13 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C12" t="s">
-        <v>540</v>
+        <v>519</v>
       </c>
       <c r="D12" t="s">
-        <v>539</v>
+        <v>518</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -24457,21 +24457,21 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C13" t="s">
-        <v>538</v>
+        <v>517</v>
       </c>
       <c r="D13" t="s">
-        <v>537</v>
+        <v>516</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D15" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -24479,13 +24479,13 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C16" t="s">
-        <v>549</v>
+        <v>528</v>
       </c>
       <c r="D16" t="s">
-        <v>548</v>
+        <v>527</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -24493,21 +24493,21 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C17" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D17" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D19" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -24515,13 +24515,13 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>541</v>
+        <v>520</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>542</v>
+        <v>521</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -24529,13 +24529,13 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C21" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D21" t="s">
-        <v>547</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -24562,24 +24562,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -24587,13 +24587,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24601,13 +24601,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C4" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D4" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -24615,13 +24615,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D5" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -24629,13 +24629,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -24643,7 +24643,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Le fichier suivant va être généré : &lt;br/&gt;&lt;br/&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24659,13 +24659,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C8" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D8" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -24673,13 +24673,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C9" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D9" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -24687,13 +24687,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C10" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D10" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -24701,13 +24701,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C11" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D11" t="s">
-        <v>552</v>
+        <v>531</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -24715,13 +24715,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C12" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D12" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -24729,13 +24729,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C13" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D13" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -24743,13 +24743,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C14" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D14" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -24757,13 +24757,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C15" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D15" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -24791,24 +24791,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D2" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -24816,13 +24816,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>494</v>
+        <v>475</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24830,21 +24830,21 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C4" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D4" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D6" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -24852,13 +24852,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C7" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D7" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -24866,13 +24866,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C8" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D8" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -24880,13 +24880,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C9" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D9" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -24894,21 +24894,21 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D12" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -24916,7 +24916,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Les fichiers suivants n'ont pas pu être déplacé, car ils y sont déjà dans la bibliothéque : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24932,7 +24932,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Les fichiers suivants ont été déplacé : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24948,7 +24948,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Une erreur inconnu s'est produite : &lt;br /&gt;&lt;br /&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -24964,13 +24964,13 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C16" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D16" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -24978,21 +24978,21 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C17" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D17" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -25000,13 +25000,13 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C20" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D20" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -25014,13 +25014,13 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>555</v>
+        <v>534</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>554</v>
+        <v>533</v>
       </c>
     </row>
   </sheetData>
@@ -25036,7 +25036,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25047,24 +25047,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -25072,13 +25072,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -25086,13 +25086,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C4" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D4" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -25100,13 +25100,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C5" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D5" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -25114,13 +25114,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D6" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -25128,15 +25128,15 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C7" s="1" t="str">
-        <f>CONCATENATE("&lt;html&gt;&lt;p&gt;La configuration de l’application Caerus est basée sur un fichier qui vous permet de configurer complètement l’interface en fonction des corpus textuels créés.&lt;br/&gt;","Vous pouvez modifier la configuration des corpus et les utiliser avec l'interface de Caerus, vous pouvez également ajouter , modifier ou supprimer les paramètres en agissant dans le répertoire '%s'&lt;br/&gt;","Des fenêtres graphiques seront bientôt ajoutées à l’application pour faciliter vos modifications&lt;/p&gt;&lt;/html&gt;")</f>
-        <v>&lt;html&gt;&lt;p&gt;La configuration de l’application Caerus est basée sur un fichier qui vous permet de configurer complètement l’interface en fonction des corpus textuels créés.&lt;br/&gt;Vous pouvez modifier la configuration des corpus et les utiliser avec l'interface de Caerus, vous pouvez également ajouter , modifier ou supprimer les paramètres en agissant dans le répertoire '%s'&lt;br/&gt;Des fenêtres graphiques seront bientôt ajoutées à l’application pour faciliter vos modifications&lt;/p&gt;&lt;/html&gt;</v>
+        <f>CONCATENATE("&lt;html&gt;&lt;p&gt;La configuration de l’application Caerus est basée sur un fichier qui vous permet de configurer complètement l’interface en fonction des matériels textuels créés.&lt;br/&gt;","Vous pouvez modifier la configuration des matériels et les utiliser avec l'interface de Caerus, vous pouvez également ajouter , modifier ou supprimer les paramètres en agissant dans le répertoire '%s'&lt;br/&gt;","Des fenêtres graphiques seront bientôt ajoutées à l’application pour faciliter vos modifications&lt;/p&gt;&lt;/html&gt;")</f>
+        <v>&lt;html&gt;&lt;p&gt;La configuration de l’application Caerus est basée sur un fichier qui vous permet de configurer complètement l’interface en fonction des matériels textuels créés.&lt;br/&gt;Vous pouvez modifier la configuration des matériels et les utiliser avec l'interface de Caerus, vous pouvez également ajouter , modifier ou supprimer les paramètres en agissant dans le répertoire '%s'&lt;br/&gt;Des fenêtres graphiques seront bientôt ajoutées à l’application pour faciliter vos modifications&lt;/p&gt;&lt;/html&gt;</v>
       </c>
       <c r="D7" s="1" t="str">
-        <f>CONCATENATE("&lt;html&gt;&lt;p&gt;La configuración de la aplicación Caerus se basa en un archivo que le permite configurar completamente la  interfaz en función de los corpus textuales creados.&lt;br/&gt;","Puede modificar la configuración de los corpus y usarlos con el interfaz de Caerus, también puede agregar , modificar o eliminar configuraciones actuando en el directorio '%s'&lt;br/&gt;","Pronto se agregarán ventanas gráficas a la aplicación para facilitar sus cambios&lt;/p&gt;&lt;/html&gt;")</f>
-        <v>&lt;html&gt;&lt;p&gt;La configuración de la aplicación Caerus se basa en un archivo que le permite configurar completamente la  interfaz en función de los corpus textuales creados.&lt;br/&gt;Puede modificar la configuración de los corpus y usarlos con el interfaz de Caerus, también puede agregar , modificar o eliminar configuraciones actuando en el directorio '%s'&lt;br/&gt;Pronto se agregarán ventanas gráficas a la aplicación para facilitar sus cambios&lt;/p&gt;&lt;/html&gt;</v>
+        <f>CONCATENATE("&lt;html&gt;&lt;p&gt;La configuración de la aplicación Caerus se basa en un archivo que le permite configurar completamente el  interfaz en función de los materiales textuales creados.&lt;br/&gt;","Puede modificar la configuración de los materiales y usarlos con el interfaz de Caerus, también puede agregar , modificar o eliminar configuraciones actuando en el directorio '%s'&lt;br/&gt;","Pronto se agregarán ventanas gráficas a la aplicación para facilitar sus cambios&lt;/p&gt;&lt;/html&gt;")</f>
+        <v>&lt;html&gt;&lt;p&gt;La configuración de la aplicación Caerus se basa en un archivo que le permite configurar completamente el  interfaz en función de los materiales textuales creados.&lt;br/&gt;Puede modificar la configuración de los materiales y usarlos con el interfaz de Caerus, también puede agregar , modificar o eliminar configuraciones actuando en el directorio '%s'&lt;br/&gt;Pronto se agregarán ventanas gráficas a la aplicación para facilitar sus cambios&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -25144,13 +25144,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C8" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D8" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -25158,13 +25158,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -25172,13 +25172,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -25223,24 +25223,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -25248,13 +25248,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -25262,13 +25262,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -25301,7 +25301,7 @@
   <dimension ref="A1:A391"/>
   <sheetViews>
     <sheetView showZeros="0" topLeftCell="A271" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A288" sqref="A1:A391"/>
+      <selection activeCell="A286" sqref="A1:A391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25354,7 +25354,7 @@
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF('Fenêtre principal'!B9&lt;&gt;"",CONCATENATE('Fenêtre principal'!B9,"=", 'Fenêtre principal'!C9),IF('Fenêtre principal'!C9&lt;&gt;"",'Fenêtre principal'!C9,""))</f>
-        <v>window.menu.level1.sublevel1.title=Charger les documents</v>
+        <v>window.menu.level1.sublevel1.title=Charger documents .txt</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -25390,7 +25390,7 @@
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF('Fenêtre principal'!B15&lt;&gt;"",CONCATENATE('Fenêtre principal'!B15,"=", 'Fenêtre principal'!C15),IF('Fenêtre principal'!C15&lt;&gt;"",'Fenêtre principal'!C15,""))</f>
-        <v xml:space="preserve">window.menu.level3.sublevel1.title=Changer la configuration </v>
+        <v xml:space="preserve">window.menu.level3.sublevel1.title=Changer configuration </v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
@@ -25408,13 +25408,13 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF('Fenêtre principal'!B18&lt;&gt;"",CONCATENATE('Fenêtre principal'!B18,"=", 'Fenêtre principal'!C18),IF('Fenêtre principal'!C18&lt;&gt;"",'Fenêtre principal'!C18,""))</f>
-        <v>window.menu.level5.sublevel2.title=Créer des matériels</v>
+        <v>window.menu.level5.sublevel2.title=Créer matériels</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF('Fenêtre principal'!B19&lt;&gt;"",CONCATENATE('Fenêtre principal'!B19,"=", 'Fenêtre principal'!C19),IF('Fenêtre principal'!C19&lt;&gt;"",'Fenêtre principal'!C19,""))</f>
-        <v>window.menu.level5.sublevel3.title=Gestion de matériels</v>
+        <v>window.menu.level5.sublevel3.title=Éditer matériels</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -25432,7 +25432,7 @@
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF('Fenêtre principal'!B22&lt;&gt;"",CONCATENATE('Fenêtre principal'!B22,"=", 'Fenêtre principal'!C22),IF('Fenêtre principal'!C22&lt;&gt;"",'Fenêtre principal'!C22,""))</f>
-        <v>window.main.configuration.library.panel.state.label=Repertoire de ma bibliothèque :</v>
+        <v>window.main.configuration.library.panel.state.label=Repertoire de la bibliothèque Caerus :</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -25534,19 +25534,19 @@
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>IF('Fenêtre principal'!B39&lt;&gt;"",CONCATENATE('Fenêtre principal'!B39,"=", 'Fenêtre principal'!C39),IF('Fenêtre principal'!C39&lt;&gt;"",'Fenêtre principal'!C39,""))</f>
-        <v>window.main.blank.line.error.fixed.button.label=Éditer balises des matériels</v>
+        <v>window.main.blank.line.error.fixed.button.label=Éditer les matériels</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>IF('Fenêtre principal'!B40&lt;&gt;"",CONCATENATE('Fenêtre principal'!B40,"=", 'Fenêtre principal'!C40),IF('Fenêtre principal'!C40&lt;&gt;"",'Fenêtre principal'!C40,""))</f>
-        <v xml:space="preserve">window.main.meta.blank.line.error.label=En-tête avec des balises vides : </v>
+        <v xml:space="preserve">window.main.meta.blank.line.error.label=Documents avec des balises vides : </v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>IF('Fenêtre principal'!B41&lt;&gt;"",CONCATENATE('Fenêtre principal'!B41,"=", 'Fenêtre principal'!C41),IF('Fenêtre principal'!C41&lt;&gt;"",'Fenêtre principal'!C41,""))</f>
-        <v xml:space="preserve">window.main.meta.blank.line.error.fixed.button.label=Éditer les en-têtes </v>
+        <v>window.main.meta.blank.line.error.fixed.button.label=Éditer les documents</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
@@ -25570,7 +25570,7 @@
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>IF('Fenêtre principal'!B45&lt;&gt;"",CONCATENATE('Fenêtre principal'!B45,"=", 'Fenêtre principal'!C45),IF('Fenêtre principal'!C45&lt;&gt;"",'Fenêtre principal'!C45,""))</f>
-        <v>window.move.file.library.button.label= Bibliothèque Caerus "library"</v>
+        <v xml:space="preserve">window.move.file.library.button.label= Bibliothèque Caerus </v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
@@ -26734,13 +26734,13 @@
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" t="str">
         <f>IF('Fenetre filtre texte'!B4&lt;&gt;"",CONCATENATE('Fenetre filtre texte'!B4,"=", 'Fenetre filtre texte'!C4),IF('Fenetre filtre texte'!C4&lt;&gt;"",'Fenetre filtre texte'!C4,""))</f>
-        <v>window.filter.type.EQUAL=L’intégralité du contenu coïncide avec</v>
+        <v>window.filter.type.EQUAL=Contenu intégral</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" t="str">
         <f>IF('Fenetre filtre texte'!B5&lt;&gt;"",CONCATENATE('Fenetre filtre texte'!B5,"=", 'Fenetre filtre texte'!C5),IF('Fenetre filtre texte'!C5&lt;&gt;"",'Fenetre filtre texte'!C5,""))</f>
-        <v>window.manage.filters.global.panel.title=Gestion du filtrage des corpus</v>
+        <v xml:space="preserve">window.manage.filters.global.panel.title=Gestion du filtrage </v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
@@ -27418,7 +27418,7 @@
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" t="str">
         <f>IF('Changer Configuration'!B7&lt;&gt;"",CONCATENATE('Changer Configuration'!B7,"=", 'Changer Configuration'!C7),IF('Changer Configuration'!C7&lt;&gt;"",'Changer Configuration'!C7,""))</f>
-        <v>window.change.configuration.message.content=&lt;html&gt;&lt;p&gt;La configuration de l’application Caerus est basée sur un fichier qui vous permet de configurer complètement l’interface en fonction des corpus textuels créés.&lt;br/&gt;Vous pouvez modifier la configuration des corpus et les utiliser avec l'interface de Caerus, vous pouvez également ajouter , modifier ou supprimer les paramètres en agissant dans le répertoire '%s'&lt;br/&gt;Des fenêtres graphiques seront bientôt ajoutées à l’application pour faciliter vos modifications&lt;/p&gt;&lt;/html&gt;</v>
+        <v>window.change.configuration.message.content=&lt;html&gt;&lt;p&gt;La configuration de l’application Caerus est basée sur un fichier qui vous permet de configurer complètement l’interface en fonction des matériels textuels créés.&lt;br/&gt;Vous pouvez modifier la configuration des matériels et les utiliser avec l'interface de Caerus, vous pouvez également ajouter , modifier ou supprimer les paramètres en agissant dans le répertoire '%s'&lt;br/&gt;Des fenêtres graphiques seront bientôt ajoutées à l’application pour faciliter vos modifications&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
@@ -27665,7 +27665,7 @@
   <dimension ref="A1:A390"/>
   <sheetViews>
     <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A1:A390"/>
+      <selection sqref="A1:A390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27718,7 +27718,7 @@
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF('Fenêtre principal'!B9&lt;&gt;"",CONCATENATE('Fenêtre principal'!B9,"=", 'Fenêtre principal'!D9),IF('Fenêtre principal'!D9&lt;&gt;"",'Fenêtre principal'!D9,""))</f>
-        <v>window.menu.level1.sublevel1.title=Cargar los documentos .txt</v>
+        <v>window.menu.level1.sublevel1.title=Cargar documentos .txt</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -27754,7 +27754,7 @@
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF('Fenêtre principal'!B15&lt;&gt;"",CONCATENATE('Fenêtre principal'!B15,"=", 'Fenêtre principal'!D15),IF('Fenêtre principal'!D15&lt;&gt;"",'Fenêtre principal'!D15,""))</f>
-        <v xml:space="preserve">window.menu.level3.sublevel1.title=Cambiar la configuración </v>
+        <v xml:space="preserve">window.menu.level3.sublevel1.title=Cambiar configuración </v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
@@ -27778,7 +27778,7 @@
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF('Fenêtre principal'!B19&lt;&gt;"",CONCATENATE('Fenêtre principal'!B19,"=", 'Fenêtre principal'!D19),IF('Fenêtre principal'!D19&lt;&gt;"",'Fenêtre principal'!D19,""))</f>
-        <v>window.menu.level5.sublevel3.title=Gestión de materiales</v>
+        <v>window.menu.level5.sublevel3.title=Editar materiales</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -27796,7 +27796,7 @@
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF('Fenêtre principal'!B22&lt;&gt;"",CONCATENATE('Fenêtre principal'!B22,"=", 'Fenêtre principal'!D22),IF('Fenêtre principal'!D22&lt;&gt;"",'Fenêtre principal'!D22,""))</f>
-        <v>window.main.configuration.library.panel.state.label=Directorio de mi biblioteca :</v>
+        <v>window.main.configuration.library.panel.state.label=Directorio de la biblioteca Caerus :</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -27898,19 +27898,19 @@
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>IF('Fenêtre principal'!B39&lt;&gt;"",CONCATENATE('Fenêtre principal'!B39,"=", 'Fenêtre principal'!D39),IF('Fenêtre principal'!D39&lt;&gt;"",'Fenêtre principal'!D39,""))</f>
-        <v>window.main.blank.line.error.fixed.button.label=Editar etiquetas de materiales</v>
+        <v>window.main.blank.line.error.fixed.button.label=Editar los materiales</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>IF('Fenêtre principal'!B40&lt;&gt;"",CONCATENATE('Fenêtre principal'!B40,"=", 'Fenêtre principal'!D40),IF('Fenêtre principal'!D40&lt;&gt;"",'Fenêtre principal'!D40,""))</f>
-        <v xml:space="preserve">window.main.meta.blank.line.error.label=Encabezados con etiquetas vacías : </v>
+        <v xml:space="preserve">window.main.meta.blank.line.error.label=Documentos con etiquetas vacías : </v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>IF('Fenêtre principal'!B41&lt;&gt;"",CONCATENATE('Fenêtre principal'!B41,"=", 'Fenêtre principal'!D41),IF('Fenêtre principal'!D41&lt;&gt;"",'Fenêtre principal'!D41,""))</f>
-        <v>window.main.meta.blank.line.error.fixed.button.label=Editar las cabeceras</v>
+        <v>window.main.meta.blank.line.error.fixed.button.label=Editar los documentos</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
@@ -27934,7 +27934,7 @@
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>IF('Fenêtre principal'!B45&lt;&gt;"",CONCATENATE('Fenêtre principal'!B45,"=", 'Fenêtre principal'!D45),IF('Fenêtre principal'!D45&lt;&gt;"",'Fenêtre principal'!D45,""))</f>
-        <v>window.move.file.library.button.label=Biblioteca Caerus "library"</v>
+        <v xml:space="preserve">window.move.file.library.button.label=Biblioteca Caerus </v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
@@ -29098,13 +29098,13 @@
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" t="str">
         <f>IF('Fenetre filtre texte'!B4&lt;&gt;"",CONCATENATE('Fenetre filtre texte'!B4,"=", 'Fenetre filtre texte'!D4),IF('Fenetre filtre texte'!D4&lt;&gt;"",'Fenetre filtre texte'!D4,""))</f>
-        <v>window.filter.type.EQUAL=La integralidad del contenido coincide con</v>
+        <v>window.filter.type.EQUAL=Contenido integral</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" t="str">
         <f>IF('Fenetre filtre texte'!B5&lt;&gt;"",CONCATENATE('Fenetre filtre texte'!B5,"=", 'Fenetre filtre texte'!D5),IF('Fenetre filtre texte'!D5&lt;&gt;"",'Fenetre filtre texte'!D5,""))</f>
-        <v>window.manage.filters.global.panel.title=Gestión de filtrado de corpus</v>
+        <v xml:space="preserve">window.manage.filters.global.panel.title=Gestión de filtrado </v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
@@ -29788,7 +29788,7 @@
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" t="str">
         <f>IF('Changer Configuration'!B7&lt;&gt;"",CONCATENATE('Changer Configuration'!B7,"=", 'Changer Configuration'!D7),IF('Changer Configuration'!D7&lt;&gt;"",'Changer Configuration'!D7,""))</f>
-        <v>window.change.configuration.message.content=&lt;html&gt;&lt;p&gt;La configuración de la aplicación Caerus se basa en un archivo que le permite configurar completamente la  interfaz en función de los corpus textuales creados.&lt;br/&gt;Puede modificar la configuración de los corpus y usarlos con el interfaz de Caerus, también puede agregar , modificar o eliminar configuraciones actuando en el directorio '%s'&lt;br/&gt;Pronto se agregarán ventanas gráficas a la aplicación para facilitar sus cambios&lt;/p&gt;&lt;/html&gt;</v>
+        <v>window.change.configuration.message.content=&lt;html&gt;&lt;p&gt;La configuración de la aplicación Caerus se basa en un archivo que le permite configurar completamente el  interfaz en función de los materiales textuales creados.&lt;br/&gt;Puede modificar la configuración de los materiales y usarlos con el interfaz de Caerus, también puede agregar , modificar o eliminar configuraciones actuando en el directorio '%s'&lt;br/&gt;Pronto se agregarán ventanas gráficas a la aplicación para facilitar sus cambios&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
@@ -32367,26 +32367,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -32394,13 +32394,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>488</v>
+        <v>469</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -32408,13 +32408,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -32422,13 +32422,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>562</v>
+        <v>541</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -32436,13 +32436,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>489</v>
+        <v>470</v>
       </c>
       <c r="D6" t="s">
-        <v>490</v>
+        <v>471</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -32450,13 +32450,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -32464,13 +32464,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -32478,13 +32478,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>491</v>
+        <v>472</v>
       </c>
       <c r="D9" t="s">
-        <v>492</v>
+        <v>473</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -32492,13 +32492,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -32506,13 +32506,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>493</v>
+        <v>474</v>
       </c>
       <c r="D11" t="s">
-        <v>561</v>
+        <v>540</v>
       </c>
     </row>
   </sheetData>
@@ -32528,7 +32528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56DE331-9367-41C8-8048-603F1BE40CC9}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -32539,26 +32539,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -32566,13 +32566,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="D3" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -32580,13 +32580,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -32594,13 +32594,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>496</v>
+        <v>477</v>
       </c>
       <c r="D5" t="s">
-        <v>495</v>
+        <v>476</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -32608,13 +32608,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -32622,13 +32622,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -32637,10 +32637,10 @@
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="C9" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -32648,13 +32648,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" t="s">
         <v>114</v>
-      </c>
-      <c r="C10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D10" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -32662,13 +32662,13 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -32676,21 +32676,21 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>559</v>
+        <v>538</v>
       </c>
       <c r="D12" t="s">
-        <v>560</v>
+        <v>539</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -32698,13 +32698,13 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D15" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -32712,13 +32712,13 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C16" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D16" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -32726,21 +32726,21 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D17" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D19" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -32748,13 +32748,13 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D20" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -32762,13 +32762,13 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -32784,7 +32784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A0CBF-D1EA-4398-BF25-4CB619502DB4}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B29" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -32795,26 +32795,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32822,13 +32822,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32837,10 +32837,10 @@
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="C5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D5" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32848,13 +32848,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D6" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32863,10 +32863,10 @@
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D8" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32874,13 +32874,13 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32888,13 +32888,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32902,13 +32902,13 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>557</v>
+        <v>536</v>
       </c>
       <c r="D11" t="s">
-        <v>558</v>
+        <v>537</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32916,13 +32916,13 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D12" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32930,13 +32930,13 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32944,13 +32944,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32958,13 +32958,13 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32972,13 +32972,13 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32986,13 +32986,13 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33000,13 +33000,13 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33014,13 +33014,13 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D19" t="s">
         <v>165</v>
-      </c>
-      <c r="C19" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33028,10 +33028,10 @@
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D21" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -33039,13 +33039,13 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="216.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -33053,7 +33053,7 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C23" s="1" t="str">
         <f>CONCATENATE("&lt;html&gt;&lt;p&gt;Ajouter :&lt;br/&gt;Pour ajouter des nouvelles données, c'est à dire une nouvelle file, il faut remplir toutes les cases vides et cliquer sur"," Ajouter. Cela va permettre d'effectuer un ajout de nouvelles informations au texte en cours.&lt;br/&gt;Éditer :","&lt;br/&gt;Sélectionne exactement l'information de la colonne dans la file qui correspond, de cette manière on modifie l'information ","de cette case dans la ligne sélectionnée, sans créer une nouvelle file et donc sans doublons.&lt;br/&gt;","Supprimer :&lt;br/&gt;fonctionne en sélectionnant la file entière et donc, on doit faire attention car l'on efface une file complète d'informations (la ligne entière), et pas seulement une case spécifique .&lt;/p&gt;&lt;/html&gt;")</f>
@@ -33069,13 +33069,13 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C24" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" t="s">
         <v>174</v>
-      </c>
-      <c r="D24" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -33083,7 +33083,7 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C25" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;ATTENTION : &lt;/u&gt;&lt;/b&gt;&lt;br/&gt;&lt;br/&gt;Des erreurs structurels ont été detectés.&lt;br/&gt;Completer les tableaux ci-dessous pour les rectifier.&lt;br/&gt;Une fois les erreurs corrigés ce message disparaitra.&lt;/p&gt;&lt;/html&gt;"</f>
@@ -33137,26 +33137,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -33164,13 +33164,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>497</v>
+        <v>478</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -33178,13 +33178,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -33192,13 +33192,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>498</v>
+        <v>479</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>499</v>
+        <v>480</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -33206,13 +33206,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -33220,13 +33220,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -33234,13 +33234,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -33248,13 +33248,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>501</v>
+        <v>482</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>502</v>
+        <v>483</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -33262,13 +33262,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>503</v>
+        <v>484</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>504</v>
+        <v>485</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -33276,13 +33276,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -33290,13 +33290,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>500</v>
+        <v>481</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>502</v>
+        <v>483</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -33304,13 +33304,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>506</v>
+        <v>487</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>505</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -33340,26 +33340,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -33367,13 +33367,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>501</v>
+        <v>482</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>502</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -33402,26 +33402,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -33429,13 +33429,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -33443,13 +33443,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -33457,13 +33457,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>556</v>
+        <v>535</v>
       </c>
       <c r="D5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -33471,13 +33471,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -33485,13 +33485,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -33499,13 +33499,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -33513,13 +33513,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>508</v>
+        <v>489</v>
       </c>
       <c r="D9" t="s">
-        <v>507</v>
+        <v>488</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -33527,13 +33527,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -33541,13 +33541,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -33555,13 +33555,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -33569,13 +33569,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -33602,26 +33602,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -33629,13 +33629,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -33643,13 +33643,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -33657,13 +33657,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -33671,13 +33671,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -33685,13 +33685,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -33713,7 +33713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F59160BD-885A-4DEA-9FEE-62F72A09FE0A}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -33726,24 +33726,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D2" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -33751,13 +33751,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C3" t="s">
-        <v>521</v>
+        <v>502</v>
       </c>
       <c r="D3" t="s">
-        <v>520</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -33765,13 +33765,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C4" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="D4" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -33779,13 +33779,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="D5" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -33793,13 +33793,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C6" t="s">
-        <v>512</v>
+        <v>493</v>
       </c>
       <c r="D6" t="s">
-        <v>513</v>
+        <v>494</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -33807,13 +33807,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -33821,13 +33821,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -33835,13 +33835,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -33849,13 +33849,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C10" t="s">
-        <v>514</v>
+        <v>495</v>
       </c>
       <c r="D10" t="s">
-        <v>515</v>
+        <v>496</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -33863,13 +33863,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C11" t="s">
-        <v>511</v>
+        <v>492</v>
       </c>
       <c r="D11" t="s">
-        <v>516</v>
+        <v>497</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -33877,13 +33877,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C12" t="s">
-        <v>524</v>
+        <v>505</v>
       </c>
       <c r="D12" t="s">
-        <v>525</v>
+        <v>506</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -33891,13 +33891,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C13" t="s">
-        <v>522</v>
+        <v>503</v>
       </c>
       <c r="D13" t="s">
-        <v>523</v>
+        <v>504</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -33905,13 +33905,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C14" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="D14" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -33919,13 +33919,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C15" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="D15" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -33933,13 +33933,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C16" t="s">
-        <v>509</v>
+        <v>490</v>
       </c>
       <c r="D16" t="s">
-        <v>510</v>
+        <v>491</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -33947,13 +33947,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="329.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -33961,7 +33961,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C18" s="1" t="str">
         <f>CONCATENATE("&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Filtrer le contenu :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Cette fonction vous permet de créer des filtres pour effectuer des recherches dans la bibliothèque en fonction du contenu des documents","&lt;br /&gt;N'oubliez pas de fermer la fenêtre du filtre avant  de pouvoir continuer a faire toute autre opération","&lt;br /&gt;&lt;b&gt;&lt;u&gt;Consulter/Éditer le document :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Cette fonction vous permet de gérer manuellement le contenu de votre bibliothèque. Lorsque vous éditez un document, vous pouvez ajouter du matériel au document. &lt;br /&gt;"," Pensez à enregistrer les modifications pour que le nouveau matériel soit écrit physiquement dans le document .txt, &lt;br /&gt;sinon il sera perdu après la fermeture de l'application","&lt;br /&gt;&lt;b&gt;&lt;u&gt;Consulter/Éditer le matériel :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Cette option vous permet de modifier le texte du matériel et lui ajouter une structure additionnelle grâce aux informations spécifiques en CSV&lt;br /&gt;","&lt;b&gt;&lt;u&gt;Supprimer le matériel :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Après avoir sélectionné un texte, si vous voulez le supprimer , le texte peut être définitivement supprimé avec ce bouton (ATTENTION! vous ne pourrez pas annuler l’action)&lt;/p&gt;&lt;/html&gt;")</f>

</xml_diff>

<commit_message>
Ajout de la fonction pour le chargement des texte et readme
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\git\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96846C89-B743-4FE8-B02A-9A5E7B98D02D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27134F94-BA8B-4ED5-8B14-2BB6645BFE1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="579">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -1737,6 +1737,54 @@
   </si>
   <si>
     <t>Éditer les matériels</t>
+  </si>
+  <si>
+    <t>window.load.texts.start.panel.title</t>
+  </si>
+  <si>
+    <t>window.load.texts.informations.panel.title</t>
+  </si>
+  <si>
+    <t>window.load.texts.informations.message</t>
+  </si>
+  <si>
+    <t>window.load.texts.warning.panel.title</t>
+  </si>
+  <si>
+    <t>window.load.texts.warning.message</t>
+  </si>
+  <si>
+    <t>Informations</t>
+  </si>
+  <si>
+    <t>&lt;HTML&gt;&lt;P&gt;Se cargarán los siguientes archivos : &lt;BR /&gt;&lt;BR /&gt; %s &lt;/P&gt;&lt;/HTML&gt;</t>
+  </si>
+  <si>
+    <t>Informaciones</t>
+  </si>
+  <si>
+    <t>Impossible de charger les documents</t>
+  </si>
+  <si>
+    <t>&lt;HTML&gt;&lt;P&gt;Les fichiers ne peuvent pas être chargés.&lt;BR /&gt;Des fichiers qui ne sont pas au format .txt ont été détectés.&lt;/P&gt;&lt;/HTML&gt;</t>
+  </si>
+  <si>
+    <t>&lt;HTML&gt;&lt;P&gt;Los archivos no se pueden cargar.&lt;BR /&gt;Se han detectado archivos que no tienen el formato . txt.&lt;/P&gt;&lt;/HTML&gt;</t>
+  </si>
+  <si>
+    <t>No se pudo cargar los documentos</t>
+  </si>
+  <si>
+    <t>window.load.texts.informations.message.default</t>
+  </si>
+  <si>
+    <t>&lt;HTML&gt;&lt;P&gt;Sélectionnez un dossier avec le bouton Ouvrir&lt;/P&gt;&lt;/HTML&gt;</t>
+  </si>
+  <si>
+    <t>&lt;HTML&gt;&lt;P&gt;Seleccione una carpeta con el botón Abrir&lt;/P&gt;&lt;/HTML&gt;</t>
+  </si>
+  <si>
+    <t>&lt;HTML&gt;&lt;P&gt;Les fichiers suivants vont être chargés :  &lt;BR /&gt;&lt;BR /&gt; %s &lt;/P&gt;&lt;/HTML&gt;</t>
   </si>
 </sst>
 </file>
@@ -1835,7 +1883,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1854,6 +1902,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -17524,7 +17578,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>142498</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>133088</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -18560,16 +18614,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>542925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -18584,8 +18638,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11572875" y="3314700"/>
-          <a:ext cx="390525" cy="257175"/>
+          <a:off x="11696700" y="3343275"/>
+          <a:ext cx="390525" cy="638175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18631,15 +18685,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>4763</xdr:rowOff>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>414338</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -18656,8 +18710,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="11963400" y="3400426"/>
-          <a:ext cx="695325" cy="42862"/>
+          <a:off x="12087225" y="3429001"/>
+          <a:ext cx="695325" cy="423862"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -18686,15 +18740,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2181225</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>2171700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>370856</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>37674</xdr:rowOff>
+      <xdr:colOff>361331</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>180549</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -18717,7 +18771,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6324600" y="2924175"/>
+          <a:off x="6315075" y="4400550"/>
           <a:ext cx="4952381" cy="3409524"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -18730,15 +18784,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1381125</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>1371600</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1771650</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>1762125</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -18753,7 +18807,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5524500" y="2962275"/>
+          <a:off x="5514975" y="4438650"/>
           <a:ext cx="390525" cy="257175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -18800,15 +18854,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1771650</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:colOff>1762125</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2466975</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>33338</xdr:rowOff>
+      <xdr:colOff>2457450</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -18825,7 +18879,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5915025" y="3048001"/>
+          <a:off x="5905500" y="4524376"/>
           <a:ext cx="695325" cy="42862"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -23069,8 +23123,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EBF64311-7537-42EE-8E54-E84D0BF4D4AE}" name="Tableau5" displayName="Tableau5" ref="A1:D13" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23">
-  <autoFilter ref="A1:D13" xr:uid="{41D717A8-3858-4753-BC64-5539E3609195}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EBF64311-7537-42EE-8E54-E84D0BF4D4AE}" name="Tableau5" displayName="Tableau5" ref="A1:D19" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23">
+  <autoFilter ref="A1:D19" xr:uid="{41D717A8-3858-4753-BC64-5539E3609195}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D48463A3-F25C-4F92-A0EB-AE7A06E3CCAE}" name="Numero" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{7BC87355-4EBC-49E3-918B-5DDC49F9416D}" name="Code" dataDxfId="21"/>
@@ -23432,8 +23486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF59B93E-40E9-44D6-98FA-7D0A802C1DCE}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25301,7 +25355,7 @@
   <dimension ref="A1:A391"/>
   <sheetViews>
     <sheetView showZeros="0" topLeftCell="A271" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A286" sqref="A1:A391"/>
+      <selection activeCell="A289" sqref="A1:A391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26200,37 +26254,37 @@
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
         <f>IF('Fenêtre Chargement document'!B14&lt;&gt;"",CONCATENATE('Fenêtre Chargement document'!B14,"=", 'Fenêtre Chargement document'!C14),IF('Fenêtre Chargement document'!C14&lt;&gt;"",'Fenêtre Chargement document'!C14,""))</f>
-        <v/>
+        <v>window.load.texts.start.panel.title=Actions</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="str">
         <f>IF('Fenêtre Chargement document'!B15&lt;&gt;"",CONCATENATE('Fenêtre Chargement document'!B15,"=", 'Fenêtre Chargement document'!C15),IF('Fenêtre Chargement document'!C15&lt;&gt;"",'Fenêtre Chargement document'!C15,""))</f>
-        <v/>
+        <v>window.load.texts.informations.panel.title=Informations</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="str">
         <f>IF('Fenêtre Chargement document'!B16&lt;&gt;"",CONCATENATE('Fenêtre Chargement document'!B16,"=", 'Fenêtre Chargement document'!C16),IF('Fenêtre Chargement document'!C16&lt;&gt;"",'Fenêtre Chargement document'!C16,""))</f>
-        <v/>
+        <v>window.load.texts.informations.message=&lt;HTML&gt;&lt;P&gt;Les fichiers suivants vont être chargés :  &lt;BR /&gt;&lt;BR /&gt; %s &lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="str">
         <f>IF('Fenêtre Chargement document'!B17&lt;&gt;"",CONCATENATE('Fenêtre Chargement document'!B17,"=", 'Fenêtre Chargement document'!C17),IF('Fenêtre Chargement document'!C17&lt;&gt;"",'Fenêtre Chargement document'!C17,""))</f>
-        <v/>
+        <v>window.load.texts.warning.panel.title=Impossible de charger les documents</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="str">
         <f>IF('Fenêtre Chargement document'!B18&lt;&gt;"",CONCATENATE('Fenêtre Chargement document'!B18,"=", 'Fenêtre Chargement document'!C18),IF('Fenêtre Chargement document'!C18&lt;&gt;"",'Fenêtre Chargement document'!C18,""))</f>
-        <v/>
+        <v>window.load.texts.warning.message=&lt;HTML&gt;&lt;P&gt;Les fichiers ne peuvent pas être chargés.&lt;BR /&gt;Des fichiers qui ne sont pas au format .txt ont été détectés.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="str">
         <f>IF('Fenêtre Chargement document'!B19&lt;&gt;"",CONCATENATE('Fenêtre Chargement document'!B19,"=", 'Fenêtre Chargement document'!C19),IF('Fenêtre Chargement document'!C19&lt;&gt;"",'Fenêtre Chargement document'!C19,""))</f>
-        <v/>
+        <v>window.load.texts.informations.message.default=&lt;HTML&gt;&lt;P&gt;Sélectionnez un dossier avec le bouton Ouvrir&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
@@ -28564,37 +28618,37 @@
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
         <f>IF('Fenêtre Chargement document'!B14&lt;&gt;"",CONCATENATE('Fenêtre Chargement document'!B14,"=", 'Fenêtre Chargement document'!D14),IF('Fenêtre Chargement document'!D14&lt;&gt;"",'Fenêtre Chargement document'!D14,""))</f>
-        <v/>
+        <v>window.load.texts.start.panel.title=Acciones</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="str">
         <f>IF('Fenêtre Chargement document'!B15&lt;&gt;"",CONCATENATE('Fenêtre Chargement document'!B15,"=", 'Fenêtre Chargement document'!D15),IF('Fenêtre Chargement document'!D15&lt;&gt;"",'Fenêtre Chargement document'!D15,""))</f>
-        <v/>
+        <v>window.load.texts.informations.panel.title=Informaciones</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="str">
         <f>IF('Fenêtre Chargement document'!B16&lt;&gt;"",CONCATENATE('Fenêtre Chargement document'!B16,"=", 'Fenêtre Chargement document'!D16),IF('Fenêtre Chargement document'!D16&lt;&gt;"",'Fenêtre Chargement document'!D16,""))</f>
-        <v/>
+        <v>window.load.texts.informations.message=&lt;HTML&gt;&lt;P&gt;Se cargarán los siguientes archivos : &lt;BR /&gt;&lt;BR /&gt; %s &lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="str">
         <f>IF('Fenêtre Chargement document'!B17&lt;&gt;"",CONCATENATE('Fenêtre Chargement document'!B17,"=", 'Fenêtre Chargement document'!D17),IF('Fenêtre Chargement document'!D17&lt;&gt;"",'Fenêtre Chargement document'!D17,""))</f>
-        <v/>
+        <v>window.load.texts.warning.panel.title=No se pudo cargar los documentos</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="str">
         <f>IF('Fenêtre Chargement document'!B18&lt;&gt;"",CONCATENATE('Fenêtre Chargement document'!B18,"=", 'Fenêtre Chargement document'!D18),IF('Fenêtre Chargement document'!D18&lt;&gt;"",'Fenêtre Chargement document'!D18,""))</f>
-        <v/>
+        <v>window.load.texts.warning.message=&lt;HTML&gt;&lt;P&gt;Los archivos no se pueden cargar.&lt;BR /&gt;Se han detectado archivos que no tienen el formato . txt.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="str">
         <f>IF('Fenêtre Chargement document'!B19&lt;&gt;"",CONCATENATE('Fenêtre Chargement document'!B19,"=", 'Fenêtre Chargement document'!D19),IF('Fenêtre Chargement document'!D19&lt;&gt;"",'Fenêtre Chargement document'!D19,""))</f>
-        <v/>
+        <v>window.load.texts.informations.message.default=&lt;HTML&gt;&lt;P&gt;Seleccione una carpeta con el botón Abrir&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
@@ -30022,8 +30076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
   <dimension ref="A1:A386"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A154" sqref="A154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30922,37 +30976,37 @@
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
         <f>IF('Fenêtre Chargement document'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Fenêtre Chargement document'!B14),".","_"),"=""", 'Fenêtre Chargement document'!B14,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_LOAD_TEXTS_START_PANEL_TITLE="window.load.texts.start.panel.title";</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="str">
         <f>IF('Fenêtre Chargement document'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Fenêtre Chargement document'!B15),".","_"),"=""", 'Fenêtre Chargement document'!B15,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_LOAD_TEXTS_INFORMATIONS_PANEL_TITLE="window.load.texts.informations.panel.title";</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="str">
         <f>IF('Fenêtre Chargement document'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Fenêtre Chargement document'!B16),".","_"),"=""", 'Fenêtre Chargement document'!B16,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_LOAD_TEXTS_INFORMATIONS_MESSAGE="window.load.texts.informations.message";</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="str">
         <f>IF('Fenêtre Chargement document'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Fenêtre Chargement document'!B17),".","_"),"=""", 'Fenêtre Chargement document'!B17,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_LOAD_TEXTS_WARNING_PANEL_TITLE="window.load.texts.warning.panel.title";</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="str">
         <f>IF('Fenêtre Chargement document'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Fenêtre Chargement document'!B18),".","_"),"=""", 'Fenêtre Chargement document'!B18,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_LOAD_TEXTS_WARNING_MESSAGE="window.load.texts.warning.message";</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="str">
         <f>IF('Fenêtre Chargement document'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Fenêtre Chargement document'!B19),".","_"),"=""", 'Fenêtre Chargement document'!B19,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_LOAD_TEXTS_INFORMATIONS_MESSAGE_DEFAULT="window.load.texts.informations.message.default";</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
@@ -32784,7 +32838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A0CBF-D1EA-4398-BF25-4CB619502DB4}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="B29" workbookViewId="0">
+    <sheetView topLeftCell="B16" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -33124,10 +33178,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F50E13-E608-4097-A6DA-288DD69EAB08}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33311,6 +33365,90 @@
       </c>
       <c r="D13" s="11" t="s">
         <v>486</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>563</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>564</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>565</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>578</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>15</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>566</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>567</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>572</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>17</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>575</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>576</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>577</v>
       </c>
     </row>
   </sheetData>
@@ -33390,7 +33528,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ajout de la fonctionnalité d'export => version 1.1.0
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\git\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59721F61-3195-4619-9DE5-1C23342AF663}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB63D5D-1264-4572-B6E5-441D4BEC543A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="12" activeTab="15" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,10 @@
     <sheet name="Autres" sheetId="13" r:id="rId13"/>
     <sheet name="Changer Configuration" sheetId="17" r:id="rId14"/>
     <sheet name="A propos" sheetId="19" r:id="rId15"/>
-    <sheet name="FR_Properties" sheetId="14" r:id="rId16"/>
-    <sheet name="ES_Properties" sheetId="16" r:id="rId17"/>
-    <sheet name="Constants" sheetId="18" r:id="rId18"/>
+    <sheet name="Export Document Materiel" sheetId="20" r:id="rId16"/>
+    <sheet name="FR_Properties" sheetId="14" r:id="rId17"/>
+    <sheet name="ES_Properties" sheetId="16" r:id="rId18"/>
+    <sheet name="Constants" sheetId="18" r:id="rId19"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="682">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -1343,12 +1344,6 @@
     <t>Abrir</t>
   </si>
   <si>
-    <t>&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;A propos de l'application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nom de l'application : &lt;/u&gt; Caerus&lt;br /&gt;&lt;u&gt;Version : &lt;/u&gt; 1.0.0&lt;br /&gt;&lt;u&gt;Editeur : &lt;/u&gt; Jeremy, Leda&lt;br /&gt;&lt;u&gt;Site web : &lt;/u&gt;https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</t>
-  </si>
-  <si>
-    <t>&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Acerca de la application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nombre de la application :&lt;/u&gt; Caerus&lt;BR /&gt;&lt;u&gt;Versión :&lt;/u&gt; 1.0.0&lt;br /&gt;&lt;u&gt;Editor :&lt;/u&gt; Jeremy, Leda&lt;br/&gt;&lt;u&gt;Sitio web :&lt;/u&gt; https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</t>
-  </si>
-  <si>
     <t>Acerca de</t>
   </si>
   <si>
@@ -1941,6 +1936,165 @@
   </si>
   <si>
     <t>&lt;HTML&gt;&lt;P&gt;Modo experto: En modo experto puede cambiar la etiqueta corregida arriba&lt;BR/&gt;Y cuando todo está bien puede hacer clic en el botón de corrección y pasar al siguiente&lt;/P&gt;&lt;/HTML&gt;</t>
+  </si>
+  <si>
+    <t>window.manage.texts.export.document.text.button.label</t>
+  </si>
+  <si>
+    <t>Exporter Document/Matériel</t>
+  </si>
+  <si>
+    <t>Exportar Documento/Material</t>
+  </si>
+  <si>
+    <t>#Message pour l'export de document et matériel</t>
+  </si>
+  <si>
+    <t>window.export.document.title</t>
+  </si>
+  <si>
+    <t>window.export.document.choose.directory.panel.title</t>
+  </si>
+  <si>
+    <t>window.export.document.choose.directory.label</t>
+  </si>
+  <si>
+    <t>Exporter les documents/matériels</t>
+  </si>
+  <si>
+    <t>Dossier de destination</t>
+  </si>
+  <si>
+    <t>Choix du dossier de destination</t>
+  </si>
+  <si>
+    <t>window.export.document.mode.panel.title</t>
+  </si>
+  <si>
+    <t>Choix des données à exporter</t>
+  </si>
+  <si>
+    <t>window.export.document.mode.document.label</t>
+  </si>
+  <si>
+    <t>Un document</t>
+  </si>
+  <si>
+    <t>window.export.document.mode.all.documents.label</t>
+  </si>
+  <si>
+    <t>Tous les documents</t>
+  </si>
+  <si>
+    <t>window.export.document.mode.result.search.label</t>
+  </si>
+  <si>
+    <t>Le résultat de la recherche</t>
+  </si>
+  <si>
+    <t>window.export.document.choose.document.panel.title</t>
+  </si>
+  <si>
+    <t>window.export.document.choose.document.label</t>
+  </si>
+  <si>
+    <t>Choix du document à exporter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document à exporter : </t>
+  </si>
+  <si>
+    <t>window.export.document.choose.file.panel.title</t>
+  </si>
+  <si>
+    <t>Choix du nom du document</t>
+  </si>
+  <si>
+    <t>window.export.document.choose.file.label</t>
+  </si>
+  <si>
+    <t>window.export.document.button.panel.title</t>
+  </si>
+  <si>
+    <t>Export effectué</t>
+  </si>
+  <si>
+    <t>window.export.document.information.message.title</t>
+  </si>
+  <si>
+    <t>window.export.document.information.message</t>
+  </si>
+  <si>
+    <t>Exportar documentos/materiales</t>
+  </si>
+  <si>
+    <t>Elección de la carpeta de destino</t>
+  </si>
+  <si>
+    <t>Carpeta de destino</t>
+  </si>
+  <si>
+    <t>Elección de los datos a exportar</t>
+  </si>
+  <si>
+    <t>Un documento</t>
+  </si>
+  <si>
+    <t>Todos documentos</t>
+  </si>
+  <si>
+    <t>El resultado de la búsqueda</t>
+  </si>
+  <si>
+    <t>Elección del documento a exportar</t>
+  </si>
+  <si>
+    <t>Documento para exportar :</t>
+  </si>
+  <si>
+    <t>Elección del nombre del documento</t>
+  </si>
+  <si>
+    <t>window.export.document.button.export.label</t>
+  </si>
+  <si>
+    <t>window.export.document.button.close.label</t>
+  </si>
+  <si>
+    <t>Exportación completada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom du document pour le resultat de la recherche : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre del documento para el resultado de la búsqueda : </t>
+  </si>
+  <si>
+    <t>window.export.document.choose.directory.dialog.title</t>
+  </si>
+  <si>
+    <t>Choisissez le dossier de destination</t>
+  </si>
+  <si>
+    <t>Seleccione la carpeta de destino</t>
+  </si>
+  <si>
+    <t>&lt;HTML&gt;&lt;P&gt;Export réalisé avec succés&lt;/P&gt;&lt;/HTML&gt;</t>
+  </si>
+  <si>
+    <t>&lt;HTML&gt;&lt;P&gt;Exportación realizada con éxito&lt;/P&gt;&lt;/HTML&gt;</t>
+  </si>
+  <si>
+    <t>Exporter et fermer</t>
+  </si>
+  <si>
+    <t>Exportar y cerrar</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;A propos de l'application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nom de l'application : &lt;/u&gt; Caerus&lt;br /&gt;&lt;u&gt;Version : &lt;/u&gt; 1.1.0&lt;br /&gt;&lt;u&gt;Editeur : &lt;/u&gt; Jeremy, Leda&lt;br /&gt;&lt;u&gt;Site web : &lt;/u&gt;https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Acerca de la application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nombre de la application :&lt;/u&gt; Caerus&lt;BR /&gt;&lt;u&gt;Versión :&lt;/u&gt; 1.1.0&lt;br /&gt;&lt;u&gt;Editor :&lt;/u&gt; Jeremy, Leda&lt;br/&gt;&lt;u&gt;Sitio web :&lt;/u&gt; https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</t>
   </si>
 </sst>
 </file>
@@ -13138,6 +13292,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>246970</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133104</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Image 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EFD940E-42F3-41DE-873B-C07F1BD2C477}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12020550" y="1019175"/>
+          <a:ext cx="5438095" cy="1971429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -23235,6 +23438,19 @@
     <tableColumn id="2" xr3:uid="{23137A6E-4186-404B-8C24-F3653D56A29E}" name="Code"/>
     <tableColumn id="3" xr3:uid="{AD125158-21C5-4047-A063-80C29885C631}" name="Français"/>
     <tableColumn id="4" xr3:uid="{F3A203CF-2262-4BDF-AA75-7DA21118D925}" name="Español"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{ACF16CE4-3CFE-4EE6-9A66-F2E289DD58BC}" name="Tableau161015" displayName="Tableau161015" ref="A1:D19" totalsRowShown="0">
+  <autoFilter ref="A1:D19" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{7BE777E6-80D5-4607-B506-C54D0BCAA26D}" name="Numero"/>
+    <tableColumn id="2" xr3:uid="{37941F86-4BA1-4EBC-90AD-63A762519C13}" name="Code"/>
+    <tableColumn id="3" xr3:uid="{CA488D13-6ECB-4365-A588-0ADAC244988F}" name="Français"/>
+    <tableColumn id="4" xr3:uid="{BE1263A3-D3DD-44B0-A9A1-949F5F986210}" name="Español"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -23643,7 +23859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF59B93E-40E9-44D6-98FA-7D0A802C1DCE}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
@@ -23734,10 +23950,10 @@
         <v>357</v>
       </c>
       <c r="C9" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D9" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -23748,10 +23964,10 @@
         <v>358</v>
       </c>
       <c r="C10" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D10" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -23762,10 +23978,10 @@
         <v>359</v>
       </c>
       <c r="C11" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D11" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -23818,10 +24034,10 @@
         <v>363</v>
       </c>
       <c r="C15" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D15" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -23846,10 +24062,10 @@
         <v>365</v>
       </c>
       <c r="C17" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D17" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -23860,10 +24076,10 @@
         <v>366</v>
       </c>
       <c r="C18" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D18" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -23874,10 +24090,10 @@
         <v>367</v>
       </c>
       <c r="C19" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D19" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -23897,10 +24113,10 @@
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D22" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -24107,10 +24323,10 @@
         <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D37" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -24121,10 +24337,10 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D38" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -24135,10 +24351,10 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D39" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -24149,10 +24365,10 @@
         <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D40" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -24163,10 +24379,10 @@
         <v>65</v>
       </c>
       <c r="C41" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D41" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -24205,10 +24421,10 @@
         <v>72</v>
       </c>
       <c r="C44" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D44" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -24219,10 +24435,10 @@
         <v>73</v>
       </c>
       <c r="C45" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D45" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -24250,7 +24466,7 @@
         <v>423</v>
       </c>
       <c r="D47" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -24321,10 +24537,10 @@
         <v>240</v>
       </c>
       <c r="C3" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D3" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24335,10 +24551,10 @@
         <v>241</v>
       </c>
       <c r="C4" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D4" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -24349,10 +24565,10 @@
         <v>242</v>
       </c>
       <c r="C5" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D5" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -24363,10 +24579,10 @@
         <v>243</v>
       </c>
       <c r="C6" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D6" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -24377,10 +24593,10 @@
         <v>244</v>
       </c>
       <c r="C7" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D7" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -24391,10 +24607,10 @@
         <v>245</v>
       </c>
       <c r="C8" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D8" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -24419,10 +24635,10 @@
         <v>248</v>
       </c>
       <c r="C10" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D10" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -24433,10 +24649,10 @@
         <v>249</v>
       </c>
       <c r="C11" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D11" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -24475,10 +24691,10 @@
         <v>254</v>
       </c>
       <c r="C14" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D14" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -24549,10 +24765,10 @@
         <v>278</v>
       </c>
       <c r="C3" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D3" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24591,10 +24807,10 @@
         <v>266</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -24635,10 +24851,10 @@
         <v>270</v>
       </c>
       <c r="C9" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D9" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -24657,10 +24873,10 @@
         <v>271</v>
       </c>
       <c r="C12" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D12" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -24671,10 +24887,10 @@
         <v>272</v>
       </c>
       <c r="C13" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D13" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -24693,10 +24909,10 @@
         <v>274</v>
       </c>
       <c r="C16" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D16" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -24729,10 +24945,10 @@
         <v>283</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -24746,7 +24962,7 @@
         <v>285</v>
       </c>
       <c r="D21" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -24918,7 +25134,7 @@
         <v>303</v>
       </c>
       <c r="D11" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -24992,7 +25208,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25033,7 +25249,7 @@
         <v>326</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -25228,18 +25444,18 @@
         <v>347</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D23" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -25247,13 +25463,13 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C24" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D24" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -25261,7 +25477,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C25" t="s">
         <v>145</v>
@@ -25275,7 +25491,7 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C26" t="s">
         <v>147</v>
@@ -25297,7 +25513,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25473,7 +25689,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25515,7 +25731,7 @@
         <v>423</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -25526,10 +25742,10 @@
         <v>426</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>431</v>
+        <v>680</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>432</v>
+        <v>681</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -25558,11 +25774,299 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA2BF44D-1BCC-419E-8C75-D4A062A89580}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="53.85546875" customWidth="1"/>
+    <col min="3" max="4" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>633</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>634</v>
+      </c>
+      <c r="C4" t="s">
+        <v>638</v>
+      </c>
+      <c r="D4" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>635</v>
+      </c>
+      <c r="C5" t="s">
+        <v>637</v>
+      </c>
+      <c r="D5" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>639</v>
+      </c>
+      <c r="C6" t="s">
+        <v>640</v>
+      </c>
+      <c r="D6" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>641</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>643</v>
+      </c>
+      <c r="C8" t="s">
+        <v>644</v>
+      </c>
+      <c r="D8" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>645</v>
+      </c>
+      <c r="C9" t="s">
+        <v>646</v>
+      </c>
+      <c r="D9" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>647</v>
+      </c>
+      <c r="C10" t="s">
+        <v>649</v>
+      </c>
+      <c r="D10" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>648</v>
+      </c>
+      <c r="C11" t="s">
+        <v>650</v>
+      </c>
+      <c r="D11" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>651</v>
+      </c>
+      <c r="C12" t="s">
+        <v>652</v>
+      </c>
+      <c r="D12" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>653</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>654</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>668</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>656</v>
+      </c>
+      <c r="C16" t="s">
+        <v>655</v>
+      </c>
+      <c r="D16" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>657</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>669</v>
+      </c>
+      <c r="C18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>673</v>
+      </c>
+      <c r="C19" t="s">
+        <v>674</v>
+      </c>
+      <c r="D19" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904B2FA-CBC2-495A-A197-D0CDD47EB1AE}">
-  <dimension ref="A1:A403"/>
+  <dimension ref="A1:A436"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A81" sqref="A1:A403"/>
+    <sheetView showZeros="0" topLeftCell="A397" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A418" sqref="A1:A436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27001,7 +27505,7 @@
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" t="str">
         <f>IF('Fenetre Gerer les textes'!B19&lt;&gt;"",CONCATENATE('Fenetre Gerer les textes'!B19,"=", 'Fenetre Gerer les textes'!C19),IF('Fenetre Gerer les textes'!C19&lt;&gt;"",'Fenetre Gerer les textes'!C19,""))</f>
-        <v/>
+        <v>window.manage.texts.export.document.text.button.label=Exporter Document/Matériel</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
@@ -27865,7 +28369,7 @@
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" t="str">
         <f>IF('A propos'!B4&lt;&gt;"",CONCATENATE('A propos'!B4,"=", 'A propos'!C4),IF('A propos'!C4&lt;&gt;"",'A propos'!C4,""))</f>
-        <v>window.about.message.content=&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;A propos de l'application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nom de l'application : &lt;/u&gt; Caerus&lt;br /&gt;&lt;u&gt;Version : &lt;/u&gt; 1.0.0&lt;br /&gt;&lt;u&gt;Editeur : &lt;/u&gt; Jeremy, Leda&lt;br /&gt;&lt;u&gt;Site web : &lt;/u&gt;https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</v>
+        <v>window.about.message.content=&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;A propos de l'application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nom de l'application : &lt;/u&gt; Caerus&lt;br /&gt;&lt;u&gt;Version : &lt;/u&gt; 1.1.0&lt;br /&gt;&lt;u&gt;Editeur : &lt;/u&gt; Jeremy, Leda&lt;br /&gt;&lt;u&gt;Site web : &lt;/u&gt;https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
@@ -27985,6 +28489,204 @@
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" t="str">
         <f>IF('A propos'!B22&lt;&gt;"",CONCATENATE('A propos'!B22,"=", 'A propos'!C44),IF('A propos'!C22&lt;&gt;"",'A propos'!C22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" t="str">
+        <f>IF('Export Document Materiel'!B2&lt;&gt;"",CONCATENATE('Export Document Materiel'!B2,"=", 'Export Document Materiel'!C2),IF('Export Document Materiel'!C2&lt;&gt;"",'Export Document Materiel'!C2,""))</f>
+        <v>#Message pour l'export de document et matériel</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" t="str">
+        <f>IF('Export Document Materiel'!B3&lt;&gt;"",CONCATENATE('Export Document Materiel'!B3,"=", 'Export Document Materiel'!C3),IF('Export Document Materiel'!C3&lt;&gt;"",'Export Document Materiel'!C3,""))</f>
+        <v>window.export.document.title=Exporter les documents/matériels</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" t="str">
+        <f>IF('Export Document Materiel'!B4&lt;&gt;"",CONCATENATE('Export Document Materiel'!B4,"=", 'Export Document Materiel'!C4),IF('Export Document Materiel'!C4&lt;&gt;"",'Export Document Materiel'!C4,""))</f>
+        <v>window.export.document.choose.directory.panel.title=Choix du dossier de destination</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" t="str">
+        <f>IF('Export Document Materiel'!B5&lt;&gt;"",CONCATENATE('Export Document Materiel'!B5,"=", 'Export Document Materiel'!C5),IF('Export Document Materiel'!C5&lt;&gt;"",'Export Document Materiel'!C5,""))</f>
+        <v>window.export.document.choose.directory.label=Dossier de destination</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" t="str">
+        <f>IF('Export Document Materiel'!B6&lt;&gt;"",CONCATENATE('Export Document Materiel'!B6,"=", 'Export Document Materiel'!C6),IF('Export Document Materiel'!C6&lt;&gt;"",'Export Document Materiel'!C6,""))</f>
+        <v>window.export.document.mode.panel.title=Choix des données à exporter</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" t="str">
+        <f>IF('Export Document Materiel'!B7&lt;&gt;"",CONCATENATE('Export Document Materiel'!B7,"=", 'Export Document Materiel'!C7),IF('Export Document Materiel'!C7&lt;&gt;"",'Export Document Materiel'!C7,""))</f>
+        <v>window.export.document.mode.document.label=Un document</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" t="str">
+        <f>IF('Export Document Materiel'!B8&lt;&gt;"",CONCATENATE('Export Document Materiel'!B8,"=", 'Export Document Materiel'!C8),IF('Export Document Materiel'!C8&lt;&gt;"",'Export Document Materiel'!C8,""))</f>
+        <v>window.export.document.mode.all.documents.label=Tous les documents</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" t="str">
+        <f>IF('Export Document Materiel'!B9&lt;&gt;"",CONCATENATE('Export Document Materiel'!B9,"=", 'Export Document Materiel'!C9),IF('Export Document Materiel'!C9&lt;&gt;"",'Export Document Materiel'!C9,""))</f>
+        <v>window.export.document.mode.result.search.label=Le résultat de la recherche</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" t="str">
+        <f>IF('Export Document Materiel'!B10&lt;&gt;"",CONCATENATE('Export Document Materiel'!B10,"=", 'Export Document Materiel'!C10),IF('Export Document Materiel'!C10&lt;&gt;"",'Export Document Materiel'!C10,""))</f>
+        <v>window.export.document.choose.document.panel.title=Choix du document à exporter</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" t="str">
+        <f>IF('Export Document Materiel'!B11&lt;&gt;"",CONCATENATE('Export Document Materiel'!B11,"=", 'Export Document Materiel'!C11),IF('Export Document Materiel'!C11&lt;&gt;"",'Export Document Materiel'!C11,""))</f>
+        <v xml:space="preserve">window.export.document.choose.document.label=Document à exporter : </v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" t="str">
+        <f>IF('Export Document Materiel'!B12&lt;&gt;"",CONCATENATE('Export Document Materiel'!B12,"=", 'Export Document Materiel'!C12),IF('Export Document Materiel'!C12&lt;&gt;"",'Export Document Materiel'!C12,""))</f>
+        <v>window.export.document.choose.file.panel.title=Choix du nom du document</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" t="str">
+        <f>IF('Export Document Materiel'!B13&lt;&gt;"",CONCATENATE('Export Document Materiel'!B13,"=", 'Export Document Materiel'!C13),IF('Export Document Materiel'!C13&lt;&gt;"",'Export Document Materiel'!C13,""))</f>
+        <v xml:space="preserve">window.export.document.choose.file.label=Nom du document pour le resultat de la recherche : </v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" t="str">
+        <f>IF('Export Document Materiel'!B14&lt;&gt;"",CONCATENATE('Export Document Materiel'!B14,"=", 'Export Document Materiel'!C14),IF('Export Document Materiel'!C14&lt;&gt;"",'Export Document Materiel'!C14,""))</f>
+        <v>window.export.document.button.panel.title=Actions</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" t="str">
+        <f>IF('Export Document Materiel'!B15&lt;&gt;"",CONCATENATE('Export Document Materiel'!B15,"=", 'Export Document Materiel'!C15),IF('Export Document Materiel'!C15&lt;&gt;"",'Export Document Materiel'!C15,""))</f>
+        <v>window.export.document.button.export.label=Exporter et fermer</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="str">
+        <f>IF('Export Document Materiel'!B16&lt;&gt;"",CONCATENATE('Export Document Materiel'!B16,"=", 'Export Document Materiel'!C16),IF('Export Document Materiel'!C16&lt;&gt;"",'Export Document Materiel'!C16,""))</f>
+        <v>window.export.document.information.message.title=Export effectué</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" t="str">
+        <f>IF('Export Document Materiel'!B17&lt;&gt;"",CONCATENATE('Export Document Materiel'!B17,"=", 'Export Document Materiel'!C17),IF('Export Document Materiel'!C17&lt;&gt;"",'Export Document Materiel'!C17,""))</f>
+        <v>window.export.document.information.message=&lt;HTML&gt;&lt;P&gt;Export réalisé avec succés&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" t="str">
+        <f>IF('Export Document Materiel'!B18&lt;&gt;"",CONCATENATE('Export Document Materiel'!B18,"=", 'Export Document Materiel'!C18),IF('Export Document Materiel'!C18&lt;&gt;"",'Export Document Materiel'!C18,""))</f>
+        <v>window.export.document.button.close.label=Fermer</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" t="str">
+        <f>IF('Export Document Materiel'!B19&lt;&gt;"",CONCATENATE('Export Document Materiel'!B19,"=", 'Export Document Materiel'!C19),IF('Export Document Materiel'!C19&lt;&gt;"",'Export Document Materiel'!C19,""))</f>
+        <v>window.export.document.choose.directory.dialog.title=Choisissez le dossier de destination</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" t="str">
+        <f>IF('Export Document Materiel'!B20&lt;&gt;"",CONCATENATE('Export Document Materiel'!B20,"=", 'Export Document Materiel'!C20),IF('Export Document Materiel'!C20&lt;&gt;"",'Export Document Materiel'!C20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" t="str">
+        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE('Export Document Materiel'!B21,"=", 'Export Document Materiel'!C21),IF('Export Document Materiel'!C21&lt;&gt;"",'Export Document Materiel'!C21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" t="str">
+        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE('Export Document Materiel'!B22,"=", 'Export Document Materiel'!C22),IF('Export Document Materiel'!C22&lt;&gt;"",'Export Document Materiel'!C22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" t="str">
+        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE('Export Document Materiel'!B23,"=", 'Export Document Materiel'!C23),IF('Export Document Materiel'!C23&lt;&gt;"",'Export Document Materiel'!C23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" t="str">
+        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE('Export Document Materiel'!B24,"=", 'Export Document Materiel'!C24),IF('Export Document Materiel'!C24&lt;&gt;"",'Export Document Materiel'!C24,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" t="str">
+        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE('Export Document Materiel'!B25,"=", 'Export Document Materiel'!C25),IF('Export Document Materiel'!C25&lt;&gt;"",'Export Document Materiel'!C25,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" t="str">
+        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE('Export Document Materiel'!B26,"=", 'Export Document Materiel'!C26),IF('Export Document Materiel'!C26&lt;&gt;"",'Export Document Materiel'!C26,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" t="str">
+        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE('Export Document Materiel'!B27,"=", 'Export Document Materiel'!C27),IF('Export Document Materiel'!C27&lt;&gt;"",'Export Document Materiel'!C27,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" t="str">
+        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE('Export Document Materiel'!B28,"=", 'Export Document Materiel'!C28),IF('Export Document Materiel'!C28&lt;&gt;"",'Export Document Materiel'!C28,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" t="str">
+        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE('Export Document Materiel'!B29,"=", 'Export Document Materiel'!C29),IF('Export Document Materiel'!C29&lt;&gt;"",'Export Document Materiel'!C29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" t="str">
+        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE('Export Document Materiel'!B30,"=", 'Export Document Materiel'!C30),IF('Export Document Materiel'!C30&lt;&gt;"",'Export Document Materiel'!C30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" t="str">
+        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE('Export Document Materiel'!B31,"=", 'Export Document Materiel'!C31),IF('Export Document Materiel'!C31&lt;&gt;"",'Export Document Materiel'!C31,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" t="str">
+        <f>IF('Export Document Materiel'!B32&lt;&gt;"",CONCATENATE('Export Document Materiel'!B32,"=", 'Export Document Materiel'!C32),IF('Export Document Materiel'!C32&lt;&gt;"",'Export Document Materiel'!C32,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" t="str">
+        <f>IF('Export Document Materiel'!B33&lt;&gt;"",CONCATENATE('Export Document Materiel'!B33,"=", 'Export Document Materiel'!C33),IF('Export Document Materiel'!C33&lt;&gt;"",'Export Document Materiel'!C33,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" t="str">
+        <f>IF('Export Document Materiel'!B34&lt;&gt;"",CONCATENATE('Export Document Materiel'!B34,"=", 'Export Document Materiel'!C34),IF('Export Document Materiel'!C34&lt;&gt;"",'Export Document Materiel'!C34,""))</f>
         <v/>
       </c>
     </row>
@@ -27993,12 +28695,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
-  <dimension ref="A1:A401"/>
+  <dimension ref="A1:A434"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A73" sqref="A1:A401"/>
+    <sheetView showZeros="0" topLeftCell="A396" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A417" sqref="A1:A434"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29431,7 +30133,7 @@
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" t="str">
         <f>IF('Fenetre Gerer les textes'!B19&lt;&gt;"",CONCATENATE('Fenetre Gerer les textes'!B19,"=", 'Fenetre Gerer les textes'!D19),IF('Fenetre Gerer les textes'!D19&lt;&gt;"",'Fenetre Gerer les textes'!D19,""))</f>
-        <v/>
+        <v>window.manage.texts.export.document.text.button.label=Exportar Documento/Material</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
@@ -30301,7 +31003,7 @@
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" t="str">
         <f>IF('A propos'!B4&lt;&gt;"",CONCATENATE('A propos'!B4,"=", 'A propos'!D4),IF('A propos'!D4&lt;&gt;"",'A propos'!D4,""))</f>
-        <v>window.about.message.content=&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Acerca de la application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nombre de la application :&lt;/u&gt; Caerus&lt;BR /&gt;&lt;u&gt;Versión :&lt;/u&gt; 1.0.0&lt;br /&gt;&lt;u&gt;Editor :&lt;/u&gt; Jeremy, Leda&lt;br/&gt;&lt;u&gt;Sitio web :&lt;/u&gt; https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</v>
+        <v>window.about.message.content=&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Acerca de la application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nombre de la application :&lt;/u&gt; Caerus&lt;BR /&gt;&lt;u&gt;Versión :&lt;/u&gt; 1.1.0&lt;br /&gt;&lt;u&gt;Editor :&lt;/u&gt; Jeremy, Leda&lt;br/&gt;&lt;u&gt;Sitio web :&lt;/u&gt; https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
@@ -30409,6 +31111,204 @@
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" t="str">
         <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE('A propos'!B20,"=", 'A propos'!D20),IF('A propos'!D20&lt;&gt;"",'A propos'!D20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" t="str">
+        <f>IF('Export Document Materiel'!B2&lt;&gt;"",CONCATENATE('Export Document Materiel'!B2,"=", 'Export Document Materiel'!D2),IF('Export Document Materiel'!D2&lt;&gt;"",'Export Document Materiel'!D2,""))</f>
+        <v>#Mensaje para el cambio de configuración</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" t="str">
+        <f>IF('Export Document Materiel'!B3&lt;&gt;"",CONCATENATE('Export Document Materiel'!B3,"=", 'Export Document Materiel'!D3),IF('Export Document Materiel'!D3&lt;&gt;"",'Export Document Materiel'!D3,""))</f>
+        <v>window.export.document.title=Exportar documentos/materiales</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" t="str">
+        <f>IF('Export Document Materiel'!B4&lt;&gt;"",CONCATENATE('Export Document Materiel'!B4,"=", 'Export Document Materiel'!D4),IF('Export Document Materiel'!D4&lt;&gt;"",'Export Document Materiel'!D4,""))</f>
+        <v>window.export.document.choose.directory.panel.title=Elección de la carpeta de destino</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" t="str">
+        <f>IF('Export Document Materiel'!B5&lt;&gt;"",CONCATENATE('Export Document Materiel'!B5,"=", 'Export Document Materiel'!D5),IF('Export Document Materiel'!D5&lt;&gt;"",'Export Document Materiel'!D5,""))</f>
+        <v>window.export.document.choose.directory.label=Carpeta de destino</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" t="str">
+        <f>IF('Export Document Materiel'!B6&lt;&gt;"",CONCATENATE('Export Document Materiel'!B6,"=", 'Export Document Materiel'!D6),IF('Export Document Materiel'!D6&lt;&gt;"",'Export Document Materiel'!D6,""))</f>
+        <v>window.export.document.mode.panel.title=Elección de los datos a exportar</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" t="str">
+        <f>IF('Export Document Materiel'!B7&lt;&gt;"",CONCATENATE('Export Document Materiel'!B7,"=", 'Export Document Materiel'!D7),IF('Export Document Materiel'!D7&lt;&gt;"",'Export Document Materiel'!D7,""))</f>
+        <v>window.export.document.mode.document.label=Un documento</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" t="str">
+        <f>IF('Export Document Materiel'!B8&lt;&gt;"",CONCATENATE('Export Document Materiel'!B8,"=", 'Export Document Materiel'!D8),IF('Export Document Materiel'!D8&lt;&gt;"",'Export Document Materiel'!D8,""))</f>
+        <v>window.export.document.mode.all.documents.label=Todos documentos</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" t="str">
+        <f>IF('Export Document Materiel'!B9&lt;&gt;"",CONCATENATE('Export Document Materiel'!B9,"=", 'Export Document Materiel'!D9),IF('Export Document Materiel'!D9&lt;&gt;"",'Export Document Materiel'!D9,""))</f>
+        <v>window.export.document.mode.result.search.label=El resultado de la búsqueda</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" t="str">
+        <f>IF('Export Document Materiel'!B10&lt;&gt;"",CONCATENATE('Export Document Materiel'!B10,"=", 'Export Document Materiel'!D10),IF('Export Document Materiel'!D10&lt;&gt;"",'Export Document Materiel'!D10,""))</f>
+        <v>window.export.document.choose.document.panel.title=Elección del documento a exportar</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" t="str">
+        <f>IF('Export Document Materiel'!B11&lt;&gt;"",CONCATENATE('Export Document Materiel'!B11,"=", 'Export Document Materiel'!D11),IF('Export Document Materiel'!D11&lt;&gt;"",'Export Document Materiel'!D11,""))</f>
+        <v>window.export.document.choose.document.label=Documento para exportar :</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" t="str">
+        <f>IF('Export Document Materiel'!B12&lt;&gt;"",CONCATENATE('Export Document Materiel'!B12,"=", 'Export Document Materiel'!D12),IF('Export Document Materiel'!D12&lt;&gt;"",'Export Document Materiel'!D12,""))</f>
+        <v>window.export.document.choose.file.panel.title=Elección del nombre del documento</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" t="str">
+        <f>IF('Export Document Materiel'!B13&lt;&gt;"",CONCATENATE('Export Document Materiel'!B13,"=", 'Export Document Materiel'!D13),IF('Export Document Materiel'!D13&lt;&gt;"",'Export Document Materiel'!D13,""))</f>
+        <v xml:space="preserve">window.export.document.choose.file.label=Nombre del documento para el resultado de la búsqueda : </v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" t="str">
+        <f>IF('Export Document Materiel'!B14&lt;&gt;"",CONCATENATE('Export Document Materiel'!B14,"=", 'Export Document Materiel'!D14),IF('Export Document Materiel'!D14&lt;&gt;"",'Export Document Materiel'!D14,""))</f>
+        <v>window.export.document.button.panel.title=Acciones</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" t="str">
+        <f>IF('Export Document Materiel'!B15&lt;&gt;"",CONCATENATE('Export Document Materiel'!B15,"=", 'Export Document Materiel'!D15),IF('Export Document Materiel'!D15&lt;&gt;"",'Export Document Materiel'!D15,""))</f>
+        <v>window.export.document.button.export.label=Exportar y cerrar</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" t="str">
+        <f>IF('Export Document Materiel'!B16&lt;&gt;"",CONCATENATE('Export Document Materiel'!B16,"=", 'Export Document Materiel'!D16),IF('Export Document Materiel'!D16&lt;&gt;"",'Export Document Materiel'!D16,""))</f>
+        <v>window.export.document.information.message.title=Exportación completada</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" t="str">
+        <f>IF('Export Document Materiel'!B17&lt;&gt;"",CONCATENATE('Export Document Materiel'!B17,"=", 'Export Document Materiel'!D17),IF('Export Document Materiel'!D17&lt;&gt;"",'Export Document Materiel'!D17,""))</f>
+        <v>window.export.document.information.message=&lt;HTML&gt;&lt;P&gt;Exportación realizada con éxito&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="str">
+        <f>IF('Export Document Materiel'!B18&lt;&gt;"",CONCATENATE('Export Document Materiel'!B18,"=", 'Export Document Materiel'!D18),IF('Export Document Materiel'!D18&lt;&gt;"",'Export Document Materiel'!D18,""))</f>
+        <v>window.export.document.button.close.label=Cerrar</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" t="str">
+        <f>IF('Export Document Materiel'!B19&lt;&gt;"",CONCATENATE('Export Document Materiel'!B19,"=", 'Export Document Materiel'!D19),IF('Export Document Materiel'!D19&lt;&gt;"",'Export Document Materiel'!D19,""))</f>
+        <v>window.export.document.choose.directory.dialog.title=Seleccione la carpeta de destino</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" t="str">
+        <f>IF('Export Document Materiel'!B20&lt;&gt;"",CONCATENATE('Export Document Materiel'!B20,"=", 'Export Document Materiel'!D20),IF('Export Document Materiel'!D20&lt;&gt;"",'Export Document Materiel'!D20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" t="str">
+        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE('Export Document Materiel'!B21,"=", 'Export Document Materiel'!D21),IF('Export Document Materiel'!D21&lt;&gt;"",'Export Document Materiel'!D21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" t="str">
+        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE('Export Document Materiel'!B22,"=", 'Export Document Materiel'!D22),IF('Export Document Materiel'!D22&lt;&gt;"",'Export Document Materiel'!D22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" t="str">
+        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE('Export Document Materiel'!B23,"=", 'Export Document Materiel'!D23),IF('Export Document Materiel'!D23&lt;&gt;"",'Export Document Materiel'!D23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" t="str">
+        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE('Export Document Materiel'!B24,"=", 'Export Document Materiel'!D24),IF('Export Document Materiel'!D24&lt;&gt;"",'Export Document Materiel'!D24,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" t="str">
+        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE('Export Document Materiel'!B25,"=", 'Export Document Materiel'!D25),IF('Export Document Materiel'!D25&lt;&gt;"",'Export Document Materiel'!D25,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" t="str">
+        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE('Export Document Materiel'!B26,"=", 'Export Document Materiel'!D26),IF('Export Document Materiel'!D26&lt;&gt;"",'Export Document Materiel'!D26,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" t="str">
+        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE('Export Document Materiel'!B27,"=", 'Export Document Materiel'!D27),IF('Export Document Materiel'!D27&lt;&gt;"",'Export Document Materiel'!D27,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" t="str">
+        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE('Export Document Materiel'!B28,"=", 'Export Document Materiel'!D28),IF('Export Document Materiel'!D28&lt;&gt;"",'Export Document Materiel'!D28,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" t="str">
+        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE('Export Document Materiel'!B29,"=", 'Export Document Materiel'!D29),IF('Export Document Materiel'!D29&lt;&gt;"",'Export Document Materiel'!D29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" t="str">
+        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE('Export Document Materiel'!B30,"=", 'Export Document Materiel'!D30),IF('Export Document Materiel'!D30&lt;&gt;"",'Export Document Materiel'!D30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" t="str">
+        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE('Export Document Materiel'!B31,"=", 'Export Document Materiel'!D31),IF('Export Document Materiel'!D31&lt;&gt;"",'Export Document Materiel'!D31,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" t="str">
+        <f>IF('Export Document Materiel'!B32&lt;&gt;"",CONCATENATE('Export Document Materiel'!B32,"=", 'Export Document Materiel'!D32),IF('Export Document Materiel'!D32&lt;&gt;"",'Export Document Materiel'!D32,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" t="str">
+        <f>IF('Export Document Materiel'!B33&lt;&gt;"",CONCATENATE('Export Document Materiel'!B33,"=", 'Export Document Materiel'!D33),IF('Export Document Materiel'!D33&lt;&gt;"",'Export Document Materiel'!D33,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" t="str">
+        <f>IF('Export Document Materiel'!B34&lt;&gt;"",CONCATENATE('Export Document Materiel'!B34,"=", 'Export Document Materiel'!D34),IF('Export Document Materiel'!D34&lt;&gt;"",'Export Document Materiel'!D34,""))</f>
         <v/>
       </c>
     </row>
@@ -30417,12 +31317,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
-  <dimension ref="A1:A396"/>
+  <dimension ref="A1:A432"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:A85"/>
+    <sheetView topLeftCell="A398" workbookViewId="0">
+      <selection activeCell="A420" sqref="A420"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31849,7 +32749,7 @@
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" t="str">
         <f>IF('Fenetre Gerer les textes'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Fenetre Gerer les textes'!B19),".","_"),"=""", 'Fenetre Gerer les textes'!B19,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_MANAGE_TEXTS_EXPORT_DOCUMENT_TEXT_BUTTON_LABEL="window.manage.texts.export.document.text.button.label";</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
@@ -32803,6 +33703,222 @@
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" t="str">
         <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B18),".","_"),"=""", 'A propos'!B18,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" t="str">
+        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B19),".","_"),"=""", 'A propos'!B19,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" t="str">
+        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B20),".","_"),"=""", 'A propos'!B20,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" t="str">
+        <f>IF('A propos'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B21),".","_"),"=""", 'A propos'!B21,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" t="str">
+        <f>IF('A propos'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B22),".","_"),"=""", 'A propos'!B22,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" t="str">
+        <f>IF('A propos'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B23),".","_"),"=""", 'A propos'!B23,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" t="str">
+        <f>IF('A propos'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B24),".","_"),"=""", 'A propos'!B24,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" t="str">
+        <f>IF('Export Document Materiel'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B2),".","_"),"=""", 'Export Document Materiel'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" t="str">
+        <f>IF('Export Document Materiel'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B3),".","_"),"=""", 'Export Document Materiel'!B3,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_TITLE="window.export.document.title";</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" t="str">
+        <f>IF('Export Document Materiel'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B4),".","_"),"=""", 'Export Document Materiel'!B4,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DIRECTORY_PANEL_TITLE="window.export.document.choose.directory.panel.title";</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" t="str">
+        <f>IF('Export Document Materiel'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B5),".","_"),"=""", 'Export Document Materiel'!B5,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DIRECTORY_LABEL="window.export.document.choose.directory.label";</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" t="str">
+        <f>IF('Export Document Materiel'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B6),".","_"),"=""", 'Export Document Materiel'!B6,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_MODE_PANEL_TITLE="window.export.document.mode.panel.title";</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" t="str">
+        <f>IF('Export Document Materiel'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B7),".","_"),"=""", 'Export Document Materiel'!B7,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_MODE_DOCUMENT_LABEL="window.export.document.mode.document.label";</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" t="str">
+        <f>IF('Export Document Materiel'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B8),".","_"),"=""", 'Export Document Materiel'!B8,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_MODE_ALL_DOCUMENTS_LABEL="window.export.document.mode.all.documents.label";</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" t="str">
+        <f>IF('Export Document Materiel'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B9),".","_"),"=""", 'Export Document Materiel'!B9,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_MODE_RESULT_SEARCH_LABEL="window.export.document.mode.result.search.label";</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" t="str">
+        <f>IF('Export Document Materiel'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B10),".","_"),"=""", 'Export Document Materiel'!B10,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DOCUMENT_PANEL_TITLE="window.export.document.choose.document.panel.title";</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" t="str">
+        <f>IF('Export Document Materiel'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B11),".","_"),"=""", 'Export Document Materiel'!B11,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DOCUMENT_LABEL="window.export.document.choose.document.label";</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" t="str">
+        <f>IF('Export Document Materiel'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B12),".","_"),"=""", 'Export Document Materiel'!B12,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_FILE_PANEL_TITLE="window.export.document.choose.file.panel.title";</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" t="str">
+        <f>IF('Export Document Materiel'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B13),".","_"),"=""", 'Export Document Materiel'!B13,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_FILE_LABEL="window.export.document.choose.file.label";</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" t="str">
+        <f>IF('Export Document Materiel'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B14),".","_"),"=""", 'Export Document Materiel'!B14,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_BUTTON_PANEL_TITLE="window.export.document.button.panel.title";</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" t="str">
+        <f>IF('Export Document Materiel'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B15),".","_"),"=""", 'Export Document Materiel'!B15,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_BUTTON_EXPORT_LABEL="window.export.document.button.export.label";</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" t="str">
+        <f>IF('Export Document Materiel'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B16),".","_"),"=""", 'Export Document Materiel'!B16,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_INFORMATION_MESSAGE_TITLE="window.export.document.information.message.title";</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="str">
+        <f>IF('Export Document Materiel'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B17),".","_"),"=""", 'Export Document Materiel'!B17,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_INFORMATION_MESSAGE="window.export.document.information.message";</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" t="str">
+        <f>IF('Export Document Materiel'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B18),".","_"),"=""", 'Export Document Materiel'!B18,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_BUTTON_CLOSE_LABEL="window.export.document.button.close.label";</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" t="str">
+        <f>IF('Export Document Materiel'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B19),".","_"),"=""", 'Export Document Materiel'!B19,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DIRECTORY_DIALOG_TITLE="window.export.document.choose.directory.dialog.title";</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" t="str">
+        <f>IF('Export Document Materiel'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B20),".","_"),"=""", 'Export Document Materiel'!B20,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" t="str">
+        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B21),".","_"),"=""", 'Export Document Materiel'!B21,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" t="str">
+        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B22),".","_"),"=""", 'Export Document Materiel'!B22,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" t="str">
+        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B23),".","_"),"=""", 'Export Document Materiel'!B23,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" t="str">
+        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B24),".","_"),"=""", 'Export Document Materiel'!B24,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" t="str">
+        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B25),".","_"),"=""", 'Export Document Materiel'!B25,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" t="str">
+        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B26),".","_"),"=""", 'Export Document Materiel'!B26,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" t="str">
+        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B27),".","_"),"=""", 'Export Document Materiel'!B27,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" t="str">
+        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B28),".","_"),"=""", 'Export Document Materiel'!B28,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" t="str">
+        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B29),".","_"),"=""", 'Export Document Materiel'!B29,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" t="str">
+        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B30),".","_"),"=""", 'Export Document Materiel'!B30,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" t="str">
+        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B31),".","_"),"=""", 'Export Document Materiel'!B31,""";"),"")</f>
         <v/>
       </c>
     </row>
@@ -32857,10 +33973,10 @@
         <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -32888,7 +34004,7 @@
         <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -32899,10 +34015,10 @@
         <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D6" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -32941,10 +34057,10 @@
         <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D9" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -32969,10 +34085,10 @@
         <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -32980,13 +34096,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C12" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D12" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -32994,13 +34110,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C13" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D13" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -33008,13 +34124,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C14" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D14" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -33022,7 +34138,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quelle est la balise correspondante à cette ligne ?&lt;BR/&gt;",
@@ -33042,7 +34158,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C16" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quel est le contenu de la balise ?&lt;BR/&gt;",
@@ -33072,7 +34188,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C17" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Tout est bon ?&lt;BR/&gt;",
@@ -33100,13 +34216,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C18" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D18" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -33114,13 +34230,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C19" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D19" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -33128,13 +34244,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C20" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D20" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -33142,13 +34258,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C21" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D21" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -33156,13 +34272,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C22" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D22" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -33170,13 +34286,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="C23" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D23" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -33184,13 +34300,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C24" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D24" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -33198,13 +34314,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C25" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D25" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -33212,13 +34328,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="120" x14ac:dyDescent="0.25">
@@ -33226,7 +34342,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C27" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Bienvenue sur l'assistant de correction des lignes.&lt;BR/&gt;",
@@ -33300,10 +34416,10 @@
         <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D3" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -33328,10 +34444,10 @@
         <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -33410,10 +34526,10 @@
         <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D12" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -33432,10 +34548,10 @@
         <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D15" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -33446,10 +34562,10 @@
         <v>126</v>
       </c>
       <c r="C16" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D16" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -33463,7 +34579,7 @@
         <v>136</v>
       </c>
       <c r="D17" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -33485,7 +34601,7 @@
         <v>128</v>
       </c>
       <c r="D20" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -33585,7 +34701,7 @@
         <v>373</v>
       </c>
       <c r="D6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33636,10 +34752,10 @@
         <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D11" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33650,10 +34766,10 @@
         <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D12" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33898,7 +35014,7 @@
         <v>176</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>177</v>
@@ -33926,10 +35042,10 @@
         <v>180</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -33968,10 +35084,10 @@
         <v>185</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -33982,10 +35098,10 @@
         <v>186</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -33996,10 +35112,10 @@
         <v>187</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -34024,10 +35140,10 @@
         <v>190</v>
       </c>
       <c r="C12" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>479</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -34038,10 +35154,10 @@
         <v>191</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -34049,7 +35165,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>88</v>
@@ -34063,13 +35179,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>564</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>566</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -34077,13 +35193,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -34091,13 +35207,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -34105,13 +35221,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -34119,13 +35235,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>572</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>573</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>574</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -34133,13 +35249,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -34147,13 +35263,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C21" s="13" t="s">
+        <v>586</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>588</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>590</v>
       </c>
     </row>
   </sheetData>
@@ -34213,10 +35329,10 @@
         <v>197</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
   </sheetData>
@@ -34303,7 +35419,7 @@
         <v>200</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D5" t="s">
         <v>212</v>
@@ -34359,10 +35475,10 @@
         <v>206</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D9" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -34401,10 +35517,10 @@
         <v>369</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -34554,10 +35670,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F59160BD-885A-4DEA-9FEE-62F72A09FE0A}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34597,10 +35713,10 @@
         <v>223</v>
       </c>
       <c r="C3" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D3" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -34611,10 +35727,10 @@
         <v>224</v>
       </c>
       <c r="C4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -34625,10 +35741,10 @@
         <v>225</v>
       </c>
       <c r="C5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -34639,10 +35755,10 @@
         <v>226</v>
       </c>
       <c r="C6" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -34695,10 +35811,10 @@
         <v>231</v>
       </c>
       <c r="C10" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D10" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -34709,10 +35825,10 @@
         <v>232</v>
       </c>
       <c r="C11" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D11" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -34723,10 +35839,10 @@
         <v>233</v>
       </c>
       <c r="C12" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D12" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -34737,10 +35853,10 @@
         <v>234</v>
       </c>
       <c r="C13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D13" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -34751,10 +35867,10 @@
         <v>235</v>
       </c>
       <c r="C14" t="s">
+        <v>450</v>
+      </c>
+      <c r="D14" t="s">
         <v>452</v>
-      </c>
-      <c r="D14" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -34765,10 +35881,10 @@
         <v>236</v>
       </c>
       <c r="C15" t="s">
+        <v>451</v>
+      </c>
+      <c r="D15" t="s">
         <v>453</v>
-      </c>
-      <c r="D15" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -34779,10 +35895,10 @@
         <v>238</v>
       </c>
       <c r="C16" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D16" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -34813,6 +35929,20 @@
       <c r="D18" s="1" t="str">
         <f>CONCATENATE("&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Filtrar el contenido:&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Esta función le permite crear filtros para realizar búsquedas en la biblioteca en función del contenido de los materiales,","&lt;br /&gt;No olvide cerrar la ventana del filtro para poder continuar haciendo otras operaciones","&lt;br /&gt;&lt;b&gt;&lt;u&gt;Consultar/Editar el documento :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Esta función le permite hacer una gestión manual del contenido de los materiales de su biblioteca. Al editar un documento, puede añadir material al documento.  &lt;br /&gt;","Recuerde guardar los cambios para que el nuevo material textual se escriba físicamente en el documento .txt, &lt;br /&gt;de lo contrario se perderá después de cerrar la aplicación","&lt;br /&gt;&lt;b&gt;&lt;u&gt;Consultar/Editar el material :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Esta opción le permite modificar el texto del material y añadirle una estructura adicional gracias a las informaciones específicas en CSV&lt;br /&gt;","&lt;b&gt;&lt;u&gt;Suprimir un material:&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Después de seleccionar un texto, si desea eliminarlo , el texto podrá ser definitivamente eliminado con este botón (¡ATENCIÓN! no se podrá deshacer la acción)&lt;/p&gt;&lt;/html&gt;")</f>
         <v>&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Filtrar el contenido:&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Esta función le permite crear filtros para realizar búsquedas en la biblioteca en función del contenido de los materiales,&lt;br /&gt;No olvide cerrar la ventana del filtro para poder continuar haciendo otras operaciones&lt;br /&gt;&lt;b&gt;&lt;u&gt;Consultar/Editar el documento :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Esta función le permite hacer una gestión manual del contenido de los materiales de su biblioteca. Al editar un documento, puede añadir material al documento.  &lt;br /&gt;Recuerde guardar los cambios para que el nuevo material textual se escriba físicamente en el documento .txt, &lt;br /&gt;de lo contrario se perderá después de cerrar la aplicación&lt;br /&gt;&lt;b&gt;&lt;u&gt;Consultar/Editar el material :&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Esta opción le permite modificar el texto del material y añadirle una estructura adicional gracias a las informaciones específicas en CSV&lt;br /&gt;&lt;b&gt;&lt;u&gt;Suprimir un material:&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;Después de seleccionar un texto, si desea eliminarlo , el texto podrá ser definitivamente eliminado con este botón (¡ATENCIÓN! no se podrá deshacer la acción)&lt;/p&gt;&lt;/html&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>629</v>
+      </c>
+      <c r="C19" t="s">
+        <v>630</v>
+      </c>
+      <c r="D19" t="s">
+        <v>631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modification du message d'information
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\git\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB63D5D-1264-4572-B6E5-441D4BEC543A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FC27AD-1DC4-4926-8049-3A73DBE9B026}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="12" activeTab="15" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="12" activeTab="18" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="685">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -2095,6 +2095,15 @@
   </si>
   <si>
     <t>&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Acerca de la application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nombre de la application :&lt;/u&gt; Caerus&lt;BR /&gt;&lt;u&gt;Versión :&lt;/u&gt; 1.1.0&lt;br /&gt;&lt;u&gt;Editor :&lt;/u&gt; Jeremy, Leda&lt;br/&gt;&lt;u&gt;Sitio web :&lt;/u&gt; https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>window.export.document.information.search.message</t>
+  </si>
+  <si>
+    <t>&lt;HTML&gt;&lt;P&gt;Export réalisé avec succés&lt;BR/&gt;Pour information, le document ne contient aucune données d'en-tête&lt;/P&gt;&lt;/HTML&gt;</t>
+  </si>
+  <si>
+    <t>&lt;HTML&gt;&lt;P&gt;Exportación realizada con éxito&lt;BR/&gt;A título informativo, el documento no contiene datos de cabecera&lt;/P&gt;&lt;/HTML&gt;</t>
   </si>
 </sst>
 </file>
@@ -23444,8 +23453,8 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{ACF16CE4-3CFE-4EE6-9A66-F2E289DD58BC}" name="Tableau161015" displayName="Tableau161015" ref="A1:D19" totalsRowShown="0">
-  <autoFilter ref="A1:D19" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{ACF16CE4-3CFE-4EE6-9A66-F2E289DD58BC}" name="Tableau161015" displayName="Tableau161015" ref="A1:D21" totalsRowShown="0">
+  <autoFilter ref="A1:D21" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7BE777E6-80D5-4607-B506-C54D0BCAA26D}" name="Numero"/>
     <tableColumn id="2" xr3:uid="{37941F86-4BA1-4EBC-90AD-63A762519C13}" name="Code"/>
@@ -25777,8 +25786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA2BF44D-1BCC-419E-8C75-D4A062A89580}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26045,6 +26054,20 @@
       </c>
       <c r="D19" t="s">
         <v>675</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>682</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -26066,7 +26089,7 @@
   <dimension ref="A1:A436"/>
   <sheetViews>
     <sheetView showZeros="0" topLeftCell="A397" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A418" sqref="A1:A436"/>
+      <selection activeCell="A421" sqref="A1:A436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28603,7 +28626,7 @@
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A422" t="str">
         <f>IF('Export Document Materiel'!B20&lt;&gt;"",CONCATENATE('Export Document Materiel'!B20,"=", 'Export Document Materiel'!C20),IF('Export Document Materiel'!C20&lt;&gt;"",'Export Document Materiel'!C20,""))</f>
-        <v/>
+        <v>window.export.document.information.search.message=&lt;HTML&gt;&lt;P&gt;Export réalisé avec succés&lt;BR/&gt;Pour information, le document ne contient aucune données d'en-tête&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
@@ -28700,7 +28723,7 @@
   <dimension ref="A1:A434"/>
   <sheetViews>
     <sheetView showZeros="0" topLeftCell="A396" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A417" sqref="A1:A434"/>
+      <selection activeCell="A416" sqref="A1:A434"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31225,7 +31248,7 @@
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" t="str">
         <f>IF('Export Document Materiel'!B20&lt;&gt;"",CONCATENATE('Export Document Materiel'!B20,"=", 'Export Document Materiel'!D20),IF('Export Document Materiel'!D20&lt;&gt;"",'Export Document Materiel'!D20,""))</f>
-        <v/>
+        <v>window.export.document.information.search.message=&lt;HTML&gt;&lt;P&gt;Exportación realizada con éxito&lt;BR/&gt;A título informativo, el documento no contiene datos de cabecera&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
@@ -31321,8 +31344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
   <dimension ref="A1:A432"/>
   <sheetViews>
-    <sheetView topLeftCell="A398" workbookViewId="0">
-      <selection activeCell="A420" sqref="A420"/>
+    <sheetView tabSelected="1" topLeftCell="A398" workbookViewId="0">
+      <selection activeCell="A421" sqref="A421"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33853,7 +33876,7 @@
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A421" t="str">
         <f>IF('Export Document Materiel'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B20),".","_"),"=""", 'Export Document Materiel'!B20,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_EXPORT_DOCUMENT_INFORMATION_SEARCH_MESSAGE="window.export.document.information.search.message";</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix for 1.1.1 version
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\git\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FC27AD-1DC4-4926-8049-3A73DBE9B026}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B5613B-8DC7-47EE-BC7B-2F110349C6EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="12" activeTab="18" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="12" activeTab="14" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -2091,12 +2091,6 @@
     <t>Exportar y cerrar</t>
   </si>
   <si>
-    <t>&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;A propos de l'application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nom de l'application : &lt;/u&gt; Caerus&lt;br /&gt;&lt;u&gt;Version : &lt;/u&gt; 1.1.0&lt;br /&gt;&lt;u&gt;Editeur : &lt;/u&gt; Jeremy, Leda&lt;br /&gt;&lt;u&gt;Site web : &lt;/u&gt;https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</t>
-  </si>
-  <si>
-    <t>&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Acerca de la application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nombre de la application :&lt;/u&gt; Caerus&lt;BR /&gt;&lt;u&gt;Versión :&lt;/u&gt; 1.1.0&lt;br /&gt;&lt;u&gt;Editor :&lt;/u&gt; Jeremy, Leda&lt;br/&gt;&lt;u&gt;Sitio web :&lt;/u&gt; https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</t>
-  </si>
-  <si>
     <t>window.export.document.information.search.message</t>
   </si>
   <si>
@@ -2104,6 +2098,12 @@
   </si>
   <si>
     <t>&lt;HTML&gt;&lt;P&gt;Exportación realizada con éxito&lt;BR/&gt;A título informativo, el documento no contiene datos de cabecera&lt;/P&gt;&lt;/HTML&gt;</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;A propos de l'application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nom de l'application : &lt;/u&gt; Caerus&lt;br /&gt;&lt;u&gt;Version : &lt;/u&gt; 1.1.1&lt;br /&gt;&lt;u&gt;Editeur : &lt;/u&gt; Jeremy, Leda&lt;br /&gt;&lt;u&gt;Site web : &lt;/u&gt;https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Acerca de la application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nombre de la application :&lt;/u&gt; Caerus&lt;BR /&gt;&lt;u&gt;Versión :&lt;/u&gt; 1.1.1&lt;br /&gt;&lt;u&gt;Editor :&lt;/u&gt; Jeremy, Leda&lt;br/&gt;&lt;u&gt;Sitio web :&lt;/u&gt; https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</t>
   </si>
 </sst>
 </file>
@@ -25697,8 +25697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357A141E-D5BD-46DF-8EEC-B92516C123B1}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25751,10 +25751,10 @@
         <v>426</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -26061,13 +26061,13 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
+        <v>680</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>682</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -28392,7 +28392,7 @@
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" t="str">
         <f>IF('A propos'!B4&lt;&gt;"",CONCATENATE('A propos'!B4,"=", 'A propos'!C4),IF('A propos'!C4&lt;&gt;"",'A propos'!C4,""))</f>
-        <v>window.about.message.content=&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;A propos de l'application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nom de l'application : &lt;/u&gt; Caerus&lt;br /&gt;&lt;u&gt;Version : &lt;/u&gt; 1.1.0&lt;br /&gt;&lt;u&gt;Editeur : &lt;/u&gt; Jeremy, Leda&lt;br /&gt;&lt;u&gt;Site web : &lt;/u&gt;https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</v>
+        <v>window.about.message.content=&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;A propos de l'application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nom de l'application : &lt;/u&gt; Caerus&lt;br /&gt;&lt;u&gt;Version : &lt;/u&gt; 1.1.1&lt;br /&gt;&lt;u&gt;Editeur : &lt;/u&gt; Jeremy, Leda&lt;br /&gt;&lt;u&gt;Site web : &lt;/u&gt;https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
@@ -31026,7 +31026,7 @@
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" t="str">
         <f>IF('A propos'!B4&lt;&gt;"",CONCATENATE('A propos'!B4,"=", 'A propos'!D4),IF('A propos'!D4&lt;&gt;"",'A propos'!D4,""))</f>
-        <v>window.about.message.content=&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Acerca de la application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nombre de la application :&lt;/u&gt; Caerus&lt;BR /&gt;&lt;u&gt;Versión :&lt;/u&gt; 1.1.0&lt;br /&gt;&lt;u&gt;Editor :&lt;/u&gt; Jeremy, Leda&lt;br/&gt;&lt;u&gt;Sitio web :&lt;/u&gt; https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</v>
+        <v>window.about.message.content=&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Acerca de la application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nombre de la application :&lt;/u&gt; Caerus&lt;BR /&gt;&lt;u&gt;Versión :&lt;/u&gt; 1.1.1&lt;br /&gt;&lt;u&gt;Editor :&lt;/u&gt; Jeremy, Leda&lt;br/&gt;&lt;u&gt;Sitio web :&lt;/u&gt; https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
@@ -31344,7 +31344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
   <dimension ref="A1:A432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A398" workbookViewId="0">
+    <sheetView topLeftCell="A398" workbookViewId="0">
       <selection activeCell="A421" sqref="A421"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajout d'une barre de progression pour consultation et export
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\git\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AB4C5E-242A-40EB-B3E9-A5B4185326B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB81D6F-A13A-468D-9818-1ACDA13CFAA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="13" activeTab="19" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="756">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -2280,6 +2280,39 @@
   </si>
   <si>
     <t>Consultar / Editar materiales</t>
+  </si>
+  <si>
+    <t>#Barre de progression</t>
+  </si>
+  <si>
+    <t>Veuillez patienter</t>
+  </si>
+  <si>
+    <t>Chargement des textes….</t>
+  </si>
+  <si>
+    <t>Export Excel….</t>
+  </si>
+  <si>
+    <t>window.progress.bar.panel.title</t>
+  </si>
+  <si>
+    <t>window.progress.bar.load.text.label</t>
+  </si>
+  <si>
+    <t>window.progress.bar.export.excel.label</t>
+  </si>
+  <si>
+    <t>Espere por favor</t>
+  </si>
+  <si>
+    <t>#Barra de progreso</t>
+  </si>
+  <si>
+    <t>Cargando textos….</t>
+  </si>
+  <si>
+    <t>Exportar Excel….</t>
   </si>
 </sst>
 </file>
@@ -23590,8 +23623,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{028E31B7-3FC3-4143-B5FF-43FD17AAB26D}" name="Tableau16" displayName="Tableau16" ref="A1:D33" totalsRowShown="0">
-  <autoFilter ref="A1:D33" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{028E31B7-3FC3-4143-B5FF-43FD17AAB26D}" name="Tableau16" displayName="Tableau16" ref="A1:D40" totalsRowShown="0">
+  <autoFilter ref="A1:D40" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{EE0F9B50-F787-4253-A164-BB17836F12B4}" name="Numero"/>
     <tableColumn id="2" xr3:uid="{58CBB508-E960-4269-90E7-903193963B86}" name="Code"/>
@@ -25458,10 +25491,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B861A8A-1131-4099-83D4-ECA745EBF0ED}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25797,6 +25830,56 @@
       </c>
       <c r="D32" t="s">
         <v>737</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>745</v>
+      </c>
+      <c r="D34" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>19</v>
+      </c>
+      <c r="B35" t="s">
+        <v>749</v>
+      </c>
+      <c r="C35" t="s">
+        <v>746</v>
+      </c>
+      <c r="D35" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>20</v>
+      </c>
+      <c r="B36" t="s">
+        <v>750</v>
+      </c>
+      <c r="C36" t="s">
+        <v>747</v>
+      </c>
+      <c r="D36" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>21</v>
+      </c>
+      <c r="B37" t="s">
+        <v>751</v>
+      </c>
+      <c r="C37" t="s">
+        <v>748</v>
+      </c>
+      <c r="D37" t="s">
+        <v>755</v>
       </c>
     </row>
   </sheetData>
@@ -26759,10 +26842,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904B2FA-CBC2-495A-A197-D0CDD47EB1AE}">
-  <dimension ref="A1:A493"/>
+  <dimension ref="A1:A499"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A334" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A360" sqref="A1:A493"/>
+    <sheetView showZeros="0" topLeftCell="A358" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A378" sqref="A1:A499"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28909,821 +28992,857 @@
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" t="str">
         <f>IF(Autres!B34&lt;&gt;"",CONCATENATE(Autres!B34,"=", Autres!C34),IF(Autres!C34&lt;&gt;"",Autres!C34,""))</f>
-        <v/>
+        <v>#Barre de progression</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" t="str">
         <f>IF(Autres!B35&lt;&gt;"",CONCATENATE(Autres!B35,"=", Autres!C35),IF(Autres!C35&lt;&gt;"",Autres!C35,""))</f>
-        <v/>
+        <v>window.progress.bar.panel.title=Veuillez patienter</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" t="str">
+        <f>IF(Autres!B36&lt;&gt;"",CONCATENATE(Autres!B36,"=", Autres!C36),IF(Autres!C36&lt;&gt;"",Autres!C36,""))</f>
+        <v>window.progress.bar.load.text.label=Chargement des textes….</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" t="str">
+        <f>IF(Autres!B37&lt;&gt;"",CONCATENATE(Autres!B37,"=", Autres!C37),IF(Autres!C37&lt;&gt;"",Autres!C37,""))</f>
+        <v>window.progress.bar.export.excel.label=Export Excel….</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" t="str">
+        <f>IF(Autres!B38&lt;&gt;"",CONCATENATE(Autres!B38,"=", Autres!C38),IF(Autres!C38&lt;&gt;"",Autres!C38,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" t="str">
+        <f>IF(Autres!B39&lt;&gt;"",CONCATENATE(Autres!B39,"=", Autres!C39),IF(Autres!C39&lt;&gt;"",Autres!C39,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" t="str">
+        <f>IF(Autres!B40&lt;&gt;"",CONCATENATE(Autres!B40,"=", Autres!C40),IF(Autres!C40&lt;&gt;"",Autres!C40,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" t="str">
+        <f>IF(Autres!B41&lt;&gt;"",CONCATENATE(Autres!B41,"=", Autres!C41),IF(Autres!C41&lt;&gt;"",Autres!C41,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" t="str">
         <f>IF('Changer Configuration'!B2&lt;&gt;"",CONCATENATE('Changer Configuration'!B2,"=", 'Changer Configuration'!C2),IF('Changer Configuration'!C2&lt;&gt;"",'Changer Configuration'!C2,""))</f>
         <v>#Message pour le changement de la configuration</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A360" t="str">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" t="str">
         <f>IF('Changer Configuration'!B3&lt;&gt;"",CONCATENATE('Changer Configuration'!B3,"=", 'Changer Configuration'!C3),IF('Changer Configuration'!C3&lt;&gt;"",'Changer Configuration'!C3,""))</f>
         <v>window.change.configuration.title=Configuration courante</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" t="str">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" t="str">
         <f>IF('Changer Configuration'!B4&lt;&gt;"",CONCATENATE('Changer Configuration'!B4,"=", 'Changer Configuration'!C4),IF('Changer Configuration'!C4&lt;&gt;"",'Changer Configuration'!C4,""))</f>
         <v>window.change.configuration.list.label=Configuration à utiliser :</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" t="str">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" t="str">
         <f>IF('Changer Configuration'!B5&lt;&gt;"",CONCATENATE('Changer Configuration'!B5,"=", 'Changer Configuration'!C5),IF('Changer Configuration'!C5&lt;&gt;"",'Changer Configuration'!C5,""))</f>
         <v>window.change.configuration.panel.title=Changement de la configuration</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" t="str">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" t="str">
         <f>IF('Changer Configuration'!B6&lt;&gt;"",CONCATENATE('Changer Configuration'!B6,"=", 'Changer Configuration'!C6),IF('Changer Configuration'!C6&lt;&gt;"",'Changer Configuration'!C6,""))</f>
         <v>window.change.configuration.message.panel.title=Message d'information</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" t="str">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" t="str">
         <f>IF('Changer Configuration'!B7&lt;&gt;"",CONCATENATE('Changer Configuration'!B7,"=", 'Changer Configuration'!C7),IF('Changer Configuration'!C7&lt;&gt;"",'Changer Configuration'!C7,""))</f>
         <v>window.change.configuration.message.content=&lt;html&gt;&lt;p&gt;La configuration de l’application Caerus est basée sur un fichier qui vous permet de configurer complètement l’interface en fonction des matériels textuels créés.&lt;br/&gt;Vous pouvez modifier la configuration des matériels et les utiliser avec l'interface de Caerus, vous pouvez également ajouter , modifier ou supprimer les paramètres en agissant dans le répertoire '%s'&lt;br/&gt;Des fenêtres graphiques seront bientôt ajoutées à l’application pour faciliter vos modifications&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" t="str">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="str">
         <f>IF('Changer Configuration'!B8&lt;&gt;"",CONCATENATE('Changer Configuration'!B8,"=", 'Changer Configuration'!C8),IF('Changer Configuration'!C8&lt;&gt;"",'Changer Configuration'!C8,""))</f>
         <v>window.change.configuration.button.apply.and.close=Choisir cette configuration et fermer</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" t="str">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="str">
         <f>IF('Changer Configuration'!B9&lt;&gt;"",CONCATENATE('Changer Configuration'!B9,"=", 'Changer Configuration'!C9),IF('Changer Configuration'!C9&lt;&gt;"",'Changer Configuration'!C9,""))</f>
         <v>window.change.configuration.button.close=Fermer</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" t="str">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="str">
         <f>IF('Changer Configuration'!B10&lt;&gt;"",CONCATENATE('Changer Configuration'!B10,"=", 'Changer Configuration'!C10),IF('Changer Configuration'!C10&lt;&gt;"",'Changer Configuration'!C10,""))</f>
         <v>window.change.configuration.buttons.panel.title=Actions</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" t="str">
-        <f>IF('Changer Configuration'!B11&lt;&gt;"",CONCATENATE('Changer Configuration'!B11,"=", 'Changer Configuration'!C11),IF('Changer Configuration'!C11&lt;&gt;"",'Changer Configuration'!C11,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" t="str">
-        <f>IF('Changer Configuration'!B12&lt;&gt;"",CONCATENATE('Changer Configuration'!B12,"=", 'Changer Configuration'!C12),IF('Changer Configuration'!C12&lt;&gt;"",'Changer Configuration'!C12,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" t="str">
-        <f>IF('Changer Configuration'!B13&lt;&gt;"",CONCATENATE('Changer Configuration'!B13,"=", 'Changer Configuration'!C13),IF('Changer Configuration'!C13&lt;&gt;"",'Changer Configuration'!C13,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" t="str">
-        <f>IF('Changer Configuration'!B14&lt;&gt;"",CONCATENATE('Changer Configuration'!B14,"=", 'Changer Configuration'!C14),IF('Changer Configuration'!C14&lt;&gt;"",'Changer Configuration'!C14,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" t="str">
-        <f>IF('Changer Configuration'!B15&lt;&gt;"",CONCATENATE('Changer Configuration'!B15,"=", 'Changer Configuration'!C15),IF('Changer Configuration'!C15&lt;&gt;"",'Changer Configuration'!C15,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" t="str">
-        <f>IF('Changer Configuration'!B16&lt;&gt;"",CONCATENATE('Changer Configuration'!B16,"=", 'Changer Configuration'!C16),IF('Changer Configuration'!C16&lt;&gt;"",'Changer Configuration'!C16,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" t="str">
-        <f>IF('Changer Configuration'!B17&lt;&gt;"",CONCATENATE('Changer Configuration'!B17,"=", 'Changer Configuration'!C17),IF('Changer Configuration'!C17&lt;&gt;"",'Changer Configuration'!C17,""))</f>
+        <f>IF('Changer Configuration'!B11&lt;&gt;"",CONCATENATE('Changer Configuration'!B11,"=", 'Changer Configuration'!C11),IF('Changer Configuration'!C11&lt;&gt;"",'Changer Configuration'!C11,""))</f>
         <v/>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" t="str">
-        <f>IF('Changer Configuration'!B18&lt;&gt;"",CONCATENATE('Changer Configuration'!B18,"=", 'Changer Configuration'!C18),IF('Changer Configuration'!C18&lt;&gt;"",'Changer Configuration'!C18,""))</f>
+        <f>IF('Changer Configuration'!B12&lt;&gt;"",CONCATENATE('Changer Configuration'!B12,"=", 'Changer Configuration'!C12),IF('Changer Configuration'!C12&lt;&gt;"",'Changer Configuration'!C12,""))</f>
         <v/>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" t="str">
-        <f>IF('Changer Configuration'!B19&lt;&gt;"",CONCATENATE('Changer Configuration'!B19,"=", 'Changer Configuration'!C19),IF('Changer Configuration'!C19&lt;&gt;"",'Changer Configuration'!C19,""))</f>
+        <f>IF('Changer Configuration'!B13&lt;&gt;"",CONCATENATE('Changer Configuration'!B13,"=", 'Changer Configuration'!C13),IF('Changer Configuration'!C13&lt;&gt;"",'Changer Configuration'!C13,""))</f>
         <v/>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" t="str">
-        <f>IF('Changer Configuration'!B20&lt;&gt;"",CONCATENATE('Changer Configuration'!B20,"=", 'Changer Configuration'!C20),IF('Changer Configuration'!C20&lt;&gt;"",'Changer Configuration'!C20,""))</f>
+        <f>IF('Changer Configuration'!B14&lt;&gt;"",CONCATENATE('Changer Configuration'!B14,"=", 'Changer Configuration'!C14),IF('Changer Configuration'!C14&lt;&gt;"",'Changer Configuration'!C14,""))</f>
         <v/>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" t="str">
-        <f>IF('Changer Configuration'!B21&lt;&gt;"",CONCATENATE('Changer Configuration'!B21,"=", 'Changer Configuration'!C21),IF('Changer Configuration'!C21&lt;&gt;"",'Changer Configuration'!C21,""))</f>
+        <f>IF('Changer Configuration'!B15&lt;&gt;"",CONCATENATE('Changer Configuration'!B15,"=", 'Changer Configuration'!C15),IF('Changer Configuration'!C15&lt;&gt;"",'Changer Configuration'!C15,""))</f>
         <v/>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" t="str">
-        <f>IF('Changer Configuration'!B22&lt;&gt;"",CONCATENATE('Changer Configuration'!B22,"=", 'Changer Configuration'!C22),IF('Changer Configuration'!C22&lt;&gt;"",'Changer Configuration'!C22,""))</f>
+        <f>IF('Changer Configuration'!B16&lt;&gt;"",CONCATENATE('Changer Configuration'!B16,"=", 'Changer Configuration'!C16),IF('Changer Configuration'!C16&lt;&gt;"",'Changer Configuration'!C16,""))</f>
         <v/>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" t="str">
-        <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE('Changer Configuration'!B23,"=", 'Changer Configuration'!C23),IF('Changer Configuration'!C23&lt;&gt;"",'Changer Configuration'!C23,""))</f>
+        <f>IF('Changer Configuration'!B17&lt;&gt;"",CONCATENATE('Changer Configuration'!B17,"=", 'Changer Configuration'!C17),IF('Changer Configuration'!C17&lt;&gt;"",'Changer Configuration'!C17,""))</f>
         <v/>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" t="str">
+        <f>IF('Changer Configuration'!B18&lt;&gt;"",CONCATENATE('Changer Configuration'!B18,"=", 'Changer Configuration'!C18),IF('Changer Configuration'!C18&lt;&gt;"",'Changer Configuration'!C18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" t="str">
+        <f>IF('Changer Configuration'!B19&lt;&gt;"",CONCATENATE('Changer Configuration'!B19,"=", 'Changer Configuration'!C19),IF('Changer Configuration'!C19&lt;&gt;"",'Changer Configuration'!C19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" t="str">
+        <f>IF('Changer Configuration'!B20&lt;&gt;"",CONCATENATE('Changer Configuration'!B20,"=", 'Changer Configuration'!C20),IF('Changer Configuration'!C20&lt;&gt;"",'Changer Configuration'!C20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" t="str">
+        <f>IF('Changer Configuration'!B21&lt;&gt;"",CONCATENATE('Changer Configuration'!B21,"=", 'Changer Configuration'!C21),IF('Changer Configuration'!C21&lt;&gt;"",'Changer Configuration'!C21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" t="str">
+        <f>IF('Changer Configuration'!B22&lt;&gt;"",CONCATENATE('Changer Configuration'!B22,"=", 'Changer Configuration'!C22),IF('Changer Configuration'!C22&lt;&gt;"",'Changer Configuration'!C22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" t="str">
+        <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE('Changer Configuration'!B23,"=", 'Changer Configuration'!C23),IF('Changer Configuration'!C23&lt;&gt;"",'Changer Configuration'!C23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" t="str">
         <f>IF('A propos'!B2&lt;&gt;"",CONCATENATE('A propos'!B2,"=", 'A propos'!C2),IF('A propos'!C2&lt;&gt;"",'A propos'!C2,""))</f>
         <v>#Message pour la fenêtre a propos</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" t="str">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" t="str">
         <f>IF('A propos'!B3&lt;&gt;"",CONCATENATE('A propos'!B3,"=", 'A propos'!C3),IF('A propos'!C3&lt;&gt;"",'A propos'!C3,""))</f>
         <v>window.about.title=A propos</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" t="str">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" t="str">
         <f>IF('A propos'!B4&lt;&gt;"",CONCATENATE('A propos'!B4,"=", 'A propos'!C4),IF('A propos'!C4&lt;&gt;"",'A propos'!C4,""))</f>
         <v>window.about.message.content=&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;A propos de l'application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nom de l'application : &lt;/u&gt; Caerus&lt;br /&gt;&lt;u&gt;Version : &lt;/u&gt; 1.1.2&lt;br /&gt;&lt;u&gt;Editeur : &lt;/u&gt; Jeremy, Leda&lt;br /&gt;&lt;u&gt;Site web : &lt;/u&gt;https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" t="str">
-        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE('A propos'!B5,"=", 'A propos'!C5),IF('A propos'!C5&lt;&gt;"",'A propos'!C5,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385" t="str">
-        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE('A propos'!B6,"=", 'A propos'!C6),IF('A propos'!C6&lt;&gt;"",'A propos'!C6,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" t="str">
-        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE('A propos'!B7,"=", 'A propos'!C7),IF('A propos'!C7&lt;&gt;"",'A propos'!C7,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" t="str">
-        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE('A propos'!B8,"=", 'A propos'!C8),IF('A propos'!C8&lt;&gt;"",'A propos'!C8,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" t="str">
-        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE('A propos'!B9,"=", 'A propos'!C9),IF('A propos'!C9&lt;&gt;"",'A propos'!C9,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" t="str">
-        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE('A propos'!B10,"=", 'A propos'!C10),IF('A propos'!C10&lt;&gt;"",'A propos'!C10,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A390" t="str">
-        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE('A propos'!B11,"=", 'A propos'!C11),IF('A propos'!C11&lt;&gt;"",'A propos'!C11,""))</f>
+        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE('A propos'!B5,"=", 'A propos'!C5),IF('A propos'!C5&lt;&gt;"",'A propos'!C5,""))</f>
         <v/>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" t="str">
-        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE('A propos'!B12,"=", 'A propos'!C12),IF('A propos'!C12&lt;&gt;"",'A propos'!C12,""))</f>
+        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE('A propos'!B6,"=", 'A propos'!C6),IF('A propos'!C6&lt;&gt;"",'A propos'!C6,""))</f>
         <v/>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" t="str">
-        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE('A propos'!B13,"=", 'A propos'!C13),IF('A propos'!C13&lt;&gt;"",'A propos'!C13,""))</f>
+        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE('A propos'!B7,"=", 'A propos'!C7),IF('A propos'!C7&lt;&gt;"",'A propos'!C7,""))</f>
         <v/>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" t="str">
-        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE('A propos'!B14,"=", 'A propos'!C14),IF('A propos'!C14&lt;&gt;"",'A propos'!C14,""))</f>
+        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE('A propos'!B8,"=", 'A propos'!C8),IF('A propos'!C8&lt;&gt;"",'A propos'!C8,""))</f>
         <v/>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" t="str">
-        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE('A propos'!B15,"=", 'A propos'!C15),IF('A propos'!C15&lt;&gt;"",'A propos'!C15,""))</f>
+        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE('A propos'!B9,"=", 'A propos'!C9),IF('A propos'!C9&lt;&gt;"",'A propos'!C9,""))</f>
         <v/>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" t="str">
-        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE('A propos'!B16,"=", 'A propos'!C16),IF('A propos'!C16&lt;&gt;"",'A propos'!C16,""))</f>
+        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE('A propos'!B10,"=", 'A propos'!C10),IF('A propos'!C10&lt;&gt;"",'A propos'!C10,""))</f>
         <v/>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" t="str">
-        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!C17),IF('A propos'!C17&lt;&gt;"",'A propos'!C17,""))</f>
+        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE('A propos'!B11,"=", 'A propos'!C11),IF('A propos'!C11&lt;&gt;"",'A propos'!C11,""))</f>
         <v/>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" t="str">
-        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!C18),IF('A propos'!C18&lt;&gt;"",'A propos'!C18,""))</f>
+        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE('A propos'!B12,"=", 'A propos'!C12),IF('A propos'!C12&lt;&gt;"",'A propos'!C12,""))</f>
         <v/>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" t="str">
-        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!C17),IF('A propos'!C17&lt;&gt;"",'A propos'!C17,""))</f>
+        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE('A propos'!B13,"=", 'A propos'!C13),IF('A propos'!C13&lt;&gt;"",'A propos'!C13,""))</f>
         <v/>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" t="str">
-        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!C18),IF('A propos'!C18&lt;&gt;"",'A propos'!C18,""))</f>
+        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE('A propos'!B14,"=", 'A propos'!C14),IF('A propos'!C14&lt;&gt;"",'A propos'!C14,""))</f>
         <v/>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" t="str">
-        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!C19),IF('A propos'!C19&lt;&gt;"",'A propos'!C19,""))</f>
+        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE('A propos'!B15,"=", 'A propos'!C15),IF('A propos'!C15&lt;&gt;"",'A propos'!C15,""))</f>
         <v/>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" t="str">
-        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE('A propos'!B20,"=", 'A propos'!C42),IF('A propos'!C20&lt;&gt;"",'A propos'!C20,""))</f>
+        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE('A propos'!B16,"=", 'A propos'!C16),IF('A propos'!C16&lt;&gt;"",'A propos'!C16,""))</f>
         <v/>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402" t="str">
-        <f>IF('A propos'!B21&lt;&gt;"",CONCATENATE('A propos'!B21,"=", 'A propos'!C43),IF('A propos'!C21&lt;&gt;"",'A propos'!C21,""))</f>
+        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!C17),IF('A propos'!C17&lt;&gt;"",'A propos'!C17,""))</f>
         <v/>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" t="str">
-        <f>IF('A propos'!B22&lt;&gt;"",CONCATENATE('A propos'!B22,"=", 'A propos'!C44),IF('A propos'!C22&lt;&gt;"",'A propos'!C22,""))</f>
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!C18),IF('A propos'!C18&lt;&gt;"",'A propos'!C18,""))</f>
         <v/>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" t="str">
+        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!C17),IF('A propos'!C17&lt;&gt;"",'A propos'!C17,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" t="str">
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!C18),IF('A propos'!C18&lt;&gt;"",'A propos'!C18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" t="str">
+        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!C19),IF('A propos'!C19&lt;&gt;"",'A propos'!C19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" t="str">
+        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE('A propos'!B20,"=", 'A propos'!C42),IF('A propos'!C20&lt;&gt;"",'A propos'!C20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" t="str">
+        <f>IF('A propos'!B21&lt;&gt;"",CONCATENATE('A propos'!B21,"=", 'A propos'!C43),IF('A propos'!C21&lt;&gt;"",'A propos'!C21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" t="str">
+        <f>IF('A propos'!B22&lt;&gt;"",CONCATENATE('A propos'!B22,"=", 'A propos'!C44),IF('A propos'!C22&lt;&gt;"",'A propos'!C22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" t="str">
         <f>IF('Export Document Materiel'!B2&lt;&gt;"",CONCATENATE('Export Document Materiel'!B2,"=", 'Export Document Materiel'!C2),IF('Export Document Materiel'!C2&lt;&gt;"",'Export Document Materiel'!C2,""))</f>
         <v>#Message pour l'export de document et matériel</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" t="str">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" t="str">
         <f>IF('Export Document Materiel'!B3&lt;&gt;"",CONCATENATE('Export Document Materiel'!B3,"=", 'Export Document Materiel'!C3),IF('Export Document Materiel'!C3&lt;&gt;"",'Export Document Materiel'!C3,""))</f>
         <v>window.export.document.title=Exporter les documents/matériels</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A406" t="str">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" t="str">
         <f>IF('Export Document Materiel'!B4&lt;&gt;"",CONCATENATE('Export Document Materiel'!B4,"=", 'Export Document Materiel'!C4),IF('Export Document Materiel'!C4&lt;&gt;"",'Export Document Materiel'!C4,""))</f>
         <v>window.export.document.choose.directory.panel.title=Choix du dossier de destination</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" t="str">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" t="str">
         <f>IF('Export Document Materiel'!B5&lt;&gt;"",CONCATENATE('Export Document Materiel'!B5,"=", 'Export Document Materiel'!C5),IF('Export Document Materiel'!C5&lt;&gt;"",'Export Document Materiel'!C5,""))</f>
         <v>window.export.document.choose.directory.label=Dossier de destination</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" t="str">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" t="str">
         <f>IF('Export Document Materiel'!B6&lt;&gt;"",CONCATENATE('Export Document Materiel'!B6,"=", 'Export Document Materiel'!C6),IF('Export Document Materiel'!C6&lt;&gt;"",'Export Document Materiel'!C6,""))</f>
         <v>window.export.document.mode.panel.title=Choix des données à exporter</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A409" t="str">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" t="str">
         <f>IF('Export Document Materiel'!B7&lt;&gt;"",CONCATENATE('Export Document Materiel'!B7,"=", 'Export Document Materiel'!C7),IF('Export Document Materiel'!C7&lt;&gt;"",'Export Document Materiel'!C7,""))</f>
         <v>window.export.document.mode.document.label=Un document</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" t="str">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" t="str">
         <f>IF('Export Document Materiel'!B8&lt;&gt;"",CONCATENATE('Export Document Materiel'!B8,"=", 'Export Document Materiel'!C8),IF('Export Document Materiel'!C8&lt;&gt;"",'Export Document Materiel'!C8,""))</f>
         <v>window.export.document.mode.all.documents.label=Tous les documents</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" t="str">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" t="str">
         <f>IF('Export Document Materiel'!B9&lt;&gt;"",CONCATENATE('Export Document Materiel'!B9,"=", 'Export Document Materiel'!C9),IF('Export Document Materiel'!C9&lt;&gt;"",'Export Document Materiel'!C9,""))</f>
         <v>window.export.document.mode.result.search.label=Le résultat de la recherche</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" t="str">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="str">
         <f>IF('Export Document Materiel'!B10&lt;&gt;"",CONCATENATE('Export Document Materiel'!B10,"=", 'Export Document Materiel'!C10),IF('Export Document Materiel'!C10&lt;&gt;"",'Export Document Materiel'!C10,""))</f>
         <v>window.export.document.choose.document.panel.title=Choix du document à exporter</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" t="str">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" t="str">
         <f>IF('Export Document Materiel'!B11&lt;&gt;"",CONCATENATE('Export Document Materiel'!B11,"=", 'Export Document Materiel'!C11),IF('Export Document Materiel'!C11&lt;&gt;"",'Export Document Materiel'!C11,""))</f>
         <v xml:space="preserve">window.export.document.choose.document.label=Document à exporter : </v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" t="str">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" t="str">
         <f>IF('Export Document Materiel'!B12&lt;&gt;"",CONCATENATE('Export Document Materiel'!B12,"=", 'Export Document Materiel'!C12),IF('Export Document Materiel'!C12&lt;&gt;"",'Export Document Materiel'!C12,""))</f>
         <v>window.export.document.choose.file.panel.title=Choix du nom du document</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415" t="str">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" t="str">
         <f>IF('Export Document Materiel'!B13&lt;&gt;"",CONCATENATE('Export Document Materiel'!B13,"=", 'Export Document Materiel'!C13),IF('Export Document Materiel'!C13&lt;&gt;"",'Export Document Materiel'!C13,""))</f>
         <v xml:space="preserve">window.export.document.choose.file.label=Nom du document pour le resultat de la recherche : </v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" t="str">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" t="str">
         <f>IF('Export Document Materiel'!B14&lt;&gt;"",CONCATENATE('Export Document Materiel'!B14,"=", 'Export Document Materiel'!C14),IF('Export Document Materiel'!C14&lt;&gt;"",'Export Document Materiel'!C14,""))</f>
         <v>window.export.document.button.panel.title=Actions</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" t="str">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" t="str">
         <f>IF('Export Document Materiel'!B15&lt;&gt;"",CONCATENATE('Export Document Materiel'!B15,"=", 'Export Document Materiel'!C15),IF('Export Document Materiel'!C15&lt;&gt;"",'Export Document Materiel'!C15,""))</f>
         <v>window.export.document.button.export.label=Exporter et fermer</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418" t="str">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" t="str">
         <f>IF('Export Document Materiel'!B16&lt;&gt;"",CONCATENATE('Export Document Materiel'!B16,"=", 'Export Document Materiel'!C16),IF('Export Document Materiel'!C16&lt;&gt;"",'Export Document Materiel'!C16,""))</f>
         <v>window.export.document.information.message.title=Export effectué</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" t="str">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" t="str">
         <f>IF('Export Document Materiel'!B17&lt;&gt;"",CONCATENATE('Export Document Materiel'!B17,"=", 'Export Document Materiel'!C17),IF('Export Document Materiel'!C17&lt;&gt;"",'Export Document Materiel'!C17,""))</f>
         <v>window.export.document.information.message=&lt;HTML&gt;&lt;P&gt;Export réalisé avec succés&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A420" t="str">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" t="str">
         <f>IF('Export Document Materiel'!B18&lt;&gt;"",CONCATENATE('Export Document Materiel'!B18,"=", 'Export Document Materiel'!C18),IF('Export Document Materiel'!C18&lt;&gt;"",'Export Document Materiel'!C18,""))</f>
         <v>window.export.document.button.close.label=Fermer</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" t="str">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" t="str">
         <f>IF('Export Document Materiel'!B19&lt;&gt;"",CONCATENATE('Export Document Materiel'!B19,"=", 'Export Document Materiel'!C19),IF('Export Document Materiel'!C19&lt;&gt;"",'Export Document Materiel'!C19,""))</f>
         <v>window.export.document.choose.directory.dialog.title=Choisissez le dossier de destination</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" t="str">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" t="str">
         <f>IF('Export Document Materiel'!B20&lt;&gt;"",CONCATENATE('Export Document Materiel'!B20,"=", 'Export Document Materiel'!C20),IF('Export Document Materiel'!C20&lt;&gt;"",'Export Document Materiel'!C20,""))</f>
         <v>window.export.document.information.search.message=&lt;HTML&gt;&lt;P&gt;Export réalisé avec succés&lt;BR/&gt;Pour information, le document ne contient aucune données d'en-tête&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" t="str">
-        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE('Export Document Materiel'!B21,"=", 'Export Document Materiel'!C21),IF('Export Document Materiel'!C21&lt;&gt;"",'Export Document Materiel'!C21,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" t="str">
-        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE('Export Document Materiel'!B22,"=", 'Export Document Materiel'!C22),IF('Export Document Materiel'!C22&lt;&gt;"",'Export Document Materiel'!C22,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" t="str">
-        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE('Export Document Materiel'!B23,"=", 'Export Document Materiel'!C23),IF('Export Document Materiel'!C23&lt;&gt;"",'Export Document Materiel'!C23,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" t="str">
-        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE('Export Document Materiel'!B24,"=", 'Export Document Materiel'!C24),IF('Export Document Materiel'!C24&lt;&gt;"",'Export Document Materiel'!C24,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" t="str">
-        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE('Export Document Materiel'!B25,"=", 'Export Document Materiel'!C25),IF('Export Document Materiel'!C25&lt;&gt;"",'Export Document Materiel'!C25,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" t="str">
-        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE('Export Document Materiel'!B26,"=", 'Export Document Materiel'!C26),IF('Export Document Materiel'!C26&lt;&gt;"",'Export Document Materiel'!C26,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" t="str">
-        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE('Export Document Materiel'!B27,"=", 'Export Document Materiel'!C27),IF('Export Document Materiel'!C27&lt;&gt;"",'Export Document Materiel'!C27,""))</f>
+        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE('Export Document Materiel'!B21,"=", 'Export Document Materiel'!C21),IF('Export Document Materiel'!C21&lt;&gt;"",'Export Document Materiel'!C21,""))</f>
         <v/>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A430" t="str">
-        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE('Export Document Materiel'!B28,"=", 'Export Document Materiel'!C28),IF('Export Document Materiel'!C28&lt;&gt;"",'Export Document Materiel'!C28,""))</f>
+        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE('Export Document Materiel'!B22,"=", 'Export Document Materiel'!C22),IF('Export Document Materiel'!C22&lt;&gt;"",'Export Document Materiel'!C22,""))</f>
         <v/>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" t="str">
-        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE('Export Document Materiel'!B29,"=", 'Export Document Materiel'!C29),IF('Export Document Materiel'!C29&lt;&gt;"",'Export Document Materiel'!C29,""))</f>
+        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE('Export Document Materiel'!B23,"=", 'Export Document Materiel'!C23),IF('Export Document Materiel'!C23&lt;&gt;"",'Export Document Materiel'!C23,""))</f>
         <v/>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A432" t="str">
-        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE('Export Document Materiel'!B30,"=", 'Export Document Materiel'!C30),IF('Export Document Materiel'!C30&lt;&gt;"",'Export Document Materiel'!C30,""))</f>
+        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE('Export Document Materiel'!B24,"=", 'Export Document Materiel'!C24),IF('Export Document Materiel'!C24&lt;&gt;"",'Export Document Materiel'!C24,""))</f>
         <v/>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" t="str">
-        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE('Export Document Materiel'!B31,"=", 'Export Document Materiel'!C31),IF('Export Document Materiel'!C31&lt;&gt;"",'Export Document Materiel'!C31,""))</f>
+        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE('Export Document Materiel'!B25,"=", 'Export Document Materiel'!C25),IF('Export Document Materiel'!C25&lt;&gt;"",'Export Document Materiel'!C25,""))</f>
         <v/>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" t="str">
-        <f>IF('Export Document Materiel'!B32&lt;&gt;"",CONCATENATE('Export Document Materiel'!B32,"=", 'Export Document Materiel'!C32),IF('Export Document Materiel'!C32&lt;&gt;"",'Export Document Materiel'!C32,""))</f>
+        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE('Export Document Materiel'!B26,"=", 'Export Document Materiel'!C26),IF('Export Document Materiel'!C26&lt;&gt;"",'Export Document Materiel'!C26,""))</f>
         <v/>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A435" t="str">
-        <f>IF('Export Document Materiel'!B33&lt;&gt;"",CONCATENATE('Export Document Materiel'!B33,"=", 'Export Document Materiel'!C33),IF('Export Document Materiel'!C33&lt;&gt;"",'Export Document Materiel'!C33,""))</f>
+        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE('Export Document Materiel'!B27,"=", 'Export Document Materiel'!C27),IF('Export Document Materiel'!C27&lt;&gt;"",'Export Document Materiel'!C27,""))</f>
         <v/>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" t="str">
-        <f>IF('Export Document Materiel'!B34&lt;&gt;"",CONCATENATE('Export Document Materiel'!B34,"=", 'Export Document Materiel'!C34),IF('Export Document Materiel'!C34&lt;&gt;"",'Export Document Materiel'!C34,""))</f>
+        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE('Export Document Materiel'!B28,"=", 'Export Document Materiel'!C28),IF('Export Document Materiel'!C28&lt;&gt;"",'Export Document Materiel'!C28,""))</f>
         <v/>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" t="str">
+        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE('Export Document Materiel'!B29,"=", 'Export Document Materiel'!C29),IF('Export Document Materiel'!C29&lt;&gt;"",'Export Document Materiel'!C29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" t="str">
+        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE('Export Document Materiel'!B30,"=", 'Export Document Materiel'!C30),IF('Export Document Materiel'!C30&lt;&gt;"",'Export Document Materiel'!C30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" t="str">
+        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE('Export Document Materiel'!B31,"=", 'Export Document Materiel'!C31),IF('Export Document Materiel'!C31&lt;&gt;"",'Export Document Materiel'!C31,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" t="str">
+        <f>IF('Export Document Materiel'!B32&lt;&gt;"",CONCATENATE('Export Document Materiel'!B32,"=", 'Export Document Materiel'!C32),IF('Export Document Materiel'!C32&lt;&gt;"",'Export Document Materiel'!C32,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" t="str">
+        <f>IF('Export Document Materiel'!B33&lt;&gt;"",CONCATENATE('Export Document Materiel'!B33,"=", 'Export Document Materiel'!C33),IF('Export Document Materiel'!C33&lt;&gt;"",'Export Document Materiel'!C33,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" t="str">
+        <f>IF('Export Document Materiel'!B34&lt;&gt;"",CONCATENATE('Export Document Materiel'!B34,"=", 'Export Document Materiel'!C34),IF('Export Document Materiel'!C34&lt;&gt;"",'Export Document Materiel'!C34,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" t="str">
         <f>IF('Erreur incoherence'!B2&lt;&gt;"",CONCATENATE('Erreur incoherence'!B2,"=", 'Erreur incoherence'!C2),IF('Erreur incoherence'!C2&lt;&gt;"",'Erreur incoherence'!C2,""))</f>
         <v>#Message pour les erreurs d'incohérence</v>
       </c>
     </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" t="str">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" t="str">
         <f>IF('Erreur incoherence'!B3&lt;&gt;"",CONCATENATE('Erreur incoherence'!B3,"=", 'Erreur incoherence'!C3),IF('Erreur incoherence'!C3&lt;&gt;"",'Erreur incoherence'!C3,""))</f>
         <v>window.error.inconsistency.title=Erreurs de duplications</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A439" t="str">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" t="str">
         <f>IF('Erreur incoherence'!B4&lt;&gt;"",CONCATENATE('Erreur incoherence'!B4,"=", 'Erreur incoherence'!C4),IF('Erreur incoherence'!C4&lt;&gt;"",'Erreur incoherence'!C4,""))</f>
         <v>window.error.inconsistency.panel.title=Liste des incohérences</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" t="str">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" t="str">
         <f>IF('Erreur incoherence'!B5&lt;&gt;"",CONCATENATE('Erreur incoherence'!B5,"=", 'Erreur incoherence'!C5),IF('Erreur incoherence'!C5&lt;&gt;"",'Erreur incoherence'!C5,""))</f>
         <v xml:space="preserve">window.error.inconsistency.field.label=Balise : </v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" t="str">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" t="str">
         <f>IF('Erreur incoherence'!B6&lt;&gt;"",CONCATENATE('Erreur incoherence'!B6,"=", 'Erreur incoherence'!C6),IF('Erreur incoherence'!C6&lt;&gt;"",'Erreur incoherence'!C6,""))</f>
         <v xml:space="preserve">window.error.inconsistency.number.line.label=Numéro de la ligne : </v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" t="str">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" t="str">
         <f>IF('Erreur incoherence'!B7&lt;&gt;"",CONCATENATE('Erreur incoherence'!B7,"=", 'Erreur incoherence'!C7),IF('Erreur incoherence'!C7&lt;&gt;"",'Erreur incoherence'!C7,""))</f>
         <v xml:space="preserve">window.error.inconsistency.name.file.label=Nom du fichier : </v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" t="str">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" t="str">
         <f>IF('Erreur incoherence'!B8&lt;&gt;"",CONCATENATE('Erreur incoherence'!B8,"=", 'Erreur incoherence'!C8),IF('Erreur incoherence'!C8&lt;&gt;"",'Erreur incoherence'!C8,""))</f>
         <v>window.error.inconsistency.message.panel.title=Message d'information</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" t="str">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" t="str">
         <f>IF('Erreur incoherence'!B9&lt;&gt;"",CONCATENATE('Erreur incoherence'!B9,"=", 'Erreur incoherence'!C9),IF('Erreur incoherence'!C9&lt;&gt;"",'Erreur incoherence'!C9,""))</f>
         <v>window.error.inconsistency.message=&lt;HTML&gt;&lt;P&gt;Des erreurs d'incohérence ont été détectées.&lt;BR/&gt;Celles-ci peuvent causer des décalages d'information.&lt;BR/&gt;Vous devez corriger manuellement les informations.&lt;BR/&gt;Rechargez les documents corrigés.&lt;BR/&gt;De nouvelles erreurs peuvent être détectées en raison de lacunes dans l'information.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" t="str">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" t="str">
         <f>IF('Erreur incoherence'!B10&lt;&gt;"",CONCATENATE('Erreur incoherence'!B10,"=", 'Erreur incoherence'!C10),IF('Erreur incoherence'!C10&lt;&gt;"",'Erreur incoherence'!C10,""))</f>
         <v>window.error.inconsistency.buttons.panel.title=Actions</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" t="str">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" t="str">
         <f>IF('Erreur incoherence'!B11&lt;&gt;"",CONCATENATE('Erreur incoherence'!B11,"=", 'Erreur incoherence'!C11),IF('Erreur incoherence'!C11&lt;&gt;"",'Erreur incoherence'!C11,""))</f>
         <v>window.error.inconsistency.buttons.close.button.label=Fermer et recharger les documents</v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A447" t="str">
-        <f>IF('Erreur incoherence'!B12&lt;&gt;"",CONCATENATE('Erreur incoherence'!B12,"=", 'Erreur incoherence'!C12),IF('Erreur incoherence'!C12&lt;&gt;"",'Erreur incoherence'!C12,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" t="str">
-        <f>IF('Erreur incoherence'!B13&lt;&gt;"",CONCATENATE('Erreur incoherence'!B13,"=", 'Erreur incoherence'!C13),IF('Erreur incoherence'!C13&lt;&gt;"",'Erreur incoherence'!C13,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" t="str">
-        <f>IF('Erreur incoherence'!B14&lt;&gt;"",CONCATENATE('Erreur incoherence'!B14,"=", 'Erreur incoherence'!C14),IF('Erreur incoherence'!C14&lt;&gt;"",'Erreur incoherence'!C14,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" t="str">
-        <f>IF('Erreur incoherence'!B15&lt;&gt;"",CONCATENATE('Erreur incoherence'!B15,"=", 'Erreur incoherence'!C15),IF('Erreur incoherence'!C15&lt;&gt;"",'Erreur incoherence'!C15,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" t="str">
-        <f>IF('Erreur incoherence'!B16&lt;&gt;"",CONCATENATE('Erreur incoherence'!B16,"=", 'Erreur incoherence'!C16),IF('Erreur incoherence'!C16&lt;&gt;"",'Erreur incoherence'!C16,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" t="str">
-        <f>IF('Erreur incoherence'!B17&lt;&gt;"",CONCATENATE('Erreur incoherence'!B17,"=", 'Erreur incoherence'!C17),IF('Erreur incoherence'!C17&lt;&gt;"",'Erreur incoherence'!C17,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453" t="str">
-        <f>IF('Erreur incoherence'!B18&lt;&gt;"",CONCATENATE('Erreur incoherence'!B18,"=", 'Erreur incoherence'!C18),IF('Erreur incoherence'!C18&lt;&gt;"",'Erreur incoherence'!C18,""))</f>
+        <f>IF('Erreur incoherence'!B12&lt;&gt;"",CONCATENATE('Erreur incoherence'!B12,"=", 'Erreur incoherence'!C12),IF('Erreur incoherence'!C12&lt;&gt;"",'Erreur incoherence'!C12,""))</f>
         <v/>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A454" t="str">
-        <f>IF('Erreur incoherence'!B19&lt;&gt;"",CONCATENATE('Erreur incoherence'!B19,"=", 'Erreur incoherence'!C19),IF('Erreur incoherence'!C19&lt;&gt;"",'Erreur incoherence'!C19,""))</f>
+        <f>IF('Erreur incoherence'!B13&lt;&gt;"",CONCATENATE('Erreur incoherence'!B13,"=", 'Erreur incoherence'!C13),IF('Erreur incoherence'!C13&lt;&gt;"",'Erreur incoherence'!C13,""))</f>
         <v/>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" t="str">
-        <f>IF('Erreur incoherence'!B20&lt;&gt;"",CONCATENATE('Erreur incoherence'!B20,"=", 'Erreur incoherence'!C20),IF('Erreur incoherence'!C20&lt;&gt;"",'Erreur incoherence'!C20,""))</f>
+        <f>IF('Erreur incoherence'!B14&lt;&gt;"",CONCATENATE('Erreur incoherence'!B14,"=", 'Erreur incoherence'!C14),IF('Erreur incoherence'!C14&lt;&gt;"",'Erreur incoherence'!C14,""))</f>
         <v/>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A456" t="str">
-        <f>IF('Erreur incoherence'!B21&lt;&gt;"",CONCATENATE('Erreur incoherence'!B21,"=", 'Erreur incoherence'!C21),IF('Erreur incoherence'!C21&lt;&gt;"",'Erreur incoherence'!C21,""))</f>
+        <f>IF('Erreur incoherence'!B15&lt;&gt;"",CONCATENATE('Erreur incoherence'!B15,"=", 'Erreur incoherence'!C15),IF('Erreur incoherence'!C15&lt;&gt;"",'Erreur incoherence'!C15,""))</f>
         <v/>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A457" t="str">
-        <f>IF('Erreur incoherence'!B22&lt;&gt;"",CONCATENATE('Erreur incoherence'!B22,"=", 'Erreur incoherence'!C22),IF('Erreur incoherence'!C22&lt;&gt;"",'Erreur incoherence'!C22,""))</f>
+        <f>IF('Erreur incoherence'!B16&lt;&gt;"",CONCATENATE('Erreur incoherence'!B16,"=", 'Erreur incoherence'!C16),IF('Erreur incoherence'!C16&lt;&gt;"",'Erreur incoherence'!C16,""))</f>
         <v/>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" t="str">
-        <f>IF('Erreur incoherence'!B23&lt;&gt;"",CONCATENATE('Erreur incoherence'!B23,"=", 'Erreur incoherence'!C23),IF('Erreur incoherence'!C23&lt;&gt;"",'Erreur incoherence'!C23,""))</f>
+        <f>IF('Erreur incoherence'!B17&lt;&gt;"",CONCATENATE('Erreur incoherence'!B17,"=", 'Erreur incoherence'!C17),IF('Erreur incoherence'!C17&lt;&gt;"",'Erreur incoherence'!C17,""))</f>
         <v/>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" t="str">
-        <f>IF('Erreur incoherence'!B24&lt;&gt;"",CONCATENATE('Erreur incoherence'!B24,"=", 'Erreur incoherence'!C24),IF('Erreur incoherence'!C24&lt;&gt;"",'Erreur incoherence'!C24,""))</f>
+        <f>IF('Erreur incoherence'!B18&lt;&gt;"",CONCATENATE('Erreur incoherence'!B18,"=", 'Erreur incoherence'!C18),IF('Erreur incoherence'!C18&lt;&gt;"",'Erreur incoherence'!C18,""))</f>
         <v/>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" t="str">
-        <f>IF('Erreur incoherence'!B25&lt;&gt;"",CONCATENATE('Erreur incoherence'!B25,"=", 'Erreur incoherence'!C25),IF('Erreur incoherence'!C25&lt;&gt;"",'Erreur incoherence'!C25,""))</f>
+        <f>IF('Erreur incoherence'!B19&lt;&gt;"",CONCATENATE('Erreur incoherence'!B19,"=", 'Erreur incoherence'!C19),IF('Erreur incoherence'!C19&lt;&gt;"",'Erreur incoherence'!C19,""))</f>
         <v/>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" t="str">
-        <f>IF('Erreur incoherence'!B26&lt;&gt;"",CONCATENATE('Erreur incoherence'!B26,"=", 'Erreur incoherence'!C26),IF('Erreur incoherence'!C26&lt;&gt;"",'Erreur incoherence'!C26,""))</f>
+        <f>IF('Erreur incoherence'!B20&lt;&gt;"",CONCATENATE('Erreur incoherence'!B20,"=", 'Erreur incoherence'!C20),IF('Erreur incoherence'!C20&lt;&gt;"",'Erreur incoherence'!C20,""))</f>
         <v/>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" t="str">
-        <f>IF('Erreur incoherence'!B27&lt;&gt;"",CONCATENATE('Erreur incoherence'!B27,"=", 'Erreur incoherence'!C27),IF('Erreur incoherence'!C27&lt;&gt;"",'Erreur incoherence'!C27,""))</f>
+        <f>IF('Erreur incoherence'!B21&lt;&gt;"",CONCATENATE('Erreur incoherence'!B21,"=", 'Erreur incoherence'!C21),IF('Erreur incoherence'!C21&lt;&gt;"",'Erreur incoherence'!C21,""))</f>
         <v/>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A463" t="str">
-        <f>IF('Erreur incoherence'!B28&lt;&gt;"",CONCATENATE('Erreur incoherence'!B28,"=", 'Erreur incoherence'!C28),IF('Erreur incoherence'!C28&lt;&gt;"",'Erreur incoherence'!C28,""))</f>
+        <f>IF('Erreur incoherence'!B22&lt;&gt;"",CONCATENATE('Erreur incoherence'!B22,"=", 'Erreur incoherence'!C22),IF('Erreur incoherence'!C22&lt;&gt;"",'Erreur incoherence'!C22,""))</f>
         <v/>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" t="str">
-        <f>IF('Erreur incoherence'!B29&lt;&gt;"",CONCATENATE('Erreur incoherence'!B29,"=", 'Erreur incoherence'!C29),IF('Erreur incoherence'!C29&lt;&gt;"",'Erreur incoherence'!C29,""))</f>
+        <f>IF('Erreur incoherence'!B23&lt;&gt;"",CONCATENATE('Erreur incoherence'!B23,"=", 'Erreur incoherence'!C23),IF('Erreur incoherence'!C23&lt;&gt;"",'Erreur incoherence'!C23,""))</f>
         <v/>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A465" t="str">
-        <f>IF('Erreur incoherence'!B30&lt;&gt;"",CONCATENATE('Erreur incoherence'!B30,"=", 'Erreur incoherence'!C30),IF('Erreur incoherence'!C30&lt;&gt;"",'Erreur incoherence'!C30,""))</f>
+        <f>IF('Erreur incoherence'!B24&lt;&gt;"",CONCATENATE('Erreur incoherence'!B24,"=", 'Erreur incoherence'!C24),IF('Erreur incoherence'!C24&lt;&gt;"",'Erreur incoherence'!C24,""))</f>
         <v/>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466" t="str">
-        <f>IF('Erreur incoherence'!B31&lt;&gt;"",CONCATENATE('Erreur incoherence'!B31,"=", 'Erreur incoherence'!C31),IF('Erreur incoherence'!C31&lt;&gt;"",'Erreur incoherence'!C31,""))</f>
+        <f>IF('Erreur incoherence'!B25&lt;&gt;"",CONCATENATE('Erreur incoherence'!B25,"=", 'Erreur incoherence'!C25),IF('Erreur incoherence'!C25&lt;&gt;"",'Erreur incoherence'!C25,""))</f>
         <v/>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A467" t="str">
+        <f>IF('Erreur incoherence'!B26&lt;&gt;"",CONCATENATE('Erreur incoherence'!B26,"=", 'Erreur incoherence'!C26),IF('Erreur incoherence'!C26&lt;&gt;"",'Erreur incoherence'!C26,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" t="str">
+        <f>IF('Erreur incoherence'!B27&lt;&gt;"",CONCATENATE('Erreur incoherence'!B27,"=", 'Erreur incoherence'!C27),IF('Erreur incoherence'!C27&lt;&gt;"",'Erreur incoherence'!C27,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" t="str">
+        <f>IF('Erreur incoherence'!B28&lt;&gt;"",CONCATENATE('Erreur incoherence'!B28,"=", 'Erreur incoherence'!C28),IF('Erreur incoherence'!C28&lt;&gt;"",'Erreur incoherence'!C28,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" t="str">
+        <f>IF('Erreur incoherence'!B29&lt;&gt;"",CONCATENATE('Erreur incoherence'!B29,"=", 'Erreur incoherence'!C29),IF('Erreur incoherence'!C29&lt;&gt;"",'Erreur incoherence'!C29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" t="str">
+        <f>IF('Erreur incoherence'!B30&lt;&gt;"",CONCATENATE('Erreur incoherence'!B30,"=", 'Erreur incoherence'!C30),IF('Erreur incoherence'!C30&lt;&gt;"",'Erreur incoherence'!C30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" t="str">
+        <f>IF('Erreur incoherence'!B31&lt;&gt;"",CONCATENATE('Erreur incoherence'!B31,"=", 'Erreur incoherence'!C31),IF('Erreur incoherence'!C31&lt;&gt;"",'Erreur incoherence'!C31,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" t="str">
         <f>IF('Erreur balise introductive'!B2&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B2,"=", 'Erreur balise introductive'!C2),IF('Erreur balise introductive'!C2&lt;&gt;"",'Erreur balise introductive'!C2,""))</f>
         <v>#Message pour les erreurs de balise introductive</v>
       </c>
     </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A468" t="str">
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" t="str">
         <f>IF('Erreur balise introductive'!B3&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B3,"=", 'Erreur balise introductive'!C3),IF('Erreur balise introductive'!C3&lt;&gt;"",'Erreur balise introductive'!C3,""))</f>
         <v>window.error.missing.base.code.title=Erreurs de balises introductives</v>
       </c>
     </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" t="str">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" t="str">
         <f>IF('Erreur balise introductive'!B4&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B4,"=", 'Erreur balise introductive'!C4),IF('Erreur balise introductive'!C4&lt;&gt;"",'Erreur balise introductive'!C4,""))</f>
         <v>window.error.missing.base.code.panel.title=Liste des balises introductives</v>
       </c>
     </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" t="str">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" t="str">
         <f>IF('Erreur balise introductive'!B5&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B5,"=", 'Erreur balise introductive'!C5),IF('Erreur balise introductive'!C5&lt;&gt;"",'Erreur balise introductive'!C5,""))</f>
         <v xml:space="preserve">window.error.missing.base.code.field.label=Balise : </v>
       </c>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A471" t="str">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" t="str">
         <f>IF('Erreur balise introductive'!B6&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B6,"=", 'Erreur balise introductive'!C6),IF('Erreur balise introductive'!C6&lt;&gt;"",'Erreur balise introductive'!C6,""))</f>
         <v xml:space="preserve">window.error.missing.base.code.number.line.label=Numéro de la ligne : </v>
       </c>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" t="str">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" t="str">
         <f>IF('Erreur balise introductive'!B7&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B7,"=", 'Erreur balise introductive'!C7),IF('Erreur balise introductive'!C7&lt;&gt;"",'Erreur balise introductive'!C7,""))</f>
         <v xml:space="preserve">window.error.missing.base.code.name.file.label=Nom du fichier : </v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" t="str">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" t="str">
         <f>IF('Erreur balise introductive'!B8&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B8,"=", 'Erreur balise introductive'!C8),IF('Erreur balise introductive'!C8&lt;&gt;"",'Erreur balise introductive'!C8,""))</f>
         <v>window.error.missing.base.code.message.panel.title=Message d'information</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" t="str">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" t="str">
         <f>IF('Erreur balise introductive'!B9&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B9,"=", 'Erreur balise introductive'!C9),IF('Erreur balise introductive'!C9&lt;&gt;"",'Erreur balise introductive'!C9,""))</f>
         <v>window.error.missing.base.code.message=&lt;HTML&gt;&lt;P&gt;Des erreurs de balises introductives ont été détectées.&lt;BR/&gt;Vous devez corriger manuellement les informations sur vos documents.&lt;BR/&gt;En refermant cette fenêtre les documents se rechargeront automatiquement.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" t="str">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" t="str">
         <f>IF('Erreur balise introductive'!B10&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B10,"=", 'Erreur balise introductive'!C10),IF('Erreur balise introductive'!C10&lt;&gt;"",'Erreur balise introductive'!C10,""))</f>
         <v>window.error.missing.base.code.buttons.panel.title=Actions</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" t="str">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" t="str">
         <f>IF('Erreur balise introductive'!B11&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B11,"=", 'Erreur balise introductive'!C11),IF('Erreur balise introductive'!C11&lt;&gt;"",'Erreur balise introductive'!C11,""))</f>
         <v>window.error.missing.base.code.buttons.close.button.label=Fermer et recharger les documents</v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A477" t="str">
-        <f>IF('Erreur balise introductive'!B12&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B12,"=", 'Erreur balise introductive'!C12),IF('Erreur balise introductive'!C12&lt;&gt;"",'Erreur balise introductive'!C12,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" t="str">
-        <f>IF('Erreur balise introductive'!B13&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B13,"=", 'Erreur balise introductive'!C13),IF('Erreur balise introductive'!C13&lt;&gt;"",'Erreur balise introductive'!C13,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" t="str">
-        <f>IF('Erreur balise introductive'!B14&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B14,"=", 'Erreur balise introductive'!C14),IF('Erreur balise introductive'!C14&lt;&gt;"",'Erreur balise introductive'!C14,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A480" t="str">
-        <f>IF('Erreur balise introductive'!B15&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B15,"=", 'Erreur balise introductive'!C15),IF('Erreur balise introductive'!C15&lt;&gt;"",'Erreur balise introductive'!C15,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" t="str">
-        <f>IF('Erreur balise introductive'!B16&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B16,"=", 'Erreur balise introductive'!C16),IF('Erreur balise introductive'!C16&lt;&gt;"",'Erreur balise introductive'!C16,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A482" t="str">
-        <f>IF('Erreur balise introductive'!B17&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B17,"=", 'Erreur balise introductive'!C17),IF('Erreur balise introductive'!C17&lt;&gt;"",'Erreur balise introductive'!C17,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A483" t="str">
-        <f>IF('Erreur balise introductive'!B18&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B18,"=", 'Erreur balise introductive'!C18),IF('Erreur balise introductive'!C18&lt;&gt;"",'Erreur balise introductive'!C18,""))</f>
+        <f>IF('Erreur balise introductive'!B12&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B12,"=", 'Erreur balise introductive'!C12),IF('Erreur balise introductive'!C12&lt;&gt;"",'Erreur balise introductive'!C12,""))</f>
         <v/>
       </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A484" t="str">
-        <f>IF('Erreur balise introductive'!B19&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B19,"=", 'Erreur balise introductive'!C19),IF('Erreur balise introductive'!C19&lt;&gt;"",'Erreur balise introductive'!C19,""))</f>
+        <f>IF('Erreur balise introductive'!B13&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B13,"=", 'Erreur balise introductive'!C13),IF('Erreur balise introductive'!C13&lt;&gt;"",'Erreur balise introductive'!C13,""))</f>
         <v/>
       </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A485" t="str">
-        <f>IF('Erreur balise introductive'!B20&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B20,"=", 'Erreur balise introductive'!C20),IF('Erreur balise introductive'!C20&lt;&gt;"",'Erreur balise introductive'!C20,""))</f>
+        <f>IF('Erreur balise introductive'!B14&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B14,"=", 'Erreur balise introductive'!C14),IF('Erreur balise introductive'!C14&lt;&gt;"",'Erreur balise introductive'!C14,""))</f>
         <v/>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A486" t="str">
-        <f>IF('Erreur balise introductive'!B21&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B21,"=", 'Erreur balise introductive'!C21),IF('Erreur balise introductive'!C21&lt;&gt;"",'Erreur balise introductive'!C21,""))</f>
+        <f>IF('Erreur balise introductive'!B15&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B15,"=", 'Erreur balise introductive'!C15),IF('Erreur balise introductive'!C15&lt;&gt;"",'Erreur balise introductive'!C15,""))</f>
         <v/>
       </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A487" t="str">
-        <f>IF('Erreur balise introductive'!B22&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B22,"=", 'Erreur balise introductive'!C22),IF('Erreur balise introductive'!C22&lt;&gt;"",'Erreur balise introductive'!C22,""))</f>
+        <f>IF('Erreur balise introductive'!B16&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B16,"=", 'Erreur balise introductive'!C16),IF('Erreur balise introductive'!C16&lt;&gt;"",'Erreur balise introductive'!C16,""))</f>
         <v/>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" t="str">
-        <f>IF('Erreur balise introductive'!B23&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B23,"=", 'Erreur balise introductive'!C23),IF('Erreur balise introductive'!C23&lt;&gt;"",'Erreur balise introductive'!C23,""))</f>
+        <f>IF('Erreur balise introductive'!B17&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B17,"=", 'Erreur balise introductive'!C17),IF('Erreur balise introductive'!C17&lt;&gt;"",'Erreur balise introductive'!C17,""))</f>
         <v/>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" t="str">
-        <f>IF('Erreur balise introductive'!B24&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B24,"=", 'Erreur balise introductive'!C24),IF('Erreur balise introductive'!C24&lt;&gt;"",'Erreur balise introductive'!C24,""))</f>
+        <f>IF('Erreur balise introductive'!B18&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B18,"=", 'Erreur balise introductive'!C18),IF('Erreur balise introductive'!C18&lt;&gt;"",'Erreur balise introductive'!C18,""))</f>
         <v/>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" t="str">
-        <f>IF('Erreur balise introductive'!B25&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B25,"=", 'Erreur balise introductive'!C25),IF('Erreur balise introductive'!C25&lt;&gt;"",'Erreur balise introductive'!C25,""))</f>
+        <f>IF('Erreur balise introductive'!B19&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B19,"=", 'Erreur balise introductive'!C19),IF('Erreur balise introductive'!C19&lt;&gt;"",'Erreur balise introductive'!C19,""))</f>
         <v/>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" t="str">
-        <f>IF('Erreur balise introductive'!B26&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B26,"=", 'Erreur balise introductive'!C26),IF('Erreur balise introductive'!C26&lt;&gt;"",'Erreur balise introductive'!C26,""))</f>
+        <f>IF('Erreur balise introductive'!B20&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B20,"=", 'Erreur balise introductive'!C20),IF('Erreur balise introductive'!C20&lt;&gt;"",'Erreur balise introductive'!C20,""))</f>
         <v/>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" t="str">
-        <f>IF('Erreur balise introductive'!B27&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B27,"=", 'Erreur balise introductive'!C27),IF('Erreur balise introductive'!C27&lt;&gt;"",'Erreur balise introductive'!C27,""))</f>
+        <f>IF('Erreur balise introductive'!B21&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B21,"=", 'Erreur balise introductive'!C21),IF('Erreur balise introductive'!C21&lt;&gt;"",'Erreur balise introductive'!C21,""))</f>
         <v/>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A493" t="str">
+        <f>IF('Erreur balise introductive'!B22&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B22,"=", 'Erreur balise introductive'!C22),IF('Erreur balise introductive'!C22&lt;&gt;"",'Erreur balise introductive'!C22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" t="str">
+        <f>IF('Erreur balise introductive'!B23&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B23,"=", 'Erreur balise introductive'!C23),IF('Erreur balise introductive'!C23&lt;&gt;"",'Erreur balise introductive'!C23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" t="str">
+        <f>IF('Erreur balise introductive'!B24&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B24,"=", 'Erreur balise introductive'!C24),IF('Erreur balise introductive'!C24&lt;&gt;"",'Erreur balise introductive'!C24,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" t="str">
+        <f>IF('Erreur balise introductive'!B25&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B25,"=", 'Erreur balise introductive'!C25),IF('Erreur balise introductive'!C25&lt;&gt;"",'Erreur balise introductive'!C25,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" t="str">
+        <f>IF('Erreur balise introductive'!B26&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B26,"=", 'Erreur balise introductive'!C26),IF('Erreur balise introductive'!C26&lt;&gt;"",'Erreur balise introductive'!C26,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" t="str">
+        <f>IF('Erreur balise introductive'!B27&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B27,"=", 'Erreur balise introductive'!C27),IF('Erreur balise introductive'!C27&lt;&gt;"",'Erreur balise introductive'!C27,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" t="str">
         <f>IF('Erreur balise introductive'!B28&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B28,"=", 'Erreur balise introductive'!C28),IF('Erreur balise introductive'!C28&lt;&gt;"",'Erreur balise introductive'!C28,""))</f>
         <v/>
       </c>
@@ -30179,10 +30298,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
-  <dimension ref="A1:A495"/>
+  <dimension ref="A1:A501"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A439" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A462" sqref="A1:A495"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A340" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A353" sqref="A1:A501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32329,833 +32448,869 @@
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" t="str">
         <f>IF(Autres!B34&lt;&gt;"",CONCATENATE(Autres!B34,"=", Autres!D34),IF(Autres!D34&lt;&gt;"",Autres!D34,""))</f>
-        <v/>
+        <v>#Barra de progreso</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" t="str">
-        <f>IF(Autres!B35&lt;&gt;"",CONCATENATE(Autres!B35,"=", Autres!C35),IF(Autres!C35&lt;&gt;"",Autres!C35,""))</f>
-        <v/>
+        <f>IF(Autres!B35&lt;&gt;"",CONCATENATE(Autres!B35,"=", Autres!D35),IF(Autres!D35&lt;&gt;"",Autres!D35,""))</f>
+        <v>window.progress.bar.panel.title=Espere por favor</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" t="str">
+        <f>IF(Autres!B36&lt;&gt;"",CONCATENATE(Autres!B36,"=", Autres!D36),IF(Autres!D36&lt;&gt;"",Autres!D36,""))</f>
+        <v>window.progress.bar.load.text.label=Cargando textos….</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" t="str">
+        <f>IF(Autres!B37&lt;&gt;"",CONCATENATE(Autres!B37,"=", Autres!D37),IF(Autres!D37&lt;&gt;"",Autres!D37,""))</f>
+        <v>window.progress.bar.export.excel.label=Exportar Excel….</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" t="str">
+        <f>IF(Autres!B38&lt;&gt;"",CONCATENATE(Autres!B38,"=", Autres!D38),IF(Autres!D38&lt;&gt;"",Autres!D38,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" t="str">
+        <f>IF(Autres!B39&lt;&gt;"",CONCATENATE(Autres!B39,"=", Autres!D39),IF(Autres!D39&lt;&gt;"",Autres!D39,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" t="str">
+        <f>IF(Autres!B40&lt;&gt;"",CONCATENATE(Autres!B40,"=", Autres!D40),IF(Autres!D40&lt;&gt;"",Autres!D40,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" t="str">
+        <f>IF(Autres!B41&lt;&gt;"",CONCATENATE(Autres!B41,"=", Autres!D41),IF(Autres!D41&lt;&gt;"",Autres!D41,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" t="str">
         <f>IF('Changer Configuration'!B2&lt;&gt;"",CONCATENATE('Changer Configuration'!B2,"=", 'Changer Configuration'!D2),IF('Changer Configuration'!D2&lt;&gt;"",'Changer Configuration'!D2,""))</f>
         <v>#Mensaje para el cambio de configuración</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A360" t="str">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" t="str">
         <f>IF('Changer Configuration'!B3&lt;&gt;"",CONCATENATE('Changer Configuration'!B3,"=", 'Changer Configuration'!D3),IF('Changer Configuration'!D3&lt;&gt;"",'Changer Configuration'!D3,""))</f>
         <v>window.change.configuration.title=Configuración actual</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" t="str">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" t="str">
         <f>IF('Changer Configuration'!B4&lt;&gt;"",CONCATENATE('Changer Configuration'!B4,"=", 'Changer Configuration'!D4),IF('Changer Configuration'!D4&lt;&gt;"",'Changer Configuration'!D4,""))</f>
         <v>window.change.configuration.list.label=Configuración a utilizar :</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" t="str">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" t="str">
         <f>IF('Changer Configuration'!B5&lt;&gt;"",CONCATENATE('Changer Configuration'!B5,"=", 'Changer Configuration'!D5),IF('Changer Configuration'!D5&lt;&gt;"",'Changer Configuration'!D5,""))</f>
         <v>window.change.configuration.panel.title=Cambio de configuración</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" t="str">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" t="str">
         <f>IF('Changer Configuration'!B6&lt;&gt;"",CONCATENATE('Changer Configuration'!B6,"=", 'Changer Configuration'!D6),IF('Changer Configuration'!D6&lt;&gt;"",'Changer Configuration'!D6,""))</f>
         <v>window.change.configuration.message.panel.title=Mensaje informativo</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" t="str">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" t="str">
         <f>IF('Changer Configuration'!B7&lt;&gt;"",CONCATENATE('Changer Configuration'!B7,"=", 'Changer Configuration'!D7),IF('Changer Configuration'!D7&lt;&gt;"",'Changer Configuration'!D7,""))</f>
         <v>window.change.configuration.message.content=&lt;html&gt;&lt;p&gt;La configuración de la aplicación Caerus se basa en un archivo que le permite configurar completamente el  interfaz en función de los materiales textuales creados.&lt;br/&gt;Puede modificar la configuración de los materiales y usarlos con el interfaz de Caerus, también puede agregar , modificar o eliminar configuraciones actuando en el directorio '%s'&lt;br/&gt;Pronto se agregarán ventanas gráficas a la aplicación para facilitar sus cambios&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" t="str">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="str">
         <f>IF('Changer Configuration'!B8&lt;&gt;"",CONCATENATE('Changer Configuration'!B8,"=", 'Changer Configuration'!D8),IF('Changer Configuration'!D8&lt;&gt;"",'Changer Configuration'!D8,""))</f>
         <v>window.change.configuration.button.apply.and.close=Elija esta configuración y cerrar</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" t="str">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="str">
         <f>IF('Changer Configuration'!B9&lt;&gt;"",CONCATENATE('Changer Configuration'!B9,"=", 'Changer Configuration'!D9),IF('Changer Configuration'!D9&lt;&gt;"",'Changer Configuration'!D9,""))</f>
         <v>window.change.configuration.button.close=Cerrar</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" t="str">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="str">
         <f>IF('Changer Configuration'!B10&lt;&gt;"",CONCATENATE('Changer Configuration'!B10,"=", 'Changer Configuration'!D10),IF('Changer Configuration'!D10&lt;&gt;"",'Changer Configuration'!D10,""))</f>
         <v>window.change.configuration.buttons.panel.title=Acciones</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" t="str">
-        <f>IF('Changer Configuration'!B11&lt;&gt;"",CONCATENATE('Changer Configuration'!B11,"=", 'Changer Configuration'!D11),IF('Changer Configuration'!D11&lt;&gt;"",'Changer Configuration'!D11,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" t="str">
-        <f>IF('Changer Configuration'!B12&lt;&gt;"",CONCATENATE('Changer Configuration'!B12,"=", 'Changer Configuration'!D12),IF('Changer Configuration'!D12&lt;&gt;"",'Changer Configuration'!D12,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" t="str">
-        <f>IF('Changer Configuration'!B13&lt;&gt;"",CONCATENATE('Changer Configuration'!B13,"=", 'Changer Configuration'!D13),IF('Changer Configuration'!D13&lt;&gt;"",'Changer Configuration'!D13,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" t="str">
-        <f>IF('Changer Configuration'!B14&lt;&gt;"",CONCATENATE('Changer Configuration'!B14,"=", 'Changer Configuration'!D14),IF('Changer Configuration'!D14&lt;&gt;"",'Changer Configuration'!D14,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" t="str">
-        <f>IF('Changer Configuration'!B15&lt;&gt;"",CONCATENATE('Changer Configuration'!B15,"=", 'Changer Configuration'!D15),IF('Changer Configuration'!D15&lt;&gt;"",'Changer Configuration'!D15,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" t="str">
-        <f>IF('Changer Configuration'!B16&lt;&gt;"",CONCATENATE('Changer Configuration'!B16,"=", 'Changer Configuration'!D16),IF('Changer Configuration'!D16&lt;&gt;"",'Changer Configuration'!D16,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" t="str">
-        <f>IF('Changer Configuration'!B17&lt;&gt;"",CONCATENATE('Changer Configuration'!B17,"=", 'Changer Configuration'!D17),IF('Changer Configuration'!D17&lt;&gt;"",'Changer Configuration'!D17,""))</f>
+        <f>IF('Changer Configuration'!B11&lt;&gt;"",CONCATENATE('Changer Configuration'!B11,"=", 'Changer Configuration'!D11),IF('Changer Configuration'!D11&lt;&gt;"",'Changer Configuration'!D11,""))</f>
         <v/>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" t="str">
-        <f>IF('Changer Configuration'!B18&lt;&gt;"",CONCATENATE('Changer Configuration'!B18,"=", 'Changer Configuration'!D18),IF('Changer Configuration'!D18&lt;&gt;"",'Changer Configuration'!D18,""))</f>
+        <f>IF('Changer Configuration'!B12&lt;&gt;"",CONCATENATE('Changer Configuration'!B12,"=", 'Changer Configuration'!D12),IF('Changer Configuration'!D12&lt;&gt;"",'Changer Configuration'!D12,""))</f>
         <v/>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" t="str">
-        <f>IF('Changer Configuration'!B19&lt;&gt;"",CONCATENATE('Changer Configuration'!B19,"=", 'Changer Configuration'!D19),IF('Changer Configuration'!D19&lt;&gt;"",'Changer Configuration'!D19,""))</f>
+        <f>IF('Changer Configuration'!B13&lt;&gt;"",CONCATENATE('Changer Configuration'!B13,"=", 'Changer Configuration'!D13),IF('Changer Configuration'!D13&lt;&gt;"",'Changer Configuration'!D13,""))</f>
         <v/>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" t="str">
-        <f>IF('Changer Configuration'!B20&lt;&gt;"",CONCATENATE('Changer Configuration'!B20,"=", 'Changer Configuration'!C20),IF('Changer Configuration'!C20&lt;&gt;"",'Changer Configuration'!C20,""))</f>
+        <f>IF('Changer Configuration'!B14&lt;&gt;"",CONCATENATE('Changer Configuration'!B14,"=", 'Changer Configuration'!D14),IF('Changer Configuration'!D14&lt;&gt;"",'Changer Configuration'!D14,""))</f>
         <v/>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" t="str">
-        <f>IF('Changer Configuration'!B21&lt;&gt;"",CONCATENATE('Changer Configuration'!B21,"=", 'Changer Configuration'!C21),IF('Changer Configuration'!C21&lt;&gt;"",'Changer Configuration'!C21,""))</f>
+        <f>IF('Changer Configuration'!B15&lt;&gt;"",CONCATENATE('Changer Configuration'!B15,"=", 'Changer Configuration'!D15),IF('Changer Configuration'!D15&lt;&gt;"",'Changer Configuration'!D15,""))</f>
         <v/>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" t="str">
-        <f>IF('Changer Configuration'!B22&lt;&gt;"",CONCATENATE('Changer Configuration'!B22,"=", 'Changer Configuration'!C22),IF('Changer Configuration'!C22&lt;&gt;"",'Changer Configuration'!C22,""))</f>
+        <f>IF('Changer Configuration'!B16&lt;&gt;"",CONCATENATE('Changer Configuration'!B16,"=", 'Changer Configuration'!D16),IF('Changer Configuration'!D16&lt;&gt;"",'Changer Configuration'!D16,""))</f>
         <v/>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" t="str">
-        <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE('Changer Configuration'!B23,"=", 'Changer Configuration'!C23),IF('Changer Configuration'!C23&lt;&gt;"",'Changer Configuration'!C23,""))</f>
+        <f>IF('Changer Configuration'!B17&lt;&gt;"",CONCATENATE('Changer Configuration'!B17,"=", 'Changer Configuration'!D17),IF('Changer Configuration'!D17&lt;&gt;"",'Changer Configuration'!D17,""))</f>
         <v/>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" t="str">
+        <f>IF('Changer Configuration'!B18&lt;&gt;"",CONCATENATE('Changer Configuration'!B18,"=", 'Changer Configuration'!D18),IF('Changer Configuration'!D18&lt;&gt;"",'Changer Configuration'!D18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" t="str">
+        <f>IF('Changer Configuration'!B19&lt;&gt;"",CONCATENATE('Changer Configuration'!B19,"=", 'Changer Configuration'!D19),IF('Changer Configuration'!D19&lt;&gt;"",'Changer Configuration'!D19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" t="str">
+        <f>IF('Changer Configuration'!B20&lt;&gt;"",CONCATENATE('Changer Configuration'!B20,"=", 'Changer Configuration'!C20),IF('Changer Configuration'!C20&lt;&gt;"",'Changer Configuration'!C20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" t="str">
+        <f>IF('Changer Configuration'!B21&lt;&gt;"",CONCATENATE('Changer Configuration'!B21,"=", 'Changer Configuration'!C21),IF('Changer Configuration'!C21&lt;&gt;"",'Changer Configuration'!C21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" t="str">
+        <f>IF('Changer Configuration'!B22&lt;&gt;"",CONCATENATE('Changer Configuration'!B22,"=", 'Changer Configuration'!C22),IF('Changer Configuration'!C22&lt;&gt;"",'Changer Configuration'!C22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" t="str">
+        <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE('Changer Configuration'!B23,"=", 'Changer Configuration'!C23),IF('Changer Configuration'!C23&lt;&gt;"",'Changer Configuration'!C23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" t="str">
         <f>IF('A propos'!B2&lt;&gt;"",CONCATENATE('A propos'!B2,"=", 'A propos'!D2),IF('A propos'!D2&lt;&gt;"",'A propos'!D2,""))</f>
         <v>#Mensaje para el cambio de configuración</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" t="str">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" t="str">
         <f>IF('A propos'!B3&lt;&gt;"",CONCATENATE('A propos'!B3,"=", 'A propos'!D3),IF('A propos'!D3&lt;&gt;"",'A propos'!D3,""))</f>
         <v>window.about.title=Acerca de</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" t="str">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" t="str">
         <f>IF('A propos'!B4&lt;&gt;"",CONCATENATE('A propos'!B4,"=", 'A propos'!D4),IF('A propos'!D4&lt;&gt;"",'A propos'!D4,""))</f>
         <v>window.about.message.content=&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Acerca de la application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nombre de la application :&lt;/u&gt; Caerus&lt;BR /&gt;&lt;u&gt;Versión :&lt;/u&gt; 1.1.2&lt;br /&gt;&lt;u&gt;Editor :&lt;/u&gt; Jeremy, Leda&lt;br/&gt;&lt;u&gt;Sitio web :&lt;/u&gt; https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" t="str">
-        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE('A propos'!B5,"=", 'A propos'!D5),IF('A propos'!D5&lt;&gt;"",'A propos'!D5,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385" t="str">
-        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE('A propos'!B6,"=", 'A propos'!D6),IF('A propos'!D6&lt;&gt;"",'A propos'!D6,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" t="str">
-        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE('A propos'!B7,"=", 'A propos'!D7),IF('A propos'!D7&lt;&gt;"",'A propos'!D7,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" t="str">
-        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE('A propos'!B8,"=", 'A propos'!D8),IF('A propos'!D8&lt;&gt;"",'A propos'!D8,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" t="str">
-        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE('A propos'!B9,"=", 'A propos'!D9),IF('A propos'!D9&lt;&gt;"",'A propos'!D9,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" t="str">
-        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE('A propos'!B10,"=", 'A propos'!D10),IF('A propos'!D10&lt;&gt;"",'A propos'!D10,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A390" t="str">
-        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE('A propos'!B11,"=", 'A propos'!D11),IF('A propos'!D11&lt;&gt;"",'A propos'!D11,""))</f>
+        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE('A propos'!B5,"=", 'A propos'!D5),IF('A propos'!D5&lt;&gt;"",'A propos'!D5,""))</f>
         <v/>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" t="str">
-        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE('A propos'!B12,"=", 'A propos'!D12),IF('A propos'!D12&lt;&gt;"",'A propos'!D12,""))</f>
+        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE('A propos'!B6,"=", 'A propos'!D6),IF('A propos'!D6&lt;&gt;"",'A propos'!D6,""))</f>
         <v/>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" t="str">
-        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE('A propos'!B13,"=", 'A propos'!D13),IF('A propos'!D13&lt;&gt;"",'A propos'!D13,""))</f>
+        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE('A propos'!B7,"=", 'A propos'!D7),IF('A propos'!D7&lt;&gt;"",'A propos'!D7,""))</f>
         <v/>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" t="str">
-        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE('A propos'!B14,"=", 'A propos'!D14),IF('A propos'!D14&lt;&gt;"",'A propos'!D14,""))</f>
+        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE('A propos'!B8,"=", 'A propos'!D8),IF('A propos'!D8&lt;&gt;"",'A propos'!D8,""))</f>
         <v/>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" t="str">
-        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE('A propos'!B15,"=", 'A propos'!D15),IF('A propos'!D15&lt;&gt;"",'A propos'!D15,""))</f>
+        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE('A propos'!B9,"=", 'A propos'!D9),IF('A propos'!D9&lt;&gt;"",'A propos'!D9,""))</f>
         <v/>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" t="str">
-        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE('A propos'!B16,"=", 'A propos'!D16),IF('A propos'!D16&lt;&gt;"",'A propos'!D16,""))</f>
+        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE('A propos'!B10,"=", 'A propos'!D10),IF('A propos'!D10&lt;&gt;"",'A propos'!D10,""))</f>
         <v/>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" t="str">
-        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!D17),IF('A propos'!D17&lt;&gt;"",'A propos'!D17,""))</f>
+        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE('A propos'!B11,"=", 'A propos'!D11),IF('A propos'!D11&lt;&gt;"",'A propos'!D11,""))</f>
         <v/>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" t="str">
-        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!D18),IF('A propos'!D18&lt;&gt;"",'A propos'!D18,""))</f>
+        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE('A propos'!B12,"=", 'A propos'!D12),IF('A propos'!D12&lt;&gt;"",'A propos'!D12,""))</f>
         <v/>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" t="str">
-        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!D19),IF('A propos'!D19&lt;&gt;"",'A propos'!D19,""))</f>
+        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE('A propos'!B13,"=", 'A propos'!D13),IF('A propos'!D13&lt;&gt;"",'A propos'!D13,""))</f>
         <v/>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" t="str">
-        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!D18),IF('A propos'!D18&lt;&gt;"",'A propos'!D18,""))</f>
+        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE('A propos'!B14,"=", 'A propos'!D14),IF('A propos'!D14&lt;&gt;"",'A propos'!D14,""))</f>
         <v/>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" t="str">
-        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!D19),IF('A propos'!D19&lt;&gt;"",'A propos'!D19,""))</f>
+        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE('A propos'!B15,"=", 'A propos'!D15),IF('A propos'!D15&lt;&gt;"",'A propos'!D15,""))</f>
         <v/>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" t="str">
-        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE('A propos'!B20,"=", 'A propos'!D20),IF('A propos'!D20&lt;&gt;"",'A propos'!D20,""))</f>
+        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE('A propos'!B16,"=", 'A propos'!D16),IF('A propos'!D16&lt;&gt;"",'A propos'!D16,""))</f>
         <v/>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402" t="str">
+        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!D17),IF('A propos'!D17&lt;&gt;"",'A propos'!D17,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" t="str">
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!D18),IF('A propos'!D18&lt;&gt;"",'A propos'!D18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" t="str">
+        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!D19),IF('A propos'!D19&lt;&gt;"",'A propos'!D19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" t="str">
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!D18),IF('A propos'!D18&lt;&gt;"",'A propos'!D18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" t="str">
+        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!D19),IF('A propos'!D19&lt;&gt;"",'A propos'!D19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" t="str">
+        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE('A propos'!B20,"=", 'A propos'!D20),IF('A propos'!D20&lt;&gt;"",'A propos'!D20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" t="str">
         <f>IF('Export Document Materiel'!B2&lt;&gt;"",CONCATENATE('Export Document Materiel'!B2,"=", 'Export Document Materiel'!D2),IF('Export Document Materiel'!D2&lt;&gt;"",'Export Document Materiel'!D2,""))</f>
         <v>#Mensaje para el cambio de configuración</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" t="str">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" t="str">
         <f>IF('Export Document Materiel'!B3&lt;&gt;"",CONCATENATE('Export Document Materiel'!B3,"=", 'Export Document Materiel'!D3),IF('Export Document Materiel'!D3&lt;&gt;"",'Export Document Materiel'!D3,""))</f>
         <v>window.export.document.title=Exportar documentos/materiales</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" t="str">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" t="str">
         <f>IF('Export Document Materiel'!B4&lt;&gt;"",CONCATENATE('Export Document Materiel'!B4,"=", 'Export Document Materiel'!D4),IF('Export Document Materiel'!D4&lt;&gt;"",'Export Document Materiel'!D4,""))</f>
         <v>window.export.document.choose.directory.panel.title=Elección de la carpeta de destino</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" t="str">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" t="str">
         <f>IF('Export Document Materiel'!B5&lt;&gt;"",CONCATENATE('Export Document Materiel'!B5,"=", 'Export Document Materiel'!D5),IF('Export Document Materiel'!D5&lt;&gt;"",'Export Document Materiel'!D5,""))</f>
         <v>window.export.document.choose.directory.label=Carpeta de destino</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A406" t="str">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" t="str">
         <f>IF('Export Document Materiel'!B6&lt;&gt;"",CONCATENATE('Export Document Materiel'!B6,"=", 'Export Document Materiel'!D6),IF('Export Document Materiel'!D6&lt;&gt;"",'Export Document Materiel'!D6,""))</f>
         <v>window.export.document.mode.panel.title=Elección de los datos a exportar</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" t="str">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" t="str">
         <f>IF('Export Document Materiel'!B7&lt;&gt;"",CONCATENATE('Export Document Materiel'!B7,"=", 'Export Document Materiel'!D7),IF('Export Document Materiel'!D7&lt;&gt;"",'Export Document Materiel'!D7,""))</f>
         <v>window.export.document.mode.document.label=Un documento</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" t="str">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" t="str">
         <f>IF('Export Document Materiel'!B8&lt;&gt;"",CONCATENATE('Export Document Materiel'!B8,"=", 'Export Document Materiel'!D8),IF('Export Document Materiel'!D8&lt;&gt;"",'Export Document Materiel'!D8,""))</f>
         <v>window.export.document.mode.all.documents.label=Todos documentos</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A409" t="str">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" t="str">
         <f>IF('Export Document Materiel'!B9&lt;&gt;"",CONCATENATE('Export Document Materiel'!B9,"=", 'Export Document Materiel'!D9),IF('Export Document Materiel'!D9&lt;&gt;"",'Export Document Materiel'!D9,""))</f>
         <v>window.export.document.mode.result.search.label=El resultado de la búsqueda</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" t="str">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" t="str">
         <f>IF('Export Document Materiel'!B10&lt;&gt;"",CONCATENATE('Export Document Materiel'!B10,"=", 'Export Document Materiel'!D10),IF('Export Document Materiel'!D10&lt;&gt;"",'Export Document Materiel'!D10,""))</f>
         <v>window.export.document.choose.document.panel.title=Elección del documento a exportar</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" t="str">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" t="str">
         <f>IF('Export Document Materiel'!B11&lt;&gt;"",CONCATENATE('Export Document Materiel'!B11,"=", 'Export Document Materiel'!D11),IF('Export Document Materiel'!D11&lt;&gt;"",'Export Document Materiel'!D11,""))</f>
         <v>window.export.document.choose.document.label=Documento para exportar :</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" t="str">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="str">
         <f>IF('Export Document Materiel'!B12&lt;&gt;"",CONCATENATE('Export Document Materiel'!B12,"=", 'Export Document Materiel'!D12),IF('Export Document Materiel'!D12&lt;&gt;"",'Export Document Materiel'!D12,""))</f>
         <v>window.export.document.choose.file.panel.title=Elección del nombre del documento</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" t="str">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" t="str">
         <f>IF('Export Document Materiel'!B13&lt;&gt;"",CONCATENATE('Export Document Materiel'!B13,"=", 'Export Document Materiel'!D13),IF('Export Document Materiel'!D13&lt;&gt;"",'Export Document Materiel'!D13,""))</f>
         <v xml:space="preserve">window.export.document.choose.file.label=Nombre del documento para el resultado de la búsqueda : </v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" t="str">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" t="str">
         <f>IF('Export Document Materiel'!B14&lt;&gt;"",CONCATENATE('Export Document Materiel'!B14,"=", 'Export Document Materiel'!D14),IF('Export Document Materiel'!D14&lt;&gt;"",'Export Document Materiel'!D14,""))</f>
         <v>window.export.document.button.panel.title=Acciones</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415" t="str">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" t="str">
         <f>IF('Export Document Materiel'!B15&lt;&gt;"",CONCATENATE('Export Document Materiel'!B15,"=", 'Export Document Materiel'!D15),IF('Export Document Materiel'!D15&lt;&gt;"",'Export Document Materiel'!D15,""))</f>
         <v>window.export.document.button.export.label=Exportar y cerrar</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" t="str">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" t="str">
         <f>IF('Export Document Materiel'!B16&lt;&gt;"",CONCATENATE('Export Document Materiel'!B16,"=", 'Export Document Materiel'!D16),IF('Export Document Materiel'!D16&lt;&gt;"",'Export Document Materiel'!D16,""))</f>
         <v>window.export.document.information.message.title=Exportación completada</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" t="str">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" t="str">
         <f>IF('Export Document Materiel'!B17&lt;&gt;"",CONCATENATE('Export Document Materiel'!B17,"=", 'Export Document Materiel'!D17),IF('Export Document Materiel'!D17&lt;&gt;"",'Export Document Materiel'!D17,""))</f>
         <v>window.export.document.information.message=&lt;HTML&gt;&lt;P&gt;Exportación realizada con éxito&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418" t="str">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" t="str">
         <f>IF('Export Document Materiel'!B18&lt;&gt;"",CONCATENATE('Export Document Materiel'!B18,"=", 'Export Document Materiel'!D18),IF('Export Document Materiel'!D18&lt;&gt;"",'Export Document Materiel'!D18,""))</f>
         <v>window.export.document.button.close.label=Cerrar</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" t="str">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" t="str">
         <f>IF('Export Document Materiel'!B19&lt;&gt;"",CONCATENATE('Export Document Materiel'!B19,"=", 'Export Document Materiel'!D19),IF('Export Document Materiel'!D19&lt;&gt;"",'Export Document Materiel'!D19,""))</f>
         <v>window.export.document.choose.directory.dialog.title=Seleccione la carpeta de destino</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A420" t="str">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" t="str">
         <f>IF('Export Document Materiel'!B20&lt;&gt;"",CONCATENATE('Export Document Materiel'!B20,"=", 'Export Document Materiel'!D20),IF('Export Document Materiel'!D20&lt;&gt;"",'Export Document Materiel'!D20,""))</f>
         <v>window.export.document.information.search.message=&lt;HTML&gt;&lt;P&gt;Exportación realizada con éxito&lt;BR/&gt;A título informativo, el documento no contiene datos de cabecera&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" t="str">
-        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE('Export Document Materiel'!B21,"=", 'Export Document Materiel'!D21),IF('Export Document Materiel'!D21&lt;&gt;"",'Export Document Materiel'!D21,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" t="str">
-        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE('Export Document Materiel'!B22,"=", 'Export Document Materiel'!D22),IF('Export Document Materiel'!D22&lt;&gt;"",'Export Document Materiel'!D22,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" t="str">
-        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE('Export Document Materiel'!B23,"=", 'Export Document Materiel'!D23),IF('Export Document Materiel'!D23&lt;&gt;"",'Export Document Materiel'!D23,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" t="str">
-        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE('Export Document Materiel'!B24,"=", 'Export Document Materiel'!D24),IF('Export Document Materiel'!D24&lt;&gt;"",'Export Document Materiel'!D24,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" t="str">
-        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE('Export Document Materiel'!B25,"=", 'Export Document Materiel'!D25),IF('Export Document Materiel'!D25&lt;&gt;"",'Export Document Materiel'!D25,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" t="str">
-        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE('Export Document Materiel'!B26,"=", 'Export Document Materiel'!D26),IF('Export Document Materiel'!D26&lt;&gt;"",'Export Document Materiel'!D26,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" t="str">
-        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE('Export Document Materiel'!B27,"=", 'Export Document Materiel'!D27),IF('Export Document Materiel'!D27&lt;&gt;"",'Export Document Materiel'!D27,""))</f>
+        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE('Export Document Materiel'!B21,"=", 'Export Document Materiel'!D21),IF('Export Document Materiel'!D21&lt;&gt;"",'Export Document Materiel'!D21,""))</f>
         <v/>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428" t="str">
-        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE('Export Document Materiel'!B28,"=", 'Export Document Materiel'!D28),IF('Export Document Materiel'!D28&lt;&gt;"",'Export Document Materiel'!D28,""))</f>
+        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE('Export Document Materiel'!B22,"=", 'Export Document Materiel'!D22),IF('Export Document Materiel'!D22&lt;&gt;"",'Export Document Materiel'!D22,""))</f>
         <v/>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" t="str">
-        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE('Export Document Materiel'!B29,"=", 'Export Document Materiel'!D29),IF('Export Document Materiel'!D29&lt;&gt;"",'Export Document Materiel'!D29,""))</f>
+        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE('Export Document Materiel'!B23,"=", 'Export Document Materiel'!D23),IF('Export Document Materiel'!D23&lt;&gt;"",'Export Document Materiel'!D23,""))</f>
         <v/>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A430" t="str">
-        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE('Export Document Materiel'!B30,"=", 'Export Document Materiel'!D30),IF('Export Document Materiel'!D30&lt;&gt;"",'Export Document Materiel'!D30,""))</f>
+        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE('Export Document Materiel'!B24,"=", 'Export Document Materiel'!D24),IF('Export Document Materiel'!D24&lt;&gt;"",'Export Document Materiel'!D24,""))</f>
         <v/>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" t="str">
-        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE('Export Document Materiel'!B31,"=", 'Export Document Materiel'!D31),IF('Export Document Materiel'!D31&lt;&gt;"",'Export Document Materiel'!D31,""))</f>
+        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE('Export Document Materiel'!B25,"=", 'Export Document Materiel'!D25),IF('Export Document Materiel'!D25&lt;&gt;"",'Export Document Materiel'!D25,""))</f>
         <v/>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A432" t="str">
-        <f>IF('Export Document Materiel'!B32&lt;&gt;"",CONCATENATE('Export Document Materiel'!B32,"=", 'Export Document Materiel'!D32),IF('Export Document Materiel'!D32&lt;&gt;"",'Export Document Materiel'!D32,""))</f>
+        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE('Export Document Materiel'!B26,"=", 'Export Document Materiel'!D26),IF('Export Document Materiel'!D26&lt;&gt;"",'Export Document Materiel'!D26,""))</f>
         <v/>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" t="str">
-        <f>IF('Export Document Materiel'!B33&lt;&gt;"",CONCATENATE('Export Document Materiel'!B33,"=", 'Export Document Materiel'!D33),IF('Export Document Materiel'!D33&lt;&gt;"",'Export Document Materiel'!D33,""))</f>
+        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE('Export Document Materiel'!B27,"=", 'Export Document Materiel'!D27),IF('Export Document Materiel'!D27&lt;&gt;"",'Export Document Materiel'!D27,""))</f>
         <v/>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" t="str">
-        <f>IF('Export Document Materiel'!B34&lt;&gt;"",CONCATENATE('Export Document Materiel'!B34,"=", 'Export Document Materiel'!D34),IF('Export Document Materiel'!D34&lt;&gt;"",'Export Document Materiel'!D34,""))</f>
+        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE('Export Document Materiel'!B28,"=", 'Export Document Materiel'!D28),IF('Export Document Materiel'!D28&lt;&gt;"",'Export Document Materiel'!D28,""))</f>
         <v/>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A435" t="str">
+        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE('Export Document Materiel'!B29,"=", 'Export Document Materiel'!D29),IF('Export Document Materiel'!D29&lt;&gt;"",'Export Document Materiel'!D29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" t="str">
+        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE('Export Document Materiel'!B30,"=", 'Export Document Materiel'!D30),IF('Export Document Materiel'!D30&lt;&gt;"",'Export Document Materiel'!D30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" t="str">
+        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE('Export Document Materiel'!B31,"=", 'Export Document Materiel'!D31),IF('Export Document Materiel'!D31&lt;&gt;"",'Export Document Materiel'!D31,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" t="str">
+        <f>IF('Export Document Materiel'!B32&lt;&gt;"",CONCATENATE('Export Document Materiel'!B32,"=", 'Export Document Materiel'!D32),IF('Export Document Materiel'!D32&lt;&gt;"",'Export Document Materiel'!D32,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" t="str">
+        <f>IF('Export Document Materiel'!B33&lt;&gt;"",CONCATENATE('Export Document Materiel'!B33,"=", 'Export Document Materiel'!D33),IF('Export Document Materiel'!D33&lt;&gt;"",'Export Document Materiel'!D33,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" t="str">
+        <f>IF('Export Document Materiel'!B34&lt;&gt;"",CONCATENATE('Export Document Materiel'!B34,"=", 'Export Document Materiel'!D34),IF('Export Document Materiel'!D34&lt;&gt;"",'Export Document Materiel'!D34,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" t="str">
         <f>IF('Erreur incoherence'!B2&lt;&gt;"",CONCATENATE('Erreur incoherence'!B2,"=", 'Erreur incoherence'!D2),IF('Erreur incoherence'!D2&lt;&gt;"",'Erreur incoherence'!D2,""))</f>
         <v>#Mensaje para el cambio de configuración</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" t="str">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" t="str">
         <f>IF('Erreur incoherence'!B3&lt;&gt;"",CONCATENATE('Erreur incoherence'!B3,"=", 'Erreur incoherence'!D3),IF('Erreur incoherence'!D3&lt;&gt;"",'Erreur incoherence'!D3,""))</f>
         <v>window.error.inconsistency.title=Errores de duplicados</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437" t="str">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" t="str">
         <f>IF('Erreur incoherence'!B4&lt;&gt;"",CONCATENATE('Erreur incoherence'!B4,"=", 'Erreur incoherence'!D4),IF('Erreur incoherence'!D4&lt;&gt;"",'Erreur incoherence'!D4,""))</f>
         <v>window.error.inconsistency.panel.title=Lista de incoherencias</v>
       </c>
     </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" t="str">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" t="str">
         <f>IF('Erreur incoherence'!B5&lt;&gt;"",CONCATENATE('Erreur incoherence'!B5,"=", 'Erreur incoherence'!D5),IF('Erreur incoherence'!D5&lt;&gt;"",'Erreur incoherence'!D5,""))</f>
         <v>window.error.inconsistency.field.label=Etiqueta :</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A439" t="str">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" t="str">
         <f>IF('Erreur incoherence'!B6&lt;&gt;"",CONCATENATE('Erreur incoherence'!B6,"=", 'Erreur incoherence'!D6),IF('Erreur incoherence'!D6&lt;&gt;"",'Erreur incoherence'!D6,""))</f>
         <v>window.error.inconsistency.number.line.label=Número de línea :</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" t="str">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" t="str">
         <f>IF('Erreur incoherence'!B7&lt;&gt;"",CONCATENATE('Erreur incoherence'!B7,"=", 'Erreur incoherence'!D7),IF('Erreur incoherence'!D7&lt;&gt;"",'Erreur incoherence'!D7,""))</f>
         <v xml:space="preserve">window.error.inconsistency.name.file.label=Nombre del documento : </v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" t="str">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" t="str">
         <f>IF('Erreur incoherence'!B8&lt;&gt;"",CONCATENATE('Erreur incoherence'!B8,"=", 'Erreur incoherence'!D8),IF('Erreur incoherence'!D8&lt;&gt;"",'Erreur incoherence'!D8,""))</f>
         <v>window.error.inconsistency.message.panel.title=Mensaje informativo</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" t="str">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" t="str">
         <f>IF('Erreur incoherence'!B9&lt;&gt;"",CONCATENATE('Erreur incoherence'!B9,"=", 'Erreur incoherence'!D9),IF('Erreur incoherence'!D9&lt;&gt;"",'Erreur incoherence'!D9,""))</f>
         <v>window.error.inconsistency.message=&lt;HTML&gt;&lt;P&gt;Vuelva a cargar los documentos corregidos.&lt;BR/&gt;Los desfases de información pueden hacer&lt;BR/&gt;que se detecten nuevos errores.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" t="str">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" t="str">
         <f>IF('Erreur incoherence'!B10&lt;&gt;"",CONCATENATE('Erreur incoherence'!B10,"=", 'Erreur incoherence'!D10),IF('Erreur incoherence'!D10&lt;&gt;"",'Erreur incoherence'!D10,""))</f>
         <v>window.error.inconsistency.buttons.panel.title=Acciones</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" t="str">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" t="str">
         <f>IF('Erreur incoherence'!B11&lt;&gt;"",CONCATENATE('Erreur incoherence'!B11,"=", 'Erreur incoherence'!D11),IF('Erreur incoherence'!D11&lt;&gt;"",'Erreur incoherence'!D11,""))</f>
         <v>window.error.inconsistency.buttons.close.button.label=Cerrar y cargar lors documentos</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" t="str">
-        <f>IF('Erreur incoherence'!B12&lt;&gt;"",CONCATENATE('Erreur incoherence'!B12,"=", 'Erreur incoherence'!D12),IF('Erreur incoherence'!D12&lt;&gt;"",'Erreur incoherence'!D12,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" t="str">
-        <f>IF('Erreur incoherence'!B13&lt;&gt;"",CONCATENATE('Erreur incoherence'!B13,"=", 'Erreur incoherence'!D13),IF('Erreur incoherence'!D13&lt;&gt;"",'Erreur incoherence'!D13,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A447" t="str">
-        <f>IF('Erreur incoherence'!B14&lt;&gt;"",CONCATENATE('Erreur incoherence'!B14,"=", 'Erreur incoherence'!D14),IF('Erreur incoherence'!D14&lt;&gt;"",'Erreur incoherence'!D14,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" t="str">
-        <f>IF('Erreur incoherence'!B15&lt;&gt;"",CONCATENATE('Erreur incoherence'!B15,"=", 'Erreur incoherence'!D15),IF('Erreur incoherence'!D15&lt;&gt;"",'Erreur incoherence'!D15,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" t="str">
-        <f>IF('Erreur incoherence'!B16&lt;&gt;"",CONCATENATE('Erreur incoherence'!B16,"=", 'Erreur incoherence'!D16),IF('Erreur incoherence'!D16&lt;&gt;"",'Erreur incoherence'!D16,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" t="str">
-        <f>IF('Erreur incoherence'!B17&lt;&gt;"",CONCATENATE('Erreur incoherence'!B17,"=", 'Erreur incoherence'!D17),IF('Erreur incoherence'!D17&lt;&gt;"",'Erreur incoherence'!D17,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A451" t="str">
-        <f>IF('Erreur incoherence'!B18&lt;&gt;"",CONCATENATE('Erreur incoherence'!B18,"=", 'Erreur incoherence'!D18),IF('Erreur incoherence'!D18&lt;&gt;"",'Erreur incoherence'!D18,""))</f>
+        <f>IF('Erreur incoherence'!B12&lt;&gt;"",CONCATENATE('Erreur incoherence'!B12,"=", 'Erreur incoherence'!D12),IF('Erreur incoherence'!D12&lt;&gt;"",'Erreur incoherence'!D12,""))</f>
         <v/>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A452" t="str">
-        <f>IF('Erreur incoherence'!B19&lt;&gt;"",CONCATENATE('Erreur incoherence'!B19,"=", 'Erreur incoherence'!D19),IF('Erreur incoherence'!D19&lt;&gt;"",'Erreur incoherence'!D19,""))</f>
+        <f>IF('Erreur incoherence'!B13&lt;&gt;"",CONCATENATE('Erreur incoherence'!B13,"=", 'Erreur incoherence'!D13),IF('Erreur incoherence'!D13&lt;&gt;"",'Erreur incoherence'!D13,""))</f>
         <v/>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453" t="str">
-        <f>IF('Erreur incoherence'!B20&lt;&gt;"",CONCATENATE('Erreur incoherence'!B20,"=", 'Erreur incoherence'!D20),IF('Erreur incoherence'!D20&lt;&gt;"",'Erreur incoherence'!D20,""))</f>
+        <f>IF('Erreur incoherence'!B14&lt;&gt;"",CONCATENATE('Erreur incoherence'!B14,"=", 'Erreur incoherence'!D14),IF('Erreur incoherence'!D14&lt;&gt;"",'Erreur incoherence'!D14,""))</f>
         <v/>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A454" t="str">
-        <f>IF('Erreur incoherence'!B21&lt;&gt;"",CONCATENATE('Erreur incoherence'!B21,"=", 'Erreur incoherence'!D21),IF('Erreur incoherence'!D21&lt;&gt;"",'Erreur incoherence'!D21,""))</f>
+        <f>IF('Erreur incoherence'!B15&lt;&gt;"",CONCATENATE('Erreur incoherence'!B15,"=", 'Erreur incoherence'!D15),IF('Erreur incoherence'!D15&lt;&gt;"",'Erreur incoherence'!D15,""))</f>
         <v/>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" t="str">
-        <f>IF('Erreur incoherence'!B22&lt;&gt;"",CONCATENATE('Erreur incoherence'!B22,"=", 'Erreur incoherence'!D22),IF('Erreur incoherence'!D22&lt;&gt;"",'Erreur incoherence'!D22,""))</f>
+        <f>IF('Erreur incoherence'!B16&lt;&gt;"",CONCATENATE('Erreur incoherence'!B16,"=", 'Erreur incoherence'!D16),IF('Erreur incoherence'!D16&lt;&gt;"",'Erreur incoherence'!D16,""))</f>
         <v/>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A456" t="str">
-        <f>IF('Erreur incoherence'!B23&lt;&gt;"",CONCATENATE('Erreur incoherence'!B23,"=", 'Erreur incoherence'!D23),IF('Erreur incoherence'!D23&lt;&gt;"",'Erreur incoherence'!D23,""))</f>
+        <f>IF('Erreur incoherence'!B17&lt;&gt;"",CONCATENATE('Erreur incoherence'!B17,"=", 'Erreur incoherence'!D17),IF('Erreur incoherence'!D17&lt;&gt;"",'Erreur incoherence'!D17,""))</f>
         <v/>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A457" t="str">
-        <f>IF('Erreur incoherence'!B24&lt;&gt;"",CONCATENATE('Erreur incoherence'!B24,"=", 'Erreur incoherence'!D24),IF('Erreur incoherence'!D24&lt;&gt;"",'Erreur incoherence'!D24,""))</f>
+        <f>IF('Erreur incoherence'!B18&lt;&gt;"",CONCATENATE('Erreur incoherence'!B18,"=", 'Erreur incoherence'!D18),IF('Erreur incoherence'!D18&lt;&gt;"",'Erreur incoherence'!D18,""))</f>
         <v/>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" t="str">
-        <f>IF('Erreur incoherence'!B25&lt;&gt;"",CONCATENATE('Erreur incoherence'!B25,"=", 'Erreur incoherence'!D25),IF('Erreur incoherence'!D25&lt;&gt;"",'Erreur incoherence'!D25,""))</f>
+        <f>IF('Erreur incoherence'!B19&lt;&gt;"",CONCATENATE('Erreur incoherence'!B19,"=", 'Erreur incoherence'!D19),IF('Erreur incoherence'!D19&lt;&gt;"",'Erreur incoherence'!D19,""))</f>
         <v/>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" t="str">
-        <f>IF('Erreur incoherence'!B26&lt;&gt;"",CONCATENATE('Erreur incoherence'!B26,"=", 'Erreur incoherence'!D26),IF('Erreur incoherence'!D26&lt;&gt;"",'Erreur incoherence'!D26,""))</f>
+        <f>IF('Erreur incoherence'!B20&lt;&gt;"",CONCATENATE('Erreur incoherence'!B20,"=", 'Erreur incoherence'!D20),IF('Erreur incoherence'!D20&lt;&gt;"",'Erreur incoherence'!D20,""))</f>
         <v/>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" t="str">
-        <f>IF('Erreur incoherence'!B27&lt;&gt;"",CONCATENATE('Erreur incoherence'!B27,"=", 'Erreur incoherence'!D27),IF('Erreur incoherence'!D27&lt;&gt;"",'Erreur incoherence'!D27,""))</f>
+        <f>IF('Erreur incoherence'!B21&lt;&gt;"",CONCATENATE('Erreur incoherence'!B21,"=", 'Erreur incoherence'!D21),IF('Erreur incoherence'!D21&lt;&gt;"",'Erreur incoherence'!D21,""))</f>
         <v/>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" t="str">
-        <f>IF('Erreur incoherence'!B28&lt;&gt;"",CONCATENATE('Erreur incoherence'!B28,"=", 'Erreur incoherence'!D28),IF('Erreur incoherence'!D28&lt;&gt;"",'Erreur incoherence'!D28,""))</f>
+        <f>IF('Erreur incoherence'!B22&lt;&gt;"",CONCATENATE('Erreur incoherence'!B22,"=", 'Erreur incoherence'!D22),IF('Erreur incoherence'!D22&lt;&gt;"",'Erreur incoherence'!D22,""))</f>
         <v/>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" t="str">
-        <f>IF('Erreur incoherence'!B29&lt;&gt;"",CONCATENATE('Erreur incoherence'!B29,"=", 'Erreur incoherence'!D29),IF('Erreur incoherence'!D29&lt;&gt;"",'Erreur incoherence'!D29,""))</f>
+        <f>IF('Erreur incoherence'!B23&lt;&gt;"",CONCATENATE('Erreur incoherence'!B23,"=", 'Erreur incoherence'!D23),IF('Erreur incoherence'!D23&lt;&gt;"",'Erreur incoherence'!D23,""))</f>
         <v/>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A463" t="str">
-        <f>IF('Erreur incoherence'!B30&lt;&gt;"",CONCATENATE('Erreur incoherence'!B30,"=", 'Erreur incoherence'!D30),IF('Erreur incoherence'!D30&lt;&gt;"",'Erreur incoherence'!D30,""))</f>
+        <f>IF('Erreur incoherence'!B24&lt;&gt;"",CONCATENATE('Erreur incoherence'!B24,"=", 'Erreur incoherence'!D24),IF('Erreur incoherence'!D24&lt;&gt;"",'Erreur incoherence'!D24,""))</f>
         <v/>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" t="str">
-        <f>IF('Erreur incoherence'!B31&lt;&gt;"",CONCATENATE('Erreur incoherence'!B31,"=", 'Erreur incoherence'!D31),IF('Erreur incoherence'!D31&lt;&gt;"",'Erreur incoherence'!D31,""))</f>
+        <f>IF('Erreur incoherence'!B25&lt;&gt;"",CONCATENATE('Erreur incoherence'!B25,"=", 'Erreur incoherence'!D25),IF('Erreur incoherence'!D25&lt;&gt;"",'Erreur incoherence'!D25,""))</f>
         <v/>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A465" t="str">
-        <f>IF('Erreur incoherence'!B32&lt;&gt;"",CONCATENATE('Erreur incoherence'!B32,"=", 'Erreur incoherence'!D32),IF('Erreur incoherence'!D32&lt;&gt;"",'Erreur incoherence'!D32,""))</f>
+        <f>IF('Erreur incoherence'!B26&lt;&gt;"",CONCATENATE('Erreur incoherence'!B26,"=", 'Erreur incoherence'!D26),IF('Erreur incoherence'!D26&lt;&gt;"",'Erreur incoherence'!D26,""))</f>
         <v/>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466" t="str">
+        <f>IF('Erreur incoherence'!B27&lt;&gt;"",CONCATENATE('Erreur incoherence'!B27,"=", 'Erreur incoherence'!D27),IF('Erreur incoherence'!D27&lt;&gt;"",'Erreur incoherence'!D27,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" t="str">
+        <f>IF('Erreur incoherence'!B28&lt;&gt;"",CONCATENATE('Erreur incoherence'!B28,"=", 'Erreur incoherence'!D28),IF('Erreur incoherence'!D28&lt;&gt;"",'Erreur incoherence'!D28,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" t="str">
+        <f>IF('Erreur incoherence'!B29&lt;&gt;"",CONCATENATE('Erreur incoherence'!B29,"=", 'Erreur incoherence'!D29),IF('Erreur incoherence'!D29&lt;&gt;"",'Erreur incoherence'!D29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" t="str">
+        <f>IF('Erreur incoherence'!B30&lt;&gt;"",CONCATENATE('Erreur incoherence'!B30,"=", 'Erreur incoherence'!D30),IF('Erreur incoherence'!D30&lt;&gt;"",'Erreur incoherence'!D30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" t="str">
+        <f>IF('Erreur incoherence'!B31&lt;&gt;"",CONCATENATE('Erreur incoherence'!B31,"=", 'Erreur incoherence'!D31),IF('Erreur incoherence'!D31&lt;&gt;"",'Erreur incoherence'!D31,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" t="str">
+        <f>IF('Erreur incoherence'!B32&lt;&gt;"",CONCATENATE('Erreur incoherence'!B32,"=", 'Erreur incoherence'!D32),IF('Erreur incoherence'!D32&lt;&gt;"",'Erreur incoherence'!D32,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" t="str">
         <f>IF('Erreur balise introductive'!B2&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B2,"=", 'Erreur balise introductive'!D2),IF('Erreur balise introductive'!D2&lt;&gt;"",'Erreur balise introductive'!D2,""))</f>
         <v>#Mensaje para etiquetas introductoria</v>
       </c>
     </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" t="str">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" t="str">
         <f>IF('Erreur balise introductive'!B3&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B3,"=", 'Erreur balise introductive'!D3),IF('Erreur balise introductive'!D3&lt;&gt;"",'Erreur balise introductive'!D3,""))</f>
         <v>window.error.missing.base.code.title=Errores de etiquetas introductorias</v>
       </c>
     </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A468" t="str">
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" t="str">
         <f>IF('Erreur balise introductive'!B4&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B4,"=", 'Erreur balise introductive'!D4),IF('Erreur balise introductive'!D4&lt;&gt;"",'Erreur balise introductive'!D4,""))</f>
         <v>window.error.missing.base.code.panel.title=Lista de etiquetas introductorias</v>
       </c>
     </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" t="str">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" t="str">
         <f>IF('Erreur balise introductive'!B5&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B5,"=", 'Erreur balise introductive'!D5),IF('Erreur balise introductive'!D5&lt;&gt;"",'Erreur balise introductive'!D5,""))</f>
         <v>window.error.missing.base.code.field.label=Etiqueta :</v>
       </c>
     </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" t="str">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" t="str">
         <f>IF('Erreur balise introductive'!B6&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B6,"=", 'Erreur balise introductive'!D6),IF('Erreur balise introductive'!D6&lt;&gt;"",'Erreur balise introductive'!D6,""))</f>
         <v>window.error.missing.base.code.number.line.label=Número de línea :</v>
       </c>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A471" t="str">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" t="str">
         <f>IF('Erreur balise introductive'!B7&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B7,"=", 'Erreur balise introductive'!D7),IF('Erreur balise introductive'!D7&lt;&gt;"",'Erreur balise introductive'!D7,""))</f>
         <v xml:space="preserve">window.error.missing.base.code.name.file.label=Nombre del documento : </v>
       </c>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" t="str">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" t="str">
         <f>IF('Erreur balise introductive'!B8&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B8,"=", 'Erreur balise introductive'!D8),IF('Erreur balise introductive'!D8&lt;&gt;"",'Erreur balise introductive'!D8,""))</f>
         <v>window.error.missing.base.code.message.panel.title=Mensaje informativo</v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" t="str">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" t="str">
         <f>IF('Erreur balise introductive'!B9&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B9,"=", 'Erreur balise introductive'!D9),IF('Erreur balise introductive'!D9&lt;&gt;"",'Erreur balise introductive'!D9,""))</f>
         <v>window.error.missing.base.code.message=&lt;HTML&gt;&lt;P&gt;Se han detectado errores en las etiquetas de introducción.&lt;BR/&gt;Debe corregir manualmente la información directamente en sus documentos.&lt;BR/&gt;Al cerrar esta ventana, los documentos se recargarán automáticamente.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" t="str">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" t="str">
         <f>IF('Erreur balise introductive'!B10&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B10,"=", 'Erreur balise introductive'!D10),IF('Erreur balise introductive'!D10&lt;&gt;"",'Erreur balise introductive'!D10,""))</f>
         <v>window.error.missing.base.code.buttons.panel.title=Acciones</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" t="str">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" t="str">
         <f>IF('Erreur balise introductive'!B11&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B11,"=", 'Erreur balise introductive'!D11),IF('Erreur balise introductive'!D11&lt;&gt;"",'Erreur balise introductive'!D11,""))</f>
         <v>window.error.missing.base.code.buttons.close.button.label=Cerrar y cargar lors documentos</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" t="str">
-        <f>IF('Erreur balise introductive'!B12&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B12,"=", 'Erreur balise introductive'!D12),IF('Erreur balise introductive'!D12&lt;&gt;"",'Erreur balise introductive'!D12,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A477" t="str">
-        <f>IF('Erreur balise introductive'!B13&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B13,"=", 'Erreur balise introductive'!D13),IF('Erreur balise introductive'!D13&lt;&gt;"",'Erreur balise introductive'!D13,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" t="str">
-        <f>IF('Erreur balise introductive'!B14&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B14,"=", 'Erreur balise introductive'!D14),IF('Erreur balise introductive'!D14&lt;&gt;"",'Erreur balise introductive'!D14,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" t="str">
-        <f>IF('Erreur balise introductive'!B15&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B15,"=", 'Erreur balise introductive'!D15),IF('Erreur balise introductive'!D15&lt;&gt;"",'Erreur balise introductive'!D15,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A480" t="str">
-        <f>IF('Erreur balise introductive'!B16&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B16,"=", 'Erreur balise introductive'!D16),IF('Erreur balise introductive'!D16&lt;&gt;"",'Erreur balise introductive'!D16,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" t="str">
-        <f>IF('Erreur balise introductive'!B17&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B17,"=", 'Erreur balise introductive'!D17),IF('Erreur balise introductive'!D17&lt;&gt;"",'Erreur balise introductive'!D17,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482" t="str">
-        <f>IF('Erreur balise introductive'!B18&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B18,"=", 'Erreur balise introductive'!D18),IF('Erreur balise introductive'!D18&lt;&gt;"",'Erreur balise introductive'!D18,""))</f>
+        <f>IF('Erreur balise introductive'!B12&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B12,"=", 'Erreur balise introductive'!D12),IF('Erreur balise introductive'!D12&lt;&gt;"",'Erreur balise introductive'!D12,""))</f>
         <v/>
       </c>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A483" t="str">
-        <f>IF('Erreur balise introductive'!B19&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B19,"=", 'Erreur balise introductive'!D19),IF('Erreur balise introductive'!D19&lt;&gt;"",'Erreur balise introductive'!D19,""))</f>
+        <f>IF('Erreur balise introductive'!B13&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B13,"=", 'Erreur balise introductive'!D13),IF('Erreur balise introductive'!D13&lt;&gt;"",'Erreur balise introductive'!D13,""))</f>
         <v/>
       </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A484" t="str">
-        <f>IF('Erreur balise introductive'!B20&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B20,"=", 'Erreur balise introductive'!D20),IF('Erreur balise introductive'!D20&lt;&gt;"",'Erreur balise introductive'!D20,""))</f>
+        <f>IF('Erreur balise introductive'!B14&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B14,"=", 'Erreur balise introductive'!D14),IF('Erreur balise introductive'!D14&lt;&gt;"",'Erreur balise introductive'!D14,""))</f>
         <v/>
       </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A485" t="str">
-        <f>IF('Erreur balise introductive'!B21&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B21,"=", 'Erreur balise introductive'!D21),IF('Erreur balise introductive'!D21&lt;&gt;"",'Erreur balise introductive'!D21,""))</f>
+        <f>IF('Erreur balise introductive'!B15&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B15,"=", 'Erreur balise introductive'!D15),IF('Erreur balise introductive'!D15&lt;&gt;"",'Erreur balise introductive'!D15,""))</f>
         <v/>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A486" t="str">
-        <f>IF('Erreur balise introductive'!B22&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B22,"=", 'Erreur balise introductive'!D22),IF('Erreur balise introductive'!D22&lt;&gt;"",'Erreur balise introductive'!D22,""))</f>
+        <f>IF('Erreur balise introductive'!B16&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B16,"=", 'Erreur balise introductive'!D16),IF('Erreur balise introductive'!D16&lt;&gt;"",'Erreur balise introductive'!D16,""))</f>
         <v/>
       </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A487" t="str">
-        <f>IF('Erreur balise introductive'!B23&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B23,"=", 'Erreur balise introductive'!D23),IF('Erreur balise introductive'!D23&lt;&gt;"",'Erreur balise introductive'!D23,""))</f>
+        <f>IF('Erreur balise introductive'!B17&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B17,"=", 'Erreur balise introductive'!D17),IF('Erreur balise introductive'!D17&lt;&gt;"",'Erreur balise introductive'!D17,""))</f>
         <v/>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" t="str">
-        <f>IF('Erreur balise introductive'!B24&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B24,"=", 'Erreur balise introductive'!D24),IF('Erreur balise introductive'!D24&lt;&gt;"",'Erreur balise introductive'!D24,""))</f>
+        <f>IF('Erreur balise introductive'!B18&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B18,"=", 'Erreur balise introductive'!D18),IF('Erreur balise introductive'!D18&lt;&gt;"",'Erreur balise introductive'!D18,""))</f>
         <v/>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" t="str">
-        <f>IF('Erreur balise introductive'!B25&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B25,"=", 'Erreur balise introductive'!D25),IF('Erreur balise introductive'!D25&lt;&gt;"",'Erreur balise introductive'!D25,""))</f>
+        <f>IF('Erreur balise introductive'!B19&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B19,"=", 'Erreur balise introductive'!D19),IF('Erreur balise introductive'!D19&lt;&gt;"",'Erreur balise introductive'!D19,""))</f>
         <v/>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" t="str">
-        <f>IF('Erreur balise introductive'!B26&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B26,"=", 'Erreur balise introductive'!D26),IF('Erreur balise introductive'!D26&lt;&gt;"",'Erreur balise introductive'!D26,""))</f>
+        <f>IF('Erreur balise introductive'!B20&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B20,"=", 'Erreur balise introductive'!D20),IF('Erreur balise introductive'!D20&lt;&gt;"",'Erreur balise introductive'!D20,""))</f>
         <v/>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" t="str">
-        <f>IF('Erreur balise introductive'!B27&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B27,"=", 'Erreur balise introductive'!D27),IF('Erreur balise introductive'!D27&lt;&gt;"",'Erreur balise introductive'!D27,""))</f>
+        <f>IF('Erreur balise introductive'!B21&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B21,"=", 'Erreur balise introductive'!D21),IF('Erreur balise introductive'!D21&lt;&gt;"",'Erreur balise introductive'!D21,""))</f>
         <v/>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" t="str">
-        <f>IF('Erreur balise introductive'!B28&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B28,"=", 'Erreur balise introductive'!D28),IF('Erreur balise introductive'!D28&lt;&gt;"",'Erreur balise introductive'!D28,""))</f>
+        <f>IF('Erreur balise introductive'!B22&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B22,"=", 'Erreur balise introductive'!D22),IF('Erreur balise introductive'!D22&lt;&gt;"",'Erreur balise introductive'!D22,""))</f>
         <v/>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A493" t="str">
-        <f>IF('Erreur balise introductive'!B29&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B29,"=", 'Erreur balise introductive'!D29),IF('Erreur balise introductive'!D29&lt;&gt;"",'Erreur balise introductive'!D29,""))</f>
+        <f>IF('Erreur balise introductive'!B23&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B23,"=", 'Erreur balise introductive'!D23),IF('Erreur balise introductive'!D23&lt;&gt;"",'Erreur balise introductive'!D23,""))</f>
         <v/>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A494" t="str">
-        <f>IF('Erreur balise introductive'!B30&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B30,"=", 'Erreur balise introductive'!D30),IF('Erreur balise introductive'!D30&lt;&gt;"",'Erreur balise introductive'!D30,""))</f>
+        <f>IF('Erreur balise introductive'!B24&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B24,"=", 'Erreur balise introductive'!D24),IF('Erreur balise introductive'!D24&lt;&gt;"",'Erreur balise introductive'!D24,""))</f>
         <v/>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A495" t="str">
+        <f>IF('Erreur balise introductive'!B25&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B25,"=", 'Erreur balise introductive'!D25),IF('Erreur balise introductive'!D25&lt;&gt;"",'Erreur balise introductive'!D25,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" t="str">
+        <f>IF('Erreur balise introductive'!B26&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B26,"=", 'Erreur balise introductive'!D26),IF('Erreur balise introductive'!D26&lt;&gt;"",'Erreur balise introductive'!D26,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" t="str">
+        <f>IF('Erreur balise introductive'!B27&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B27,"=", 'Erreur balise introductive'!D27),IF('Erreur balise introductive'!D27&lt;&gt;"",'Erreur balise introductive'!D27,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" t="str">
+        <f>IF('Erreur balise introductive'!B28&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B28,"=", 'Erreur balise introductive'!D28),IF('Erreur balise introductive'!D28&lt;&gt;"",'Erreur balise introductive'!D28,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" t="str">
+        <f>IF('Erreur balise introductive'!B29&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B29,"=", 'Erreur balise introductive'!D29),IF('Erreur balise introductive'!D29&lt;&gt;"",'Erreur balise introductive'!D29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" t="str">
+        <f>IF('Erreur balise introductive'!B30&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B30,"=", 'Erreur balise introductive'!D30),IF('Erreur balise introductive'!D30&lt;&gt;"",'Erreur balise introductive'!D30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" t="str">
         <f>IF('Erreur balise introductive'!B31&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B31,"=", 'Erreur balise introductive'!D31),IF('Erreur balise introductive'!D31&lt;&gt;"",'Erreur balise introductive'!D31,""))</f>
         <v/>
       </c>
@@ -33167,10 +33322,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
-  <dimension ref="A1:A491"/>
+  <dimension ref="A1:A496"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A338" workbookViewId="0">
+      <selection activeCell="A357" sqref="A357:A359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35317,809 +35472,839 @@
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" t="str">
         <f>IF(Autres!B35&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B35),".","_"),"=""", Autres!B35,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_PROGRESS_BAR_PANEL_TITLE="window.progress.bar.panel.title";</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" t="str">
-        <f>IF('Changer Configuration'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B2),".","_"),"=""", 'Changer Configuration'!B2,""";"),"")</f>
-        <v/>
+        <f>IF(Autres!B36&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B36),".","_"),"=""", Autres!B36,""";"),"")</f>
+        <v>public static final String WINDOW_PROGRESS_BAR_LOAD_TEXT_LABEL="window.progress.bar.load.text.label";</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" t="str">
+        <f>IF(Autres!B37&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B37),".","_"),"=""", Autres!B37,""";"),"")</f>
+        <v>public static final String WINDOW_PROGRESS_BAR_EXPORT_EXCEL_LABEL="window.progress.bar.export.excel.label";</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" t="str">
+        <f>IF(Autres!B38&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B38),".","_"),"=""", Autres!B38,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" t="str">
+        <f>IF(Autres!B39&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B39),".","_"),"=""", Autres!B39,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" t="str">
+        <f>IF(Autres!B40&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B40),".","_"),"=""", Autres!B40,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" t="str">
+        <f>IF('Changer Configuration'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B2),".","_"),"=""", 'Changer Configuration'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" t="str">
         <f>IF('Changer Configuration'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B3),".","_"),"=""", 'Changer Configuration'!B3,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_TITLE="window.change.configuration.title";</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A360" t="str">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" t="str">
         <f>IF('Changer Configuration'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B4),".","_"),"=""", 'Changer Configuration'!B4,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_LIST_LABEL="window.change.configuration.list.label";</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" t="str">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" t="str">
         <f>IF('Changer Configuration'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B5),".","_"),"=""", 'Changer Configuration'!B5,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_PANEL_TITLE="window.change.configuration.panel.title";</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" t="str">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" t="str">
         <f>IF('Changer Configuration'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B6),".","_"),"=""", 'Changer Configuration'!B6,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_MESSAGE_PANEL_TITLE="window.change.configuration.message.panel.title";</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" t="str">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" t="str">
         <f>IF('Changer Configuration'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B7),".","_"),"=""", 'Changer Configuration'!B7,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_MESSAGE_CONTENT="window.change.configuration.message.content";</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" t="str">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" t="str">
         <f>IF('Changer Configuration'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B8),".","_"),"=""", 'Changer Configuration'!B8,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_BUTTON_APPLY_AND_CLOSE="window.change.configuration.button.apply.and.close";</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" t="str">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" t="str">
         <f>IF('Changer Configuration'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B9),".","_"),"=""", 'Changer Configuration'!B9,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_BUTTON_CLOSE="window.change.configuration.button.close";</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" t="str">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="str">
         <f>IF('Changer Configuration'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B10),".","_"),"=""", 'Changer Configuration'!B10,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_BUTTONS_PANEL_TITLE="window.change.configuration.buttons.panel.title";</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" t="str">
-        <f>IF('Changer Configuration'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B11),".","_"),"=""", 'Changer Configuration'!B11,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" t="str">
-        <f>IF('Changer Configuration'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B12),".","_"),"=""", 'Changer Configuration'!B12,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" t="str">
-        <f>IF('Changer Configuration'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B13),".","_"),"=""", 'Changer Configuration'!B13,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" t="str">
-        <f>IF('Changer Configuration'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B14),".","_"),"=""", 'Changer Configuration'!B14,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" t="str">
-        <f>IF('Changer Configuration'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B15),".","_"),"=""", 'Changer Configuration'!B15,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" t="str">
-        <f>IF('Changer Configuration'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B16),".","_"),"=""", 'Changer Configuration'!B16,""";"),"")</f>
+        <f>IF('Changer Configuration'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B11),".","_"),"=""", 'Changer Configuration'!B11,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" t="str">
-        <f>IF('Changer Configuration'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B17),".","_"),"=""", 'Changer Configuration'!B17,""";"),"")</f>
+        <f>IF('Changer Configuration'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B12),".","_"),"=""", 'Changer Configuration'!B12,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" t="str">
-        <f>IF('Changer Configuration'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B18),".","_"),"=""", 'Changer Configuration'!B18,""";"),"")</f>
+        <f>IF('Changer Configuration'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B13),".","_"),"=""", 'Changer Configuration'!B13,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" t="str">
-        <f>IF('Changer Configuration'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B19),".","_"),"=""", 'Changer Configuration'!B19,""";"),"")</f>
+        <f>IF('Changer Configuration'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B14),".","_"),"=""", 'Changer Configuration'!B14,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" t="str">
-        <f>IF('Changer Configuration'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B20),".","_"),"=""", 'Changer Configuration'!B20,""";"),"")</f>
+        <f>IF('Changer Configuration'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B15),".","_"),"=""", 'Changer Configuration'!B15,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" t="str">
-        <f>IF('Changer Configuration'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B21),".","_"),"=""", 'Changer Configuration'!B21,""";"),"")</f>
+        <f>IF('Changer Configuration'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B16),".","_"),"=""", 'Changer Configuration'!B16,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" t="str">
-        <f>IF('Changer Configuration'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B22),".","_"),"=""", 'Changer Configuration'!B22,""";"),"")</f>
+        <f>IF('Changer Configuration'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B17),".","_"),"=""", 'Changer Configuration'!B17,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" t="str">
-        <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B23),".","_"),"=""", 'Changer Configuration'!B23,""";"),"")</f>
+        <f>IF('Changer Configuration'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B18),".","_"),"=""", 'Changer Configuration'!B18,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" t="str">
-        <f>IF('A propos'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B2),".","_"),"=""", 'A propos'!B2,""";"),"")</f>
+        <f>IF('Changer Configuration'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B19),".","_"),"=""", 'Changer Configuration'!B19,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" t="str">
+        <f>IF('Changer Configuration'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B20),".","_"),"=""", 'Changer Configuration'!B20,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" t="str">
+        <f>IF('Changer Configuration'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B21),".","_"),"=""", 'Changer Configuration'!B21,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" t="str">
+        <f>IF('Changer Configuration'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B22),".","_"),"=""", 'Changer Configuration'!B22,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" t="str">
+        <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B23),".","_"),"=""", 'Changer Configuration'!B23,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" t="str">
+        <f>IF('A propos'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B2),".","_"),"=""", 'A propos'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" t="str">
         <f>IF('A propos'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B3),".","_"),"=""", 'A propos'!B3,""";"),"")</f>
         <v>public static final String WINDOW_ABOUT_TITLE="window.about.title";</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" t="str">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" t="str">
         <f>IF('A propos'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B4),".","_"),"=""", 'A propos'!B4,""";"),"")</f>
         <v>public static final String WINDOW_ABOUT_MESSAGE_CONTENT="window.about.message.content";</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" t="str">
-        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B5),".","_"),"=""", 'A propos'!B5,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" t="str">
-        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B6),".","_"),"=""", 'A propos'!B6,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385" t="str">
-        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B7),".","_"),"=""", 'A propos'!B7,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" t="str">
-        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B8),".","_"),"=""", 'A propos'!B8,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" t="str">
-        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B9),".","_"),"=""", 'A propos'!B9,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388" t="str">
-        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B10),".","_"),"=""", 'A propos'!B10,""";"),"")</f>
+        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B5),".","_"),"=""", 'A propos'!B5,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" t="str">
-        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B11),".","_"),"=""", 'A propos'!B11,""";"),"")</f>
+        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B6),".","_"),"=""", 'A propos'!B6,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A390" t="str">
-        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B12),".","_"),"=""", 'A propos'!B12,""";"),"")</f>
+        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B7),".","_"),"=""", 'A propos'!B7,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" t="str">
-        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B13),".","_"),"=""", 'A propos'!B13,""";"),"")</f>
+        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B8),".","_"),"=""", 'A propos'!B8,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" t="str">
-        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B14),".","_"),"=""", 'A propos'!B14,""";"),"")</f>
+        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B9),".","_"),"=""", 'A propos'!B9,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" t="str">
-        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B15),".","_"),"=""", 'A propos'!B15,""";"),"")</f>
+        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B10),".","_"),"=""", 'A propos'!B10,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" t="str">
-        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B16),".","_"),"=""", 'A propos'!B16,""";"),"")</f>
+        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B11),".","_"),"=""", 'A propos'!B11,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" t="str">
-        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B17),".","_"),"=""", 'A propos'!B17,""";"),"")</f>
+        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B12),".","_"),"=""", 'A propos'!B12,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" t="str">
-        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B18),".","_"),"=""", 'A propos'!B18,""";"),"")</f>
+        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B13),".","_"),"=""", 'A propos'!B13,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" t="str">
-        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B19),".","_"),"=""", 'A propos'!B19,""";"),"")</f>
+        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B14),".","_"),"=""", 'A propos'!B14,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" t="str">
-        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B20),".","_"),"=""", 'A propos'!B20,""";"),"")</f>
+        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B15),".","_"),"=""", 'A propos'!B15,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" t="str">
-        <f>IF('A propos'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B21),".","_"),"=""", 'A propos'!B21,""";"),"")</f>
+        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B16),".","_"),"=""", 'A propos'!B16,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" t="str">
-        <f>IF('A propos'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B22),".","_"),"=""", 'A propos'!B22,""";"),"")</f>
+        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B17),".","_"),"=""", 'A propos'!B17,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" t="str">
-        <f>IF('A propos'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B23),".","_"),"=""", 'A propos'!B23,""";"),"")</f>
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B18),".","_"),"=""", 'A propos'!B18,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402" t="str">
-        <f>IF('A propos'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B24),".","_"),"=""", 'A propos'!B24,""";"),"")</f>
+        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B19),".","_"),"=""", 'A propos'!B19,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" t="str">
-        <f>IF('Export Document Materiel'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B2),".","_"),"=""", 'Export Document Materiel'!B2,""";"),"")</f>
+        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B20),".","_"),"=""", 'A propos'!B20,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" t="str">
+        <f>IF('A propos'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B21),".","_"),"=""", 'A propos'!B21,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" t="str">
+        <f>IF('A propos'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B22),".","_"),"=""", 'A propos'!B22,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" t="str">
+        <f>IF('A propos'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B23),".","_"),"=""", 'A propos'!B23,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" t="str">
+        <f>IF('A propos'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B24),".","_"),"=""", 'A propos'!B24,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" t="str">
+        <f>IF('Export Document Materiel'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B2),".","_"),"=""", 'Export Document Materiel'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" t="str">
         <f>IF('Export Document Materiel'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B3),".","_"),"=""", 'Export Document Materiel'!B3,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_TITLE="window.export.document.title";</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" t="str">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" t="str">
         <f>IF('Export Document Materiel'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B4),".","_"),"=""", 'Export Document Materiel'!B4,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DIRECTORY_PANEL_TITLE="window.export.document.choose.directory.panel.title";</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A406" t="str">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" t="str">
         <f>IF('Export Document Materiel'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B5),".","_"),"=""", 'Export Document Materiel'!B5,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DIRECTORY_LABEL="window.export.document.choose.directory.label";</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" t="str">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" t="str">
         <f>IF('Export Document Materiel'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B6),".","_"),"=""", 'Export Document Materiel'!B6,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_MODE_PANEL_TITLE="window.export.document.mode.panel.title";</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" t="str">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" t="str">
         <f>IF('Export Document Materiel'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B7),".","_"),"=""", 'Export Document Materiel'!B7,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_MODE_DOCUMENT_LABEL="window.export.document.mode.document.label";</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A409" t="str">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" t="str">
         <f>IF('Export Document Materiel'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B8),".","_"),"=""", 'Export Document Materiel'!B8,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_MODE_ALL_DOCUMENTS_LABEL="window.export.document.mode.all.documents.label";</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" t="str">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" t="str">
         <f>IF('Export Document Materiel'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B9),".","_"),"=""", 'Export Document Materiel'!B9,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_MODE_RESULT_SEARCH_LABEL="window.export.document.mode.result.search.label";</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" t="str">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" t="str">
         <f>IF('Export Document Materiel'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B10),".","_"),"=""", 'Export Document Materiel'!B10,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DOCUMENT_PANEL_TITLE="window.export.document.choose.document.panel.title";</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" t="str">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" t="str">
         <f>IF('Export Document Materiel'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B11),".","_"),"=""", 'Export Document Materiel'!B11,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DOCUMENT_LABEL="window.export.document.choose.document.label";</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" t="str">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="str">
         <f>IF('Export Document Materiel'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B12),".","_"),"=""", 'Export Document Materiel'!B12,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_FILE_PANEL_TITLE="window.export.document.choose.file.panel.title";</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" t="str">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" t="str">
         <f>IF('Export Document Materiel'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B13),".","_"),"=""", 'Export Document Materiel'!B13,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_FILE_LABEL="window.export.document.choose.file.label";</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415" t="str">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" t="str">
         <f>IF('Export Document Materiel'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B14),".","_"),"=""", 'Export Document Materiel'!B14,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_BUTTON_PANEL_TITLE="window.export.document.button.panel.title";</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" t="str">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" t="str">
         <f>IF('Export Document Materiel'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B15),".","_"),"=""", 'Export Document Materiel'!B15,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_BUTTON_EXPORT_LABEL="window.export.document.button.export.label";</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" t="str">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" t="str">
         <f>IF('Export Document Materiel'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B16),".","_"),"=""", 'Export Document Materiel'!B16,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_INFORMATION_MESSAGE_TITLE="window.export.document.information.message.title";</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418" t="str">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" t="str">
         <f>IF('Export Document Materiel'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B17),".","_"),"=""", 'Export Document Materiel'!B17,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_INFORMATION_MESSAGE="window.export.document.information.message";</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" t="str">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" t="str">
         <f>IF('Export Document Materiel'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B18),".","_"),"=""", 'Export Document Materiel'!B18,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_BUTTON_CLOSE_LABEL="window.export.document.button.close.label";</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A420" t="str">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" t="str">
         <f>IF('Export Document Materiel'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B19),".","_"),"=""", 'Export Document Materiel'!B19,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DIRECTORY_DIALOG_TITLE="window.export.document.choose.directory.dialog.title";</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" t="str">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" t="str">
         <f>IF('Export Document Materiel'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B20),".","_"),"=""", 'Export Document Materiel'!B20,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_INFORMATION_SEARCH_MESSAGE="window.export.document.information.search.message";</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" t="str">
-        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B21),".","_"),"=""", 'Export Document Materiel'!B21,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" t="str">
-        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B22),".","_"),"=""", 'Export Document Materiel'!B22,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" t="str">
-        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B23),".","_"),"=""", 'Export Document Materiel'!B23,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" t="str">
-        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B24),".","_"),"=""", 'Export Document Materiel'!B24,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" t="str">
-        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B25),".","_"),"=""", 'Export Document Materiel'!B25,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" t="str">
-        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B26),".","_"),"=""", 'Export Document Materiel'!B26,""";"),"")</f>
+        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B21),".","_"),"=""", 'Export Document Materiel'!B21,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428" t="str">
-        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B27),".","_"),"=""", 'Export Document Materiel'!B27,""";"),"")</f>
+        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B22),".","_"),"=""", 'Export Document Materiel'!B22,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" t="str">
-        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B28),".","_"),"=""", 'Export Document Materiel'!B28,""";"),"")</f>
+        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B23),".","_"),"=""", 'Export Document Materiel'!B23,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A430" t="str">
-        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B29),".","_"),"=""", 'Export Document Materiel'!B29,""";"),"")</f>
+        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B24),".","_"),"=""", 'Export Document Materiel'!B24,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" t="str">
-        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B30),".","_"),"=""", 'Export Document Materiel'!B30,""";"),"")</f>
+        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B25),".","_"),"=""", 'Export Document Materiel'!B25,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A432" t="str">
-        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B31),".","_"),"=""", 'Export Document Materiel'!B31,""";"),"")</f>
+        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B26),".","_"),"=""", 'Export Document Materiel'!B26,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" t="str">
-        <f>IF('Erreur incoherence'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B2),".","_"),"=""", 'Erreur incoherence'!B2,""";"),"")</f>
+        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B27),".","_"),"=""", 'Export Document Materiel'!B27,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" t="str">
+        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B28),".","_"),"=""", 'Export Document Materiel'!B28,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" t="str">
+        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B29),".","_"),"=""", 'Export Document Materiel'!B29,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" t="str">
+        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B30),".","_"),"=""", 'Export Document Materiel'!B30,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" t="str">
+        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B31),".","_"),"=""", 'Export Document Materiel'!B31,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" t="str">
+        <f>IF('Erreur incoherence'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B2),".","_"),"=""", 'Erreur incoherence'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" t="str">
         <f>IF('Erreur incoherence'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B3),".","_"),"=""", 'Erreur incoherence'!B3,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_TITLE="window.error.inconsistency.title";</v>
       </c>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A435" t="str">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" t="str">
         <f>IF('Erreur incoherence'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B4),".","_"),"=""", 'Erreur incoherence'!B4,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_PANEL_TITLE="window.error.inconsistency.panel.title";</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" t="str">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" t="str">
         <f>IF('Erreur incoherence'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B5),".","_"),"=""", 'Erreur incoherence'!B5,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_FIELD_LABEL="window.error.inconsistency.field.label";</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437" t="str">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" t="str">
         <f>IF('Erreur incoherence'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B6),".","_"),"=""", 'Erreur incoherence'!B6,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_NUMBER_LINE_LABEL="window.error.inconsistency.number.line.label";</v>
       </c>
     </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" t="str">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" t="str">
         <f>IF('Erreur incoherence'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B7),".","_"),"=""", 'Erreur incoherence'!B7,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_NAME_FILE_LABEL="window.error.inconsistency.name.file.label";</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A439" t="str">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" t="str">
         <f>IF('Erreur incoherence'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B8),".","_"),"=""", 'Erreur incoherence'!B8,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_MESSAGE_PANEL_TITLE="window.error.inconsistency.message.panel.title";</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" t="str">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" t="str">
         <f>IF('Erreur incoherence'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B9),".","_"),"=""", 'Erreur incoherence'!B9,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_MESSAGE="window.error.inconsistency.message";</v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" t="str">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" t="str">
         <f>IF('Erreur incoherence'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B10),".","_"),"=""", 'Erreur incoherence'!B10,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_BUTTONS_PANEL_TITLE="window.error.inconsistency.buttons.panel.title";</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" t="str">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" t="str">
         <f>IF('Erreur incoherence'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B11),".","_"),"=""", 'Erreur incoherence'!B11,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_BUTTONS_CLOSE_BUTTON_LABEL="window.error.inconsistency.buttons.close.button.label";</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" t="str">
-        <f>IF('Erreur incoherence'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B12),".","_"),"=""", 'Erreur incoherence'!B12,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" t="str">
-        <f>IF('Erreur incoherence'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B13),".","_"),"=""", 'Erreur incoherence'!B13,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" t="str">
-        <f>IF('Erreur incoherence'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B14),".","_"),"=""", 'Erreur incoherence'!B14,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" t="str">
-        <f>IF('Erreur incoherence'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B15),".","_"),"=""", 'Erreur incoherence'!B15,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A447" t="str">
-        <f>IF('Erreur incoherence'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B16),".","_"),"=""", 'Erreur incoherence'!B16,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A448" t="str">
-        <f>IF('Erreur incoherence'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B17),".","_"),"=""", 'Erreur incoherence'!B17,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B12),".","_"),"=""", 'Erreur incoherence'!B12,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A449" t="str">
-        <f>IF('Erreur incoherence'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B18),".","_"),"=""", 'Erreur incoherence'!B18,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B13),".","_"),"=""", 'Erreur incoherence'!B13,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A450" t="str">
-        <f>IF('Erreur incoherence'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B19),".","_"),"=""", 'Erreur incoherence'!B19,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B14),".","_"),"=""", 'Erreur incoherence'!B14,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A451" t="str">
-        <f>IF('Erreur incoherence'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B20),".","_"),"=""", 'Erreur incoherence'!B20,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B15),".","_"),"=""", 'Erreur incoherence'!B15,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A452" t="str">
-        <f>IF('Erreur incoherence'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B21),".","_"),"=""", 'Erreur incoherence'!B21,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B16),".","_"),"=""", 'Erreur incoherence'!B16,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453" t="str">
-        <f>IF('Erreur incoherence'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B22),".","_"),"=""", 'Erreur incoherence'!B22,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B17),".","_"),"=""", 'Erreur incoherence'!B17,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A454" t="str">
-        <f>IF('Erreur incoherence'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B23),".","_"),"=""", 'Erreur incoherence'!B23,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B18),".","_"),"=""", 'Erreur incoherence'!B18,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" t="str">
-        <f>IF('Erreur incoherence'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B24),".","_"),"=""", 'Erreur incoherence'!B24,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B19),".","_"),"=""", 'Erreur incoherence'!B19,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A456" t="str">
-        <f>IF('Erreur incoherence'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B25),".","_"),"=""", 'Erreur incoherence'!B25,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B20),".","_"),"=""", 'Erreur incoherence'!B20,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A457" t="str">
-        <f>IF('Erreur incoherence'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B26),".","_"),"=""", 'Erreur incoherence'!B26,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B21),".","_"),"=""", 'Erreur incoherence'!B21,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" t="str">
-        <f>IF('Erreur incoherence'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B27),".","_"),"=""", 'Erreur incoherence'!B27,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B22),".","_"),"=""", 'Erreur incoherence'!B22,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" t="str">
-        <f>IF('Erreur incoherence'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B28),".","_"),"=""", 'Erreur incoherence'!B28,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B23),".","_"),"=""", 'Erreur incoherence'!B23,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" t="str">
-        <f>IF('Erreur incoherence'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B29),".","_"),"=""", 'Erreur incoherence'!B29,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B24),".","_"),"=""", 'Erreur incoherence'!B24,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" t="str">
-        <f>IF('Erreur incoherence'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B30),".","_"),"=""", 'Erreur incoherence'!B30,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B25),".","_"),"=""", 'Erreur incoherence'!B25,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" t="str">
-        <f>IF('Erreur incoherence'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B31),".","_"),"=""", 'Erreur incoherence'!B31,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B26),".","_"),"=""", 'Erreur incoherence'!B26,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A463" t="str">
-        <f>IF('Erreur incoherence'!B32&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B32),".","_"),"=""", 'Erreur incoherence'!B32,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B27),".","_"),"=""", 'Erreur incoherence'!B27,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" t="str">
-        <f>IF('Erreur balise introductive'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B2),".","_"),"=""", 'Erreur balise introductive'!B2,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B28),".","_"),"=""", 'Erreur incoherence'!B28,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A465" t="str">
+        <f>IF('Erreur incoherence'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B29),".","_"),"=""", 'Erreur incoherence'!B29,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" t="str">
+        <f>IF('Erreur incoherence'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B30),".","_"),"=""", 'Erreur incoherence'!B30,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" t="str">
+        <f>IF('Erreur incoherence'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B31),".","_"),"=""", 'Erreur incoherence'!B31,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" t="str">
+        <f>IF('Erreur incoherence'!B32&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B32),".","_"),"=""", 'Erreur incoherence'!B32,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" t="str">
+        <f>IF('Erreur balise introductive'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B2),".","_"),"=""", 'Erreur balise introductive'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" t="str">
         <f>IF('Erreur balise introductive'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B3),".","_"),"=""", 'Erreur balise introductive'!B3,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_TITLE="window.error.missing.base.code.title";</v>
       </c>
     </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466" t="str">
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" t="str">
         <f>IF('Erreur balise introductive'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B4),".","_"),"=""", 'Erreur balise introductive'!B4,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_PANEL_TITLE="window.error.missing.base.code.panel.title";</v>
       </c>
     </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" t="str">
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" t="str">
         <f>IF('Erreur balise introductive'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B5),".","_"),"=""", 'Erreur balise introductive'!B5,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_FIELD_LABEL="window.error.missing.base.code.field.label";</v>
       </c>
     </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A468" t="str">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" t="str">
         <f>IF('Erreur balise introductive'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B6),".","_"),"=""", 'Erreur balise introductive'!B6,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_NUMBER_LINE_LABEL="window.error.missing.base.code.number.line.label";</v>
       </c>
     </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" t="str">
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" t="str">
         <f>IF('Erreur balise introductive'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B7),".","_"),"=""", 'Erreur balise introductive'!B7,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_NAME_FILE_LABEL="window.error.missing.base.code.name.file.label";</v>
       </c>
     </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" t="str">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" t="str">
         <f>IF('Erreur balise introductive'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B8),".","_"),"=""", 'Erreur balise introductive'!B8,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_MESSAGE_PANEL_TITLE="window.error.missing.base.code.message.panel.title";</v>
       </c>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A471" t="str">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" t="str">
         <f>IF('Erreur balise introductive'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B9),".","_"),"=""", 'Erreur balise introductive'!B9,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_MESSAGE="window.error.missing.base.code.message";</v>
       </c>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" t="str">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" t="str">
         <f>IF('Erreur balise introductive'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B10),".","_"),"=""", 'Erreur balise introductive'!B10,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_BUTTONS_PANEL_TITLE="window.error.missing.base.code.buttons.panel.title";</v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" t="str">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" t="str">
         <f>IF('Erreur balise introductive'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B11),".","_"),"=""", 'Erreur balise introductive'!B11,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_BUTTONS_CLOSE_BUTTON_LABEL="window.error.missing.base.code.buttons.close.button.label";</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" t="str">
-        <f>IF('Erreur balise introductive'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B12),".","_"),"=""", 'Erreur balise introductive'!B12,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" t="str">
-        <f>IF('Erreur balise introductive'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B13),".","_"),"=""", 'Erreur balise introductive'!B13,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" t="str">
-        <f>IF('Erreur balise introductive'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B14),".","_"),"=""", 'Erreur balise introductive'!B14,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A477" t="str">
-        <f>IF('Erreur balise introductive'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B15),".","_"),"=""", 'Erreur balise introductive'!B15,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" t="str">
-        <f>IF('Erreur balise introductive'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B16),".","_"),"=""", 'Erreur balise introductive'!B16,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A479" t="str">
-        <f>IF('Erreur balise introductive'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B17),".","_"),"=""", 'Erreur balise introductive'!B17,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B12),".","_"),"=""", 'Erreur balise introductive'!B12,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A480" t="str">
-        <f>IF('Erreur balise introductive'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B18),".","_"),"=""", 'Erreur balise introductive'!B18,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B13),".","_"),"=""", 'Erreur balise introductive'!B13,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A481" t="str">
-        <f>IF('Erreur balise introductive'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B19),".","_"),"=""", 'Erreur balise introductive'!B19,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B14),".","_"),"=""", 'Erreur balise introductive'!B14,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482" t="str">
-        <f>IF('Erreur balise introductive'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B20),".","_"),"=""", 'Erreur balise introductive'!B20,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B15),".","_"),"=""", 'Erreur balise introductive'!B15,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A483" t="str">
-        <f>IF('Erreur balise introductive'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B21),".","_"),"=""", 'Erreur balise introductive'!B21,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B16),".","_"),"=""", 'Erreur balise introductive'!B16,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A484" t="str">
-        <f>IF('Erreur balise introductive'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B22),".","_"),"=""", 'Erreur balise introductive'!B22,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B17),".","_"),"=""", 'Erreur balise introductive'!B17,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A485" t="str">
-        <f>IF('Erreur balise introductive'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B23),".","_"),"=""", 'Erreur balise introductive'!B23,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B18),".","_"),"=""", 'Erreur balise introductive'!B18,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A486" t="str">
-        <f>IF('Erreur balise introductive'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B24),".","_"),"=""", 'Erreur balise introductive'!B24,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B19),".","_"),"=""", 'Erreur balise introductive'!B19,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A487" t="str">
-        <f>IF('Erreur balise introductive'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B25),".","_"),"=""", 'Erreur balise introductive'!B25,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B20),".","_"),"=""", 'Erreur balise introductive'!B20,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" t="str">
-        <f>IF('Erreur balise introductive'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B26),".","_"),"=""", 'Erreur balise introductive'!B26,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B21),".","_"),"=""", 'Erreur balise introductive'!B21,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" t="str">
-        <f>IF('Erreur balise introductive'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B27),".","_"),"=""", 'Erreur balise introductive'!B27,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B22),".","_"),"=""", 'Erreur balise introductive'!B22,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" t="str">
-        <f>IF('Erreur balise introductive'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B28),".","_"),"=""", 'Erreur balise introductive'!B28,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B23),".","_"),"=""", 'Erreur balise introductive'!B23,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" t="str">
+        <f>IF('Erreur balise introductive'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B24),".","_"),"=""", 'Erreur balise introductive'!B24,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" t="str">
+        <f>IF('Erreur balise introductive'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B25),".","_"),"=""", 'Erreur balise introductive'!B25,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" t="str">
+        <f>IF('Erreur balise introductive'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B26),".","_"),"=""", 'Erreur balise introductive'!B26,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" t="str">
+        <f>IF('Erreur balise introductive'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B27),".","_"),"=""", 'Erreur balise introductive'!B27,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" t="str">
+        <f>IF('Erreur balise introductive'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B28),".","_"),"=""", 'Erreur balise introductive'!B28,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" t="str">
         <f>IF('Erreur balise introductive'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B29),".","_"),"=""", 'Erreur balise introductive'!B29,""";"),"")</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Ajout du système de gestion du lancement d'une seule instance
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\git\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB81D6F-A13A-468D-9818-1ACDA13CFAA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C7429F-29E6-4A76-8871-61ACC243A9F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="13" activeTab="19" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="14" activeTab="18" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="764">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -2276,12 +2276,6 @@
     <t>Biblioteca</t>
   </si>
   <si>
-    <t>Consulter / Editer matériels</t>
-  </si>
-  <si>
-    <t>Consultar / Editar materiales</t>
-  </si>
-  <si>
     <t>#Barre de progression</t>
   </si>
   <si>
@@ -2313,6 +2307,36 @@
   </si>
   <si>
     <t>Exportar Excel….</t>
+  </si>
+  <si>
+    <t>Consultar / Editar</t>
+  </si>
+  <si>
+    <t>Consulter / Éditer</t>
+  </si>
+  <si>
+    <t>#Message si l'application est lancé plus d'une fois</t>
+  </si>
+  <si>
+    <t>window.alert.more.one.caerus.launch.message.title</t>
+  </si>
+  <si>
+    <t>window.alert.more.one.caerus.launch.message.content</t>
+  </si>
+  <si>
+    <t>Attention</t>
+  </si>
+  <si>
+    <t>#Mensaje si la aplicación se inicia más de una vez</t>
+  </si>
+  <si>
+    <t>Atención</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;&lt;p&gt;Caerus est déjà executé.&lt;br/&gt;Vous ne pouvez pas executer Caerus plus d'une fois.&lt;/p&gt;&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;&lt;p&gt;Caerus ya se está ejecutando.&lt;br/&gt;No puede ejecutar Caerus más de una vez.&lt;/p&gt;&lt;/html&gt;</t>
   </si>
 </sst>
 </file>
@@ -23623,8 +23647,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{028E31B7-3FC3-4143-B5FF-43FD17AAB26D}" name="Tableau16" displayName="Tableau16" ref="A1:D40" totalsRowShown="0">
-  <autoFilter ref="A1:D40" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{028E31B7-3FC3-4143-B5FF-43FD17AAB26D}" name="Tableau16" displayName="Tableau16" ref="A1:D41" totalsRowShown="0">
+  <autoFilter ref="A1:D41" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{EE0F9B50-F787-4253-A164-BB17836F12B4}" name="Numero"/>
     <tableColumn id="2" xr3:uid="{58CBB508-E960-4269-90E7-903193963B86}" name="Code"/>
@@ -24104,7 +24128,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24334,10 +24358,10 @@
         <v>365</v>
       </c>
       <c r="C19" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="D19" t="s">
-        <v>744</v>
+        <v>754</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -25491,10 +25515,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B861A8A-1131-4099-83D4-ECA745EBF0ED}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25834,10 +25858,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="D34" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -25845,13 +25869,13 @@
         <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C35" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="D35" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -25859,13 +25883,13 @@
         <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C36" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D36" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -25873,13 +25897,49 @@
         <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C37" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D37" t="s">
-        <v>755</v>
+        <v>753</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>756</v>
+      </c>
+      <c r="D39" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>22</v>
+      </c>
+      <c r="B40" t="s">
+        <v>757</v>
+      </c>
+      <c r="C40" t="s">
+        <v>759</v>
+      </c>
+      <c r="D40" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>23</v>
+      </c>
+      <c r="B41" t="s">
+        <v>758</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>763</v>
       </c>
     </row>
   </sheetData>
@@ -26842,10 +26902,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904B2FA-CBC2-495A-A197-D0CDD47EB1AE}">
-  <dimension ref="A1:A499"/>
+  <dimension ref="A1:A504"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A358" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A378" sqref="A1:A499"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A343" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A368" sqref="A1:A504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26958,7 +27018,7 @@
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF('Fenêtre principal'!B19&lt;&gt;"",CONCATENATE('Fenêtre principal'!B19,"=", 'Fenêtre principal'!C19),IF('Fenêtre principal'!C19&lt;&gt;"",'Fenêtre principal'!C19,""))</f>
-        <v>window.menu.level5.sublevel3.title=Consulter / Editer matériels</v>
+        <v>window.menu.level5.sublevel3.title=Consulter / Éditer</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -29022,827 +29082,857 @@
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" t="str">
         <f>IF(Autres!B39&lt;&gt;"",CONCATENATE(Autres!B39,"=", Autres!C39),IF(Autres!C39&lt;&gt;"",Autres!C39,""))</f>
-        <v/>
+        <v>#Message si l'application est lancé plus d'une fois</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" t="str">
         <f>IF(Autres!B40&lt;&gt;"",CONCATENATE(Autres!B40,"=", Autres!C40),IF(Autres!C40&lt;&gt;"",Autres!C40,""))</f>
-        <v/>
+        <v>window.alert.more.one.caerus.launch.message.title=Attention</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" t="str">
         <f>IF(Autres!B41&lt;&gt;"",CONCATENATE(Autres!B41,"=", Autres!C41),IF(Autres!C41&lt;&gt;"",Autres!C41,""))</f>
-        <v/>
+        <v>window.alert.more.one.caerus.launch.message.content=&lt;html&gt;&lt;p&gt;Caerus est déjà executé.&lt;br/&gt;Vous ne pouvez pas executer Caerus plus d'une fois.&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" t="str">
+        <f>IF(Autres!B42&lt;&gt;"",CONCATENATE(Autres!B42,"=", Autres!C42),IF(Autres!C42&lt;&gt;"",Autres!C42,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" t="str">
+        <f>IF(Autres!B43&lt;&gt;"",CONCATENATE(Autres!B43,"=", Autres!C43),IF(Autres!C43&lt;&gt;"",Autres!C43,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" t="str">
+        <f>IF(Autres!B44&lt;&gt;"",CONCATENATE(Autres!B44,"=", Autres!C44),IF(Autres!C44&lt;&gt;"",Autres!C44,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" t="str">
+        <f>IF(Autres!B45&lt;&gt;"",CONCATENATE(Autres!B45,"=", Autres!C45),IF(Autres!C45&lt;&gt;"",Autres!C45,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" t="str">
+        <f>IF(Autres!B46&lt;&gt;"",CONCATENATE(Autres!B46,"=", Autres!C46),IF(Autres!C46&lt;&gt;"",Autres!C46,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" t="str">
         <f>IF('Changer Configuration'!B2&lt;&gt;"",CONCATENATE('Changer Configuration'!B2,"=", 'Changer Configuration'!C2),IF('Changer Configuration'!C2&lt;&gt;"",'Changer Configuration'!C2,""))</f>
         <v>#Message pour le changement de la configuration</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" t="str">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="str">
         <f>IF('Changer Configuration'!B3&lt;&gt;"",CONCATENATE('Changer Configuration'!B3,"=", 'Changer Configuration'!C3),IF('Changer Configuration'!C3&lt;&gt;"",'Changer Configuration'!C3,""))</f>
         <v>window.change.configuration.title=Configuration courante</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" t="str">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="str">
         <f>IF('Changer Configuration'!B4&lt;&gt;"",CONCATENATE('Changer Configuration'!B4,"=", 'Changer Configuration'!C4),IF('Changer Configuration'!C4&lt;&gt;"",'Changer Configuration'!C4,""))</f>
         <v>window.change.configuration.list.label=Configuration à utiliser :</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" t="str">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="str">
         <f>IF('Changer Configuration'!B5&lt;&gt;"",CONCATENATE('Changer Configuration'!B5,"=", 'Changer Configuration'!C5),IF('Changer Configuration'!C5&lt;&gt;"",'Changer Configuration'!C5,""))</f>
         <v>window.change.configuration.panel.title=Changement de la configuration</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" t="str">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" t="str">
         <f>IF('Changer Configuration'!B6&lt;&gt;"",CONCATENATE('Changer Configuration'!B6,"=", 'Changer Configuration'!C6),IF('Changer Configuration'!C6&lt;&gt;"",'Changer Configuration'!C6,""))</f>
         <v>window.change.configuration.message.panel.title=Message d'information</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" t="str">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" t="str">
         <f>IF('Changer Configuration'!B7&lt;&gt;"",CONCATENATE('Changer Configuration'!B7,"=", 'Changer Configuration'!C7),IF('Changer Configuration'!C7&lt;&gt;"",'Changer Configuration'!C7,""))</f>
         <v>window.change.configuration.message.content=&lt;html&gt;&lt;p&gt;La configuration de l’application Caerus est basée sur un fichier qui vous permet de configurer complètement l’interface en fonction des matériels textuels créés.&lt;br/&gt;Vous pouvez modifier la configuration des matériels et les utiliser avec l'interface de Caerus, vous pouvez également ajouter , modifier ou supprimer les paramètres en agissant dans le répertoire '%s'&lt;br/&gt;Des fenêtres graphiques seront bientôt ajoutées à l’application pour faciliter vos modifications&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" t="str">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" t="str">
         <f>IF('Changer Configuration'!B8&lt;&gt;"",CONCATENATE('Changer Configuration'!B8,"=", 'Changer Configuration'!C8),IF('Changer Configuration'!C8&lt;&gt;"",'Changer Configuration'!C8,""))</f>
         <v>window.change.configuration.button.apply.and.close=Choisir cette configuration et fermer</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" t="str">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" t="str">
         <f>IF('Changer Configuration'!B9&lt;&gt;"",CONCATENATE('Changer Configuration'!B9,"=", 'Changer Configuration'!C9),IF('Changer Configuration'!C9&lt;&gt;"",'Changer Configuration'!C9,""))</f>
         <v>window.change.configuration.button.close=Fermer</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" t="str">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" t="str">
         <f>IF('Changer Configuration'!B10&lt;&gt;"",CONCATENATE('Changer Configuration'!B10,"=", 'Changer Configuration'!C10),IF('Changer Configuration'!C10&lt;&gt;"",'Changer Configuration'!C10,""))</f>
         <v>window.change.configuration.buttons.panel.title=Actions</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" t="str">
-        <f>IF('Changer Configuration'!B11&lt;&gt;"",CONCATENATE('Changer Configuration'!B11,"=", 'Changer Configuration'!C11),IF('Changer Configuration'!C11&lt;&gt;"",'Changer Configuration'!C11,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" t="str">
-        <f>IF('Changer Configuration'!B12&lt;&gt;"",CONCATENATE('Changer Configuration'!B12,"=", 'Changer Configuration'!C12),IF('Changer Configuration'!C12&lt;&gt;"",'Changer Configuration'!C12,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" t="str">
-        <f>IF('Changer Configuration'!B13&lt;&gt;"",CONCATENATE('Changer Configuration'!B13,"=", 'Changer Configuration'!C13),IF('Changer Configuration'!C13&lt;&gt;"",'Changer Configuration'!C13,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" t="str">
-        <f>IF('Changer Configuration'!B14&lt;&gt;"",CONCATENATE('Changer Configuration'!B14,"=", 'Changer Configuration'!C14),IF('Changer Configuration'!C14&lt;&gt;"",'Changer Configuration'!C14,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A378" t="str">
-        <f>IF('Changer Configuration'!B15&lt;&gt;"",CONCATENATE('Changer Configuration'!B15,"=", 'Changer Configuration'!C15),IF('Changer Configuration'!C15&lt;&gt;"",'Changer Configuration'!C15,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" t="str">
-        <f>IF('Changer Configuration'!B16&lt;&gt;"",CONCATENATE('Changer Configuration'!B16,"=", 'Changer Configuration'!C16),IF('Changer Configuration'!C16&lt;&gt;"",'Changer Configuration'!C16,""))</f>
+        <f>IF('Changer Configuration'!B11&lt;&gt;"",CONCATENATE('Changer Configuration'!B11,"=", 'Changer Configuration'!C11),IF('Changer Configuration'!C11&lt;&gt;"",'Changer Configuration'!C11,""))</f>
         <v/>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" t="str">
-        <f>IF('Changer Configuration'!B17&lt;&gt;"",CONCATENATE('Changer Configuration'!B17,"=", 'Changer Configuration'!C17),IF('Changer Configuration'!C17&lt;&gt;"",'Changer Configuration'!C17,""))</f>
+        <f>IF('Changer Configuration'!B12&lt;&gt;"",CONCATENATE('Changer Configuration'!B12,"=", 'Changer Configuration'!C12),IF('Changer Configuration'!C12&lt;&gt;"",'Changer Configuration'!C12,""))</f>
         <v/>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" t="str">
-        <f>IF('Changer Configuration'!B18&lt;&gt;"",CONCATENATE('Changer Configuration'!B18,"=", 'Changer Configuration'!C18),IF('Changer Configuration'!C18&lt;&gt;"",'Changer Configuration'!C18,""))</f>
+        <f>IF('Changer Configuration'!B13&lt;&gt;"",CONCATENATE('Changer Configuration'!B13,"=", 'Changer Configuration'!C13),IF('Changer Configuration'!C13&lt;&gt;"",'Changer Configuration'!C13,""))</f>
         <v/>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" t="str">
-        <f>IF('Changer Configuration'!B19&lt;&gt;"",CONCATENATE('Changer Configuration'!B19,"=", 'Changer Configuration'!C19),IF('Changer Configuration'!C19&lt;&gt;"",'Changer Configuration'!C19,""))</f>
+        <f>IF('Changer Configuration'!B14&lt;&gt;"",CONCATENATE('Changer Configuration'!B14,"=", 'Changer Configuration'!C14),IF('Changer Configuration'!C14&lt;&gt;"",'Changer Configuration'!C14,""))</f>
         <v/>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" t="str">
-        <f>IF('Changer Configuration'!B20&lt;&gt;"",CONCATENATE('Changer Configuration'!B20,"=", 'Changer Configuration'!C20),IF('Changer Configuration'!C20&lt;&gt;"",'Changer Configuration'!C20,""))</f>
+        <f>IF('Changer Configuration'!B15&lt;&gt;"",CONCATENATE('Changer Configuration'!B15,"=", 'Changer Configuration'!C15),IF('Changer Configuration'!C15&lt;&gt;"",'Changer Configuration'!C15,""))</f>
         <v/>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" t="str">
-        <f>IF('Changer Configuration'!B21&lt;&gt;"",CONCATENATE('Changer Configuration'!B21,"=", 'Changer Configuration'!C21),IF('Changer Configuration'!C21&lt;&gt;"",'Changer Configuration'!C21,""))</f>
+        <f>IF('Changer Configuration'!B16&lt;&gt;"",CONCATENATE('Changer Configuration'!B16,"=", 'Changer Configuration'!C16),IF('Changer Configuration'!C16&lt;&gt;"",'Changer Configuration'!C16,""))</f>
         <v/>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" t="str">
-        <f>IF('Changer Configuration'!B22&lt;&gt;"",CONCATENATE('Changer Configuration'!B22,"=", 'Changer Configuration'!C22),IF('Changer Configuration'!C22&lt;&gt;"",'Changer Configuration'!C22,""))</f>
+        <f>IF('Changer Configuration'!B17&lt;&gt;"",CONCATENATE('Changer Configuration'!B17,"=", 'Changer Configuration'!C17),IF('Changer Configuration'!C17&lt;&gt;"",'Changer Configuration'!C17,""))</f>
         <v/>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" t="str">
-        <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE('Changer Configuration'!B23,"=", 'Changer Configuration'!C23),IF('Changer Configuration'!C23&lt;&gt;"",'Changer Configuration'!C23,""))</f>
+        <f>IF('Changer Configuration'!B18&lt;&gt;"",CONCATENATE('Changer Configuration'!B18,"=", 'Changer Configuration'!C18),IF('Changer Configuration'!C18&lt;&gt;"",'Changer Configuration'!C18,""))</f>
         <v/>
       </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A387" t="str">
+        <f>IF('Changer Configuration'!B19&lt;&gt;"",CONCATENATE('Changer Configuration'!B19,"=", 'Changer Configuration'!C19),IF('Changer Configuration'!C19&lt;&gt;"",'Changer Configuration'!C19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" t="str">
+        <f>IF('Changer Configuration'!B20&lt;&gt;"",CONCATENATE('Changer Configuration'!B20,"=", 'Changer Configuration'!C20),IF('Changer Configuration'!C20&lt;&gt;"",'Changer Configuration'!C20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" t="str">
+        <f>IF('Changer Configuration'!B21&lt;&gt;"",CONCATENATE('Changer Configuration'!B21,"=", 'Changer Configuration'!C21),IF('Changer Configuration'!C21&lt;&gt;"",'Changer Configuration'!C21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" t="str">
+        <f>IF('Changer Configuration'!B22&lt;&gt;"",CONCATENATE('Changer Configuration'!B22,"=", 'Changer Configuration'!C22),IF('Changer Configuration'!C22&lt;&gt;"",'Changer Configuration'!C22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" t="str">
+        <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE('Changer Configuration'!B23,"=", 'Changer Configuration'!C23),IF('Changer Configuration'!C23&lt;&gt;"",'Changer Configuration'!C23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" t="str">
         <f>IF('A propos'!B2&lt;&gt;"",CONCATENATE('A propos'!B2,"=", 'A propos'!C2),IF('A propos'!C2&lt;&gt;"",'A propos'!C2,""))</f>
         <v>#Message pour la fenêtre a propos</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" t="str">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" t="str">
         <f>IF('A propos'!B3&lt;&gt;"",CONCATENATE('A propos'!B3,"=", 'A propos'!C3),IF('A propos'!C3&lt;&gt;"",'A propos'!C3,""))</f>
         <v>window.about.title=A propos</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" t="str">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" t="str">
         <f>IF('A propos'!B4&lt;&gt;"",CONCATENATE('A propos'!B4,"=", 'A propos'!C4),IF('A propos'!C4&lt;&gt;"",'A propos'!C4,""))</f>
         <v>window.about.message.content=&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;A propos de l'application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nom de l'application : &lt;/u&gt; Caerus&lt;br /&gt;&lt;u&gt;Version : &lt;/u&gt; 1.1.2&lt;br /&gt;&lt;u&gt;Editeur : &lt;/u&gt; Jeremy, Leda&lt;br /&gt;&lt;u&gt;Site web : &lt;/u&gt;https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" t="str">
-        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE('A propos'!B5,"=", 'A propos'!C5),IF('A propos'!C5&lt;&gt;"",'A propos'!C5,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" t="str">
-        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE('A propos'!B6,"=", 'A propos'!C6),IF('A propos'!C6&lt;&gt;"",'A propos'!C6,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" t="str">
-        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE('A propos'!B7,"=", 'A propos'!C7),IF('A propos'!C7&lt;&gt;"",'A propos'!C7,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A393" t="str">
-        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE('A propos'!B8,"=", 'A propos'!C8),IF('A propos'!C8&lt;&gt;"",'A propos'!C8,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" t="str">
-        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE('A propos'!B9,"=", 'A propos'!C9),IF('A propos'!C9&lt;&gt;"",'A propos'!C9,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" t="str">
-        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE('A propos'!B10,"=", 'A propos'!C10),IF('A propos'!C10&lt;&gt;"",'A propos'!C10,""))</f>
+        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE('A propos'!B5,"=", 'A propos'!C5),IF('A propos'!C5&lt;&gt;"",'A propos'!C5,""))</f>
         <v/>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" t="str">
-        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE('A propos'!B11,"=", 'A propos'!C11),IF('A propos'!C11&lt;&gt;"",'A propos'!C11,""))</f>
+        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE('A propos'!B6,"=", 'A propos'!C6),IF('A propos'!C6&lt;&gt;"",'A propos'!C6,""))</f>
         <v/>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" t="str">
-        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE('A propos'!B12,"=", 'A propos'!C12),IF('A propos'!C12&lt;&gt;"",'A propos'!C12,""))</f>
+        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE('A propos'!B7,"=", 'A propos'!C7),IF('A propos'!C7&lt;&gt;"",'A propos'!C7,""))</f>
         <v/>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" t="str">
-        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE('A propos'!B13,"=", 'A propos'!C13),IF('A propos'!C13&lt;&gt;"",'A propos'!C13,""))</f>
+        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE('A propos'!B8,"=", 'A propos'!C8),IF('A propos'!C8&lt;&gt;"",'A propos'!C8,""))</f>
         <v/>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" t="str">
-        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE('A propos'!B14,"=", 'A propos'!C14),IF('A propos'!C14&lt;&gt;"",'A propos'!C14,""))</f>
+        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE('A propos'!B9,"=", 'A propos'!C9),IF('A propos'!C9&lt;&gt;"",'A propos'!C9,""))</f>
         <v/>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" t="str">
-        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE('A propos'!B15,"=", 'A propos'!C15),IF('A propos'!C15&lt;&gt;"",'A propos'!C15,""))</f>
+        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE('A propos'!B10,"=", 'A propos'!C10),IF('A propos'!C10&lt;&gt;"",'A propos'!C10,""))</f>
         <v/>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" t="str">
-        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE('A propos'!B16,"=", 'A propos'!C16),IF('A propos'!C16&lt;&gt;"",'A propos'!C16,""))</f>
+        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE('A propos'!B11,"=", 'A propos'!C11),IF('A propos'!C11&lt;&gt;"",'A propos'!C11,""))</f>
         <v/>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402" t="str">
-        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!C17),IF('A propos'!C17&lt;&gt;"",'A propos'!C17,""))</f>
+        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE('A propos'!B12,"=", 'A propos'!C12),IF('A propos'!C12&lt;&gt;"",'A propos'!C12,""))</f>
         <v/>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" t="str">
-        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!C18),IF('A propos'!C18&lt;&gt;"",'A propos'!C18,""))</f>
+        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE('A propos'!B13,"=", 'A propos'!C13),IF('A propos'!C13&lt;&gt;"",'A propos'!C13,""))</f>
         <v/>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" t="str">
-        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!C17),IF('A propos'!C17&lt;&gt;"",'A propos'!C17,""))</f>
+        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE('A propos'!B14,"=", 'A propos'!C14),IF('A propos'!C14&lt;&gt;"",'A propos'!C14,""))</f>
         <v/>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A405" t="str">
-        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!C18),IF('A propos'!C18&lt;&gt;"",'A propos'!C18,""))</f>
+        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE('A propos'!B15,"=", 'A propos'!C15),IF('A propos'!C15&lt;&gt;"",'A propos'!C15,""))</f>
         <v/>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" t="str">
-        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!C19),IF('A propos'!C19&lt;&gt;"",'A propos'!C19,""))</f>
+        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE('A propos'!B16,"=", 'A propos'!C16),IF('A propos'!C16&lt;&gt;"",'A propos'!C16,""))</f>
         <v/>
       </c>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A407" t="str">
-        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE('A propos'!B20,"=", 'A propos'!C42),IF('A propos'!C20&lt;&gt;"",'A propos'!C20,""))</f>
+        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!C17),IF('A propos'!C17&lt;&gt;"",'A propos'!C17,""))</f>
         <v/>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A408" t="str">
-        <f>IF('A propos'!B21&lt;&gt;"",CONCATENATE('A propos'!B21,"=", 'A propos'!C43),IF('A propos'!C21&lt;&gt;"",'A propos'!C21,""))</f>
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!C18),IF('A propos'!C18&lt;&gt;"",'A propos'!C18,""))</f>
         <v/>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" t="str">
-        <f>IF('A propos'!B22&lt;&gt;"",CONCATENATE('A propos'!B22,"=", 'A propos'!C44),IF('A propos'!C22&lt;&gt;"",'A propos'!C22,""))</f>
+        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!C17),IF('A propos'!C17&lt;&gt;"",'A propos'!C17,""))</f>
         <v/>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A410" t="str">
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!C18),IF('A propos'!C18&lt;&gt;"",'A propos'!C18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" t="str">
+        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!C19),IF('A propos'!C19&lt;&gt;"",'A propos'!C19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" t="str">
+        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE('A propos'!B20,"=", 'A propos'!C42),IF('A propos'!C20&lt;&gt;"",'A propos'!C20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" t="str">
+        <f>IF('A propos'!B21&lt;&gt;"",CONCATENATE('A propos'!B21,"=", 'A propos'!C43),IF('A propos'!C21&lt;&gt;"",'A propos'!C21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" t="str">
+        <f>IF('A propos'!B22&lt;&gt;"",CONCATENATE('A propos'!B22,"=", 'A propos'!C44),IF('A propos'!C22&lt;&gt;"",'A propos'!C22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" t="str">
         <f>IF('Export Document Materiel'!B2&lt;&gt;"",CONCATENATE('Export Document Materiel'!B2,"=", 'Export Document Materiel'!C2),IF('Export Document Materiel'!C2&lt;&gt;"",'Export Document Materiel'!C2,""))</f>
         <v>#Message pour l'export de document et matériel</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" t="str">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" t="str">
         <f>IF('Export Document Materiel'!B3&lt;&gt;"",CONCATENATE('Export Document Materiel'!B3,"=", 'Export Document Materiel'!C3),IF('Export Document Materiel'!C3&lt;&gt;"",'Export Document Materiel'!C3,""))</f>
         <v>window.export.document.title=Exporter les documents/matériels</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" t="str">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" t="str">
         <f>IF('Export Document Materiel'!B4&lt;&gt;"",CONCATENATE('Export Document Materiel'!B4,"=", 'Export Document Materiel'!C4),IF('Export Document Materiel'!C4&lt;&gt;"",'Export Document Materiel'!C4,""))</f>
         <v>window.export.document.choose.directory.panel.title=Choix du dossier de destination</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" t="str">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="str">
         <f>IF('Export Document Materiel'!B5&lt;&gt;"",CONCATENATE('Export Document Materiel'!B5,"=", 'Export Document Materiel'!C5),IF('Export Document Materiel'!C5&lt;&gt;"",'Export Document Materiel'!C5,""))</f>
         <v>window.export.document.choose.directory.label=Dossier de destination</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" t="str">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" t="str">
         <f>IF('Export Document Materiel'!B6&lt;&gt;"",CONCATENATE('Export Document Materiel'!B6,"=", 'Export Document Materiel'!C6),IF('Export Document Materiel'!C6&lt;&gt;"",'Export Document Materiel'!C6,""))</f>
         <v>window.export.document.mode.panel.title=Choix des données à exporter</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415" t="str">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" t="str">
         <f>IF('Export Document Materiel'!B7&lt;&gt;"",CONCATENATE('Export Document Materiel'!B7,"=", 'Export Document Materiel'!C7),IF('Export Document Materiel'!C7&lt;&gt;"",'Export Document Materiel'!C7,""))</f>
         <v>window.export.document.mode.document.label=Un document</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" t="str">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" t="str">
         <f>IF('Export Document Materiel'!B8&lt;&gt;"",CONCATENATE('Export Document Materiel'!B8,"=", 'Export Document Materiel'!C8),IF('Export Document Materiel'!C8&lt;&gt;"",'Export Document Materiel'!C8,""))</f>
         <v>window.export.document.mode.all.documents.label=Tous les documents</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" t="str">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" t="str">
         <f>IF('Export Document Materiel'!B9&lt;&gt;"",CONCATENATE('Export Document Materiel'!B9,"=", 'Export Document Materiel'!C9),IF('Export Document Materiel'!C9&lt;&gt;"",'Export Document Materiel'!C9,""))</f>
         <v>window.export.document.mode.result.search.label=Le résultat de la recherche</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418" t="str">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" t="str">
         <f>IF('Export Document Materiel'!B10&lt;&gt;"",CONCATENATE('Export Document Materiel'!B10,"=", 'Export Document Materiel'!C10),IF('Export Document Materiel'!C10&lt;&gt;"",'Export Document Materiel'!C10,""))</f>
         <v>window.export.document.choose.document.panel.title=Choix du document à exporter</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" t="str">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" t="str">
         <f>IF('Export Document Materiel'!B11&lt;&gt;"",CONCATENATE('Export Document Materiel'!B11,"=", 'Export Document Materiel'!C11),IF('Export Document Materiel'!C11&lt;&gt;"",'Export Document Materiel'!C11,""))</f>
         <v xml:space="preserve">window.export.document.choose.document.label=Document à exporter : </v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A420" t="str">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" t="str">
         <f>IF('Export Document Materiel'!B12&lt;&gt;"",CONCATENATE('Export Document Materiel'!B12,"=", 'Export Document Materiel'!C12),IF('Export Document Materiel'!C12&lt;&gt;"",'Export Document Materiel'!C12,""))</f>
         <v>window.export.document.choose.file.panel.title=Choix du nom du document</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" t="str">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" t="str">
         <f>IF('Export Document Materiel'!B13&lt;&gt;"",CONCATENATE('Export Document Materiel'!B13,"=", 'Export Document Materiel'!C13),IF('Export Document Materiel'!C13&lt;&gt;"",'Export Document Materiel'!C13,""))</f>
         <v xml:space="preserve">window.export.document.choose.file.label=Nom du document pour le resultat de la recherche : </v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" t="str">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" t="str">
         <f>IF('Export Document Materiel'!B14&lt;&gt;"",CONCATENATE('Export Document Materiel'!B14,"=", 'Export Document Materiel'!C14),IF('Export Document Materiel'!C14&lt;&gt;"",'Export Document Materiel'!C14,""))</f>
         <v>window.export.document.button.panel.title=Actions</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" t="str">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" t="str">
         <f>IF('Export Document Materiel'!B15&lt;&gt;"",CONCATENATE('Export Document Materiel'!B15,"=", 'Export Document Materiel'!C15),IF('Export Document Materiel'!C15&lt;&gt;"",'Export Document Materiel'!C15,""))</f>
         <v>window.export.document.button.export.label=Exporter et fermer</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" t="str">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" t="str">
         <f>IF('Export Document Materiel'!B16&lt;&gt;"",CONCATENATE('Export Document Materiel'!B16,"=", 'Export Document Materiel'!C16),IF('Export Document Materiel'!C16&lt;&gt;"",'Export Document Materiel'!C16,""))</f>
         <v>window.export.document.information.message.title=Export effectué</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" t="str">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" t="str">
         <f>IF('Export Document Materiel'!B17&lt;&gt;"",CONCATENATE('Export Document Materiel'!B17,"=", 'Export Document Materiel'!C17),IF('Export Document Materiel'!C17&lt;&gt;"",'Export Document Materiel'!C17,""))</f>
         <v>window.export.document.information.message=&lt;HTML&gt;&lt;P&gt;Export réalisé avec succés&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" t="str">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" t="str">
         <f>IF('Export Document Materiel'!B18&lt;&gt;"",CONCATENATE('Export Document Materiel'!B18,"=", 'Export Document Materiel'!C18),IF('Export Document Materiel'!C18&lt;&gt;"",'Export Document Materiel'!C18,""))</f>
         <v>window.export.document.button.close.label=Fermer</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" t="str">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" t="str">
         <f>IF('Export Document Materiel'!B19&lt;&gt;"",CONCATENATE('Export Document Materiel'!B19,"=", 'Export Document Materiel'!C19),IF('Export Document Materiel'!C19&lt;&gt;"",'Export Document Materiel'!C19,""))</f>
         <v>window.export.document.choose.directory.dialog.title=Choisissez le dossier de destination</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" t="str">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" t="str">
         <f>IF('Export Document Materiel'!B20&lt;&gt;"",CONCATENATE('Export Document Materiel'!B20,"=", 'Export Document Materiel'!C20),IF('Export Document Materiel'!C20&lt;&gt;"",'Export Document Materiel'!C20,""))</f>
         <v>window.export.document.information.search.message=&lt;HTML&gt;&lt;P&gt;Export réalisé avec succés&lt;BR/&gt;Pour information, le document ne contient aucune données d'en-tête&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A429" t="str">
-        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE('Export Document Materiel'!B21,"=", 'Export Document Materiel'!C21),IF('Export Document Materiel'!C21&lt;&gt;"",'Export Document Materiel'!C21,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" t="str">
-        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE('Export Document Materiel'!B22,"=", 'Export Document Materiel'!C22),IF('Export Document Materiel'!C22&lt;&gt;"",'Export Document Materiel'!C22,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" t="str">
-        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE('Export Document Materiel'!B23,"=", 'Export Document Materiel'!C23),IF('Export Document Materiel'!C23&lt;&gt;"",'Export Document Materiel'!C23,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A432" t="str">
-        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE('Export Document Materiel'!B24,"=", 'Export Document Materiel'!C24),IF('Export Document Materiel'!C24&lt;&gt;"",'Export Document Materiel'!C24,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A433" t="str">
-        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE('Export Document Materiel'!B25,"=", 'Export Document Materiel'!C25),IF('Export Document Materiel'!C25&lt;&gt;"",'Export Document Materiel'!C25,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" t="str">
-        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE('Export Document Materiel'!B26,"=", 'Export Document Materiel'!C26),IF('Export Document Materiel'!C26&lt;&gt;"",'Export Document Materiel'!C26,""))</f>
+        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE('Export Document Materiel'!B21,"=", 'Export Document Materiel'!C21),IF('Export Document Materiel'!C21&lt;&gt;"",'Export Document Materiel'!C21,""))</f>
         <v/>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A435" t="str">
-        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE('Export Document Materiel'!B27,"=", 'Export Document Materiel'!C27),IF('Export Document Materiel'!C27&lt;&gt;"",'Export Document Materiel'!C27,""))</f>
+        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE('Export Document Materiel'!B22,"=", 'Export Document Materiel'!C22),IF('Export Document Materiel'!C22&lt;&gt;"",'Export Document Materiel'!C22,""))</f>
         <v/>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" t="str">
-        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE('Export Document Materiel'!B28,"=", 'Export Document Materiel'!C28),IF('Export Document Materiel'!C28&lt;&gt;"",'Export Document Materiel'!C28,""))</f>
+        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE('Export Document Materiel'!B23,"=", 'Export Document Materiel'!C23),IF('Export Document Materiel'!C23&lt;&gt;"",'Export Document Materiel'!C23,""))</f>
         <v/>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" t="str">
-        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE('Export Document Materiel'!B29,"=", 'Export Document Materiel'!C29),IF('Export Document Materiel'!C29&lt;&gt;"",'Export Document Materiel'!C29,""))</f>
+        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE('Export Document Materiel'!B24,"=", 'Export Document Materiel'!C24),IF('Export Document Materiel'!C24&lt;&gt;"",'Export Document Materiel'!C24,""))</f>
         <v/>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A438" t="str">
-        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE('Export Document Materiel'!B30,"=", 'Export Document Materiel'!C30),IF('Export Document Materiel'!C30&lt;&gt;"",'Export Document Materiel'!C30,""))</f>
+        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE('Export Document Materiel'!B25,"=", 'Export Document Materiel'!C25),IF('Export Document Materiel'!C25&lt;&gt;"",'Export Document Materiel'!C25,""))</f>
         <v/>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" t="str">
-        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE('Export Document Materiel'!B31,"=", 'Export Document Materiel'!C31),IF('Export Document Materiel'!C31&lt;&gt;"",'Export Document Materiel'!C31,""))</f>
+        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE('Export Document Materiel'!B26,"=", 'Export Document Materiel'!C26),IF('Export Document Materiel'!C26&lt;&gt;"",'Export Document Materiel'!C26,""))</f>
         <v/>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A440" t="str">
-        <f>IF('Export Document Materiel'!B32&lt;&gt;"",CONCATENATE('Export Document Materiel'!B32,"=", 'Export Document Materiel'!C32),IF('Export Document Materiel'!C32&lt;&gt;"",'Export Document Materiel'!C32,""))</f>
+        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE('Export Document Materiel'!B27,"=", 'Export Document Materiel'!C27),IF('Export Document Materiel'!C27&lt;&gt;"",'Export Document Materiel'!C27,""))</f>
         <v/>
       </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A441" t="str">
-        <f>IF('Export Document Materiel'!B33&lt;&gt;"",CONCATENATE('Export Document Materiel'!B33,"=", 'Export Document Materiel'!C33),IF('Export Document Materiel'!C33&lt;&gt;"",'Export Document Materiel'!C33,""))</f>
+        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE('Export Document Materiel'!B28,"=", 'Export Document Materiel'!C28),IF('Export Document Materiel'!C28&lt;&gt;"",'Export Document Materiel'!C28,""))</f>
         <v/>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A442" t="str">
-        <f>IF('Export Document Materiel'!B34&lt;&gt;"",CONCATENATE('Export Document Materiel'!B34,"=", 'Export Document Materiel'!C34),IF('Export Document Materiel'!C34&lt;&gt;"",'Export Document Materiel'!C34,""))</f>
+        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE('Export Document Materiel'!B29,"=", 'Export Document Materiel'!C29),IF('Export Document Materiel'!C29&lt;&gt;"",'Export Document Materiel'!C29,""))</f>
         <v/>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A443" t="str">
+        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE('Export Document Materiel'!B30,"=", 'Export Document Materiel'!C30),IF('Export Document Materiel'!C30&lt;&gt;"",'Export Document Materiel'!C30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" t="str">
+        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE('Export Document Materiel'!B31,"=", 'Export Document Materiel'!C31),IF('Export Document Materiel'!C31&lt;&gt;"",'Export Document Materiel'!C31,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" t="str">
+        <f>IF('Export Document Materiel'!B32&lt;&gt;"",CONCATENATE('Export Document Materiel'!B32,"=", 'Export Document Materiel'!C32),IF('Export Document Materiel'!C32&lt;&gt;"",'Export Document Materiel'!C32,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" t="str">
+        <f>IF('Export Document Materiel'!B33&lt;&gt;"",CONCATENATE('Export Document Materiel'!B33,"=", 'Export Document Materiel'!C33),IF('Export Document Materiel'!C33&lt;&gt;"",'Export Document Materiel'!C33,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" t="str">
+        <f>IF('Export Document Materiel'!B34&lt;&gt;"",CONCATENATE('Export Document Materiel'!B34,"=", 'Export Document Materiel'!C34),IF('Export Document Materiel'!C34&lt;&gt;"",'Export Document Materiel'!C34,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" t="str">
         <f>IF('Erreur incoherence'!B2&lt;&gt;"",CONCATENATE('Erreur incoherence'!B2,"=", 'Erreur incoherence'!C2),IF('Erreur incoherence'!C2&lt;&gt;"",'Erreur incoherence'!C2,""))</f>
         <v>#Message pour les erreurs d'incohérence</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" t="str">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" t="str">
         <f>IF('Erreur incoherence'!B3&lt;&gt;"",CONCATENATE('Erreur incoherence'!B3,"=", 'Erreur incoherence'!C3),IF('Erreur incoherence'!C3&lt;&gt;"",'Erreur incoherence'!C3,""))</f>
         <v>window.error.inconsistency.title=Erreurs de duplications</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" t="str">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" t="str">
         <f>IF('Erreur incoherence'!B4&lt;&gt;"",CONCATENATE('Erreur incoherence'!B4,"=", 'Erreur incoherence'!C4),IF('Erreur incoherence'!C4&lt;&gt;"",'Erreur incoherence'!C4,""))</f>
         <v>window.error.inconsistency.panel.title=Liste des incohérences</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" t="str">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" t="str">
         <f>IF('Erreur incoherence'!B5&lt;&gt;"",CONCATENATE('Erreur incoherence'!B5,"=", 'Erreur incoherence'!C5),IF('Erreur incoherence'!C5&lt;&gt;"",'Erreur incoherence'!C5,""))</f>
         <v xml:space="preserve">window.error.inconsistency.field.label=Balise : </v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A447" t="str">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" t="str">
         <f>IF('Erreur incoherence'!B6&lt;&gt;"",CONCATENATE('Erreur incoherence'!B6,"=", 'Erreur incoherence'!C6),IF('Erreur incoherence'!C6&lt;&gt;"",'Erreur incoherence'!C6,""))</f>
         <v xml:space="preserve">window.error.inconsistency.number.line.label=Numéro de la ligne : </v>
       </c>
     </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" t="str">
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" t="str">
         <f>IF('Erreur incoherence'!B7&lt;&gt;"",CONCATENATE('Erreur incoherence'!B7,"=", 'Erreur incoherence'!C7),IF('Erreur incoherence'!C7&lt;&gt;"",'Erreur incoherence'!C7,""))</f>
         <v xml:space="preserve">window.error.inconsistency.name.file.label=Nom du fichier : </v>
       </c>
     </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" t="str">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" t="str">
         <f>IF('Erreur incoherence'!B8&lt;&gt;"",CONCATENATE('Erreur incoherence'!B8,"=", 'Erreur incoherence'!C8),IF('Erreur incoherence'!C8&lt;&gt;"",'Erreur incoherence'!C8,""))</f>
         <v>window.error.inconsistency.message.panel.title=Message d'information</v>
       </c>
     </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" t="str">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" t="str">
         <f>IF('Erreur incoherence'!B9&lt;&gt;"",CONCATENATE('Erreur incoherence'!B9,"=", 'Erreur incoherence'!C9),IF('Erreur incoherence'!C9&lt;&gt;"",'Erreur incoherence'!C9,""))</f>
         <v>window.error.inconsistency.message=&lt;HTML&gt;&lt;P&gt;Des erreurs d'incohérence ont été détectées.&lt;BR/&gt;Celles-ci peuvent causer des décalages d'information.&lt;BR/&gt;Vous devez corriger manuellement les informations.&lt;BR/&gt;Rechargez les documents corrigés.&lt;BR/&gt;De nouvelles erreurs peuvent être détectées en raison de lacunes dans l'information.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" t="str">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" t="str">
         <f>IF('Erreur incoherence'!B10&lt;&gt;"",CONCATENATE('Erreur incoherence'!B10,"=", 'Erreur incoherence'!C10),IF('Erreur incoherence'!C10&lt;&gt;"",'Erreur incoherence'!C10,""))</f>
         <v>window.error.inconsistency.buttons.panel.title=Actions</v>
       </c>
     </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" t="str">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" t="str">
         <f>IF('Erreur incoherence'!B11&lt;&gt;"",CONCATENATE('Erreur incoherence'!B11,"=", 'Erreur incoherence'!C11),IF('Erreur incoherence'!C11&lt;&gt;"",'Erreur incoherence'!C11,""))</f>
         <v>window.error.inconsistency.buttons.close.button.label=Fermer et recharger les documents</v>
       </c>
     </row>
-    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453" t="str">
-        <f>IF('Erreur incoherence'!B12&lt;&gt;"",CONCATENATE('Erreur incoherence'!B12,"=", 'Erreur incoherence'!C12),IF('Erreur incoherence'!C12&lt;&gt;"",'Erreur incoherence'!C12,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A454" t="str">
-        <f>IF('Erreur incoherence'!B13&lt;&gt;"",CONCATENATE('Erreur incoherence'!B13,"=", 'Erreur incoherence'!C13),IF('Erreur incoherence'!C13&lt;&gt;"",'Erreur incoherence'!C13,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A455" t="str">
-        <f>IF('Erreur incoherence'!B14&lt;&gt;"",CONCATENATE('Erreur incoherence'!B14,"=", 'Erreur incoherence'!C14),IF('Erreur incoherence'!C14&lt;&gt;"",'Erreur incoherence'!C14,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456" t="str">
-        <f>IF('Erreur incoherence'!B15&lt;&gt;"",CONCATENATE('Erreur incoherence'!B15,"=", 'Erreur incoherence'!C15),IF('Erreur incoherence'!C15&lt;&gt;"",'Erreur incoherence'!C15,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457" t="str">
-        <f>IF('Erreur incoherence'!B16&lt;&gt;"",CONCATENATE('Erreur incoherence'!B16,"=", 'Erreur incoherence'!C16),IF('Erreur incoherence'!C16&lt;&gt;"",'Erreur incoherence'!C16,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" t="str">
-        <f>IF('Erreur incoherence'!B17&lt;&gt;"",CONCATENATE('Erreur incoherence'!B17,"=", 'Erreur incoherence'!C17),IF('Erreur incoherence'!C17&lt;&gt;"",'Erreur incoherence'!C17,""))</f>
+        <f>IF('Erreur incoherence'!B12&lt;&gt;"",CONCATENATE('Erreur incoherence'!B12,"=", 'Erreur incoherence'!C12),IF('Erreur incoherence'!C12&lt;&gt;"",'Erreur incoherence'!C12,""))</f>
         <v/>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" t="str">
-        <f>IF('Erreur incoherence'!B18&lt;&gt;"",CONCATENATE('Erreur incoherence'!B18,"=", 'Erreur incoherence'!C18),IF('Erreur incoherence'!C18&lt;&gt;"",'Erreur incoherence'!C18,""))</f>
+        <f>IF('Erreur incoherence'!B13&lt;&gt;"",CONCATENATE('Erreur incoherence'!B13,"=", 'Erreur incoherence'!C13),IF('Erreur incoherence'!C13&lt;&gt;"",'Erreur incoherence'!C13,""))</f>
         <v/>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" t="str">
-        <f>IF('Erreur incoherence'!B19&lt;&gt;"",CONCATENATE('Erreur incoherence'!B19,"=", 'Erreur incoherence'!C19),IF('Erreur incoherence'!C19&lt;&gt;"",'Erreur incoherence'!C19,""))</f>
+        <f>IF('Erreur incoherence'!B14&lt;&gt;"",CONCATENATE('Erreur incoherence'!B14,"=", 'Erreur incoherence'!C14),IF('Erreur incoherence'!C14&lt;&gt;"",'Erreur incoherence'!C14,""))</f>
         <v/>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" t="str">
-        <f>IF('Erreur incoherence'!B20&lt;&gt;"",CONCATENATE('Erreur incoherence'!B20,"=", 'Erreur incoherence'!C20),IF('Erreur incoherence'!C20&lt;&gt;"",'Erreur incoherence'!C20,""))</f>
+        <f>IF('Erreur incoherence'!B15&lt;&gt;"",CONCATENATE('Erreur incoherence'!B15,"=", 'Erreur incoherence'!C15),IF('Erreur incoherence'!C15&lt;&gt;"",'Erreur incoherence'!C15,""))</f>
         <v/>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" t="str">
-        <f>IF('Erreur incoherence'!B21&lt;&gt;"",CONCATENATE('Erreur incoherence'!B21,"=", 'Erreur incoherence'!C21),IF('Erreur incoherence'!C21&lt;&gt;"",'Erreur incoherence'!C21,""))</f>
+        <f>IF('Erreur incoherence'!B16&lt;&gt;"",CONCATENATE('Erreur incoherence'!B16,"=", 'Erreur incoherence'!C16),IF('Erreur incoherence'!C16&lt;&gt;"",'Erreur incoherence'!C16,""))</f>
         <v/>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A463" t="str">
-        <f>IF('Erreur incoherence'!B22&lt;&gt;"",CONCATENATE('Erreur incoherence'!B22,"=", 'Erreur incoherence'!C22),IF('Erreur incoherence'!C22&lt;&gt;"",'Erreur incoherence'!C22,""))</f>
+        <f>IF('Erreur incoherence'!B17&lt;&gt;"",CONCATENATE('Erreur incoherence'!B17,"=", 'Erreur incoherence'!C17),IF('Erreur incoherence'!C17&lt;&gt;"",'Erreur incoherence'!C17,""))</f>
         <v/>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" t="str">
-        <f>IF('Erreur incoherence'!B23&lt;&gt;"",CONCATENATE('Erreur incoherence'!B23,"=", 'Erreur incoherence'!C23),IF('Erreur incoherence'!C23&lt;&gt;"",'Erreur incoherence'!C23,""))</f>
+        <f>IF('Erreur incoherence'!B18&lt;&gt;"",CONCATENATE('Erreur incoherence'!B18,"=", 'Erreur incoherence'!C18),IF('Erreur incoherence'!C18&lt;&gt;"",'Erreur incoherence'!C18,""))</f>
         <v/>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A465" t="str">
-        <f>IF('Erreur incoherence'!B24&lt;&gt;"",CONCATENATE('Erreur incoherence'!B24,"=", 'Erreur incoherence'!C24),IF('Erreur incoherence'!C24&lt;&gt;"",'Erreur incoherence'!C24,""))</f>
+        <f>IF('Erreur incoherence'!B19&lt;&gt;"",CONCATENATE('Erreur incoherence'!B19,"=", 'Erreur incoherence'!C19),IF('Erreur incoherence'!C19&lt;&gt;"",'Erreur incoherence'!C19,""))</f>
         <v/>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466" t="str">
-        <f>IF('Erreur incoherence'!B25&lt;&gt;"",CONCATENATE('Erreur incoherence'!B25,"=", 'Erreur incoherence'!C25),IF('Erreur incoherence'!C25&lt;&gt;"",'Erreur incoherence'!C25,""))</f>
+        <f>IF('Erreur incoherence'!B20&lt;&gt;"",CONCATENATE('Erreur incoherence'!B20,"=", 'Erreur incoherence'!C20),IF('Erreur incoherence'!C20&lt;&gt;"",'Erreur incoherence'!C20,""))</f>
         <v/>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A467" t="str">
-        <f>IF('Erreur incoherence'!B26&lt;&gt;"",CONCATENATE('Erreur incoherence'!B26,"=", 'Erreur incoherence'!C26),IF('Erreur incoherence'!C26&lt;&gt;"",'Erreur incoherence'!C26,""))</f>
+        <f>IF('Erreur incoherence'!B21&lt;&gt;"",CONCATENATE('Erreur incoherence'!B21,"=", 'Erreur incoherence'!C21),IF('Erreur incoherence'!C21&lt;&gt;"",'Erreur incoherence'!C21,""))</f>
         <v/>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468" t="str">
-        <f>IF('Erreur incoherence'!B27&lt;&gt;"",CONCATENATE('Erreur incoherence'!B27,"=", 'Erreur incoherence'!C27),IF('Erreur incoherence'!C27&lt;&gt;"",'Erreur incoherence'!C27,""))</f>
+        <f>IF('Erreur incoherence'!B22&lt;&gt;"",CONCATENATE('Erreur incoherence'!B22,"=", 'Erreur incoherence'!C22),IF('Erreur incoherence'!C22&lt;&gt;"",'Erreur incoherence'!C22,""))</f>
         <v/>
       </c>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A469" t="str">
-        <f>IF('Erreur incoherence'!B28&lt;&gt;"",CONCATENATE('Erreur incoherence'!B28,"=", 'Erreur incoherence'!C28),IF('Erreur incoherence'!C28&lt;&gt;"",'Erreur incoherence'!C28,""))</f>
+        <f>IF('Erreur incoherence'!B23&lt;&gt;"",CONCATENATE('Erreur incoherence'!B23,"=", 'Erreur incoherence'!C23),IF('Erreur incoherence'!C23&lt;&gt;"",'Erreur incoherence'!C23,""))</f>
         <v/>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A470" t="str">
-        <f>IF('Erreur incoherence'!B29&lt;&gt;"",CONCATENATE('Erreur incoherence'!B29,"=", 'Erreur incoherence'!C29),IF('Erreur incoherence'!C29&lt;&gt;"",'Erreur incoherence'!C29,""))</f>
+        <f>IF('Erreur incoherence'!B24&lt;&gt;"",CONCATENATE('Erreur incoherence'!B24,"=", 'Erreur incoherence'!C24),IF('Erreur incoherence'!C24&lt;&gt;"",'Erreur incoherence'!C24,""))</f>
         <v/>
       </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" t="str">
-        <f>IF('Erreur incoherence'!B30&lt;&gt;"",CONCATENATE('Erreur incoherence'!B30,"=", 'Erreur incoherence'!C30),IF('Erreur incoherence'!C30&lt;&gt;"",'Erreur incoherence'!C30,""))</f>
+        <f>IF('Erreur incoherence'!B25&lt;&gt;"",CONCATENATE('Erreur incoherence'!B25,"=", 'Erreur incoherence'!C25),IF('Erreur incoherence'!C25&lt;&gt;"",'Erreur incoherence'!C25,""))</f>
         <v/>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A472" t="str">
-        <f>IF('Erreur incoherence'!B31&lt;&gt;"",CONCATENATE('Erreur incoherence'!B31,"=", 'Erreur incoherence'!C31),IF('Erreur incoherence'!C31&lt;&gt;"",'Erreur incoherence'!C31,""))</f>
+        <f>IF('Erreur incoherence'!B26&lt;&gt;"",CONCATENATE('Erreur incoherence'!B26,"=", 'Erreur incoherence'!C26),IF('Erreur incoherence'!C26&lt;&gt;"",'Erreur incoherence'!C26,""))</f>
         <v/>
       </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A473" t="str">
+        <f>IF('Erreur incoherence'!B27&lt;&gt;"",CONCATENATE('Erreur incoherence'!B27,"=", 'Erreur incoherence'!C27),IF('Erreur incoherence'!C27&lt;&gt;"",'Erreur incoherence'!C27,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" t="str">
+        <f>IF('Erreur incoherence'!B28&lt;&gt;"",CONCATENATE('Erreur incoherence'!B28,"=", 'Erreur incoherence'!C28),IF('Erreur incoherence'!C28&lt;&gt;"",'Erreur incoherence'!C28,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" t="str">
+        <f>IF('Erreur incoherence'!B29&lt;&gt;"",CONCATENATE('Erreur incoherence'!B29,"=", 'Erreur incoherence'!C29),IF('Erreur incoherence'!C29&lt;&gt;"",'Erreur incoherence'!C29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" t="str">
+        <f>IF('Erreur incoherence'!B30&lt;&gt;"",CONCATENATE('Erreur incoherence'!B30,"=", 'Erreur incoherence'!C30),IF('Erreur incoherence'!C30&lt;&gt;"",'Erreur incoherence'!C30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" t="str">
+        <f>IF('Erreur incoherence'!B31&lt;&gt;"",CONCATENATE('Erreur incoherence'!B31,"=", 'Erreur incoherence'!C31),IF('Erreur incoherence'!C31&lt;&gt;"",'Erreur incoherence'!C31,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" t="str">
         <f>IF('Erreur balise introductive'!B2&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B2,"=", 'Erreur balise introductive'!C2),IF('Erreur balise introductive'!C2&lt;&gt;"",'Erreur balise introductive'!C2,""))</f>
         <v>#Message pour les erreurs de balise introductive</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" t="str">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" t="str">
         <f>IF('Erreur balise introductive'!B3&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B3,"=", 'Erreur balise introductive'!C3),IF('Erreur balise introductive'!C3&lt;&gt;"",'Erreur balise introductive'!C3,""))</f>
         <v>window.error.missing.base.code.title=Erreurs de balises introductives</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" t="str">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" t="str">
         <f>IF('Erreur balise introductive'!B4&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B4,"=", 'Erreur balise introductive'!C4),IF('Erreur balise introductive'!C4&lt;&gt;"",'Erreur balise introductive'!C4,""))</f>
         <v>window.error.missing.base.code.panel.title=Liste des balises introductives</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" t="str">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" t="str">
         <f>IF('Erreur balise introductive'!B5&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B5,"=", 'Erreur balise introductive'!C5),IF('Erreur balise introductive'!C5&lt;&gt;"",'Erreur balise introductive'!C5,""))</f>
         <v xml:space="preserve">window.error.missing.base.code.field.label=Balise : </v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A477" t="str">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" t="str">
         <f>IF('Erreur balise introductive'!B6&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B6,"=", 'Erreur balise introductive'!C6),IF('Erreur balise introductive'!C6&lt;&gt;"",'Erreur balise introductive'!C6,""))</f>
         <v xml:space="preserve">window.error.missing.base.code.number.line.label=Numéro de la ligne : </v>
       </c>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" t="str">
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" t="str">
         <f>IF('Erreur balise introductive'!B7&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B7,"=", 'Erreur balise introductive'!C7),IF('Erreur balise introductive'!C7&lt;&gt;"",'Erreur balise introductive'!C7,""))</f>
         <v xml:space="preserve">window.error.missing.base.code.name.file.label=Nom du fichier : </v>
       </c>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" t="str">
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" t="str">
         <f>IF('Erreur balise introductive'!B8&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B8,"=", 'Erreur balise introductive'!C8),IF('Erreur balise introductive'!C8&lt;&gt;"",'Erreur balise introductive'!C8,""))</f>
         <v>window.error.missing.base.code.message.panel.title=Message d'information</v>
       </c>
     </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A480" t="str">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" t="str">
         <f>IF('Erreur balise introductive'!B9&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B9,"=", 'Erreur balise introductive'!C9),IF('Erreur balise introductive'!C9&lt;&gt;"",'Erreur balise introductive'!C9,""))</f>
         <v>window.error.missing.base.code.message=&lt;HTML&gt;&lt;P&gt;Des erreurs de balises introductives ont été détectées.&lt;BR/&gt;Vous devez corriger manuellement les informations sur vos documents.&lt;BR/&gt;En refermant cette fenêtre les documents se rechargeront automatiquement.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" t="str">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" t="str">
         <f>IF('Erreur balise introductive'!B10&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B10,"=", 'Erreur balise introductive'!C10),IF('Erreur balise introductive'!C10&lt;&gt;"",'Erreur balise introductive'!C10,""))</f>
         <v>window.error.missing.base.code.buttons.panel.title=Actions</v>
       </c>
     </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A482" t="str">
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" t="str">
         <f>IF('Erreur balise introductive'!B11&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B11,"=", 'Erreur balise introductive'!C11),IF('Erreur balise introductive'!C11&lt;&gt;"",'Erreur balise introductive'!C11,""))</f>
         <v>window.error.missing.base.code.buttons.close.button.label=Fermer et recharger les documents</v>
       </c>
     </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A483" t="str">
-        <f>IF('Erreur balise introductive'!B12&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B12,"=", 'Erreur balise introductive'!C12),IF('Erreur balise introductive'!C12&lt;&gt;"",'Erreur balise introductive'!C12,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A484" t="str">
-        <f>IF('Erreur balise introductive'!B13&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B13,"=", 'Erreur balise introductive'!C13),IF('Erreur balise introductive'!C13&lt;&gt;"",'Erreur balise introductive'!C13,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A485" t="str">
-        <f>IF('Erreur balise introductive'!B14&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B14,"=", 'Erreur balise introductive'!C14),IF('Erreur balise introductive'!C14&lt;&gt;"",'Erreur balise introductive'!C14,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A486" t="str">
-        <f>IF('Erreur balise introductive'!B15&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B15,"=", 'Erreur balise introductive'!C15),IF('Erreur balise introductive'!C15&lt;&gt;"",'Erreur balise introductive'!C15,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A487" t="str">
-        <f>IF('Erreur balise introductive'!B16&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B16,"=", 'Erreur balise introductive'!C16),IF('Erreur balise introductive'!C16&lt;&gt;"",'Erreur balise introductive'!C16,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" t="str">
-        <f>IF('Erreur balise introductive'!B17&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B17,"=", 'Erreur balise introductive'!C17),IF('Erreur balise introductive'!C17&lt;&gt;"",'Erreur balise introductive'!C17,""))</f>
+        <f>IF('Erreur balise introductive'!B12&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B12,"=", 'Erreur balise introductive'!C12),IF('Erreur balise introductive'!C12&lt;&gt;"",'Erreur balise introductive'!C12,""))</f>
         <v/>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" t="str">
-        <f>IF('Erreur balise introductive'!B18&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B18,"=", 'Erreur balise introductive'!C18),IF('Erreur balise introductive'!C18&lt;&gt;"",'Erreur balise introductive'!C18,""))</f>
+        <f>IF('Erreur balise introductive'!B13&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B13,"=", 'Erreur balise introductive'!C13),IF('Erreur balise introductive'!C13&lt;&gt;"",'Erreur balise introductive'!C13,""))</f>
         <v/>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" t="str">
-        <f>IF('Erreur balise introductive'!B19&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B19,"=", 'Erreur balise introductive'!C19),IF('Erreur balise introductive'!C19&lt;&gt;"",'Erreur balise introductive'!C19,""))</f>
+        <f>IF('Erreur balise introductive'!B14&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B14,"=", 'Erreur balise introductive'!C14),IF('Erreur balise introductive'!C14&lt;&gt;"",'Erreur balise introductive'!C14,""))</f>
         <v/>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" t="str">
-        <f>IF('Erreur balise introductive'!B20&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B20,"=", 'Erreur balise introductive'!C20),IF('Erreur balise introductive'!C20&lt;&gt;"",'Erreur balise introductive'!C20,""))</f>
+        <f>IF('Erreur balise introductive'!B15&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B15,"=", 'Erreur balise introductive'!C15),IF('Erreur balise introductive'!C15&lt;&gt;"",'Erreur balise introductive'!C15,""))</f>
         <v/>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" t="str">
-        <f>IF('Erreur balise introductive'!B21&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B21,"=", 'Erreur balise introductive'!C21),IF('Erreur balise introductive'!C21&lt;&gt;"",'Erreur balise introductive'!C21,""))</f>
+        <f>IF('Erreur balise introductive'!B16&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B16,"=", 'Erreur balise introductive'!C16),IF('Erreur balise introductive'!C16&lt;&gt;"",'Erreur balise introductive'!C16,""))</f>
         <v/>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A493" t="str">
-        <f>IF('Erreur balise introductive'!B22&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B22,"=", 'Erreur balise introductive'!C22),IF('Erreur balise introductive'!C22&lt;&gt;"",'Erreur balise introductive'!C22,""))</f>
+        <f>IF('Erreur balise introductive'!B17&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B17,"=", 'Erreur balise introductive'!C17),IF('Erreur balise introductive'!C17&lt;&gt;"",'Erreur balise introductive'!C17,""))</f>
         <v/>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A494" t="str">
-        <f>IF('Erreur balise introductive'!B23&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B23,"=", 'Erreur balise introductive'!C23),IF('Erreur balise introductive'!C23&lt;&gt;"",'Erreur balise introductive'!C23,""))</f>
+        <f>IF('Erreur balise introductive'!B18&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B18,"=", 'Erreur balise introductive'!C18),IF('Erreur balise introductive'!C18&lt;&gt;"",'Erreur balise introductive'!C18,""))</f>
         <v/>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A495" t="str">
-        <f>IF('Erreur balise introductive'!B24&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B24,"=", 'Erreur balise introductive'!C24),IF('Erreur balise introductive'!C24&lt;&gt;"",'Erreur balise introductive'!C24,""))</f>
+        <f>IF('Erreur balise introductive'!B19&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B19,"=", 'Erreur balise introductive'!C19),IF('Erreur balise introductive'!C19&lt;&gt;"",'Erreur balise introductive'!C19,""))</f>
         <v/>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A496" t="str">
-        <f>IF('Erreur balise introductive'!B25&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B25,"=", 'Erreur balise introductive'!C25),IF('Erreur balise introductive'!C25&lt;&gt;"",'Erreur balise introductive'!C25,""))</f>
+        <f>IF('Erreur balise introductive'!B20&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B20,"=", 'Erreur balise introductive'!C20),IF('Erreur balise introductive'!C20&lt;&gt;"",'Erreur balise introductive'!C20,""))</f>
         <v/>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A497" t="str">
-        <f>IF('Erreur balise introductive'!B26&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B26,"=", 'Erreur balise introductive'!C26),IF('Erreur balise introductive'!C26&lt;&gt;"",'Erreur balise introductive'!C26,""))</f>
+        <f>IF('Erreur balise introductive'!B21&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B21,"=", 'Erreur balise introductive'!C21),IF('Erreur balise introductive'!C21&lt;&gt;"",'Erreur balise introductive'!C21,""))</f>
         <v/>
       </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A498" t="str">
-        <f>IF('Erreur balise introductive'!B27&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B27,"=", 'Erreur balise introductive'!C27),IF('Erreur balise introductive'!C27&lt;&gt;"",'Erreur balise introductive'!C27,""))</f>
+        <f>IF('Erreur balise introductive'!B22&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B22,"=", 'Erreur balise introductive'!C22),IF('Erreur balise introductive'!C22&lt;&gt;"",'Erreur balise introductive'!C22,""))</f>
         <v/>
       </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A499" t="str">
+        <f>IF('Erreur balise introductive'!B23&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B23,"=", 'Erreur balise introductive'!C23),IF('Erreur balise introductive'!C23&lt;&gt;"",'Erreur balise introductive'!C23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" t="str">
+        <f>IF('Erreur balise introductive'!B24&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B24,"=", 'Erreur balise introductive'!C24),IF('Erreur balise introductive'!C24&lt;&gt;"",'Erreur balise introductive'!C24,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" t="str">
+        <f>IF('Erreur balise introductive'!B25&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B25,"=", 'Erreur balise introductive'!C25),IF('Erreur balise introductive'!C25&lt;&gt;"",'Erreur balise introductive'!C25,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" t="str">
+        <f>IF('Erreur balise introductive'!B26&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B26,"=", 'Erreur balise introductive'!C26),IF('Erreur balise introductive'!C26&lt;&gt;"",'Erreur balise introductive'!C26,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" t="str">
+        <f>IF('Erreur balise introductive'!B27&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B27,"=", 'Erreur balise introductive'!C27),IF('Erreur balise introductive'!C27&lt;&gt;"",'Erreur balise introductive'!C27,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504" t="str">
         <f>IF('Erreur balise introductive'!B28&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B28,"=", 'Erreur balise introductive'!C28),IF('Erreur balise introductive'!C28&lt;&gt;"",'Erreur balise introductive'!C28,""))</f>
         <v/>
       </c>
@@ -30298,10 +30388,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
-  <dimension ref="A1:A501"/>
+  <dimension ref="A1:A507"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A340" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A353" sqref="A1:A501"/>
+    <sheetView showZeros="0" topLeftCell="A358" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A375" sqref="A1:A507"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30414,7 +30504,7 @@
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF('Fenêtre principal'!B19&lt;&gt;"",CONCATENATE('Fenêtre principal'!B19,"=", 'Fenêtre principal'!D19),IF('Fenêtre principal'!D19&lt;&gt;"",'Fenêtre principal'!D19,""))</f>
-        <v>window.menu.level5.sublevel3.title=Consultar / Editar materiales</v>
+        <v>window.menu.level5.sublevel3.title=Consultar / Editar</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -32478,839 +32568,875 @@
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" t="str">
         <f>IF(Autres!B39&lt;&gt;"",CONCATENATE(Autres!B39,"=", Autres!D39),IF(Autres!D39&lt;&gt;"",Autres!D39,""))</f>
-        <v/>
+        <v>#Mensaje si la aplicación se inicia más de una vez</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" t="str">
         <f>IF(Autres!B40&lt;&gt;"",CONCATENATE(Autres!B40,"=", Autres!D40),IF(Autres!D40&lt;&gt;"",Autres!D40,""))</f>
-        <v/>
+        <v>window.alert.more.one.caerus.launch.message.title=Atención</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" t="str">
         <f>IF(Autres!B41&lt;&gt;"",CONCATENATE(Autres!B41,"=", Autres!D41),IF(Autres!D41&lt;&gt;"",Autres!D41,""))</f>
-        <v/>
+        <v>window.alert.more.one.caerus.launch.message.content=&lt;html&gt;&lt;p&gt;Caerus ya se está ejecutando.&lt;br/&gt;No puede ejecutar Caerus más de una vez.&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" t="str">
+        <f>IF(Autres!B42&lt;&gt;"",CONCATENATE(Autres!B42,"=", Autres!D42),IF(Autres!D42&lt;&gt;"",Autres!D42,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" t="str">
+        <f>IF(Autres!B43&lt;&gt;"",CONCATENATE(Autres!B43,"=", Autres!D43),IF(Autres!D43&lt;&gt;"",Autres!D43,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" t="str">
+        <f>IF(Autres!B44&lt;&gt;"",CONCATENATE(Autres!B44,"=", Autres!D44),IF(Autres!D44&lt;&gt;"",Autres!D44,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" t="str">
+        <f>IF(Autres!B45&lt;&gt;"",CONCATENATE(Autres!B45,"=", Autres!D45),IF(Autres!D45&lt;&gt;"",Autres!D45,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" t="str">
+        <f>IF(Autres!B46&lt;&gt;"",CONCATENATE(Autres!B46,"=", Autres!D46),IF(Autres!D46&lt;&gt;"",Autres!D46,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" t="str">
+        <f>IF(Autres!B47&lt;&gt;"",CONCATENATE(Autres!B47,"=", Autres!D47),IF(Autres!D47&lt;&gt;"",Autres!D47,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="str">
         <f>IF('Changer Configuration'!B2&lt;&gt;"",CONCATENATE('Changer Configuration'!B2,"=", 'Changer Configuration'!D2),IF('Changer Configuration'!D2&lt;&gt;"",'Changer Configuration'!D2,""))</f>
         <v>#Mensaje para el cambio de configuración</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" t="str">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="str">
         <f>IF('Changer Configuration'!B3&lt;&gt;"",CONCATENATE('Changer Configuration'!B3,"=", 'Changer Configuration'!D3),IF('Changer Configuration'!D3&lt;&gt;"",'Changer Configuration'!D3,""))</f>
         <v>window.change.configuration.title=Configuración actual</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" t="str">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="str">
         <f>IF('Changer Configuration'!B4&lt;&gt;"",CONCATENATE('Changer Configuration'!B4,"=", 'Changer Configuration'!D4),IF('Changer Configuration'!D4&lt;&gt;"",'Changer Configuration'!D4,""))</f>
         <v>window.change.configuration.list.label=Configuración a utilizar :</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" t="str">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" t="str">
         <f>IF('Changer Configuration'!B5&lt;&gt;"",CONCATENATE('Changer Configuration'!B5,"=", 'Changer Configuration'!D5),IF('Changer Configuration'!D5&lt;&gt;"",'Changer Configuration'!D5,""))</f>
         <v>window.change.configuration.panel.title=Cambio de configuración</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" t="str">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" t="str">
         <f>IF('Changer Configuration'!B6&lt;&gt;"",CONCATENATE('Changer Configuration'!B6,"=", 'Changer Configuration'!D6),IF('Changer Configuration'!D6&lt;&gt;"",'Changer Configuration'!D6,""))</f>
         <v>window.change.configuration.message.panel.title=Mensaje informativo</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" t="str">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" t="str">
         <f>IF('Changer Configuration'!B7&lt;&gt;"",CONCATENATE('Changer Configuration'!B7,"=", 'Changer Configuration'!D7),IF('Changer Configuration'!D7&lt;&gt;"",'Changer Configuration'!D7,""))</f>
         <v>window.change.configuration.message.content=&lt;html&gt;&lt;p&gt;La configuración de la aplicación Caerus se basa en un archivo que le permite configurar completamente el  interfaz en función de los materiales textuales creados.&lt;br/&gt;Puede modificar la configuración de los materiales y usarlos con el interfaz de Caerus, también puede agregar , modificar o eliminar configuraciones actuando en el directorio '%s'&lt;br/&gt;Pronto se agregarán ventanas gráficas a la aplicación para facilitar sus cambios&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" t="str">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" t="str">
         <f>IF('Changer Configuration'!B8&lt;&gt;"",CONCATENATE('Changer Configuration'!B8,"=", 'Changer Configuration'!D8),IF('Changer Configuration'!D8&lt;&gt;"",'Changer Configuration'!D8,""))</f>
         <v>window.change.configuration.button.apply.and.close=Elija esta configuración y cerrar</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" t="str">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" t="str">
         <f>IF('Changer Configuration'!B9&lt;&gt;"",CONCATENATE('Changer Configuration'!B9,"=", 'Changer Configuration'!D9),IF('Changer Configuration'!D9&lt;&gt;"",'Changer Configuration'!D9,""))</f>
         <v>window.change.configuration.button.close=Cerrar</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" t="str">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" t="str">
         <f>IF('Changer Configuration'!B10&lt;&gt;"",CONCATENATE('Changer Configuration'!B10,"=", 'Changer Configuration'!D10),IF('Changer Configuration'!D10&lt;&gt;"",'Changer Configuration'!D10,""))</f>
         <v>window.change.configuration.buttons.panel.title=Acciones</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" t="str">
-        <f>IF('Changer Configuration'!B11&lt;&gt;"",CONCATENATE('Changer Configuration'!B11,"=", 'Changer Configuration'!D11),IF('Changer Configuration'!D11&lt;&gt;"",'Changer Configuration'!D11,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" t="str">
-        <f>IF('Changer Configuration'!B12&lt;&gt;"",CONCATENATE('Changer Configuration'!B12,"=", 'Changer Configuration'!D12),IF('Changer Configuration'!D12&lt;&gt;"",'Changer Configuration'!D12,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" t="str">
-        <f>IF('Changer Configuration'!B13&lt;&gt;"",CONCATENATE('Changer Configuration'!B13,"=", 'Changer Configuration'!D13),IF('Changer Configuration'!D13&lt;&gt;"",'Changer Configuration'!D13,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" t="str">
-        <f>IF('Changer Configuration'!B14&lt;&gt;"",CONCATENATE('Changer Configuration'!B14,"=", 'Changer Configuration'!D14),IF('Changer Configuration'!D14&lt;&gt;"",'Changer Configuration'!D14,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A378" t="str">
-        <f>IF('Changer Configuration'!B15&lt;&gt;"",CONCATENATE('Changer Configuration'!B15,"=", 'Changer Configuration'!D15),IF('Changer Configuration'!D15&lt;&gt;"",'Changer Configuration'!D15,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" t="str">
-        <f>IF('Changer Configuration'!B16&lt;&gt;"",CONCATENATE('Changer Configuration'!B16,"=", 'Changer Configuration'!D16),IF('Changer Configuration'!D16&lt;&gt;"",'Changer Configuration'!D16,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" t="str">
-        <f>IF('Changer Configuration'!B17&lt;&gt;"",CONCATENATE('Changer Configuration'!B17,"=", 'Changer Configuration'!D17),IF('Changer Configuration'!D17&lt;&gt;"",'Changer Configuration'!D17,""))</f>
+        <f>IF('Changer Configuration'!B11&lt;&gt;"",CONCATENATE('Changer Configuration'!B11,"=", 'Changer Configuration'!D11),IF('Changer Configuration'!D11&lt;&gt;"",'Changer Configuration'!D11,""))</f>
         <v/>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" t="str">
-        <f>IF('Changer Configuration'!B18&lt;&gt;"",CONCATENATE('Changer Configuration'!B18,"=", 'Changer Configuration'!D18),IF('Changer Configuration'!D18&lt;&gt;"",'Changer Configuration'!D18,""))</f>
+        <f>IF('Changer Configuration'!B12&lt;&gt;"",CONCATENATE('Changer Configuration'!B12,"=", 'Changer Configuration'!D12),IF('Changer Configuration'!D12&lt;&gt;"",'Changer Configuration'!D12,""))</f>
         <v/>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" t="str">
-        <f>IF('Changer Configuration'!B19&lt;&gt;"",CONCATENATE('Changer Configuration'!B19,"=", 'Changer Configuration'!D19),IF('Changer Configuration'!D19&lt;&gt;"",'Changer Configuration'!D19,""))</f>
+        <f>IF('Changer Configuration'!B13&lt;&gt;"",CONCATENATE('Changer Configuration'!B13,"=", 'Changer Configuration'!D13),IF('Changer Configuration'!D13&lt;&gt;"",'Changer Configuration'!D13,""))</f>
         <v/>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" t="str">
-        <f>IF('Changer Configuration'!B20&lt;&gt;"",CONCATENATE('Changer Configuration'!B20,"=", 'Changer Configuration'!C20),IF('Changer Configuration'!C20&lt;&gt;"",'Changer Configuration'!C20,""))</f>
+        <f>IF('Changer Configuration'!B14&lt;&gt;"",CONCATENATE('Changer Configuration'!B14,"=", 'Changer Configuration'!D14),IF('Changer Configuration'!D14&lt;&gt;"",'Changer Configuration'!D14,""))</f>
         <v/>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" t="str">
-        <f>IF('Changer Configuration'!B21&lt;&gt;"",CONCATENATE('Changer Configuration'!B21,"=", 'Changer Configuration'!C21),IF('Changer Configuration'!C21&lt;&gt;"",'Changer Configuration'!C21,""))</f>
+        <f>IF('Changer Configuration'!B15&lt;&gt;"",CONCATENATE('Changer Configuration'!B15,"=", 'Changer Configuration'!D15),IF('Changer Configuration'!D15&lt;&gt;"",'Changer Configuration'!D15,""))</f>
         <v/>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" t="str">
-        <f>IF('Changer Configuration'!B22&lt;&gt;"",CONCATENATE('Changer Configuration'!B22,"=", 'Changer Configuration'!C22),IF('Changer Configuration'!C22&lt;&gt;"",'Changer Configuration'!C22,""))</f>
+        <f>IF('Changer Configuration'!B16&lt;&gt;"",CONCATENATE('Changer Configuration'!B16,"=", 'Changer Configuration'!D16),IF('Changer Configuration'!D16&lt;&gt;"",'Changer Configuration'!D16,""))</f>
         <v/>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" t="str">
-        <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE('Changer Configuration'!B23,"=", 'Changer Configuration'!C23),IF('Changer Configuration'!C23&lt;&gt;"",'Changer Configuration'!C23,""))</f>
+        <f>IF('Changer Configuration'!B17&lt;&gt;"",CONCATENATE('Changer Configuration'!B17,"=", 'Changer Configuration'!D17),IF('Changer Configuration'!D17&lt;&gt;"",'Changer Configuration'!D17,""))</f>
         <v/>
       </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A387" t="str">
+        <f>IF('Changer Configuration'!B18&lt;&gt;"",CONCATENATE('Changer Configuration'!B18,"=", 'Changer Configuration'!D18),IF('Changer Configuration'!D18&lt;&gt;"",'Changer Configuration'!D18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" t="str">
+        <f>IF('Changer Configuration'!B19&lt;&gt;"",CONCATENATE('Changer Configuration'!B19,"=", 'Changer Configuration'!D19),IF('Changer Configuration'!D19&lt;&gt;"",'Changer Configuration'!D19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" t="str">
+        <f>IF('Changer Configuration'!B20&lt;&gt;"",CONCATENATE('Changer Configuration'!B20,"=", 'Changer Configuration'!C20),IF('Changer Configuration'!C20&lt;&gt;"",'Changer Configuration'!C20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" t="str">
+        <f>IF('Changer Configuration'!B21&lt;&gt;"",CONCATENATE('Changer Configuration'!B21,"=", 'Changer Configuration'!C21),IF('Changer Configuration'!C21&lt;&gt;"",'Changer Configuration'!C21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" t="str">
+        <f>IF('Changer Configuration'!B22&lt;&gt;"",CONCATENATE('Changer Configuration'!B22,"=", 'Changer Configuration'!C22),IF('Changer Configuration'!C22&lt;&gt;"",'Changer Configuration'!C22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" t="str">
+        <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE('Changer Configuration'!B23,"=", 'Changer Configuration'!C23),IF('Changer Configuration'!C23&lt;&gt;"",'Changer Configuration'!C23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" t="str">
         <f>IF('A propos'!B2&lt;&gt;"",CONCATENATE('A propos'!B2,"=", 'A propos'!D2),IF('A propos'!D2&lt;&gt;"",'A propos'!D2,""))</f>
         <v>#Mensaje para el cambio de configuración</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" t="str">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" t="str">
         <f>IF('A propos'!B3&lt;&gt;"",CONCATENATE('A propos'!B3,"=", 'A propos'!D3),IF('A propos'!D3&lt;&gt;"",'A propos'!D3,""))</f>
         <v>window.about.title=Acerca de</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" t="str">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" t="str">
         <f>IF('A propos'!B4&lt;&gt;"",CONCATENATE('A propos'!B4,"=", 'A propos'!D4),IF('A propos'!D4&lt;&gt;"",'A propos'!D4,""))</f>
         <v>window.about.message.content=&lt;html&gt;&lt;p&gt;&lt;b&gt;&lt;u&gt;Acerca de la application&lt;/b&gt;&lt;/u&gt;&lt;br /&gt;&lt;br /&gt;&lt;u&gt;Nombre de la application :&lt;/u&gt; Caerus&lt;BR /&gt;&lt;u&gt;Versión :&lt;/u&gt; 1.1.2&lt;br /&gt;&lt;u&gt;Editor :&lt;/u&gt; Jeremy, Leda&lt;br/&gt;&lt;u&gt;Sitio web :&lt;/u&gt; https://github.com/Jeremy-Leda/Caerus&lt;/p&gt;&lt;/html&gt;</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" t="str">
-        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE('A propos'!B5,"=", 'A propos'!D5),IF('A propos'!D5&lt;&gt;"",'A propos'!D5,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" t="str">
-        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE('A propos'!B6,"=", 'A propos'!D6),IF('A propos'!D6&lt;&gt;"",'A propos'!D6,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" t="str">
-        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE('A propos'!B7,"=", 'A propos'!D7),IF('A propos'!D7&lt;&gt;"",'A propos'!D7,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A393" t="str">
-        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE('A propos'!B8,"=", 'A propos'!D8),IF('A propos'!D8&lt;&gt;"",'A propos'!D8,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" t="str">
-        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE('A propos'!B9,"=", 'A propos'!D9),IF('A propos'!D9&lt;&gt;"",'A propos'!D9,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" t="str">
-        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE('A propos'!B10,"=", 'A propos'!D10),IF('A propos'!D10&lt;&gt;"",'A propos'!D10,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" t="str">
-        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE('A propos'!B11,"=", 'A propos'!D11),IF('A propos'!D11&lt;&gt;"",'A propos'!D11,""))</f>
+        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE('A propos'!B5,"=", 'A propos'!D5),IF('A propos'!D5&lt;&gt;"",'A propos'!D5,""))</f>
         <v/>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" t="str">
-        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE('A propos'!B12,"=", 'A propos'!D12),IF('A propos'!D12&lt;&gt;"",'A propos'!D12,""))</f>
+        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE('A propos'!B6,"=", 'A propos'!D6),IF('A propos'!D6&lt;&gt;"",'A propos'!D6,""))</f>
         <v/>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" t="str">
-        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE('A propos'!B13,"=", 'A propos'!D13),IF('A propos'!D13&lt;&gt;"",'A propos'!D13,""))</f>
+        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE('A propos'!B7,"=", 'A propos'!D7),IF('A propos'!D7&lt;&gt;"",'A propos'!D7,""))</f>
         <v/>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" t="str">
-        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE('A propos'!B14,"=", 'A propos'!D14),IF('A propos'!D14&lt;&gt;"",'A propos'!D14,""))</f>
+        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE('A propos'!B8,"=", 'A propos'!D8),IF('A propos'!D8&lt;&gt;"",'A propos'!D8,""))</f>
         <v/>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" t="str">
-        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE('A propos'!B15,"=", 'A propos'!D15),IF('A propos'!D15&lt;&gt;"",'A propos'!D15,""))</f>
+        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE('A propos'!B9,"=", 'A propos'!D9),IF('A propos'!D9&lt;&gt;"",'A propos'!D9,""))</f>
         <v/>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" t="str">
-        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE('A propos'!B16,"=", 'A propos'!D16),IF('A propos'!D16&lt;&gt;"",'A propos'!D16,""))</f>
+        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE('A propos'!B10,"=", 'A propos'!D10),IF('A propos'!D10&lt;&gt;"",'A propos'!D10,""))</f>
         <v/>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402" t="str">
-        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!D17),IF('A propos'!D17&lt;&gt;"",'A propos'!D17,""))</f>
+        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE('A propos'!B11,"=", 'A propos'!D11),IF('A propos'!D11&lt;&gt;"",'A propos'!D11,""))</f>
         <v/>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" t="str">
-        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!D18),IF('A propos'!D18&lt;&gt;"",'A propos'!D18,""))</f>
+        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE('A propos'!B12,"=", 'A propos'!D12),IF('A propos'!D12&lt;&gt;"",'A propos'!D12,""))</f>
         <v/>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" t="str">
-        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!D19),IF('A propos'!D19&lt;&gt;"",'A propos'!D19,""))</f>
+        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE('A propos'!B13,"=", 'A propos'!D13),IF('A propos'!D13&lt;&gt;"",'A propos'!D13,""))</f>
         <v/>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A405" t="str">
-        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!D18),IF('A propos'!D18&lt;&gt;"",'A propos'!D18,""))</f>
+        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE('A propos'!B14,"=", 'A propos'!D14),IF('A propos'!D14&lt;&gt;"",'A propos'!D14,""))</f>
         <v/>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" t="str">
-        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!D19),IF('A propos'!D19&lt;&gt;"",'A propos'!D19,""))</f>
+        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE('A propos'!B15,"=", 'A propos'!D15),IF('A propos'!D15&lt;&gt;"",'A propos'!D15,""))</f>
         <v/>
       </c>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A407" t="str">
-        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE('A propos'!B20,"=", 'A propos'!D20),IF('A propos'!D20&lt;&gt;"",'A propos'!D20,""))</f>
+        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE('A propos'!B16,"=", 'A propos'!D16),IF('A propos'!D16&lt;&gt;"",'A propos'!D16,""))</f>
         <v/>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A408" t="str">
+        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE('A propos'!B17,"=", 'A propos'!D17),IF('A propos'!D17&lt;&gt;"",'A propos'!D17,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" t="str">
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!D18),IF('A propos'!D18&lt;&gt;"",'A propos'!D18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" t="str">
+        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!D19),IF('A propos'!D19&lt;&gt;"",'A propos'!D19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" t="str">
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE('A propos'!B18,"=", 'A propos'!D18),IF('A propos'!D18&lt;&gt;"",'A propos'!D18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" t="str">
+        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE('A propos'!B19,"=", 'A propos'!D19),IF('A propos'!D19&lt;&gt;"",'A propos'!D19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" t="str">
+        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE('A propos'!B20,"=", 'A propos'!D20),IF('A propos'!D20&lt;&gt;"",'A propos'!D20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" t="str">
         <f>IF('Export Document Materiel'!B2&lt;&gt;"",CONCATENATE('Export Document Materiel'!B2,"=", 'Export Document Materiel'!D2),IF('Export Document Materiel'!D2&lt;&gt;"",'Export Document Materiel'!D2,""))</f>
         <v>#Mensaje para el cambio de configuración</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A409" t="str">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" t="str">
         <f>IF('Export Document Materiel'!B3&lt;&gt;"",CONCATENATE('Export Document Materiel'!B3,"=", 'Export Document Materiel'!D3),IF('Export Document Materiel'!D3&lt;&gt;"",'Export Document Materiel'!D3,""))</f>
         <v>window.export.document.title=Exportar documentos/materiales</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" t="str">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" t="str">
         <f>IF('Export Document Materiel'!B4&lt;&gt;"",CONCATENATE('Export Document Materiel'!B4,"=", 'Export Document Materiel'!D4),IF('Export Document Materiel'!D4&lt;&gt;"",'Export Document Materiel'!D4,""))</f>
         <v>window.export.document.choose.directory.panel.title=Elección de la carpeta de destino</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" t="str">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" t="str">
         <f>IF('Export Document Materiel'!B5&lt;&gt;"",CONCATENATE('Export Document Materiel'!B5,"=", 'Export Document Materiel'!D5),IF('Export Document Materiel'!D5&lt;&gt;"",'Export Document Materiel'!D5,""))</f>
         <v>window.export.document.choose.directory.label=Carpeta de destino</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" t="str">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="str">
         <f>IF('Export Document Materiel'!B6&lt;&gt;"",CONCATENATE('Export Document Materiel'!B6,"=", 'Export Document Materiel'!D6),IF('Export Document Materiel'!D6&lt;&gt;"",'Export Document Materiel'!D6,""))</f>
         <v>window.export.document.mode.panel.title=Elección de los datos a exportar</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" t="str">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" t="str">
         <f>IF('Export Document Materiel'!B7&lt;&gt;"",CONCATENATE('Export Document Materiel'!B7,"=", 'Export Document Materiel'!D7),IF('Export Document Materiel'!D7&lt;&gt;"",'Export Document Materiel'!D7,""))</f>
         <v>window.export.document.mode.document.label=Un documento</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" t="str">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" t="str">
         <f>IF('Export Document Materiel'!B8&lt;&gt;"",CONCATENATE('Export Document Materiel'!B8,"=", 'Export Document Materiel'!D8),IF('Export Document Materiel'!D8&lt;&gt;"",'Export Document Materiel'!D8,""))</f>
         <v>window.export.document.mode.all.documents.label=Todos documentos</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415" t="str">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" t="str">
         <f>IF('Export Document Materiel'!B9&lt;&gt;"",CONCATENATE('Export Document Materiel'!B9,"=", 'Export Document Materiel'!D9),IF('Export Document Materiel'!D9&lt;&gt;"",'Export Document Materiel'!D9,""))</f>
         <v>window.export.document.mode.result.search.label=El resultado de la búsqueda</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" t="str">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" t="str">
         <f>IF('Export Document Materiel'!B10&lt;&gt;"",CONCATENATE('Export Document Materiel'!B10,"=", 'Export Document Materiel'!D10),IF('Export Document Materiel'!D10&lt;&gt;"",'Export Document Materiel'!D10,""))</f>
         <v>window.export.document.choose.document.panel.title=Elección del documento a exportar</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" t="str">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" t="str">
         <f>IF('Export Document Materiel'!B11&lt;&gt;"",CONCATENATE('Export Document Materiel'!B11,"=", 'Export Document Materiel'!D11),IF('Export Document Materiel'!D11&lt;&gt;"",'Export Document Materiel'!D11,""))</f>
         <v>window.export.document.choose.document.label=Documento para exportar :</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418" t="str">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" t="str">
         <f>IF('Export Document Materiel'!B12&lt;&gt;"",CONCATENATE('Export Document Materiel'!B12,"=", 'Export Document Materiel'!D12),IF('Export Document Materiel'!D12&lt;&gt;"",'Export Document Materiel'!D12,""))</f>
         <v>window.export.document.choose.file.panel.title=Elección del nombre del documento</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" t="str">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" t="str">
         <f>IF('Export Document Materiel'!B13&lt;&gt;"",CONCATENATE('Export Document Materiel'!B13,"=", 'Export Document Materiel'!D13),IF('Export Document Materiel'!D13&lt;&gt;"",'Export Document Materiel'!D13,""))</f>
         <v xml:space="preserve">window.export.document.choose.file.label=Nombre del documento para el resultado de la búsqueda : </v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A420" t="str">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" t="str">
         <f>IF('Export Document Materiel'!B14&lt;&gt;"",CONCATENATE('Export Document Materiel'!B14,"=", 'Export Document Materiel'!D14),IF('Export Document Materiel'!D14&lt;&gt;"",'Export Document Materiel'!D14,""))</f>
         <v>window.export.document.button.panel.title=Acciones</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" t="str">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" t="str">
         <f>IF('Export Document Materiel'!B15&lt;&gt;"",CONCATENATE('Export Document Materiel'!B15,"=", 'Export Document Materiel'!D15),IF('Export Document Materiel'!D15&lt;&gt;"",'Export Document Materiel'!D15,""))</f>
         <v>window.export.document.button.export.label=Exportar y cerrar</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" t="str">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" t="str">
         <f>IF('Export Document Materiel'!B16&lt;&gt;"",CONCATENATE('Export Document Materiel'!B16,"=", 'Export Document Materiel'!D16),IF('Export Document Materiel'!D16&lt;&gt;"",'Export Document Materiel'!D16,""))</f>
         <v>window.export.document.information.message.title=Exportación completada</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" t="str">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" t="str">
         <f>IF('Export Document Materiel'!B17&lt;&gt;"",CONCATENATE('Export Document Materiel'!B17,"=", 'Export Document Materiel'!D17),IF('Export Document Materiel'!D17&lt;&gt;"",'Export Document Materiel'!D17,""))</f>
         <v>window.export.document.information.message=&lt;HTML&gt;&lt;P&gt;Exportación realizada con éxito&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" t="str">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" t="str">
         <f>IF('Export Document Materiel'!B18&lt;&gt;"",CONCATENATE('Export Document Materiel'!B18,"=", 'Export Document Materiel'!D18),IF('Export Document Materiel'!D18&lt;&gt;"",'Export Document Materiel'!D18,""))</f>
         <v>window.export.document.button.close.label=Cerrar</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" t="str">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" t="str">
         <f>IF('Export Document Materiel'!B19&lt;&gt;"",CONCATENATE('Export Document Materiel'!B19,"=", 'Export Document Materiel'!D19),IF('Export Document Materiel'!D19&lt;&gt;"",'Export Document Materiel'!D19,""))</f>
         <v>window.export.document.choose.directory.dialog.title=Seleccione la carpeta de destino</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" t="str">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" t="str">
         <f>IF('Export Document Materiel'!B20&lt;&gt;"",CONCATENATE('Export Document Materiel'!B20,"=", 'Export Document Materiel'!D20),IF('Export Document Materiel'!D20&lt;&gt;"",'Export Document Materiel'!D20,""))</f>
         <v>window.export.document.information.search.message=&lt;HTML&gt;&lt;P&gt;Exportación realizada con éxito&lt;BR/&gt;A título informativo, el documento no contiene datos de cabecera&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" t="str">
-        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE('Export Document Materiel'!B21,"=", 'Export Document Materiel'!D21),IF('Export Document Materiel'!D21&lt;&gt;"",'Export Document Materiel'!D21,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" t="str">
-        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE('Export Document Materiel'!B22,"=", 'Export Document Materiel'!D22),IF('Export Document Materiel'!D22&lt;&gt;"",'Export Document Materiel'!D22,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A429" t="str">
-        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE('Export Document Materiel'!B23,"=", 'Export Document Materiel'!D23),IF('Export Document Materiel'!D23&lt;&gt;"",'Export Document Materiel'!D23,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" t="str">
-        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE('Export Document Materiel'!B24,"=", 'Export Document Materiel'!D24),IF('Export Document Materiel'!D24&lt;&gt;"",'Export Document Materiel'!D24,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" t="str">
-        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE('Export Document Materiel'!B25,"=", 'Export Document Materiel'!D25),IF('Export Document Materiel'!D25&lt;&gt;"",'Export Document Materiel'!D25,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A432" t="str">
-        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE('Export Document Materiel'!B26,"=", 'Export Document Materiel'!D26),IF('Export Document Materiel'!D26&lt;&gt;"",'Export Document Materiel'!D26,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" t="str">
-        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE('Export Document Materiel'!B27,"=", 'Export Document Materiel'!D27),IF('Export Document Materiel'!D27&lt;&gt;"",'Export Document Materiel'!D27,""))</f>
+        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE('Export Document Materiel'!B21,"=", 'Export Document Materiel'!D21),IF('Export Document Materiel'!D21&lt;&gt;"",'Export Document Materiel'!D21,""))</f>
         <v/>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" t="str">
-        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE('Export Document Materiel'!B28,"=", 'Export Document Materiel'!D28),IF('Export Document Materiel'!D28&lt;&gt;"",'Export Document Materiel'!D28,""))</f>
+        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE('Export Document Materiel'!B22,"=", 'Export Document Materiel'!D22),IF('Export Document Materiel'!D22&lt;&gt;"",'Export Document Materiel'!D22,""))</f>
         <v/>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A435" t="str">
-        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE('Export Document Materiel'!B29,"=", 'Export Document Materiel'!D29),IF('Export Document Materiel'!D29&lt;&gt;"",'Export Document Materiel'!D29,""))</f>
+        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE('Export Document Materiel'!B23,"=", 'Export Document Materiel'!D23),IF('Export Document Materiel'!D23&lt;&gt;"",'Export Document Materiel'!D23,""))</f>
         <v/>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" t="str">
-        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE('Export Document Materiel'!B30,"=", 'Export Document Materiel'!D30),IF('Export Document Materiel'!D30&lt;&gt;"",'Export Document Materiel'!D30,""))</f>
+        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE('Export Document Materiel'!B24,"=", 'Export Document Materiel'!D24),IF('Export Document Materiel'!D24&lt;&gt;"",'Export Document Materiel'!D24,""))</f>
         <v/>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" t="str">
-        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE('Export Document Materiel'!B31,"=", 'Export Document Materiel'!D31),IF('Export Document Materiel'!D31&lt;&gt;"",'Export Document Materiel'!D31,""))</f>
+        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE('Export Document Materiel'!B25,"=", 'Export Document Materiel'!D25),IF('Export Document Materiel'!D25&lt;&gt;"",'Export Document Materiel'!D25,""))</f>
         <v/>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A438" t="str">
-        <f>IF('Export Document Materiel'!B32&lt;&gt;"",CONCATENATE('Export Document Materiel'!B32,"=", 'Export Document Materiel'!D32),IF('Export Document Materiel'!D32&lt;&gt;"",'Export Document Materiel'!D32,""))</f>
+        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE('Export Document Materiel'!B26,"=", 'Export Document Materiel'!D26),IF('Export Document Materiel'!D26&lt;&gt;"",'Export Document Materiel'!D26,""))</f>
         <v/>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" t="str">
-        <f>IF('Export Document Materiel'!B33&lt;&gt;"",CONCATENATE('Export Document Materiel'!B33,"=", 'Export Document Materiel'!D33),IF('Export Document Materiel'!D33&lt;&gt;"",'Export Document Materiel'!D33,""))</f>
+        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE('Export Document Materiel'!B27,"=", 'Export Document Materiel'!D27),IF('Export Document Materiel'!D27&lt;&gt;"",'Export Document Materiel'!D27,""))</f>
         <v/>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A440" t="str">
-        <f>IF('Export Document Materiel'!B34&lt;&gt;"",CONCATENATE('Export Document Materiel'!B34,"=", 'Export Document Materiel'!D34),IF('Export Document Materiel'!D34&lt;&gt;"",'Export Document Materiel'!D34,""))</f>
+        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE('Export Document Materiel'!B28,"=", 'Export Document Materiel'!D28),IF('Export Document Materiel'!D28&lt;&gt;"",'Export Document Materiel'!D28,""))</f>
         <v/>
       </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A441" t="str">
+        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE('Export Document Materiel'!B29,"=", 'Export Document Materiel'!D29),IF('Export Document Materiel'!D29&lt;&gt;"",'Export Document Materiel'!D29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" t="str">
+        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE('Export Document Materiel'!B30,"=", 'Export Document Materiel'!D30),IF('Export Document Materiel'!D30&lt;&gt;"",'Export Document Materiel'!D30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" t="str">
+        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE('Export Document Materiel'!B31,"=", 'Export Document Materiel'!D31),IF('Export Document Materiel'!D31&lt;&gt;"",'Export Document Materiel'!D31,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" t="str">
+        <f>IF('Export Document Materiel'!B32&lt;&gt;"",CONCATENATE('Export Document Materiel'!B32,"=", 'Export Document Materiel'!D32),IF('Export Document Materiel'!D32&lt;&gt;"",'Export Document Materiel'!D32,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" t="str">
+        <f>IF('Export Document Materiel'!B33&lt;&gt;"",CONCATENATE('Export Document Materiel'!B33,"=", 'Export Document Materiel'!D33),IF('Export Document Materiel'!D33&lt;&gt;"",'Export Document Materiel'!D33,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" t="str">
+        <f>IF('Export Document Materiel'!B34&lt;&gt;"",CONCATENATE('Export Document Materiel'!B34,"=", 'Export Document Materiel'!D34),IF('Export Document Materiel'!D34&lt;&gt;"",'Export Document Materiel'!D34,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" t="str">
         <f>IF('Erreur incoherence'!B2&lt;&gt;"",CONCATENATE('Erreur incoherence'!B2,"=", 'Erreur incoherence'!D2),IF('Erreur incoherence'!D2&lt;&gt;"",'Erreur incoherence'!D2,""))</f>
         <v>#Mensaje para el cambio de configuración</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" t="str">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" t="str">
         <f>IF('Erreur incoherence'!B3&lt;&gt;"",CONCATENATE('Erreur incoherence'!B3,"=", 'Erreur incoherence'!D3),IF('Erreur incoherence'!D3&lt;&gt;"",'Erreur incoherence'!D3,""))</f>
         <v>window.error.inconsistency.title=Errores de duplicados</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" t="str">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" t="str">
         <f>IF('Erreur incoherence'!B4&lt;&gt;"",CONCATENATE('Erreur incoherence'!B4,"=", 'Erreur incoherence'!D4),IF('Erreur incoherence'!D4&lt;&gt;"",'Erreur incoherence'!D4,""))</f>
         <v>window.error.inconsistency.panel.title=Lista de incoherencias</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" t="str">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" t="str">
         <f>IF('Erreur incoherence'!B5&lt;&gt;"",CONCATENATE('Erreur incoherence'!B5,"=", 'Erreur incoherence'!D5),IF('Erreur incoherence'!D5&lt;&gt;"",'Erreur incoherence'!D5,""))</f>
         <v>window.error.inconsistency.field.label=Etiqueta :</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" t="str">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" t="str">
         <f>IF('Erreur incoherence'!B6&lt;&gt;"",CONCATENATE('Erreur incoherence'!B6,"=", 'Erreur incoherence'!D6),IF('Erreur incoherence'!D6&lt;&gt;"",'Erreur incoherence'!D6,""))</f>
         <v>window.error.inconsistency.number.line.label=Número de línea :</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" t="str">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" t="str">
         <f>IF('Erreur incoherence'!B7&lt;&gt;"",CONCATENATE('Erreur incoherence'!B7,"=", 'Erreur incoherence'!D7),IF('Erreur incoherence'!D7&lt;&gt;"",'Erreur incoherence'!D7,""))</f>
         <v xml:space="preserve">window.error.inconsistency.name.file.label=Nombre del documento : </v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A447" t="str">
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" t="str">
         <f>IF('Erreur incoherence'!B8&lt;&gt;"",CONCATENATE('Erreur incoherence'!B8,"=", 'Erreur incoherence'!D8),IF('Erreur incoherence'!D8&lt;&gt;"",'Erreur incoherence'!D8,""))</f>
         <v>window.error.inconsistency.message.panel.title=Mensaje informativo</v>
       </c>
     </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" t="str">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" t="str">
         <f>IF('Erreur incoherence'!B9&lt;&gt;"",CONCATENATE('Erreur incoherence'!B9,"=", 'Erreur incoherence'!D9),IF('Erreur incoherence'!D9&lt;&gt;"",'Erreur incoherence'!D9,""))</f>
         <v>window.error.inconsistency.message=&lt;HTML&gt;&lt;P&gt;Vuelva a cargar los documentos corregidos.&lt;BR/&gt;Los desfases de información pueden hacer&lt;BR/&gt;que se detecten nuevos errores.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" t="str">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" t="str">
         <f>IF('Erreur incoherence'!B10&lt;&gt;"",CONCATENATE('Erreur incoherence'!B10,"=", 'Erreur incoherence'!D10),IF('Erreur incoherence'!D10&lt;&gt;"",'Erreur incoherence'!D10,""))</f>
         <v>window.error.inconsistency.buttons.panel.title=Acciones</v>
       </c>
     </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" t="str">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" t="str">
         <f>IF('Erreur incoherence'!B11&lt;&gt;"",CONCATENATE('Erreur incoherence'!B11,"=", 'Erreur incoherence'!D11),IF('Erreur incoherence'!D11&lt;&gt;"",'Erreur incoherence'!D11,""))</f>
         <v>window.error.inconsistency.buttons.close.button.label=Cerrar y cargar lors documentos</v>
       </c>
     </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" t="str">
-        <f>IF('Erreur incoherence'!B12&lt;&gt;"",CONCATENATE('Erreur incoherence'!B12,"=", 'Erreur incoherence'!D12),IF('Erreur incoherence'!D12&lt;&gt;"",'Erreur incoherence'!D12,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" t="str">
-        <f>IF('Erreur incoherence'!B13&lt;&gt;"",CONCATENATE('Erreur incoherence'!B13,"=", 'Erreur incoherence'!D13),IF('Erreur incoherence'!D13&lt;&gt;"",'Erreur incoherence'!D13,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453" t="str">
-        <f>IF('Erreur incoherence'!B14&lt;&gt;"",CONCATENATE('Erreur incoherence'!B14,"=", 'Erreur incoherence'!D14),IF('Erreur incoherence'!D14&lt;&gt;"",'Erreur incoherence'!D14,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A454" t="str">
-        <f>IF('Erreur incoherence'!B15&lt;&gt;"",CONCATENATE('Erreur incoherence'!B15,"=", 'Erreur incoherence'!D15),IF('Erreur incoherence'!D15&lt;&gt;"",'Erreur incoherence'!D15,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A455" t="str">
-        <f>IF('Erreur incoherence'!B16&lt;&gt;"",CONCATENATE('Erreur incoherence'!B16,"=", 'Erreur incoherence'!D16),IF('Erreur incoherence'!D16&lt;&gt;"",'Erreur incoherence'!D16,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456" t="str">
-        <f>IF('Erreur incoherence'!B17&lt;&gt;"",CONCATENATE('Erreur incoherence'!B17,"=", 'Erreur incoherence'!D17),IF('Erreur incoherence'!D17&lt;&gt;"",'Erreur incoherence'!D17,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A457" t="str">
-        <f>IF('Erreur incoherence'!B18&lt;&gt;"",CONCATENATE('Erreur incoherence'!B18,"=", 'Erreur incoherence'!D18),IF('Erreur incoherence'!D18&lt;&gt;"",'Erreur incoherence'!D18,""))</f>
+        <f>IF('Erreur incoherence'!B12&lt;&gt;"",CONCATENATE('Erreur incoherence'!B12,"=", 'Erreur incoherence'!D12),IF('Erreur incoherence'!D12&lt;&gt;"",'Erreur incoherence'!D12,""))</f>
         <v/>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" t="str">
-        <f>IF('Erreur incoherence'!B19&lt;&gt;"",CONCATENATE('Erreur incoherence'!B19,"=", 'Erreur incoherence'!D19),IF('Erreur incoherence'!D19&lt;&gt;"",'Erreur incoherence'!D19,""))</f>
+        <f>IF('Erreur incoherence'!B13&lt;&gt;"",CONCATENATE('Erreur incoherence'!B13,"=", 'Erreur incoherence'!D13),IF('Erreur incoherence'!D13&lt;&gt;"",'Erreur incoherence'!D13,""))</f>
         <v/>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" t="str">
-        <f>IF('Erreur incoherence'!B20&lt;&gt;"",CONCATENATE('Erreur incoherence'!B20,"=", 'Erreur incoherence'!D20),IF('Erreur incoherence'!D20&lt;&gt;"",'Erreur incoherence'!D20,""))</f>
+        <f>IF('Erreur incoherence'!B14&lt;&gt;"",CONCATENATE('Erreur incoherence'!B14,"=", 'Erreur incoherence'!D14),IF('Erreur incoherence'!D14&lt;&gt;"",'Erreur incoherence'!D14,""))</f>
         <v/>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" t="str">
-        <f>IF('Erreur incoherence'!B21&lt;&gt;"",CONCATENATE('Erreur incoherence'!B21,"=", 'Erreur incoherence'!D21),IF('Erreur incoherence'!D21&lt;&gt;"",'Erreur incoherence'!D21,""))</f>
+        <f>IF('Erreur incoherence'!B15&lt;&gt;"",CONCATENATE('Erreur incoherence'!B15,"=", 'Erreur incoherence'!D15),IF('Erreur incoherence'!D15&lt;&gt;"",'Erreur incoherence'!D15,""))</f>
         <v/>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" t="str">
-        <f>IF('Erreur incoherence'!B22&lt;&gt;"",CONCATENATE('Erreur incoherence'!B22,"=", 'Erreur incoherence'!D22),IF('Erreur incoherence'!D22&lt;&gt;"",'Erreur incoherence'!D22,""))</f>
+        <f>IF('Erreur incoherence'!B16&lt;&gt;"",CONCATENATE('Erreur incoherence'!B16,"=", 'Erreur incoherence'!D16),IF('Erreur incoherence'!D16&lt;&gt;"",'Erreur incoherence'!D16,""))</f>
         <v/>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" t="str">
-        <f>IF('Erreur incoherence'!B23&lt;&gt;"",CONCATENATE('Erreur incoherence'!B23,"=", 'Erreur incoherence'!D23),IF('Erreur incoherence'!D23&lt;&gt;"",'Erreur incoherence'!D23,""))</f>
+        <f>IF('Erreur incoherence'!B17&lt;&gt;"",CONCATENATE('Erreur incoherence'!B17,"=", 'Erreur incoherence'!D17),IF('Erreur incoherence'!D17&lt;&gt;"",'Erreur incoherence'!D17,""))</f>
         <v/>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A463" t="str">
-        <f>IF('Erreur incoherence'!B24&lt;&gt;"",CONCATENATE('Erreur incoherence'!B24,"=", 'Erreur incoherence'!D24),IF('Erreur incoherence'!D24&lt;&gt;"",'Erreur incoherence'!D24,""))</f>
+        <f>IF('Erreur incoherence'!B18&lt;&gt;"",CONCATENATE('Erreur incoherence'!B18,"=", 'Erreur incoherence'!D18),IF('Erreur incoherence'!D18&lt;&gt;"",'Erreur incoherence'!D18,""))</f>
         <v/>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" t="str">
-        <f>IF('Erreur incoherence'!B25&lt;&gt;"",CONCATENATE('Erreur incoherence'!B25,"=", 'Erreur incoherence'!D25),IF('Erreur incoherence'!D25&lt;&gt;"",'Erreur incoherence'!D25,""))</f>
+        <f>IF('Erreur incoherence'!B19&lt;&gt;"",CONCATENATE('Erreur incoherence'!B19,"=", 'Erreur incoherence'!D19),IF('Erreur incoherence'!D19&lt;&gt;"",'Erreur incoherence'!D19,""))</f>
         <v/>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A465" t="str">
-        <f>IF('Erreur incoherence'!B26&lt;&gt;"",CONCATENATE('Erreur incoherence'!B26,"=", 'Erreur incoherence'!D26),IF('Erreur incoherence'!D26&lt;&gt;"",'Erreur incoherence'!D26,""))</f>
+        <f>IF('Erreur incoherence'!B20&lt;&gt;"",CONCATENATE('Erreur incoherence'!B20,"=", 'Erreur incoherence'!D20),IF('Erreur incoherence'!D20&lt;&gt;"",'Erreur incoherence'!D20,""))</f>
         <v/>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466" t="str">
-        <f>IF('Erreur incoherence'!B27&lt;&gt;"",CONCATENATE('Erreur incoherence'!B27,"=", 'Erreur incoherence'!D27),IF('Erreur incoherence'!D27&lt;&gt;"",'Erreur incoherence'!D27,""))</f>
+        <f>IF('Erreur incoherence'!B21&lt;&gt;"",CONCATENATE('Erreur incoherence'!B21,"=", 'Erreur incoherence'!D21),IF('Erreur incoherence'!D21&lt;&gt;"",'Erreur incoherence'!D21,""))</f>
         <v/>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A467" t="str">
-        <f>IF('Erreur incoherence'!B28&lt;&gt;"",CONCATENATE('Erreur incoherence'!B28,"=", 'Erreur incoherence'!D28),IF('Erreur incoherence'!D28&lt;&gt;"",'Erreur incoherence'!D28,""))</f>
+        <f>IF('Erreur incoherence'!B22&lt;&gt;"",CONCATENATE('Erreur incoherence'!B22,"=", 'Erreur incoherence'!D22),IF('Erreur incoherence'!D22&lt;&gt;"",'Erreur incoherence'!D22,""))</f>
         <v/>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468" t="str">
-        <f>IF('Erreur incoherence'!B29&lt;&gt;"",CONCATENATE('Erreur incoherence'!B29,"=", 'Erreur incoherence'!D29),IF('Erreur incoherence'!D29&lt;&gt;"",'Erreur incoherence'!D29,""))</f>
+        <f>IF('Erreur incoherence'!B23&lt;&gt;"",CONCATENATE('Erreur incoherence'!B23,"=", 'Erreur incoherence'!D23),IF('Erreur incoherence'!D23&lt;&gt;"",'Erreur incoherence'!D23,""))</f>
         <v/>
       </c>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A469" t="str">
-        <f>IF('Erreur incoherence'!B30&lt;&gt;"",CONCATENATE('Erreur incoherence'!B30,"=", 'Erreur incoherence'!D30),IF('Erreur incoherence'!D30&lt;&gt;"",'Erreur incoherence'!D30,""))</f>
+        <f>IF('Erreur incoherence'!B24&lt;&gt;"",CONCATENATE('Erreur incoherence'!B24,"=", 'Erreur incoherence'!D24),IF('Erreur incoherence'!D24&lt;&gt;"",'Erreur incoherence'!D24,""))</f>
         <v/>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A470" t="str">
-        <f>IF('Erreur incoherence'!B31&lt;&gt;"",CONCATENATE('Erreur incoherence'!B31,"=", 'Erreur incoherence'!D31),IF('Erreur incoherence'!D31&lt;&gt;"",'Erreur incoherence'!D31,""))</f>
+        <f>IF('Erreur incoherence'!B25&lt;&gt;"",CONCATENATE('Erreur incoherence'!B25,"=", 'Erreur incoherence'!D25),IF('Erreur incoherence'!D25&lt;&gt;"",'Erreur incoherence'!D25,""))</f>
         <v/>
       </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" t="str">
-        <f>IF('Erreur incoherence'!B32&lt;&gt;"",CONCATENATE('Erreur incoherence'!B32,"=", 'Erreur incoherence'!D32),IF('Erreur incoherence'!D32&lt;&gt;"",'Erreur incoherence'!D32,""))</f>
+        <f>IF('Erreur incoherence'!B26&lt;&gt;"",CONCATENATE('Erreur incoherence'!B26,"=", 'Erreur incoherence'!D26),IF('Erreur incoherence'!D26&lt;&gt;"",'Erreur incoherence'!D26,""))</f>
         <v/>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A472" t="str">
+        <f>IF('Erreur incoherence'!B27&lt;&gt;"",CONCATENATE('Erreur incoherence'!B27,"=", 'Erreur incoherence'!D27),IF('Erreur incoherence'!D27&lt;&gt;"",'Erreur incoherence'!D27,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" t="str">
+        <f>IF('Erreur incoherence'!B28&lt;&gt;"",CONCATENATE('Erreur incoherence'!B28,"=", 'Erreur incoherence'!D28),IF('Erreur incoherence'!D28&lt;&gt;"",'Erreur incoherence'!D28,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" t="str">
+        <f>IF('Erreur incoherence'!B29&lt;&gt;"",CONCATENATE('Erreur incoherence'!B29,"=", 'Erreur incoherence'!D29),IF('Erreur incoherence'!D29&lt;&gt;"",'Erreur incoherence'!D29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" t="str">
+        <f>IF('Erreur incoherence'!B30&lt;&gt;"",CONCATENATE('Erreur incoherence'!B30,"=", 'Erreur incoherence'!D30),IF('Erreur incoherence'!D30&lt;&gt;"",'Erreur incoherence'!D30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" t="str">
+        <f>IF('Erreur incoherence'!B31&lt;&gt;"",CONCATENATE('Erreur incoherence'!B31,"=", 'Erreur incoherence'!D31),IF('Erreur incoherence'!D31&lt;&gt;"",'Erreur incoherence'!D31,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" t="str">
+        <f>IF('Erreur incoherence'!B32&lt;&gt;"",CONCATENATE('Erreur incoherence'!B32,"=", 'Erreur incoherence'!D32),IF('Erreur incoherence'!D32&lt;&gt;"",'Erreur incoherence'!D32,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" t="str">
         <f>IF('Erreur balise introductive'!B2&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B2,"=", 'Erreur balise introductive'!D2),IF('Erreur balise introductive'!D2&lt;&gt;"",'Erreur balise introductive'!D2,""))</f>
         <v>#Mensaje para etiquetas introductoria</v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" t="str">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" t="str">
         <f>IF('Erreur balise introductive'!B3&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B3,"=", 'Erreur balise introductive'!D3),IF('Erreur balise introductive'!D3&lt;&gt;"",'Erreur balise introductive'!D3,""))</f>
         <v>window.error.missing.base.code.title=Errores de etiquetas introductorias</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" t="str">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" t="str">
         <f>IF('Erreur balise introductive'!B4&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B4,"=", 'Erreur balise introductive'!D4),IF('Erreur balise introductive'!D4&lt;&gt;"",'Erreur balise introductive'!D4,""))</f>
         <v>window.error.missing.base.code.panel.title=Lista de etiquetas introductorias</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" t="str">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" t="str">
         <f>IF('Erreur balise introductive'!B5&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B5,"=", 'Erreur balise introductive'!D5),IF('Erreur balise introductive'!D5&lt;&gt;"",'Erreur balise introductive'!D5,""))</f>
         <v>window.error.missing.base.code.field.label=Etiqueta :</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" t="str">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" t="str">
         <f>IF('Erreur balise introductive'!B6&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B6,"=", 'Erreur balise introductive'!D6),IF('Erreur balise introductive'!D6&lt;&gt;"",'Erreur balise introductive'!D6,""))</f>
         <v>window.error.missing.base.code.number.line.label=Número de línea :</v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A477" t="str">
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" t="str">
         <f>IF('Erreur balise introductive'!B7&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B7,"=", 'Erreur balise introductive'!D7),IF('Erreur balise introductive'!D7&lt;&gt;"",'Erreur balise introductive'!D7,""))</f>
         <v xml:space="preserve">window.error.missing.base.code.name.file.label=Nombre del documento : </v>
       </c>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" t="str">
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" t="str">
         <f>IF('Erreur balise introductive'!B8&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B8,"=", 'Erreur balise introductive'!D8),IF('Erreur balise introductive'!D8&lt;&gt;"",'Erreur balise introductive'!D8,""))</f>
         <v>window.error.missing.base.code.message.panel.title=Mensaje informativo</v>
       </c>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" t="str">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" t="str">
         <f>IF('Erreur balise introductive'!B9&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B9,"=", 'Erreur balise introductive'!D9),IF('Erreur balise introductive'!D9&lt;&gt;"",'Erreur balise introductive'!D9,""))</f>
         <v>window.error.missing.base.code.message=&lt;HTML&gt;&lt;P&gt;Se han detectado errores en las etiquetas de introducción.&lt;BR/&gt;Debe corregir manualmente la información directamente en sus documentos.&lt;BR/&gt;Al cerrar esta ventana, los documentos se recargarán automáticamente.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A480" t="str">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" t="str">
         <f>IF('Erreur balise introductive'!B10&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B10,"=", 'Erreur balise introductive'!D10),IF('Erreur balise introductive'!D10&lt;&gt;"",'Erreur balise introductive'!D10,""))</f>
         <v>window.error.missing.base.code.buttons.panel.title=Acciones</v>
       </c>
     </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" t="str">
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" t="str">
         <f>IF('Erreur balise introductive'!B11&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B11,"=", 'Erreur balise introductive'!D11),IF('Erreur balise introductive'!D11&lt;&gt;"",'Erreur balise introductive'!D11,""))</f>
         <v>window.error.missing.base.code.buttons.close.button.label=Cerrar y cargar lors documentos</v>
       </c>
     </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A482" t="str">
-        <f>IF('Erreur balise introductive'!B12&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B12,"=", 'Erreur balise introductive'!D12),IF('Erreur balise introductive'!D12&lt;&gt;"",'Erreur balise introductive'!D12,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A483" t="str">
-        <f>IF('Erreur balise introductive'!B13&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B13,"=", 'Erreur balise introductive'!D13),IF('Erreur balise introductive'!D13&lt;&gt;"",'Erreur balise introductive'!D13,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A484" t="str">
-        <f>IF('Erreur balise introductive'!B14&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B14,"=", 'Erreur balise introductive'!D14),IF('Erreur balise introductive'!D14&lt;&gt;"",'Erreur balise introductive'!D14,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A485" t="str">
-        <f>IF('Erreur balise introductive'!B15&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B15,"=", 'Erreur balise introductive'!D15),IF('Erreur balise introductive'!D15&lt;&gt;"",'Erreur balise introductive'!D15,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A486" t="str">
-        <f>IF('Erreur balise introductive'!B16&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B16,"=", 'Erreur balise introductive'!D16),IF('Erreur balise introductive'!D16&lt;&gt;"",'Erreur balise introductive'!D16,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A487" t="str">
-        <f>IF('Erreur balise introductive'!B17&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B17,"=", 'Erreur balise introductive'!D17),IF('Erreur balise introductive'!D17&lt;&gt;"",'Erreur balise introductive'!D17,""))</f>
-        <v/>
-      </c>
-    </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" t="str">
-        <f>IF('Erreur balise introductive'!B18&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B18,"=", 'Erreur balise introductive'!D18),IF('Erreur balise introductive'!D18&lt;&gt;"",'Erreur balise introductive'!D18,""))</f>
+        <f>IF('Erreur balise introductive'!B12&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B12,"=", 'Erreur balise introductive'!D12),IF('Erreur balise introductive'!D12&lt;&gt;"",'Erreur balise introductive'!D12,""))</f>
         <v/>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" t="str">
-        <f>IF('Erreur balise introductive'!B19&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B19,"=", 'Erreur balise introductive'!D19),IF('Erreur balise introductive'!D19&lt;&gt;"",'Erreur balise introductive'!D19,""))</f>
+        <f>IF('Erreur balise introductive'!B13&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B13,"=", 'Erreur balise introductive'!D13),IF('Erreur balise introductive'!D13&lt;&gt;"",'Erreur balise introductive'!D13,""))</f>
         <v/>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" t="str">
-        <f>IF('Erreur balise introductive'!B20&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B20,"=", 'Erreur balise introductive'!D20),IF('Erreur balise introductive'!D20&lt;&gt;"",'Erreur balise introductive'!D20,""))</f>
+        <f>IF('Erreur balise introductive'!B14&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B14,"=", 'Erreur balise introductive'!D14),IF('Erreur balise introductive'!D14&lt;&gt;"",'Erreur balise introductive'!D14,""))</f>
         <v/>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" t="str">
-        <f>IF('Erreur balise introductive'!B21&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B21,"=", 'Erreur balise introductive'!D21),IF('Erreur balise introductive'!D21&lt;&gt;"",'Erreur balise introductive'!D21,""))</f>
+        <f>IF('Erreur balise introductive'!B15&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B15,"=", 'Erreur balise introductive'!D15),IF('Erreur balise introductive'!D15&lt;&gt;"",'Erreur balise introductive'!D15,""))</f>
         <v/>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" t="str">
-        <f>IF('Erreur balise introductive'!B22&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B22,"=", 'Erreur balise introductive'!D22),IF('Erreur balise introductive'!D22&lt;&gt;"",'Erreur balise introductive'!D22,""))</f>
+        <f>IF('Erreur balise introductive'!B16&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B16,"=", 'Erreur balise introductive'!D16),IF('Erreur balise introductive'!D16&lt;&gt;"",'Erreur balise introductive'!D16,""))</f>
         <v/>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A493" t="str">
-        <f>IF('Erreur balise introductive'!B23&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B23,"=", 'Erreur balise introductive'!D23),IF('Erreur balise introductive'!D23&lt;&gt;"",'Erreur balise introductive'!D23,""))</f>
+        <f>IF('Erreur balise introductive'!B17&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B17,"=", 'Erreur balise introductive'!D17),IF('Erreur balise introductive'!D17&lt;&gt;"",'Erreur balise introductive'!D17,""))</f>
         <v/>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A494" t="str">
-        <f>IF('Erreur balise introductive'!B24&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B24,"=", 'Erreur balise introductive'!D24),IF('Erreur balise introductive'!D24&lt;&gt;"",'Erreur balise introductive'!D24,""))</f>
+        <f>IF('Erreur balise introductive'!B18&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B18,"=", 'Erreur balise introductive'!D18),IF('Erreur balise introductive'!D18&lt;&gt;"",'Erreur balise introductive'!D18,""))</f>
         <v/>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A495" t="str">
-        <f>IF('Erreur balise introductive'!B25&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B25,"=", 'Erreur balise introductive'!D25),IF('Erreur balise introductive'!D25&lt;&gt;"",'Erreur balise introductive'!D25,""))</f>
+        <f>IF('Erreur balise introductive'!B19&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B19,"=", 'Erreur balise introductive'!D19),IF('Erreur balise introductive'!D19&lt;&gt;"",'Erreur balise introductive'!D19,""))</f>
         <v/>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A496" t="str">
-        <f>IF('Erreur balise introductive'!B26&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B26,"=", 'Erreur balise introductive'!D26),IF('Erreur balise introductive'!D26&lt;&gt;"",'Erreur balise introductive'!D26,""))</f>
+        <f>IF('Erreur balise introductive'!B20&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B20,"=", 'Erreur balise introductive'!D20),IF('Erreur balise introductive'!D20&lt;&gt;"",'Erreur balise introductive'!D20,""))</f>
         <v/>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A497" t="str">
-        <f>IF('Erreur balise introductive'!B27&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B27,"=", 'Erreur balise introductive'!D27),IF('Erreur balise introductive'!D27&lt;&gt;"",'Erreur balise introductive'!D27,""))</f>
+        <f>IF('Erreur balise introductive'!B21&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B21,"=", 'Erreur balise introductive'!D21),IF('Erreur balise introductive'!D21&lt;&gt;"",'Erreur balise introductive'!D21,""))</f>
         <v/>
       </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A498" t="str">
-        <f>IF('Erreur balise introductive'!B28&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B28,"=", 'Erreur balise introductive'!D28),IF('Erreur balise introductive'!D28&lt;&gt;"",'Erreur balise introductive'!D28,""))</f>
+        <f>IF('Erreur balise introductive'!B22&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B22,"=", 'Erreur balise introductive'!D22),IF('Erreur balise introductive'!D22&lt;&gt;"",'Erreur balise introductive'!D22,""))</f>
         <v/>
       </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A499" t="str">
-        <f>IF('Erreur balise introductive'!B29&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B29,"=", 'Erreur balise introductive'!D29),IF('Erreur balise introductive'!D29&lt;&gt;"",'Erreur balise introductive'!D29,""))</f>
+        <f>IF('Erreur balise introductive'!B23&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B23,"=", 'Erreur balise introductive'!D23),IF('Erreur balise introductive'!D23&lt;&gt;"",'Erreur balise introductive'!D23,""))</f>
         <v/>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A500" t="str">
-        <f>IF('Erreur balise introductive'!B30&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B30,"=", 'Erreur balise introductive'!D30),IF('Erreur balise introductive'!D30&lt;&gt;"",'Erreur balise introductive'!D30,""))</f>
+        <f>IF('Erreur balise introductive'!B24&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B24,"=", 'Erreur balise introductive'!D24),IF('Erreur balise introductive'!D24&lt;&gt;"",'Erreur balise introductive'!D24,""))</f>
         <v/>
       </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A501" t="str">
+        <f>IF('Erreur balise introductive'!B25&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B25,"=", 'Erreur balise introductive'!D25),IF('Erreur balise introductive'!D25&lt;&gt;"",'Erreur balise introductive'!D25,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" t="str">
+        <f>IF('Erreur balise introductive'!B26&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B26,"=", 'Erreur balise introductive'!D26),IF('Erreur balise introductive'!D26&lt;&gt;"",'Erreur balise introductive'!D26,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" t="str">
+        <f>IF('Erreur balise introductive'!B27&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B27,"=", 'Erreur balise introductive'!D27),IF('Erreur balise introductive'!D27&lt;&gt;"",'Erreur balise introductive'!D27,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504" t="str">
+        <f>IF('Erreur balise introductive'!B28&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B28,"=", 'Erreur balise introductive'!D28),IF('Erreur balise introductive'!D28&lt;&gt;"",'Erreur balise introductive'!D28,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" t="str">
+        <f>IF('Erreur balise introductive'!B29&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B29,"=", 'Erreur balise introductive'!D29),IF('Erreur balise introductive'!D29&lt;&gt;"",'Erreur balise introductive'!D29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" t="str">
+        <f>IF('Erreur balise introductive'!B30&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B30,"=", 'Erreur balise introductive'!D30),IF('Erreur balise introductive'!D30&lt;&gt;"",'Erreur balise introductive'!D30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" t="str">
         <f>IF('Erreur balise introductive'!B31&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B31,"=", 'Erreur balise introductive'!D31),IF('Erreur balise introductive'!D31&lt;&gt;"",'Erreur balise introductive'!D31,""))</f>
         <v/>
       </c>
@@ -33322,10 +33448,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
-  <dimension ref="A1:A496"/>
+  <dimension ref="A1:A501"/>
   <sheetViews>
-    <sheetView topLeftCell="A338" workbookViewId="0">
-      <selection activeCell="A357" sqref="A357:A359"/>
+    <sheetView topLeftCell="A335" workbookViewId="0">
+      <selection activeCell="A362" sqref="A362:A363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35502,809 +35628,839 @@
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" t="str">
         <f>IF(Autres!B40&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B40),".","_"),"=""", Autres!B40,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_ALERT_MORE_ONE_CAERUS_LAUNCH_MESSAGE_TITLE="window.alert.more.one.caerus.launch.message.title";</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" t="str">
-        <f>IF('Changer Configuration'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B2),".","_"),"=""", 'Changer Configuration'!B2,""";"),"")</f>
-        <v/>
+        <f>IF(Autres!B41&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B41),".","_"),"=""", Autres!B41,""";"),"")</f>
+        <v>public static final String WINDOW_ALERT_MORE_ONE_CAERUS_LAUNCH_MESSAGE_CONTENT="window.alert.more.one.caerus.launch.message.content";</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" t="str">
+        <f>IF(Autres!B42&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B42),".","_"),"=""", Autres!B42,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" t="str">
+        <f>IF(Autres!B43&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B43),".","_"),"=""", Autres!B43,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" t="str">
+        <f>IF(Autres!B44&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B44),".","_"),"=""", Autres!B44,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" t="str">
+        <f>IF(Autres!B45&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B45),".","_"),"=""", Autres!B45,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" t="str">
+        <f>IF(Autres!B46&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B46),".","_"),"=""", Autres!B46,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" t="str">
         <f>IF('Changer Configuration'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B3),".","_"),"=""", 'Changer Configuration'!B3,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_TITLE="window.change.configuration.title";</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" t="str">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" t="str">
         <f>IF('Changer Configuration'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B4),".","_"),"=""", 'Changer Configuration'!B4,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_LIST_LABEL="window.change.configuration.list.label";</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" t="str">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="str">
         <f>IF('Changer Configuration'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B5),".","_"),"=""", 'Changer Configuration'!B5,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_PANEL_TITLE="window.change.configuration.panel.title";</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" t="str">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="str">
         <f>IF('Changer Configuration'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B6),".","_"),"=""", 'Changer Configuration'!B6,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_MESSAGE_PANEL_TITLE="window.change.configuration.message.panel.title";</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" t="str">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="str">
         <f>IF('Changer Configuration'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B7),".","_"),"=""", 'Changer Configuration'!B7,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_MESSAGE_CONTENT="window.change.configuration.message.content";</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" t="str">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" t="str">
         <f>IF('Changer Configuration'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B8),".","_"),"=""", 'Changer Configuration'!B8,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_BUTTON_APPLY_AND_CLOSE="window.change.configuration.button.apply.and.close";</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" t="str">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" t="str">
         <f>IF('Changer Configuration'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B9),".","_"),"=""", 'Changer Configuration'!B9,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_BUTTON_CLOSE="window.change.configuration.button.close";</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" t="str">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" t="str">
         <f>IF('Changer Configuration'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B10),".","_"),"=""", 'Changer Configuration'!B10,""";"),"")</f>
         <v>public static final String WINDOW_CHANGE_CONFIGURATION_BUTTONS_PANEL_TITLE="window.change.configuration.buttons.panel.title";</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" t="str">
-        <f>IF('Changer Configuration'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B11),".","_"),"=""", 'Changer Configuration'!B11,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" t="str">
-        <f>IF('Changer Configuration'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B12),".","_"),"=""", 'Changer Configuration'!B12,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" t="str">
-        <f>IF('Changer Configuration'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B13),".","_"),"=""", 'Changer Configuration'!B13,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" t="str">
-        <f>IF('Changer Configuration'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B14),".","_"),"=""", 'Changer Configuration'!B14,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" t="str">
-        <f>IF('Changer Configuration'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B15),".","_"),"=""", 'Changer Configuration'!B15,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" t="str">
-        <f>IF('Changer Configuration'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B16),".","_"),"=""", 'Changer Configuration'!B16,""";"),"")</f>
+        <f>IF('Changer Configuration'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B11),".","_"),"=""", 'Changer Configuration'!B11,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" t="str">
-        <f>IF('Changer Configuration'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B17),".","_"),"=""", 'Changer Configuration'!B17,""";"),"")</f>
+        <f>IF('Changer Configuration'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B12),".","_"),"=""", 'Changer Configuration'!B12,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" t="str">
-        <f>IF('Changer Configuration'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B18),".","_"),"=""", 'Changer Configuration'!B18,""";"),"")</f>
+        <f>IF('Changer Configuration'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B13),".","_"),"=""", 'Changer Configuration'!B13,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" t="str">
-        <f>IF('Changer Configuration'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B19),".","_"),"=""", 'Changer Configuration'!B19,""";"),"")</f>
+        <f>IF('Changer Configuration'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B14),".","_"),"=""", 'Changer Configuration'!B14,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" t="str">
-        <f>IF('Changer Configuration'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B20),".","_"),"=""", 'Changer Configuration'!B20,""";"),"")</f>
+        <f>IF('Changer Configuration'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B15),".","_"),"=""", 'Changer Configuration'!B15,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" t="str">
-        <f>IF('Changer Configuration'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B21),".","_"),"=""", 'Changer Configuration'!B21,""";"),"")</f>
+        <f>IF('Changer Configuration'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B16),".","_"),"=""", 'Changer Configuration'!B16,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" t="str">
-        <f>IF('Changer Configuration'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B22),".","_"),"=""", 'Changer Configuration'!B22,""";"),"")</f>
+        <f>IF('Changer Configuration'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B17),".","_"),"=""", 'Changer Configuration'!B17,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" t="str">
-        <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B23),".","_"),"=""", 'Changer Configuration'!B23,""";"),"")</f>
+        <f>IF('Changer Configuration'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B18),".","_"),"=""", 'Changer Configuration'!B18,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" t="str">
-        <f>IF('A propos'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B2),".","_"),"=""", 'A propos'!B2,""";"),"")</f>
+        <f>IF('Changer Configuration'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B19),".","_"),"=""", 'Changer Configuration'!B19,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" t="str">
+        <f>IF('Changer Configuration'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B20),".","_"),"=""", 'Changer Configuration'!B20,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" t="str">
+        <f>IF('Changer Configuration'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B21),".","_"),"=""", 'Changer Configuration'!B21,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" t="str">
+        <f>IF('Changer Configuration'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B22),".","_"),"=""", 'Changer Configuration'!B22,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" t="str">
+        <f>IF('Changer Configuration'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Changer Configuration'!B23),".","_"),"=""", 'Changer Configuration'!B23,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" t="str">
+        <f>IF('A propos'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B2),".","_"),"=""", 'A propos'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" t="str">
         <f>IF('A propos'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B3),".","_"),"=""", 'A propos'!B3,""";"),"")</f>
         <v>public static final String WINDOW_ABOUT_TITLE="window.about.title";</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" t="str">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" t="str">
         <f>IF('A propos'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B4),".","_"),"=""", 'A propos'!B4,""";"),"")</f>
         <v>public static final String WINDOW_ABOUT_MESSAGE_CONTENT="window.about.message.content";</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" t="str">
-        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B5),".","_"),"=""", 'A propos'!B5,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" t="str">
-        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B6),".","_"),"=""", 'A propos'!B6,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" t="str">
-        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B7),".","_"),"=""", 'A propos'!B7,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" t="str">
-        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B8),".","_"),"=""", 'A propos'!B8,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" t="str">
-        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B9),".","_"),"=""", 'A propos'!B9,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" t="str">
-        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B10),".","_"),"=""", 'A propos'!B10,""";"),"")</f>
+        <f>IF('A propos'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B5),".","_"),"=""", 'A propos'!B5,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" t="str">
-        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B11),".","_"),"=""", 'A propos'!B11,""";"),"")</f>
+        <f>IF('A propos'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B6),".","_"),"=""", 'A propos'!B6,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" t="str">
-        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B12),".","_"),"=""", 'A propos'!B12,""";"),"")</f>
+        <f>IF('A propos'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B7),".","_"),"=""", 'A propos'!B7,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" t="str">
-        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B13),".","_"),"=""", 'A propos'!B13,""";"),"")</f>
+        <f>IF('A propos'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B8),".","_"),"=""", 'A propos'!B8,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" t="str">
-        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B14),".","_"),"=""", 'A propos'!B14,""";"),"")</f>
+        <f>IF('A propos'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B9),".","_"),"=""", 'A propos'!B9,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" t="str">
-        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B15),".","_"),"=""", 'A propos'!B15,""";"),"")</f>
+        <f>IF('A propos'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B10),".","_"),"=""", 'A propos'!B10,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" t="str">
-        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B16),".","_"),"=""", 'A propos'!B16,""";"),"")</f>
+        <f>IF('A propos'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B11),".","_"),"=""", 'A propos'!B11,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" t="str">
-        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B17),".","_"),"=""", 'A propos'!B17,""";"),"")</f>
+        <f>IF('A propos'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B12),".","_"),"=""", 'A propos'!B12,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" t="str">
-        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B18),".","_"),"=""", 'A propos'!B18,""";"),"")</f>
+        <f>IF('A propos'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B13),".","_"),"=""", 'A propos'!B13,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402" t="str">
-        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B19),".","_"),"=""", 'A propos'!B19,""";"),"")</f>
+        <f>IF('A propos'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B14),".","_"),"=""", 'A propos'!B14,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" t="str">
-        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B20),".","_"),"=""", 'A propos'!B20,""";"),"")</f>
+        <f>IF('A propos'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B15),".","_"),"=""", 'A propos'!B15,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" t="str">
-        <f>IF('A propos'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B21),".","_"),"=""", 'A propos'!B21,""";"),"")</f>
+        <f>IF('A propos'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B16),".","_"),"=""", 'A propos'!B16,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A405" t="str">
-        <f>IF('A propos'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B22),".","_"),"=""", 'A propos'!B22,""";"),"")</f>
+        <f>IF('A propos'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B17),".","_"),"=""", 'A propos'!B17,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" t="str">
-        <f>IF('A propos'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B23),".","_"),"=""", 'A propos'!B23,""";"),"")</f>
+        <f>IF('A propos'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B18),".","_"),"=""", 'A propos'!B18,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A407" t="str">
-        <f>IF('A propos'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B24),".","_"),"=""", 'A propos'!B24,""";"),"")</f>
+        <f>IF('A propos'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B19),".","_"),"=""", 'A propos'!B19,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A408" t="str">
-        <f>IF('Export Document Materiel'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B2),".","_"),"=""", 'Export Document Materiel'!B2,""";"),"")</f>
+        <f>IF('A propos'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B20),".","_"),"=""", 'A propos'!B20,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" t="str">
+        <f>IF('A propos'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B21),".","_"),"=""", 'A propos'!B21,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" t="str">
+        <f>IF('A propos'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B22),".","_"),"=""", 'A propos'!B22,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" t="str">
+        <f>IF('A propos'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B23),".","_"),"=""", 'A propos'!B23,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" t="str">
+        <f>IF('A propos'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('A propos'!B24),".","_"),"=""", 'A propos'!B24,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" t="str">
+        <f>IF('Export Document Materiel'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B2),".","_"),"=""", 'Export Document Materiel'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" t="str">
         <f>IF('Export Document Materiel'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B3),".","_"),"=""", 'Export Document Materiel'!B3,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_TITLE="window.export.document.title";</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" t="str">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" t="str">
         <f>IF('Export Document Materiel'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B4),".","_"),"=""", 'Export Document Materiel'!B4,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DIRECTORY_PANEL_TITLE="window.export.document.choose.directory.panel.title";</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" t="str">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" t="str">
         <f>IF('Export Document Materiel'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B5),".","_"),"=""", 'Export Document Materiel'!B5,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DIRECTORY_LABEL="window.export.document.choose.directory.label";</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" t="str">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" t="str">
         <f>IF('Export Document Materiel'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B6),".","_"),"=""", 'Export Document Materiel'!B6,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_MODE_PANEL_TITLE="window.export.document.mode.panel.title";</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" t="str">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="str">
         <f>IF('Export Document Materiel'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B7),".","_"),"=""", 'Export Document Materiel'!B7,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_MODE_DOCUMENT_LABEL="window.export.document.mode.document.label";</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" t="str">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" t="str">
         <f>IF('Export Document Materiel'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B8),".","_"),"=""", 'Export Document Materiel'!B8,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_MODE_ALL_DOCUMENTS_LABEL="window.export.document.mode.all.documents.label";</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415" t="str">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" t="str">
         <f>IF('Export Document Materiel'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B9),".","_"),"=""", 'Export Document Materiel'!B9,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_MODE_RESULT_SEARCH_LABEL="window.export.document.mode.result.search.label";</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" t="str">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" t="str">
         <f>IF('Export Document Materiel'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B10),".","_"),"=""", 'Export Document Materiel'!B10,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DOCUMENT_PANEL_TITLE="window.export.document.choose.document.panel.title";</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" t="str">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" t="str">
         <f>IF('Export Document Materiel'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B11),".","_"),"=""", 'Export Document Materiel'!B11,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DOCUMENT_LABEL="window.export.document.choose.document.label";</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418" t="str">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" t="str">
         <f>IF('Export Document Materiel'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B12),".","_"),"=""", 'Export Document Materiel'!B12,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_FILE_PANEL_TITLE="window.export.document.choose.file.panel.title";</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" t="str">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" t="str">
         <f>IF('Export Document Materiel'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B13),".","_"),"=""", 'Export Document Materiel'!B13,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_FILE_LABEL="window.export.document.choose.file.label";</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A420" t="str">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" t="str">
         <f>IF('Export Document Materiel'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B14),".","_"),"=""", 'Export Document Materiel'!B14,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_BUTTON_PANEL_TITLE="window.export.document.button.panel.title";</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" t="str">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" t="str">
         <f>IF('Export Document Materiel'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B15),".","_"),"=""", 'Export Document Materiel'!B15,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_BUTTON_EXPORT_LABEL="window.export.document.button.export.label";</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" t="str">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" t="str">
         <f>IF('Export Document Materiel'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B16),".","_"),"=""", 'Export Document Materiel'!B16,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_INFORMATION_MESSAGE_TITLE="window.export.document.information.message.title";</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" t="str">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" t="str">
         <f>IF('Export Document Materiel'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B17),".","_"),"=""", 'Export Document Materiel'!B17,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_INFORMATION_MESSAGE="window.export.document.information.message";</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" t="str">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" t="str">
         <f>IF('Export Document Materiel'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B18),".","_"),"=""", 'Export Document Materiel'!B18,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_BUTTON_CLOSE_LABEL="window.export.document.button.close.label";</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" t="str">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" t="str">
         <f>IF('Export Document Materiel'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B19),".","_"),"=""", 'Export Document Materiel'!B19,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_CHOOSE_DIRECTORY_DIALOG_TITLE="window.export.document.choose.directory.dialog.title";</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" t="str">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" t="str">
         <f>IF('Export Document Materiel'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B20),".","_"),"=""", 'Export Document Materiel'!B20,""";"),"")</f>
         <v>public static final String WINDOW_EXPORT_DOCUMENT_INFORMATION_SEARCH_MESSAGE="window.export.document.information.search.message";</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" t="str">
-        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B21),".","_"),"=""", 'Export Document Materiel'!B21,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" t="str">
-        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B22),".","_"),"=""", 'Export Document Materiel'!B22,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A429" t="str">
-        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B23),".","_"),"=""", 'Export Document Materiel'!B23,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" t="str">
-        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B24),".","_"),"=""", 'Export Document Materiel'!B24,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" t="str">
-        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B25),".","_"),"=""", 'Export Document Materiel'!B25,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A432" t="str">
-        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B26),".","_"),"=""", 'Export Document Materiel'!B26,""";"),"")</f>
+        <f>IF('Export Document Materiel'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B21),".","_"),"=""", 'Export Document Materiel'!B21,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" t="str">
-        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B27),".","_"),"=""", 'Export Document Materiel'!B27,""";"),"")</f>
+        <f>IF('Export Document Materiel'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B22),".","_"),"=""", 'Export Document Materiel'!B22,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" t="str">
-        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B28),".","_"),"=""", 'Export Document Materiel'!B28,""";"),"")</f>
+        <f>IF('Export Document Materiel'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B23),".","_"),"=""", 'Export Document Materiel'!B23,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A435" t="str">
-        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B29),".","_"),"=""", 'Export Document Materiel'!B29,""";"),"")</f>
+        <f>IF('Export Document Materiel'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B24),".","_"),"=""", 'Export Document Materiel'!B24,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" t="str">
-        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B30),".","_"),"=""", 'Export Document Materiel'!B30,""";"),"")</f>
+        <f>IF('Export Document Materiel'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B25),".","_"),"=""", 'Export Document Materiel'!B25,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" t="str">
-        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B31),".","_"),"=""", 'Export Document Materiel'!B31,""";"),"")</f>
+        <f>IF('Export Document Materiel'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B26),".","_"),"=""", 'Export Document Materiel'!B26,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A438" t="str">
-        <f>IF('Erreur incoherence'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B2),".","_"),"=""", 'Erreur incoherence'!B2,""";"),"")</f>
+        <f>IF('Export Document Materiel'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B27),".","_"),"=""", 'Export Document Materiel'!B27,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" t="str">
+        <f>IF('Export Document Materiel'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B28),".","_"),"=""", 'Export Document Materiel'!B28,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" t="str">
+        <f>IF('Export Document Materiel'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B29),".","_"),"=""", 'Export Document Materiel'!B29,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" t="str">
+        <f>IF('Export Document Materiel'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B30),".","_"),"=""", 'Export Document Materiel'!B30,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" t="str">
+        <f>IF('Export Document Materiel'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Document Materiel'!B31),".","_"),"=""", 'Export Document Materiel'!B31,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" t="str">
+        <f>IF('Erreur incoherence'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B2),".","_"),"=""", 'Erreur incoherence'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" t="str">
         <f>IF('Erreur incoherence'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B3),".","_"),"=""", 'Erreur incoherence'!B3,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_TITLE="window.error.inconsistency.title";</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" t="str">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" t="str">
         <f>IF('Erreur incoherence'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B4),".","_"),"=""", 'Erreur incoherence'!B4,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_PANEL_TITLE="window.error.inconsistency.panel.title";</v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" t="str">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" t="str">
         <f>IF('Erreur incoherence'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B5),".","_"),"=""", 'Erreur incoherence'!B5,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_FIELD_LABEL="window.error.inconsistency.field.label";</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" t="str">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" t="str">
         <f>IF('Erreur incoherence'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B6),".","_"),"=""", 'Erreur incoherence'!B6,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_NUMBER_LINE_LABEL="window.error.inconsistency.number.line.label";</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" t="str">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" t="str">
         <f>IF('Erreur incoherence'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B7),".","_"),"=""", 'Erreur incoherence'!B7,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_NAME_FILE_LABEL="window.error.inconsistency.name.file.label";</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" t="str">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" t="str">
         <f>IF('Erreur incoherence'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B8),".","_"),"=""", 'Erreur incoherence'!B8,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_MESSAGE_PANEL_TITLE="window.error.inconsistency.message.panel.title";</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" t="str">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" t="str">
         <f>IF('Erreur incoherence'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B9),".","_"),"=""", 'Erreur incoherence'!B9,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_MESSAGE="window.error.inconsistency.message";</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" t="str">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" t="str">
         <f>IF('Erreur incoherence'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B10),".","_"),"=""", 'Erreur incoherence'!B10,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_BUTTONS_PANEL_TITLE="window.error.inconsistency.buttons.panel.title";</v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A447" t="str">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" t="str">
         <f>IF('Erreur incoherence'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B11),".","_"),"=""", 'Erreur incoherence'!B11,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_INCONSISTENCY_BUTTONS_CLOSE_BUTTON_LABEL="window.error.inconsistency.buttons.close.button.label";</v>
       </c>
     </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" t="str">
-        <f>IF('Erreur incoherence'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B12),".","_"),"=""", 'Erreur incoherence'!B12,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" t="str">
-        <f>IF('Erreur incoherence'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B13),".","_"),"=""", 'Erreur incoherence'!B13,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" t="str">
-        <f>IF('Erreur incoherence'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B14),".","_"),"=""", 'Erreur incoherence'!B14,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" t="str">
-        <f>IF('Erreur incoherence'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B15),".","_"),"=""", 'Erreur incoherence'!B15,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" t="str">
-        <f>IF('Erreur incoherence'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B16),".","_"),"=""", 'Erreur incoherence'!B16,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453" t="str">
-        <f>IF('Erreur incoherence'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B17),".","_"),"=""", 'Erreur incoherence'!B17,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B12),".","_"),"=""", 'Erreur incoherence'!B12,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A454" t="str">
-        <f>IF('Erreur incoherence'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B18),".","_"),"=""", 'Erreur incoherence'!B18,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B13),".","_"),"=""", 'Erreur incoherence'!B13,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" t="str">
-        <f>IF('Erreur incoherence'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B19),".","_"),"=""", 'Erreur incoherence'!B19,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B14),".","_"),"=""", 'Erreur incoherence'!B14,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A456" t="str">
-        <f>IF('Erreur incoherence'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B20),".","_"),"=""", 'Erreur incoherence'!B20,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B15),".","_"),"=""", 'Erreur incoherence'!B15,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A457" t="str">
-        <f>IF('Erreur incoherence'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B21),".","_"),"=""", 'Erreur incoherence'!B21,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B16),".","_"),"=""", 'Erreur incoherence'!B16,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" t="str">
-        <f>IF('Erreur incoherence'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B22),".","_"),"=""", 'Erreur incoherence'!B22,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B17),".","_"),"=""", 'Erreur incoherence'!B17,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" t="str">
-        <f>IF('Erreur incoherence'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B23),".","_"),"=""", 'Erreur incoherence'!B23,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B18),".","_"),"=""", 'Erreur incoherence'!B18,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" t="str">
-        <f>IF('Erreur incoherence'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B24),".","_"),"=""", 'Erreur incoherence'!B24,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B19),".","_"),"=""", 'Erreur incoherence'!B19,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" t="str">
-        <f>IF('Erreur incoherence'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B25),".","_"),"=""", 'Erreur incoherence'!B25,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B20),".","_"),"=""", 'Erreur incoherence'!B20,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" t="str">
-        <f>IF('Erreur incoherence'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B26),".","_"),"=""", 'Erreur incoherence'!B26,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B21),".","_"),"=""", 'Erreur incoherence'!B21,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A463" t="str">
-        <f>IF('Erreur incoherence'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B27),".","_"),"=""", 'Erreur incoherence'!B27,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B22),".","_"),"=""", 'Erreur incoherence'!B22,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" t="str">
-        <f>IF('Erreur incoherence'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B28),".","_"),"=""", 'Erreur incoherence'!B28,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B23),".","_"),"=""", 'Erreur incoherence'!B23,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A465" t="str">
-        <f>IF('Erreur incoherence'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B29),".","_"),"=""", 'Erreur incoherence'!B29,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B24),".","_"),"=""", 'Erreur incoherence'!B24,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466" t="str">
-        <f>IF('Erreur incoherence'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B30),".","_"),"=""", 'Erreur incoherence'!B30,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B25),".","_"),"=""", 'Erreur incoherence'!B25,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A467" t="str">
-        <f>IF('Erreur incoherence'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B31),".","_"),"=""", 'Erreur incoherence'!B31,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B26),".","_"),"=""", 'Erreur incoherence'!B26,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468" t="str">
-        <f>IF('Erreur incoherence'!B32&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B32),".","_"),"=""", 'Erreur incoherence'!B32,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B27),".","_"),"=""", 'Erreur incoherence'!B27,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A469" t="str">
-        <f>IF('Erreur balise introductive'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B2),".","_"),"=""", 'Erreur balise introductive'!B2,""";"),"")</f>
+        <f>IF('Erreur incoherence'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B28),".","_"),"=""", 'Erreur incoherence'!B28,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A470" t="str">
+        <f>IF('Erreur incoherence'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B29),".","_"),"=""", 'Erreur incoherence'!B29,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" t="str">
+        <f>IF('Erreur incoherence'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B30),".","_"),"=""", 'Erreur incoherence'!B30,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" t="str">
+        <f>IF('Erreur incoherence'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B31),".","_"),"=""", 'Erreur incoherence'!B31,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" t="str">
+        <f>IF('Erreur incoherence'!B32&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur incoherence'!B32),".","_"),"=""", 'Erreur incoherence'!B32,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" t="str">
+        <f>IF('Erreur balise introductive'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B2),".","_"),"=""", 'Erreur balise introductive'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" t="str">
         <f>IF('Erreur balise introductive'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B3),".","_"),"=""", 'Erreur balise introductive'!B3,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_TITLE="window.error.missing.base.code.title";</v>
       </c>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A471" t="str">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" t="str">
         <f>IF('Erreur balise introductive'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B4),".","_"),"=""", 'Erreur balise introductive'!B4,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_PANEL_TITLE="window.error.missing.base.code.panel.title";</v>
       </c>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" t="str">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" t="str">
         <f>IF('Erreur balise introductive'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B5),".","_"),"=""", 'Erreur balise introductive'!B5,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_FIELD_LABEL="window.error.missing.base.code.field.label";</v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" t="str">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" t="str">
         <f>IF('Erreur balise introductive'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B6),".","_"),"=""", 'Erreur balise introductive'!B6,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_NUMBER_LINE_LABEL="window.error.missing.base.code.number.line.label";</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" t="str">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" t="str">
         <f>IF('Erreur balise introductive'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B7),".","_"),"=""", 'Erreur balise introductive'!B7,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_NAME_FILE_LABEL="window.error.missing.base.code.name.file.label";</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" t="str">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" t="str">
         <f>IF('Erreur balise introductive'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B8),".","_"),"=""", 'Erreur balise introductive'!B8,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_MESSAGE_PANEL_TITLE="window.error.missing.base.code.message.panel.title";</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" t="str">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" t="str">
         <f>IF('Erreur balise introductive'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B9),".","_"),"=""", 'Erreur balise introductive'!B9,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_MESSAGE="window.error.missing.base.code.message";</v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A477" t="str">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" t="str">
         <f>IF('Erreur balise introductive'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B10),".","_"),"=""", 'Erreur balise introductive'!B10,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_BUTTONS_PANEL_TITLE="window.error.missing.base.code.buttons.panel.title";</v>
       </c>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" t="str">
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" t="str">
         <f>IF('Erreur balise introductive'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B11),".","_"),"=""", 'Erreur balise introductive'!B11,""";"),"")</f>
         <v>public static final String WINDOW_ERROR_MISSING_BASE_CODE_BUTTONS_CLOSE_BUTTON_LABEL="window.error.missing.base.code.buttons.close.button.label";</v>
       </c>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" t="str">
-        <f>IF('Erreur balise introductive'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B12),".","_"),"=""", 'Erreur balise introductive'!B12,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A480" t="str">
-        <f>IF('Erreur balise introductive'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B13),".","_"),"=""", 'Erreur balise introductive'!B13,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" t="str">
-        <f>IF('Erreur balise introductive'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B14),".","_"),"=""", 'Erreur balise introductive'!B14,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A482" t="str">
-        <f>IF('Erreur balise introductive'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B15),".","_"),"=""", 'Erreur balise introductive'!B15,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A483" t="str">
-        <f>IF('Erreur balise introductive'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B16),".","_"),"=""", 'Erreur balise introductive'!B16,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A484" t="str">
-        <f>IF('Erreur balise introductive'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B17),".","_"),"=""", 'Erreur balise introductive'!B17,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B12),".","_"),"=""", 'Erreur balise introductive'!B12,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A485" t="str">
-        <f>IF('Erreur balise introductive'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B18),".","_"),"=""", 'Erreur balise introductive'!B18,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B13),".","_"),"=""", 'Erreur balise introductive'!B13,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A486" t="str">
-        <f>IF('Erreur balise introductive'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B19),".","_"),"=""", 'Erreur balise introductive'!B19,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B14),".","_"),"=""", 'Erreur balise introductive'!B14,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A487" t="str">
-        <f>IF('Erreur balise introductive'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B20),".","_"),"=""", 'Erreur balise introductive'!B20,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B15),".","_"),"=""", 'Erreur balise introductive'!B15,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" t="str">
-        <f>IF('Erreur balise introductive'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B21),".","_"),"=""", 'Erreur balise introductive'!B21,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B16),".","_"),"=""", 'Erreur balise introductive'!B16,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" t="str">
-        <f>IF('Erreur balise introductive'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B22),".","_"),"=""", 'Erreur balise introductive'!B22,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B17),".","_"),"=""", 'Erreur balise introductive'!B17,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" t="str">
-        <f>IF('Erreur balise introductive'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B23),".","_"),"=""", 'Erreur balise introductive'!B23,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B18),".","_"),"=""", 'Erreur balise introductive'!B18,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" t="str">
-        <f>IF('Erreur balise introductive'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B24),".","_"),"=""", 'Erreur balise introductive'!B24,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B19),".","_"),"=""", 'Erreur balise introductive'!B19,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" t="str">
-        <f>IF('Erreur balise introductive'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B25),".","_"),"=""", 'Erreur balise introductive'!B25,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B20),".","_"),"=""", 'Erreur balise introductive'!B20,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A493" t="str">
-        <f>IF('Erreur balise introductive'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B26),".","_"),"=""", 'Erreur balise introductive'!B26,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B21),".","_"),"=""", 'Erreur balise introductive'!B21,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A494" t="str">
-        <f>IF('Erreur balise introductive'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B27),".","_"),"=""", 'Erreur balise introductive'!B27,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B22),".","_"),"=""", 'Erreur balise introductive'!B22,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A495" t="str">
-        <f>IF('Erreur balise introductive'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B28),".","_"),"=""", 'Erreur balise introductive'!B28,""";"),"")</f>
+        <f>IF('Erreur balise introductive'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B23),".","_"),"=""", 'Erreur balise introductive'!B23,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A496" t="str">
+        <f>IF('Erreur balise introductive'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B24),".","_"),"=""", 'Erreur balise introductive'!B24,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" t="str">
+        <f>IF('Erreur balise introductive'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B25),".","_"),"=""", 'Erreur balise introductive'!B25,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" t="str">
+        <f>IF('Erreur balise introductive'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B26),".","_"),"=""", 'Erreur balise introductive'!B26,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" t="str">
+        <f>IF('Erreur balise introductive'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B27),".","_"),"=""", 'Erreur balise introductive'!B27,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" t="str">
+        <f>IF('Erreur balise introductive'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B28),".","_"),"=""", 'Erreur balise introductive'!B28,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" t="str">
         <f>IF('Erreur balise introductive'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B29),".","_"),"=""", 'Erreur balise introductive'!B29,""";"),"")</f>
         <v/>
       </c>
@@ -36318,8 +36474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56DE331-9367-41C8-8048-603F1BE40CC9}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ajout des premiers test unitaires Début de création des analyses lexicométriques
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\git\Caerus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\IdeaProjects\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C7429F-29E6-4A76-8871-61ACC243A9F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D102F1EA-A1FC-4916-BCCE-A245A160FD21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="14" activeTab="18" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="15" activeTab="18" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,10 @@
     <sheet name="Export Document Materiel" sheetId="20" r:id="rId16"/>
     <sheet name="Erreur incoherence" sheetId="21" r:id="rId17"/>
     <sheet name="Erreur balise introductive" sheetId="22" r:id="rId18"/>
-    <sheet name="FR_Properties" sheetId="14" r:id="rId19"/>
-    <sheet name="ES_Properties" sheetId="16" r:id="rId20"/>
-    <sheet name="Constants" sheetId="18" r:id="rId21"/>
+    <sheet name="Commencer analyse" sheetId="23" r:id="rId19"/>
+    <sheet name="FR_Properties" sheetId="14" r:id="rId20"/>
+    <sheet name="ES_Properties" sheetId="16" r:id="rId21"/>
+    <sheet name="Constants" sheetId="18" r:id="rId22"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="794">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -2337,6 +2338,96 @@
   </si>
   <si>
     <t>&lt;html&gt;&lt;p&gt;Caerus ya se está ejecutando.&lt;br/&gt;No puede ejecutar Caerus más de una vez.&lt;/p&gt;&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>window.menu.level6.title</t>
+  </si>
+  <si>
+    <t>Analyse</t>
+  </si>
+  <si>
+    <t>Análisis</t>
+  </si>
+  <si>
+    <t>window.menu.level6.sublevel1.title</t>
+  </si>
+  <si>
+    <t>Commencer une analyse</t>
+  </si>
+  <si>
+    <t>Iniciar un análisis</t>
+  </si>
+  <si>
+    <t>window.menu.level6.sublevel2.title</t>
+  </si>
+  <si>
+    <t>Charger une analyse</t>
+  </si>
+  <si>
+    <t>Cargar un análisis</t>
+  </si>
+  <si>
+    <t>#Message pour commencer une analyse</t>
+  </si>
+  <si>
+    <t>#Mensaje para iniciar un análisis</t>
+  </si>
+  <si>
+    <t>Assistant d'analyse lexicométrique</t>
+  </si>
+  <si>
+    <t>Asistente de análisis lexicométrico</t>
+  </si>
+  <si>
+    <t>window.start.analysis.code.title</t>
+  </si>
+  <si>
+    <t>window.start.analysis.information.panel.title</t>
+  </si>
+  <si>
+    <t>window.start.analysis.information.message.etape1</t>
+  </si>
+  <si>
+    <t>window.start.analysis.wizard.panel.title</t>
+  </si>
+  <si>
+    <t>window.start.analysis.information.message.etape2</t>
+  </si>
+  <si>
+    <t>window.start.analysis.option.tokenization</t>
+  </si>
+  <si>
+    <t>window.start.analysis.option.lemmatization</t>
+  </si>
+  <si>
+    <t>window.start.analysis.option.frequency</t>
+  </si>
+  <si>
+    <t>Tokenisation</t>
+  </si>
+  <si>
+    <t>Lemmatisation</t>
+  </si>
+  <si>
+    <t>Fréquence</t>
+  </si>
+  <si>
+    <t>Tokenización</t>
+  </si>
+  <si>
+    <t>Lematización</t>
+  </si>
+  <si>
+    <t>Frecuencia</t>
+  </si>
+  <si>
+    <t>window.start.analysis.option.panel.title</t>
+  </si>
+  <si>
+    <t>Choix des options d'analyse</t>
+  </si>
+  <si>
+    <t>Elección de opciones de análisis</t>
   </si>
 </sst>
 </file>
@@ -23595,8 +23686,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08B73F6F-6897-453A-A261-1E8F78D02F2C}" name="Tableau1" displayName="Tableau1" ref="A1:D53" totalsRowShown="0" headerRowDxfId="36">
-  <autoFilter ref="A1:D53" xr:uid="{5A1C5E6C-13F0-43D6-93E5-7F1D2D7A93ED}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08B73F6F-6897-453A-A261-1E8F78D02F2C}" name="Tableau1" displayName="Tableau1" ref="A1:D54" totalsRowShown="0" headerRowDxfId="36">
+  <autoFilter ref="A1:D54" xr:uid="{5A1C5E6C-13F0-43D6-93E5-7F1D2D7A93ED}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{581AA08F-F8B9-4EB9-9270-F690B4699028}" name="Numero"/>
     <tableColumn id="2" xr3:uid="{86F9FD87-A94B-4F9B-BA16-3BEE622BE071}" name="Code"/>
@@ -23719,6 +23810,19 @@
     <tableColumn id="2" xr3:uid="{2C49E31E-260D-410C-9B35-30DC774DB1F7}" name="Code"/>
     <tableColumn id="3" xr3:uid="{E6C617D7-CF79-4A76-A064-CB852BCC7498}" name="Français"/>
     <tableColumn id="4" xr3:uid="{D9CA1A11-EFBE-44C9-8E3E-B2C31B6EF7D5}" name="Español"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{3A067453-0998-4B6F-A015-C36FFF350274}" name="Tableau161015181920" displayName="Tableau161015181920" ref="A1:D58" totalsRowShown="0">
+  <autoFilter ref="A1:D58" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{93EBCA28-6850-4E5B-95B0-10E875DF804E}" name="Numero"/>
+    <tableColumn id="2" xr3:uid="{C2EDFC63-75B8-42C6-A92C-19BA73C907B7}" name="Code"/>
+    <tableColumn id="3" xr3:uid="{6F6B82DE-8489-4B2E-AE1B-00AABFE45815}" name="Français"/>
+    <tableColumn id="4" xr3:uid="{55961DE2-FCFF-4038-B649-D06B3C7FF340}" name="Español"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -24125,10 +24229,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF59B93E-40E9-44D6-98FA-7D0A802C1DCE}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24791,6 +24895,48 @@
       </c>
       <c r="D51" t="s">
         <v>726</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>44</v>
+      </c>
+      <c r="B52" t="s">
+        <v>764</v>
+      </c>
+      <c r="C52" t="s">
+        <v>765</v>
+      </c>
+      <c r="D52" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>45</v>
+      </c>
+      <c r="B53" t="s">
+        <v>767</v>
+      </c>
+      <c r="C53" t="s">
+        <v>768</v>
+      </c>
+      <c r="D53" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>46</v>
+      </c>
+      <c r="B54" t="s">
+        <v>770</v>
+      </c>
+      <c r="C54" t="s">
+        <v>771</v>
+      </c>
+      <c r="D54" t="s">
+        <v>772</v>
       </c>
     </row>
   </sheetData>
@@ -26522,7 +26668,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:D11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26901,11 +27047,662 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757EF7E0-E814-48B2-A4AF-487C809E6C10}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="65" customWidth="1"/>
+    <col min="3" max="4" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>773</v>
+      </c>
+      <c r="D2" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>777</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>778</v>
+      </c>
+      <c r="C4" t="s">
+        <v>558</v>
+      </c>
+      <c r="D4" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>779</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Bienvenue sur l'assistant d'analyse lexicométrique.&lt;BR/&gt;",
+"Vous allez pouvoir configurer l'analyse que vous souhaitez effectuer.&lt;BR/&gt;",
+"Cliquez sur suivant pour commencer l'analyse&lt;BR/&gt;",
+"NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Bienvenue sur l'assistant d'analyse lexicométrique.&lt;BR/&gt;Vous allez pouvoir configurer l'analyse que vous souhaitez effectuer.&lt;BR/&gt;Cliquez sur suivant pour commencer l'analyse&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Bienvenido al asistente de análisis lexicométrico.&lt;BR/&gt;",
+"Podrás configurar el análisis que quieras realizar.&lt;BR/&gt;",
+"Haga clic en siguiente para iniciar el análisis.&lt;BR/&gt;",
+"NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Bienvenido al asistente de análisis lexicométrico.&lt;BR/&gt;Podrás configurar el análisis que quieras realizar.&lt;BR/&gt;Haga clic en siguiente para iniciar el análisis.&lt;BR/&gt;NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>780</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>781</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Sélectionnez les options d'analyse que vous souhaitez effectuer.&lt;BR/&gt;",
+"Tokenisation : Pour nettoyer le texte des éléments qui ne sont pas à analyser.&lt;BR/&gt;",
+"Lemmatisation : Pour remplacer l'ensemble des variations par son lemme.&lt;BR/&gt;",
+"Fréquence : Analyse par fréquence des mots d'un texte.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Sélectionnez les options d'analyse que vous souhaitez effectuer.&lt;BR/&gt;Tokenisation : Pour nettoyer le texte des éléments qui ne sont pas à analyser.&lt;BR/&gt;Lemmatisation : Pour remplacer l'ensemble des variations par son lemme.&lt;BR/&gt;Fréquence : Analyse par fréquence des mots d'un texte.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Seleccione las opciones de análisis que desea realizar. &lt;BR/&gt; ",
+"&lt;U&gt;&lt;B&gt;Tokenización :&lt;/U&gt; &lt;/B&gt; Para limpiar texto de elementos que no se van a escanear. &lt;BR/&gt;",
+"&lt;U&gt;&lt;B&gt;Lematización :&lt;/U&gt; &lt;/B&gt; Reemplazar el conjunto de variaciones por su lema. &lt;BR/&gt;",
+"&lt;U&gt;&lt;B&gt;Frecuencia :&lt;/U&gt; &lt;/B&gt; Análisis de frecuencia de palabras en un texto.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Seleccione las opciones de análisis que desea realizar. &lt;BR/&gt; &lt;U&gt;&lt;B&gt;Tokenización :&lt;/U&gt; &lt;/B&gt; Para limpiar texto de elementos que no se van a escanear. &lt;BR/&gt;&lt;U&gt;&lt;B&gt;Lematización :&lt;/U&gt; &lt;/B&gt; Reemplazar el conjunto de variaciones por su lema. &lt;BR/&gt;&lt;U&gt;&lt;B&gt;Frecuencia :&lt;/U&gt; &lt;/B&gt; Análisis de frecuencia de palabras en un texto.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>782</v>
+      </c>
+      <c r="C8" t="s">
+        <v>785</v>
+      </c>
+      <c r="D8" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>783</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>784</v>
+      </c>
+      <c r="C10" t="s">
+        <v>787</v>
+      </c>
+      <c r="D10" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>791</v>
+      </c>
+      <c r="C11" t="s">
+        <v>792</v>
+      </c>
+      <c r="D11" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B77FE015-45ED-4C89-B5D1-EDB5C6B1F7DA}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="B7:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="58.140625" customWidth="1"/>
+    <col min="3" max="4" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>464</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>575</v>
+      </c>
+      <c r="D6" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>466</v>
+      </c>
+      <c r="D9" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" t="s">
+        <v>468</v>
+      </c>
+      <c r="D11" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>569</v>
+      </c>
+      <c r="C12" t="s">
+        <v>558</v>
+      </c>
+      <c r="D12" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>570</v>
+      </c>
+      <c r="C13" t="s">
+        <v>573</v>
+      </c>
+      <c r="D13" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>571</v>
+      </c>
+      <c r="C14" t="s">
+        <v>590</v>
+      </c>
+      <c r="D14" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>592</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quelle est la balise correspondante à cette ligne ?&lt;BR/&gt;",
+"Utilisez la liste, pour sélectionner la balise adéquate.&lt;BR/&gt;",
+"Puis cliquez sur suivant.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Quelle est la balise correspondante à cette ligne ?&lt;BR/&gt;Utilisez la liste, pour sélectionner la balise adéquate.&lt;BR/&gt;Puis cliquez sur suivant.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;¿Cuál es la etiqueta correspondiente a esta línea?&lt;BR/&gt;",
+"Utilice la lista para seleccionar la etiqueta adecuada.&lt;BR/&gt;",
+"Luego haga clic en siguiente.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;¿Cuál es la etiqueta correspondiente a esta línea?&lt;BR/&gt;Utilice la lista para seleccionar la etiqueta adecuada.&lt;BR/&gt;Luego haga clic en siguiente.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>593</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quel est le contenu de la balise ?&lt;BR/&gt;",
+"Pour sélectionner les données textuelles de la balise, utilisez la souris,&lt;BR/&gt;",
+"sélectionnez la partie correspondante aux données textuelles&lt;BR/&gt;",
+"dans la zone à gauche du bouton 'identifier' et cliquez dessus ce bouton.&lt;BR/&gt;",
+"La zone de texte en dessous a été mise à jour avec le contenu que vous&lt;BR/&gt;",
+"avez sélectionné, ci cela vous convient cliquez sur suivant sinon, recommencez.&lt;BR/&gt;",
+"NB : Si le texte n'est pas complet ou erroné, vous pourrez le modifier&lt;BR/&gt;",
+"à l'étape suivante.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Quel est le contenu de la balise ?&lt;BR/&gt;Pour sélectionner les données textuelles de la balise, utilisez la souris,&lt;BR/&gt;sélectionnez la partie correspondante aux données textuelles&lt;BR/&gt;dans la zone à gauche du bouton 'identifier' et cliquez dessus ce bouton.&lt;BR/&gt;La zone de texte en dessous a été mise à jour avec le contenu que vous&lt;BR/&gt;avez sélectionné, ci cela vous convient cliquez sur suivant sinon, recommencez.&lt;BR/&gt;NB : Si le texte n'est pas complet ou erroné, vous pourrez le modifier&lt;BR/&gt;à l'étape suivante.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;¿Cuál es el contenido de la etiqueta?&lt;BR/&gt;",
+"Para seleccionar los datos de texto de la etiqueta, utilice el ratón,&lt;BR/&gt;",
+"seleccione la parte correspondiente a los datos de texto&lt;BR/&gt;",
+"en el área a la izquierda del botón 'identificar ' y haga clic en él.&lt;BR/&gt;",
+"El cuadro de texto de abajo se ha actualizado con el contenido que usted&lt;BR/&gt;",
+"ha seleccionado, esto le conviene haga clic en siguiente si no, reinicie.&lt;BR/&gt;",
+"Nota: Si el texto no es completo o erróneo, podrá editarlo&lt;BR/&gt;",
+"en el siguiente paso.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;¿Cuál es el contenido de la etiqueta?&lt;BR/&gt;Para seleccionar los datos de texto de la etiqueta, utilice el ratón,&lt;BR/&gt;seleccione la parte correspondiente a los datos de texto&lt;BR/&gt;en el área a la izquierda del botón 'identificar ' y haga clic en él.&lt;BR/&gt;El cuadro de texto de abajo se ha actualizado con el contenido que usted&lt;BR/&gt;ha seleccionado, esto le conviene haga clic en siguiente si no, reinicie.&lt;BR/&gt;Nota: Si el texto no es completo o erróneo, podrá editarlo&lt;BR/&gt;en el siguiente paso.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>594</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Tout est bon ?&lt;BR/&gt;",
+"Nous avons affiché la ligne corrigé dans l'encadré ci-dessus.&lt;BR/&gt;",
+"Si le contenu de la balise ne vous convient pas, vous pouvez faire&lt;BR/&gt;",
+"précédent et effectuer des modifications,&lt;BR/&gt;",
+"la ligne sera alors mise à jour en conséquences.&lt;BR/&gt;",
+"Une fois que tout est bon, cliquez sur le bouton de correction de&lt;BR/&gt;",
+"la ligne tout en bas de la fenêtre&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Tout est bon ?&lt;BR/&gt;Nous avons affiché la ligne corrigé dans l'encadré ci-dessus.&lt;BR/&gt;Si le contenu de la balise ne vous convient pas, vous pouvez faire&lt;BR/&gt;précédent et effectuer des modifications,&lt;BR/&gt;la ligne sera alors mise à jour en conséquences.&lt;BR/&gt;Une fois que tout est bon, cliquez sur le bouton de correction de&lt;BR/&gt;la ligne tout en bas de la fenêtre&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;¿Está todo bien aquí?&lt;BR/&gt;",
+"Hemos publicado la línea corregida en el recuadro anterior.&lt;BR/&gt;",
+"Si el contenido de la etiqueta no es adecuado para usted, puede hacer&lt;BR/&gt;",
+"anterior y realizar modificaciones,&lt;BR/&gt;",
+"la línea se actualizará en consecuencia.&lt;BR/&gt;",
+"Una vez que todo está bien, haga clic en el botón de corrección de&lt;BR/&gt;",
+"la línea en la parte inferior de la pantalla&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;¿Está todo bien aquí?&lt;BR/&gt;Hemos publicado la línea corregida en el recuadro anterior.&lt;BR/&gt;Si el contenido de la etiqueta no es adecuado para usted, puede hacer&lt;BR/&gt;anterior y realizar modificaciones,&lt;BR/&gt;la línea se actualizará en consecuencia.&lt;BR/&gt;Una vez que todo está bien, haga clic en el botón de corrección de&lt;BR/&gt;la línea en la parte inferior de la pantalla&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>595</v>
+      </c>
+      <c r="C18" t="s">
+        <v>613</v>
+      </c>
+      <c r="D18" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>596</v>
+      </c>
+      <c r="C19" t="s">
+        <v>601</v>
+      </c>
+      <c r="D19" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>597</v>
+      </c>
+      <c r="C20" t="s">
+        <v>600</v>
+      </c>
+      <c r="D20" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>598</v>
+      </c>
+      <c r="C21" t="s">
+        <v>599</v>
+      </c>
+      <c r="D21" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>602</v>
+      </c>
+      <c r="C22" t="s">
+        <v>603</v>
+      </c>
+      <c r="D22" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>604</v>
+      </c>
+      <c r="C23" t="s">
+        <v>605</v>
+      </c>
+      <c r="D23" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>606</v>
+      </c>
+      <c r="C24" t="s">
+        <v>607</v>
+      </c>
+      <c r="D24" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>608</v>
+      </c>
+      <c r="C25" t="s">
+        <v>609</v>
+      </c>
+      <c r="D25" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>610</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>591</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Bienvenue sur l'assistant de correction des lignes.&lt;BR/&gt;",
+"Suite à l'analyse, des lignes n'ont pas pu être interprété par le système.&lt;BR/&gt;",
+"Dans l'encadré ci-dessus, vous pouvez voir les informations en question.&lt;BR/&gt;",
+"Cliquez sur suivant pour commencer la correction.&lt;BR/&gt;",
+"NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Bienvenue sur l'assistant de correction des lignes.&lt;BR/&gt;Suite à l'analyse, des lignes n'ont pas pu être interprété par le système.&lt;BR/&gt;Dans l'encadré ci-dessus, vous pouvez voir les informations en question.&lt;BR/&gt;Cliquez sur suivant pour commencer la correction.&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Bienvenido al asistente de corrección de líneas.&lt;BR/&gt;",
+"Como resultado del análisis, las líneas no pudieron ser interpretadas por el sistema.&lt;BR/&gt;",
+"En el recuadro anterior se puede ver la información en cuestión.&lt;BR/&gt;",
+"Haga clic en siguiente para comenzar la corrección.&lt;BR/&gt;",
+"NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Bienvenido al asistente de corrección de líneas.&lt;BR/&gt;Como resultado del análisis, las líneas no pudieron ser interpretadas por el sistema.&lt;BR/&gt;En el recuadro anterior se puede ver la información en cuestión.&lt;BR/&gt;Haga clic en siguiente para comenzar la corrección.&lt;BR/&gt;NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904B2FA-CBC2-495A-A197-D0CDD47EB1AE}">
-  <dimension ref="A1:A504"/>
+  <dimension ref="A1:A563"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A343" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A368" sqref="A1:A504"/>
+    <sheetView showZeros="0" topLeftCell="A490" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A510" sqref="A510:A513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27216,19 +28013,19 @@
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>IF('Fenêtre principal'!B52&lt;&gt;"",CONCATENATE('Fenêtre principal'!B52,"=", 'Fenêtre principal'!C52),IF('Fenêtre principal'!C52&lt;&gt;"",'Fenêtre principal'!C52,""))</f>
-        <v/>
+        <v>window.menu.level6.title=Analyse</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>IF('Fenêtre principal'!B53&lt;&gt;"",CONCATENATE('Fenêtre principal'!B53,"=", 'Fenêtre principal'!C53),IF('Fenêtre principal'!C53&lt;&gt;"",'Fenêtre principal'!C53,""))</f>
-        <v/>
+        <v>window.menu.level6.sublevel1.title=Commencer une analyse</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>IF('Fenêtre principal'!B54&lt;&gt;"",CONCATENATE('Fenêtre principal'!B54,"=", 'Fenêtre principal'!C54),IF('Fenêtre principal'!C54&lt;&gt;"",'Fenêtre principal'!C54,""))</f>
-        <v/>
+        <v>window.menu.level6.sublevel2.title=Charger une analyse</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
@@ -29937,461 +30734,372 @@
         <v/>
       </c>
     </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" t="str">
+        <f>IF('Commencer analyse'!B2&lt;&gt;"",CONCATENATE('Commencer analyse'!B2,"=", 'Commencer analyse'!C2),IF('Commencer analyse'!C2&lt;&gt;"",'Commencer analyse'!C2,""))</f>
+        <v>#Message pour commencer une analyse</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" t="str">
+        <f>IF('Commencer analyse'!B3&lt;&gt;"",CONCATENATE('Commencer analyse'!B3,"=", 'Commencer analyse'!C3),IF('Commencer analyse'!C3&lt;&gt;"",'Commencer analyse'!C3,""))</f>
+        <v>window.start.analysis.code.title=Analyse</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" t="str">
+        <f>IF('Commencer analyse'!B4&lt;&gt;"",CONCATENATE('Commencer analyse'!B4,"=", 'Commencer analyse'!C4),IF('Commencer analyse'!C4&lt;&gt;"",'Commencer analyse'!C4,""))</f>
+        <v>window.start.analysis.information.panel.title=Informations</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" t="str">
+        <f>IF('Commencer analyse'!B5&lt;&gt;"",CONCATENATE('Commencer analyse'!B5,"=", 'Commencer analyse'!C5),IF('Commencer analyse'!C5&lt;&gt;"",'Commencer analyse'!C5,""))</f>
+        <v>window.start.analysis.information.message.etape1=&lt;HTML&gt;&lt;P&gt;Bienvenue sur l'assistant d'analyse lexicométrique.&lt;BR/&gt;Vous allez pouvoir configurer l'analyse que vous souhaitez effectuer.&lt;BR/&gt;Cliquez sur suivant pour commencer l'analyse&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" t="str">
+        <f>IF('Commencer analyse'!B6&lt;&gt;"",CONCATENATE('Commencer analyse'!B6,"=", 'Commencer analyse'!C6),IF('Commencer analyse'!C6&lt;&gt;"",'Commencer analyse'!C6,""))</f>
+        <v>window.start.analysis.wizard.panel.title=Assistant d'analyse lexicométrique</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" t="str">
+        <f>IF('Commencer analyse'!B7&lt;&gt;"",CONCATENATE('Commencer analyse'!B7,"=", 'Commencer analyse'!C7),IF('Commencer analyse'!C7&lt;&gt;"",'Commencer analyse'!C7,""))</f>
+        <v>window.start.analysis.information.message.etape2=&lt;HTML&gt;&lt;P&gt;Sélectionnez les options d'analyse que vous souhaitez effectuer.&lt;BR/&gt;Tokenisation : Pour nettoyer le texte des éléments qui ne sont pas à analyser.&lt;BR/&gt;Lemmatisation : Pour remplacer l'ensemble des variations par son lemme.&lt;BR/&gt;Fréquence : Analyse par fréquence des mots d'un texte.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" t="str">
+        <f>IF('Commencer analyse'!B8&lt;&gt;"",CONCATENATE('Commencer analyse'!B8,"=", 'Commencer analyse'!C8),IF('Commencer analyse'!C8&lt;&gt;"",'Commencer analyse'!C8,""))</f>
+        <v>window.start.analysis.option.tokenization=Tokenisation</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" t="str">
+        <f>IF('Commencer analyse'!B9&lt;&gt;"",CONCATENATE('Commencer analyse'!B9,"=", 'Commencer analyse'!C9),IF('Commencer analyse'!C9&lt;&gt;"",'Commencer analyse'!C9,""))</f>
+        <v>window.start.analysis.option.lemmatization=Lemmatisation</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" t="str">
+        <f>IF('Commencer analyse'!B10&lt;&gt;"",CONCATENATE('Commencer analyse'!B10,"=", 'Commencer analyse'!C10),IF('Commencer analyse'!C10&lt;&gt;"",'Commencer analyse'!C10,""))</f>
+        <v>window.start.analysis.option.frequency=Fréquence</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" t="str">
+        <f>IF('Commencer analyse'!B11&lt;&gt;"",CONCATENATE('Commencer analyse'!B11,"=", 'Commencer analyse'!C11),IF('Commencer analyse'!C11&lt;&gt;"",'Commencer analyse'!C11,""))</f>
+        <v>window.start.analysis.option.panel.title=Choix des options d'analyse</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" t="str">
+        <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE('Commencer analyse'!B12,"=", 'Commencer analyse'!C12),IF('Commencer analyse'!C12&lt;&gt;"",'Commencer analyse'!C12,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" t="str">
+        <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE('Commencer analyse'!B13,"=", 'Commencer analyse'!C13),IF('Commencer analyse'!C13&lt;&gt;"",'Commencer analyse'!C13,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" t="str">
+        <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE('Commencer analyse'!B14,"=", 'Commencer analyse'!C14),IF('Commencer analyse'!C14&lt;&gt;"",'Commencer analyse'!C14,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" t="str">
+        <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE('Commencer analyse'!B15,"=", 'Commencer analyse'!C15),IF('Commencer analyse'!C15&lt;&gt;"",'Commencer analyse'!C15,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" t="str">
+        <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE('Commencer analyse'!B16,"=", 'Commencer analyse'!C16),IF('Commencer analyse'!C16&lt;&gt;"",'Commencer analyse'!C16,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" t="str">
+        <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE('Commencer analyse'!B17,"=", 'Commencer analyse'!C17),IF('Commencer analyse'!C17&lt;&gt;"",'Commencer analyse'!C17,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" t="str">
+        <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE('Commencer analyse'!B18,"=", 'Commencer analyse'!C18),IF('Commencer analyse'!C18&lt;&gt;"",'Commencer analyse'!C18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" t="str">
+        <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE('Commencer analyse'!B19,"=", 'Commencer analyse'!C19),IF('Commencer analyse'!C19&lt;&gt;"",'Commencer analyse'!C19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" t="str">
+        <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE('Commencer analyse'!B20,"=", 'Commencer analyse'!C20),IF('Commencer analyse'!C20&lt;&gt;"",'Commencer analyse'!C20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" t="str">
+        <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE('Commencer analyse'!B21,"=", 'Commencer analyse'!C21),IF('Commencer analyse'!C21&lt;&gt;"",'Commencer analyse'!C21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525" t="str">
+        <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE('Commencer analyse'!B22,"=", 'Commencer analyse'!C22),IF('Commencer analyse'!C22&lt;&gt;"",'Commencer analyse'!C22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526" t="str">
+        <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE('Commencer analyse'!B23,"=", 'Commencer analyse'!C23),IF('Commencer analyse'!C23&lt;&gt;"",'Commencer analyse'!C23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527" t="str">
+        <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE('Commencer analyse'!B24,"=", 'Commencer analyse'!C24),IF('Commencer analyse'!C24&lt;&gt;"",'Commencer analyse'!C24,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A528" t="str">
+        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE('Commencer analyse'!B25,"=", 'Commencer analyse'!C25),IF('Commencer analyse'!C25&lt;&gt;"",'Commencer analyse'!C25,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A529" t="str">
+        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE('Commencer analyse'!B26,"=", 'Commencer analyse'!C26),IF('Commencer analyse'!C26&lt;&gt;"",'Commencer analyse'!C26,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A530" t="str">
+        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE('Commencer analyse'!B27,"=", 'Commencer analyse'!C27),IF('Commencer analyse'!C27&lt;&gt;"",'Commencer analyse'!C27,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A531" t="str">
+        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE('Commencer analyse'!B28,"=", 'Commencer analyse'!C28),IF('Commencer analyse'!C28&lt;&gt;"",'Commencer analyse'!C28,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A532" t="str">
+        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE('Commencer analyse'!B29,"=", 'Commencer analyse'!C29),IF('Commencer analyse'!C29&lt;&gt;"",'Commencer analyse'!C29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A533" t="str">
+        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE('Commencer analyse'!B30,"=", 'Commencer analyse'!C30),IF('Commencer analyse'!C30&lt;&gt;"",'Commencer analyse'!C30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A534" t="str">
+        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE('Commencer analyse'!B31,"=", 'Commencer analyse'!C31),IF('Commencer analyse'!C31&lt;&gt;"",'Commencer analyse'!C31,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A535" t="str">
+        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE('Commencer analyse'!B32,"=", 'Commencer analyse'!C32),IF('Commencer analyse'!C32&lt;&gt;"",'Commencer analyse'!C32,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A536" t="str">
+        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE('Commencer analyse'!B33,"=", 'Commencer analyse'!C33),IF('Commencer analyse'!C33&lt;&gt;"",'Commencer analyse'!C33,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A537" t="str">
+        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE('Commencer analyse'!B34,"=", 'Commencer analyse'!C34),IF('Commencer analyse'!C34&lt;&gt;"",'Commencer analyse'!C34,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A538" t="str">
+        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE('Commencer analyse'!B35,"=", 'Commencer analyse'!C35),IF('Commencer analyse'!C35&lt;&gt;"",'Commencer analyse'!C35,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A539" t="str">
+        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE('Commencer analyse'!B36,"=", 'Commencer analyse'!C36),IF('Commencer analyse'!C36&lt;&gt;"",'Commencer analyse'!C36,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A540" t="str">
+        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE('Commencer analyse'!B37,"=", 'Commencer analyse'!C37),IF('Commencer analyse'!C37&lt;&gt;"",'Commencer analyse'!C37,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A541" t="str">
+        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE('Commencer analyse'!B38,"=", 'Commencer analyse'!C38),IF('Commencer analyse'!C38&lt;&gt;"",'Commencer analyse'!C38,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A542" t="str">
+        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE('Commencer analyse'!B39,"=", 'Commencer analyse'!C39),IF('Commencer analyse'!C39&lt;&gt;"",'Commencer analyse'!C39,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A543" t="str">
+        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE('Commencer analyse'!B40,"=", 'Commencer analyse'!C40),IF('Commencer analyse'!C40&lt;&gt;"",'Commencer analyse'!C40,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A544" t="str">
+        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE('Commencer analyse'!B41,"=", 'Commencer analyse'!C41),IF('Commencer analyse'!C41&lt;&gt;"",'Commencer analyse'!C41,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A545" t="str">
+        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE('Commencer analyse'!B42,"=", 'Commencer analyse'!C42),IF('Commencer analyse'!C42&lt;&gt;"",'Commencer analyse'!C42,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A546" t="str">
+        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE('Commencer analyse'!B43,"=", 'Commencer analyse'!C43),IF('Commencer analyse'!C43&lt;&gt;"",'Commencer analyse'!C43,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A547" t="str">
+        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE('Commencer analyse'!B44,"=", 'Commencer analyse'!C44),IF('Commencer analyse'!C44&lt;&gt;"",'Commencer analyse'!C44,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A548" t="str">
+        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE('Commencer analyse'!B45,"=", 'Commencer analyse'!C45),IF('Commencer analyse'!C45&lt;&gt;"",'Commencer analyse'!C45,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A549" t="str">
+        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE('Commencer analyse'!B46,"=", 'Commencer analyse'!C46),IF('Commencer analyse'!C46&lt;&gt;"",'Commencer analyse'!C46,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A550" t="str">
+        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE('Commencer analyse'!B47,"=", 'Commencer analyse'!C47),IF('Commencer analyse'!C47&lt;&gt;"",'Commencer analyse'!C47,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A551" t="str">
+        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE('Commencer analyse'!B48,"=", 'Commencer analyse'!C48),IF('Commencer analyse'!C48&lt;&gt;"",'Commencer analyse'!C48,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A552" t="str">
+        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE('Commencer analyse'!B49,"=", 'Commencer analyse'!C49),IF('Commencer analyse'!C49&lt;&gt;"",'Commencer analyse'!C49,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A553" t="str">
+        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE('Commencer analyse'!B50,"=", 'Commencer analyse'!C50),IF('Commencer analyse'!C50&lt;&gt;"",'Commencer analyse'!C50,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A554" t="str">
+        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE('Commencer analyse'!B51,"=", 'Commencer analyse'!C51),IF('Commencer analyse'!C51&lt;&gt;"",'Commencer analyse'!C51,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A555" t="str">
+        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE('Commencer analyse'!B52,"=", 'Commencer analyse'!C52),IF('Commencer analyse'!C52&lt;&gt;"",'Commencer analyse'!C52,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A556" t="str">
+        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE('Commencer analyse'!B53,"=", 'Commencer analyse'!C53),IF('Commencer analyse'!C53&lt;&gt;"",'Commencer analyse'!C53,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A557" t="str">
+        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE('Commencer analyse'!B54,"=", 'Commencer analyse'!C54),IF('Commencer analyse'!C54&lt;&gt;"",'Commencer analyse'!C54,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A558" t="str">
+        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE('Commencer analyse'!B55,"=", 'Commencer analyse'!C55),IF('Commencer analyse'!C55&lt;&gt;"",'Commencer analyse'!C55,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A559" t="str">
+        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE('Commencer analyse'!B56,"=", 'Commencer analyse'!C56),IF('Commencer analyse'!C56&lt;&gt;"",'Commencer analyse'!C56,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A560" t="str">
+        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE('Commencer analyse'!B57,"=", 'Commencer analyse'!C57),IF('Commencer analyse'!C57&lt;&gt;"",'Commencer analyse'!C57,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A561" t="str">
+        <f>IF('Commencer analyse'!B58&lt;&gt;"",CONCATENATE('Commencer analyse'!B58,"=", 'Commencer analyse'!C58),IF('Commencer analyse'!C58&lt;&gt;"",'Commencer analyse'!C58,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A562" t="str">
+        <f>IF('Commencer analyse'!B59&lt;&gt;"",CONCATENATE('Commencer analyse'!B59,"=", 'Commencer analyse'!C59),IF('Commencer analyse'!C59&lt;&gt;"",'Commencer analyse'!C59,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A563" t="str">
+        <f>IF('Commencer analyse'!B60&lt;&gt;"",CONCATENATE('Commencer analyse'!B60,"=", 'Commencer analyse'!C60),IF('Commencer analyse'!C60&lt;&gt;"",'Commencer analyse'!C60,""))</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B77FE015-45ED-4C89-B5D1-EDB5C6B1F7DA}">
-  <dimension ref="A1:D27"/>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
+  <dimension ref="A1:A563"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:A27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="58.140625" customWidth="1"/>
-    <col min="3" max="4" width="50.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>464</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" t="s">
-        <v>575</v>
-      </c>
-      <c r="D6" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" t="s">
-        <v>466</v>
-      </c>
-      <c r="D9" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" t="s">
-        <v>468</v>
-      </c>
-      <c r="D11" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>569</v>
-      </c>
-      <c r="C12" t="s">
-        <v>558</v>
-      </c>
-      <c r="D12" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>570</v>
-      </c>
-      <c r="C13" t="s">
-        <v>573</v>
-      </c>
-      <c r="D13" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>571</v>
-      </c>
-      <c r="C14" t="s">
-        <v>590</v>
-      </c>
-      <c r="D14" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>592</v>
-      </c>
-      <c r="C15" s="1" t="str">
-        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quelle est la balise correspondante à cette ligne ?&lt;BR/&gt;",
-"Utilisez la liste, pour sélectionner la balise adéquate.&lt;BR/&gt;",
-"Puis cliquez sur suivant.&lt;/P&gt;&lt;/HTML&gt;")</f>
-        <v>&lt;HTML&gt;&lt;P&gt;Quelle est la balise correspondante à cette ligne ?&lt;BR/&gt;Utilisez la liste, pour sélectionner la balise adéquate.&lt;BR/&gt;Puis cliquez sur suivant.&lt;/P&gt;&lt;/HTML&gt;</v>
-      </c>
-      <c r="D15" s="1" t="str">
-        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;¿Cuál es la etiqueta correspondiente a esta línea?&lt;BR/&gt;",
-"Utilice la lista para seleccionar la etiqueta adecuada.&lt;BR/&gt;",
-"Luego haga clic en siguiente.&lt;/P&gt;&lt;/HTML&gt;")</f>
-        <v>&lt;HTML&gt;&lt;P&gt;¿Cuál es la etiqueta correspondiente a esta línea?&lt;BR/&gt;Utilice la lista para seleccionar la etiqueta adecuada.&lt;BR/&gt;Luego haga clic en siguiente.&lt;/P&gt;&lt;/HTML&gt;</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="165" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>593</v>
-      </c>
-      <c r="C16" s="1" t="str">
-        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quel est le contenu de la balise ?&lt;BR/&gt;",
-"Pour sélectionner les données textuelles de la balise, utilisez la souris,&lt;BR/&gt;",
-"sélectionnez la partie correspondante aux données textuelles&lt;BR/&gt;",
-"dans la zone à gauche du bouton 'identifier' et cliquez dessus ce bouton.&lt;BR/&gt;",
-"La zone de texte en dessous a été mise à jour avec le contenu que vous&lt;BR/&gt;",
-"avez sélectionné, ci cela vous convient cliquez sur suivant sinon, recommencez.&lt;BR/&gt;",
-"NB : Si le texte n'est pas complet ou erroné, vous pourrez le modifier&lt;BR/&gt;",
-"à l'étape suivante.&lt;/P&gt;&lt;/HTML&gt;")</f>
-        <v>&lt;HTML&gt;&lt;P&gt;Quel est le contenu de la balise ?&lt;BR/&gt;Pour sélectionner les données textuelles de la balise, utilisez la souris,&lt;BR/&gt;sélectionnez la partie correspondante aux données textuelles&lt;BR/&gt;dans la zone à gauche du bouton 'identifier' et cliquez dessus ce bouton.&lt;BR/&gt;La zone de texte en dessous a été mise à jour avec le contenu que vous&lt;BR/&gt;avez sélectionné, ci cela vous convient cliquez sur suivant sinon, recommencez.&lt;BR/&gt;NB : Si le texte n'est pas complet ou erroné, vous pourrez le modifier&lt;BR/&gt;à l'étape suivante.&lt;/P&gt;&lt;/HTML&gt;</v>
-      </c>
-      <c r="D16" s="1" t="str">
-        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;¿Cuál es el contenido de la etiqueta?&lt;BR/&gt;",
-"Para seleccionar los datos de texto de la etiqueta, utilice el ratón,&lt;BR/&gt;",
-"seleccione la parte correspondiente a los datos de texto&lt;BR/&gt;",
-"en el área a la izquierda del botón 'identificar ' y haga clic en él.&lt;BR/&gt;",
-"El cuadro de texto de abajo se ha actualizado con el contenido que usted&lt;BR/&gt;",
-"ha seleccionado, esto le conviene haga clic en siguiente si no, reinicie.&lt;BR/&gt;",
-"Nota: Si el texto no es completo o erróneo, podrá editarlo&lt;BR/&gt;",
-"en el siguiente paso.&lt;/P&gt;&lt;/HTML&gt;")</f>
-        <v>&lt;HTML&gt;&lt;P&gt;¿Cuál es el contenido de la etiqueta?&lt;BR/&gt;Para seleccionar los datos de texto de la etiqueta, utilice el ratón,&lt;BR/&gt;seleccione la parte correspondiente a los datos de texto&lt;BR/&gt;en el área a la izquierda del botón 'identificar ' y haga clic en él.&lt;BR/&gt;El cuadro de texto de abajo se ha actualizado con el contenido que usted&lt;BR/&gt;ha seleccionado, esto le conviene haga clic en siguiente si no, reinicie.&lt;BR/&gt;Nota: Si el texto no es completo o erróneo, podrá editarlo&lt;BR/&gt;en el siguiente paso.&lt;/P&gt;&lt;/HTML&gt;</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>594</v>
-      </c>
-      <c r="C17" s="1" t="str">
-        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Tout est bon ?&lt;BR/&gt;",
-"Nous avons affiché la ligne corrigé dans l'encadré ci-dessus.&lt;BR/&gt;",
-"Si le contenu de la balise ne vous convient pas, vous pouvez faire&lt;BR/&gt;",
-"précédent et effectuer des modifications,&lt;BR/&gt;",
-"la ligne sera alors mise à jour en conséquences.&lt;BR/&gt;",
-"Une fois que tout est bon, cliquez sur le bouton de correction de&lt;BR/&gt;",
-"la ligne tout en bas de la fenêtre&lt;/P&gt;&lt;/HTML&gt;")</f>
-        <v>&lt;HTML&gt;&lt;P&gt;Tout est bon ?&lt;BR/&gt;Nous avons affiché la ligne corrigé dans l'encadré ci-dessus.&lt;BR/&gt;Si le contenu de la balise ne vous convient pas, vous pouvez faire&lt;BR/&gt;précédent et effectuer des modifications,&lt;BR/&gt;la ligne sera alors mise à jour en conséquences.&lt;BR/&gt;Une fois que tout est bon, cliquez sur le bouton de correction de&lt;BR/&gt;la ligne tout en bas de la fenêtre&lt;/P&gt;&lt;/HTML&gt;</v>
-      </c>
-      <c r="D17" s="1" t="str">
-        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;¿Está todo bien aquí?&lt;BR/&gt;",
-"Hemos publicado la línea corregida en el recuadro anterior.&lt;BR/&gt;",
-"Si el contenido de la etiqueta no es adecuado para usted, puede hacer&lt;BR/&gt;",
-"anterior y realizar modificaciones,&lt;BR/&gt;",
-"la línea se actualizará en consecuencia.&lt;BR/&gt;",
-"Una vez que todo está bien, haga clic en el botón de corrección de&lt;BR/&gt;",
-"la línea en la parte inferior de la pantalla&lt;/P&gt;&lt;/HTML&gt;")</f>
-        <v>&lt;HTML&gt;&lt;P&gt;¿Está todo bien aquí?&lt;BR/&gt;Hemos publicado la línea corregida en el recuadro anterior.&lt;BR/&gt;Si el contenido de la etiqueta no es adecuado para usted, puede hacer&lt;BR/&gt;anterior y realizar modificaciones,&lt;BR/&gt;la línea se actualizará en consecuencia.&lt;BR/&gt;Una vez que todo está bien, haga clic en el botón de corrección de&lt;BR/&gt;la línea en la parte inferior de la pantalla&lt;/P&gt;&lt;/HTML&gt;</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>595</v>
-      </c>
-      <c r="C18" t="s">
-        <v>613</v>
-      </c>
-      <c r="D18" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>596</v>
-      </c>
-      <c r="C19" t="s">
-        <v>601</v>
-      </c>
-      <c r="D19" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>597</v>
-      </c>
-      <c r="C20" t="s">
-        <v>600</v>
-      </c>
-      <c r="D20" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>598</v>
-      </c>
-      <c r="C21" t="s">
-        <v>599</v>
-      </c>
-      <c r="D21" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>602</v>
-      </c>
-      <c r="C22" t="s">
-        <v>603</v>
-      </c>
-      <c r="D22" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>604</v>
-      </c>
-      <c r="C23" t="s">
-        <v>605</v>
-      </c>
-      <c r="D23" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>606</v>
-      </c>
-      <c r="C24" t="s">
-        <v>607</v>
-      </c>
-      <c r="D24" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>608</v>
-      </c>
-      <c r="C25" t="s">
-        <v>609</v>
-      </c>
-      <c r="D25" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>610</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>591</v>
-      </c>
-      <c r="C27" s="1" t="str">
-        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Bienvenue sur l'assistant de correction des lignes.&lt;BR/&gt;",
-"Suite à l'analyse, des lignes n'ont pas pu être interprété par le système.&lt;BR/&gt;",
-"Dans l'encadré ci-dessus, vous pouvez voir les informations en question.&lt;BR/&gt;",
-"Cliquez sur suivant pour commencer la correction.&lt;BR/&gt;",
-"NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;")</f>
-        <v>&lt;HTML&gt;&lt;P&gt;Bienvenue sur l'assistant de correction des lignes.&lt;BR/&gt;Suite à l'analyse, des lignes n'ont pas pu être interprété par le système.&lt;BR/&gt;Dans l'encadré ci-dessus, vous pouvez voir les informations en question.&lt;BR/&gt;Cliquez sur suivant pour commencer la correction.&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
-      </c>
-      <c r="D27" s="1" t="str">
-        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Bienvenido al asistente de corrección de líneas.&lt;BR/&gt;",
-"Como resultado del análisis, las líneas no pudieron ser interpretadas por el sistema.&lt;BR/&gt;",
-"En el recuadro anterior se puede ver la información en cuestión.&lt;BR/&gt;",
-"Haga clic en siguiente para comenzar la corrección.&lt;BR/&gt;",
-"NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;")</f>
-        <v>&lt;HTML&gt;&lt;P&gt;Bienvenido al asistente de corrección de líneas.&lt;BR/&gt;Como resultado del análisis, las líneas no pudieron ser interpretadas por el sistema.&lt;BR/&gt;En el recuadro anterior se puede ver la información en cuestión.&lt;BR/&gt;Haga clic en siguiente para comenzar la corrección.&lt;BR/&gt;NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
-  <dimension ref="A1:A507"/>
-  <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A358" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A375" sqref="A1:A507"/>
+    <sheetView showZeros="0" topLeftCell="A497" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A510" sqref="A510:A513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30702,19 +31410,19 @@
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>IF('Fenêtre principal'!B52&lt;&gt;"",CONCATENATE('Fenêtre principal'!B52,"=", 'Fenêtre principal'!D52),IF('Fenêtre principal'!D52&lt;&gt;"",'Fenêtre principal'!D52,""))</f>
-        <v/>
+        <v>window.menu.level6.title=Análisis</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>IF('Fenêtre principal'!B53&lt;&gt;"",CONCATENATE('Fenêtre principal'!B53,"=", 'Fenêtre principal'!D53),IF('Fenêtre principal'!D53&lt;&gt;"",'Fenêtre principal'!D53,""))</f>
-        <v/>
+        <v>window.menu.level6.sublevel1.title=Iniciar un análisis</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>IF('Fenêtre principal'!B54&lt;&gt;"",CONCATENATE('Fenêtre principal'!B54,"=", 'Fenêtre principal'!D54),IF('Fenêtre principal'!D54&lt;&gt;"",'Fenêtre principal'!D54,""))</f>
-        <v/>
+        <v>window.menu.level6.sublevel2.title=Cargar un análisis</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
@@ -33425,33 +34133,370 @@
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A505" t="str">
-        <f>IF('Erreur balise introductive'!B29&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B29,"=", 'Erreur balise introductive'!D29),IF('Erreur balise introductive'!D29&lt;&gt;"",'Erreur balise introductive'!D29,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B2&lt;&gt;"",CONCATENATE('Commencer analyse'!B2,"=", 'Commencer analyse'!D2),IF('Commencer analyse'!D2&lt;&gt;"",'Commencer analyse'!D2,""))</f>
+        <v>#Mensaje para iniciar un análisis</v>
       </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A506" t="str">
-        <f>IF('Erreur balise introductive'!B30&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B30,"=", 'Erreur balise introductive'!D30),IF('Erreur balise introductive'!D30&lt;&gt;"",'Erreur balise introductive'!D30,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B3&lt;&gt;"",CONCATENATE('Commencer analyse'!B3,"=", 'Commencer analyse'!D3),IF('Commencer analyse'!D3&lt;&gt;"",'Commencer analyse'!D3,""))</f>
+        <v>window.start.analysis.code.title=Análisis</v>
       </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A507" t="str">
-        <f>IF('Erreur balise introductive'!B31&lt;&gt;"",CONCATENATE('Erreur balise introductive'!B31,"=", 'Erreur balise introductive'!D31),IF('Erreur balise introductive'!D31&lt;&gt;"",'Erreur balise introductive'!D31,""))</f>
+        <f>IF('Commencer analyse'!B4&lt;&gt;"",CONCATENATE('Commencer analyse'!B4,"=", 'Commencer analyse'!D4),IF('Commencer analyse'!D4&lt;&gt;"",'Commencer analyse'!D4,""))</f>
+        <v>window.start.analysis.information.panel.title=Informaciónes</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" t="str">
+        <f>IF('Commencer analyse'!B5&lt;&gt;"",CONCATENATE('Commencer analyse'!B5,"=", 'Commencer analyse'!D5),IF('Commencer analyse'!D5&lt;&gt;"",'Commencer analyse'!D5,""))</f>
+        <v>window.start.analysis.information.message.etape1=&lt;HTML&gt;&lt;P&gt;Bienvenido al asistente de análisis lexicométrico.&lt;BR/&gt;Podrás configurar el análisis que quieras realizar.&lt;BR/&gt;Haga clic en siguiente para iniciar el análisis.&lt;BR/&gt;NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" t="str">
+        <f>IF('Commencer analyse'!B6&lt;&gt;"",CONCATENATE('Commencer analyse'!B6,"=", 'Commencer analyse'!D6),IF('Commencer analyse'!D6&lt;&gt;"",'Commencer analyse'!D6,""))</f>
+        <v>window.start.analysis.wizard.panel.title=Asistente de análisis lexicométrico</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" t="str">
+        <f>IF('Commencer analyse'!B7&lt;&gt;"",CONCATENATE('Commencer analyse'!B7,"=", 'Commencer analyse'!D7),IF('Commencer analyse'!D7&lt;&gt;"",'Commencer analyse'!D7,""))</f>
+        <v>window.start.analysis.information.message.etape2=&lt;HTML&gt;&lt;P&gt;Seleccione las opciones de análisis que desea realizar. &lt;BR/&gt; &lt;U&gt;&lt;B&gt;Tokenización :&lt;/U&gt; &lt;/B&gt; Para limpiar texto de elementos que no se van a escanear. &lt;BR/&gt;&lt;U&gt;&lt;B&gt;Lematización :&lt;/U&gt; &lt;/B&gt; Reemplazar el conjunto de variaciones por su lema. &lt;BR/&gt;&lt;U&gt;&lt;B&gt;Frecuencia :&lt;/U&gt; &lt;/B&gt; Análisis de frecuencia de palabras en un texto.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" t="str">
+        <f>IF('Commencer analyse'!B8&lt;&gt;"",CONCATENATE('Commencer analyse'!B8,"=", 'Commencer analyse'!D8),IF('Commencer analyse'!D8&lt;&gt;"",'Commencer analyse'!D8,""))</f>
+        <v>window.start.analysis.option.tokenization=Tokenización</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" t="str">
+        <f>IF('Commencer analyse'!B9&lt;&gt;"",CONCATENATE('Commencer analyse'!B9,"=", 'Commencer analyse'!D9),IF('Commencer analyse'!D9&lt;&gt;"",'Commencer analyse'!D9,""))</f>
+        <v>window.start.analysis.option.lemmatization=Lematización</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" t="str">
+        <f>IF('Commencer analyse'!B10&lt;&gt;"",CONCATENATE('Commencer analyse'!B10,"=", 'Commencer analyse'!D10),IF('Commencer analyse'!D10&lt;&gt;"",'Commencer analyse'!D10,""))</f>
+        <v>window.start.analysis.option.frequency=Frecuencia</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" t="str">
+        <f>IF('Commencer analyse'!B11&lt;&gt;"",CONCATENATE('Commencer analyse'!B11,"=", 'Commencer analyse'!D11),IF('Commencer analyse'!D11&lt;&gt;"",'Commencer analyse'!D11,""))</f>
+        <v>window.start.analysis.option.panel.title=Elección de opciones de análisis</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" t="str">
+        <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE('Commencer analyse'!B12,"=", 'Commencer analyse'!D12),IF('Commencer analyse'!D12&lt;&gt;"",'Commencer analyse'!D12,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" t="str">
+        <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE('Commencer analyse'!B13,"=", 'Commencer analyse'!D13),IF('Commencer analyse'!D13&lt;&gt;"",'Commencer analyse'!D13,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" t="str">
+        <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE('Commencer analyse'!B14,"=", 'Commencer analyse'!D14),IF('Commencer analyse'!D14&lt;&gt;"",'Commencer analyse'!D14,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" t="str">
+        <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE('Commencer analyse'!B15,"=", 'Commencer analyse'!D15),IF('Commencer analyse'!D15&lt;&gt;"",'Commencer analyse'!D15,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" t="str">
+        <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE('Commencer analyse'!B16,"=", 'Commencer analyse'!D16),IF('Commencer analyse'!D16&lt;&gt;"",'Commencer analyse'!D16,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" t="str">
+        <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE('Commencer analyse'!B17,"=", 'Commencer analyse'!D17),IF('Commencer analyse'!D17&lt;&gt;"",'Commencer analyse'!D17,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" t="str">
+        <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE('Commencer analyse'!B18,"=", 'Commencer analyse'!D18),IF('Commencer analyse'!D18&lt;&gt;"",'Commencer analyse'!D18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" t="str">
+        <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE('Commencer analyse'!B19,"=", 'Commencer analyse'!D19),IF('Commencer analyse'!D19&lt;&gt;"",'Commencer analyse'!D19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" t="str">
+        <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE('Commencer analyse'!B20,"=", 'Commencer analyse'!D20),IF('Commencer analyse'!D20&lt;&gt;"",'Commencer analyse'!D20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" t="str">
+        <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE('Commencer analyse'!B21,"=", 'Commencer analyse'!D21),IF('Commencer analyse'!D21&lt;&gt;"",'Commencer analyse'!D21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525" t="str">
+        <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE('Commencer analyse'!B22,"=", 'Commencer analyse'!D22),IF('Commencer analyse'!D22&lt;&gt;"",'Commencer analyse'!D22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526" t="str">
+        <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE('Commencer analyse'!B23,"=", 'Commencer analyse'!D23),IF('Commencer analyse'!D23&lt;&gt;"",'Commencer analyse'!D23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527" t="str">
+        <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE('Commencer analyse'!B24,"=", 'Commencer analyse'!D24),IF('Commencer analyse'!D24&lt;&gt;"",'Commencer analyse'!D24,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A528" t="str">
+        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE('Commencer analyse'!B25,"=", 'Commencer analyse'!D25),IF('Commencer analyse'!D25&lt;&gt;"",'Commencer analyse'!D25,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A529" t="str">
+        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE('Commencer analyse'!B26,"=", 'Commencer analyse'!D26),IF('Commencer analyse'!D26&lt;&gt;"",'Commencer analyse'!D26,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A530" t="str">
+        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE('Commencer analyse'!B27,"=", 'Commencer analyse'!D27),IF('Commencer analyse'!D27&lt;&gt;"",'Commencer analyse'!D27,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A531" t="str">
+        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE('Commencer analyse'!B28,"=", 'Commencer analyse'!D28),IF('Commencer analyse'!D28&lt;&gt;"",'Commencer analyse'!D28,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A532" t="str">
+        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE('Commencer analyse'!B29,"=", 'Commencer analyse'!D29),IF('Commencer analyse'!D29&lt;&gt;"",'Commencer analyse'!D29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A533" t="str">
+        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE('Commencer analyse'!B30,"=", 'Commencer analyse'!D30),IF('Commencer analyse'!D30&lt;&gt;"",'Commencer analyse'!D30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A534" t="str">
+        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE('Commencer analyse'!B31,"=", 'Commencer analyse'!D31),IF('Commencer analyse'!D31&lt;&gt;"",'Commencer analyse'!D31,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A535" t="str">
+        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE('Commencer analyse'!B32,"=", 'Commencer analyse'!D32),IF('Commencer analyse'!D32&lt;&gt;"",'Commencer analyse'!D32,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A536" t="str">
+        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE('Commencer analyse'!B33,"=", 'Commencer analyse'!D33),IF('Commencer analyse'!D33&lt;&gt;"",'Commencer analyse'!D33,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A537" t="str">
+        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE('Commencer analyse'!B34,"=", 'Commencer analyse'!D34),IF('Commencer analyse'!D34&lt;&gt;"",'Commencer analyse'!D34,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A538" t="str">
+        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE('Commencer analyse'!B35,"=", 'Commencer analyse'!D35),IF('Commencer analyse'!D35&lt;&gt;"",'Commencer analyse'!D35,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A539" t="str">
+        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE('Commencer analyse'!B36,"=", 'Commencer analyse'!D36),IF('Commencer analyse'!D36&lt;&gt;"",'Commencer analyse'!D36,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A540" t="str">
+        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE('Commencer analyse'!B37,"=", 'Commencer analyse'!D37),IF('Commencer analyse'!D37&lt;&gt;"",'Commencer analyse'!D37,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A541" t="str">
+        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE('Commencer analyse'!B38,"=", 'Commencer analyse'!D38),IF('Commencer analyse'!D38&lt;&gt;"",'Commencer analyse'!D38,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A542" t="str">
+        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE('Commencer analyse'!B39,"=", 'Commencer analyse'!D39),IF('Commencer analyse'!D39&lt;&gt;"",'Commencer analyse'!D39,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A543" t="str">
+        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE('Commencer analyse'!B40,"=", 'Commencer analyse'!D40),IF('Commencer analyse'!D40&lt;&gt;"",'Commencer analyse'!D40,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A544" t="str">
+        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE('Commencer analyse'!B41,"=", 'Commencer analyse'!D41),IF('Commencer analyse'!D41&lt;&gt;"",'Commencer analyse'!D41,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A545" t="str">
+        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE('Commencer analyse'!B42,"=", 'Commencer analyse'!D42),IF('Commencer analyse'!D42&lt;&gt;"",'Commencer analyse'!D42,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A546" t="str">
+        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE('Commencer analyse'!B43,"=", 'Commencer analyse'!D43),IF('Commencer analyse'!D43&lt;&gt;"",'Commencer analyse'!D43,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A547" t="str">
+        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE('Commencer analyse'!B44,"=", 'Commencer analyse'!D44),IF('Commencer analyse'!D44&lt;&gt;"",'Commencer analyse'!D44,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A548" t="str">
+        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE('Commencer analyse'!B45,"=", 'Commencer analyse'!D45),IF('Commencer analyse'!D45&lt;&gt;"",'Commencer analyse'!D45,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A549" t="str">
+        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE('Commencer analyse'!B46,"=", 'Commencer analyse'!D46),IF('Commencer analyse'!D46&lt;&gt;"",'Commencer analyse'!D46,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A550" t="str">
+        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE('Commencer analyse'!B47,"=", 'Commencer analyse'!D47),IF('Commencer analyse'!D47&lt;&gt;"",'Commencer analyse'!D47,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A551" t="str">
+        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE('Commencer analyse'!B48,"=", 'Commencer analyse'!D48),IF('Commencer analyse'!D48&lt;&gt;"",'Commencer analyse'!D48,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A552" t="str">
+        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE('Commencer analyse'!B49,"=", 'Commencer analyse'!D49),IF('Commencer analyse'!D49&lt;&gt;"",'Commencer analyse'!D49,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A553" t="str">
+        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE('Commencer analyse'!B50,"=", 'Commencer analyse'!D50),IF('Commencer analyse'!D50&lt;&gt;"",'Commencer analyse'!D50,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A554" t="str">
+        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE('Commencer analyse'!B51,"=", 'Commencer analyse'!D51),IF('Commencer analyse'!D51&lt;&gt;"",'Commencer analyse'!D51,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A555" t="str">
+        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE('Commencer analyse'!B52,"=", 'Commencer analyse'!D52),IF('Commencer analyse'!D52&lt;&gt;"",'Commencer analyse'!D52,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A556" t="str">
+        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE('Commencer analyse'!B53,"=", 'Commencer analyse'!D53),IF('Commencer analyse'!D53&lt;&gt;"",'Commencer analyse'!D53,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A557" t="str">
+        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE('Commencer analyse'!B54,"=", 'Commencer analyse'!D54),IF('Commencer analyse'!D54&lt;&gt;"",'Commencer analyse'!D54,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A558" t="str">
+        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE('Commencer analyse'!B55,"=", 'Commencer analyse'!D55),IF('Commencer analyse'!D55&lt;&gt;"",'Commencer analyse'!D55,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A559" t="str">
+        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE('Commencer analyse'!B56,"=", 'Commencer analyse'!D56),IF('Commencer analyse'!D56&lt;&gt;"",'Commencer analyse'!D56,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A560" t="str">
+        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE('Commencer analyse'!B57,"=", 'Commencer analyse'!D57),IF('Commencer analyse'!D57&lt;&gt;"",'Commencer analyse'!D57,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A561" t="str">
+        <f>IF('Commencer analyse'!B58&lt;&gt;"",CONCATENATE('Commencer analyse'!B58,"=", 'Commencer analyse'!D58),IF('Commencer analyse'!D58&lt;&gt;"",'Commencer analyse'!D58,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A562" t="str">
+        <f>IF('Commencer analyse'!B59&lt;&gt;"",CONCATENATE('Commencer analyse'!B59,"=", 'Commencer analyse'!D59),IF('Commencer analyse'!D59&lt;&gt;"",'Commencer analyse'!D59,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A563" t="str">
+        <f>IF('Commencer analyse'!B60&lt;&gt;"",CONCATENATE('Commencer analyse'!B60,"=", 'Commencer analyse'!D60),IF('Commencer analyse'!D60&lt;&gt;"",'Commencer analyse'!D60,""))</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
-  <dimension ref="A1:A501"/>
+  <dimension ref="A1:A559"/>
   <sheetViews>
-    <sheetView topLeftCell="A335" workbookViewId="0">
-      <selection activeCell="A362" sqref="A362:A363"/>
+    <sheetView topLeftCell="A487" workbookViewId="0">
+      <selection activeCell="A506" sqref="A506:A509"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33762,19 +34807,19 @@
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>IF('Fenêtre principal'!B52&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Fenêtre principal'!B52),".","_"),"=""", 'Fenêtre principal'!B52,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_MENU_LEVEL6_TITLE="window.menu.level6.title";</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>IF('Fenêtre principal'!B53&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Fenêtre principal'!B53),".","_"),"=""", 'Fenêtre principal'!B53,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_MENU_LEVEL6_SUBLEVEL1_TITLE="window.menu.level6.sublevel1.title";</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>IF('Fenêtre principal'!B54&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Fenêtre principal'!B54),".","_"),"=""", 'Fenêtre principal'!B54,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_MENU_LEVEL6_SUBLEVEL2_TITLE="window.menu.level6.sublevel2.title";</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
@@ -36461,12 +37506,361 @@
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A501" t="str">
-        <f>IF('Erreur balise introductive'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur balise introductive'!B29),".","_"),"=""", 'Erreur balise introductive'!B29,""";"),"")</f>
+        <f>IF('Commencer analyse'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B2),".","_"),"=""", 'Commencer analyse'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" t="str">
+        <f>IF('Commencer analyse'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B3),".","_"),"=""", 'Commencer analyse'!B3,""";"),"")</f>
+        <v>public static final String WINDOW_START_ANALYSIS_CODE_TITLE="window.start.analysis.code.title";</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" t="str">
+        <f>IF('Commencer analyse'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B4),".","_"),"=""", 'Commencer analyse'!B4,""";"),"")</f>
+        <v>public static final String WINDOW_START_ANALYSIS_INFORMATION_PANEL_TITLE="window.start.analysis.information.panel.title";</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504" t="str">
+        <f>IF('Commencer analyse'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B5),".","_"),"=""", 'Commencer analyse'!B5,""";"),"")</f>
+        <v>public static final String WINDOW_START_ANALYSIS_INFORMATION_MESSAGE_ETAPE1="window.start.analysis.information.message.etape1";</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" t="str">
+        <f>IF('Commencer analyse'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B6),".","_"),"=""", 'Commencer analyse'!B6,""";"),"")</f>
+        <v>public static final String WINDOW_START_ANALYSIS_WIZARD_PANEL_TITLE="window.start.analysis.wizard.panel.title";</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" t="str">
+        <f>IF('Commencer analyse'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B7),".","_"),"=""", 'Commencer analyse'!B7,""";"),"")</f>
+        <v>public static final String WINDOW_START_ANALYSIS_INFORMATION_MESSAGE_ETAPE2="window.start.analysis.information.message.etape2";</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" t="str">
+        <f>IF('Commencer analyse'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B8),".","_"),"=""", 'Commencer analyse'!B8,""";"),"")</f>
+        <v>public static final String WINDOW_START_ANALYSIS_OPTION_TOKENIZATION="window.start.analysis.option.tokenization";</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" t="str">
+        <f>IF('Commencer analyse'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B9),".","_"),"=""", 'Commencer analyse'!B9,""";"),"")</f>
+        <v>public static final String WINDOW_START_ANALYSIS_OPTION_LEMMATIZATION="window.start.analysis.option.lemmatization";</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" t="str">
+        <f>IF('Commencer analyse'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B10),".","_"),"=""", 'Commencer analyse'!B10,""";"),"")</f>
+        <v>public static final String WINDOW_START_ANALYSIS_OPTION_FREQUENCY="window.start.analysis.option.frequency";</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" t="str">
+        <f>IF('Commencer analyse'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B11),".","_"),"=""", 'Commencer analyse'!B11,""";"),"")</f>
+        <v>public static final String WINDOW_START_ANALYSIS_OPTION_PANEL_TITLE="window.start.analysis.option.panel.title";</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" t="str">
+        <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B12),".","_"),"=""", 'Commencer analyse'!B12,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" t="str">
+        <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B13),".","_"),"=""", 'Commencer analyse'!B13,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" t="str">
+        <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B14),".","_"),"=""", 'Commencer analyse'!B14,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" t="str">
+        <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B15),".","_"),"=""", 'Commencer analyse'!B15,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" t="str">
+        <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B16),".","_"),"=""", 'Commencer analyse'!B16,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" t="str">
+        <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B17),".","_"),"=""", 'Commencer analyse'!B17,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" t="str">
+        <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B18),".","_"),"=""", 'Commencer analyse'!B18,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" t="str">
+        <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B19),".","_"),"=""", 'Commencer analyse'!B19,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" t="str">
+        <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B20),".","_"),"=""", 'Commencer analyse'!B20,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" t="str">
+        <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B21),".","_"),"=""", 'Commencer analyse'!B21,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" t="str">
+        <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B22),".","_"),"=""", 'Commencer analyse'!B22,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" t="str">
+        <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B23),".","_"),"=""", 'Commencer analyse'!B23,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" t="str">
+        <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B24),".","_"),"=""", 'Commencer analyse'!B24,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" t="str">
+        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B25),".","_"),"=""", 'Commencer analyse'!B25,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525" t="str">
+        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B26),".","_"),"=""", 'Commencer analyse'!B26,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526" t="str">
+        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B27),".","_"),"=""", 'Commencer analyse'!B27,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527" t="str">
+        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B28),".","_"),"=""", 'Commencer analyse'!B28,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A528" t="str">
+        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B29),".","_"),"=""", 'Commencer analyse'!B29,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A529" t="str">
+        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B30),".","_"),"=""", 'Commencer analyse'!B30,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A530" t="str">
+        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B31),".","_"),"=""", 'Commencer analyse'!B31,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A531" t="str">
+        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B32),".","_"),"=""", 'Commencer analyse'!B32,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A532" t="str">
+        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B33),".","_"),"=""", 'Commencer analyse'!B33,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A533" t="str">
+        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B34),".","_"),"=""", 'Commencer analyse'!B34,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A534" t="str">
+        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B35),".","_"),"=""", 'Commencer analyse'!B35,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A535" t="str">
+        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B36),".","_"),"=""", 'Commencer analyse'!B36,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A536" t="str">
+        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B37),".","_"),"=""", 'Commencer analyse'!B37,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A537" t="str">
+        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B38),".","_"),"=""", 'Commencer analyse'!B38,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A538" t="str">
+        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B39),".","_"),"=""", 'Commencer analyse'!B39,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A539" t="str">
+        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B40),".","_"),"=""", 'Commencer analyse'!B40,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A540" t="str">
+        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B41),".","_"),"=""", 'Commencer analyse'!B41,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A541" t="str">
+        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B42),".","_"),"=""", 'Commencer analyse'!B42,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A542" t="str">
+        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B43),".","_"),"=""", 'Commencer analyse'!B43,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A543" t="str">
+        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B44),".","_"),"=""", 'Commencer analyse'!B44,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A544" t="str">
+        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B45),".","_"),"=""", 'Commencer analyse'!B45,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A545" t="str">
+        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B46),".","_"),"=""", 'Commencer analyse'!B46,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A546" t="str">
+        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B47),".","_"),"=""", 'Commencer analyse'!B47,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A547" t="str">
+        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B48),".","_"),"=""", 'Commencer analyse'!B48,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A548" t="str">
+        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B49),".","_"),"=""", 'Commencer analyse'!B49,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A549" t="str">
+        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B50),".","_"),"=""", 'Commencer analyse'!B50,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A550" t="str">
+        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B51),".","_"),"=""", 'Commencer analyse'!B51,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A551" t="str">
+        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B52),".","_"),"=""", 'Commencer analyse'!B52,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A552" t="str">
+        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B53),".","_"),"=""", 'Commencer analyse'!B53,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A553" t="str">
+        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B54),".","_"),"=""", 'Commencer analyse'!B54,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A554" t="str">
+        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B55),".","_"),"=""", 'Commencer analyse'!B55,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A555" t="str">
+        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B56),".","_"),"=""", 'Commencer analyse'!B56,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A556" t="str">
+        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B57),".","_"),"=""", 'Commencer analyse'!B57,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A557" t="str">
+        <f>IF('Commencer analyse'!B58&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B58),".","_"),"=""", 'Commencer analyse'!B58,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A558" t="str">
+        <f>IF('Commencer analyse'!B59&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B59),".","_"),"=""", 'Commencer analyse'!B59,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A559" t="str">
+        <f>IF('Commencer analyse'!B60&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B60),".","_"),"=""", 'Commencer analyse'!B60,""";"),"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -36474,7 +37868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56DE331-9367-41C8-8048-603F1BE40CC9}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19:D22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Avancement sur l'analyse avec prise en charge de l'édition des liste pour la lemmatisation et la tokenization
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\IdeaProjects\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFDA61D-AEC2-40DE-B2E6-DFE7F1039CAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB8B5AF-05B6-4089-B850-E3C34F4EEE70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="17" activeTab="20" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="17" activeTab="18" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="929">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -2384,9 +2384,6 @@
     <t>window.start.analysis.option.frequency</t>
   </si>
   <si>
-    <t>Tokenisation</t>
-  </si>
-  <si>
     <t>Lemmatisation</t>
   </si>
   <si>
@@ -2727,6 +2724,117 @@
   </si>
   <si>
     <t xml:space="preserve">El archivo de Excel proporcionado no es compatible con la configuración específica solicitada </t>
+  </si>
+  <si>
+    <t>window.functional.error.invalid.analysis.folder</t>
+  </si>
+  <si>
+    <t>Le dossier à analyser n'est pas valide (chemin inexistant)</t>
+  </si>
+  <si>
+    <t>La carpeta a analizar no es válida (la ruta no existe)</t>
+  </si>
+  <si>
+    <t>window.start.analysis.token.panel.title</t>
+  </si>
+  <si>
+    <t>Filtre</t>
+  </si>
+  <si>
+    <t>window.start.analysis.information.message.token</t>
+  </si>
+  <si>
+    <t>window.start.analysis.edit.filter.label</t>
+  </si>
+  <si>
+    <t>window.start.analysis.edit.profile.label</t>
+  </si>
+  <si>
+    <t>window.start.analysis.edit.profile.new.button.label</t>
+  </si>
+  <si>
+    <t>window.start.analysis.edit.filter.add.button.label</t>
+  </si>
+  <si>
+    <t>window.start.analysis.edit.filter.remove.button.label</t>
+  </si>
+  <si>
+    <t>window.start.analysis.token.table.header.label</t>
+  </si>
+  <si>
+    <t>window.start.analysis.token.add.information.message</t>
+  </si>
+  <si>
+    <t>window.operation.validate</t>
+  </si>
+  <si>
+    <t>Valider</t>
+  </si>
+  <si>
+    <t>Validar</t>
+  </si>
+  <si>
+    <t>window.start.analysis.token.add.text.label</t>
+  </si>
+  <si>
+    <t>window.information.answer.user.panel.title</t>
+  </si>
+  <si>
+    <t>Réponse</t>
+  </si>
+  <si>
+    <t>Respuesta</t>
+  </si>
+  <si>
+    <t>window.information.question.user.panel.title</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Pregunta</t>
+  </si>
+  <si>
+    <t>Nouveau StopWord</t>
+  </si>
+  <si>
+    <t>StopWord</t>
+  </si>
+  <si>
+    <t>Gestion des StopWords</t>
+  </si>
+  <si>
+    <t>Liste</t>
+  </si>
+  <si>
+    <t>Nouvelle liste</t>
+  </si>
+  <si>
+    <t>window.start.analysis.token.table.panel.title</t>
+  </si>
+  <si>
+    <t>Gestion des données StopWords</t>
+  </si>
+  <si>
+    <t>window.start.analysis.edit.profile.remove.button.label</t>
+  </si>
+  <si>
+    <t>window.start.analysis.edit.profile.save.button.label</t>
+  </si>
+  <si>
+    <t>Sauvegarder la liste</t>
+  </si>
+  <si>
+    <t>Supprimer la liste</t>
+  </si>
+  <si>
+    <t>window.start.analysis.edit.profile.remove.button.confirmation.message</t>
+  </si>
+  <si>
+    <t>window.start.analysis.edit.profile.new.button.copy.or.new.message</t>
+  </si>
+  <si>
+    <t>window.start.analysis.edit.profile.new.button.new.name.message</t>
   </si>
 </sst>
 </file>
@@ -24037,8 +24145,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{028E31B7-3FC3-4143-B5FF-43FD17AAB26D}" name="Tableau16" displayName="Tableau16" ref="A1:D52" totalsRowShown="0">
-  <autoFilter ref="A1:D52" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{028E31B7-3FC3-4143-B5FF-43FD17AAB26D}" name="Tableau16" displayName="Tableau16" ref="A1:D53" totalsRowShown="0">
+  <autoFilter ref="A1:D53" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{EE0F9B50-F787-4253-A164-BB17836F12B4}" name="Numero"/>
     <tableColumn id="2" xr3:uid="{58CBB508-E960-4269-90E7-903193963B86}" name="Code"/>
@@ -24154,8 +24262,8 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{2AFE4382-896C-46EC-B1F3-BDE0F359B30F}" name="Tableau152122" displayName="Tableau152122" ref="A1:D20" totalsRowShown="0">
-  <autoFilter ref="A1:D20" xr:uid="{1C0F8CDE-76C5-4629-A51B-1F75FFD867D6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{2AFE4382-896C-46EC-B1F3-BDE0F359B30F}" name="Tableau152122" displayName="Tableau152122" ref="A1:D19" totalsRowShown="0">
+  <autoFilter ref="A1:D19" xr:uid="{1C0F8CDE-76C5-4629-A51B-1F75FFD867D6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C133F70E-E4F0-479A-B56B-1FD60660F6B4}" name="Numero"/>
     <tableColumn id="2" xr3:uid="{CD5F6150-2167-4652-B8D9-683106F96182}" name="Code"/>
@@ -24647,10 +24755,10 @@
         <v>355</v>
       </c>
       <c r="C9" t="s">
+        <v>842</v>
+      </c>
+      <c r="D9" t="s">
         <v>843</v>
-      </c>
-      <c r="D9" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -25269,13 +25377,13 @@
         <v>47</v>
       </c>
       <c r="B55" t="s">
+        <v>844</v>
+      </c>
+      <c r="C55" t="s">
         <v>845</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>846</v>
-      </c>
-      <c r="D55" t="s">
-        <v>847</v>
       </c>
     </row>
   </sheetData>
@@ -25754,10 +25862,10 @@
         <v>282</v>
       </c>
       <c r="C21" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D21" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -25765,13 +25873,13 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C23" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D23" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -25779,13 +25887,13 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D24" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
   </sheetData>
@@ -26028,10 +26136,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B861A8A-1131-4099-83D4-ECA745EBF0ED}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26399,10 +26507,10 @@
         <v>743</v>
       </c>
       <c r="C36" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D36" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -26413,10 +26521,10 @@
         <v>744</v>
       </c>
       <c r="C37" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="D37" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -26424,13 +26532,13 @@
         <v>22</v>
       </c>
       <c r="B38" t="s">
+        <v>833</v>
+      </c>
+      <c r="C38" t="s">
         <v>834</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>835</v>
-      </c>
-      <c r="D38" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -26474,13 +26582,13 @@
         <v>25</v>
       </c>
       <c r="B43" t="s">
+        <v>810</v>
+      </c>
+      <c r="C43" t="s">
         <v>811</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>812</v>
-      </c>
-      <c r="D43" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -26488,13 +26596,13 @@
         <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C44" t="s">
+        <v>850</v>
+      </c>
+      <c r="D44" t="s">
         <v>851</v>
-      </c>
-      <c r="D44" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -26502,13 +26610,13 @@
         <v>27</v>
       </c>
       <c r="B45" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C45" t="s">
         <v>283</v>
       </c>
       <c r="D45" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -26516,13 +26624,13 @@
         <v>28</v>
       </c>
       <c r="B46" t="s">
+        <v>852</v>
+      </c>
+      <c r="C46" t="s">
         <v>853</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>854</v>
-      </c>
-      <c r="D46" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -26530,13 +26638,13 @@
         <v>29</v>
       </c>
       <c r="B47" t="s">
+        <v>855</v>
+      </c>
+      <c r="C47" t="s">
         <v>856</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>857</v>
-      </c>
-      <c r="D47" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -26544,13 +26652,13 @@
         <v>30</v>
       </c>
       <c r="B48" t="s">
+        <v>858</v>
+      </c>
+      <c r="C48" t="s">
         <v>859</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>860</v>
-      </c>
-      <c r="D48" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -26558,13 +26666,13 @@
         <v>31</v>
       </c>
       <c r="B49" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C49" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D49" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -26572,13 +26680,55 @@
         <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C50" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D50" t="s">
-        <v>867</v>
+        <v>866</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>33</v>
+      </c>
+      <c r="B51" t="s">
+        <v>905</v>
+      </c>
+      <c r="C51" t="s">
+        <v>906</v>
+      </c>
+      <c r="D51" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>34</v>
+      </c>
+      <c r="B52" t="s">
+        <v>909</v>
+      </c>
+      <c r="C52" t="s">
+        <v>910</v>
+      </c>
+      <c r="D52" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>35</v>
+      </c>
+      <c r="B53" t="s">
+        <v>912</v>
+      </c>
+      <c r="C53" t="s">
+        <v>913</v>
+      </c>
+      <c r="D53" t="s">
+        <v>914</v>
       </c>
     </row>
   </sheetData>
@@ -26770,7 +26920,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27541,10 +27691,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757EF7E0-E814-48B2-A4AF-487C809E6C10}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27645,10 +27795,10 @@
       </c>
       <c r="C7" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Sélectionnez les options d'analyse que vous souhaitez effectuer.&lt;BR/&gt;",
-"Tokenisation : Pour nettoyer le texte des éléments qui ne sont pas à analyser.&lt;BR/&gt;",
+"StopWord : Pour nettoyer le texte des éléments qui ne sont pas à analyser.&lt;BR/&gt;",
 "Lemmatisation : Pour remplacer l'ensemble des variations par son lemme.&lt;BR/&gt;",
 "Fréquence : Analyse par fréquence des mots d'un texte.&lt;/P&gt;&lt;/HTML&gt;")</f>
-        <v>&lt;HTML&gt;&lt;P&gt;Sélectionnez les options d'analyse que vous souhaitez effectuer.&lt;BR/&gt;Tokenisation : Pour nettoyer le texte des éléments qui ne sont pas à analyser.&lt;BR/&gt;Lemmatisation : Pour remplacer l'ensemble des variations par son lemme.&lt;BR/&gt;Fréquence : Analyse par fréquence des mots d'un texte.&lt;/P&gt;&lt;/HTML&gt;</v>
+        <v>&lt;HTML&gt;&lt;P&gt;Sélectionnez les options d'analyse que vous souhaitez effectuer.&lt;BR/&gt;StopWord : Pour nettoyer le texte des éléments qui ne sont pas à analyser.&lt;BR/&gt;Lemmatisation : Pour remplacer l'ensemble des variations par son lemme.&lt;BR/&gt;Fréquence : Analyse par fréquence des mots d'un texte.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
       <c r="D7" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Seleccione las opciones de análisis que desea realizar. &lt;BR/&gt; ",
@@ -27666,10 +27816,10 @@
         <v>775</v>
       </c>
       <c r="C8" t="s">
-        <v>778</v>
+        <v>916</v>
       </c>
       <c r="D8" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -27680,10 +27830,10 @@
         <v>776</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -27694,10 +27844,10 @@
         <v>777</v>
       </c>
       <c r="C10" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D10" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -27705,37 +27855,205 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
+        <v>783</v>
+      </c>
+      <c r="C11" t="s">
         <v>784</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>785</v>
       </c>
-      <c r="D11" t="s">
-        <v>786</v>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>895</v>
+      </c>
+      <c r="C12" t="s">
+        <v>917</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="1"/>
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>898</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>896</v>
+      </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
+    <row r="14" spans="1:4" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>897</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Dans cette étape vous pouvez gérer les StopWord à nettoyer&lt;BR/&gt;",
+"Vous pouvez gérer différentes liste avec le menu déroulant prévus à cet effet.&lt;BR/&gt;",
+"Vous pouvez filtrer/éditer la liste des StopWord.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Dans cette étape vous pouvez gérer les StopWord à nettoyer&lt;BR/&gt;Vous pouvez gérer différentes liste avec le menu déroulant prévus à cet effet.&lt;BR/&gt;Vous pouvez filtrer/éditer la liste des StopWord.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="1"/>
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>899</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>918</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>900</v>
+      </c>
+      <c r="C16" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>901</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>902</v>
+      </c>
+      <c r="C18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>903</v>
+      </c>
+      <c r="C19" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>904</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quelle est le nouveau StopWord à ajouter ?&lt;BR/&gt;",
+"&lt;I&gt;NB : La liste des StopWord ne peut pas contenir de doublon, si le token existe déjà, l'ajout n'aura aucun effet.&lt;/I&gt;&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Quelle est le nouveau StopWord à ajouter ?&lt;BR/&gt;&lt;I&gt;NB : La liste des StopWord ne peut pas contenir de doublon, si le token existe déjà, l'ajout n'aura aucun effet.&lt;/I&gt;&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>908</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>915</v>
+      </c>
       <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>920</v>
+      </c>
+      <c r="C22" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>922</v>
+      </c>
+      <c r="C23" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>923</v>
+      </c>
+      <c r="C24" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>926</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;La suppression de la liste est définitive et ne peut pas être annulé.&lt;BR/&gt;",
+"Confirmer que vous désirez réellement supprimer la liste en cliquant sur Oui.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;La suppression de la liste est définitive et ne peut pas être annulé.&lt;BR/&gt;Confirmer que vous désirez réellement supprimer la liste en cliquant sur Oui.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>927</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Voulez vous créer une copie de la liste en cours ?&lt;BR/&gt;",
+"Cliquez sur Oui pour créer une copie de la liste, ou sur Non pour créer une liste vierge&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Voulez vous créer une copie de la liste en cours ?&lt;BR/&gt;Cliquez sur Oui pour créer une copie de la liste, ou sur Non pour créer une liste vierge&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>928</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quelle est le nom de la nouvelle liste ?&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Quelle est le nom de la nouvelle liste ?&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28219,10 +28537,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2" t="s">
         <v>797</v>
-      </c>
-      <c r="D2" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -28230,13 +28548,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C3" t="s">
+        <v>798</v>
+      </c>
+      <c r="D3" t="s">
         <v>799</v>
-      </c>
-      <c r="D3" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -28244,13 +28562,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C4" t="s">
+        <v>800</v>
+      </c>
+      <c r="D4" t="s">
         <v>801</v>
-      </c>
-      <c r="D4" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -28258,13 +28576,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C5" t="s">
+        <v>802</v>
+      </c>
+      <c r="D5" t="s">
         <v>803</v>
-      </c>
-      <c r="D5" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -28272,13 +28590,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -28286,7 +28604,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Le fichier suivant va être importé : &lt;br/&gt;&lt;br/&gt;%s&lt;/p&gt;&lt;/html&gt;"</f>
@@ -28302,13 +28620,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C8" t="s">
+        <v>806</v>
+      </c>
+      <c r="D8" t="s">
         <v>807</v>
-      </c>
-      <c r="D8" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -28316,7 +28634,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C9" t="s">
         <v>297</v>
@@ -28330,7 +28648,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C10" t="s">
         <v>299</v>
@@ -28344,13 +28662,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>836</v>
+      </c>
+      <c r="C11" t="s">
         <v>837</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>838</v>
-      </c>
-      <c r="D11" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -28358,7 +28676,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C12" t="s">
         <v>301</v>
@@ -28372,13 +28690,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C13" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D13" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -28386,7 +28704,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C14" t="s">
         <v>305</v>
@@ -28400,7 +28718,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C15" t="s">
         <v>307</v>
@@ -28414,7 +28732,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C16" t="s">
         <v>309</v>
@@ -28428,13 +28746,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C17" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D17" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -28442,13 +28760,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C18" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D18" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -28456,13 +28774,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>839</v>
+      </c>
+      <c r="C19" t="s">
         <v>840</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>841</v>
-      </c>
-      <c r="D19" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -28479,10 +28797,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD31F70A-F934-4E15-ACEB-A430E2D8A684}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28511,13 +28829,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>868</v>
+      </c>
+      <c r="C3" t="s">
         <v>869</v>
       </c>
-      <c r="C3" t="s">
-        <v>870</v>
-      </c>
       <c r="D3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -28525,7 +28843,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C4" t="str">
         <f>"&lt;html&gt;&lt;p&gt;Les erreurs suivantes ont été rencontrés : &lt;ul&gt;%s&lt;/ul&gt;&lt;/p&gt;&lt;/html&gt;"</f>
@@ -28541,13 +28859,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="C5" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D5" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -28555,13 +28873,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>872</v>
+      </c>
+      <c r="C6" t="s">
         <v>873</v>
       </c>
-      <c r="C6" t="s">
-        <v>874</v>
-      </c>
       <c r="D6" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -28569,13 +28887,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>877</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>879</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -28583,13 +28901,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>881</v>
+      </c>
+      <c r="C8" t="s">
+        <v>880</v>
+      </c>
+      <c r="D8" t="s">
         <v>882</v>
-      </c>
-      <c r="C8" t="s">
-        <v>881</v>
-      </c>
-      <c r="D8" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -28597,13 +28915,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>883</v>
+      </c>
+      <c r="C9" t="s">
         <v>884</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>885</v>
-      </c>
-      <c r="D9" t="s">
-        <v>886</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -28611,13 +28929,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>886</v>
+      </c>
+      <c r="C10" t="s">
         <v>887</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>888</v>
-      </c>
-      <c r="D10" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -28625,18 +28943,32 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>889</v>
+      </c>
+      <c r="C11" t="s">
         <v>890</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>891</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>892</v>
       </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="C12" t="s">
+        <v>893</v>
+      </c>
+      <c r="D12" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28648,10 +28980,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904B2FA-CBC2-495A-A197-D0CDD47EB1AE}">
-  <dimension ref="A1:A678"/>
+  <dimension ref="A1:A677"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A598" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A618" sqref="A1:A678"/>
+    <sheetView showZeros="0" topLeftCell="A511" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A528" sqref="A1:A677"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30900,19 +31232,19 @@
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" t="str">
         <f>IF(Autres!B51&lt;&gt;"",CONCATENATE(Autres!B51,"=", Autres!C51),IF(Autres!C51&lt;&gt;"",Autres!C51,""))</f>
-        <v/>
+        <v>window.operation.validate=Valider</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" t="str">
         <f>IF(Autres!B52&lt;&gt;"",CONCATENATE(Autres!B52,"=", Autres!C52),IF(Autres!C52&lt;&gt;"",Autres!C52,""))</f>
-        <v/>
+        <v>window.information.answer.user.panel.title=Réponse</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" t="str">
         <f>IF(Autres!B53&lt;&gt;"",CONCATENATE(Autres!B53,"=", Autres!C53),IF(Autres!C53&lt;&gt;"",Autres!C53,""))</f>
-        <v/>
+        <v>window.information.question.user.panel.title=Question</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
@@ -31794,13 +32126,13 @@
     <row r="523" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A523" t="str">
         <f>IF('Commencer analyse'!B7&lt;&gt;"",CONCATENATE('Commencer analyse'!B7,"=", 'Commencer analyse'!C7),IF('Commencer analyse'!C7&lt;&gt;"",'Commencer analyse'!C7,""))</f>
-        <v>window.start.analysis.information.message.etape2=&lt;HTML&gt;&lt;P&gt;Sélectionnez les options d'analyse que vous souhaitez effectuer.&lt;BR/&gt;Tokenisation : Pour nettoyer le texte des éléments qui ne sont pas à analyser.&lt;BR/&gt;Lemmatisation : Pour remplacer l'ensemble des variations par son lemme.&lt;BR/&gt;Fréquence : Analyse par fréquence des mots d'un texte.&lt;/P&gt;&lt;/HTML&gt;</v>
+        <v>window.start.analysis.information.message.etape2=&lt;HTML&gt;&lt;P&gt;Sélectionnez les options d'analyse que vous souhaitez effectuer.&lt;BR/&gt;StopWord : Pour nettoyer le texte des éléments qui ne sont pas à analyser.&lt;BR/&gt;Lemmatisation : Pour remplacer l'ensemble des variations par son lemme.&lt;BR/&gt;Fréquence : Analyse par fréquence des mots d'un texte.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A524" t="str">
         <f>IF('Commencer analyse'!B8&lt;&gt;"",CONCATENATE('Commencer analyse'!B8,"=", 'Commencer analyse'!C8),IF('Commencer analyse'!C8&lt;&gt;"",'Commencer analyse'!C8,""))</f>
-        <v>window.start.analysis.option.tokenization=Tokenisation</v>
+        <v>window.start.analysis.option.tokenization=StopWord</v>
       </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.25">
@@ -31824,97 +32156,97 @@
     <row r="528" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A528" t="str">
         <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE('Commencer analyse'!B12,"=", 'Commencer analyse'!C12),IF('Commencer analyse'!C12&lt;&gt;"",'Commencer analyse'!C12,""))</f>
-        <v/>
+        <v>window.start.analysis.token.panel.title=Gestion des StopWords</v>
       </c>
     </row>
     <row r="529" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A529" t="str">
         <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE('Commencer analyse'!B13,"=", 'Commencer analyse'!C13),IF('Commencer analyse'!C13&lt;&gt;"",'Commencer analyse'!C13,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.filter.label=Filtre</v>
       </c>
     </row>
     <row r="530" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A530" t="str">
         <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE('Commencer analyse'!B14,"=", 'Commencer analyse'!C14),IF('Commencer analyse'!C14&lt;&gt;"",'Commencer analyse'!C14,""))</f>
-        <v/>
+        <v>window.start.analysis.information.message.token=&lt;HTML&gt;&lt;P&gt;Dans cette étape vous pouvez gérer les StopWord à nettoyer&lt;BR/&gt;Vous pouvez gérer différentes liste avec le menu déroulant prévus à cet effet.&lt;BR/&gt;Vous pouvez filtrer/éditer la liste des StopWord.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="531" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A531" t="str">
         <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE('Commencer analyse'!B15,"=", 'Commencer analyse'!C15),IF('Commencer analyse'!C15&lt;&gt;"",'Commencer analyse'!C15,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.profile.label=Liste</v>
       </c>
     </row>
     <row r="532" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A532" t="str">
         <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE('Commencer analyse'!B16,"=", 'Commencer analyse'!C16),IF('Commencer analyse'!C16&lt;&gt;"",'Commencer analyse'!C16,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.profile.new.button.label=Nouvelle liste</v>
       </c>
     </row>
     <row r="533" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A533" t="str">
         <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE('Commencer analyse'!B17,"=", 'Commencer analyse'!C17),IF('Commencer analyse'!C17&lt;&gt;"",'Commencer analyse'!C17,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.filter.add.button.label=Ajouter</v>
       </c>
     </row>
     <row r="534" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A534" t="str">
         <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE('Commencer analyse'!B18,"=", 'Commencer analyse'!C18),IF('Commencer analyse'!C18&lt;&gt;"",'Commencer analyse'!C18,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.filter.remove.button.label=Supprimer</v>
       </c>
     </row>
     <row r="535" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A535" t="str">
         <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE('Commencer analyse'!B19,"=", 'Commencer analyse'!C19),IF('Commencer analyse'!C19&lt;&gt;"",'Commencer analyse'!C19,""))</f>
-        <v/>
+        <v>window.start.analysis.token.table.header.label=StopWord</v>
       </c>
     </row>
     <row r="536" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A536" t="str">
         <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE('Commencer analyse'!B20,"=", 'Commencer analyse'!C20),IF('Commencer analyse'!C20&lt;&gt;"",'Commencer analyse'!C20,""))</f>
-        <v/>
+        <v>window.start.analysis.token.add.information.message=&lt;HTML&gt;&lt;P&gt;Quelle est le nouveau StopWord à ajouter ?&lt;BR/&gt;&lt;I&gt;NB : La liste des StopWord ne peut pas contenir de doublon, si le token existe déjà, l'ajout n'aura aucun effet.&lt;/I&gt;&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="537" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A537" t="str">
         <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE('Commencer analyse'!B21,"=", 'Commencer analyse'!C21),IF('Commencer analyse'!C21&lt;&gt;"",'Commencer analyse'!C21,""))</f>
-        <v/>
+        <v>window.start.analysis.token.add.text.label=Nouveau StopWord</v>
       </c>
     </row>
     <row r="538" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A538" t="str">
         <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE('Commencer analyse'!B22,"=", 'Commencer analyse'!C22),IF('Commencer analyse'!C22&lt;&gt;"",'Commencer analyse'!C22,""))</f>
-        <v/>
+        <v>window.start.analysis.token.table.panel.title=Gestion des données StopWords</v>
       </c>
     </row>
     <row r="539" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A539" t="str">
         <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE('Commencer analyse'!B23,"=", 'Commencer analyse'!C23),IF('Commencer analyse'!C23&lt;&gt;"",'Commencer analyse'!C23,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.profile.remove.button.label=Supprimer la liste</v>
       </c>
     </row>
     <row r="540" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A540" t="str">
         <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE('Commencer analyse'!B24,"=", 'Commencer analyse'!C24),IF('Commencer analyse'!C24&lt;&gt;"",'Commencer analyse'!C24,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.profile.save.button.label=Sauvegarder la liste</v>
       </c>
     </row>
     <row r="541" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A541" t="str">
         <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE('Commencer analyse'!B25,"=", 'Commencer analyse'!C25),IF('Commencer analyse'!C25&lt;&gt;"",'Commencer analyse'!C25,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.profile.remove.button.confirmation.message=&lt;HTML&gt;&lt;P&gt;La suppression de la liste est définitive et ne peut pas être annulé.&lt;BR/&gt;Confirmer que vous désirez réellement supprimer la liste en cliquant sur Oui.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="542" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A542" t="str">
         <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE('Commencer analyse'!B26,"=", 'Commencer analyse'!C26),IF('Commencer analyse'!C26&lt;&gt;"",'Commencer analyse'!C26,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.profile.new.button.copy.or.new.message=&lt;HTML&gt;&lt;P&gt;Voulez vous créer une copie de la liste en cours ?&lt;BR/&gt;Cliquez sur Oui pour créer une copie de la liste, ou sur Non pour créer une liste vierge&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="543" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A543" t="str">
         <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE('Commencer analyse'!B27,"=", 'Commencer analyse'!C27),IF('Commencer analyse'!C27&lt;&gt;"",'Commencer analyse'!C27,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.profile.new.button.new.name.message=&lt;HTML&gt;&lt;P&gt;Quelle est le nom de la nouvelle liste ?&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="544" spans="1:1" x14ac:dyDescent="0.25">
@@ -32364,7 +32696,7 @@
     <row r="618" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A618" t="str">
         <f>IF('Erreur Fonctionnelle'!B12&lt;&gt;"",CONCATENATE('Erreur Fonctionnelle'!B12,"=", 'Erreur Fonctionnelle'!C12),IF('Erreur Fonctionnelle'!C12&lt;&gt;"",'Erreur Fonctionnelle'!C12,""))</f>
-        <v/>
+        <v>window.functional.error.invalid.analysis.folder=Le dossier à analyser n'est pas valide (chemin inexistant)</v>
       </c>
     </row>
     <row r="619" spans="1:1" x14ac:dyDescent="0.25">
@@ -32718,12 +33050,6 @@
     <row r="677" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A677" t="str">
         <f>IF('Erreur Fonctionnelle'!B71&lt;&gt;"",CONCATENATE('Erreur Fonctionnelle'!B71,"=", 'Erreur Fonctionnelle'!C71),IF('Erreur Fonctionnelle'!C71&lt;&gt;"",'Erreur Fonctionnelle'!C71,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="678" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A678" t="str">
-        <f>IF('Erreur Fonctionnelle'!B72&lt;&gt;"",CONCATENATE('Erreur Fonctionnelle'!B72,"=", 'Erreur Fonctionnelle'!C72),IF('Erreur Fonctionnelle'!C72&lt;&gt;"",'Erreur Fonctionnelle'!C72,""))</f>
         <v/>
       </c>
     </row>
@@ -32735,10 +33061,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
-  <dimension ref="A1:A677"/>
+  <dimension ref="A1:A676"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A677"/>
+    <sheetView showZeros="0" topLeftCell="A592" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A618" sqref="A618:XFD618"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34987,19 +35313,19 @@
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" t="str">
         <f>IF(Autres!B51&lt;&gt;"",CONCATENATE(Autres!B51,"=", Autres!D51),IF(Autres!D51&lt;&gt;"",Autres!D51,""))</f>
-        <v/>
+        <v>window.operation.validate=Validar</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" t="str">
         <f>IF(Autres!B52&lt;&gt;"",CONCATENATE(Autres!B52,"=", Autres!D52),IF(Autres!D52&lt;&gt;"",Autres!D52,""))</f>
-        <v/>
+        <v>window.information.answer.user.panel.title=Respuesta</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" t="str">
         <f>IF(Autres!B53&lt;&gt;"",CONCATENATE(Autres!B53,"=", Autres!D53),IF(Autres!D53&lt;&gt;"",Autres!D53,""))</f>
-        <v/>
+        <v>window.information.question.user.panel.title=Pregunta</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
@@ -35905,97 +36231,97 @@
     <row r="527" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A527" t="str">
         <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE('Commencer analyse'!B12,"=", 'Commencer analyse'!D12),IF('Commencer analyse'!D12&lt;&gt;"",'Commencer analyse'!D12,""))</f>
-        <v/>
+        <v>window.start.analysis.token.panel.title=</v>
       </c>
     </row>
     <row r="528" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A528" t="str">
         <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE('Commencer analyse'!B13,"=", 'Commencer analyse'!D13),IF('Commencer analyse'!D13&lt;&gt;"",'Commencer analyse'!D13,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.filter.label=</v>
       </c>
     </row>
     <row r="529" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A529" t="str">
         <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE('Commencer analyse'!B14,"=", 'Commencer analyse'!D14),IF('Commencer analyse'!D14&lt;&gt;"",'Commencer analyse'!D14,""))</f>
-        <v/>
+        <v>window.start.analysis.information.message.token=</v>
       </c>
     </row>
     <row r="530" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A530" t="str">
         <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE('Commencer analyse'!B15,"=", 'Commencer analyse'!D15),IF('Commencer analyse'!D15&lt;&gt;"",'Commencer analyse'!D15,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.profile.label=</v>
       </c>
     </row>
     <row r="531" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A531" t="str">
         <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE('Commencer analyse'!B16,"=", 'Commencer analyse'!D16),IF('Commencer analyse'!D16&lt;&gt;"",'Commencer analyse'!D16,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.profile.new.button.label=</v>
       </c>
     </row>
     <row r="532" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A532" t="str">
         <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE('Commencer analyse'!B17,"=", 'Commencer analyse'!D17),IF('Commencer analyse'!D17&lt;&gt;"",'Commencer analyse'!D17,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.filter.add.button.label=</v>
       </c>
     </row>
     <row r="533" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A533" t="str">
         <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE('Commencer analyse'!B18,"=", 'Commencer analyse'!D18),IF('Commencer analyse'!D18&lt;&gt;"",'Commencer analyse'!D18,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.filter.remove.button.label=</v>
       </c>
     </row>
     <row r="534" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A534" t="str">
         <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE('Commencer analyse'!B19,"=", 'Commencer analyse'!D19),IF('Commencer analyse'!D19&lt;&gt;"",'Commencer analyse'!D19,""))</f>
-        <v/>
+        <v>window.start.analysis.token.table.header.label=</v>
       </c>
     </row>
     <row r="535" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A535" t="str">
         <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE('Commencer analyse'!B20,"=", 'Commencer analyse'!D20),IF('Commencer analyse'!D20&lt;&gt;"",'Commencer analyse'!D20,""))</f>
-        <v/>
+        <v>window.start.analysis.token.add.information.message=</v>
       </c>
     </row>
     <row r="536" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A536" t="str">
         <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE('Commencer analyse'!B21,"=", 'Commencer analyse'!D21),IF('Commencer analyse'!D21&lt;&gt;"",'Commencer analyse'!D21,""))</f>
-        <v/>
+        <v>window.start.analysis.token.add.text.label=</v>
       </c>
     </row>
     <row r="537" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A537" t="str">
         <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE('Commencer analyse'!B22,"=", 'Commencer analyse'!D22),IF('Commencer analyse'!D22&lt;&gt;"",'Commencer analyse'!D22,""))</f>
-        <v/>
+        <v>window.start.analysis.token.table.panel.title=</v>
       </c>
     </row>
     <row r="538" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A538" t="str">
         <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE('Commencer analyse'!B23,"=", 'Commencer analyse'!D23),IF('Commencer analyse'!D23&lt;&gt;"",'Commencer analyse'!D23,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.profile.remove.button.label=</v>
       </c>
     </row>
     <row r="539" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A539" t="str">
         <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE('Commencer analyse'!B24,"=", 'Commencer analyse'!D24),IF('Commencer analyse'!D24&lt;&gt;"",'Commencer analyse'!D24,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.profile.save.button.label=</v>
       </c>
     </row>
     <row r="540" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A540" t="str">
         <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE('Commencer analyse'!B25,"=", 'Commencer analyse'!D25),IF('Commencer analyse'!D25&lt;&gt;"",'Commencer analyse'!D25,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.profile.remove.button.confirmation.message=</v>
       </c>
     </row>
     <row r="541" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A541" t="str">
         <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE('Commencer analyse'!B26,"=", 'Commencer analyse'!D26),IF('Commencer analyse'!D26&lt;&gt;"",'Commencer analyse'!D26,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.profile.new.button.copy.or.new.message=</v>
       </c>
     </row>
     <row r="542" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A542" t="str">
         <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE('Commencer analyse'!B27,"=", 'Commencer analyse'!D27),IF('Commencer analyse'!D27&lt;&gt;"",'Commencer analyse'!D27,""))</f>
-        <v/>
+        <v>window.start.analysis.edit.profile.new.button.new.name.message=</v>
       </c>
     </row>
     <row r="543" spans="1:1" x14ac:dyDescent="0.25">
@@ -36451,7 +36777,7 @@
     <row r="618" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A618" t="str">
         <f>IF('Erreur Fonctionnelle'!B12&lt;&gt;"",CONCATENATE('Erreur Fonctionnelle'!B12,"=", 'Erreur Fonctionnelle'!D12),IF('Erreur Fonctionnelle'!D12&lt;&gt;"",'Erreur Fonctionnelle'!D12,""))</f>
-        <v/>
+        <v>window.functional.error.invalid.analysis.folder=La carpeta a analizar no es válida (la ruta no existe)</v>
       </c>
     </row>
     <row r="619" spans="1:1" x14ac:dyDescent="0.25">
@@ -36666,7 +36992,7 @@
     </row>
     <row r="654" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A654" t="str">
-        <f>IF('Erreur Fonctionnelle'!B48&lt;&gt;"",CONCATENATE('Erreur Fonctionnelle'!B48,"=", 'Erreur Fonctionnelle'!D48),IF('Erreur Fonctionnelle'!D48&lt;&gt;"",'Erreur Fonctionnelle'!D48,""))</f>
+        <f>IF('Erreur Fonctionnelle'!B48&lt;&gt;"",CONCATENATE('Erreur Fonctionnelle'!B48,"=", 'Erreur Fonctionnelle'!C48),IF('Erreur Fonctionnelle'!C48&lt;&gt;"",'Erreur Fonctionnelle'!C48,""))</f>
         <v/>
       </c>
     </row>
@@ -36799,12 +37125,6 @@
     <row r="676" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A676" t="str">
         <f>IF('Erreur Fonctionnelle'!B70&lt;&gt;"",CONCATENATE('Erreur Fonctionnelle'!B70,"=", 'Erreur Fonctionnelle'!C70),IF('Erreur Fonctionnelle'!C70&lt;&gt;"",'Erreur Fonctionnelle'!C70,""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="677" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A677" t="str">
-        <f>IF('Erreur Fonctionnelle'!B71&lt;&gt;"",CONCATENATE('Erreur Fonctionnelle'!B71,"=", 'Erreur Fonctionnelle'!C71),IF('Erreur Fonctionnelle'!C71&lt;&gt;"",'Erreur Fonctionnelle'!C71,""))</f>
         <v/>
       </c>
     </row>
@@ -36816,10 +37136,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
-  <dimension ref="A1:A650"/>
+  <dimension ref="A1:A649"/>
   <sheetViews>
-    <sheetView topLeftCell="A599" workbookViewId="0">
-      <selection activeCell="A614" sqref="A614:A616"/>
+    <sheetView topLeftCell="A521" workbookViewId="0">
+      <selection activeCell="A534" sqref="A534:A537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39062,19 +39382,19 @@
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" t="str">
         <f>IF(Autres!B51&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B51),".","_"),"=""", Autres!B51,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_OPERATION_VALIDATE="window.operation.validate";</v>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" t="str">
         <f>IF(Autres!B52&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B52),".","_"),"=""", Autres!B52,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_INFORMATION_ANSWER_USER_PANEL_TITLE="window.information.answer.user.panel.title";</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" t="str">
         <f>IF(Autres!B53&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B53),".","_"),"=""", Autres!B53,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_INFORMATION_QUESTION_USER_PANEL_TITLE="window.information.question.user.panel.title";</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
@@ -39962,97 +40282,97 @@
     <row r="523" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A523" t="str">
         <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B12),".","_"),"=""", 'Commencer analyse'!B12,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_TOKEN_PANEL_TITLE="window.start.analysis.token.panel.title";</v>
       </c>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A524" t="str">
         <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B13),".","_"),"=""", 'Commencer analyse'!B13,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_EDIT_FILTER_LABEL="window.start.analysis.edit.filter.label";</v>
       </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A525" t="str">
         <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B14),".","_"),"=""", 'Commencer analyse'!B14,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_INFORMATION_MESSAGE_TOKEN="window.start.analysis.information.message.token";</v>
       </c>
     </row>
     <row r="526" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A526" t="str">
         <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B15),".","_"),"=""", 'Commencer analyse'!B15,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_EDIT_PROFILE_LABEL="window.start.analysis.edit.profile.label";</v>
       </c>
     </row>
     <row r="527" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A527" t="str">
         <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B16),".","_"),"=""", 'Commencer analyse'!B16,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_EDIT_PROFILE_NEW_BUTTON_LABEL="window.start.analysis.edit.profile.new.button.label";</v>
       </c>
     </row>
     <row r="528" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A528" t="str">
         <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B17),".","_"),"=""", 'Commencer analyse'!B17,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_EDIT_FILTER_ADD_BUTTON_LABEL="window.start.analysis.edit.filter.add.button.label";</v>
       </c>
     </row>
     <row r="529" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A529" t="str">
         <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B18),".","_"),"=""", 'Commencer analyse'!B18,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_EDIT_FILTER_REMOVE_BUTTON_LABEL="window.start.analysis.edit.filter.remove.button.label";</v>
       </c>
     </row>
     <row r="530" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A530" t="str">
         <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B19),".","_"),"=""", 'Commencer analyse'!B19,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_TOKEN_TABLE_HEADER_LABEL="window.start.analysis.token.table.header.label";</v>
       </c>
     </row>
     <row r="531" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A531" t="str">
         <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B20),".","_"),"=""", 'Commencer analyse'!B20,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_TOKEN_ADD_INFORMATION_MESSAGE="window.start.analysis.token.add.information.message";</v>
       </c>
     </row>
     <row r="532" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A532" t="str">
         <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B21),".","_"),"=""", 'Commencer analyse'!B21,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_TOKEN_ADD_TEXT_LABEL="window.start.analysis.token.add.text.label";</v>
       </c>
     </row>
     <row r="533" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A533" t="str">
         <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B22),".","_"),"=""", 'Commencer analyse'!B22,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_TOKEN_TABLE_PANEL_TITLE="window.start.analysis.token.table.panel.title";</v>
       </c>
     </row>
     <row r="534" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A534" t="str">
         <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B23),".","_"),"=""", 'Commencer analyse'!B23,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_EDIT_PROFILE_REMOVE_BUTTON_LABEL="window.start.analysis.edit.profile.remove.button.label";</v>
       </c>
     </row>
     <row r="535" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A535" t="str">
         <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B24),".","_"),"=""", 'Commencer analyse'!B24,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_EDIT_PROFILE_SAVE_BUTTON_LABEL="window.start.analysis.edit.profile.save.button.label";</v>
       </c>
     </row>
     <row r="536" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A536" t="str">
         <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B25),".","_"),"=""", 'Commencer analyse'!B25,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_EDIT_PROFILE_REMOVE_BUTTON_CONFIRMATION_MESSAGE="window.start.analysis.edit.profile.remove.button.confirmation.message";</v>
       </c>
     </row>
     <row r="537" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A537" t="str">
         <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B26),".","_"),"=""", 'Commencer analyse'!B26,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_EDIT_PROFILE_NEW_BUTTON_COPY_OR_NEW_MESSAGE="window.start.analysis.edit.profile.new.button.copy.or.new.message";</v>
       </c>
     </row>
     <row r="538" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A538" t="str">
         <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B27),".","_"),"=""", 'Commencer analyse'!B27,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_EDIT_PROFILE_NEW_BUTTON_NEW_NAME_MESSAGE="window.start.analysis.edit.profile.new.button.new.name.message";</v>
       </c>
     </row>
     <row r="539" spans="1:1" x14ac:dyDescent="0.25">
@@ -40526,7 +40846,7 @@
     <row r="617" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A617" t="str">
         <f>IF('Erreur Fonctionnelle'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B12),".","_"),"=""", 'Erreur Fonctionnelle'!B12,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_FUNCTIONAL_ERROR_INVALID_ANALYSIS_FOLDER="window.functional.error.invalid.analysis.folder";</v>
       </c>
     </row>
     <row r="618" spans="1:1" x14ac:dyDescent="0.25">
@@ -40718,12 +41038,6 @@
     <row r="649" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A649" t="str">
         <f>IF('Erreur Fonctionnelle'!B44&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B44),".","_"),"=""", 'Erreur Fonctionnelle'!B44,""";"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="650" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A650" t="str">
-        <f>IF('Erreur Fonctionnelle'!B45&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B45),".","_"),"=""", 'Erreur Fonctionnelle'!B45,""";"),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Avancement sur l'analyse avec prise en charge de l'édition des liste pour la lemmatisation et la tokenization : - Optimisation des performances - Prise en charge du contrôle des doublons
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\IdeaProjects\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB8B5AF-05B6-4089-B850-E3C34F4EEE70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F08FFA-8DB1-42B6-B6B2-611803F90584}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="17" activeTab="18" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="690" yWindow="4215" windowWidth="21600" windowHeight="11385" firstSheet="17" activeTab="20" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="932">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -2835,6 +2835,15 @@
   </si>
   <si>
     <t>window.start.analysis.edit.profile.new.button.new.name.message</t>
+  </si>
+  <si>
+    <t>window.functional.error.value.exist</t>
+  </si>
+  <si>
+    <t>La nouvelle valeur est déjà présente dans la liste. Votre action a été annulé par le système</t>
+  </si>
+  <si>
+    <t>El nuevo valor ya está presente en la lista. Su acción ha sido cancelada por el sistema</t>
   </si>
 </sst>
 </file>
@@ -27693,7 +27702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757EF7E0-E814-48B2-A4AF-487C809E6C10}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -28017,7 +28026,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -28799,8 +28808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD31F70A-F934-4E15-ACEB-A430E2D8A684}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28964,6 +28973,20 @@
       </c>
       <c r="D12" t="s">
         <v>894</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>929</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
@@ -28983,7 +29006,7 @@
   <dimension ref="A1:A677"/>
   <sheetViews>
     <sheetView showZeros="0" topLeftCell="A511" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A528" sqref="A1:A677"/>
+      <selection activeCell="A532" sqref="A1:A677"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32702,7 +32725,7 @@
     <row r="619" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A619" t="str">
         <f>IF('Erreur Fonctionnelle'!B13&lt;&gt;"",CONCATENATE('Erreur Fonctionnelle'!B13,"=", 'Erreur Fonctionnelle'!C13),IF('Erreur Fonctionnelle'!C13&lt;&gt;"",'Erreur Fonctionnelle'!C13,""))</f>
-        <v/>
+        <v>window.functional.error.value.exist=La nouvelle valeur est déjà présente dans la liste. Votre action a été annulé par le système</v>
       </c>
     </row>
     <row r="620" spans="1:1" x14ac:dyDescent="0.25">
@@ -33064,7 +33087,7 @@
   <dimension ref="A1:A676"/>
   <sheetViews>
     <sheetView showZeros="0" topLeftCell="A592" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A618" sqref="A618:XFD618"/>
+      <selection activeCell="A611" sqref="A1:A676"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36783,7 +36806,7 @@
     <row r="619" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A619" t="str">
         <f>IF('Erreur Fonctionnelle'!B13&lt;&gt;"",CONCATENATE('Erreur Fonctionnelle'!B13,"=", 'Erreur Fonctionnelle'!D13),IF('Erreur Fonctionnelle'!D13&lt;&gt;"",'Erreur Fonctionnelle'!D13,""))</f>
-        <v/>
+        <v>window.functional.error.value.exist=El nuevo valor ya está presente en la lista. Su acción ha sido cancelada por el sistema</v>
       </c>
     </row>
     <row r="620" spans="1:1" x14ac:dyDescent="0.25">
@@ -37138,8 +37161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
   <dimension ref="A1:A649"/>
   <sheetViews>
-    <sheetView topLeftCell="A521" workbookViewId="0">
-      <selection activeCell="A534" sqref="A534:A537"/>
+    <sheetView topLeftCell="A596" workbookViewId="0">
+      <selection activeCell="A618" sqref="A618"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40852,7 +40875,7 @@
     <row r="618" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A618" t="str">
         <f>IF('Erreur Fonctionnelle'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B13),".","_"),"=""", 'Erreur Fonctionnelle'!B13,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_FUNCTIONAL_ERROR_VALUE_EXIST="window.functional.error.value.exist";</v>
       </c>
     </row>
     <row r="619" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Avancement sur le module d'analyse : - création des première fenêtre de l'assistant
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\IdeaProjects\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8005CA-470B-40AB-8A1B-9E8A03905D6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5D4E44-FD75-49E5-BBD1-64E4612DEF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="19" activeTab="26" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="17" activeTab="18" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="1026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="1068">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -2778,24 +2778,12 @@
     <t>window.menu.level6.sublevel3.sublevel2.title</t>
   </si>
   <si>
-    <t>Radicaux</t>
-  </si>
-  <si>
     <t>window.menu.level6.sublevel3.sublevel3.title</t>
   </si>
   <si>
-    <t>Radicaux par classe</t>
-  </si>
-  <si>
     <t>Gestión de listas</t>
   </si>
   <si>
-    <t>Radicales</t>
-  </si>
-  <si>
-    <t>Radicales por clase</t>
-  </si>
-  <si>
     <t>Gestión de StopWords</t>
   </si>
   <si>
@@ -3130,6 +3118,144 @@
   </si>
   <si>
     <t>Clase</t>
+  </si>
+  <si>
+    <t>window.start.analysis.information.message.etape2</t>
+  </si>
+  <si>
+    <t>window.start.analysis.type.panel.title</t>
+  </si>
+  <si>
+    <t>Choix des analyses</t>
+  </si>
+  <si>
+    <t>Elección de análisis</t>
+  </si>
+  <si>
+    <t>window.start.analysis.information.message.etape3</t>
+  </si>
+  <si>
+    <t>window.start.analysis.field.material.panel.title</t>
+  </si>
+  <si>
+    <t>Choix des champs à analyser</t>
+  </si>
+  <si>
+    <t>window.start.analysis.information.message.etape4</t>
+  </si>
+  <si>
+    <t>window.start.analysis.choose.analyse.label</t>
+  </si>
+  <si>
+    <t>Choix de l'analyse</t>
+  </si>
+  <si>
+    <t>window.start.analysis.choose.analyse.panel.title</t>
+  </si>
+  <si>
+    <t>Analyse Lexicométrique</t>
+  </si>
+  <si>
+    <t>Análisis lexicométrico</t>
+  </si>
+  <si>
+    <t>window.start.analysis.choose.analyse.option.panel.title</t>
+  </si>
+  <si>
+    <t>Options disponibles/nécessaires pour l'analyse</t>
+  </si>
+  <si>
+    <t>Opciones disponibles/requeridas para el análisis</t>
+  </si>
+  <si>
+    <t>window.start.analysis.start.button.label</t>
+  </si>
+  <si>
+    <t>Lancer l'analyse</t>
+  </si>
+  <si>
+    <t>Iniciar el análisis</t>
+  </si>
+  <si>
+    <t>window.start.analysis.consult.results.button.label</t>
+  </si>
+  <si>
+    <t>Consulter les résultats</t>
+  </si>
+  <si>
+    <t>Consultar los resultados</t>
+  </si>
+  <si>
+    <t>window.start.analysis.token.number.label</t>
+  </si>
+  <si>
+    <t>Nombre de tokens</t>
+  </si>
+  <si>
+    <t>Numero de tokens</t>
+  </si>
+  <si>
+    <t>Lemmatisation et numéro type</t>
+  </si>
+  <si>
+    <t>Type token ratio</t>
+  </si>
+  <si>
+    <t>Fréquence</t>
+  </si>
+  <si>
+    <t>window.start.analysis.frequency.label</t>
+  </si>
+  <si>
+    <t>window.start.analysis.token.ratio.label</t>
+  </si>
+  <si>
+    <t>window.start.analysis.lemme.type.label</t>
+  </si>
+  <si>
+    <t>Lematización y número de tipo</t>
+  </si>
+  <si>
+    <t>Tipo de proporción de tokens</t>
+  </si>
+  <si>
+    <t>Frecuencia</t>
+  </si>
+  <si>
+    <t>window.start.analysis.choose.type.treatment.optional.list.panel.title</t>
+  </si>
+  <si>
+    <t>Choix de la liste à utiliser</t>
+  </si>
+  <si>
+    <t>window.start.analysis.choose.profile.treatment.optional.list.panel.title</t>
+  </si>
+  <si>
+    <t>Elegir qué lista usar</t>
+  </si>
+  <si>
+    <t>window.start.analysis.choose.type.treatment.optional.list.label</t>
+  </si>
+  <si>
+    <t>window.start.analysis.choose.profile.treatment.optional.list.label</t>
+  </si>
+  <si>
+    <t>Type de prétraitement des données</t>
+  </si>
+  <si>
+    <t>Modèle pour le prétaritement des données</t>
+  </si>
+  <si>
+    <t>Tipo de preprocesamiento de datos</t>
+  </si>
+  <si>
+    <t>Modelo de pretratamiento de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choix du type de liste </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elegir el tipo de lista </t>
   </si>
 </sst>
 </file>
@@ -24518,8 +24644,8 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{3A067453-0998-4B6F-A015-C36FFF350274}" name="Tableau161015181920" displayName="Tableau161015181920" ref="A1:D58" totalsRowShown="0">
-  <autoFilter ref="A1:D58" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{3A067453-0998-4B6F-A015-C36FFF350274}" name="Tableau161015181920" displayName="Tableau161015181920" ref="A1:D55" totalsRowShown="0">
+  <autoFilter ref="A1:D55" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{93EBCA28-6850-4E5B-95B0-10E875DF804E}" name="Numero"/>
     <tableColumn id="2" xr3:uid="{C2EDFC63-75B8-42C6-A92C-19BA73C907B7}" name="Code"/>
@@ -25011,8 +25137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF59B93E-40E9-44D6-98FA-7D0A802C1DCE}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59:D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25744,7 +25870,7 @@
         <v>904</v>
       </c>
       <c r="D56" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -25769,10 +25895,10 @@
         <v>907</v>
       </c>
       <c r="C58" t="s">
-        <v>908</v>
+        <v>989</v>
       </c>
       <c r="D58" t="s">
-        <v>912</v>
+        <v>999</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -25780,13 +25906,13 @@
         <v>51</v>
       </c>
       <c r="B59" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C59" t="s">
-        <v>910</v>
+        <v>1010</v>
       </c>
       <c r="D59" t="s">
-        <v>913</v>
+        <v>1014</v>
       </c>
     </row>
   </sheetData>
@@ -28094,10 +28220,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757EF7E0-E814-48B2-A4AF-487C809E6C10}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28192,46 +28318,269 @@
         <v>769</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+    <row r="7" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner les matériaux sur lesquels vous souhaitez effectuer l'analyse.&lt;BR/&gt;",
+"NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner les matériaux sur lesquels vous souhaitez effectuer l'analyse.&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar los materiales en los que desea realizar el análisis.&lt;BR/&gt;",
+"NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar los materiales en los que desea realizar el análisis.&lt;BR/&gt;NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner les champs correspondant aux matériaux sur lesquels vous souhaitez effectuer l'analyse.&lt;BR/&gt;",
+"NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner les champs correspondant aux matériaux sur lesquels vous souhaitez effectuer l'analyse.&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar los campos correspondientes a los materiales sobre los que desea realizar el análisis.&lt;BR/&gt;",
+"NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar los campos correspondientes a los materiales sobre los que desea realizar el análisis.&lt;BR/&gt;NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner le type d'analyse que vous souhaitez effectuer.&lt;BR/&gt;","Puis de consulter les résultats.&lt;BR/&gt;",
+"NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner le type d'analyse que vous souhaitez effectuer.&lt;BR/&gt;Puis de consulter les résultats.&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f xml:space="preserve"> CONCATENATE("&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar el tipo de análisis que desea realizar.&lt;BR/&gt;", "Luego consulte los resultados.&lt;BR/&gt;",
+"NB: En cualquier momento puede volver con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar el tipo de análisis que desea realizar.&lt;BR/&gt;Luego consulte los resultados.&lt;BR/&gt;NB: En cualquier momento puede volver con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1025</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1037</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="3:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="1"/>
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1059</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -29204,13 +29553,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>895</v>
       </c>
       <c r="D3" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -29218,13 +29567,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
       <c r="C4" t="s">
         <v>896</v>
       </c>
       <c r="D4" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -29232,13 +29581,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
       <c r="C5" t="s">
         <v>899</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -29246,13 +29595,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
       <c r="C6" t="s">
         <v>898</v>
       </c>
       <c r="D6" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -29260,7 +29609,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;La suppression de la liste est définitive et ne peut pas être annulé.&lt;BR/&gt;",
@@ -29278,7 +29627,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Voulez vous créer une copie de la liste en cours ?&lt;BR/&gt;",
@@ -29296,7 +29645,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quelle est le nom de la nouvelle liste ?&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;")</f>
@@ -29312,13 +29661,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="C10" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="D10" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -29343,7 +29692,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:D12"/>
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29372,13 +29721,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="C3" t="s">
         <v>894</v>
       </c>
       <c r="D3" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -29386,7 +29735,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Dans cette étape vous pouvez gérer les StopWord à nettoyer&lt;BR/&gt;",
@@ -29406,7 +29755,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="C5" t="s">
         <v>893</v>
@@ -29420,7 +29769,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quelle est le nouveau StopWord à ajouter ?&lt;BR/&gt;",
@@ -29438,13 +29787,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>892</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -29452,13 +29801,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="C8" t="s">
         <v>897</v>
       </c>
       <c r="D8" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -29466,13 +29815,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>949</v>
+      </c>
+      <c r="C9" t="s">
+        <v>951</v>
+      </c>
+      <c r="D9" t="s">
         <v>953</v>
-      </c>
-      <c r="C9" t="s">
-        <v>955</v>
-      </c>
-      <c r="D9" t="s">
-        <v>957</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -29480,13 +29829,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>950</v>
+      </c>
+      <c r="C10" t="s">
+        <v>952</v>
+      </c>
+      <c r="D10" t="s">
         <v>954</v>
-      </c>
-      <c r="C10" t="s">
-        <v>956</v>
-      </c>
-      <c r="D10" t="s">
-        <v>958</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -29494,13 +29843,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
       <c r="C11" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
       <c r="D11" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -29508,13 +29857,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
       <c r="C12" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="D12" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -29534,7 +29883,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29563,13 +29912,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="C3" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
       <c r="D3" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -29577,7 +29926,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Dans cette étape vous pouvez gérer les lemmes à nettoyer&lt;BR/&gt;",
@@ -29597,13 +29946,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="C5" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
       <c r="D5" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -29611,7 +29960,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>926</v>
+        <v>922</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quelle est le nouveau lemme à ajouter ?&lt;BR/&gt;",
@@ -29629,13 +29978,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -29643,13 +29992,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>928</v>
+        <v>924</v>
       </c>
       <c r="C8" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="D8" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -29657,7 +30006,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quelle est la nouvelle forme à ajouter ?&lt;BR/&gt;",
@@ -29675,13 +30024,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -29689,13 +30038,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
       <c r="C11" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="D11" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -29703,13 +30052,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
       <c r="C12" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="D12" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -29717,13 +30066,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
       <c r="C13" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="D13" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -29731,13 +30080,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="C14" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="D14" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -29745,13 +30094,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="C15" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
       <c r="D15" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -29759,13 +30108,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="C16" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="D16" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -29773,13 +30122,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
       <c r="C17" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="D17" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -29787,13 +30136,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="C18" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="D18" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
     </row>
   </sheetData>
@@ -29808,8 +30157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C55C70F-72D6-4EA0-AEB3-AE97300CBF17}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29838,13 +30187,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
       <c r="C3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D3" t="s">
         <v>1013</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -29852,7 +30201,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Dans cette étape vous pouvez gérer les lemmes par classe&lt;BR/&gt;",
@@ -29872,13 +30221,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
       <c r="C5" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D5" t="s">
         <v>1014</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1018</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -29886,7 +30235,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quelle est le nouveau lemme à ajouter ?&lt;BR/&gt;",
@@ -29904,13 +30253,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -29918,13 +30267,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="C8" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="D8" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -29932,7 +30281,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quelle est la nouvelle forme à ajouter ?&lt;BR/&gt;",
@@ -29950,13 +30299,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -29964,7 +30313,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
       <c r="C11" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quelle est la nouvelle classe à ajouter ?&lt;BR/&gt;",
@@ -29982,13 +30331,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -29996,13 +30345,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="C13" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="D13" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -30010,13 +30359,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="C14" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="D14" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -30024,13 +30373,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
       <c r="C15" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="D15" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -30038,13 +30387,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
       <c r="C16" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="D16" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -30052,13 +30401,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
       <c r="C17" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
       <c r="D17" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -30066,13 +30415,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
       <c r="C18" t="s">
-        <v>970</v>
+        <v>966</v>
       </c>
       <c r="D18" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -30080,13 +30429,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
       <c r="C19" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
       <c r="D19" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -30094,13 +30443,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
       <c r="C20" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="D20" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -30108,13 +30457,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
       <c r="C21" t="s">
+        <v>975</v>
+      </c>
+      <c r="D21" t="s">
         <v>979</v>
-      </c>
-      <c r="D21" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -30122,13 +30471,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="C22" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="D22" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -30136,13 +30485,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="C23" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="D23" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -30150,13 +30499,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="C24" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="D24" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
     </row>
   </sheetData>
@@ -30171,8 +30520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904B2FA-CBC2-495A-A197-D0CDD47EB1AE}">
   <dimension ref="A1:A781"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A763" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A772" sqref="A1:A781"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A781" sqref="A1:A781"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30519,13 +30868,13 @@
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>IF('Fenêtre principal'!B58&lt;&gt;"",CONCATENATE('Fenêtre principal'!B58,"=", 'Fenêtre principal'!C58),IF('Fenêtre principal'!C58&lt;&gt;"",'Fenêtre principal'!C58,""))</f>
-        <v>window.menu.level6.sublevel3.sublevel2.title=Radicaux</v>
+        <v>window.menu.level6.sublevel3.sublevel2.title=Lemmes</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>IF('Fenêtre principal'!B59&lt;&gt;"",CONCATENATE('Fenêtre principal'!B59,"=", 'Fenêtre principal'!C59),IF('Fenêtre principal'!C59&lt;&gt;"",'Fenêtre principal'!C59,""))</f>
-        <v>window.menu.level6.sublevel3.sublevel3.title=Radicaux par classe</v>
+        <v>window.menu.level6.sublevel3.sublevel3.title=Lemmes par classes</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
@@ -33439,326 +33788,326 @@
       </c>
     </row>
     <row r="544" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A544" t="str">
-        <f>IF('Commencer analyse'!B7&lt;&gt;"",CONCATENATE('Commencer analyse'!B7,"=", 'Commencer analyse'!C7),IF('Commencer analyse'!C7&lt;&gt;"",'Commencer analyse'!C7,""))</f>
-        <v/>
+      <c r="A544" t="e">
+        <f>IF('Commencer analyse'!#REF!&lt;&gt;"",CONCATENATE('Commencer analyse'!#REF!,"=", 'Commencer analyse'!#REF!),IF('Commencer analyse'!#REF!&lt;&gt;"",'Commencer analyse'!#REF!,""))</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="545" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A545" t="str">
-        <f>IF('Commencer analyse'!B8&lt;&gt;"",CONCATENATE('Commencer analyse'!B8,"=", 'Commencer analyse'!C8),IF('Commencer analyse'!C8&lt;&gt;"",'Commencer analyse'!C8,""))</f>
-        <v/>
+      <c r="A545" t="e">
+        <f>IF('Commencer analyse'!#REF!&lt;&gt;"",CONCATENATE('Commencer analyse'!#REF!,"=", 'Commencer analyse'!#REF!),IF('Commencer analyse'!#REF!&lt;&gt;"",'Commencer analyse'!#REF!,""))</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="546" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A546" t="str">
-        <f>IF('Commencer analyse'!B9&lt;&gt;"",CONCATENATE('Commencer analyse'!B9,"=", 'Commencer analyse'!C9),IF('Commencer analyse'!C9&lt;&gt;"",'Commencer analyse'!C9,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B7&lt;&gt;"",CONCATENATE('Commencer analyse'!B7,"=", 'Commencer analyse'!C7),IF('Commencer analyse'!C7&lt;&gt;"",'Commencer analyse'!C7,""))</f>
+        <v>window.start.analysis.information.message.etape2=&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner les matériaux sur lesquels vous souhaitez effectuer l'analyse.&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="547" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A547" t="str">
-        <f>IF('Commencer analyse'!B10&lt;&gt;"",CONCATENATE('Commencer analyse'!B10,"=", 'Commencer analyse'!C10),IF('Commencer analyse'!C10&lt;&gt;"",'Commencer analyse'!C10,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B8&lt;&gt;"",CONCATENATE('Commencer analyse'!B8,"=", 'Commencer analyse'!C8),IF('Commencer analyse'!C8&lt;&gt;"",'Commencer analyse'!C8,""))</f>
+        <v>window.start.analysis.type.panel.title=Choix des analyses</v>
       </c>
     </row>
     <row r="548" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A548" t="str">
-        <f>IF('Commencer analyse'!B11&lt;&gt;"",CONCATENATE('Commencer analyse'!B11,"=", 'Commencer analyse'!C11),IF('Commencer analyse'!C11&lt;&gt;"",'Commencer analyse'!C11,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B9&lt;&gt;"",CONCATENATE('Commencer analyse'!B9,"=", 'Commencer analyse'!C9),IF('Commencer analyse'!C9&lt;&gt;"",'Commencer analyse'!C9,""))</f>
+        <v>window.start.analysis.information.message.etape3=&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner les champs correspondant aux matériaux sur lesquels vous souhaitez effectuer l'analyse.&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="549" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A549" t="str">
-        <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE('Commencer analyse'!B12,"=", 'Commencer analyse'!C12),IF('Commencer analyse'!C12&lt;&gt;"",'Commencer analyse'!C12,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B10&lt;&gt;"",CONCATENATE('Commencer analyse'!B10,"=", 'Commencer analyse'!C10),IF('Commencer analyse'!C10&lt;&gt;"",'Commencer analyse'!C10,""))</f>
+        <v>window.start.analysis.field.material.panel.title=Choix des champs à analyser</v>
       </c>
     </row>
     <row r="550" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A550" t="str">
-        <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE('Commencer analyse'!B13,"=", 'Commencer analyse'!C13),IF('Commencer analyse'!C13&lt;&gt;"",'Commencer analyse'!C13,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B11&lt;&gt;"",CONCATENATE('Commencer analyse'!B11,"=", 'Commencer analyse'!C11),IF('Commencer analyse'!C11&lt;&gt;"",'Commencer analyse'!C11,""))</f>
+        <v>window.start.analysis.information.message.etape4=&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner le type d'analyse que vous souhaitez effectuer.&lt;BR/&gt;Puis de consulter les résultats.&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="551" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A551" t="str">
-        <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE('Commencer analyse'!B14,"=", 'Commencer analyse'!C14),IF('Commencer analyse'!C14&lt;&gt;"",'Commencer analyse'!C14,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE('Commencer analyse'!B12,"=", 'Commencer analyse'!C12),IF('Commencer analyse'!C12&lt;&gt;"",'Commencer analyse'!C12,""))</f>
+        <v>window.start.analysis.choose.analyse.label=Choix de l'analyse</v>
       </c>
     </row>
     <row r="552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A552" t="str">
-        <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE('Commencer analyse'!B15,"=", 'Commencer analyse'!C15),IF('Commencer analyse'!C15&lt;&gt;"",'Commencer analyse'!C15,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE('Commencer analyse'!B13,"=", 'Commencer analyse'!C13),IF('Commencer analyse'!C13&lt;&gt;"",'Commencer analyse'!C13,""))</f>
+        <v>window.start.analysis.choose.analyse.panel.title=Analyse Lexicométrique</v>
       </c>
     </row>
     <row r="553" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A553" t="str">
-        <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE('Commencer analyse'!B16,"=", 'Commencer analyse'!C16),IF('Commencer analyse'!C16&lt;&gt;"",'Commencer analyse'!C16,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE('Commencer analyse'!B14,"=", 'Commencer analyse'!C14),IF('Commencer analyse'!C14&lt;&gt;"",'Commencer analyse'!C14,""))</f>
+        <v>window.start.analysis.choose.analyse.option.panel.title=Options disponibles/nécessaires pour l'analyse</v>
       </c>
     </row>
     <row r="554" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A554" t="str">
-        <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE('Commencer analyse'!B17,"=", 'Commencer analyse'!C17),IF('Commencer analyse'!C17&lt;&gt;"",'Commencer analyse'!C17,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE('Commencer analyse'!B15,"=", 'Commencer analyse'!C15),IF('Commencer analyse'!C15&lt;&gt;"",'Commencer analyse'!C15,""))</f>
+        <v>window.start.analysis.start.button.label=Lancer l'analyse</v>
       </c>
     </row>
     <row r="555" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A555" t="str">
-        <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE('Commencer analyse'!B18,"=", 'Commencer analyse'!C18),IF('Commencer analyse'!C18&lt;&gt;"",'Commencer analyse'!C18,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE('Commencer analyse'!B16,"=", 'Commencer analyse'!C16),IF('Commencer analyse'!C16&lt;&gt;"",'Commencer analyse'!C16,""))</f>
+        <v>window.start.analysis.consult.results.button.label=Consulter les résultats</v>
       </c>
     </row>
     <row r="556" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A556" t="str">
-        <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE('Commencer analyse'!B19,"=", 'Commencer analyse'!C19),IF('Commencer analyse'!C19&lt;&gt;"",'Commencer analyse'!C19,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE('Commencer analyse'!B17,"=", 'Commencer analyse'!C17),IF('Commencer analyse'!C17&lt;&gt;"",'Commencer analyse'!C17,""))</f>
+        <v>window.start.analysis.token.number.label=Nombre de tokens</v>
       </c>
     </row>
     <row r="557" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A557" t="str">
-        <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE('Commencer analyse'!B20,"=", 'Commencer analyse'!C20),IF('Commencer analyse'!C20&lt;&gt;"",'Commencer analyse'!C20,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE('Commencer analyse'!B18,"=", 'Commencer analyse'!C18),IF('Commencer analyse'!C18&lt;&gt;"",'Commencer analyse'!C18,""))</f>
+        <v>window.start.analysis.lemme.type.label=Lemmatisation et numéro type</v>
       </c>
     </row>
     <row r="558" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A558" t="str">
-        <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE('Commencer analyse'!B21,"=", 'Commencer analyse'!C21),IF('Commencer analyse'!C21&lt;&gt;"",'Commencer analyse'!C21,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE('Commencer analyse'!B19,"=", 'Commencer analyse'!C19),IF('Commencer analyse'!C19&lt;&gt;"",'Commencer analyse'!C19,""))</f>
+        <v>window.start.analysis.token.ratio.label=Type token ratio</v>
       </c>
     </row>
     <row r="559" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A559" t="str">
-        <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE('Commencer analyse'!B22,"=", 'Commencer analyse'!C22),IF('Commencer analyse'!C22&lt;&gt;"",'Commencer analyse'!C22,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE('Commencer analyse'!B20,"=", 'Commencer analyse'!C20),IF('Commencer analyse'!C20&lt;&gt;"",'Commencer analyse'!C20,""))</f>
+        <v>window.start.analysis.frequency.label=Fréquence</v>
       </c>
     </row>
     <row r="560" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A560" t="str">
-        <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE('Commencer analyse'!B23,"=", 'Commencer analyse'!C23),IF('Commencer analyse'!C23&lt;&gt;"",'Commencer analyse'!C23,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE('Commencer analyse'!B21,"=", 'Commencer analyse'!C21),IF('Commencer analyse'!C21&lt;&gt;"",'Commencer analyse'!C21,""))</f>
+        <v>window.start.analysis.choose.type.treatment.optional.list.panel.title=Type de prétraitement des données</v>
       </c>
     </row>
     <row r="561" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A561" t="str">
-        <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE('Commencer analyse'!B24,"=", 'Commencer analyse'!C24),IF('Commencer analyse'!C24&lt;&gt;"",'Commencer analyse'!C24,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE('Commencer analyse'!B22,"=", 'Commencer analyse'!C22),IF('Commencer analyse'!C22&lt;&gt;"",'Commencer analyse'!C22,""))</f>
+        <v>window.start.analysis.choose.profile.treatment.optional.list.panel.title=Modèle pour le prétaritement des données</v>
       </c>
     </row>
     <row r="562" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A562" t="str">
-        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE('Commencer analyse'!B25,"=", 'Commencer analyse'!C25),IF('Commencer analyse'!C25&lt;&gt;"",'Commencer analyse'!C25,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE('Commencer analyse'!B23,"=", 'Commencer analyse'!C23),IF('Commencer analyse'!C23&lt;&gt;"",'Commencer analyse'!C23,""))</f>
+        <v xml:space="preserve">window.start.analysis.choose.type.treatment.optional.list.label=Choix du type de liste </v>
       </c>
     </row>
     <row r="563" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A563" t="str">
-        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE('Commencer analyse'!B26,"=", 'Commencer analyse'!C26),IF('Commencer analyse'!C26&lt;&gt;"",'Commencer analyse'!C26,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE('Commencer analyse'!B24,"=", 'Commencer analyse'!C24),IF('Commencer analyse'!C24&lt;&gt;"",'Commencer analyse'!C24,""))</f>
+        <v>window.start.analysis.choose.profile.treatment.optional.list.label=Choix de la liste à utiliser</v>
       </c>
     </row>
     <row r="564" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A564" t="str">
-        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE('Commencer analyse'!B27,"=", 'Commencer analyse'!C27),IF('Commencer analyse'!C27&lt;&gt;"",'Commencer analyse'!C27,""))</f>
-        <v/>
+      <c r="A564" t="e">
+        <f>IF('Commencer analyse'!#REF!&lt;&gt;"",CONCATENATE('Commencer analyse'!#REF!,"=", 'Commencer analyse'!#REF!),IF('Commencer analyse'!#REF!&lt;&gt;"",'Commencer analyse'!#REF!,""))</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="565" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A565" t="str">
-        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE('Commencer analyse'!B28,"=", 'Commencer analyse'!C28),IF('Commencer analyse'!C28&lt;&gt;"",'Commencer analyse'!C28,""))</f>
+        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE('Commencer analyse'!B25,"=", 'Commencer analyse'!C25),IF('Commencer analyse'!C25&lt;&gt;"",'Commencer analyse'!C25,""))</f>
         <v/>
       </c>
     </row>
     <row r="566" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A566" t="str">
-        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE('Commencer analyse'!B29,"=", 'Commencer analyse'!C29),IF('Commencer analyse'!C29&lt;&gt;"",'Commencer analyse'!C29,""))</f>
+        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE('Commencer analyse'!B26,"=", 'Commencer analyse'!C26),IF('Commencer analyse'!C26&lt;&gt;"",'Commencer analyse'!C26,""))</f>
         <v/>
       </c>
     </row>
     <row r="567" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A567" t="str">
-        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE('Commencer analyse'!B30,"=", 'Commencer analyse'!C30),IF('Commencer analyse'!C30&lt;&gt;"",'Commencer analyse'!C30,""))</f>
+        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE('Commencer analyse'!B27,"=", 'Commencer analyse'!C27),IF('Commencer analyse'!C27&lt;&gt;"",'Commencer analyse'!C27,""))</f>
         <v/>
       </c>
     </row>
     <row r="568" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A568" t="str">
-        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE('Commencer analyse'!B31,"=", 'Commencer analyse'!C31),IF('Commencer analyse'!C31&lt;&gt;"",'Commencer analyse'!C31,""))</f>
+        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE('Commencer analyse'!B28,"=", 'Commencer analyse'!C28),IF('Commencer analyse'!C28&lt;&gt;"",'Commencer analyse'!C28,""))</f>
         <v/>
       </c>
     </row>
     <row r="569" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A569" t="str">
-        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE('Commencer analyse'!B32,"=", 'Commencer analyse'!C32),IF('Commencer analyse'!C32&lt;&gt;"",'Commencer analyse'!C32,""))</f>
+        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE('Commencer analyse'!B29,"=", 'Commencer analyse'!C29),IF('Commencer analyse'!C29&lt;&gt;"",'Commencer analyse'!C29,""))</f>
         <v/>
       </c>
     </row>
     <row r="570" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A570" t="str">
-        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE('Commencer analyse'!B33,"=", 'Commencer analyse'!C33),IF('Commencer analyse'!C33&lt;&gt;"",'Commencer analyse'!C33,""))</f>
+        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE('Commencer analyse'!B30,"=", 'Commencer analyse'!C30),IF('Commencer analyse'!C30&lt;&gt;"",'Commencer analyse'!C30,""))</f>
         <v/>
       </c>
     </row>
     <row r="571" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A571" t="str">
-        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE('Commencer analyse'!B34,"=", 'Commencer analyse'!C34),IF('Commencer analyse'!C34&lt;&gt;"",'Commencer analyse'!C34,""))</f>
+        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE('Commencer analyse'!B31,"=", 'Commencer analyse'!C31),IF('Commencer analyse'!C31&lt;&gt;"",'Commencer analyse'!C31,""))</f>
         <v/>
       </c>
     </row>
     <row r="572" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A572" t="str">
-        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE('Commencer analyse'!B35,"=", 'Commencer analyse'!C35),IF('Commencer analyse'!C35&lt;&gt;"",'Commencer analyse'!C35,""))</f>
+        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE('Commencer analyse'!B32,"=", 'Commencer analyse'!C32),IF('Commencer analyse'!C32&lt;&gt;"",'Commencer analyse'!C32,""))</f>
         <v/>
       </c>
     </row>
     <row r="573" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A573" t="str">
-        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE('Commencer analyse'!B36,"=", 'Commencer analyse'!C36),IF('Commencer analyse'!C36&lt;&gt;"",'Commencer analyse'!C36,""))</f>
+        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE('Commencer analyse'!B33,"=", 'Commencer analyse'!C33),IF('Commencer analyse'!C33&lt;&gt;"",'Commencer analyse'!C33,""))</f>
         <v/>
       </c>
     </row>
     <row r="574" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A574" t="str">
-        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE('Commencer analyse'!B37,"=", 'Commencer analyse'!C37),IF('Commencer analyse'!C37&lt;&gt;"",'Commencer analyse'!C37,""))</f>
+        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE('Commencer analyse'!B34,"=", 'Commencer analyse'!C34),IF('Commencer analyse'!C34&lt;&gt;"",'Commencer analyse'!C34,""))</f>
         <v/>
       </c>
     </row>
     <row r="575" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A575" t="str">
-        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE('Commencer analyse'!B38,"=", 'Commencer analyse'!C38),IF('Commencer analyse'!C38&lt;&gt;"",'Commencer analyse'!C38,""))</f>
+        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE('Commencer analyse'!B35,"=", 'Commencer analyse'!C35),IF('Commencer analyse'!C35&lt;&gt;"",'Commencer analyse'!C35,""))</f>
         <v/>
       </c>
     </row>
     <row r="576" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A576" t="str">
-        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE('Commencer analyse'!B39,"=", 'Commencer analyse'!C39),IF('Commencer analyse'!C39&lt;&gt;"",'Commencer analyse'!C39,""))</f>
+        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE('Commencer analyse'!B36,"=", 'Commencer analyse'!C36),IF('Commencer analyse'!C36&lt;&gt;"",'Commencer analyse'!C36,""))</f>
         <v/>
       </c>
     </row>
     <row r="577" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A577" t="str">
-        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE('Commencer analyse'!B40,"=", 'Commencer analyse'!C40),IF('Commencer analyse'!C40&lt;&gt;"",'Commencer analyse'!C40,""))</f>
+        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE('Commencer analyse'!B37,"=", 'Commencer analyse'!C37),IF('Commencer analyse'!C37&lt;&gt;"",'Commencer analyse'!C37,""))</f>
         <v/>
       </c>
     </row>
     <row r="578" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A578" t="str">
-        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE('Commencer analyse'!B41,"=", 'Commencer analyse'!C41),IF('Commencer analyse'!C41&lt;&gt;"",'Commencer analyse'!C41,""))</f>
+        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE('Commencer analyse'!B38,"=", 'Commencer analyse'!C38),IF('Commencer analyse'!C38&lt;&gt;"",'Commencer analyse'!C38,""))</f>
         <v/>
       </c>
     </row>
     <row r="579" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A579" t="str">
-        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE('Commencer analyse'!B42,"=", 'Commencer analyse'!C42),IF('Commencer analyse'!C42&lt;&gt;"",'Commencer analyse'!C42,""))</f>
+        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE('Commencer analyse'!B39,"=", 'Commencer analyse'!C39),IF('Commencer analyse'!C39&lt;&gt;"",'Commencer analyse'!C39,""))</f>
         <v/>
       </c>
     </row>
     <row r="580" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A580" t="str">
-        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE('Commencer analyse'!B43,"=", 'Commencer analyse'!C43),IF('Commencer analyse'!C43&lt;&gt;"",'Commencer analyse'!C43,""))</f>
+        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE('Commencer analyse'!B40,"=", 'Commencer analyse'!C40),IF('Commencer analyse'!C40&lt;&gt;"",'Commencer analyse'!C40,""))</f>
         <v/>
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A581" t="str">
-        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE('Commencer analyse'!B44,"=", 'Commencer analyse'!C44),IF('Commencer analyse'!C44&lt;&gt;"",'Commencer analyse'!C44,""))</f>
+        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE('Commencer analyse'!B41,"=", 'Commencer analyse'!C41),IF('Commencer analyse'!C41&lt;&gt;"",'Commencer analyse'!C41,""))</f>
         <v/>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A582" t="str">
-        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE('Commencer analyse'!B45,"=", 'Commencer analyse'!C45),IF('Commencer analyse'!C45&lt;&gt;"",'Commencer analyse'!C45,""))</f>
+        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE('Commencer analyse'!B42,"=", 'Commencer analyse'!C42),IF('Commencer analyse'!C42&lt;&gt;"",'Commencer analyse'!C42,""))</f>
         <v/>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A583" t="str">
-        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE('Commencer analyse'!B46,"=", 'Commencer analyse'!C46),IF('Commencer analyse'!C46&lt;&gt;"",'Commencer analyse'!C46,""))</f>
+        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE('Commencer analyse'!B43,"=", 'Commencer analyse'!C43),IF('Commencer analyse'!C43&lt;&gt;"",'Commencer analyse'!C43,""))</f>
         <v/>
       </c>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A584" t="str">
-        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE('Commencer analyse'!B47,"=", 'Commencer analyse'!C47),IF('Commencer analyse'!C47&lt;&gt;"",'Commencer analyse'!C47,""))</f>
+        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE('Commencer analyse'!B44,"=", 'Commencer analyse'!C44),IF('Commencer analyse'!C44&lt;&gt;"",'Commencer analyse'!C44,""))</f>
         <v/>
       </c>
     </row>
     <row r="585" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A585" t="str">
-        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE('Commencer analyse'!B48,"=", 'Commencer analyse'!C48),IF('Commencer analyse'!C48&lt;&gt;"",'Commencer analyse'!C48,""))</f>
+        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE('Commencer analyse'!B45,"=", 'Commencer analyse'!C45),IF('Commencer analyse'!C45&lt;&gt;"",'Commencer analyse'!C45,""))</f>
         <v/>
       </c>
     </row>
     <row r="586" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A586" t="str">
-        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE('Commencer analyse'!B49,"=", 'Commencer analyse'!C49),IF('Commencer analyse'!C49&lt;&gt;"",'Commencer analyse'!C49,""))</f>
+        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE('Commencer analyse'!B46,"=", 'Commencer analyse'!C46),IF('Commencer analyse'!C46&lt;&gt;"",'Commencer analyse'!C46,""))</f>
         <v/>
       </c>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A587" t="str">
-        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE('Commencer analyse'!B50,"=", 'Commencer analyse'!C50),IF('Commencer analyse'!C50&lt;&gt;"",'Commencer analyse'!C50,""))</f>
+        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE('Commencer analyse'!B47,"=", 'Commencer analyse'!C47),IF('Commencer analyse'!C47&lt;&gt;"",'Commencer analyse'!C47,""))</f>
         <v/>
       </c>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A588" t="str">
-        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE('Commencer analyse'!B51,"=", 'Commencer analyse'!C51),IF('Commencer analyse'!C51&lt;&gt;"",'Commencer analyse'!C51,""))</f>
+        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE('Commencer analyse'!B48,"=", 'Commencer analyse'!C48),IF('Commencer analyse'!C48&lt;&gt;"",'Commencer analyse'!C48,""))</f>
         <v/>
       </c>
     </row>
     <row r="589" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A589" t="str">
-        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE('Commencer analyse'!B52,"=", 'Commencer analyse'!C52),IF('Commencer analyse'!C52&lt;&gt;"",'Commencer analyse'!C52,""))</f>
+        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE('Commencer analyse'!B49,"=", 'Commencer analyse'!C49),IF('Commencer analyse'!C49&lt;&gt;"",'Commencer analyse'!C49,""))</f>
         <v/>
       </c>
     </row>
     <row r="590" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A590" t="str">
-        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE('Commencer analyse'!B53,"=", 'Commencer analyse'!C53),IF('Commencer analyse'!C53&lt;&gt;"",'Commencer analyse'!C53,""))</f>
+        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE('Commencer analyse'!B50,"=", 'Commencer analyse'!C50),IF('Commencer analyse'!C50&lt;&gt;"",'Commencer analyse'!C50,""))</f>
         <v/>
       </c>
     </row>
     <row r="591" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A591" t="str">
-        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE('Commencer analyse'!B54,"=", 'Commencer analyse'!C54),IF('Commencer analyse'!C54&lt;&gt;"",'Commencer analyse'!C54,""))</f>
+        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE('Commencer analyse'!B51,"=", 'Commencer analyse'!C51),IF('Commencer analyse'!C51&lt;&gt;"",'Commencer analyse'!C51,""))</f>
         <v/>
       </c>
     </row>
     <row r="592" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A592" t="str">
-        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE('Commencer analyse'!B55,"=", 'Commencer analyse'!C55),IF('Commencer analyse'!C55&lt;&gt;"",'Commencer analyse'!C55,""))</f>
+        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE('Commencer analyse'!B52,"=", 'Commencer analyse'!C52),IF('Commencer analyse'!C52&lt;&gt;"",'Commencer analyse'!C52,""))</f>
         <v/>
       </c>
     </row>
     <row r="593" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A593" t="str">
-        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE('Commencer analyse'!B56,"=", 'Commencer analyse'!C56),IF('Commencer analyse'!C56&lt;&gt;"",'Commencer analyse'!C56,""))</f>
+        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE('Commencer analyse'!B53,"=", 'Commencer analyse'!C53),IF('Commencer analyse'!C53&lt;&gt;"",'Commencer analyse'!C53,""))</f>
         <v/>
       </c>
     </row>
     <row r="594" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A594" t="str">
-        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE('Commencer analyse'!B57,"=", 'Commencer analyse'!C57),IF('Commencer analyse'!C57&lt;&gt;"",'Commencer analyse'!C57,""))</f>
+        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE('Commencer analyse'!B54,"=", 'Commencer analyse'!C54),IF('Commencer analyse'!C54&lt;&gt;"",'Commencer analyse'!C54,""))</f>
         <v/>
       </c>
     </row>
     <row r="595" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A595" t="str">
-        <f>IF('Commencer analyse'!B58&lt;&gt;"",CONCATENATE('Commencer analyse'!B58,"=", 'Commencer analyse'!C58),IF('Commencer analyse'!C58&lt;&gt;"",'Commencer analyse'!C58,""))</f>
+        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE('Commencer analyse'!B55,"=", 'Commencer analyse'!C55),IF('Commencer analyse'!C55&lt;&gt;"",'Commencer analyse'!C55,""))</f>
         <v/>
       </c>
     </row>
     <row r="596" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A596" t="str">
-        <f>IF('Commencer analyse'!B59&lt;&gt;"",CONCATENATE('Commencer analyse'!B59,"=", 'Commencer analyse'!C59),IF('Commencer analyse'!C59&lt;&gt;"",'Commencer analyse'!C59,""))</f>
+        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE('Commencer analyse'!B56,"=", 'Commencer analyse'!C56),IF('Commencer analyse'!C56&lt;&gt;"",'Commencer analyse'!C56,""))</f>
         <v/>
       </c>
     </row>
     <row r="597" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A597" t="str">
-        <f>IF('Commencer analyse'!B60&lt;&gt;"",CONCATENATE('Commencer analyse'!B60,"=", 'Commencer analyse'!C60),IF('Commencer analyse'!C60&lt;&gt;"",'Commencer analyse'!C60,""))</f>
+        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE('Commencer analyse'!B57,"=", 'Commencer analyse'!C57),IF('Commencer analyse'!C57&lt;&gt;"",'Commencer analyse'!C57,""))</f>
         <v/>
       </c>
     </row>
@@ -34876,8 +35225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
   <dimension ref="A1:A771"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A740" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A759" sqref="A1:A771"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A1:A771"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35224,13 +35573,13 @@
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>IF('Fenêtre principal'!B58&lt;&gt;"",CONCATENATE('Fenêtre principal'!B58,"=", 'Fenêtre principal'!D58),IF('Fenêtre principal'!D58&lt;&gt;"",'Fenêtre principal'!D58,""))</f>
-        <v>window.menu.level6.sublevel3.sublevel2.title=Radicales</v>
+        <v>window.menu.level6.sublevel3.sublevel2.title=Lemas</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>IF('Fenêtre principal'!B59&lt;&gt;"",CONCATENATE('Fenêtre principal'!B59,"=", 'Fenêtre principal'!D59),IF('Fenêtre principal'!D59&lt;&gt;"",'Fenêtre principal'!D59,""))</f>
-        <v>window.menu.level6.sublevel3.sublevel3.title=Radicales por clase</v>
+        <v>window.menu.level6.sublevel3.sublevel3.title=Lemas por clase</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
@@ -38120,326 +38469,326 @@
       </c>
     </row>
     <row r="540" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A540" t="str">
-        <f>IF('Commencer analyse'!B7&lt;&gt;"",CONCATENATE('Commencer analyse'!B7,"=", 'Commencer analyse'!D7),IF('Commencer analyse'!D7&lt;&gt;"",'Commencer analyse'!D7,""))</f>
-        <v/>
+      <c r="A540" t="e">
+        <f>IF('Commencer analyse'!#REF!&lt;&gt;"",CONCATENATE('Commencer analyse'!#REF!,"=", 'Commencer analyse'!#REF!),IF('Commencer analyse'!#REF!&lt;&gt;"",'Commencer analyse'!#REF!,""))</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="541" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A541" t="str">
-        <f>IF('Commencer analyse'!B8&lt;&gt;"",CONCATENATE('Commencer analyse'!B8,"=", 'Commencer analyse'!D8),IF('Commencer analyse'!D8&lt;&gt;"",'Commencer analyse'!D8,""))</f>
-        <v/>
+      <c r="A541" t="e">
+        <f>IF('Commencer analyse'!#REF!&lt;&gt;"",CONCATENATE('Commencer analyse'!#REF!,"=", 'Commencer analyse'!#REF!),IF('Commencer analyse'!#REF!&lt;&gt;"",'Commencer analyse'!#REF!,""))</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="542" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A542" t="str">
-        <f>IF('Commencer analyse'!B9&lt;&gt;"",CONCATENATE('Commencer analyse'!B9,"=", 'Commencer analyse'!D9),IF('Commencer analyse'!D9&lt;&gt;"",'Commencer analyse'!D9,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B7&lt;&gt;"",CONCATENATE('Commencer analyse'!B7,"=", 'Commencer analyse'!D7),IF('Commencer analyse'!D7&lt;&gt;"",'Commencer analyse'!D7,""))</f>
+        <v>window.start.analysis.information.message.etape2=&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar los materiales en los que desea realizar el análisis.&lt;BR/&gt;NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="543" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A543" t="str">
-        <f>IF('Commencer analyse'!B10&lt;&gt;"",CONCATENATE('Commencer analyse'!B10,"=", 'Commencer analyse'!D10),IF('Commencer analyse'!D10&lt;&gt;"",'Commencer analyse'!D10,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B8&lt;&gt;"",CONCATENATE('Commencer analyse'!B8,"=", 'Commencer analyse'!D8),IF('Commencer analyse'!D8&lt;&gt;"",'Commencer analyse'!D8,""))</f>
+        <v>window.start.analysis.type.panel.title=Elección de análisis</v>
       </c>
     </row>
     <row r="544" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A544" t="str">
-        <f>IF('Commencer analyse'!B11&lt;&gt;"",CONCATENATE('Commencer analyse'!B11,"=", 'Commencer analyse'!D11),IF('Commencer analyse'!D11&lt;&gt;"",'Commencer analyse'!D11,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B9&lt;&gt;"",CONCATENATE('Commencer analyse'!B9,"=", 'Commencer analyse'!D9),IF('Commencer analyse'!D9&lt;&gt;"",'Commencer analyse'!D9,""))</f>
+        <v>window.start.analysis.information.message.etape3=&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar los campos correspondientes a los materiales sobre los que desea realizar el análisis.&lt;BR/&gt;NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="545" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A545" t="str">
-        <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE('Commencer analyse'!B12,"=", 'Commencer analyse'!D12),IF('Commencer analyse'!D12&lt;&gt;"",'Commencer analyse'!D12,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B10&lt;&gt;"",CONCATENATE('Commencer analyse'!B10,"=", 'Commencer analyse'!D10),IF('Commencer analyse'!D10&lt;&gt;"",'Commencer analyse'!D10,""))</f>
+        <v>window.start.analysis.field.material.panel.title=Choix des champs à analyser</v>
       </c>
     </row>
     <row r="546" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A546" t="str">
-        <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE('Commencer analyse'!B13,"=", 'Commencer analyse'!D13),IF('Commencer analyse'!D13&lt;&gt;"",'Commencer analyse'!D13,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B11&lt;&gt;"",CONCATENATE('Commencer analyse'!B11,"=", 'Commencer analyse'!D11),IF('Commencer analyse'!D11&lt;&gt;"",'Commencer analyse'!D11,""))</f>
+        <v>window.start.analysis.information.message.etape4=&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar el tipo de análisis que desea realizar.&lt;BR/&gt;Luego consulte los resultados.&lt;BR/&gt;NB: En cualquier momento puede volver con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="547" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A547" t="str">
-        <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE('Commencer analyse'!B14,"=", 'Commencer analyse'!D14),IF('Commencer analyse'!D14&lt;&gt;"",'Commencer analyse'!D14,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE('Commencer analyse'!B12,"=", 'Commencer analyse'!D12),IF('Commencer analyse'!D12&lt;&gt;"",'Commencer analyse'!D12,""))</f>
+        <v>window.start.analysis.choose.analyse.label=Elección de análisis</v>
       </c>
     </row>
     <row r="548" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A548" t="str">
-        <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE('Commencer analyse'!B15,"=", 'Commencer analyse'!D15),IF('Commencer analyse'!D15&lt;&gt;"",'Commencer analyse'!D15,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE('Commencer analyse'!B13,"=", 'Commencer analyse'!D13),IF('Commencer analyse'!D13&lt;&gt;"",'Commencer analyse'!D13,""))</f>
+        <v>window.start.analysis.choose.analyse.panel.title=Análisis lexicométrico</v>
       </c>
     </row>
     <row r="549" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A549" t="str">
-        <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE('Commencer analyse'!B16,"=", 'Commencer analyse'!D16),IF('Commencer analyse'!D16&lt;&gt;"",'Commencer analyse'!D16,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE('Commencer analyse'!B14,"=", 'Commencer analyse'!D14),IF('Commencer analyse'!D14&lt;&gt;"",'Commencer analyse'!D14,""))</f>
+        <v>window.start.analysis.choose.analyse.option.panel.title=Opciones disponibles/requeridas para el análisis</v>
       </c>
     </row>
     <row r="550" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A550" t="str">
-        <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE('Commencer analyse'!B17,"=", 'Commencer analyse'!D17),IF('Commencer analyse'!D17&lt;&gt;"",'Commencer analyse'!D17,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE('Commencer analyse'!B15,"=", 'Commencer analyse'!D15),IF('Commencer analyse'!D15&lt;&gt;"",'Commencer analyse'!D15,""))</f>
+        <v>window.start.analysis.start.button.label=Iniciar el análisis</v>
       </c>
     </row>
     <row r="551" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A551" t="str">
-        <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE('Commencer analyse'!B18,"=", 'Commencer analyse'!D18),IF('Commencer analyse'!D18&lt;&gt;"",'Commencer analyse'!D18,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE('Commencer analyse'!B16,"=", 'Commencer analyse'!D16),IF('Commencer analyse'!D16&lt;&gt;"",'Commencer analyse'!D16,""))</f>
+        <v>window.start.analysis.consult.results.button.label=Consultar los resultados</v>
       </c>
     </row>
     <row r="552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A552" t="str">
-        <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE('Commencer analyse'!B19,"=", 'Commencer analyse'!D19),IF('Commencer analyse'!D19&lt;&gt;"",'Commencer analyse'!D19,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE('Commencer analyse'!B17,"=", 'Commencer analyse'!D17),IF('Commencer analyse'!D17&lt;&gt;"",'Commencer analyse'!D17,""))</f>
+        <v>window.start.analysis.token.number.label=Numero de tokens</v>
       </c>
     </row>
     <row r="553" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A553" t="str">
-        <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE('Commencer analyse'!B20,"=", 'Commencer analyse'!D20),IF('Commencer analyse'!D20&lt;&gt;"",'Commencer analyse'!D20,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE('Commencer analyse'!B18,"=", 'Commencer analyse'!D18),IF('Commencer analyse'!D18&lt;&gt;"",'Commencer analyse'!D18,""))</f>
+        <v>window.start.analysis.lemme.type.label=Lematización y número de tipo</v>
       </c>
     </row>
     <row r="554" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A554" t="str">
-        <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE('Commencer analyse'!B21,"=", 'Commencer analyse'!D21),IF('Commencer analyse'!D21&lt;&gt;"",'Commencer analyse'!D21,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE('Commencer analyse'!B19,"=", 'Commencer analyse'!D19),IF('Commencer analyse'!D19&lt;&gt;"",'Commencer analyse'!D19,""))</f>
+        <v>window.start.analysis.token.ratio.label=Tipo de proporción de tokens</v>
       </c>
     </row>
     <row r="555" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A555" t="str">
-        <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE('Commencer analyse'!B22,"=", 'Commencer analyse'!D22),IF('Commencer analyse'!D22&lt;&gt;"",'Commencer analyse'!D22,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE('Commencer analyse'!B20,"=", 'Commencer analyse'!D20),IF('Commencer analyse'!D20&lt;&gt;"",'Commencer analyse'!D20,""))</f>
+        <v>window.start.analysis.frequency.label=Frecuencia</v>
       </c>
     </row>
     <row r="556" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A556" t="str">
-        <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE('Commencer analyse'!B23,"=", 'Commencer analyse'!D23),IF('Commencer analyse'!D23&lt;&gt;"",'Commencer analyse'!D23,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE('Commencer analyse'!B21,"=", 'Commencer analyse'!D21),IF('Commencer analyse'!D21&lt;&gt;"",'Commencer analyse'!D21,""))</f>
+        <v>window.start.analysis.choose.type.treatment.optional.list.panel.title=Tipo de preprocesamiento de datos</v>
       </c>
     </row>
     <row r="557" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A557" t="str">
-        <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE('Commencer analyse'!B24,"=", 'Commencer analyse'!D24),IF('Commencer analyse'!D24&lt;&gt;"",'Commencer analyse'!D24,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE('Commencer analyse'!B22,"=", 'Commencer analyse'!D22),IF('Commencer analyse'!D22&lt;&gt;"",'Commencer analyse'!D22,""))</f>
+        <v>window.start.analysis.choose.profile.treatment.optional.list.panel.title=Modelo de pretratamiento de datos</v>
       </c>
     </row>
     <row r="558" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A558" t="str">
-        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE('Commencer analyse'!B25,"=", 'Commencer analyse'!D25),IF('Commencer analyse'!D25&lt;&gt;"",'Commencer analyse'!D25,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE('Commencer analyse'!B23,"=", 'Commencer analyse'!D23),IF('Commencer analyse'!D23&lt;&gt;"",'Commencer analyse'!D23,""))</f>
+        <v xml:space="preserve">window.start.analysis.choose.type.treatment.optional.list.label=Elegir el tipo de lista </v>
       </c>
     </row>
     <row r="559" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A559" t="str">
-        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE('Commencer analyse'!B26,"=", 'Commencer analyse'!D26),IF('Commencer analyse'!D26&lt;&gt;"",'Commencer analyse'!D26,""))</f>
-        <v/>
+        <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE('Commencer analyse'!B24,"=", 'Commencer analyse'!D24),IF('Commencer analyse'!D24&lt;&gt;"",'Commencer analyse'!D24,""))</f>
+        <v>window.start.analysis.choose.profile.treatment.optional.list.label=Elegir qué lista usar</v>
       </c>
     </row>
     <row r="560" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A560" t="str">
-        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE('Commencer analyse'!B27,"=", 'Commencer analyse'!D27),IF('Commencer analyse'!D27&lt;&gt;"",'Commencer analyse'!D27,""))</f>
-        <v/>
+      <c r="A560" t="e">
+        <f>IF('Commencer analyse'!#REF!&lt;&gt;"",CONCATENATE('Commencer analyse'!#REF!,"=", 'Commencer analyse'!#REF!),IF('Commencer analyse'!#REF!&lt;&gt;"",'Commencer analyse'!#REF!,""))</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="561" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A561" t="str">
-        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE('Commencer analyse'!B28,"=", 'Commencer analyse'!D28),IF('Commencer analyse'!D28&lt;&gt;"",'Commencer analyse'!D28,""))</f>
+        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE('Commencer analyse'!B25,"=", 'Commencer analyse'!D25),IF('Commencer analyse'!D25&lt;&gt;"",'Commencer analyse'!D25,""))</f>
         <v/>
       </c>
     </row>
     <row r="562" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A562" t="str">
-        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE('Commencer analyse'!B29,"=", 'Commencer analyse'!D29),IF('Commencer analyse'!D29&lt;&gt;"",'Commencer analyse'!D29,""))</f>
+        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE('Commencer analyse'!B26,"=", 'Commencer analyse'!D26),IF('Commencer analyse'!D26&lt;&gt;"",'Commencer analyse'!D26,""))</f>
         <v/>
       </c>
     </row>
     <row r="563" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A563" t="str">
-        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE('Commencer analyse'!B30,"=", 'Commencer analyse'!D30),IF('Commencer analyse'!D30&lt;&gt;"",'Commencer analyse'!D30,""))</f>
+        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE('Commencer analyse'!B27,"=", 'Commencer analyse'!D27),IF('Commencer analyse'!D27&lt;&gt;"",'Commencer analyse'!D27,""))</f>
         <v/>
       </c>
     </row>
     <row r="564" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A564" t="str">
-        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE('Commencer analyse'!B31,"=", 'Commencer analyse'!D31),IF('Commencer analyse'!D31&lt;&gt;"",'Commencer analyse'!D31,""))</f>
+        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE('Commencer analyse'!B28,"=", 'Commencer analyse'!D28),IF('Commencer analyse'!D28&lt;&gt;"",'Commencer analyse'!D28,""))</f>
         <v/>
       </c>
     </row>
     <row r="565" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A565" t="str">
-        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE('Commencer analyse'!B32,"=", 'Commencer analyse'!D32),IF('Commencer analyse'!D32&lt;&gt;"",'Commencer analyse'!D32,""))</f>
+        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE('Commencer analyse'!B29,"=", 'Commencer analyse'!D29),IF('Commencer analyse'!D29&lt;&gt;"",'Commencer analyse'!D29,""))</f>
         <v/>
       </c>
     </row>
     <row r="566" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A566" t="str">
-        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE('Commencer analyse'!B33,"=", 'Commencer analyse'!D33),IF('Commencer analyse'!D33&lt;&gt;"",'Commencer analyse'!D33,""))</f>
+        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE('Commencer analyse'!B30,"=", 'Commencer analyse'!D30),IF('Commencer analyse'!D30&lt;&gt;"",'Commencer analyse'!D30,""))</f>
         <v/>
       </c>
     </row>
     <row r="567" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A567" t="str">
-        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE('Commencer analyse'!B34,"=", 'Commencer analyse'!D34),IF('Commencer analyse'!D34&lt;&gt;"",'Commencer analyse'!D34,""))</f>
+        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE('Commencer analyse'!B31,"=", 'Commencer analyse'!D31),IF('Commencer analyse'!D31&lt;&gt;"",'Commencer analyse'!D31,""))</f>
         <v/>
       </c>
     </row>
     <row r="568" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A568" t="str">
-        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE('Commencer analyse'!B35,"=", 'Commencer analyse'!D35),IF('Commencer analyse'!D35&lt;&gt;"",'Commencer analyse'!D35,""))</f>
+        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE('Commencer analyse'!B32,"=", 'Commencer analyse'!D32),IF('Commencer analyse'!D32&lt;&gt;"",'Commencer analyse'!D32,""))</f>
         <v/>
       </c>
     </row>
     <row r="569" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A569" t="str">
-        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE('Commencer analyse'!B36,"=", 'Commencer analyse'!D36),IF('Commencer analyse'!D36&lt;&gt;"",'Commencer analyse'!D36,""))</f>
+        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE('Commencer analyse'!B33,"=", 'Commencer analyse'!D33),IF('Commencer analyse'!D33&lt;&gt;"",'Commencer analyse'!D33,""))</f>
         <v/>
       </c>
     </row>
     <row r="570" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A570" t="str">
-        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE('Commencer analyse'!B37,"=", 'Commencer analyse'!D37),IF('Commencer analyse'!D37&lt;&gt;"",'Commencer analyse'!D37,""))</f>
+        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE('Commencer analyse'!B34,"=", 'Commencer analyse'!D34),IF('Commencer analyse'!D34&lt;&gt;"",'Commencer analyse'!D34,""))</f>
         <v/>
       </c>
     </row>
     <row r="571" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A571" t="str">
-        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE('Commencer analyse'!B38,"=", 'Commencer analyse'!D38),IF('Commencer analyse'!D38&lt;&gt;"",'Commencer analyse'!D38,""))</f>
+        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE('Commencer analyse'!B35,"=", 'Commencer analyse'!D35),IF('Commencer analyse'!D35&lt;&gt;"",'Commencer analyse'!D35,""))</f>
         <v/>
       </c>
     </row>
     <row r="572" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A572" t="str">
-        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE('Commencer analyse'!B39,"=", 'Commencer analyse'!D39),IF('Commencer analyse'!D39&lt;&gt;"",'Commencer analyse'!D39,""))</f>
+        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE('Commencer analyse'!B36,"=", 'Commencer analyse'!D36),IF('Commencer analyse'!D36&lt;&gt;"",'Commencer analyse'!D36,""))</f>
         <v/>
       </c>
     </row>
     <row r="573" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A573" t="str">
-        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE('Commencer analyse'!B40,"=", 'Commencer analyse'!D40),IF('Commencer analyse'!D40&lt;&gt;"",'Commencer analyse'!D40,""))</f>
+        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE('Commencer analyse'!B37,"=", 'Commencer analyse'!D37),IF('Commencer analyse'!D37&lt;&gt;"",'Commencer analyse'!D37,""))</f>
         <v/>
       </c>
     </row>
     <row r="574" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A574" t="str">
-        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE('Commencer analyse'!B41,"=", 'Commencer analyse'!D41),IF('Commencer analyse'!D41&lt;&gt;"",'Commencer analyse'!D41,""))</f>
+        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE('Commencer analyse'!B38,"=", 'Commencer analyse'!D38),IF('Commencer analyse'!D38&lt;&gt;"",'Commencer analyse'!D38,""))</f>
         <v/>
       </c>
     </row>
     <row r="575" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A575" t="str">
-        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE('Commencer analyse'!B42,"=", 'Commencer analyse'!D42),IF('Commencer analyse'!D42&lt;&gt;"",'Commencer analyse'!D42,""))</f>
+        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE('Commencer analyse'!B39,"=", 'Commencer analyse'!D39),IF('Commencer analyse'!D39&lt;&gt;"",'Commencer analyse'!D39,""))</f>
         <v/>
       </c>
     </row>
     <row r="576" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A576" t="str">
-        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE('Commencer analyse'!B43,"=", 'Commencer analyse'!D43),IF('Commencer analyse'!D43&lt;&gt;"",'Commencer analyse'!D43,""))</f>
+        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE('Commencer analyse'!B40,"=", 'Commencer analyse'!D40),IF('Commencer analyse'!D40&lt;&gt;"",'Commencer analyse'!D40,""))</f>
         <v/>
       </c>
     </row>
     <row r="577" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A577" t="str">
-        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE('Commencer analyse'!B44,"=", 'Commencer analyse'!D44),IF('Commencer analyse'!D44&lt;&gt;"",'Commencer analyse'!D44,""))</f>
+        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE('Commencer analyse'!B41,"=", 'Commencer analyse'!D41),IF('Commencer analyse'!D41&lt;&gt;"",'Commencer analyse'!D41,""))</f>
         <v/>
       </c>
     </row>
     <row r="578" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A578" t="str">
-        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE('Commencer analyse'!B45,"=", 'Commencer analyse'!D45),IF('Commencer analyse'!D45&lt;&gt;"",'Commencer analyse'!D45,""))</f>
+        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE('Commencer analyse'!B42,"=", 'Commencer analyse'!D42),IF('Commencer analyse'!D42&lt;&gt;"",'Commencer analyse'!D42,""))</f>
         <v/>
       </c>
     </row>
     <row r="579" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A579" t="str">
-        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE('Commencer analyse'!B46,"=", 'Commencer analyse'!D46),IF('Commencer analyse'!D46&lt;&gt;"",'Commencer analyse'!D46,""))</f>
+        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE('Commencer analyse'!B43,"=", 'Commencer analyse'!D43),IF('Commencer analyse'!D43&lt;&gt;"",'Commencer analyse'!D43,""))</f>
         <v/>
       </c>
     </row>
     <row r="580" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A580" t="str">
-        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE('Commencer analyse'!B47,"=", 'Commencer analyse'!D47),IF('Commencer analyse'!D47&lt;&gt;"",'Commencer analyse'!D47,""))</f>
+        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE('Commencer analyse'!B44,"=", 'Commencer analyse'!D44),IF('Commencer analyse'!D44&lt;&gt;"",'Commencer analyse'!D44,""))</f>
         <v/>
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A581" t="str">
-        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE('Commencer analyse'!B48,"=", 'Commencer analyse'!D48),IF('Commencer analyse'!D48&lt;&gt;"",'Commencer analyse'!D48,""))</f>
+        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE('Commencer analyse'!B45,"=", 'Commencer analyse'!D45),IF('Commencer analyse'!D45&lt;&gt;"",'Commencer analyse'!D45,""))</f>
         <v/>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A582" t="str">
-        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE('Commencer analyse'!B49,"=", 'Commencer analyse'!D49),IF('Commencer analyse'!D49&lt;&gt;"",'Commencer analyse'!D49,""))</f>
+        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE('Commencer analyse'!B46,"=", 'Commencer analyse'!D46),IF('Commencer analyse'!D46&lt;&gt;"",'Commencer analyse'!D46,""))</f>
         <v/>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A583" t="str">
-        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE('Commencer analyse'!B50,"=", 'Commencer analyse'!D50),IF('Commencer analyse'!D50&lt;&gt;"",'Commencer analyse'!D50,""))</f>
+        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE('Commencer analyse'!B47,"=", 'Commencer analyse'!D47),IF('Commencer analyse'!D47&lt;&gt;"",'Commencer analyse'!D47,""))</f>
         <v/>
       </c>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A584" t="str">
-        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE('Commencer analyse'!B51,"=", 'Commencer analyse'!D51),IF('Commencer analyse'!D51&lt;&gt;"",'Commencer analyse'!D51,""))</f>
+        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE('Commencer analyse'!B48,"=", 'Commencer analyse'!D48),IF('Commencer analyse'!D48&lt;&gt;"",'Commencer analyse'!D48,""))</f>
         <v/>
       </c>
     </row>
     <row r="585" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A585" t="str">
-        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE('Commencer analyse'!B52,"=", 'Commencer analyse'!D52),IF('Commencer analyse'!D52&lt;&gt;"",'Commencer analyse'!D52,""))</f>
+        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE('Commencer analyse'!B49,"=", 'Commencer analyse'!D49),IF('Commencer analyse'!D49&lt;&gt;"",'Commencer analyse'!D49,""))</f>
         <v/>
       </c>
     </row>
     <row r="586" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A586" t="str">
-        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE('Commencer analyse'!B53,"=", 'Commencer analyse'!D53),IF('Commencer analyse'!D53&lt;&gt;"",'Commencer analyse'!D53,""))</f>
+        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE('Commencer analyse'!B50,"=", 'Commencer analyse'!D50),IF('Commencer analyse'!D50&lt;&gt;"",'Commencer analyse'!D50,""))</f>
         <v/>
       </c>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A587" t="str">
-        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE('Commencer analyse'!B54,"=", 'Commencer analyse'!D54),IF('Commencer analyse'!D54&lt;&gt;"",'Commencer analyse'!D54,""))</f>
+        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE('Commencer analyse'!B51,"=", 'Commencer analyse'!D51),IF('Commencer analyse'!D51&lt;&gt;"",'Commencer analyse'!D51,""))</f>
         <v/>
       </c>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A588" t="str">
-        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE('Commencer analyse'!B55,"=", 'Commencer analyse'!D55),IF('Commencer analyse'!D55&lt;&gt;"",'Commencer analyse'!D55,""))</f>
+        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE('Commencer analyse'!B52,"=", 'Commencer analyse'!D52),IF('Commencer analyse'!D52&lt;&gt;"",'Commencer analyse'!D52,""))</f>
         <v/>
       </c>
     </row>
     <row r="589" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A589" t="str">
-        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE('Commencer analyse'!B56,"=", 'Commencer analyse'!D56),IF('Commencer analyse'!D56&lt;&gt;"",'Commencer analyse'!D56,""))</f>
+        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE('Commencer analyse'!B53,"=", 'Commencer analyse'!D53),IF('Commencer analyse'!D53&lt;&gt;"",'Commencer analyse'!D53,""))</f>
         <v/>
       </c>
     </row>
     <row r="590" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A590" t="str">
-        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE('Commencer analyse'!B57,"=", 'Commencer analyse'!D57),IF('Commencer analyse'!D57&lt;&gt;"",'Commencer analyse'!D57,""))</f>
+        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE('Commencer analyse'!B54,"=", 'Commencer analyse'!D54),IF('Commencer analyse'!D54&lt;&gt;"",'Commencer analyse'!D54,""))</f>
         <v/>
       </c>
     </row>
     <row r="591" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A591" t="str">
-        <f>IF('Commencer analyse'!B58&lt;&gt;"",CONCATENATE('Commencer analyse'!B58,"=", 'Commencer analyse'!D58),IF('Commencer analyse'!D58&lt;&gt;"",'Commencer analyse'!D58,""))</f>
+        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE('Commencer analyse'!B55,"=", 'Commencer analyse'!D55),IF('Commencer analyse'!D55&lt;&gt;"",'Commencer analyse'!D55,""))</f>
         <v/>
       </c>
     </row>
     <row r="592" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A592" t="str">
-        <f>IF('Commencer analyse'!B59&lt;&gt;"",CONCATENATE('Commencer analyse'!B59,"=", 'Commencer analyse'!D59),IF('Commencer analyse'!D59&lt;&gt;"",'Commencer analyse'!D59,""))</f>
+        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE('Commencer analyse'!B56,"=", 'Commencer analyse'!D56),IF('Commencer analyse'!D56&lt;&gt;"",'Commencer analyse'!D56,""))</f>
         <v/>
       </c>
     </row>
     <row r="593" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A593" t="str">
-        <f>IF('Commencer analyse'!B60&lt;&gt;"",CONCATENATE('Commencer analyse'!B60,"=", 'Commencer analyse'!D60),IF('Commencer analyse'!D60&lt;&gt;"",'Commencer analyse'!D60,""))</f>
+        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE('Commencer analyse'!B57,"=", 'Commencer analyse'!D57),IF('Commencer analyse'!D57&lt;&gt;"",'Commencer analyse'!D57,""))</f>
         <v/>
       </c>
     </row>
@@ -39519,10 +39868,10 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
-  <dimension ref="A1:A739"/>
+  <dimension ref="A1:A737"/>
   <sheetViews>
-    <sheetView topLeftCell="A709" workbookViewId="0">
-      <selection activeCell="A737" sqref="A737:A738"/>
+    <sheetView topLeftCell="A529" workbookViewId="0">
+      <selection activeCell="A550" sqref="A550:A553"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42743,1223 +43092,1211 @@
     <row r="536" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A536" t="str">
         <f>IF('Commencer analyse'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B7),".","_"),"=""", 'Commencer analyse'!B7,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_INFORMATION_MESSAGE_ETAPE2="window.start.analysis.information.message.etape2";</v>
       </c>
     </row>
     <row r="537" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A537" t="str">
         <f>IF('Commencer analyse'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B8),".","_"),"=""", 'Commencer analyse'!B8,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_TYPE_PANEL_TITLE="window.start.analysis.type.panel.title";</v>
       </c>
     </row>
     <row r="538" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A538" t="str">
         <f>IF('Commencer analyse'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B9),".","_"),"=""", 'Commencer analyse'!B9,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_INFORMATION_MESSAGE_ETAPE3="window.start.analysis.information.message.etape3";</v>
       </c>
     </row>
     <row r="539" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A539" t="str">
         <f>IF('Commencer analyse'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B10),".","_"),"=""", 'Commencer analyse'!B10,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_FIELD_MATERIAL_PANEL_TITLE="window.start.analysis.field.material.panel.title";</v>
       </c>
     </row>
     <row r="540" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A540" t="str">
         <f>IF('Commencer analyse'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B11),".","_"),"=""", 'Commencer analyse'!B11,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_INFORMATION_MESSAGE_ETAPE4="window.start.analysis.information.message.etape4";</v>
       </c>
     </row>
     <row r="541" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A541" t="str">
         <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B12),".","_"),"=""", 'Commencer analyse'!B12,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_CHOOSE_ANALYSE_LABEL="window.start.analysis.choose.analyse.label";</v>
       </c>
     </row>
     <row r="542" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A542" t="str">
         <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B13),".","_"),"=""", 'Commencer analyse'!B13,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_CHOOSE_ANALYSE_PANEL_TITLE="window.start.analysis.choose.analyse.panel.title";</v>
       </c>
     </row>
     <row r="543" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A543" t="str">
         <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B14),".","_"),"=""", 'Commencer analyse'!B14,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_CHOOSE_ANALYSE_OPTION_PANEL_TITLE="window.start.analysis.choose.analyse.option.panel.title";</v>
       </c>
     </row>
     <row r="544" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A544" t="str">
         <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B15),".","_"),"=""", 'Commencer analyse'!B15,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_START_BUTTON_LABEL="window.start.analysis.start.button.label";</v>
       </c>
     </row>
     <row r="545" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A545" t="str">
         <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B16),".","_"),"=""", 'Commencer analyse'!B16,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_CONSULT_RESULTS_BUTTON_LABEL="window.start.analysis.consult.results.button.label";</v>
       </c>
     </row>
     <row r="546" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A546" t="str">
         <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B17),".","_"),"=""", 'Commencer analyse'!B17,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_TOKEN_NUMBER_LABEL="window.start.analysis.token.number.label";</v>
       </c>
     </row>
     <row r="547" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A547" t="str">
         <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B18),".","_"),"=""", 'Commencer analyse'!B18,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_LEMME_TYPE_LABEL="window.start.analysis.lemme.type.label";</v>
       </c>
     </row>
     <row r="548" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A548" t="str">
         <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B19),".","_"),"=""", 'Commencer analyse'!B19,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_TOKEN_RATIO_LABEL="window.start.analysis.token.ratio.label";</v>
       </c>
     </row>
     <row r="549" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A549" t="str">
         <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B20),".","_"),"=""", 'Commencer analyse'!B20,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_FREQUENCY_LABEL="window.start.analysis.frequency.label";</v>
       </c>
     </row>
     <row r="550" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A550" t="str">
         <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B21),".","_"),"=""", 'Commencer analyse'!B21,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_CHOOSE_TYPE_TREATMENT_OPTIONAL_LIST_PANEL_TITLE="window.start.analysis.choose.type.treatment.optional.list.panel.title";</v>
       </c>
     </row>
     <row r="551" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A551" t="str">
         <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B22),".","_"),"=""", 'Commencer analyse'!B22,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_CHOOSE_PROFILE_TREATMENT_OPTIONAL_LIST_PANEL_TITLE="window.start.analysis.choose.profile.treatment.optional.list.panel.title";</v>
       </c>
     </row>
     <row r="552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A552" t="str">
         <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B23),".","_"),"=""", 'Commencer analyse'!B23,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_CHOOSE_TYPE_TREATMENT_OPTIONAL_LIST_LABEL="window.start.analysis.choose.type.treatment.optional.list.label";</v>
       </c>
     </row>
     <row r="553" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A553" t="str">
         <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B24),".","_"),"=""", 'Commencer analyse'!B24,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_CHOOSE_PROFILE_TREATMENT_OPTIONAL_LIST_LABEL="window.start.analysis.choose.profile.treatment.optional.list.label";</v>
       </c>
     </row>
     <row r="554" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A554" t="str">
-        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B25),".","_"),"=""", 'Commencer analyse'!B25,""";"),"")</f>
-        <v/>
+      <c r="A554" t="e">
+        <f>IF('Commencer analyse'!#REF!&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!#REF!),".","_"),"=""", 'Commencer analyse'!#REF!,""";"),"")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="555" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A555" t="str">
-        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B26),".","_"),"=""", 'Commencer analyse'!B26,""";"),"")</f>
+        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B25),".","_"),"=""", 'Commencer analyse'!B25,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="556" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A556" t="str">
-        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B27),".","_"),"=""", 'Commencer analyse'!B27,""";"),"")</f>
+        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B26),".","_"),"=""", 'Commencer analyse'!B26,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="557" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A557" t="str">
-        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B28),".","_"),"=""", 'Commencer analyse'!B28,""";"),"")</f>
+        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B27),".","_"),"=""", 'Commencer analyse'!B27,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="558" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A558" t="str">
-        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B29),".","_"),"=""", 'Commencer analyse'!B29,""";"),"")</f>
+        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B28),".","_"),"=""", 'Commencer analyse'!B28,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="559" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A559" t="str">
-        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B30),".","_"),"=""", 'Commencer analyse'!B30,""";"),"")</f>
+        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B29),".","_"),"=""", 'Commencer analyse'!B29,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="560" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A560" t="str">
-        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B31),".","_"),"=""", 'Commencer analyse'!B31,""";"),"")</f>
+        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B30),".","_"),"=""", 'Commencer analyse'!B30,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="561" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A561" t="str">
-        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B32),".","_"),"=""", 'Commencer analyse'!B32,""";"),"")</f>
+        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B31),".","_"),"=""", 'Commencer analyse'!B31,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="562" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A562" t="str">
-        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B33),".","_"),"=""", 'Commencer analyse'!B33,""";"),"")</f>
+        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B32),".","_"),"=""", 'Commencer analyse'!B32,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="563" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A563" t="str">
-        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B34),".","_"),"=""", 'Commencer analyse'!B34,""";"),"")</f>
+        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B33),".","_"),"=""", 'Commencer analyse'!B33,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="564" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A564" t="str">
-        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B35),".","_"),"=""", 'Commencer analyse'!B35,""";"),"")</f>
+        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B34),".","_"),"=""", 'Commencer analyse'!B34,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="565" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A565" t="str">
-        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B36),".","_"),"=""", 'Commencer analyse'!B36,""";"),"")</f>
+        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B35),".","_"),"=""", 'Commencer analyse'!B35,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="566" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A566" t="str">
-        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B37),".","_"),"=""", 'Commencer analyse'!B37,""";"),"")</f>
+        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B36),".","_"),"=""", 'Commencer analyse'!B36,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="567" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A567" t="str">
-        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B38),".","_"),"=""", 'Commencer analyse'!B38,""";"),"")</f>
+        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B37),".","_"),"=""", 'Commencer analyse'!B37,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="568" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A568" t="str">
-        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B39),".","_"),"=""", 'Commencer analyse'!B39,""";"),"")</f>
+        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B38),".","_"),"=""", 'Commencer analyse'!B38,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="569" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A569" t="str">
-        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B40),".","_"),"=""", 'Commencer analyse'!B40,""";"),"")</f>
+        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B39),".","_"),"=""", 'Commencer analyse'!B39,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="570" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A570" t="str">
-        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B41),".","_"),"=""", 'Commencer analyse'!B41,""";"),"")</f>
+        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B40),".","_"),"=""", 'Commencer analyse'!B40,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="571" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A571" t="str">
-        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B42),".","_"),"=""", 'Commencer analyse'!B42,""";"),"")</f>
+        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B41),".","_"),"=""", 'Commencer analyse'!B41,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="572" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A572" t="str">
-        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B43),".","_"),"=""", 'Commencer analyse'!B43,""";"),"")</f>
+        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B42),".","_"),"=""", 'Commencer analyse'!B42,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="573" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A573" t="str">
-        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B44),".","_"),"=""", 'Commencer analyse'!B44,""";"),"")</f>
+        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B43),".","_"),"=""", 'Commencer analyse'!B43,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="574" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A574" t="str">
-        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B45),".","_"),"=""", 'Commencer analyse'!B45,""";"),"")</f>
+        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B44),".","_"),"=""", 'Commencer analyse'!B44,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="575" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A575" t="str">
-        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B46),".","_"),"=""", 'Commencer analyse'!B46,""";"),"")</f>
+        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B45),".","_"),"=""", 'Commencer analyse'!B45,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="576" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A576" t="str">
-        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B47),".","_"),"=""", 'Commencer analyse'!B47,""";"),"")</f>
+        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B46),".","_"),"=""", 'Commencer analyse'!B46,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="577" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A577" t="str">
-        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B48),".","_"),"=""", 'Commencer analyse'!B48,""";"),"")</f>
+        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B47),".","_"),"=""", 'Commencer analyse'!B47,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="578" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A578" t="str">
-        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B49),".","_"),"=""", 'Commencer analyse'!B49,""";"),"")</f>
+        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B48),".","_"),"=""", 'Commencer analyse'!B48,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="579" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A579" t="str">
-        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B50),".","_"),"=""", 'Commencer analyse'!B50,""";"),"")</f>
+        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B49),".","_"),"=""", 'Commencer analyse'!B49,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="580" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A580" t="str">
-        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B51),".","_"),"=""", 'Commencer analyse'!B51,""";"),"")</f>
+        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B50),".","_"),"=""", 'Commencer analyse'!B50,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A581" t="str">
-        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B52),".","_"),"=""", 'Commencer analyse'!B52,""";"),"")</f>
+        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B51),".","_"),"=""", 'Commencer analyse'!B51,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A582" t="str">
-        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B53),".","_"),"=""", 'Commencer analyse'!B53,""";"),"")</f>
+        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B52),".","_"),"=""", 'Commencer analyse'!B52,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A583" t="str">
-        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B54),".","_"),"=""", 'Commencer analyse'!B54,""";"),"")</f>
+        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B53),".","_"),"=""", 'Commencer analyse'!B53,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A584" t="str">
-        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B55),".","_"),"=""", 'Commencer analyse'!B55,""";"),"")</f>
+        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B54),".","_"),"=""", 'Commencer analyse'!B54,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="585" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A585" t="str">
-        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B56),".","_"),"=""", 'Commencer analyse'!B56,""";"),"")</f>
+        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B55),".","_"),"=""", 'Commencer analyse'!B55,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="586" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A586" t="str">
-        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B57),".","_"),"=""", 'Commencer analyse'!B57,""";"),"")</f>
+        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B56),".","_"),"=""", 'Commencer analyse'!B56,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A587" t="str">
-        <f>IF('Commencer analyse'!B58&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B58),".","_"),"=""", 'Commencer analyse'!B58,""";"),"")</f>
+        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B57),".","_"),"=""", 'Commencer analyse'!B57,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A588" t="str">
-        <f>IF('Commencer analyse'!B59&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B59),".","_"),"=""", 'Commencer analyse'!B59,""";"),"")</f>
+        <f>IF('Importer Excel'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B2),".","_"),"=""", 'Importer Excel'!B2,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="589" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A589" t="str">
-        <f>IF('Commencer analyse'!B60&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B60),".","_"),"=""", 'Commencer analyse'!B60,""";"),"")</f>
-        <v/>
+        <f>IF('Importer Excel'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B3),".","_"),"=""", 'Importer Excel'!B3,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_FILE_PICKER_PANEL_TITLE="window.import.excel.file.picker.panel.title";</v>
       </c>
     </row>
     <row r="590" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A590" t="str">
-        <f>IF('Importer Excel'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B2),".","_"),"=""", 'Importer Excel'!B2,""";"),"")</f>
-        <v/>
+        <f>IF('Importer Excel'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B4),".","_"),"=""", 'Importer Excel'!B4,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_PANEL_TITLE="window.import.excel.panel.title";</v>
       </c>
     </row>
     <row r="591" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A591" t="str">
-        <f>IF('Importer Excel'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B3),".","_"),"=""", 'Importer Excel'!B3,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_FILE_PICKER_PANEL_TITLE="window.import.excel.file.picker.panel.title";</v>
+        <f>IF('Importer Excel'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B5),".","_"),"=""", 'Importer Excel'!B5,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_INFORMATION_PANEL_TITLE="window.import.excel.information.panel.title";</v>
       </c>
     </row>
     <row r="592" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A592" t="str">
-        <f>IF('Importer Excel'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B4),".","_"),"=""", 'Importer Excel'!B4,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_PANEL_TITLE="window.import.excel.panel.title";</v>
+        <f>IF('Importer Excel'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B6),".","_"),"=""", 'Importer Excel'!B6,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_INFORMATION_PANEL_TEXT_NOTHING="window.import.excel.information.panel.text.nothing";</v>
       </c>
     </row>
     <row r="593" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A593" t="str">
-        <f>IF('Importer Excel'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B5),".","_"),"=""", 'Importer Excel'!B5,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_INFORMATION_PANEL_TITLE="window.import.excel.information.panel.title";</v>
+        <f>IF('Importer Excel'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B7),".","_"),"=""", 'Importer Excel'!B7,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_INFORMATION_PANEL_TEXT="window.import.excel.information.panel.text";</v>
       </c>
     </row>
     <row r="594" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A594" t="str">
-        <f>IF('Importer Excel'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B6),".","_"),"=""", 'Importer Excel'!B6,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_INFORMATION_PANEL_TEXT_NOTHING="window.import.excel.information.panel.text.nothing";</v>
+        <f>IF('Importer Excel'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B8),".","_"),"=""", 'Importer Excel'!B8,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_LIST_SPECIFIC_PANEL_TITLE="window.import.excel.list.specific.panel.title";</v>
       </c>
     </row>
     <row r="595" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A595" t="str">
-        <f>IF('Importer Excel'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B7),".","_"),"=""", 'Importer Excel'!B7,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_INFORMATION_PANEL_TEXT="window.import.excel.information.panel.text";</v>
+        <f>IF('Importer Excel'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B9),".","_"),"=""", 'Importer Excel'!B9,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_LIST_SPECIFIC_LABEL="window.import.excel.list.specific.label";</v>
       </c>
     </row>
     <row r="596" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A596" t="str">
-        <f>IF('Importer Excel'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B8),".","_"),"=""", 'Importer Excel'!B8,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_LIST_SPECIFIC_PANEL_TITLE="window.import.excel.list.specific.panel.title";</v>
+        <f>IF('Importer Excel'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B10),".","_"),"=""", 'Importer Excel'!B10,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_LIST_SPECIFIC_LABEL_NOTHING="window.import.excel.list.specific.label.nothing";</v>
       </c>
     </row>
     <row r="597" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A597" t="str">
-        <f>IF('Importer Excel'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B9),".","_"),"=""", 'Importer Excel'!B9,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_LIST_SPECIFIC_LABEL="window.import.excel.list.specific.label";</v>
+        <f>IF('Importer Excel'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B11),".","_"),"=""", 'Importer Excel'!B11,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_SHEET_NAME_LABEL="window.import.excel.sheet.name.label";</v>
       </c>
     </row>
     <row r="598" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A598" t="str">
-        <f>IF('Importer Excel'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B10),".","_"),"=""", 'Importer Excel'!B10,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_LIST_SPECIFIC_LABEL_NOTHING="window.import.excel.list.specific.label.nothing";</v>
+        <f>IF('Importer Excel'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B12),".","_"),"=""", 'Importer Excel'!B12,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_LIST_FIELDS_TITLE_PANEL="window.import.excel.list.fields.title.panel";</v>
       </c>
     </row>
     <row r="599" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A599" t="str">
-        <f>IF('Importer Excel'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B11),".","_"),"=""", 'Importer Excel'!B11,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_SHEET_NAME_LABEL="window.import.excel.sheet.name.label";</v>
+        <f>IF('Importer Excel'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B13),".","_"),"=""", 'Importer Excel'!B13,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_FILE_LABEL="window.import.excel.file.label";</v>
       </c>
     </row>
     <row r="600" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A600" t="str">
-        <f>IF('Importer Excel'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B12),".","_"),"=""", 'Importer Excel'!B12,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_LIST_FIELDS_TITLE_PANEL="window.import.excel.list.fields.title.panel";</v>
+        <f>IF('Importer Excel'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B14),".","_"),"=""", 'Importer Excel'!B14,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_ACTION_TITLE_PANEL="window.import.excel.action.title.panel";</v>
       </c>
     </row>
     <row r="601" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A601" t="str">
-        <f>IF('Importer Excel'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B13),".","_"),"=""", 'Importer Excel'!B13,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_FILE_LABEL="window.import.excel.file.label";</v>
+        <f>IF('Importer Excel'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B15),".","_"),"=""", 'Importer Excel'!B15,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_ACTION_SELECT_ALL="window.import.excel.action.select.all";</v>
       </c>
     </row>
     <row r="602" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A602" t="str">
-        <f>IF('Importer Excel'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B14),".","_"),"=""", 'Importer Excel'!B14,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_ACTION_TITLE_PANEL="window.import.excel.action.title.panel";</v>
+        <f>IF('Importer Excel'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B16),".","_"),"=""", 'Importer Excel'!B16,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_ACTION_DESELECT_ALL="window.import.excel.action.deselect.all";</v>
       </c>
     </row>
     <row r="603" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A603" t="str">
-        <f>IF('Importer Excel'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B15),".","_"),"=""", 'Importer Excel'!B15,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_ACTION_SELECT_ALL="window.import.excel.action.select.all";</v>
+        <f>IF('Importer Excel'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B17),".","_"),"=""", 'Importer Excel'!B17,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_PRINCIPAL_ACTION_TITLE_PANEL="window.import.excel.principal.action.title.panel";</v>
       </c>
     </row>
     <row r="604" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A604" t="str">
-        <f>IF('Importer Excel'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B16),".","_"),"=""", 'Importer Excel'!B16,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_ACTION_DESELECT_ALL="window.import.excel.action.deselect.all";</v>
+        <f>IF('Importer Excel'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B18),".","_"),"=""", 'Importer Excel'!B18,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_PRINCIPAL_ACTION_BUTTON_LABEL="window.import.excel.principal.action.button.label";</v>
       </c>
     </row>
     <row r="605" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A605" t="str">
-        <f>IF('Importer Excel'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B17),".","_"),"=""", 'Importer Excel'!B17,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_PRINCIPAL_ACTION_TITLE_PANEL="window.import.excel.principal.action.title.panel";</v>
+        <f>IF('Importer Excel'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B19),".","_"),"=""", 'Importer Excel'!B19,""";"),"")</f>
+        <v>public static final String WINDOW_IMPORT_EXCEL_SHEET_NAME_PANEL_TITLE="window.import.excel.sheet.name.panel.title";</v>
       </c>
     </row>
     <row r="606" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A606" t="str">
-        <f>IF('Importer Excel'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B18),".","_"),"=""", 'Importer Excel'!B18,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_PRINCIPAL_ACTION_BUTTON_LABEL="window.import.excel.principal.action.button.label";</v>
+        <f>IF('Importer Excel'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B20),".","_"),"=""", 'Importer Excel'!B20,""";"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="607" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A607" t="str">
-        <f>IF('Importer Excel'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B19),".","_"),"=""", 'Importer Excel'!B19,""";"),"")</f>
-        <v>public static final String WINDOW_IMPORT_EXCEL_SHEET_NAME_PANEL_TITLE="window.import.excel.sheet.name.panel.title";</v>
+        <f>IF('Importer Excel'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B21),".","_"),"=""", 'Importer Excel'!B21,""";"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="608" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A608" t="str">
-        <f>IF('Importer Excel'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B20),".","_"),"=""", 'Importer Excel'!B20,""";"),"")</f>
+        <f>IF('Importer Excel'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B22),".","_"),"=""", 'Importer Excel'!B22,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="609" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A609" t="str">
-        <f>IF('Importer Excel'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B21),".","_"),"=""", 'Importer Excel'!B21,""";"),"")</f>
+        <f>IF('Importer Excel'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B23),".","_"),"=""", 'Importer Excel'!B23,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="610" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A610" t="str">
-        <f>IF('Importer Excel'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B22),".","_"),"=""", 'Importer Excel'!B22,""";"),"")</f>
+        <f>IF('Importer Excel'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B24),".","_"),"=""", 'Importer Excel'!B24,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="611" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A611" t="str">
-        <f>IF('Importer Excel'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B23),".","_"),"=""", 'Importer Excel'!B23,""";"),"")</f>
+        <f>IF('Importer Excel'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B25),".","_"),"=""", 'Importer Excel'!B25,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="612" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A612" t="str">
-        <f>IF('Importer Excel'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B24),".","_"),"=""", 'Importer Excel'!B24,""";"),"")</f>
+        <f>IF('Importer Excel'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B26),".","_"),"=""", 'Importer Excel'!B26,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="613" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A613" t="str">
-        <f>IF('Importer Excel'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B25),".","_"),"=""", 'Importer Excel'!B25,""";"),"")</f>
+        <f>IF('Importer Excel'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B27),".","_"),"=""", 'Importer Excel'!B27,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="614" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A614" t="str">
-        <f>IF('Importer Excel'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B26),".","_"),"=""", 'Importer Excel'!B26,""";"),"")</f>
+        <f>IF('Importer Excel'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B28),".","_"),"=""", 'Importer Excel'!B28,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="615" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A615" t="str">
-        <f>IF('Importer Excel'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B27),".","_"),"=""", 'Importer Excel'!B27,""";"),"")</f>
+        <f>IF('Importer Excel'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B29),".","_"),"=""", 'Importer Excel'!B29,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="616" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A616" t="str">
-        <f>IF('Importer Excel'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B28),".","_"),"=""", 'Importer Excel'!B28,""";"),"")</f>
+        <f>IF('Importer Excel'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B30),".","_"),"=""", 'Importer Excel'!B30,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="617" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A617" t="str">
-        <f>IF('Importer Excel'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B29),".","_"),"=""", 'Importer Excel'!B29,""";"),"")</f>
+        <f>IF('Importer Excel'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B31),".","_"),"=""", 'Importer Excel'!B31,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="618" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A618" t="str">
-        <f>IF('Importer Excel'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B30),".","_"),"=""", 'Importer Excel'!B30,""";"),"")</f>
+        <f>IF('Importer Excel'!B32&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B32),".","_"),"=""", 'Importer Excel'!B32,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="619" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A619" t="str">
-        <f>IF('Importer Excel'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B31),".","_"),"=""", 'Importer Excel'!B31,""";"),"")</f>
+        <f>IF('Importer Excel'!B33&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B33),".","_"),"=""", 'Importer Excel'!B33,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="620" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A620" t="str">
-        <f>IF('Importer Excel'!B32&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B32),".","_"),"=""", 'Importer Excel'!B32,""";"),"")</f>
+        <f>IF('Importer Excel'!B34&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B34),".","_"),"=""", 'Importer Excel'!B34,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="621" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A621" t="str">
-        <f>IF('Importer Excel'!B33&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B33),".","_"),"=""", 'Importer Excel'!B33,""";"),"")</f>
+        <f>IF('Importer Excel'!B35&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B35),".","_"),"=""", 'Importer Excel'!B35,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="622" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A622" t="str">
-        <f>IF('Importer Excel'!B34&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B34),".","_"),"=""", 'Importer Excel'!B34,""";"),"")</f>
+        <f>IF('Importer Excel'!B36&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B36),".","_"),"=""", 'Importer Excel'!B36,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="623" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A623" t="str">
-        <f>IF('Importer Excel'!B35&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B35),".","_"),"=""", 'Importer Excel'!B35,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B2),".","_"),"=""", 'Erreur Fonctionnelle'!B2,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="624" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A624" t="str">
-        <f>IF('Importer Excel'!B36&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B36),".","_"),"=""", 'Importer Excel'!B36,""";"),"")</f>
-        <v/>
+        <f>IF('Erreur Fonctionnelle'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B3),".","_"),"=""", 'Erreur Fonctionnelle'!B3,""";"),"")</f>
+        <v>public static final String WINDOW_FUNCTIONAL_ERROR_PANEL_TITLE="window.functional.error.panel.title";</v>
       </c>
     </row>
     <row r="625" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A625" t="str">
-        <f>IF('Erreur Fonctionnelle'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B2),".","_"),"=""", 'Erreur Fonctionnelle'!B2,""";"),"")</f>
-        <v/>
+        <f>IF('Erreur Fonctionnelle'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B4),".","_"),"=""", 'Erreur Fonctionnelle'!B4,""";"),"")</f>
+        <v>public static final String WINDOW_FUNCTIONAL_ERROR_LIST_LABEL="window.functional.error.list.label";</v>
       </c>
     </row>
     <row r="626" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A626" t="str">
-        <f>IF('Erreur Fonctionnelle'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B3),".","_"),"=""", 'Erreur Fonctionnelle'!B3,""";"),"")</f>
-        <v>public static final String WINDOW_FUNCTIONAL_ERROR_PANEL_TITLE="window.functional.error.panel.title";</v>
+        <f>IF('Erreur Fonctionnelle'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B5),".","_"),"=""", 'Erreur Fonctionnelle'!B5,""";"),"")</f>
+        <v>public static final String WINDOW_FUNCTIONAL_ERROR_FILE_NOT_EXIST="window.functional.error.file.not.exist";</v>
       </c>
     </row>
     <row r="627" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A627" t="str">
-        <f>IF('Erreur Fonctionnelle'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B4),".","_"),"=""", 'Erreur Fonctionnelle'!B4,""";"),"")</f>
-        <v>public static final String WINDOW_FUNCTIONAL_ERROR_LIST_LABEL="window.functional.error.list.label";</v>
+        <f>IF('Erreur Fonctionnelle'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B6),".","_"),"=""", 'Erreur Fonctionnelle'!B6,""";"),"")</f>
+        <v>public static final String WINDOW_FUNCTIONAL_ERROR_NONE_FIELD_SELECTED="window.functional.error.none.field.selected";</v>
       </c>
     </row>
     <row r="628" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A628" t="str">
-        <f>IF('Erreur Fonctionnelle'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B5),".","_"),"=""", 'Erreur Fonctionnelle'!B5,""";"),"")</f>
-        <v>public static final String WINDOW_FUNCTIONAL_ERROR_FILE_NOT_EXIST="window.functional.error.file.not.exist";</v>
+        <f>IF('Erreur Fonctionnelle'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B7),".","_"),"=""", 'Erreur Fonctionnelle'!B7,""";"),"")</f>
+        <v>public static final String WINDOW_FUNCTIONAL_ERROR_INVALID_CONFIGURATION="window.functional.error.invalid.configuration";</v>
       </c>
     </row>
     <row r="629" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A629" t="str">
-        <f>IF('Erreur Fonctionnelle'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B6),".","_"),"=""", 'Erreur Fonctionnelle'!B6,""";"),"")</f>
-        <v>public static final String WINDOW_FUNCTIONAL_ERROR_NONE_FIELD_SELECTED="window.functional.error.none.field.selected";</v>
+        <f>IF('Erreur Fonctionnelle'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B8),".","_"),"=""", 'Erreur Fonctionnelle'!B8,""";"),"")</f>
+        <v>public static final String WINDOW_FUNCTIONAL_ERROR_INVALID_FIELD_WITH_CONFIGURATION="window.functional.error.invalid.field.with.configuration";</v>
       </c>
     </row>
     <row r="630" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A630" t="str">
-        <f>IF('Erreur Fonctionnelle'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B7),".","_"),"=""", 'Erreur Fonctionnelle'!B7,""";"),"")</f>
-        <v>public static final String WINDOW_FUNCTIONAL_ERROR_INVALID_CONFIGURATION="window.functional.error.invalid.configuration";</v>
+        <f>IF('Erreur Fonctionnelle'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B9),".","_"),"=""", 'Erreur Fonctionnelle'!B9,""";"),"")</f>
+        <v>public static final String WINDOW_FUNCTIONAL_ERROR_INVALID_FILE_EXCEL="window.functional.error.invalid.file.excel";</v>
       </c>
     </row>
     <row r="631" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A631" t="str">
-        <f>IF('Erreur Fonctionnelle'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B8),".","_"),"=""", 'Erreur Fonctionnelle'!B8,""";"),"")</f>
-        <v>public static final String WINDOW_FUNCTIONAL_ERROR_INVALID_FIELD_WITH_CONFIGURATION="window.functional.error.invalid.field.with.configuration";</v>
+        <f>IF('Erreur Fonctionnelle'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B10),".","_"),"=""", 'Erreur Fonctionnelle'!B10,""";"),"")</f>
+        <v>public static final String WINDOW_FUNCTIONAL_ERROR_INVALID_SPECIFIC_CONFIGURATION="window.functional.error.invalid.specific.configuration";</v>
       </c>
     </row>
     <row r="632" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A632" t="str">
-        <f>IF('Erreur Fonctionnelle'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B9),".","_"),"=""", 'Erreur Fonctionnelle'!B9,""";"),"")</f>
-        <v>public static final String WINDOW_FUNCTIONAL_ERROR_INVALID_FILE_EXCEL="window.functional.error.invalid.file.excel";</v>
+        <f>IF('Erreur Fonctionnelle'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B11),".","_"),"=""", 'Erreur Fonctionnelle'!B11,""";"),"")</f>
+        <v>public static final String WINDOW_FUNCTIONAL_ERROR_INVALID_FILE_EXCEL_SPECIFIC_CONFIGURATION="window.functional.error.invalid.file.excel.specific.configuration";</v>
       </c>
     </row>
     <row r="633" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A633" t="str">
-        <f>IF('Erreur Fonctionnelle'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B10),".","_"),"=""", 'Erreur Fonctionnelle'!B10,""";"),"")</f>
-        <v>public static final String WINDOW_FUNCTIONAL_ERROR_INVALID_SPECIFIC_CONFIGURATION="window.functional.error.invalid.specific.configuration";</v>
+        <f>IF('Erreur Fonctionnelle'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B12),".","_"),"=""", 'Erreur Fonctionnelle'!B12,""";"),"")</f>
+        <v>public static final String WINDOW_FUNCTIONAL_ERROR_INVALID_ANALYSIS_FOLDER="window.functional.error.invalid.analysis.folder";</v>
       </c>
     </row>
     <row r="634" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A634" t="str">
-        <f>IF('Erreur Fonctionnelle'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B11),".","_"),"=""", 'Erreur Fonctionnelle'!B11,""";"),"")</f>
-        <v>public static final String WINDOW_FUNCTIONAL_ERROR_INVALID_FILE_EXCEL_SPECIFIC_CONFIGURATION="window.functional.error.invalid.file.excel.specific.configuration";</v>
+        <f>IF('Erreur Fonctionnelle'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B13),".","_"),"=""", 'Erreur Fonctionnelle'!B13,""";"),"")</f>
+        <v>public static final String WINDOW_FUNCTIONAL_ERROR_VALUE_EXIST="window.functional.error.value.exist";</v>
       </c>
     </row>
     <row r="635" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A635" t="str">
-        <f>IF('Erreur Fonctionnelle'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B12),".","_"),"=""", 'Erreur Fonctionnelle'!B12,""";"),"")</f>
-        <v>public static final String WINDOW_FUNCTIONAL_ERROR_INVALID_ANALYSIS_FOLDER="window.functional.error.invalid.analysis.folder";</v>
+        <f>IF('Erreur Fonctionnelle'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B14),".","_"),"=""", 'Erreur Fonctionnelle'!B14,""";"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="636" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A636" t="str">
-        <f>IF('Erreur Fonctionnelle'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B13),".","_"),"=""", 'Erreur Fonctionnelle'!B13,""";"),"")</f>
-        <v>public static final String WINDOW_FUNCTIONAL_ERROR_VALUE_EXIST="window.functional.error.value.exist";</v>
+        <f>IF('Erreur Fonctionnelle'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B15),".","_"),"=""", 'Erreur Fonctionnelle'!B15,""";"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="637" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A637" t="str">
-        <f>IF('Erreur Fonctionnelle'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B14),".","_"),"=""", 'Erreur Fonctionnelle'!B14,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B16),".","_"),"=""", 'Erreur Fonctionnelle'!B16,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="638" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A638" t="str">
-        <f>IF('Erreur Fonctionnelle'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B15),".","_"),"=""", 'Erreur Fonctionnelle'!B15,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B17),".","_"),"=""", 'Erreur Fonctionnelle'!B17,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="639" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A639" t="str">
-        <f>IF('Erreur Fonctionnelle'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B16),".","_"),"=""", 'Erreur Fonctionnelle'!B16,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B18),".","_"),"=""", 'Erreur Fonctionnelle'!B18,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="640" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A640" t="str">
-        <f>IF('Erreur Fonctionnelle'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B17),".","_"),"=""", 'Erreur Fonctionnelle'!B17,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B19),".","_"),"=""", 'Erreur Fonctionnelle'!B19,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="641" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A641" t="str">
-        <f>IF('Erreur Fonctionnelle'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B18),".","_"),"=""", 'Erreur Fonctionnelle'!B18,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B20),".","_"),"=""", 'Erreur Fonctionnelle'!B20,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="642" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A642" t="str">
-        <f>IF('Erreur Fonctionnelle'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B19),".","_"),"=""", 'Erreur Fonctionnelle'!B19,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B21),".","_"),"=""", 'Erreur Fonctionnelle'!B21,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="643" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A643" t="str">
-        <f>IF('Erreur Fonctionnelle'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B20),".","_"),"=""", 'Erreur Fonctionnelle'!B20,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B22),".","_"),"=""", 'Erreur Fonctionnelle'!B22,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="644" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A644" t="str">
-        <f>IF('Erreur Fonctionnelle'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B21),".","_"),"=""", 'Erreur Fonctionnelle'!B21,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B23),".","_"),"=""", 'Erreur Fonctionnelle'!B23,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="645" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A645" t="str">
-        <f>IF('Erreur Fonctionnelle'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B22),".","_"),"=""", 'Erreur Fonctionnelle'!B22,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B24),".","_"),"=""", 'Erreur Fonctionnelle'!B24,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="646" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A646" t="str">
-        <f>IF('Erreur Fonctionnelle'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B23),".","_"),"=""", 'Erreur Fonctionnelle'!B23,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B25),".","_"),"=""", 'Erreur Fonctionnelle'!B25,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="647" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A647" t="str">
-        <f>IF('Erreur Fonctionnelle'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B24),".","_"),"=""", 'Erreur Fonctionnelle'!B24,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B26),".","_"),"=""", 'Erreur Fonctionnelle'!B26,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="648" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A648" t="str">
-        <f>IF('Erreur Fonctionnelle'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B25),".","_"),"=""", 'Erreur Fonctionnelle'!B25,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B27),".","_"),"=""", 'Erreur Fonctionnelle'!B27,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="649" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A649" t="str">
-        <f>IF('Erreur Fonctionnelle'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B26),".","_"),"=""", 'Erreur Fonctionnelle'!B26,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B28),".","_"),"=""", 'Erreur Fonctionnelle'!B28,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="650" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A650" t="str">
-        <f>IF('Erreur Fonctionnelle'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B27),".","_"),"=""", 'Erreur Fonctionnelle'!B27,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B29),".","_"),"=""", 'Erreur Fonctionnelle'!B29,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="651" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A651" t="str">
-        <f>IF('Erreur Fonctionnelle'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B28),".","_"),"=""", 'Erreur Fonctionnelle'!B28,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B30),".","_"),"=""", 'Erreur Fonctionnelle'!B30,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="652" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A652" t="str">
-        <f>IF('Erreur Fonctionnelle'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B29),".","_"),"=""", 'Erreur Fonctionnelle'!B29,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B31),".","_"),"=""", 'Erreur Fonctionnelle'!B31,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="653" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A653" t="str">
-        <f>IF('Erreur Fonctionnelle'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B30),".","_"),"=""", 'Erreur Fonctionnelle'!B30,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B32&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B32),".","_"),"=""", 'Erreur Fonctionnelle'!B32,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="654" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A654" t="str">
-        <f>IF('Erreur Fonctionnelle'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B31),".","_"),"=""", 'Erreur Fonctionnelle'!B31,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B33&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B33),".","_"),"=""", 'Erreur Fonctionnelle'!B33,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="655" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A655" t="str">
-        <f>IF('Erreur Fonctionnelle'!B32&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B32),".","_"),"=""", 'Erreur Fonctionnelle'!B32,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B34&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B34),".","_"),"=""", 'Erreur Fonctionnelle'!B34,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="656" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A656" t="str">
-        <f>IF('Erreur Fonctionnelle'!B33&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B33),".","_"),"=""", 'Erreur Fonctionnelle'!B33,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B35&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B35),".","_"),"=""", 'Erreur Fonctionnelle'!B35,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="657" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A657" t="str">
-        <f>IF('Erreur Fonctionnelle'!B34&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B34),".","_"),"=""", 'Erreur Fonctionnelle'!B34,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B36&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B36),".","_"),"=""", 'Erreur Fonctionnelle'!B36,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="658" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A658" t="str">
-        <f>IF('Erreur Fonctionnelle'!B35&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B35),".","_"),"=""", 'Erreur Fonctionnelle'!B35,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B37&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B37),".","_"),"=""", 'Erreur Fonctionnelle'!B37,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="659" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A659" t="str">
-        <f>IF('Erreur Fonctionnelle'!B36&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B36),".","_"),"=""", 'Erreur Fonctionnelle'!B36,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B38&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B38),".","_"),"=""", 'Erreur Fonctionnelle'!B38,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="660" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A660" t="str">
-        <f>IF('Erreur Fonctionnelle'!B37&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B37),".","_"),"=""", 'Erreur Fonctionnelle'!B37,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B39&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B39),".","_"),"=""", 'Erreur Fonctionnelle'!B39,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="661" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A661" t="str">
-        <f>IF('Erreur Fonctionnelle'!B38&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B38),".","_"),"=""", 'Erreur Fonctionnelle'!B38,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B40&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B40),".","_"),"=""", 'Erreur Fonctionnelle'!B40,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="662" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A662" t="str">
-        <f>IF('Erreur Fonctionnelle'!B39&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B39),".","_"),"=""", 'Erreur Fonctionnelle'!B39,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B41&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B41),".","_"),"=""", 'Erreur Fonctionnelle'!B41,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="663" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A663" t="str">
-        <f>IF('Erreur Fonctionnelle'!B40&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B40),".","_"),"=""", 'Erreur Fonctionnelle'!B40,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B42&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B42),".","_"),"=""", 'Erreur Fonctionnelle'!B42,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="664" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A664" t="str">
-        <f>IF('Erreur Fonctionnelle'!B41&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B41),".","_"),"=""", 'Erreur Fonctionnelle'!B41,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B43&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B43),".","_"),"=""", 'Erreur Fonctionnelle'!B43,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="665" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A665" t="str">
-        <f>IF('Erreur Fonctionnelle'!B42&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B42),".","_"),"=""", 'Erreur Fonctionnelle'!B42,""";"),"")</f>
+        <f>IF('Erreur Fonctionnelle'!B44&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B44),".","_"),"=""", 'Erreur Fonctionnelle'!B44,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="666" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A666" t="str">
-        <f>IF('Erreur Fonctionnelle'!B43&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B43),".","_"),"=""", 'Erreur Fonctionnelle'!B43,""";"),"")</f>
+        <f>IF(ListeProfil!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B2),".","_"),"=""", ListeProfil!B2,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="667" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A667" t="str">
-        <f>IF('Erreur Fonctionnelle'!B44&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Erreur Fonctionnelle'!B44),".","_"),"=""", 'Erreur Fonctionnelle'!B44,""";"),"")</f>
-        <v/>
+        <f>IF(ListeProfil!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B3),".","_"),"=""", ListeProfil!B3,""";"),"")</f>
+        <v>public static final String WINDOW_EDIT_PROFILE_LABEL="window.edit.profile.label";</v>
       </c>
     </row>
     <row r="668" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A668" t="str">
-        <f>IF(ListeProfil!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B2),".","_"),"=""", ListeProfil!B2,""";"),"")</f>
-        <v/>
+        <f>IF(ListeProfil!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B4),".","_"),"=""", ListeProfil!B4,""";"),"")</f>
+        <v>public static final String WINDOW_EDIT_PROFILE_NEW_BUTTON_LABEL="window.edit.profile.new.button.label";</v>
       </c>
     </row>
     <row r="669" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A669" t="str">
-        <f>IF(ListeProfil!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B3),".","_"),"=""", ListeProfil!B3,""";"),"")</f>
-        <v>public static final String WINDOW_EDIT_PROFILE_LABEL="window.edit.profile.label";</v>
+        <f>IF(ListeProfil!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B5),".","_"),"=""", ListeProfil!B5,""";"),"")</f>
+        <v>public static final String WINDOW_EDIT_PROFILE_REMOVE_BUTTON_LABEL="window.edit.profile.remove.button.label";</v>
       </c>
     </row>
     <row r="670" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A670" t="str">
-        <f>IF(ListeProfil!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B4),".","_"),"=""", ListeProfil!B4,""";"),"")</f>
-        <v>public static final String WINDOW_EDIT_PROFILE_NEW_BUTTON_LABEL="window.edit.profile.new.button.label";</v>
+        <f>IF(ListeProfil!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B6),".","_"),"=""", ListeProfil!B6,""";"),"")</f>
+        <v>public static final String WINDOW_EDIT_PROFILE_SAVE_BUTTON_LABEL="window.edit.profile.save.button.label";</v>
       </c>
     </row>
     <row r="671" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A671" t="str">
-        <f>IF(ListeProfil!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B5),".","_"),"=""", ListeProfil!B5,""";"),"")</f>
-        <v>public static final String WINDOW_EDIT_PROFILE_REMOVE_BUTTON_LABEL="window.edit.profile.remove.button.label";</v>
+        <f>IF(ListeProfil!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B7),".","_"),"=""", ListeProfil!B7,""";"),"")</f>
+        <v>public static final String WINDOW_EDIT_PROFILE_REMOVE_BUTTON_CONFIRMATION_MESSAGE="window.edit.profile.remove.button.confirmation.message";</v>
       </c>
     </row>
     <row r="672" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A672" t="str">
-        <f>IF(ListeProfil!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B6),".","_"),"=""", ListeProfil!B6,""";"),"")</f>
-        <v>public static final String WINDOW_EDIT_PROFILE_SAVE_BUTTON_LABEL="window.edit.profile.save.button.label";</v>
+        <f>IF(ListeProfil!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B8),".","_"),"=""", ListeProfil!B8,""";"),"")</f>
+        <v>public static final String WINDOW_EDIT_PROFILE_NEW_BUTTON_COPY_OR_NEW_MESSAGE="window.edit.profile.new.button.copy.or.new.message";</v>
       </c>
     </row>
     <row r="673" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A673" t="str">
-        <f>IF(ListeProfil!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B7),".","_"),"=""", ListeProfil!B7,""";"),"")</f>
-        <v>public static final String WINDOW_EDIT_PROFILE_REMOVE_BUTTON_CONFIRMATION_MESSAGE="window.edit.profile.remove.button.confirmation.message";</v>
+        <f>IF(ListeProfil!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B9),".","_"),"=""", ListeProfil!B9,""";"),"")</f>
+        <v>public static final String WINDOW_EDIT_PROFILE_NEW_BUTTON_NEW_NAME_MESSAGE="window.edit.profile.new.button.new.name.message";</v>
       </c>
     </row>
     <row r="674" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A674" t="str">
-        <f>IF(ListeProfil!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B8),".","_"),"=""", ListeProfil!B8,""";"),"")</f>
-        <v>public static final String WINDOW_EDIT_PROFILE_NEW_BUTTON_COPY_OR_NEW_MESSAGE="window.edit.profile.new.button.copy.or.new.message";</v>
+        <f>IF(ListeProfil!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B10),".","_"),"=""", ListeProfil!B10,""";"),"")</f>
+        <v>public static final String WINDOW_EDIT_PROFILE_SAVE_ALL_PROFILES_AND_QUIT="window.edit.profile.save.all.profiles.and.quit";</v>
       </c>
     </row>
     <row r="675" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A675" t="str">
-        <f>IF(ListeProfil!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B9),".","_"),"=""", ListeProfil!B9,""";"),"")</f>
-        <v>public static final String WINDOW_EDIT_PROFILE_NEW_BUTTON_NEW_NAME_MESSAGE="window.edit.profile.new.button.new.name.message";</v>
+        <f>IF(ListeProfil!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B11),".","_"),"=""", ListeProfil!B11,""";"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="676" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A676" t="str">
-        <f>IF(ListeProfil!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B10),".","_"),"=""", ListeProfil!B10,""";"),"")</f>
-        <v>public static final String WINDOW_EDIT_PROFILE_SAVE_ALL_PROFILES_AND_QUIT="window.edit.profile.save.all.profiles.and.quit";</v>
+        <f>IF(ListeProfil!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B12),".","_"),"=""", ListeProfil!B12,""";"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="677" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A677" t="str">
-        <f>IF(ListeProfil!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B11),".","_"),"=""", ListeProfil!B11,""";"),"")</f>
+        <f>IF(ListeProfil!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B13),".","_"),"=""", ListeProfil!B13,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="678" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A678" t="str">
-        <f>IF(ListeProfil!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B12),".","_"),"=""", ListeProfil!B12,""";"),"")</f>
+        <f>IF(ListeProfil!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B14),".","_"),"=""", ListeProfil!B14,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="679" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A679" t="str">
-        <f>IF(ListeProfil!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B13),".","_"),"=""", ListeProfil!B13,""";"),"")</f>
+        <f>IF(ListeProfil!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B15),".","_"),"=""", ListeProfil!B15,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="680" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A680" t="str">
-        <f>IF(ListeProfil!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B14),".","_"),"=""", ListeProfil!B14,""";"),"")</f>
+        <f>IF(ListeProfil!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B16),".","_"),"=""", ListeProfil!B16,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="681" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A681" t="str">
-        <f>IF(ListeProfil!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B15),".","_"),"=""", ListeProfil!B15,""";"),"")</f>
+        <f>IF(ListeProfil!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B17),".","_"),"=""", ListeProfil!B17,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="682" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A682" t="str">
-        <f>IF(ListeProfil!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B16),".","_"),"=""", ListeProfil!B16,""";"),"")</f>
+        <f>IF(StopWords!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B2),".","_"),"=""", StopWords!B2,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="683" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A683" t="str">
-        <f>IF(ListeProfil!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(ListeProfil!B17),".","_"),"=""", ListeProfil!B17,""";"),"")</f>
-        <v/>
+        <f>IF(StopWords!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B3),".","_"),"=""", StopWords!B3,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_STOPWORDS_PANEL_TITLE="window.manage.stopwords.panel.title";</v>
       </c>
     </row>
     <row r="684" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A684" t="str">
-        <f>IF(StopWords!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B2),".","_"),"=""", StopWords!B2,""";"),"")</f>
-        <v/>
+        <f>IF(StopWords!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B4),".","_"),"=""", StopWords!B4,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_STOPWORDS_INFORMATION_MESSAGE="window.manage.stopwords.information.message";</v>
       </c>
     </row>
     <row r="685" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A685" t="str">
-        <f>IF(StopWords!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B3),".","_"),"=""", StopWords!B3,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_STOPWORDS_PANEL_TITLE="window.manage.stopwords.panel.title";</v>
+        <f>IF(StopWords!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B5),".","_"),"=""", StopWords!B5,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_STOPWORDS_TABLE_HEADER_LABEL="window.manage.stopwords.table.header.label";</v>
       </c>
     </row>
     <row r="686" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A686" t="str">
-        <f>IF(StopWords!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B4),".","_"),"=""", StopWords!B4,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_STOPWORDS_INFORMATION_MESSAGE="window.manage.stopwords.information.message";</v>
+        <f>IF(StopWords!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B6),".","_"),"=""", StopWords!B6,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_STOPWORDS_ADD_INFORMATION_MESSAGE="window.manage.stopwords.add.information.message";</v>
       </c>
     </row>
     <row r="687" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A687" t="str">
-        <f>IF(StopWords!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B5),".","_"),"=""", StopWords!B5,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_STOPWORDS_TABLE_HEADER_LABEL="window.manage.stopwords.table.header.label";</v>
+        <f>IF(StopWords!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B7),".","_"),"=""", StopWords!B7,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_STOPWORDS_ADD_TEXT_LABEL="window.manage.stopwords.add.text.label";</v>
       </c>
     </row>
     <row r="688" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A688" t="str">
-        <f>IF(StopWords!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B6),".","_"),"=""", StopWords!B6,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_STOPWORDS_ADD_INFORMATION_MESSAGE="window.manage.stopwords.add.information.message";</v>
+        <f>IF(StopWords!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B8),".","_"),"=""", StopWords!B8,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_STOPWORDS_TABLE_PANEL_TITLE="window.manage.stopwords.table.panel.title";</v>
       </c>
     </row>
     <row r="689" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A689" t="str">
-        <f>IF(StopWords!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B7),".","_"),"=""", StopWords!B7,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_STOPWORDS_ADD_TEXT_LABEL="window.manage.stopwords.add.text.label";</v>
+        <f>IF(StopWords!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B9),".","_"),"=""", StopWords!B9,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_STOPWORDS_ADD_BUTTON_LABEL="window.manage.stopwords.add.button.label";</v>
       </c>
     </row>
     <row r="690" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A690" t="str">
-        <f>IF(StopWords!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B8),".","_"),"=""", StopWords!B8,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_STOPWORDS_TABLE_PANEL_TITLE="window.manage.stopwords.table.panel.title";</v>
+        <f>IF(StopWords!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B10),".","_"),"=""", StopWords!B10,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_STOPWORDS_REMOVE_BUTTON_LABEL="window.manage.stopwords.remove.button.label";</v>
       </c>
     </row>
     <row r="691" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A691" t="str">
-        <f>IF(StopWords!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B9),".","_"),"=""", StopWords!B9,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_STOPWORDS_ADD_BUTTON_LABEL="window.manage.stopwords.add.button.label";</v>
+        <f>IF(StopWords!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B11),".","_"),"=""", StopWords!B11,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_STOPWORDS_FILTER_LABEL="window.manage.stopwords.filter.label";</v>
       </c>
     </row>
     <row r="692" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A692" t="str">
-        <f>IF(StopWords!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B10),".","_"),"=""", StopWords!B10,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_STOPWORDS_REMOVE_BUTTON_LABEL="window.manage.stopwords.remove.button.label";</v>
+        <f>IF(StopWords!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B12),".","_"),"=""", StopWords!B12,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_STOPWORDS_INFORMATION_LABEL="window.manage.stopwords.information.label";</v>
       </c>
     </row>
     <row r="693" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A693" t="str">
-        <f>IF(StopWords!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B11),".","_"),"=""", StopWords!B11,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_STOPWORDS_FILTER_LABEL="window.manage.stopwords.filter.label";</v>
+        <f>IF(StopWords!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B13),".","_"),"=""", StopWords!B13,""";"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="694" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A694" t="str">
-        <f>IF(StopWords!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B12),".","_"),"=""", StopWords!B12,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_STOPWORDS_INFORMATION_LABEL="window.manage.stopwords.information.label";</v>
+        <f>IF(StopWords!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B14),".","_"),"=""", StopWords!B14,""";"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="695" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A695" t="str">
-        <f>IF(StopWords!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B13),".","_"),"=""", StopWords!B13,""";"),"")</f>
+        <f>IF(StopWords!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B15),".","_"),"=""", StopWords!B15,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="696" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A696" t="str">
-        <f>IF(StopWords!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B14),".","_"),"=""", StopWords!B14,""";"),"")</f>
+        <f>IF(Radicaux!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B2),".","_"),"=""", Radicaux!B2,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="697" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A697" t="str">
-        <f>IF(StopWords!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(StopWords!B15),".","_"),"=""", StopWords!B15,""";"),"")</f>
-        <v/>
+        <f>IF(Radicaux!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B3),".","_"),"=""", Radicaux!B3,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_PANEL_TITLE="window.manage.radicals.panel.title";</v>
       </c>
     </row>
     <row r="698" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A698" t="str">
-        <f>IF(Radicaux!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B2),".","_"),"=""", Radicaux!B2,""";"),"")</f>
-        <v/>
+        <f>IF(Radicaux!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B4),".","_"),"=""", Radicaux!B4,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_INFORMATION_MESSAGE="window.manage.radicals.information.message";</v>
       </c>
     </row>
     <row r="699" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A699" t="str">
-        <f>IF(Radicaux!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B3),".","_"),"=""", Radicaux!B3,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_PANEL_TITLE="window.manage.radicals.panel.title";</v>
+        <f>IF(Radicaux!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B5),".","_"),"=""", Radicaux!B5,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_TABLE_HEADER_LABEL="window.manage.radicals.table.header.label";</v>
       </c>
     </row>
     <row r="700" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A700" t="str">
-        <f>IF(Radicaux!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B4),".","_"),"=""", Radicaux!B4,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_INFORMATION_MESSAGE="window.manage.radicals.information.message";</v>
+        <f>IF(Radicaux!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B6),".","_"),"=""", Radicaux!B6,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_ADD_INFORMATION_MESSAGE="window.manage.radicals.add.information.message";</v>
       </c>
     </row>
     <row r="701" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A701" t="str">
-        <f>IF(Radicaux!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B5),".","_"),"=""", Radicaux!B5,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_TABLE_HEADER_LABEL="window.manage.radicals.table.header.label";</v>
+        <f>IF(Radicaux!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B7),".","_"),"=""", Radicaux!B7,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_ADD_TEXT_LABEL="window.manage.radicals.add.text.label";</v>
       </c>
     </row>
     <row r="702" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A702" t="str">
-        <f>IF(Radicaux!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B6),".","_"),"=""", Radicaux!B6,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_ADD_INFORMATION_MESSAGE="window.manage.radicals.add.information.message";</v>
+        <f>IF(Radicaux!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B8),".","_"),"=""", Radicaux!B8,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_TABLE_PANEL_TITLE="window.manage.radicals.table.panel.title";</v>
       </c>
     </row>
     <row r="703" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A703" t="str">
-        <f>IF(Radicaux!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B7),".","_"),"=""", Radicaux!B7,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_ADD_TEXT_LABEL="window.manage.radicals.add.text.label";</v>
+        <f>IF(Radicaux!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B9),".","_"),"=""", Radicaux!B9,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_VARIATION_ADD_INFORMATION_MESSAGE="window.manage.radicals.variation.add.information.message";</v>
       </c>
     </row>
     <row r="704" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A704" t="str">
-        <f>IF(Radicaux!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B8),".","_"),"=""", Radicaux!B8,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_TABLE_PANEL_TITLE="window.manage.radicals.table.panel.title";</v>
+        <f>IF(Radicaux!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B10),".","_"),"=""", Radicaux!B10,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_VARIATION_ADD_TEXT_LABEL="window.manage.radicals.variation.add.text.label";</v>
       </c>
     </row>
     <row r="705" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A705" t="str">
-        <f>IF(Radicaux!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B9),".","_"),"=""", Radicaux!B9,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_VARIATION_ADD_INFORMATION_MESSAGE="window.manage.radicals.variation.add.information.message";</v>
+        <f>IF(Radicaux!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B11),".","_"),"=""", Radicaux!B11,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_ADD_BUTTON_LABEL="window.manage.radicals.add.button.label";</v>
       </c>
     </row>
     <row r="706" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A706" t="str">
-        <f>IF(Radicaux!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B10),".","_"),"=""", Radicaux!B10,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_VARIATION_ADD_TEXT_LABEL="window.manage.radicals.variation.add.text.label";</v>
+        <f>IF(Radicaux!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B12),".","_"),"=""", Radicaux!B12,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_REMOVE_BUTTON_LABEL="window.manage.radicals.remove.button.label";</v>
       </c>
     </row>
     <row r="707" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A707" t="str">
-        <f>IF(Radicaux!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B11),".","_"),"=""", Radicaux!B11,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_ADD_BUTTON_LABEL="window.manage.radicals.add.button.label";</v>
+        <f>IF(Radicaux!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B13),".","_"),"=""", Radicaux!B13,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_VARIATION_ADD_BUTTON_LABEL="window.manage.radicals.variation.add.button.label";</v>
       </c>
     </row>
     <row r="708" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A708" t="str">
-        <f>IF(Radicaux!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B12),".","_"),"=""", Radicaux!B12,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_REMOVE_BUTTON_LABEL="window.manage.radicals.remove.button.label";</v>
+        <f>IF(Radicaux!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B14),".","_"),"=""", Radicaux!B14,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_VARIATION_REMOVE_BUTTON_LABEL="window.manage.radicals.variation.remove.button.label";</v>
       </c>
     </row>
     <row r="709" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A709" t="str">
-        <f>IF(Radicaux!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B13),".","_"),"=""", Radicaux!B13,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_VARIATION_ADD_BUTTON_LABEL="window.manage.radicals.variation.add.button.label";</v>
+        <f>IF(Radicaux!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B15),".","_"),"=""", Radicaux!B15,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_FILTER_LABEL="window.manage.radicals.filter.label";</v>
       </c>
     </row>
     <row r="710" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A710" t="str">
-        <f>IF(Radicaux!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B14),".","_"),"=""", Radicaux!B14,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_VARIATION_REMOVE_BUTTON_LABEL="window.manage.radicals.variation.remove.button.label";</v>
+        <f>IF(Radicaux!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B16),".","_"),"=""", Radicaux!B16,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_VARIATION_FILTER_LABEL="window.manage.radicals.variation.filter.label";</v>
       </c>
     </row>
     <row r="711" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A711" t="str">
-        <f>IF(Radicaux!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B15),".","_"),"=""", Radicaux!B15,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_FILTER_LABEL="window.manage.radicals.filter.label";</v>
+        <f>IF(Radicaux!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B17),".","_"),"=""", Radicaux!B17,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_INFORMATION_LABEL="window.manage.radicals.information.label";</v>
       </c>
     </row>
     <row r="712" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A712" t="str">
-        <f>IF(Radicaux!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B16),".","_"),"=""", Radicaux!B16,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_VARIATION_FILTER_LABEL="window.manage.radicals.variation.filter.label";</v>
+        <f>IF(Radicaux!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B18),".","_"),"=""", Radicaux!B18,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_VARIATION_TABLE_HEADER_LABEL="window.manage.radicals.variation.table.header.label";</v>
       </c>
     </row>
     <row r="713" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A713" t="str">
-        <f>IF(Radicaux!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B17),".","_"),"=""", Radicaux!B17,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_INFORMATION_LABEL="window.manage.radicals.information.label";</v>
+        <f>IF(Radicaux!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B19),".","_"),"=""", Radicaux!B19,""";"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="714" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A714" t="str">
-        <f>IF(Radicaux!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B18),".","_"),"=""", Radicaux!B18,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_VARIATION_TABLE_HEADER_LABEL="window.manage.radicals.variation.table.header.label";</v>
+        <f>IF(Radicaux!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B20),".","_"),"=""", Radicaux!B20,""";"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="715" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A715" t="str">
-        <f>IF(Radicaux!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B19),".","_"),"=""", Radicaux!B19,""";"),"")</f>
-        <v/>
+        <f>IF('Radicaux par classe'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B3),".","_"),"=""", 'Radicaux par classe'!B3,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_PANEL_TITLE="window.manage.radicals.by.class.panel.title";</v>
       </c>
     </row>
     <row r="716" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A716" t="str">
-        <f>IF(Radicaux!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Radicaux!B20),".","_"),"=""", Radicaux!B20,""";"),"")</f>
-        <v/>
+        <f>IF('Radicaux par classe'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B4),".","_"),"=""", 'Radicaux par classe'!B4,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_INFORMATION_MESSAGE="window.manage.radicals.by.class.information.message";</v>
       </c>
     </row>
     <row r="717" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A717" t="str">
-        <f>IF('Radicaux par classe'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B3),".","_"),"=""", 'Radicaux par classe'!B3,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_PANEL_TITLE="window.manage.radicals.by.class.panel.title";</v>
+        <f>IF('Radicaux par classe'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B5),".","_"),"=""", 'Radicaux par classe'!B5,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_TABLE_HEADER_LABEL="window.manage.radicals.by.class.table.header.label";</v>
       </c>
     </row>
     <row r="718" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A718" t="str">
-        <f>IF('Radicaux par classe'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B4),".","_"),"=""", 'Radicaux par classe'!B4,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_INFORMATION_MESSAGE="window.manage.radicals.by.class.information.message";</v>
+        <f>IF('Radicaux par classe'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B6),".","_"),"=""", 'Radicaux par classe'!B6,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_ADD_INFORMATION_MESSAGE="window.manage.radicals.by.class.add.information.message";</v>
       </c>
     </row>
     <row r="719" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A719" t="str">
-        <f>IF('Radicaux par classe'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B5),".","_"),"=""", 'Radicaux par classe'!B5,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_TABLE_HEADER_LABEL="window.manage.radicals.by.class.table.header.label";</v>
+        <f>IF('Radicaux par classe'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B7),".","_"),"=""", 'Radicaux par classe'!B7,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_ADD_TEXT_LABEL="window.manage.radicals.by.class.add.text.label";</v>
       </c>
     </row>
     <row r="720" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A720" t="str">
-        <f>IF('Radicaux par classe'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B6),".","_"),"=""", 'Radicaux par classe'!B6,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_ADD_INFORMATION_MESSAGE="window.manage.radicals.by.class.add.information.message";</v>
+        <f>IF('Radicaux par classe'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B8),".","_"),"=""", 'Radicaux par classe'!B8,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_TABLE_PANEL_TITLE="window.manage.radicals.by.class.table.panel.title";</v>
       </c>
     </row>
     <row r="721" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A721" t="str">
-        <f>IF('Radicaux par classe'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B7),".","_"),"=""", 'Radicaux par classe'!B7,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_ADD_TEXT_LABEL="window.manage.radicals.by.class.add.text.label";</v>
+        <f>IF('Radicaux par classe'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B9),".","_"),"=""", 'Radicaux par classe'!B9,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_VARIATION_ADD_INFORMATION_MESSAGE="window.manage.radicals.by.class.variation.add.information.message";</v>
       </c>
     </row>
     <row r="722" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A722" t="str">
-        <f>IF('Radicaux par classe'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B8),".","_"),"=""", 'Radicaux par classe'!B8,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_TABLE_PANEL_TITLE="window.manage.radicals.by.class.table.panel.title";</v>
+        <f>IF('Radicaux par classe'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B10),".","_"),"=""", 'Radicaux par classe'!B10,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_VARIATION_ADD_TEXT_LABEL="window.manage.radicals.by.class.variation.add.text.label";</v>
       </c>
     </row>
     <row r="723" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A723" t="str">
-        <f>IF('Radicaux par classe'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B9),".","_"),"=""", 'Radicaux par classe'!B9,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_VARIATION_ADD_INFORMATION_MESSAGE="window.manage.radicals.by.class.variation.add.information.message";</v>
+        <f>IF('Radicaux par classe'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B11),".","_"),"=""", 'Radicaux par classe'!B11,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_CATEGORY_ADD_INFORMATION_MESSAGE="window.manage.radicals.by.class.category.add.information.message";</v>
       </c>
     </row>
     <row r="724" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A724" t="str">
-        <f>IF('Radicaux par classe'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B10),".","_"),"=""", 'Radicaux par classe'!B10,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_VARIATION_ADD_TEXT_LABEL="window.manage.radicals.by.class.variation.add.text.label";</v>
+        <f>IF('Radicaux par classe'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B12),".","_"),"=""", 'Radicaux par classe'!B12,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_CATEGORY_ADD_TEXT_LABEL="window.manage.radicals.by.class.category.add.text.label";</v>
       </c>
     </row>
     <row r="725" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A725" t="str">
-        <f>IF('Radicaux par classe'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B11),".","_"),"=""", 'Radicaux par classe'!B11,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_CATEGORY_ADD_INFORMATION_MESSAGE="window.manage.radicals.by.class.category.add.information.message";</v>
+        <f>IF('Radicaux par classe'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B13),".","_"),"=""", 'Radicaux par classe'!B13,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_ADD_BUTTON_LABEL="window.manage.radicals.by.class.add.button.label";</v>
       </c>
     </row>
     <row r="726" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A726" t="str">
-        <f>IF('Radicaux par classe'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B12),".","_"),"=""", 'Radicaux par classe'!B12,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_CATEGORY_ADD_TEXT_LABEL="window.manage.radicals.by.class.category.add.text.label";</v>
+        <f>IF('Radicaux par classe'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B14),".","_"),"=""", 'Radicaux par classe'!B14,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_REMOVE_BUTTON_LABEL="window.manage.radicals.by.class.remove.button.label";</v>
       </c>
     </row>
     <row r="727" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A727" t="str">
-        <f>IF('Radicaux par classe'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B13),".","_"),"=""", 'Radicaux par classe'!B13,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_ADD_BUTTON_LABEL="window.manage.radicals.by.class.add.button.label";</v>
+        <f>IF('Radicaux par classe'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B15),".","_"),"=""", 'Radicaux par classe'!B15,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_VARIATION_ADD_BUTTON_LABEL="window.manage.radicals.by.class.variation.add.button.label";</v>
       </c>
     </row>
     <row r="728" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A728" t="str">
-        <f>IF('Radicaux par classe'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B14),".","_"),"=""", 'Radicaux par classe'!B14,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_REMOVE_BUTTON_LABEL="window.manage.radicals.by.class.remove.button.label";</v>
+        <f>IF('Radicaux par classe'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B16),".","_"),"=""", 'Radicaux par classe'!B16,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_VARIATION_REMOVE_BUTTON_LABEL="window.manage.radicals.by.class.variation.remove.button.label";</v>
       </c>
     </row>
     <row r="729" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A729" t="str">
-        <f>IF('Radicaux par classe'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B15),".","_"),"=""", 'Radicaux par classe'!B15,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_VARIATION_ADD_BUTTON_LABEL="window.manage.radicals.by.class.variation.add.button.label";</v>
+        <f>IF('Radicaux par classe'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B17),".","_"),"=""", 'Radicaux par classe'!B17,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_CATEGORY_ADD_BUTTON_LABEL="window.manage.radicals.by.class.category.add.button.label";</v>
       </c>
     </row>
     <row r="730" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A730" t="str">
-        <f>IF('Radicaux par classe'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B16),".","_"),"=""", 'Radicaux par classe'!B16,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_VARIATION_REMOVE_BUTTON_LABEL="window.manage.radicals.by.class.variation.remove.button.label";</v>
+        <f>IF('Radicaux par classe'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B18),".","_"),"=""", 'Radicaux par classe'!B18,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_CATEGORY_REMOVE_BUTTON_LABEL="window.manage.radicals.by.class.category.remove.button.label";</v>
       </c>
     </row>
     <row r="731" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A731" t="str">
-        <f>IF('Radicaux par classe'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B17),".","_"),"=""", 'Radicaux par classe'!B17,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_CATEGORY_ADD_BUTTON_LABEL="window.manage.radicals.by.class.category.add.button.label";</v>
+        <f>IF('Radicaux par classe'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B19),".","_"),"=""", 'Radicaux par classe'!B19,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_FILTER_LABEL="window.manage.radicals.by.class.filter.label";</v>
       </c>
     </row>
     <row r="732" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A732" t="str">
-        <f>IF('Radicaux par classe'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B18),".","_"),"=""", 'Radicaux par classe'!B18,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_CATEGORY_REMOVE_BUTTON_LABEL="window.manage.radicals.by.class.category.remove.button.label";</v>
+        <f>IF('Radicaux par classe'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B20),".","_"),"=""", 'Radicaux par classe'!B20,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_VARIATION_FILTER_LABEL="window.manage.radicals.by.class.variation.filter.label";</v>
       </c>
     </row>
     <row r="733" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A733" t="str">
-        <f>IF('Radicaux par classe'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B19),".","_"),"=""", 'Radicaux par classe'!B19,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_FILTER_LABEL="window.manage.radicals.by.class.filter.label";</v>
+        <f>IF('Radicaux par classe'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B21),".","_"),"=""", 'Radicaux par classe'!B21,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_CATEGORY_FILTER_LABEL="window.manage.radicals.by.class.category.filter.label";</v>
       </c>
     </row>
     <row r="734" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A734" t="str">
-        <f>IF('Radicaux par classe'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B20),".","_"),"=""", 'Radicaux par classe'!B20,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_VARIATION_FILTER_LABEL="window.manage.radicals.by.class.variation.filter.label";</v>
+        <f>IF('Radicaux par classe'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B22),".","_"),"=""", 'Radicaux par classe'!B22,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_INFORMATION_LABEL="window.manage.radicals.by.class.information.label";</v>
       </c>
     </row>
     <row r="735" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A735" t="str">
-        <f>IF('Radicaux par classe'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B21),".","_"),"=""", 'Radicaux par classe'!B21,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_CATEGORY_FILTER_LABEL="window.manage.radicals.by.class.category.filter.label";</v>
+        <f>IF('Radicaux par classe'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B23),".","_"),"=""", 'Radicaux par classe'!B23,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_VARIATION_TABLE_HEADER_LABEL="window.manage.radicals.by.class.variation.table.header.label";</v>
       </c>
     </row>
     <row r="736" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A736" t="str">
-        <f>IF('Radicaux par classe'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B22),".","_"),"=""", 'Radicaux par classe'!B22,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_INFORMATION_LABEL="window.manage.radicals.by.class.information.label";</v>
+        <f>IF('Radicaux par classe'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B24),".","_"),"=""", 'Radicaux par classe'!B24,""";"),"")</f>
+        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_CATEGORY_TABLE_HEADER_LABEL="window.manage.radicals.by.class.category.table.header.label";</v>
       </c>
     </row>
     <row r="737" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A737" t="str">
-        <f>IF('Radicaux par classe'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B23),".","_"),"=""", 'Radicaux par classe'!B23,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_VARIATION_TABLE_HEADER_LABEL="window.manage.radicals.by.class.variation.table.header.label";</v>
-      </c>
-    </row>
-    <row r="738" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A738" t="str">
-        <f>IF('Radicaux par classe'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B24),".","_"),"=""", 'Radicaux par classe'!B24,""";"),"")</f>
-        <v>public static final String WINDOW_MANAGE_RADICALS_BY_CLASS_CATEGORY_TABLE_HEADER_LABEL="window.manage.radicals.by.class.category.table.header.label";</v>
-      </c>
-    </row>
-    <row r="739" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A739" t="str">
         <f>IF('Radicaux par classe'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B25),".","_"),"=""", 'Radicaux par classe'!B25,""";"),"")</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Avancement sur le module d'analyse : - Ajout jusqu'à l'analyse du nombre de tokens (WIP)
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\IdeaProjects\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5D4E44-FD75-49E5-BBD1-64E4612DEF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2A9016-9882-42DF-890B-982217CFE061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="17" activeTab="18" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="19" activeTab="26" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="1068">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="1071">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -3234,9 +3234,6 @@
     <t>Elegir qué lista usar</t>
   </si>
   <si>
-    <t>window.start.analysis.choose.type.treatment.optional.list.label</t>
-  </si>
-  <si>
     <t>window.start.analysis.choose.profile.treatment.optional.list.label</t>
   </si>
   <si>
@@ -3252,10 +3249,22 @@
     <t>Modelo de pretratamiento de datos</t>
   </si>
   <si>
-    <t xml:space="preserve">Choix du type de liste </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elegir el tipo de lista </t>
+    <t>window.start.analysis.choose.type.lemmatization.treatment.optional.list.label</t>
+  </si>
+  <si>
+    <t>Choix du type de liste pour les lemmes</t>
+  </si>
+  <si>
+    <t>Elección del tipo de lista para lemas</t>
+  </si>
+  <si>
+    <t>window.start.analysis.choose.type.tokenization.treatment.optional.list.label</t>
+  </si>
+  <si>
+    <t>Choix du type de liste pour les tokens</t>
+  </si>
+  <si>
+    <t>Elección del tipo de lista para tokens</t>
   </si>
 </sst>
 </file>
@@ -28220,10 +28229,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757EF7E0-E814-48B2-A4AF-487C809E6C10}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28534,10 +28543,10 @@
         <v>1056</v>
       </c>
       <c r="C21" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D21" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -28548,10 +28557,10 @@
         <v>1058</v>
       </c>
       <c r="C22" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="D22" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -28559,7 +28568,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>1060</v>
+        <v>1065</v>
       </c>
       <c r="C23" t="s">
         <v>1066</v>
@@ -28573,13 +28582,27 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C24" t="s">
         <v>1057</v>
       </c>
       <c r="D24" t="s">
         <v>1059</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1070</v>
       </c>
     </row>
   </sheetData>
@@ -30520,8 +30543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904B2FA-CBC2-495A-A197-D0CDD47EB1AE}">
   <dimension ref="A1:A781"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A781" sqref="A1:A781"/>
+    <sheetView showZeros="0" topLeftCell="A589" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A557" sqref="A1:A781"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33788,326 +33811,326 @@
       </c>
     </row>
     <row r="544" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A544" t="e">
-        <f>IF('Commencer analyse'!#REF!&lt;&gt;"",CONCATENATE('Commencer analyse'!#REF!,"=", 'Commencer analyse'!#REF!),IF('Commencer analyse'!#REF!&lt;&gt;"",'Commencer analyse'!#REF!,""))</f>
-        <v>#REF!</v>
+      <c r="A544" t="str">
+        <f>IF('Commencer analyse'!B7&lt;&gt;"",CONCATENATE('Commencer analyse'!B7,"=", 'Commencer analyse'!C7),IF('Commencer analyse'!C7&lt;&gt;"",'Commencer analyse'!C7,""))</f>
+        <v>window.start.analysis.information.message.etape2=&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner les matériaux sur lesquels vous souhaitez effectuer l'analyse.&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="545" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A545" t="e">
-        <f>IF('Commencer analyse'!#REF!&lt;&gt;"",CONCATENATE('Commencer analyse'!#REF!,"=", 'Commencer analyse'!#REF!),IF('Commencer analyse'!#REF!&lt;&gt;"",'Commencer analyse'!#REF!,""))</f>
-        <v>#REF!</v>
+      <c r="A545" t="str">
+        <f>IF('Commencer analyse'!B8&lt;&gt;"",CONCATENATE('Commencer analyse'!B8,"=", 'Commencer analyse'!C8),IF('Commencer analyse'!C8&lt;&gt;"",'Commencer analyse'!C8,""))</f>
+        <v>window.start.analysis.type.panel.title=Choix des analyses</v>
       </c>
     </row>
     <row r="546" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A546" t="str">
-        <f>IF('Commencer analyse'!B7&lt;&gt;"",CONCATENATE('Commencer analyse'!B7,"=", 'Commencer analyse'!C7),IF('Commencer analyse'!C7&lt;&gt;"",'Commencer analyse'!C7,""))</f>
-        <v>window.start.analysis.information.message.etape2=&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner les matériaux sur lesquels vous souhaitez effectuer l'analyse.&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
+        <f>IF('Commencer analyse'!B9&lt;&gt;"",CONCATENATE('Commencer analyse'!B9,"=", 'Commencer analyse'!C9),IF('Commencer analyse'!C9&lt;&gt;"",'Commencer analyse'!C9,""))</f>
+        <v>window.start.analysis.information.message.etape3=&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner les champs correspondant aux matériaux sur lesquels vous souhaitez effectuer l'analyse.&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="547" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A547" t="str">
-        <f>IF('Commencer analyse'!B8&lt;&gt;"",CONCATENATE('Commencer analyse'!B8,"=", 'Commencer analyse'!C8),IF('Commencer analyse'!C8&lt;&gt;"",'Commencer analyse'!C8,""))</f>
-        <v>window.start.analysis.type.panel.title=Choix des analyses</v>
+        <f>IF('Commencer analyse'!B10&lt;&gt;"",CONCATENATE('Commencer analyse'!B10,"=", 'Commencer analyse'!C10),IF('Commencer analyse'!C10&lt;&gt;"",'Commencer analyse'!C10,""))</f>
+        <v>window.start.analysis.field.material.panel.title=Choix des champs à analyser</v>
       </c>
     </row>
     <row r="548" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A548" t="str">
-        <f>IF('Commencer analyse'!B9&lt;&gt;"",CONCATENATE('Commencer analyse'!B9,"=", 'Commencer analyse'!C9),IF('Commencer analyse'!C9&lt;&gt;"",'Commencer analyse'!C9,""))</f>
-        <v>window.start.analysis.information.message.etape3=&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner les champs correspondant aux matériaux sur lesquels vous souhaitez effectuer l'analyse.&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
+        <f>IF('Commencer analyse'!B11&lt;&gt;"",CONCATENATE('Commencer analyse'!B11,"=", 'Commencer analyse'!C11),IF('Commencer analyse'!C11&lt;&gt;"",'Commencer analyse'!C11,""))</f>
+        <v>window.start.analysis.information.message.etape4=&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner le type d'analyse que vous souhaitez effectuer.&lt;BR/&gt;Puis de consulter les résultats.&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="549" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A549" t="str">
-        <f>IF('Commencer analyse'!B10&lt;&gt;"",CONCATENATE('Commencer analyse'!B10,"=", 'Commencer analyse'!C10),IF('Commencer analyse'!C10&lt;&gt;"",'Commencer analyse'!C10,""))</f>
-        <v>window.start.analysis.field.material.panel.title=Choix des champs à analyser</v>
+        <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE('Commencer analyse'!B12,"=", 'Commencer analyse'!C12),IF('Commencer analyse'!C12&lt;&gt;"",'Commencer analyse'!C12,""))</f>
+        <v>window.start.analysis.choose.analyse.label=Choix de l'analyse</v>
       </c>
     </row>
     <row r="550" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A550" t="str">
-        <f>IF('Commencer analyse'!B11&lt;&gt;"",CONCATENATE('Commencer analyse'!B11,"=", 'Commencer analyse'!C11),IF('Commencer analyse'!C11&lt;&gt;"",'Commencer analyse'!C11,""))</f>
-        <v>window.start.analysis.information.message.etape4=&lt;HTML&gt;&lt;P&gt;Cette étape vous permet de sélectionner le type d'analyse que vous souhaitez effectuer.&lt;BR/&gt;Puis de consulter les résultats.&lt;BR/&gt;NB : A tout moment vous pouvez revenir en arriére avec le bouton précédent.&lt;/P&gt;&lt;/HTML&gt;</v>
+        <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE('Commencer analyse'!B13,"=", 'Commencer analyse'!C13),IF('Commencer analyse'!C13&lt;&gt;"",'Commencer analyse'!C13,""))</f>
+        <v>window.start.analysis.choose.analyse.panel.title=Analyse Lexicométrique</v>
       </c>
     </row>
     <row r="551" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A551" t="str">
-        <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE('Commencer analyse'!B12,"=", 'Commencer analyse'!C12),IF('Commencer analyse'!C12&lt;&gt;"",'Commencer analyse'!C12,""))</f>
-        <v>window.start.analysis.choose.analyse.label=Choix de l'analyse</v>
+        <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE('Commencer analyse'!B14,"=", 'Commencer analyse'!C14),IF('Commencer analyse'!C14&lt;&gt;"",'Commencer analyse'!C14,""))</f>
+        <v>window.start.analysis.choose.analyse.option.panel.title=Options disponibles/nécessaires pour l'analyse</v>
       </c>
     </row>
     <row r="552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A552" t="str">
-        <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE('Commencer analyse'!B13,"=", 'Commencer analyse'!C13),IF('Commencer analyse'!C13&lt;&gt;"",'Commencer analyse'!C13,""))</f>
-        <v>window.start.analysis.choose.analyse.panel.title=Analyse Lexicométrique</v>
+        <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE('Commencer analyse'!B15,"=", 'Commencer analyse'!C15),IF('Commencer analyse'!C15&lt;&gt;"",'Commencer analyse'!C15,""))</f>
+        <v>window.start.analysis.start.button.label=Lancer l'analyse</v>
       </c>
     </row>
     <row r="553" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A553" t="str">
-        <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE('Commencer analyse'!B14,"=", 'Commencer analyse'!C14),IF('Commencer analyse'!C14&lt;&gt;"",'Commencer analyse'!C14,""))</f>
-        <v>window.start.analysis.choose.analyse.option.panel.title=Options disponibles/nécessaires pour l'analyse</v>
+        <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE('Commencer analyse'!B16,"=", 'Commencer analyse'!C16),IF('Commencer analyse'!C16&lt;&gt;"",'Commencer analyse'!C16,""))</f>
+        <v>window.start.analysis.consult.results.button.label=Consulter les résultats</v>
       </c>
     </row>
     <row r="554" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A554" t="str">
-        <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE('Commencer analyse'!B15,"=", 'Commencer analyse'!C15),IF('Commencer analyse'!C15&lt;&gt;"",'Commencer analyse'!C15,""))</f>
-        <v>window.start.analysis.start.button.label=Lancer l'analyse</v>
+        <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE('Commencer analyse'!B17,"=", 'Commencer analyse'!C17),IF('Commencer analyse'!C17&lt;&gt;"",'Commencer analyse'!C17,""))</f>
+        <v>window.start.analysis.token.number.label=Nombre de tokens</v>
       </c>
     </row>
     <row r="555" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A555" t="str">
-        <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE('Commencer analyse'!B16,"=", 'Commencer analyse'!C16),IF('Commencer analyse'!C16&lt;&gt;"",'Commencer analyse'!C16,""))</f>
-        <v>window.start.analysis.consult.results.button.label=Consulter les résultats</v>
+        <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE('Commencer analyse'!B18,"=", 'Commencer analyse'!C18),IF('Commencer analyse'!C18&lt;&gt;"",'Commencer analyse'!C18,""))</f>
+        <v>window.start.analysis.lemme.type.label=Lemmatisation et numéro type</v>
       </c>
     </row>
     <row r="556" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A556" t="str">
-        <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE('Commencer analyse'!B17,"=", 'Commencer analyse'!C17),IF('Commencer analyse'!C17&lt;&gt;"",'Commencer analyse'!C17,""))</f>
-        <v>window.start.analysis.token.number.label=Nombre de tokens</v>
+        <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE('Commencer analyse'!B19,"=", 'Commencer analyse'!C19),IF('Commencer analyse'!C19&lt;&gt;"",'Commencer analyse'!C19,""))</f>
+        <v>window.start.analysis.token.ratio.label=Type token ratio</v>
       </c>
     </row>
     <row r="557" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A557" t="str">
-        <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE('Commencer analyse'!B18,"=", 'Commencer analyse'!C18),IF('Commencer analyse'!C18&lt;&gt;"",'Commencer analyse'!C18,""))</f>
-        <v>window.start.analysis.lemme.type.label=Lemmatisation et numéro type</v>
+        <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE('Commencer analyse'!B20,"=", 'Commencer analyse'!C20),IF('Commencer analyse'!C20&lt;&gt;"",'Commencer analyse'!C20,""))</f>
+        <v>window.start.analysis.frequency.label=Fréquence</v>
       </c>
     </row>
     <row r="558" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A558" t="str">
-        <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE('Commencer analyse'!B19,"=", 'Commencer analyse'!C19),IF('Commencer analyse'!C19&lt;&gt;"",'Commencer analyse'!C19,""))</f>
-        <v>window.start.analysis.token.ratio.label=Type token ratio</v>
+        <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE('Commencer analyse'!B21,"=", 'Commencer analyse'!C21),IF('Commencer analyse'!C21&lt;&gt;"",'Commencer analyse'!C21,""))</f>
+        <v>window.start.analysis.choose.type.treatment.optional.list.panel.title=Type de prétraitement des données</v>
       </c>
     </row>
     <row r="559" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A559" t="str">
-        <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE('Commencer analyse'!B20,"=", 'Commencer analyse'!C20),IF('Commencer analyse'!C20&lt;&gt;"",'Commencer analyse'!C20,""))</f>
-        <v>window.start.analysis.frequency.label=Fréquence</v>
+        <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE('Commencer analyse'!B22,"=", 'Commencer analyse'!C22),IF('Commencer analyse'!C22&lt;&gt;"",'Commencer analyse'!C22,""))</f>
+        <v>window.start.analysis.choose.profile.treatment.optional.list.panel.title=Modèle pour le prétaritement des données</v>
       </c>
     </row>
     <row r="560" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A560" t="str">
-        <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE('Commencer analyse'!B21,"=", 'Commencer analyse'!C21),IF('Commencer analyse'!C21&lt;&gt;"",'Commencer analyse'!C21,""))</f>
-        <v>window.start.analysis.choose.type.treatment.optional.list.panel.title=Type de prétraitement des données</v>
+        <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE('Commencer analyse'!B23,"=", 'Commencer analyse'!C23),IF('Commencer analyse'!C23&lt;&gt;"",'Commencer analyse'!C23,""))</f>
+        <v>window.start.analysis.choose.type.lemmatization.treatment.optional.list.label=Choix du type de liste pour les lemmes</v>
       </c>
     </row>
     <row r="561" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A561" t="str">
-        <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE('Commencer analyse'!B22,"=", 'Commencer analyse'!C22),IF('Commencer analyse'!C22&lt;&gt;"",'Commencer analyse'!C22,""))</f>
-        <v>window.start.analysis.choose.profile.treatment.optional.list.panel.title=Modèle pour le prétaritement des données</v>
+        <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE('Commencer analyse'!B24,"=", 'Commencer analyse'!C24),IF('Commencer analyse'!C24&lt;&gt;"",'Commencer analyse'!C24,""))</f>
+        <v>window.start.analysis.choose.profile.treatment.optional.list.label=Choix de la liste à utiliser</v>
       </c>
     </row>
     <row r="562" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A562" t="str">
-        <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE('Commencer analyse'!B23,"=", 'Commencer analyse'!C23),IF('Commencer analyse'!C23&lt;&gt;"",'Commencer analyse'!C23,""))</f>
-        <v xml:space="preserve">window.start.analysis.choose.type.treatment.optional.list.label=Choix du type de liste </v>
+        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE('Commencer analyse'!B25,"=", 'Commencer analyse'!C25),IF('Commencer analyse'!C25&lt;&gt;"",'Commencer analyse'!C25,""))</f>
+        <v>window.start.analysis.choose.type.tokenization.treatment.optional.list.label=Choix du type de liste pour les tokens</v>
       </c>
     </row>
     <row r="563" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A563" t="str">
-        <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE('Commencer analyse'!B24,"=", 'Commencer analyse'!C24),IF('Commencer analyse'!C24&lt;&gt;"",'Commencer analyse'!C24,""))</f>
-        <v>window.start.analysis.choose.profile.treatment.optional.list.label=Choix de la liste à utiliser</v>
+        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE('Commencer analyse'!B26,"=", 'Commencer analyse'!C26),IF('Commencer analyse'!C26&lt;&gt;"",'Commencer analyse'!C26,""))</f>
+        <v/>
       </c>
     </row>
     <row r="564" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A564" t="e">
-        <f>IF('Commencer analyse'!#REF!&lt;&gt;"",CONCATENATE('Commencer analyse'!#REF!,"=", 'Commencer analyse'!#REF!),IF('Commencer analyse'!#REF!&lt;&gt;"",'Commencer analyse'!#REF!,""))</f>
-        <v>#REF!</v>
+      <c r="A564" t="str">
+        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE('Commencer analyse'!B27,"=", 'Commencer analyse'!C27),IF('Commencer analyse'!C27&lt;&gt;"",'Commencer analyse'!C27,""))</f>
+        <v/>
       </c>
     </row>
     <row r="565" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A565" t="str">
-        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE('Commencer analyse'!B25,"=", 'Commencer analyse'!C25),IF('Commencer analyse'!C25&lt;&gt;"",'Commencer analyse'!C25,""))</f>
+        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE('Commencer analyse'!B28,"=", 'Commencer analyse'!C28),IF('Commencer analyse'!C28&lt;&gt;"",'Commencer analyse'!C28,""))</f>
         <v/>
       </c>
     </row>
     <row r="566" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A566" t="str">
-        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE('Commencer analyse'!B26,"=", 'Commencer analyse'!C26),IF('Commencer analyse'!C26&lt;&gt;"",'Commencer analyse'!C26,""))</f>
+        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE('Commencer analyse'!B29,"=", 'Commencer analyse'!C29),IF('Commencer analyse'!C29&lt;&gt;"",'Commencer analyse'!C29,""))</f>
         <v/>
       </c>
     </row>
     <row r="567" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A567" t="str">
-        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE('Commencer analyse'!B27,"=", 'Commencer analyse'!C27),IF('Commencer analyse'!C27&lt;&gt;"",'Commencer analyse'!C27,""))</f>
+        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE('Commencer analyse'!B30,"=", 'Commencer analyse'!C30),IF('Commencer analyse'!C30&lt;&gt;"",'Commencer analyse'!C30,""))</f>
         <v/>
       </c>
     </row>
     <row r="568" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A568" t="str">
-        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE('Commencer analyse'!B28,"=", 'Commencer analyse'!C28),IF('Commencer analyse'!C28&lt;&gt;"",'Commencer analyse'!C28,""))</f>
+        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE('Commencer analyse'!B31,"=", 'Commencer analyse'!C31),IF('Commencer analyse'!C31&lt;&gt;"",'Commencer analyse'!C31,""))</f>
         <v/>
       </c>
     </row>
     <row r="569" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A569" t="str">
-        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE('Commencer analyse'!B29,"=", 'Commencer analyse'!C29),IF('Commencer analyse'!C29&lt;&gt;"",'Commencer analyse'!C29,""))</f>
+        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE('Commencer analyse'!B32,"=", 'Commencer analyse'!C32),IF('Commencer analyse'!C32&lt;&gt;"",'Commencer analyse'!C32,""))</f>
         <v/>
       </c>
     </row>
     <row r="570" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A570" t="str">
-        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE('Commencer analyse'!B30,"=", 'Commencer analyse'!C30),IF('Commencer analyse'!C30&lt;&gt;"",'Commencer analyse'!C30,""))</f>
+        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE('Commencer analyse'!B33,"=", 'Commencer analyse'!C33),IF('Commencer analyse'!C33&lt;&gt;"",'Commencer analyse'!C33,""))</f>
         <v/>
       </c>
     </row>
     <row r="571" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A571" t="str">
-        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE('Commencer analyse'!B31,"=", 'Commencer analyse'!C31),IF('Commencer analyse'!C31&lt;&gt;"",'Commencer analyse'!C31,""))</f>
+        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE('Commencer analyse'!B34,"=", 'Commencer analyse'!C34),IF('Commencer analyse'!C34&lt;&gt;"",'Commencer analyse'!C34,""))</f>
         <v/>
       </c>
     </row>
     <row r="572" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A572" t="str">
-        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE('Commencer analyse'!B32,"=", 'Commencer analyse'!C32),IF('Commencer analyse'!C32&lt;&gt;"",'Commencer analyse'!C32,""))</f>
+        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE('Commencer analyse'!B35,"=", 'Commencer analyse'!C35),IF('Commencer analyse'!C35&lt;&gt;"",'Commencer analyse'!C35,""))</f>
         <v/>
       </c>
     </row>
     <row r="573" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A573" t="str">
-        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE('Commencer analyse'!B33,"=", 'Commencer analyse'!C33),IF('Commencer analyse'!C33&lt;&gt;"",'Commencer analyse'!C33,""))</f>
+        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE('Commencer analyse'!B36,"=", 'Commencer analyse'!C36),IF('Commencer analyse'!C36&lt;&gt;"",'Commencer analyse'!C36,""))</f>
         <v/>
       </c>
     </row>
     <row r="574" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A574" t="str">
-        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE('Commencer analyse'!B34,"=", 'Commencer analyse'!C34),IF('Commencer analyse'!C34&lt;&gt;"",'Commencer analyse'!C34,""))</f>
+        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE('Commencer analyse'!B37,"=", 'Commencer analyse'!C37),IF('Commencer analyse'!C37&lt;&gt;"",'Commencer analyse'!C37,""))</f>
         <v/>
       </c>
     </row>
     <row r="575" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A575" t="str">
-        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE('Commencer analyse'!B35,"=", 'Commencer analyse'!C35),IF('Commencer analyse'!C35&lt;&gt;"",'Commencer analyse'!C35,""))</f>
+        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE('Commencer analyse'!B38,"=", 'Commencer analyse'!C38),IF('Commencer analyse'!C38&lt;&gt;"",'Commencer analyse'!C38,""))</f>
         <v/>
       </c>
     </row>
     <row r="576" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A576" t="str">
-        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE('Commencer analyse'!B36,"=", 'Commencer analyse'!C36),IF('Commencer analyse'!C36&lt;&gt;"",'Commencer analyse'!C36,""))</f>
+        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE('Commencer analyse'!B39,"=", 'Commencer analyse'!C39),IF('Commencer analyse'!C39&lt;&gt;"",'Commencer analyse'!C39,""))</f>
         <v/>
       </c>
     </row>
     <row r="577" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A577" t="str">
-        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE('Commencer analyse'!B37,"=", 'Commencer analyse'!C37),IF('Commencer analyse'!C37&lt;&gt;"",'Commencer analyse'!C37,""))</f>
+        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE('Commencer analyse'!B40,"=", 'Commencer analyse'!C40),IF('Commencer analyse'!C40&lt;&gt;"",'Commencer analyse'!C40,""))</f>
         <v/>
       </c>
     </row>
     <row r="578" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A578" t="str">
-        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE('Commencer analyse'!B38,"=", 'Commencer analyse'!C38),IF('Commencer analyse'!C38&lt;&gt;"",'Commencer analyse'!C38,""))</f>
+        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE('Commencer analyse'!B41,"=", 'Commencer analyse'!C41),IF('Commencer analyse'!C41&lt;&gt;"",'Commencer analyse'!C41,""))</f>
         <v/>
       </c>
     </row>
     <row r="579" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A579" t="str">
-        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE('Commencer analyse'!B39,"=", 'Commencer analyse'!C39),IF('Commencer analyse'!C39&lt;&gt;"",'Commencer analyse'!C39,""))</f>
+        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE('Commencer analyse'!B42,"=", 'Commencer analyse'!C42),IF('Commencer analyse'!C42&lt;&gt;"",'Commencer analyse'!C42,""))</f>
         <v/>
       </c>
     </row>
     <row r="580" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A580" t="str">
-        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE('Commencer analyse'!B40,"=", 'Commencer analyse'!C40),IF('Commencer analyse'!C40&lt;&gt;"",'Commencer analyse'!C40,""))</f>
+        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE('Commencer analyse'!B43,"=", 'Commencer analyse'!C43),IF('Commencer analyse'!C43&lt;&gt;"",'Commencer analyse'!C43,""))</f>
         <v/>
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A581" t="str">
-        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE('Commencer analyse'!B41,"=", 'Commencer analyse'!C41),IF('Commencer analyse'!C41&lt;&gt;"",'Commencer analyse'!C41,""))</f>
+        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE('Commencer analyse'!B44,"=", 'Commencer analyse'!C44),IF('Commencer analyse'!C44&lt;&gt;"",'Commencer analyse'!C44,""))</f>
         <v/>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A582" t="str">
-        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE('Commencer analyse'!B42,"=", 'Commencer analyse'!C42),IF('Commencer analyse'!C42&lt;&gt;"",'Commencer analyse'!C42,""))</f>
+        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE('Commencer analyse'!B45,"=", 'Commencer analyse'!C45),IF('Commencer analyse'!C45&lt;&gt;"",'Commencer analyse'!C45,""))</f>
         <v/>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A583" t="str">
-        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE('Commencer analyse'!B43,"=", 'Commencer analyse'!C43),IF('Commencer analyse'!C43&lt;&gt;"",'Commencer analyse'!C43,""))</f>
+        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE('Commencer analyse'!B46,"=", 'Commencer analyse'!C46),IF('Commencer analyse'!C46&lt;&gt;"",'Commencer analyse'!C46,""))</f>
         <v/>
       </c>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A584" t="str">
-        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE('Commencer analyse'!B44,"=", 'Commencer analyse'!C44),IF('Commencer analyse'!C44&lt;&gt;"",'Commencer analyse'!C44,""))</f>
+        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE('Commencer analyse'!B47,"=", 'Commencer analyse'!C47),IF('Commencer analyse'!C47&lt;&gt;"",'Commencer analyse'!C47,""))</f>
         <v/>
       </c>
     </row>
     <row r="585" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A585" t="str">
-        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE('Commencer analyse'!B45,"=", 'Commencer analyse'!C45),IF('Commencer analyse'!C45&lt;&gt;"",'Commencer analyse'!C45,""))</f>
+        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE('Commencer analyse'!B48,"=", 'Commencer analyse'!C48),IF('Commencer analyse'!C48&lt;&gt;"",'Commencer analyse'!C48,""))</f>
         <v/>
       </c>
     </row>
     <row r="586" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A586" t="str">
-        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE('Commencer analyse'!B46,"=", 'Commencer analyse'!C46),IF('Commencer analyse'!C46&lt;&gt;"",'Commencer analyse'!C46,""))</f>
+        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE('Commencer analyse'!B49,"=", 'Commencer analyse'!C49),IF('Commencer analyse'!C49&lt;&gt;"",'Commencer analyse'!C49,""))</f>
         <v/>
       </c>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A587" t="str">
-        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE('Commencer analyse'!B47,"=", 'Commencer analyse'!C47),IF('Commencer analyse'!C47&lt;&gt;"",'Commencer analyse'!C47,""))</f>
+        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE('Commencer analyse'!B50,"=", 'Commencer analyse'!C50),IF('Commencer analyse'!C50&lt;&gt;"",'Commencer analyse'!C50,""))</f>
         <v/>
       </c>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A588" t="str">
-        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE('Commencer analyse'!B48,"=", 'Commencer analyse'!C48),IF('Commencer analyse'!C48&lt;&gt;"",'Commencer analyse'!C48,""))</f>
+        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE('Commencer analyse'!B51,"=", 'Commencer analyse'!C51),IF('Commencer analyse'!C51&lt;&gt;"",'Commencer analyse'!C51,""))</f>
         <v/>
       </c>
     </row>
     <row r="589" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A589" t="str">
-        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE('Commencer analyse'!B49,"=", 'Commencer analyse'!C49),IF('Commencer analyse'!C49&lt;&gt;"",'Commencer analyse'!C49,""))</f>
+        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE('Commencer analyse'!B52,"=", 'Commencer analyse'!C52),IF('Commencer analyse'!C52&lt;&gt;"",'Commencer analyse'!C52,""))</f>
         <v/>
       </c>
     </row>
     <row r="590" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A590" t="str">
-        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE('Commencer analyse'!B50,"=", 'Commencer analyse'!C50),IF('Commencer analyse'!C50&lt;&gt;"",'Commencer analyse'!C50,""))</f>
+        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE('Commencer analyse'!B53,"=", 'Commencer analyse'!C53),IF('Commencer analyse'!C53&lt;&gt;"",'Commencer analyse'!C53,""))</f>
         <v/>
       </c>
     </row>
     <row r="591" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A591" t="str">
-        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE('Commencer analyse'!B51,"=", 'Commencer analyse'!C51),IF('Commencer analyse'!C51&lt;&gt;"",'Commencer analyse'!C51,""))</f>
+        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE('Commencer analyse'!B54,"=", 'Commencer analyse'!C54),IF('Commencer analyse'!C54&lt;&gt;"",'Commencer analyse'!C54,""))</f>
         <v/>
       </c>
     </row>
     <row r="592" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A592" t="str">
-        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE('Commencer analyse'!B52,"=", 'Commencer analyse'!C52),IF('Commencer analyse'!C52&lt;&gt;"",'Commencer analyse'!C52,""))</f>
+        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE('Commencer analyse'!B55,"=", 'Commencer analyse'!C55),IF('Commencer analyse'!C55&lt;&gt;"",'Commencer analyse'!C55,""))</f>
         <v/>
       </c>
     </row>
     <row r="593" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A593" t="str">
-        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE('Commencer analyse'!B53,"=", 'Commencer analyse'!C53),IF('Commencer analyse'!C53&lt;&gt;"",'Commencer analyse'!C53,""))</f>
+        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE('Commencer analyse'!B56,"=", 'Commencer analyse'!C56),IF('Commencer analyse'!C56&lt;&gt;"",'Commencer analyse'!C56,""))</f>
         <v/>
       </c>
     </row>
     <row r="594" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A594" t="str">
-        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE('Commencer analyse'!B54,"=", 'Commencer analyse'!C54),IF('Commencer analyse'!C54&lt;&gt;"",'Commencer analyse'!C54,""))</f>
+        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE('Commencer analyse'!B57,"=", 'Commencer analyse'!C57),IF('Commencer analyse'!C57&lt;&gt;"",'Commencer analyse'!C57,""))</f>
         <v/>
       </c>
     </row>
     <row r="595" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A595" t="str">
-        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE('Commencer analyse'!B55,"=", 'Commencer analyse'!C55),IF('Commencer analyse'!C55&lt;&gt;"",'Commencer analyse'!C55,""))</f>
+        <f>IF('Commencer analyse'!B58&lt;&gt;"",CONCATENATE('Commencer analyse'!B58,"=", 'Commencer analyse'!C58),IF('Commencer analyse'!C58&lt;&gt;"",'Commencer analyse'!C58,""))</f>
         <v/>
       </c>
     </row>
     <row r="596" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A596" t="str">
-        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE('Commencer analyse'!B56,"=", 'Commencer analyse'!C56),IF('Commencer analyse'!C56&lt;&gt;"",'Commencer analyse'!C56,""))</f>
+        <f>IF('Commencer analyse'!B59&lt;&gt;"",CONCATENATE('Commencer analyse'!B59,"=", 'Commencer analyse'!C59),IF('Commencer analyse'!C59&lt;&gt;"",'Commencer analyse'!C59,""))</f>
         <v/>
       </c>
     </row>
     <row r="597" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A597" t="str">
-        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE('Commencer analyse'!B57,"=", 'Commencer analyse'!C57),IF('Commencer analyse'!C57&lt;&gt;"",'Commencer analyse'!C57,""))</f>
+        <f>IF('Commencer analyse'!B60&lt;&gt;"",CONCATENATE('Commencer analyse'!B60,"=", 'Commencer analyse'!C60),IF('Commencer analyse'!C60&lt;&gt;"",'Commencer analyse'!C60,""))</f>
         <v/>
       </c>
     </row>
@@ -35225,8 +35248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
   <dimension ref="A1:A771"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A1:A771"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A519" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A541" sqref="A1:A771"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38469,326 +38492,326 @@
       </c>
     </row>
     <row r="540" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A540" t="e">
-        <f>IF('Commencer analyse'!#REF!&lt;&gt;"",CONCATENATE('Commencer analyse'!#REF!,"=", 'Commencer analyse'!#REF!),IF('Commencer analyse'!#REF!&lt;&gt;"",'Commencer analyse'!#REF!,""))</f>
-        <v>#REF!</v>
+      <c r="A540" t="str">
+        <f>IF('Commencer analyse'!B7&lt;&gt;"",CONCATENATE('Commencer analyse'!B7,"=", 'Commencer analyse'!D7),IF('Commencer analyse'!D7&lt;&gt;"",'Commencer analyse'!D7,""))</f>
+        <v>window.start.analysis.information.message.etape2=&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar los materiales en los que desea realizar el análisis.&lt;BR/&gt;NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="541" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A541" t="e">
-        <f>IF('Commencer analyse'!#REF!&lt;&gt;"",CONCATENATE('Commencer analyse'!#REF!,"=", 'Commencer analyse'!#REF!),IF('Commencer analyse'!#REF!&lt;&gt;"",'Commencer analyse'!#REF!,""))</f>
-        <v>#REF!</v>
+      <c r="A541" t="str">
+        <f>IF('Commencer analyse'!B8&lt;&gt;"",CONCATENATE('Commencer analyse'!B8,"=", 'Commencer analyse'!D8),IF('Commencer analyse'!D8&lt;&gt;"",'Commencer analyse'!D8,""))</f>
+        <v>window.start.analysis.type.panel.title=Elección de análisis</v>
       </c>
     </row>
     <row r="542" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A542" t="str">
-        <f>IF('Commencer analyse'!B7&lt;&gt;"",CONCATENATE('Commencer analyse'!B7,"=", 'Commencer analyse'!D7),IF('Commencer analyse'!D7&lt;&gt;"",'Commencer analyse'!D7,""))</f>
-        <v>window.start.analysis.information.message.etape2=&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar los materiales en los que desea realizar el análisis.&lt;BR/&gt;NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
+        <f>IF('Commencer analyse'!B9&lt;&gt;"",CONCATENATE('Commencer analyse'!B9,"=", 'Commencer analyse'!D9),IF('Commencer analyse'!D9&lt;&gt;"",'Commencer analyse'!D9,""))</f>
+        <v>window.start.analysis.information.message.etape3=&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar los campos correspondientes a los materiales sobre los que desea realizar el análisis.&lt;BR/&gt;NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="543" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A543" t="str">
-        <f>IF('Commencer analyse'!B8&lt;&gt;"",CONCATENATE('Commencer analyse'!B8,"=", 'Commencer analyse'!D8),IF('Commencer analyse'!D8&lt;&gt;"",'Commencer analyse'!D8,""))</f>
-        <v>window.start.analysis.type.panel.title=Elección de análisis</v>
+        <f>IF('Commencer analyse'!B10&lt;&gt;"",CONCATENATE('Commencer analyse'!B10,"=", 'Commencer analyse'!D10),IF('Commencer analyse'!D10&lt;&gt;"",'Commencer analyse'!D10,""))</f>
+        <v>window.start.analysis.field.material.panel.title=Choix des champs à analyser</v>
       </c>
     </row>
     <row r="544" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A544" t="str">
-        <f>IF('Commencer analyse'!B9&lt;&gt;"",CONCATENATE('Commencer analyse'!B9,"=", 'Commencer analyse'!D9),IF('Commencer analyse'!D9&lt;&gt;"",'Commencer analyse'!D9,""))</f>
-        <v>window.start.analysis.information.message.etape3=&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar los campos correspondientes a los materiales sobre los que desea realizar el análisis.&lt;BR/&gt;NB: En cualquier momento usted puede volver atrás con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
+        <f>IF('Commencer analyse'!B11&lt;&gt;"",CONCATENATE('Commencer analyse'!B11,"=", 'Commencer analyse'!D11),IF('Commencer analyse'!D11&lt;&gt;"",'Commencer analyse'!D11,""))</f>
+        <v>window.start.analysis.information.message.etape4=&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar el tipo de análisis que desea realizar.&lt;BR/&gt;Luego consulte los resultados.&lt;BR/&gt;NB: En cualquier momento puede volver con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="545" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A545" t="str">
-        <f>IF('Commencer analyse'!B10&lt;&gt;"",CONCATENATE('Commencer analyse'!B10,"=", 'Commencer analyse'!D10),IF('Commencer analyse'!D10&lt;&gt;"",'Commencer analyse'!D10,""))</f>
-        <v>window.start.analysis.field.material.panel.title=Choix des champs à analyser</v>
+        <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE('Commencer analyse'!B12,"=", 'Commencer analyse'!D12),IF('Commencer analyse'!D12&lt;&gt;"",'Commencer analyse'!D12,""))</f>
+        <v>window.start.analysis.choose.analyse.label=Elección de análisis</v>
       </c>
     </row>
     <row r="546" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A546" t="str">
-        <f>IF('Commencer analyse'!B11&lt;&gt;"",CONCATENATE('Commencer analyse'!B11,"=", 'Commencer analyse'!D11),IF('Commencer analyse'!D11&lt;&gt;"",'Commencer analyse'!D11,""))</f>
-        <v>window.start.analysis.information.message.etape4=&lt;HTML&gt;&lt;P&gt;Este paso le permite seleccionar el tipo de análisis que desea realizar.&lt;BR/&gt;Luego consulte los resultados.&lt;BR/&gt;NB: En cualquier momento puede volver con el botón anterior.&lt;/P&gt;&lt;/HTML&gt;</v>
+        <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE('Commencer analyse'!B13,"=", 'Commencer analyse'!D13),IF('Commencer analyse'!D13&lt;&gt;"",'Commencer analyse'!D13,""))</f>
+        <v>window.start.analysis.choose.analyse.panel.title=Análisis lexicométrico</v>
       </c>
     </row>
     <row r="547" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A547" t="str">
-        <f>IF('Commencer analyse'!B12&lt;&gt;"",CONCATENATE('Commencer analyse'!B12,"=", 'Commencer analyse'!D12),IF('Commencer analyse'!D12&lt;&gt;"",'Commencer analyse'!D12,""))</f>
-        <v>window.start.analysis.choose.analyse.label=Elección de análisis</v>
+        <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE('Commencer analyse'!B14,"=", 'Commencer analyse'!D14),IF('Commencer analyse'!D14&lt;&gt;"",'Commencer analyse'!D14,""))</f>
+        <v>window.start.analysis.choose.analyse.option.panel.title=Opciones disponibles/requeridas para el análisis</v>
       </c>
     </row>
     <row r="548" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A548" t="str">
-        <f>IF('Commencer analyse'!B13&lt;&gt;"",CONCATENATE('Commencer analyse'!B13,"=", 'Commencer analyse'!D13),IF('Commencer analyse'!D13&lt;&gt;"",'Commencer analyse'!D13,""))</f>
-        <v>window.start.analysis.choose.analyse.panel.title=Análisis lexicométrico</v>
+        <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE('Commencer analyse'!B15,"=", 'Commencer analyse'!D15),IF('Commencer analyse'!D15&lt;&gt;"",'Commencer analyse'!D15,""))</f>
+        <v>window.start.analysis.start.button.label=Iniciar el análisis</v>
       </c>
     </row>
     <row r="549" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A549" t="str">
-        <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE('Commencer analyse'!B14,"=", 'Commencer analyse'!D14),IF('Commencer analyse'!D14&lt;&gt;"",'Commencer analyse'!D14,""))</f>
-        <v>window.start.analysis.choose.analyse.option.panel.title=Opciones disponibles/requeridas para el análisis</v>
+        <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE('Commencer analyse'!B16,"=", 'Commencer analyse'!D16),IF('Commencer analyse'!D16&lt;&gt;"",'Commencer analyse'!D16,""))</f>
+        <v>window.start.analysis.consult.results.button.label=Consultar los resultados</v>
       </c>
     </row>
     <row r="550" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A550" t="str">
-        <f>IF('Commencer analyse'!B15&lt;&gt;"",CONCATENATE('Commencer analyse'!B15,"=", 'Commencer analyse'!D15),IF('Commencer analyse'!D15&lt;&gt;"",'Commencer analyse'!D15,""))</f>
-        <v>window.start.analysis.start.button.label=Iniciar el análisis</v>
+        <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE('Commencer analyse'!B17,"=", 'Commencer analyse'!D17),IF('Commencer analyse'!D17&lt;&gt;"",'Commencer analyse'!D17,""))</f>
+        <v>window.start.analysis.token.number.label=Numero de tokens</v>
       </c>
     </row>
     <row r="551" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A551" t="str">
-        <f>IF('Commencer analyse'!B16&lt;&gt;"",CONCATENATE('Commencer analyse'!B16,"=", 'Commencer analyse'!D16),IF('Commencer analyse'!D16&lt;&gt;"",'Commencer analyse'!D16,""))</f>
-        <v>window.start.analysis.consult.results.button.label=Consultar los resultados</v>
+        <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE('Commencer analyse'!B18,"=", 'Commencer analyse'!D18),IF('Commencer analyse'!D18&lt;&gt;"",'Commencer analyse'!D18,""))</f>
+        <v>window.start.analysis.lemme.type.label=Lematización y número de tipo</v>
       </c>
     </row>
     <row r="552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A552" t="str">
-        <f>IF('Commencer analyse'!B17&lt;&gt;"",CONCATENATE('Commencer analyse'!B17,"=", 'Commencer analyse'!D17),IF('Commencer analyse'!D17&lt;&gt;"",'Commencer analyse'!D17,""))</f>
-        <v>window.start.analysis.token.number.label=Numero de tokens</v>
+        <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE('Commencer analyse'!B19,"=", 'Commencer analyse'!D19),IF('Commencer analyse'!D19&lt;&gt;"",'Commencer analyse'!D19,""))</f>
+        <v>window.start.analysis.token.ratio.label=Tipo de proporción de tokens</v>
       </c>
     </row>
     <row r="553" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A553" t="str">
-        <f>IF('Commencer analyse'!B18&lt;&gt;"",CONCATENATE('Commencer analyse'!B18,"=", 'Commencer analyse'!D18),IF('Commencer analyse'!D18&lt;&gt;"",'Commencer analyse'!D18,""))</f>
-        <v>window.start.analysis.lemme.type.label=Lematización y número de tipo</v>
+        <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE('Commencer analyse'!B20,"=", 'Commencer analyse'!D20),IF('Commencer analyse'!D20&lt;&gt;"",'Commencer analyse'!D20,""))</f>
+        <v>window.start.analysis.frequency.label=Frecuencia</v>
       </c>
     </row>
     <row r="554" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A554" t="str">
-        <f>IF('Commencer analyse'!B19&lt;&gt;"",CONCATENATE('Commencer analyse'!B19,"=", 'Commencer analyse'!D19),IF('Commencer analyse'!D19&lt;&gt;"",'Commencer analyse'!D19,""))</f>
-        <v>window.start.analysis.token.ratio.label=Tipo de proporción de tokens</v>
+        <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE('Commencer analyse'!B21,"=", 'Commencer analyse'!D21),IF('Commencer analyse'!D21&lt;&gt;"",'Commencer analyse'!D21,""))</f>
+        <v>window.start.analysis.choose.type.treatment.optional.list.panel.title=Tipo de preprocesamiento de datos</v>
       </c>
     </row>
     <row r="555" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A555" t="str">
-        <f>IF('Commencer analyse'!B20&lt;&gt;"",CONCATENATE('Commencer analyse'!B20,"=", 'Commencer analyse'!D20),IF('Commencer analyse'!D20&lt;&gt;"",'Commencer analyse'!D20,""))</f>
-        <v>window.start.analysis.frequency.label=Frecuencia</v>
+        <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE('Commencer analyse'!B22,"=", 'Commencer analyse'!D22),IF('Commencer analyse'!D22&lt;&gt;"",'Commencer analyse'!D22,""))</f>
+        <v>window.start.analysis.choose.profile.treatment.optional.list.panel.title=Modelo de pretratamiento de datos</v>
       </c>
     </row>
     <row r="556" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A556" t="str">
-        <f>IF('Commencer analyse'!B21&lt;&gt;"",CONCATENATE('Commencer analyse'!B21,"=", 'Commencer analyse'!D21),IF('Commencer analyse'!D21&lt;&gt;"",'Commencer analyse'!D21,""))</f>
-        <v>window.start.analysis.choose.type.treatment.optional.list.panel.title=Tipo de preprocesamiento de datos</v>
+        <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE('Commencer analyse'!B23,"=", 'Commencer analyse'!D23),IF('Commencer analyse'!D23&lt;&gt;"",'Commencer analyse'!D23,""))</f>
+        <v>window.start.analysis.choose.type.lemmatization.treatment.optional.list.label=Elección del tipo de lista para lemas</v>
       </c>
     </row>
     <row r="557" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A557" t="str">
-        <f>IF('Commencer analyse'!B22&lt;&gt;"",CONCATENATE('Commencer analyse'!B22,"=", 'Commencer analyse'!D22),IF('Commencer analyse'!D22&lt;&gt;"",'Commencer analyse'!D22,""))</f>
-        <v>window.start.analysis.choose.profile.treatment.optional.list.panel.title=Modelo de pretratamiento de datos</v>
+        <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE('Commencer analyse'!B24,"=", 'Commencer analyse'!D24),IF('Commencer analyse'!D24&lt;&gt;"",'Commencer analyse'!D24,""))</f>
+        <v>window.start.analysis.choose.profile.treatment.optional.list.label=Elegir qué lista usar</v>
       </c>
     </row>
     <row r="558" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A558" t="str">
-        <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE('Commencer analyse'!B23,"=", 'Commencer analyse'!D23),IF('Commencer analyse'!D23&lt;&gt;"",'Commencer analyse'!D23,""))</f>
-        <v xml:space="preserve">window.start.analysis.choose.type.treatment.optional.list.label=Elegir el tipo de lista </v>
+        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE('Commencer analyse'!B25,"=", 'Commencer analyse'!D25),IF('Commencer analyse'!D25&lt;&gt;"",'Commencer analyse'!D25,""))</f>
+        <v>window.start.analysis.choose.type.tokenization.treatment.optional.list.label=Elección del tipo de lista para tokens</v>
       </c>
     </row>
     <row r="559" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A559" t="str">
-        <f>IF('Commencer analyse'!B24&lt;&gt;"",CONCATENATE('Commencer analyse'!B24,"=", 'Commencer analyse'!D24),IF('Commencer analyse'!D24&lt;&gt;"",'Commencer analyse'!D24,""))</f>
-        <v>window.start.analysis.choose.profile.treatment.optional.list.label=Elegir qué lista usar</v>
+        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE('Commencer analyse'!B26,"=", 'Commencer analyse'!D26),IF('Commencer analyse'!D26&lt;&gt;"",'Commencer analyse'!D26,""))</f>
+        <v/>
       </c>
     </row>
     <row r="560" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A560" t="e">
-        <f>IF('Commencer analyse'!#REF!&lt;&gt;"",CONCATENATE('Commencer analyse'!#REF!,"=", 'Commencer analyse'!#REF!),IF('Commencer analyse'!#REF!&lt;&gt;"",'Commencer analyse'!#REF!,""))</f>
-        <v>#REF!</v>
+      <c r="A560" t="str">
+        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE('Commencer analyse'!B27,"=", 'Commencer analyse'!D27),IF('Commencer analyse'!D27&lt;&gt;"",'Commencer analyse'!D27,""))</f>
+        <v/>
       </c>
     </row>
     <row r="561" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A561" t="str">
-        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE('Commencer analyse'!B25,"=", 'Commencer analyse'!D25),IF('Commencer analyse'!D25&lt;&gt;"",'Commencer analyse'!D25,""))</f>
+        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE('Commencer analyse'!B28,"=", 'Commencer analyse'!D28),IF('Commencer analyse'!D28&lt;&gt;"",'Commencer analyse'!D28,""))</f>
         <v/>
       </c>
     </row>
     <row r="562" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A562" t="str">
-        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE('Commencer analyse'!B26,"=", 'Commencer analyse'!D26),IF('Commencer analyse'!D26&lt;&gt;"",'Commencer analyse'!D26,""))</f>
+        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE('Commencer analyse'!B29,"=", 'Commencer analyse'!D29),IF('Commencer analyse'!D29&lt;&gt;"",'Commencer analyse'!D29,""))</f>
         <v/>
       </c>
     </row>
     <row r="563" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A563" t="str">
-        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE('Commencer analyse'!B27,"=", 'Commencer analyse'!D27),IF('Commencer analyse'!D27&lt;&gt;"",'Commencer analyse'!D27,""))</f>
+        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE('Commencer analyse'!B30,"=", 'Commencer analyse'!D30),IF('Commencer analyse'!D30&lt;&gt;"",'Commencer analyse'!D30,""))</f>
         <v/>
       </c>
     </row>
     <row r="564" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A564" t="str">
-        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE('Commencer analyse'!B28,"=", 'Commencer analyse'!D28),IF('Commencer analyse'!D28&lt;&gt;"",'Commencer analyse'!D28,""))</f>
+        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE('Commencer analyse'!B31,"=", 'Commencer analyse'!D31),IF('Commencer analyse'!D31&lt;&gt;"",'Commencer analyse'!D31,""))</f>
         <v/>
       </c>
     </row>
     <row r="565" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A565" t="str">
-        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE('Commencer analyse'!B29,"=", 'Commencer analyse'!D29),IF('Commencer analyse'!D29&lt;&gt;"",'Commencer analyse'!D29,""))</f>
+        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE('Commencer analyse'!B32,"=", 'Commencer analyse'!D32),IF('Commencer analyse'!D32&lt;&gt;"",'Commencer analyse'!D32,""))</f>
         <v/>
       </c>
     </row>
     <row r="566" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A566" t="str">
-        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE('Commencer analyse'!B30,"=", 'Commencer analyse'!D30),IF('Commencer analyse'!D30&lt;&gt;"",'Commencer analyse'!D30,""))</f>
+        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE('Commencer analyse'!B33,"=", 'Commencer analyse'!D33),IF('Commencer analyse'!D33&lt;&gt;"",'Commencer analyse'!D33,""))</f>
         <v/>
       </c>
     </row>
     <row r="567" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A567" t="str">
-        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE('Commencer analyse'!B31,"=", 'Commencer analyse'!D31),IF('Commencer analyse'!D31&lt;&gt;"",'Commencer analyse'!D31,""))</f>
+        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE('Commencer analyse'!B34,"=", 'Commencer analyse'!D34),IF('Commencer analyse'!D34&lt;&gt;"",'Commencer analyse'!D34,""))</f>
         <v/>
       </c>
     </row>
     <row r="568" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A568" t="str">
-        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE('Commencer analyse'!B32,"=", 'Commencer analyse'!D32),IF('Commencer analyse'!D32&lt;&gt;"",'Commencer analyse'!D32,""))</f>
+        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE('Commencer analyse'!B35,"=", 'Commencer analyse'!D35),IF('Commencer analyse'!D35&lt;&gt;"",'Commencer analyse'!D35,""))</f>
         <v/>
       </c>
     </row>
     <row r="569" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A569" t="str">
-        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE('Commencer analyse'!B33,"=", 'Commencer analyse'!D33),IF('Commencer analyse'!D33&lt;&gt;"",'Commencer analyse'!D33,""))</f>
+        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE('Commencer analyse'!B36,"=", 'Commencer analyse'!D36),IF('Commencer analyse'!D36&lt;&gt;"",'Commencer analyse'!D36,""))</f>
         <v/>
       </c>
     </row>
     <row r="570" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A570" t="str">
-        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE('Commencer analyse'!B34,"=", 'Commencer analyse'!D34),IF('Commencer analyse'!D34&lt;&gt;"",'Commencer analyse'!D34,""))</f>
+        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE('Commencer analyse'!B37,"=", 'Commencer analyse'!D37),IF('Commencer analyse'!D37&lt;&gt;"",'Commencer analyse'!D37,""))</f>
         <v/>
       </c>
     </row>
     <row r="571" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A571" t="str">
-        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE('Commencer analyse'!B35,"=", 'Commencer analyse'!D35),IF('Commencer analyse'!D35&lt;&gt;"",'Commencer analyse'!D35,""))</f>
+        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE('Commencer analyse'!B38,"=", 'Commencer analyse'!D38),IF('Commencer analyse'!D38&lt;&gt;"",'Commencer analyse'!D38,""))</f>
         <v/>
       </c>
     </row>
     <row r="572" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A572" t="str">
-        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE('Commencer analyse'!B36,"=", 'Commencer analyse'!D36),IF('Commencer analyse'!D36&lt;&gt;"",'Commencer analyse'!D36,""))</f>
+        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE('Commencer analyse'!B39,"=", 'Commencer analyse'!D39),IF('Commencer analyse'!D39&lt;&gt;"",'Commencer analyse'!D39,""))</f>
         <v/>
       </c>
     </row>
     <row r="573" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A573" t="str">
-        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE('Commencer analyse'!B37,"=", 'Commencer analyse'!D37),IF('Commencer analyse'!D37&lt;&gt;"",'Commencer analyse'!D37,""))</f>
+        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE('Commencer analyse'!B40,"=", 'Commencer analyse'!D40),IF('Commencer analyse'!D40&lt;&gt;"",'Commencer analyse'!D40,""))</f>
         <v/>
       </c>
     </row>
     <row r="574" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A574" t="str">
-        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE('Commencer analyse'!B38,"=", 'Commencer analyse'!D38),IF('Commencer analyse'!D38&lt;&gt;"",'Commencer analyse'!D38,""))</f>
+        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE('Commencer analyse'!B41,"=", 'Commencer analyse'!D41),IF('Commencer analyse'!D41&lt;&gt;"",'Commencer analyse'!D41,""))</f>
         <v/>
       </c>
     </row>
     <row r="575" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A575" t="str">
-        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE('Commencer analyse'!B39,"=", 'Commencer analyse'!D39),IF('Commencer analyse'!D39&lt;&gt;"",'Commencer analyse'!D39,""))</f>
+        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE('Commencer analyse'!B42,"=", 'Commencer analyse'!D42),IF('Commencer analyse'!D42&lt;&gt;"",'Commencer analyse'!D42,""))</f>
         <v/>
       </c>
     </row>
     <row r="576" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A576" t="str">
-        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE('Commencer analyse'!B40,"=", 'Commencer analyse'!D40),IF('Commencer analyse'!D40&lt;&gt;"",'Commencer analyse'!D40,""))</f>
+        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE('Commencer analyse'!B43,"=", 'Commencer analyse'!D43),IF('Commencer analyse'!D43&lt;&gt;"",'Commencer analyse'!D43,""))</f>
         <v/>
       </c>
     </row>
     <row r="577" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A577" t="str">
-        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE('Commencer analyse'!B41,"=", 'Commencer analyse'!D41),IF('Commencer analyse'!D41&lt;&gt;"",'Commencer analyse'!D41,""))</f>
+        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE('Commencer analyse'!B44,"=", 'Commencer analyse'!D44),IF('Commencer analyse'!D44&lt;&gt;"",'Commencer analyse'!D44,""))</f>
         <v/>
       </c>
     </row>
     <row r="578" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A578" t="str">
-        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE('Commencer analyse'!B42,"=", 'Commencer analyse'!D42),IF('Commencer analyse'!D42&lt;&gt;"",'Commencer analyse'!D42,""))</f>
+        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE('Commencer analyse'!B45,"=", 'Commencer analyse'!D45),IF('Commencer analyse'!D45&lt;&gt;"",'Commencer analyse'!D45,""))</f>
         <v/>
       </c>
     </row>
     <row r="579" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A579" t="str">
-        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE('Commencer analyse'!B43,"=", 'Commencer analyse'!D43),IF('Commencer analyse'!D43&lt;&gt;"",'Commencer analyse'!D43,""))</f>
+        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE('Commencer analyse'!B46,"=", 'Commencer analyse'!D46),IF('Commencer analyse'!D46&lt;&gt;"",'Commencer analyse'!D46,""))</f>
         <v/>
       </c>
     </row>
     <row r="580" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A580" t="str">
-        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE('Commencer analyse'!B44,"=", 'Commencer analyse'!D44),IF('Commencer analyse'!D44&lt;&gt;"",'Commencer analyse'!D44,""))</f>
+        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE('Commencer analyse'!B47,"=", 'Commencer analyse'!D47),IF('Commencer analyse'!D47&lt;&gt;"",'Commencer analyse'!D47,""))</f>
         <v/>
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A581" t="str">
-        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE('Commencer analyse'!B45,"=", 'Commencer analyse'!D45),IF('Commencer analyse'!D45&lt;&gt;"",'Commencer analyse'!D45,""))</f>
+        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE('Commencer analyse'!B48,"=", 'Commencer analyse'!D48),IF('Commencer analyse'!D48&lt;&gt;"",'Commencer analyse'!D48,""))</f>
         <v/>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A582" t="str">
-        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE('Commencer analyse'!B46,"=", 'Commencer analyse'!D46),IF('Commencer analyse'!D46&lt;&gt;"",'Commencer analyse'!D46,""))</f>
+        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE('Commencer analyse'!B49,"=", 'Commencer analyse'!D49),IF('Commencer analyse'!D49&lt;&gt;"",'Commencer analyse'!D49,""))</f>
         <v/>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A583" t="str">
-        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE('Commencer analyse'!B47,"=", 'Commencer analyse'!D47),IF('Commencer analyse'!D47&lt;&gt;"",'Commencer analyse'!D47,""))</f>
+        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE('Commencer analyse'!B50,"=", 'Commencer analyse'!D50),IF('Commencer analyse'!D50&lt;&gt;"",'Commencer analyse'!D50,""))</f>
         <v/>
       </c>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A584" t="str">
-        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE('Commencer analyse'!B48,"=", 'Commencer analyse'!D48),IF('Commencer analyse'!D48&lt;&gt;"",'Commencer analyse'!D48,""))</f>
+        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE('Commencer analyse'!B51,"=", 'Commencer analyse'!D51),IF('Commencer analyse'!D51&lt;&gt;"",'Commencer analyse'!D51,""))</f>
         <v/>
       </c>
     </row>
     <row r="585" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A585" t="str">
-        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE('Commencer analyse'!B49,"=", 'Commencer analyse'!D49),IF('Commencer analyse'!D49&lt;&gt;"",'Commencer analyse'!D49,""))</f>
+        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE('Commencer analyse'!B52,"=", 'Commencer analyse'!D52),IF('Commencer analyse'!D52&lt;&gt;"",'Commencer analyse'!D52,""))</f>
         <v/>
       </c>
     </row>
     <row r="586" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A586" t="str">
-        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE('Commencer analyse'!B50,"=", 'Commencer analyse'!D50),IF('Commencer analyse'!D50&lt;&gt;"",'Commencer analyse'!D50,""))</f>
+        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE('Commencer analyse'!B53,"=", 'Commencer analyse'!D53),IF('Commencer analyse'!D53&lt;&gt;"",'Commencer analyse'!D53,""))</f>
         <v/>
       </c>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A587" t="str">
-        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE('Commencer analyse'!B51,"=", 'Commencer analyse'!D51),IF('Commencer analyse'!D51&lt;&gt;"",'Commencer analyse'!D51,""))</f>
+        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE('Commencer analyse'!B54,"=", 'Commencer analyse'!D54),IF('Commencer analyse'!D54&lt;&gt;"",'Commencer analyse'!D54,""))</f>
         <v/>
       </c>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A588" t="str">
-        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE('Commencer analyse'!B52,"=", 'Commencer analyse'!D52),IF('Commencer analyse'!D52&lt;&gt;"",'Commencer analyse'!D52,""))</f>
+        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE('Commencer analyse'!B55,"=", 'Commencer analyse'!D55),IF('Commencer analyse'!D55&lt;&gt;"",'Commencer analyse'!D55,""))</f>
         <v/>
       </c>
     </row>
     <row r="589" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A589" t="str">
-        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE('Commencer analyse'!B53,"=", 'Commencer analyse'!D53),IF('Commencer analyse'!D53&lt;&gt;"",'Commencer analyse'!D53,""))</f>
+        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE('Commencer analyse'!B56,"=", 'Commencer analyse'!D56),IF('Commencer analyse'!D56&lt;&gt;"",'Commencer analyse'!D56,""))</f>
         <v/>
       </c>
     </row>
     <row r="590" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A590" t="str">
-        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE('Commencer analyse'!B54,"=", 'Commencer analyse'!D54),IF('Commencer analyse'!D54&lt;&gt;"",'Commencer analyse'!D54,""))</f>
+        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE('Commencer analyse'!B57,"=", 'Commencer analyse'!D57),IF('Commencer analyse'!D57&lt;&gt;"",'Commencer analyse'!D57,""))</f>
         <v/>
       </c>
     </row>
     <row r="591" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A591" t="str">
-        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE('Commencer analyse'!B55,"=", 'Commencer analyse'!D55),IF('Commencer analyse'!D55&lt;&gt;"",'Commencer analyse'!D55,""))</f>
+        <f>IF('Commencer analyse'!B58&lt;&gt;"",CONCATENATE('Commencer analyse'!B58,"=", 'Commencer analyse'!D58),IF('Commencer analyse'!D58&lt;&gt;"",'Commencer analyse'!D58,""))</f>
         <v/>
       </c>
     </row>
     <row r="592" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A592" t="str">
-        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE('Commencer analyse'!B56,"=", 'Commencer analyse'!D56),IF('Commencer analyse'!D56&lt;&gt;"",'Commencer analyse'!D56,""))</f>
+        <f>IF('Commencer analyse'!B59&lt;&gt;"",CONCATENATE('Commencer analyse'!B59,"=", 'Commencer analyse'!D59),IF('Commencer analyse'!D59&lt;&gt;"",'Commencer analyse'!D59,""))</f>
         <v/>
       </c>
     </row>
     <row r="593" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A593" t="str">
-        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE('Commencer analyse'!B57,"=", 'Commencer analyse'!D57),IF('Commencer analyse'!D57&lt;&gt;"",'Commencer analyse'!D57,""))</f>
+        <f>IF('Commencer analyse'!B60&lt;&gt;"",CONCATENATE('Commencer analyse'!B60,"=", 'Commencer analyse'!D60),IF('Commencer analyse'!D60&lt;&gt;"",'Commencer analyse'!D60,""))</f>
         <v/>
       </c>
     </row>
@@ -39870,8 +39893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
   <dimension ref="A1:A737"/>
   <sheetViews>
-    <sheetView topLeftCell="A529" workbookViewId="0">
-      <selection activeCell="A550" sqref="A550:A553"/>
+    <sheetView topLeftCell="A571" workbookViewId="0">
+      <selection activeCell="A531" sqref="A531:A588"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43188,7 +43211,7 @@
     <row r="552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A552" t="str">
         <f>IF('Commencer analyse'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B23),".","_"),"=""", 'Commencer analyse'!B23,""";"),"")</f>
-        <v>public static final String WINDOW_START_ANALYSIS_CHOOSE_TYPE_TREATMENT_OPTIONAL_LIST_LABEL="window.start.analysis.choose.type.treatment.optional.list.label";</v>
+        <v>public static final String WINDOW_START_ANALYSIS_CHOOSE_TYPE_LEMMATIZATION_TREATMENT_OPTIONAL_LIST_LABEL="window.start.analysis.choose.type.lemmatization.treatment.optional.list.label";</v>
       </c>
     </row>
     <row r="553" spans="1:1" x14ac:dyDescent="0.25">
@@ -43198,212 +43221,212 @@
       </c>
     </row>
     <row r="554" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A554" t="e">
-        <f>IF('Commencer analyse'!#REF!&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!#REF!),".","_"),"=""", 'Commencer analyse'!#REF!,""";"),"")</f>
-        <v>#REF!</v>
+      <c r="A554" t="str">
+        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B25),".","_"),"=""", 'Commencer analyse'!B25,""";"),"")</f>
+        <v>public static final String WINDOW_START_ANALYSIS_CHOOSE_TYPE_TOKENIZATION_TREATMENT_OPTIONAL_LIST_LABEL="window.start.analysis.choose.type.tokenization.treatment.optional.list.label";</v>
       </c>
     </row>
     <row r="555" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A555" t="str">
-        <f>IF('Commencer analyse'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B25),".","_"),"=""", 'Commencer analyse'!B25,""";"),"")</f>
+        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B26),".","_"),"=""", 'Commencer analyse'!B26,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="556" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A556" t="str">
-        <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B26),".","_"),"=""", 'Commencer analyse'!B26,""";"),"")</f>
+        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B27),".","_"),"=""", 'Commencer analyse'!B27,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="557" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A557" t="str">
-        <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B27),".","_"),"=""", 'Commencer analyse'!B27,""";"),"")</f>
+        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B28),".","_"),"=""", 'Commencer analyse'!B28,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="558" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A558" t="str">
-        <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B28),".","_"),"=""", 'Commencer analyse'!B28,""";"),"")</f>
+        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B29),".","_"),"=""", 'Commencer analyse'!B29,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="559" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A559" t="str">
-        <f>IF('Commencer analyse'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B29),".","_"),"=""", 'Commencer analyse'!B29,""";"),"")</f>
+        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B30),".","_"),"=""", 'Commencer analyse'!B30,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="560" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A560" t="str">
-        <f>IF('Commencer analyse'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B30),".","_"),"=""", 'Commencer analyse'!B30,""";"),"")</f>
+        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B31),".","_"),"=""", 'Commencer analyse'!B31,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="561" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A561" t="str">
-        <f>IF('Commencer analyse'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B31),".","_"),"=""", 'Commencer analyse'!B31,""";"),"")</f>
+        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B32),".","_"),"=""", 'Commencer analyse'!B32,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="562" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A562" t="str">
-        <f>IF('Commencer analyse'!B32&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B32),".","_"),"=""", 'Commencer analyse'!B32,""";"),"")</f>
+        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B33),".","_"),"=""", 'Commencer analyse'!B33,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="563" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A563" t="str">
-        <f>IF('Commencer analyse'!B33&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B33),".","_"),"=""", 'Commencer analyse'!B33,""";"),"")</f>
+        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B34),".","_"),"=""", 'Commencer analyse'!B34,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="564" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A564" t="str">
-        <f>IF('Commencer analyse'!B34&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B34),".","_"),"=""", 'Commencer analyse'!B34,""";"),"")</f>
+        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B35),".","_"),"=""", 'Commencer analyse'!B35,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="565" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A565" t="str">
-        <f>IF('Commencer analyse'!B35&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B35),".","_"),"=""", 'Commencer analyse'!B35,""";"),"")</f>
+        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B36),".","_"),"=""", 'Commencer analyse'!B36,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="566" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A566" t="str">
-        <f>IF('Commencer analyse'!B36&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B36),".","_"),"=""", 'Commencer analyse'!B36,""";"),"")</f>
+        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B37),".","_"),"=""", 'Commencer analyse'!B37,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="567" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A567" t="str">
-        <f>IF('Commencer analyse'!B37&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B37),".","_"),"=""", 'Commencer analyse'!B37,""";"),"")</f>
+        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B38),".","_"),"=""", 'Commencer analyse'!B38,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="568" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A568" t="str">
-        <f>IF('Commencer analyse'!B38&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B38),".","_"),"=""", 'Commencer analyse'!B38,""";"),"")</f>
+        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B39),".","_"),"=""", 'Commencer analyse'!B39,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="569" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A569" t="str">
-        <f>IF('Commencer analyse'!B39&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B39),".","_"),"=""", 'Commencer analyse'!B39,""";"),"")</f>
+        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B40),".","_"),"=""", 'Commencer analyse'!B40,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="570" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A570" t="str">
-        <f>IF('Commencer analyse'!B40&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B40),".","_"),"=""", 'Commencer analyse'!B40,""";"),"")</f>
+        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B41),".","_"),"=""", 'Commencer analyse'!B41,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="571" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A571" t="str">
-        <f>IF('Commencer analyse'!B41&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B41),".","_"),"=""", 'Commencer analyse'!B41,""";"),"")</f>
+        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B42),".","_"),"=""", 'Commencer analyse'!B42,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="572" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A572" t="str">
-        <f>IF('Commencer analyse'!B42&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B42),".","_"),"=""", 'Commencer analyse'!B42,""";"),"")</f>
+        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B43),".","_"),"=""", 'Commencer analyse'!B43,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="573" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A573" t="str">
-        <f>IF('Commencer analyse'!B43&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B43),".","_"),"=""", 'Commencer analyse'!B43,""";"),"")</f>
+        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B44),".","_"),"=""", 'Commencer analyse'!B44,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="574" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A574" t="str">
-        <f>IF('Commencer analyse'!B44&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B44),".","_"),"=""", 'Commencer analyse'!B44,""";"),"")</f>
+        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B45),".","_"),"=""", 'Commencer analyse'!B45,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="575" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A575" t="str">
-        <f>IF('Commencer analyse'!B45&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B45),".","_"),"=""", 'Commencer analyse'!B45,""";"),"")</f>
+        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B46),".","_"),"=""", 'Commencer analyse'!B46,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="576" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A576" t="str">
-        <f>IF('Commencer analyse'!B46&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B46),".","_"),"=""", 'Commencer analyse'!B46,""";"),"")</f>
+        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B47),".","_"),"=""", 'Commencer analyse'!B47,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="577" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A577" t="str">
-        <f>IF('Commencer analyse'!B47&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B47),".","_"),"=""", 'Commencer analyse'!B47,""";"),"")</f>
+        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B48),".","_"),"=""", 'Commencer analyse'!B48,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="578" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A578" t="str">
-        <f>IF('Commencer analyse'!B48&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B48),".","_"),"=""", 'Commencer analyse'!B48,""";"),"")</f>
+        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B49),".","_"),"=""", 'Commencer analyse'!B49,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="579" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A579" t="str">
-        <f>IF('Commencer analyse'!B49&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B49),".","_"),"=""", 'Commencer analyse'!B49,""";"),"")</f>
+        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B50),".","_"),"=""", 'Commencer analyse'!B50,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="580" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A580" t="str">
-        <f>IF('Commencer analyse'!B50&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B50),".","_"),"=""", 'Commencer analyse'!B50,""";"),"")</f>
+        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B51),".","_"),"=""", 'Commencer analyse'!B51,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A581" t="str">
-        <f>IF('Commencer analyse'!B51&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B51),".","_"),"=""", 'Commencer analyse'!B51,""";"),"")</f>
+        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B52),".","_"),"=""", 'Commencer analyse'!B52,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A582" t="str">
-        <f>IF('Commencer analyse'!B52&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B52),".","_"),"=""", 'Commencer analyse'!B52,""";"),"")</f>
+        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B53),".","_"),"=""", 'Commencer analyse'!B53,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A583" t="str">
-        <f>IF('Commencer analyse'!B53&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B53),".","_"),"=""", 'Commencer analyse'!B53,""";"),"")</f>
+        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B54),".","_"),"=""", 'Commencer analyse'!B54,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A584" t="str">
-        <f>IF('Commencer analyse'!B54&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B54),".","_"),"=""", 'Commencer analyse'!B54,""";"),"")</f>
+        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B55),".","_"),"=""", 'Commencer analyse'!B55,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="585" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A585" t="str">
-        <f>IF('Commencer analyse'!B55&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B55),".","_"),"=""", 'Commencer analyse'!B55,""";"),"")</f>
+        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B56),".","_"),"=""", 'Commencer analyse'!B56,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="586" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A586" t="str">
-        <f>IF('Commencer analyse'!B56&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B56),".","_"),"=""", 'Commencer analyse'!B56,""";"),"")</f>
+        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B57),".","_"),"=""", 'Commencer analyse'!B57,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A587" t="str">
-        <f>IF('Commencer analyse'!B57&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B57),".","_"),"=""", 'Commencer analyse'!B57,""";"),"")</f>
+        <f>IF('Commencer analyse'!B58&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B58),".","_"),"=""", 'Commencer analyse'!B58,""";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A588" t="str">
-        <f>IF('Importer Excel'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Importer Excel'!B2),".","_"),"=""", 'Importer Excel'!B2,""";"),"")</f>
+        <f>IF('Commencer analyse'!B59&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B59),".","_"),"=""", 'Commencer analyse'!B59,""";"),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Avancement sur le module d'analyse : - Création de la fenêtre d'affichage des résultats (WIP)
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\IdeaProjects\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2A9016-9882-42DF-890B-982217CFE061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4318F845-45A9-4121-B633-46CB7E78255A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="19" activeTab="26" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="20" activeTab="25" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,10 @@
     <sheet name="StopWords" sheetId="27" r:id="rId23"/>
     <sheet name="Radicaux" sheetId="29" r:id="rId24"/>
     <sheet name="Radicaux par classe" sheetId="30" r:id="rId25"/>
-    <sheet name="FR_Properties" sheetId="14" r:id="rId26"/>
-    <sheet name="ES_Properties" sheetId="16" r:id="rId27"/>
-    <sheet name="Constants" sheetId="18" r:id="rId28"/>
+    <sheet name="Resultat Analyse" sheetId="31" r:id="rId26"/>
+    <sheet name="FR_Properties" sheetId="14" r:id="rId27"/>
+    <sheet name="ES_Properties" sheetId="16" r:id="rId28"/>
+    <sheet name="Constants" sheetId="18" r:id="rId29"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="1071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="1092">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -3265,6 +3266,69 @@
   </si>
   <si>
     <t>Elección del tipo de lista para tokens</t>
+  </si>
+  <si>
+    <t>Detail des résultats</t>
+  </si>
+  <si>
+    <t>Detalle de resultados</t>
+  </si>
+  <si>
+    <t>Token</t>
+  </si>
+  <si>
+    <t>Numéro de formes qui apparaissent</t>
+  </si>
+  <si>
+    <t>Número de formas que aparecen</t>
+  </si>
+  <si>
+    <t>window.result.token.analysis.panel.title</t>
+  </si>
+  <si>
+    <t>window.result.token.analysis.table.panel.title</t>
+  </si>
+  <si>
+    <t>window.result.token.analysis.table.header.column.1.label</t>
+  </si>
+  <si>
+    <t>window.result.token.analysis.table.header.column.2.label</t>
+  </si>
+  <si>
+    <t>window.result.token.total.tokens.label</t>
+  </si>
+  <si>
+    <t>Número total de tokens</t>
+  </si>
+  <si>
+    <t>window.result.token.total.words.label</t>
+  </si>
+  <si>
+    <t>Nombre total de tokens</t>
+  </si>
+  <si>
+    <t>Número total de palabras</t>
+  </si>
+  <si>
+    <t>window.result.token.total.panel.title</t>
+  </si>
+  <si>
+    <t>Résultat de l'analyse des tokens</t>
+  </si>
+  <si>
+    <t>Resultado del análisis de tokens</t>
+  </si>
+  <si>
+    <t>Résultat global</t>
+  </si>
+  <si>
+    <t>Resultado general</t>
+  </si>
+  <si>
+    <t>Nombre total de formes</t>
+  </si>
+  <si>
+    <t>Número total de formas</t>
   </si>
 </sst>
 </file>
@@ -24756,6 +24820,19 @@
 </table>
 </file>
 
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{4CE1A1C8-FF88-4680-BE98-CCE7813CCC24}" name="Tableau15212223252627" displayName="Tableau15212223252627" ref="A1:D25" totalsRowShown="0">
+  <autoFilter ref="A1:D25" xr:uid="{1C0F8CDE-76C5-4629-A51B-1F75FFD867D6}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{531C70F4-AA20-4692-981E-2CB62CFC9C8D}" name="Numero"/>
+    <tableColumn id="2" xr3:uid="{EC2CF2DF-AD63-4EB8-B556-C89FF21D5C0D}" name="Code"/>
+    <tableColumn id="3" xr3:uid="{1CFE3E41-9DC5-46D5-83D1-13021F338E80}" name="Français"/>
+    <tableColumn id="4" xr3:uid="{98D0C9D3-B7A7-4B84-8040-64B7913FD4CB}" name="Español"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A527987-5451-48A7-ACFD-33D9B89F9100}" name="Tableau24" displayName="Tableau24" ref="A1:D22" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A1:D22" xr:uid="{A671D94F-C6D5-475C-A6B8-C3BE74B935F9}"/>
@@ -30540,11 +30617,159 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CC416E-27E9-484D-A35C-2643F99323FB}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="66.5703125" customWidth="1"/>
+    <col min="3" max="3" width="77.85546875" customWidth="1"/>
+    <col min="4" max="4" width="88.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904B2FA-CBC2-495A-A197-D0CDD47EB1AE}">
-  <dimension ref="A1:A781"/>
+  <dimension ref="A1:A824"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A589" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A557" sqref="A1:A781"/>
+    <sheetView showZeros="0" topLeftCell="A775" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A794" sqref="A1:A824"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35238,18 +35463,276 @@
         <v/>
       </c>
     </row>
+    <row r="782" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A782" t="str">
+        <f>IF('Resultat Analyse'!B2&lt;&gt;"",CONCATENATE('Resultat Analyse'!B2,"=", 'Resultat Analyse'!C2),IF('Resultat Analyse'!C2&lt;&gt;"",'Resultat Analyse'!C2,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="783" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A783" t="str">
+        <f>IF('Resultat Analyse'!B3&lt;&gt;"",CONCATENATE('Resultat Analyse'!B3,"=", 'Resultat Analyse'!C3),IF('Resultat Analyse'!C3&lt;&gt;"",'Resultat Analyse'!C3,""))</f>
+        <v>window.result.token.analysis.panel.title=Résultat de l'analyse des tokens</v>
+      </c>
+    </row>
+    <row r="784" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A784" t="str">
+        <f>IF('Resultat Analyse'!B4&lt;&gt;"",CONCATENATE('Resultat Analyse'!B4,"=", 'Resultat Analyse'!C4),IF('Resultat Analyse'!C4&lt;&gt;"",'Resultat Analyse'!C4,""))</f>
+        <v>window.result.token.analysis.table.panel.title=Detail des résultats</v>
+      </c>
+    </row>
+    <row r="785" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A785" t="str">
+        <f>IF('Resultat Analyse'!B5&lt;&gt;"",CONCATENATE('Resultat Analyse'!B5,"=", 'Resultat Analyse'!C5),IF('Resultat Analyse'!C5&lt;&gt;"",'Resultat Analyse'!C5,""))</f>
+        <v>window.result.token.analysis.table.header.column.1.label=Token</v>
+      </c>
+    </row>
+    <row r="786" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A786" t="str">
+        <f>IF('Resultat Analyse'!B6&lt;&gt;"",CONCATENATE('Resultat Analyse'!B6,"=", 'Resultat Analyse'!C6),IF('Resultat Analyse'!C6&lt;&gt;"",'Resultat Analyse'!C6,""))</f>
+        <v>window.result.token.analysis.table.header.column.2.label=Numéro de formes qui apparaissent</v>
+      </c>
+    </row>
+    <row r="787" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A787" t="str">
+        <f>IF('Resultat Analyse'!B7&lt;&gt;"",CONCATENATE('Resultat Analyse'!B7,"=", 'Resultat Analyse'!C7),IF('Resultat Analyse'!C7&lt;&gt;"",'Resultat Analyse'!C7,""))</f>
+        <v>window.result.token.total.tokens.label=Nombre total de tokens</v>
+      </c>
+    </row>
+    <row r="788" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A788" t="str">
+        <f>IF('Resultat Analyse'!B8&lt;&gt;"",CONCATENATE('Resultat Analyse'!B8,"=", 'Resultat Analyse'!C8),IF('Resultat Analyse'!C8&lt;&gt;"",'Resultat Analyse'!C8,""))</f>
+        <v>window.result.token.total.words.label=Nombre total de formes</v>
+      </c>
+    </row>
+    <row r="789" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A789" t="str">
+        <f>IF('Resultat Analyse'!B9&lt;&gt;"",CONCATENATE('Resultat Analyse'!B9,"=", 'Resultat Analyse'!C9),IF('Resultat Analyse'!C9&lt;&gt;"",'Resultat Analyse'!C9,""))</f>
+        <v>window.result.token.total.panel.title=Résultat global</v>
+      </c>
+    </row>
+    <row r="790" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A790" t="str">
+        <f>IF('Resultat Analyse'!B10&lt;&gt;"",CONCATENATE('Resultat Analyse'!B10,"=", 'Resultat Analyse'!C10),IF('Resultat Analyse'!C10&lt;&gt;"",'Resultat Analyse'!C10,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="791" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A791" t="str">
+        <f>IF('Resultat Analyse'!B11&lt;&gt;"",CONCATENATE('Resultat Analyse'!B11,"=", 'Resultat Analyse'!C11),IF('Resultat Analyse'!C11&lt;&gt;"",'Resultat Analyse'!C11,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="792" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A792" t="str">
+        <f>IF('Resultat Analyse'!B12&lt;&gt;"",CONCATENATE('Resultat Analyse'!B12,"=", 'Resultat Analyse'!C12),IF('Resultat Analyse'!C12&lt;&gt;"",'Resultat Analyse'!C12,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="793" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A793" t="str">
+        <f>IF('Resultat Analyse'!B13&lt;&gt;"",CONCATENATE('Resultat Analyse'!B13,"=", 'Resultat Analyse'!C13),IF('Resultat Analyse'!C13&lt;&gt;"",'Resultat Analyse'!C13,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="794" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A794" t="str">
+        <f>IF('Resultat Analyse'!B14&lt;&gt;"",CONCATENATE('Resultat Analyse'!B14,"=", 'Resultat Analyse'!C14),IF('Resultat Analyse'!C14&lt;&gt;"",'Resultat Analyse'!C14,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="795" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A795" t="str">
+        <f>IF('Resultat Analyse'!B15&lt;&gt;"",CONCATENATE('Resultat Analyse'!B15,"=", 'Resultat Analyse'!C15),IF('Resultat Analyse'!C15&lt;&gt;"",'Resultat Analyse'!C15,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="796" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A796" t="str">
+        <f>IF('Resultat Analyse'!B16&lt;&gt;"",CONCATENATE('Resultat Analyse'!B16,"=", 'Resultat Analyse'!C16),IF('Resultat Analyse'!C16&lt;&gt;"",'Resultat Analyse'!C16,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="797" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A797" t="str">
+        <f>IF('Resultat Analyse'!B17&lt;&gt;"",CONCATENATE('Resultat Analyse'!B17,"=", 'Resultat Analyse'!C17),IF('Resultat Analyse'!C17&lt;&gt;"",'Resultat Analyse'!C17,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="798" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A798" t="str">
+        <f>IF('Resultat Analyse'!B18&lt;&gt;"",CONCATENATE('Resultat Analyse'!B18,"=", 'Resultat Analyse'!C18),IF('Resultat Analyse'!C18&lt;&gt;"",'Resultat Analyse'!C18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="799" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A799" t="str">
+        <f>IF('Resultat Analyse'!B19&lt;&gt;"",CONCATENATE('Resultat Analyse'!B19,"=", 'Resultat Analyse'!C19),IF('Resultat Analyse'!C19&lt;&gt;"",'Resultat Analyse'!C19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="800" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A800" t="str">
+        <f>IF('Resultat Analyse'!B20&lt;&gt;"",CONCATENATE('Resultat Analyse'!B20,"=", 'Resultat Analyse'!C20),IF('Resultat Analyse'!C20&lt;&gt;"",'Resultat Analyse'!C20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="801" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A801" t="str">
+        <f>IF('Resultat Analyse'!B21&lt;&gt;"",CONCATENATE('Resultat Analyse'!B21,"=", 'Resultat Analyse'!C21),IF('Resultat Analyse'!C21&lt;&gt;"",'Resultat Analyse'!C21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="802" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A802" t="str">
+        <f>IF('Resultat Analyse'!B22&lt;&gt;"",CONCATENATE('Resultat Analyse'!B22,"=", 'Resultat Analyse'!C22),IF('Resultat Analyse'!C22&lt;&gt;"",'Resultat Analyse'!C22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="803" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A803" t="str">
+        <f>IF('Resultat Analyse'!B23&lt;&gt;"",CONCATENATE('Resultat Analyse'!B23,"=", 'Resultat Analyse'!C23),IF('Resultat Analyse'!C23&lt;&gt;"",'Resultat Analyse'!C23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="804" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A804" t="str">
+        <f>IF('Resultat Analyse'!B24&lt;&gt;"",CONCATENATE('Resultat Analyse'!B24,"=", 'Resultat Analyse'!C24),IF('Resultat Analyse'!C24&lt;&gt;"",'Resultat Analyse'!C24,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="805" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A805" t="str">
+        <f>IF('Resultat Analyse'!B25&lt;&gt;"",CONCATENATE('Resultat Analyse'!B25,"=", 'Resultat Analyse'!C25),IF('Resultat Analyse'!C25&lt;&gt;"",'Resultat Analyse'!C25,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="806" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A806" t="str">
+        <f>IF('Resultat Analyse'!B26&lt;&gt;"",CONCATENATE('Resultat Analyse'!B26,"=", 'Resultat Analyse'!C26),IF('Resultat Analyse'!C26&lt;&gt;"",'Resultat Analyse'!C26,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="807" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A807" t="str">
+        <f>IF('Resultat Analyse'!B27&lt;&gt;"",CONCATENATE('Resultat Analyse'!B27,"=", 'Resultat Analyse'!C27),IF('Resultat Analyse'!C27&lt;&gt;"",'Resultat Analyse'!C27,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="808" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A808" t="str">
+        <f>IF('Resultat Analyse'!B28&lt;&gt;"",CONCATENATE('Resultat Analyse'!B28,"=", 'Resultat Analyse'!C28),IF('Resultat Analyse'!C28&lt;&gt;"",'Resultat Analyse'!C28,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="809" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A809" t="str">
+        <f>IF('Resultat Analyse'!B29&lt;&gt;"",CONCATENATE('Resultat Analyse'!B29,"=", 'Resultat Analyse'!C29),IF('Resultat Analyse'!C29&lt;&gt;"",'Resultat Analyse'!C29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="810" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A810" t="str">
+        <f>IF('Resultat Analyse'!B30&lt;&gt;"",CONCATENATE('Resultat Analyse'!B30,"=", 'Resultat Analyse'!C30),IF('Resultat Analyse'!C30&lt;&gt;"",'Resultat Analyse'!C30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="811" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A811" t="str">
+        <f>IF('Resultat Analyse'!B31&lt;&gt;"",CONCATENATE('Resultat Analyse'!B31,"=", 'Resultat Analyse'!C31),IF('Resultat Analyse'!C31&lt;&gt;"",'Resultat Analyse'!C31,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="812" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A812" t="str">
+        <f>IF('Resultat Analyse'!B32&lt;&gt;"",CONCATENATE('Resultat Analyse'!B32,"=", 'Resultat Analyse'!C32),IF('Resultat Analyse'!C32&lt;&gt;"",'Resultat Analyse'!C32,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="813" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A813" t="str">
+        <f>IF('Resultat Analyse'!B33&lt;&gt;"",CONCATENATE('Resultat Analyse'!B33,"=", 'Resultat Analyse'!C33),IF('Resultat Analyse'!C33&lt;&gt;"",'Resultat Analyse'!C33,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="814" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A814" t="str">
+        <f>IF('Resultat Analyse'!B34&lt;&gt;"",CONCATENATE('Resultat Analyse'!B34,"=", 'Resultat Analyse'!C34),IF('Resultat Analyse'!C34&lt;&gt;"",'Resultat Analyse'!C34,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="815" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A815" t="str">
+        <f>IF('Resultat Analyse'!B35&lt;&gt;"",CONCATENATE('Resultat Analyse'!B35,"=", 'Resultat Analyse'!C35),IF('Resultat Analyse'!C35&lt;&gt;"",'Resultat Analyse'!C35,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="816" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A816" t="str">
+        <f>IF('Resultat Analyse'!B36&lt;&gt;"",CONCATENATE('Resultat Analyse'!B36,"=", 'Resultat Analyse'!C36),IF('Resultat Analyse'!C36&lt;&gt;"",'Resultat Analyse'!C36,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="817" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A817" t="str">
+        <f>IF('Resultat Analyse'!B37&lt;&gt;"",CONCATENATE('Resultat Analyse'!B37,"=", 'Resultat Analyse'!C37),IF('Resultat Analyse'!C37&lt;&gt;"",'Resultat Analyse'!C37,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="818" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A818" t="str">
+        <f>IF('Resultat Analyse'!B38&lt;&gt;"",CONCATENATE('Resultat Analyse'!B38,"=", 'Resultat Analyse'!C38),IF('Resultat Analyse'!C38&lt;&gt;"",'Resultat Analyse'!C38,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="819" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A819" t="str">
+        <f>IF('Resultat Analyse'!B39&lt;&gt;"",CONCATENATE('Resultat Analyse'!B39,"=", 'Resultat Analyse'!C39),IF('Resultat Analyse'!C39&lt;&gt;"",'Resultat Analyse'!C39,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="820" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A820" t="str">
+        <f>IF('Resultat Analyse'!B40&lt;&gt;"",CONCATENATE('Resultat Analyse'!B40,"=", 'Resultat Analyse'!C40),IF('Resultat Analyse'!C40&lt;&gt;"",'Resultat Analyse'!C40,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="821" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A821" t="str">
+        <f>IF('Resultat Analyse'!B41&lt;&gt;"",CONCATENATE('Resultat Analyse'!B41,"=", 'Resultat Analyse'!C41),IF('Resultat Analyse'!C41&lt;&gt;"",'Resultat Analyse'!C41,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="822" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A822" t="str">
+        <f>IF('Resultat Analyse'!B42&lt;&gt;"",CONCATENATE('Resultat Analyse'!B42,"=", 'Resultat Analyse'!C42),IF('Resultat Analyse'!C42&lt;&gt;"",'Resultat Analyse'!C42,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="823" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A823" t="str">
+        <f>IF('Resultat Analyse'!B43&lt;&gt;"",CONCATENATE('Resultat Analyse'!B43,"=", 'Resultat Analyse'!C43),IF('Resultat Analyse'!C43&lt;&gt;"",'Resultat Analyse'!C43,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="824" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A824" t="str">
+        <f>IF('Resultat Analyse'!B44&lt;&gt;"",CONCATENATE('Resultat Analyse'!B44,"=", 'Resultat Analyse'!C44),IF('Resultat Analyse'!C44&lt;&gt;"",'Resultat Analyse'!C44,""))</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
-  <dimension ref="A1:A771"/>
+  <dimension ref="A1:A816"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A519" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A541" sqref="A1:A771"/>
+    <sheetView showZeros="0" topLeftCell="A765" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A779" sqref="A1:A816"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39883,18 +40366,288 @@
         <v/>
       </c>
     </row>
+    <row r="772" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A772" t="str">
+        <f>IF('Resultat Analyse'!B2&lt;&gt;"",CONCATENATE('Resultat Analyse'!B2,"=", 'Resultat Analyse'!D2),IF('Resultat Analyse'!D2&lt;&gt;"",'Resultat Analyse'!D2,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="773" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A773" t="str">
+        <f>IF('Resultat Analyse'!B3&lt;&gt;"",CONCATENATE('Resultat Analyse'!B3,"=", 'Resultat Analyse'!D3),IF('Resultat Analyse'!D3&lt;&gt;"",'Resultat Analyse'!D3,""))</f>
+        <v>window.result.token.analysis.panel.title=Resultado del análisis de tokens</v>
+      </c>
+    </row>
+    <row r="774" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A774" t="str">
+        <f>IF('Resultat Analyse'!B4&lt;&gt;"",CONCATENATE('Resultat Analyse'!B4,"=", 'Resultat Analyse'!D4),IF('Resultat Analyse'!D4&lt;&gt;"",'Resultat Analyse'!D4,""))</f>
+        <v>window.result.token.analysis.table.panel.title=Detalle de resultados</v>
+      </c>
+    </row>
+    <row r="775" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A775" t="str">
+        <f>IF('Resultat Analyse'!B5&lt;&gt;"",CONCATENATE('Resultat Analyse'!B5,"=", 'Resultat Analyse'!D5),IF('Resultat Analyse'!D5&lt;&gt;"",'Resultat Analyse'!D5,""))</f>
+        <v>window.result.token.analysis.table.header.column.1.label=Token</v>
+      </c>
+    </row>
+    <row r="776" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A776" t="str">
+        <f>IF('Resultat Analyse'!B6&lt;&gt;"",CONCATENATE('Resultat Analyse'!B6,"=", 'Resultat Analyse'!D6),IF('Resultat Analyse'!D6&lt;&gt;"",'Resultat Analyse'!D6,""))</f>
+        <v>window.result.token.analysis.table.header.column.2.label=Número de formas que aparecen</v>
+      </c>
+    </row>
+    <row r="777" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A777" t="str">
+        <f>IF('Resultat Analyse'!B7&lt;&gt;"",CONCATENATE('Resultat Analyse'!B7,"=", 'Resultat Analyse'!D7),IF('Resultat Analyse'!D7&lt;&gt;"",'Resultat Analyse'!D7,""))</f>
+        <v>window.result.token.total.tokens.label=Número total de tokens</v>
+      </c>
+    </row>
+    <row r="778" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A778" t="str">
+        <f>IF('Resultat Analyse'!B8&lt;&gt;"",CONCATENATE('Resultat Analyse'!B8,"=", 'Resultat Analyse'!D8),IF('Resultat Analyse'!D8&lt;&gt;"",'Resultat Analyse'!D8,""))</f>
+        <v>window.result.token.total.words.label=Número total de formas</v>
+      </c>
+    </row>
+    <row r="779" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A779" t="str">
+        <f>IF('Resultat Analyse'!B9&lt;&gt;"",CONCATENATE('Resultat Analyse'!B9,"=", 'Resultat Analyse'!D9),IF('Resultat Analyse'!D9&lt;&gt;"",'Resultat Analyse'!D9,""))</f>
+        <v>window.result.token.total.panel.title=Resultado general</v>
+      </c>
+    </row>
+    <row r="780" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A780" t="str">
+        <f>IF('Resultat Analyse'!B10&lt;&gt;"",CONCATENATE('Resultat Analyse'!B10,"=", 'Resultat Analyse'!D10),IF('Resultat Analyse'!D10&lt;&gt;"",'Resultat Analyse'!D10,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="781" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A781" t="str">
+        <f>IF('Resultat Analyse'!B11&lt;&gt;"",CONCATENATE('Resultat Analyse'!B11,"=", 'Resultat Analyse'!D11),IF('Resultat Analyse'!D11&lt;&gt;"",'Resultat Analyse'!D11,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="782" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A782" t="str">
+        <f>IF('Resultat Analyse'!B12&lt;&gt;"",CONCATENATE('Resultat Analyse'!B12,"=", 'Resultat Analyse'!D12),IF('Resultat Analyse'!D12&lt;&gt;"",'Resultat Analyse'!D12,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="783" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A783" t="str">
+        <f>IF('Resultat Analyse'!B13&lt;&gt;"",CONCATENATE('Resultat Analyse'!B13,"=", 'Resultat Analyse'!D13),IF('Resultat Analyse'!D13&lt;&gt;"",'Resultat Analyse'!D13,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="784" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A784" t="str">
+        <f>IF('Resultat Analyse'!B14&lt;&gt;"",CONCATENATE('Resultat Analyse'!B14,"=", 'Resultat Analyse'!D14),IF('Resultat Analyse'!D14&lt;&gt;"",'Resultat Analyse'!D14,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="785" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A785" t="str">
+        <f>IF('Resultat Analyse'!B15&lt;&gt;"",CONCATENATE('Resultat Analyse'!B15,"=", 'Resultat Analyse'!D15),IF('Resultat Analyse'!D15&lt;&gt;"",'Resultat Analyse'!D15,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="786" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A786" t="str">
+        <f>IF('Resultat Analyse'!B16&lt;&gt;"",CONCATENATE('Resultat Analyse'!B16,"=", 'Resultat Analyse'!D16),IF('Resultat Analyse'!D16&lt;&gt;"",'Resultat Analyse'!D16,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="787" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A787" t="str">
+        <f>IF('Resultat Analyse'!B17&lt;&gt;"",CONCATENATE('Resultat Analyse'!B17,"=", 'Resultat Analyse'!D17),IF('Resultat Analyse'!D17&lt;&gt;"",'Resultat Analyse'!D17,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="788" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A788" t="str">
+        <f>IF('Resultat Analyse'!B18&lt;&gt;"",CONCATENATE('Resultat Analyse'!B18,"=", 'Resultat Analyse'!D18),IF('Resultat Analyse'!D18&lt;&gt;"",'Resultat Analyse'!D18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="789" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A789" t="str">
+        <f>IF('Resultat Analyse'!B19&lt;&gt;"",CONCATENATE('Resultat Analyse'!B19,"=", 'Resultat Analyse'!D19),IF('Resultat Analyse'!D19&lt;&gt;"",'Resultat Analyse'!D19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="790" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A790" t="str">
+        <f>IF('Resultat Analyse'!B20&lt;&gt;"",CONCATENATE('Resultat Analyse'!B20,"=", 'Resultat Analyse'!D20),IF('Resultat Analyse'!D20&lt;&gt;"",'Resultat Analyse'!D20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="791" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A791" t="str">
+        <f>IF('Resultat Analyse'!B21&lt;&gt;"",CONCATENATE('Resultat Analyse'!B21,"=", 'Resultat Analyse'!D21),IF('Resultat Analyse'!D21&lt;&gt;"",'Resultat Analyse'!D21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="792" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A792" t="str">
+        <f>IF('Resultat Analyse'!B22&lt;&gt;"",CONCATENATE('Resultat Analyse'!B22,"=", 'Resultat Analyse'!D22),IF('Resultat Analyse'!D22&lt;&gt;"",'Resultat Analyse'!D22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="793" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A793" t="str">
+        <f>IF('Resultat Analyse'!B23&lt;&gt;"",CONCATENATE('Resultat Analyse'!B23,"=", 'Resultat Analyse'!D23),IF('Resultat Analyse'!D23&lt;&gt;"",'Resultat Analyse'!D23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="794" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A794" t="str">
+        <f>IF('Resultat Analyse'!B24&lt;&gt;"",CONCATENATE('Resultat Analyse'!B24,"=", 'Resultat Analyse'!D24),IF('Resultat Analyse'!D24&lt;&gt;"",'Resultat Analyse'!D24,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="795" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A795" t="str">
+        <f>IF('Resultat Analyse'!B25&lt;&gt;"",CONCATENATE('Resultat Analyse'!B25,"=", 'Resultat Analyse'!D25),IF('Resultat Analyse'!D25&lt;&gt;"",'Resultat Analyse'!D25,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="796" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A796" t="str">
+        <f>IF('Resultat Analyse'!B26&lt;&gt;"",CONCATENATE('Resultat Analyse'!B26,"=", 'Resultat Analyse'!D26),IF('Resultat Analyse'!D26&lt;&gt;"",'Resultat Analyse'!D26,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="797" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A797" t="str">
+        <f>IF('Resultat Analyse'!B27&lt;&gt;"",CONCATENATE('Resultat Analyse'!B27,"=", 'Resultat Analyse'!D27),IF('Resultat Analyse'!D27&lt;&gt;"",'Resultat Analyse'!D27,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="798" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A798" t="str">
+        <f>IF('Resultat Analyse'!B28&lt;&gt;"",CONCATENATE('Resultat Analyse'!B28,"=", 'Resultat Analyse'!D28),IF('Resultat Analyse'!D28&lt;&gt;"",'Resultat Analyse'!D28,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="799" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A799" t="str">
+        <f>IF('Resultat Analyse'!B29&lt;&gt;"",CONCATENATE('Resultat Analyse'!B29,"=", 'Resultat Analyse'!D29),IF('Resultat Analyse'!D29&lt;&gt;"",'Resultat Analyse'!D29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="800" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A800" t="str">
+        <f>IF('Resultat Analyse'!B30&lt;&gt;"",CONCATENATE('Resultat Analyse'!B30,"=", 'Resultat Analyse'!D30),IF('Resultat Analyse'!D30&lt;&gt;"",'Resultat Analyse'!D30,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="801" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A801" t="str">
+        <f>IF('Resultat Analyse'!B31&lt;&gt;"",CONCATENATE('Resultat Analyse'!B31,"=", 'Resultat Analyse'!D31),IF('Resultat Analyse'!D31&lt;&gt;"",'Resultat Analyse'!D31,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="802" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A802" t="str">
+        <f>IF('Resultat Analyse'!B32&lt;&gt;"",CONCATENATE('Resultat Analyse'!B32,"=", 'Resultat Analyse'!D32),IF('Resultat Analyse'!D32&lt;&gt;"",'Resultat Analyse'!D32,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="803" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A803" t="str">
+        <f>IF('Resultat Analyse'!B33&lt;&gt;"",CONCATENATE('Resultat Analyse'!B33,"=", 'Resultat Analyse'!D33),IF('Resultat Analyse'!D33&lt;&gt;"",'Resultat Analyse'!D33,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="804" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A804" t="str">
+        <f>IF('Resultat Analyse'!B34&lt;&gt;"",CONCATENATE('Resultat Analyse'!B34,"=", 'Resultat Analyse'!D34),IF('Resultat Analyse'!D34&lt;&gt;"",'Resultat Analyse'!D34,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="805" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A805" t="str">
+        <f>IF('Resultat Analyse'!B35&lt;&gt;"",CONCATENATE('Resultat Analyse'!B35,"=", 'Resultat Analyse'!D35),IF('Resultat Analyse'!D35&lt;&gt;"",'Resultat Analyse'!D35,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="806" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A806" t="str">
+        <f>IF('Resultat Analyse'!B36&lt;&gt;"",CONCATENATE('Resultat Analyse'!B36,"=", 'Resultat Analyse'!D36),IF('Resultat Analyse'!D36&lt;&gt;"",'Resultat Analyse'!D36,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="807" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A807" t="str">
+        <f>IF('Resultat Analyse'!B37&lt;&gt;"",CONCATENATE('Resultat Analyse'!B37,"=", 'Resultat Analyse'!D37),IF('Resultat Analyse'!D37&lt;&gt;"",'Resultat Analyse'!D37,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="808" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A808" t="str">
+        <f>IF('Resultat Analyse'!B38&lt;&gt;"",CONCATENATE('Resultat Analyse'!B38,"=", 'Resultat Analyse'!D38),IF('Resultat Analyse'!D38&lt;&gt;"",'Resultat Analyse'!D38,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="809" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A809" t="str">
+        <f>IF('Resultat Analyse'!B39&lt;&gt;"",CONCATENATE('Resultat Analyse'!B39,"=", 'Resultat Analyse'!D39),IF('Resultat Analyse'!D39&lt;&gt;"",'Resultat Analyse'!D39,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="810" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A810" t="str">
+        <f>IF('Resultat Analyse'!B40&lt;&gt;"",CONCATENATE('Resultat Analyse'!B40,"=", 'Resultat Analyse'!D40),IF('Resultat Analyse'!D40&lt;&gt;"",'Resultat Analyse'!D40,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="811" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A811" t="str">
+        <f>IF('Resultat Analyse'!B41&lt;&gt;"",CONCATENATE('Resultat Analyse'!B41,"=", 'Resultat Analyse'!D41),IF('Resultat Analyse'!D41&lt;&gt;"",'Resultat Analyse'!D41,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="812" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A812" t="str">
+        <f>IF('Resultat Analyse'!B42&lt;&gt;"",CONCATENATE('Resultat Analyse'!B42,"=", 'Resultat Analyse'!D42),IF('Resultat Analyse'!D42&lt;&gt;"",'Resultat Analyse'!D42,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="813" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A813" t="str">
+        <f>IF('Resultat Analyse'!B43&lt;&gt;"",CONCATENATE('Resultat Analyse'!B43,"=", 'Resultat Analyse'!D43),IF('Resultat Analyse'!D43&lt;&gt;"",'Resultat Analyse'!D43,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="814" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A814" t="str">
+        <f>IF('Resultat Analyse'!B44&lt;&gt;"",CONCATENATE('Resultat Analyse'!B44,"=", 'Resultat Analyse'!D44),IF('Resultat Analyse'!D44&lt;&gt;"",'Resultat Analyse'!D44,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="815" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A815" t="str">
+        <f>IF('Resultat Analyse'!B45&lt;&gt;"",CONCATENATE('Resultat Analyse'!B45,"=", 'Resultat Analyse'!D45),IF('Resultat Analyse'!D45&lt;&gt;"",'Resultat Analyse'!D45,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="816" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A816" t="str">
+        <f>IF('Resultat Analyse'!B46&lt;&gt;"",CONCATENATE('Resultat Analyse'!B46,"=", 'Resultat Analyse'!D46),IF('Resultat Analyse'!D46&lt;&gt;"",'Resultat Analyse'!D46,""))</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
-  <dimension ref="A1:A737"/>
+  <dimension ref="A1:A858"/>
   <sheetViews>
-    <sheetView topLeftCell="A571" workbookViewId="0">
-      <selection activeCell="A531" sqref="A531:A588"/>
+    <sheetView topLeftCell="A723" workbookViewId="0">
+      <selection activeCell="A739" sqref="A739:A745"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44321,6 +45074,732 @@
     <row r="737" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A737" t="str">
         <f>IF('Radicaux par classe'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Radicaux par classe'!B25),".","_"),"=""", 'Radicaux par classe'!B25,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="738" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A738" t="str">
+        <f>IF('Resultat Analyse'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B2),".","_"),"=""", 'Resultat Analyse'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="739" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A739" t="str">
+        <f>IF('Resultat Analyse'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B3),".","_"),"=""", 'Resultat Analyse'!B3,""";"),"")</f>
+        <v>public static final String WINDOW_RESULT_TOKEN_ANALYSIS_PANEL_TITLE="window.result.token.analysis.panel.title";</v>
+      </c>
+    </row>
+    <row r="740" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A740" t="str">
+        <f>IF('Resultat Analyse'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B4),".","_"),"=""", 'Resultat Analyse'!B4,""";"),"")</f>
+        <v>public static final String WINDOW_RESULT_TOKEN_ANALYSIS_TABLE_PANEL_TITLE="window.result.token.analysis.table.panel.title";</v>
+      </c>
+    </row>
+    <row r="741" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A741" t="str">
+        <f>IF('Resultat Analyse'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B5),".","_"),"=""", 'Resultat Analyse'!B5,""";"),"")</f>
+        <v>public static final String WINDOW_RESULT_TOKEN_ANALYSIS_TABLE_HEADER_COLUMN_1_LABEL="window.result.token.analysis.table.header.column.1.label";</v>
+      </c>
+    </row>
+    <row r="742" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A742" t="str">
+        <f>IF('Resultat Analyse'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B6),".","_"),"=""", 'Resultat Analyse'!B6,""";"),"")</f>
+        <v>public static final String WINDOW_RESULT_TOKEN_ANALYSIS_TABLE_HEADER_COLUMN_2_LABEL="window.result.token.analysis.table.header.column.2.label";</v>
+      </c>
+    </row>
+    <row r="743" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A743" t="str">
+        <f>IF('Resultat Analyse'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B7),".","_"),"=""", 'Resultat Analyse'!B7,""";"),"")</f>
+        <v>public static final String WINDOW_RESULT_TOKEN_TOTAL_TOKENS_LABEL="window.result.token.total.tokens.label";</v>
+      </c>
+    </row>
+    <row r="744" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A744" t="str">
+        <f>IF('Resultat Analyse'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B8),".","_"),"=""", 'Resultat Analyse'!B8,""";"),"")</f>
+        <v>public static final String WINDOW_RESULT_TOKEN_TOTAL_WORDS_LABEL="window.result.token.total.words.label";</v>
+      </c>
+    </row>
+    <row r="745" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A745" t="str">
+        <f>IF('Resultat Analyse'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B9),".","_"),"=""", 'Resultat Analyse'!B9,""";"),"")</f>
+        <v>public static final String WINDOW_RESULT_TOKEN_TOTAL_PANEL_TITLE="window.result.token.total.panel.title";</v>
+      </c>
+    </row>
+    <row r="746" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A746" t="str">
+        <f>IF('Resultat Analyse'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B10),".","_"),"=""", 'Resultat Analyse'!B10,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="747" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A747" t="str">
+        <f>IF('Resultat Analyse'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B11),".","_"),"=""", 'Resultat Analyse'!B11,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="748" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A748" t="str">
+        <f>IF('Resultat Analyse'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B12),".","_"),"=""", 'Resultat Analyse'!B12,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="749" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A749" t="str">
+        <f>IF('Resultat Analyse'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B13),".","_"),"=""", 'Resultat Analyse'!B13,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="750" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A750" t="str">
+        <f>IF('Resultat Analyse'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B14),".","_"),"=""", 'Resultat Analyse'!B14,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="751" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A751" t="str">
+        <f>IF('Resultat Analyse'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B15),".","_"),"=""", 'Resultat Analyse'!B15,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="752" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A752" t="str">
+        <f>IF('Resultat Analyse'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B16),".","_"),"=""", 'Resultat Analyse'!B16,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="753" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A753" t="str">
+        <f>IF('Resultat Analyse'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B17),".","_"),"=""", 'Resultat Analyse'!B17,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="754" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A754" t="str">
+        <f>IF('Resultat Analyse'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B18),".","_"),"=""", 'Resultat Analyse'!B18,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="755" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A755" t="str">
+        <f>IF('Resultat Analyse'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B19),".","_"),"=""", 'Resultat Analyse'!B19,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="756" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A756" t="str">
+        <f>IF('Resultat Analyse'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B20),".","_"),"=""", 'Resultat Analyse'!B20,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="757" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A757" t="str">
+        <f>IF('Resultat Analyse'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B21),".","_"),"=""", 'Resultat Analyse'!B21,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="758" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A758" t="str">
+        <f>IF('Resultat Analyse'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B22),".","_"),"=""", 'Resultat Analyse'!B22,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="759" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A759" t="str">
+        <f>IF('Resultat Analyse'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B23),".","_"),"=""", 'Resultat Analyse'!B23,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="760" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A760" t="str">
+        <f>IF('Resultat Analyse'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B24),".","_"),"=""", 'Resultat Analyse'!B24,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="761" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A761" t="str">
+        <f>IF('Resultat Analyse'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B25),".","_"),"=""", 'Resultat Analyse'!B25,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="762" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A762" t="str">
+        <f>IF('Resultat Analyse'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B26),".","_"),"=""", 'Resultat Analyse'!B26,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="763" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A763" t="str">
+        <f>IF('Resultat Analyse'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B27),".","_"),"=""", 'Resultat Analyse'!B27,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="764" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A764" t="str">
+        <f>IF('Resultat Analyse'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B28),".","_"),"=""", 'Resultat Analyse'!B28,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="765" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A765" t="str">
+        <f>IF('Resultat Analyse'!B29&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B29),".","_"),"=""", 'Resultat Analyse'!B29,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="766" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A766" t="str">
+        <f>IF('Resultat Analyse'!B30&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B30),".","_"),"=""", 'Resultat Analyse'!B30,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="767" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A767" t="str">
+        <f>IF('Resultat Analyse'!B31&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B31),".","_"),"=""", 'Resultat Analyse'!B31,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="768" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A768" t="str">
+        <f>IF('Resultat Analyse'!B32&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B32),".","_"),"=""", 'Resultat Analyse'!B32,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="769" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A769" t="str">
+        <f>IF('Resultat Analyse'!B33&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B33),".","_"),"=""", 'Resultat Analyse'!B33,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="770" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A770" t="str">
+        <f>IF('Resultat Analyse'!B34&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B34),".","_"),"=""", 'Resultat Analyse'!B34,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="771" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A771" t="str">
+        <f>IF('Resultat Analyse'!B35&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B35),".","_"),"=""", 'Resultat Analyse'!B35,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="772" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A772" t="str">
+        <f>IF('Resultat Analyse'!B36&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B36),".","_"),"=""", 'Resultat Analyse'!B36,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="773" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A773" t="str">
+        <f>IF('Resultat Analyse'!B37&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B37),".","_"),"=""", 'Resultat Analyse'!B37,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="774" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A774" t="str">
+        <f>IF('Resultat Analyse'!B38&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B38),".","_"),"=""", 'Resultat Analyse'!B38,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="775" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A775" t="str">
+        <f>IF('Resultat Analyse'!B39&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B39),".","_"),"=""", 'Resultat Analyse'!B39,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="776" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A776" t="str">
+        <f>IF('Resultat Analyse'!B40&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B40),".","_"),"=""", 'Resultat Analyse'!B40,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="777" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A777" t="str">
+        <f>IF('Resultat Analyse'!B41&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B41),".","_"),"=""", 'Resultat Analyse'!B41,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="778" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A778" t="str">
+        <f>IF('Resultat Analyse'!B42&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B42),".","_"),"=""", 'Resultat Analyse'!B42,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="779" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A779" t="str">
+        <f>IF('Resultat Analyse'!B43&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B43),".","_"),"=""", 'Resultat Analyse'!B43,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="780" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A780" t="str">
+        <f>IF('Resultat Analyse'!B44&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B44),".","_"),"=""", 'Resultat Analyse'!B44,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="781" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A781" t="str">
+        <f>IF('Resultat Analyse'!B45&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B45),".","_"),"=""", 'Resultat Analyse'!B45,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="782" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A782" t="str">
+        <f>IF('Resultat Analyse'!B46&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B46),".","_"),"=""", 'Resultat Analyse'!B46,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="783" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A783" t="str">
+        <f>IF('Resultat Analyse'!B47&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B47),".","_"),"=""", 'Resultat Analyse'!B47,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="784" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A784" t="str">
+        <f>IF('Resultat Analyse'!B48&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B48),".","_"),"=""", 'Resultat Analyse'!B48,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="785" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A785" t="str">
+        <f>IF('Resultat Analyse'!B49&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B49),".","_"),"=""", 'Resultat Analyse'!B49,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="786" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A786" t="str">
+        <f>IF('Resultat Analyse'!B50&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B50),".","_"),"=""", 'Resultat Analyse'!B50,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="787" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A787" t="str">
+        <f>IF('Resultat Analyse'!B51&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B51),".","_"),"=""", 'Resultat Analyse'!B51,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="788" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A788" t="str">
+        <f>IF('Resultat Analyse'!B52&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B52),".","_"),"=""", 'Resultat Analyse'!B52,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="789" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A789" t="str">
+        <f>IF('Resultat Analyse'!B53&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B53),".","_"),"=""", 'Resultat Analyse'!B53,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="790" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A790" t="str">
+        <f>IF('Resultat Analyse'!B54&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B54),".","_"),"=""", 'Resultat Analyse'!B54,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="791" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A791" t="str">
+        <f>IF('Resultat Analyse'!B55&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B55),".","_"),"=""", 'Resultat Analyse'!B55,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="792" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A792" t="str">
+        <f>IF('Resultat Analyse'!B56&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B56),".","_"),"=""", 'Resultat Analyse'!B56,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="793" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A793" t="str">
+        <f>IF('Resultat Analyse'!B57&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B57),".","_"),"=""", 'Resultat Analyse'!B57,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="794" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A794" t="str">
+        <f>IF('Resultat Analyse'!B58&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B58),".","_"),"=""", 'Resultat Analyse'!B58,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="795" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A795" t="str">
+        <f>IF('Resultat Analyse'!B59&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B59),".","_"),"=""", 'Resultat Analyse'!B59,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="796" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A796" t="str">
+        <f>IF('Resultat Analyse'!B60&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B60),".","_"),"=""", 'Resultat Analyse'!B60,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="797" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A797" t="str">
+        <f>IF('Resultat Analyse'!B61&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B61),".","_"),"=""", 'Resultat Analyse'!B61,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="798" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A798" t="str">
+        <f>IF('Resultat Analyse'!B62&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B62),".","_"),"=""", 'Resultat Analyse'!B62,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="799" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A799" t="str">
+        <f>IF('Resultat Analyse'!B63&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B63),".","_"),"=""", 'Resultat Analyse'!B63,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="800" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A800" t="str">
+        <f>IF('Resultat Analyse'!B64&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B64),".","_"),"=""", 'Resultat Analyse'!B64,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="801" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A801" t="str">
+        <f>IF('Resultat Analyse'!B65&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B65),".","_"),"=""", 'Resultat Analyse'!B65,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="802" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A802" t="str">
+        <f>IF('Resultat Analyse'!B66&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B66),".","_"),"=""", 'Resultat Analyse'!B66,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="803" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A803" t="str">
+        <f>IF('Resultat Analyse'!B67&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B67),".","_"),"=""", 'Resultat Analyse'!B67,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="804" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A804" t="str">
+        <f>IF('Resultat Analyse'!B68&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B68),".","_"),"=""", 'Resultat Analyse'!B68,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="805" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A805" t="str">
+        <f>IF('Resultat Analyse'!B69&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B69),".","_"),"=""", 'Resultat Analyse'!B69,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="806" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A806" t="str">
+        <f>IF('Resultat Analyse'!B70&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B70),".","_"),"=""", 'Resultat Analyse'!B70,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="807" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A807" t="str">
+        <f>IF('Resultat Analyse'!B71&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B71),".","_"),"=""", 'Resultat Analyse'!B71,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="808" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A808" t="str">
+        <f>IF('Resultat Analyse'!B72&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B72),".","_"),"=""", 'Resultat Analyse'!B72,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="809" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A809" t="str">
+        <f>IF('Resultat Analyse'!B73&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B73),".","_"),"=""", 'Resultat Analyse'!B73,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="810" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A810" t="str">
+        <f>IF('Resultat Analyse'!B74&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B74),".","_"),"=""", 'Resultat Analyse'!B74,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="811" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A811" t="str">
+        <f>IF('Resultat Analyse'!B75&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B75),".","_"),"=""", 'Resultat Analyse'!B75,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="812" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A812" t="str">
+        <f>IF('Resultat Analyse'!B76&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B76),".","_"),"=""", 'Resultat Analyse'!B76,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="813" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A813" t="str">
+        <f>IF('Resultat Analyse'!B77&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B77),".","_"),"=""", 'Resultat Analyse'!B77,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="814" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A814" t="str">
+        <f>IF('Resultat Analyse'!B78&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B78),".","_"),"=""", 'Resultat Analyse'!B78,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="815" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A815" t="str">
+        <f>IF('Resultat Analyse'!B79&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B79),".","_"),"=""", 'Resultat Analyse'!B79,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="816" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A816" t="str">
+        <f>IF('Resultat Analyse'!B80&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B80),".","_"),"=""", 'Resultat Analyse'!B80,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="817" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A817" t="str">
+        <f>IF('Resultat Analyse'!B81&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B81),".","_"),"=""", 'Resultat Analyse'!B81,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="818" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A818" t="str">
+        <f>IF('Resultat Analyse'!B82&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B82),".","_"),"=""", 'Resultat Analyse'!B82,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="819" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A819" t="str">
+        <f>IF('Resultat Analyse'!B83&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B83),".","_"),"=""", 'Resultat Analyse'!B83,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="820" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A820" t="str">
+        <f>IF('Resultat Analyse'!B84&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B84),".","_"),"=""", 'Resultat Analyse'!B84,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="821" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A821" t="str">
+        <f>IF('Resultat Analyse'!B85&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B85),".","_"),"=""", 'Resultat Analyse'!B85,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="822" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A822" t="str">
+        <f>IF('Resultat Analyse'!B86&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B86),".","_"),"=""", 'Resultat Analyse'!B86,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="823" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A823" t="str">
+        <f>IF('Resultat Analyse'!B87&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B87),".","_"),"=""", 'Resultat Analyse'!B87,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="824" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A824" t="str">
+        <f>IF('Resultat Analyse'!B88&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B88),".","_"),"=""", 'Resultat Analyse'!B88,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="825" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A825" t="str">
+        <f>IF('Resultat Analyse'!B89&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B89),".","_"),"=""", 'Resultat Analyse'!B89,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="826" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A826" t="str">
+        <f>IF('Resultat Analyse'!B90&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B90),".","_"),"=""", 'Resultat Analyse'!B90,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="827" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A827" t="str">
+        <f>IF('Resultat Analyse'!B91&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B91),".","_"),"=""", 'Resultat Analyse'!B91,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="828" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A828" t="str">
+        <f>IF('Resultat Analyse'!B92&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B92),".","_"),"=""", 'Resultat Analyse'!B92,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="829" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A829" t="str">
+        <f>IF('Resultat Analyse'!B93&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B93),".","_"),"=""", 'Resultat Analyse'!B93,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="830" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A830" t="str">
+        <f>IF('Resultat Analyse'!B94&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B94),".","_"),"=""", 'Resultat Analyse'!B94,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="831" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A831" t="str">
+        <f>IF('Resultat Analyse'!B95&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B95),".","_"),"=""", 'Resultat Analyse'!B95,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="832" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A832" t="str">
+        <f>IF('Resultat Analyse'!B96&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B96),".","_"),"=""", 'Resultat Analyse'!B96,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="833" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A833" t="str">
+        <f>IF('Resultat Analyse'!B97&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B97),".","_"),"=""", 'Resultat Analyse'!B97,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="834" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A834" t="str">
+        <f>IF('Resultat Analyse'!B98&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B98),".","_"),"=""", 'Resultat Analyse'!B98,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="835" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A835" t="str">
+        <f>IF('Resultat Analyse'!B99&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B99),".","_"),"=""", 'Resultat Analyse'!B99,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="836" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A836" t="str">
+        <f>IF('Resultat Analyse'!B100&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B100),".","_"),"=""", 'Resultat Analyse'!B100,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="837" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A837" t="str">
+        <f>IF('Resultat Analyse'!B101&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B101),".","_"),"=""", 'Resultat Analyse'!B101,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="838" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A838" t="str">
+        <f>IF('Resultat Analyse'!B102&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B102),".","_"),"=""", 'Resultat Analyse'!B102,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="839" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A839" t="str">
+        <f>IF('Resultat Analyse'!B103&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B103),".","_"),"=""", 'Resultat Analyse'!B103,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="840" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A840" t="str">
+        <f>IF('Resultat Analyse'!B104&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B104),".","_"),"=""", 'Resultat Analyse'!B104,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="841" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A841" t="str">
+        <f>IF('Resultat Analyse'!B105&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B105),".","_"),"=""", 'Resultat Analyse'!B105,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="842" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A842" t="str">
+        <f>IF('Resultat Analyse'!B106&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B106),".","_"),"=""", 'Resultat Analyse'!B106,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="843" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A843" t="str">
+        <f>IF('Resultat Analyse'!B107&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B107),".","_"),"=""", 'Resultat Analyse'!B107,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="844" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A844" t="str">
+        <f>IF('Resultat Analyse'!B108&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B108),".","_"),"=""", 'Resultat Analyse'!B108,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="845" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A845" t="str">
+        <f>IF('Resultat Analyse'!B109&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B109),".","_"),"=""", 'Resultat Analyse'!B109,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="846" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A846" t="str">
+        <f>IF('Resultat Analyse'!B110&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B110),".","_"),"=""", 'Resultat Analyse'!B110,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="847" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A847" t="str">
+        <f>IF('Resultat Analyse'!B111&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B111),".","_"),"=""", 'Resultat Analyse'!B111,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="848" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A848" t="str">
+        <f>IF('Resultat Analyse'!B112&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B112),".","_"),"=""", 'Resultat Analyse'!B112,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="849" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A849" t="str">
+        <f>IF('Resultat Analyse'!B113&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B113),".","_"),"=""", 'Resultat Analyse'!B113,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="850" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A850" t="str">
+        <f>IF('Resultat Analyse'!B114&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B114),".","_"),"=""", 'Resultat Analyse'!B114,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="851" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A851" t="str">
+        <f>IF('Resultat Analyse'!B115&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B115),".","_"),"=""", 'Resultat Analyse'!B115,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="852" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A852" t="str">
+        <f>IF('Resultat Analyse'!B116&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B116),".","_"),"=""", 'Resultat Analyse'!B116,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="853" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A853" t="str">
+        <f>IF('Resultat Analyse'!B117&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B117),".","_"),"=""", 'Resultat Analyse'!B117,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="854" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A854" t="str">
+        <f>IF('Resultat Analyse'!B118&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B118),".","_"),"=""", 'Resultat Analyse'!B118,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="855" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A855" t="str">
+        <f>IF('Resultat Analyse'!B119&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B119),".","_"),"=""", 'Resultat Analyse'!B119,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="856" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A856" t="str">
+        <f>IF('Resultat Analyse'!B120&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B120),".","_"),"=""", 'Resultat Analyse'!B120,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="857" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A857" t="str">
+        <f>IF('Resultat Analyse'!B121&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B121),".","_"),"=""", 'Resultat Analyse'!B121,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="858" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A858" t="str">
+        <f>IF('Resultat Analyse'!B122&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B122),".","_"),"=""", 'Resultat Analyse'!B122,""";"),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Modification de la façon dont les textes sont affichés en création/consultation/édition Avancement sur le module d'analyse : - Ajout de la visualisation synchronisé avec la consultation des détails (WIP)
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\IdeaProjects\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B7349B-9ABA-43EF-93AF-DD77E21E4E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A67A2EA-45CE-4A79-92FF-538C95A18686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="22" activeTab="25" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="22" activeTab="27" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="1114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="1121">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -3350,9 +3350,6 @@
     <t>window.result.detail.token.analysis.action.view.meta.button.label</t>
   </si>
   <si>
-    <t>Consulter le corpus</t>
-  </si>
-  <si>
     <t>window.result.detail.token.analysis.action.view.data.button.label</t>
   </si>
   <si>
@@ -3365,12 +3362,6 @@
     <t>Campo para analizar</t>
   </si>
   <si>
-    <t>Consultar el corpus</t>
-  </si>
-  <si>
-    <t>Ver el documento</t>
-  </si>
-  <si>
     <t>window.result.detail.token.analysis.navigation.label</t>
   </si>
   <si>
@@ -3396,6 +3387,36 @@
   </si>
   <si>
     <t>Consultar el detalle por documento</t>
+  </si>
+  <si>
+    <t>window.read.corpus.title</t>
+  </si>
+  <si>
+    <t>window.read.text.title</t>
+  </si>
+  <si>
+    <t>window.read.specific.title</t>
+  </si>
+  <si>
+    <t>Consultation des informations spécifiques</t>
+  </si>
+  <si>
+    <t>Consultar información específica</t>
+  </si>
+  <si>
+    <t>Consultation du document</t>
+  </si>
+  <si>
+    <t>Consultation du matériel</t>
+  </si>
+  <si>
+    <t>Consultar el documento</t>
+  </si>
+  <si>
+    <t>Consultar el material</t>
+  </si>
+  <si>
+    <t>Consulter le matériel</t>
   </si>
 </sst>
 </file>
@@ -24706,8 +24727,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{028E31B7-3FC3-4143-B5FF-43FD17AAB26D}" name="Tableau16" displayName="Tableau16" ref="A1:D53" totalsRowShown="0">
-  <autoFilter ref="A1:D53" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{028E31B7-3FC3-4143-B5FF-43FD17AAB26D}" name="Tableau16" displayName="Tableau16" ref="A1:D63" totalsRowShown="0">
+  <autoFilter ref="A1:D63" xr:uid="{E7BA9EFA-948C-419C-8E1F-326C4CE3B620}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{EE0F9B50-F787-4253-A164-BB17836F12B4}" name="Numero"/>
     <tableColumn id="2" xr3:uid="{58CBB508-E960-4269-90E7-903193963B86}" name="Code"/>
@@ -26831,10 +26852,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B861A8A-1131-4099-83D4-ECA745EBF0ED}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27426,10 +27447,53 @@
         <v>891</v>
       </c>
     </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>36</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>37</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>38</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -30700,7 +30764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CC416E-27E9-484D-A35C-2643F99323FB}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -30828,13 +30892,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -30842,13 +30906,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -30869,7 +30933,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30918,7 +30982,7 @@
         <v>1094</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -30932,7 +30996,7 @@
         <v>1096</v>
       </c>
       <c r="D5" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -30943,10 +31007,10 @@
         <v>1097</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1103</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -30954,13 +31018,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="C7" t="s">
-        <v>1100</v>
+        <v>1120</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1104</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -30968,13 +31032,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -31002,8 +31066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904B2FA-CBC2-495A-A197-D0CDD47EB1AE}">
   <dimension ref="A1:A851"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A820" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A825" sqref="A825"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A373" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A391" sqref="A1:A851"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33396,19 +33460,19 @@
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" t="str">
         <f>IF(Autres!B54&lt;&gt;"",CONCATENATE(Autres!B54,"=", Autres!C54),IF(Autres!C54&lt;&gt;"",Autres!C54,""))</f>
-        <v/>
+        <v>window.read.corpus.title=Consultation du document</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" t="str">
         <f>IF(Autres!B55&lt;&gt;"",CONCATENATE(Autres!B55,"=", Autres!C55),IF(Autres!C55&lt;&gt;"",Autres!C55,""))</f>
-        <v/>
+        <v>window.read.text.title=Consultation du matériel</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" t="str">
         <f>IF(Autres!B56&lt;&gt;"",CONCATENATE(Autres!B56,"=", Autres!C56),IF(Autres!C56&lt;&gt;"",Autres!C56,""))</f>
-        <v/>
+        <v>window.read.specific.title=Consultation des informations spécifiques</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
@@ -35982,13 +36046,13 @@
     <row r="829" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A829" t="str">
         <f>IF('Detail Resultat Analyse Token'!B6&lt;&gt;"",CONCATENATE('Detail Resultat Analyse Token'!B6,"=", 'Detail Resultat Analyse Token'!C6),IF('Detail Resultat Analyse Token'!C6&lt;&gt;"",'Detail Resultat Analyse Token'!C6,""))</f>
-        <v>window.result.detail.token.analysis.action.view.meta.button.label=Consulter le corpus</v>
+        <v>window.result.detail.token.analysis.action.view.meta.button.label=Consulter le document</v>
       </c>
     </row>
     <row r="830" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A830" t="str">
         <f>IF('Detail Resultat Analyse Token'!B7&lt;&gt;"",CONCATENATE('Detail Resultat Analyse Token'!B7,"=", 'Detail Resultat Analyse Token'!C7),IF('Detail Resultat Analyse Token'!C7&lt;&gt;"",'Detail Resultat Analyse Token'!C7,""))</f>
-        <v>window.result.detail.token.analysis.action.view.data.button.label=Consulter le document</v>
+        <v>window.result.detail.token.analysis.action.view.data.button.label=Consulter le matériel</v>
       </c>
     </row>
     <row r="831" spans="1:1" x14ac:dyDescent="0.25">
@@ -36127,8 +36191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
   <dimension ref="A1:A841"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A810" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A817" sqref="A817:A841"/>
+    <sheetView showZeros="0" topLeftCell="A384" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A399" sqref="A1:A841"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38503,19 +38567,19 @@
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" t="str">
         <f>IF(Autres!B54&lt;&gt;"",CONCATENATE(Autres!B54,"=", Autres!D54),IF(Autres!D54&lt;&gt;"",Autres!D54,""))</f>
-        <v/>
+        <v>window.read.corpus.title=Consultar el documento</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" t="str">
         <f>IF(Autres!B55&lt;&gt;"",CONCATENATE(Autres!B55,"=", Autres!D55),IF(Autres!D55&lt;&gt;"",Autres!D55,""))</f>
-        <v/>
+        <v>window.read.text.title=Consultar el material</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" t="str">
         <f>IF(Autres!B56&lt;&gt;"",CONCATENATE(Autres!B56,"=", Autres!D56),IF(Autres!D56&lt;&gt;"",Autres!D56,""))</f>
-        <v/>
+        <v>window.read.specific.title=Consultar información específica</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
@@ -41059,13 +41123,13 @@
     <row r="821" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A821" t="str">
         <f>IF('Detail Resultat Analyse Token'!B6&lt;&gt;"",CONCATENATE('Detail Resultat Analyse Token'!B6,"=", 'Detail Resultat Analyse Token'!D6),IF('Detail Resultat Analyse Token'!D6&lt;&gt;"",'Detail Resultat Analyse Token'!D6,""))</f>
-        <v>window.result.detail.token.analysis.action.view.meta.button.label=Consultar el corpus</v>
+        <v>window.result.detail.token.analysis.action.view.meta.button.label=Consultar el documento</v>
       </c>
     </row>
     <row r="822" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A822" t="str">
         <f>IF('Detail Resultat Analyse Token'!B7&lt;&gt;"",CONCATENATE('Detail Resultat Analyse Token'!B7,"=", 'Detail Resultat Analyse Token'!D7),IF('Detail Resultat Analyse Token'!D7&lt;&gt;"",'Detail Resultat Analyse Token'!D7,""))</f>
-        <v>window.result.detail.token.analysis.action.view.data.button.label=Ver el documento</v>
+        <v>window.result.detail.token.analysis.action.view.data.button.label=Consultar el material</v>
       </c>
     </row>
     <row r="823" spans="1:1" x14ac:dyDescent="0.25">
@@ -41460,8 +41524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
   <dimension ref="A1:A858"/>
   <sheetViews>
-    <sheetView topLeftCell="A777" workbookViewId="0">
-      <selection activeCell="A789" sqref="A789"/>
+    <sheetView topLeftCell="A378" workbookViewId="0">
+      <selection activeCell="A394" sqref="A394:A396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43830,19 +43894,19 @@
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" t="str">
         <f>IF(Autres!B54&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B54),".","_"),"=""", Autres!B54,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_READ_CORPUS_TITLE="window.read.corpus.title";</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" t="str">
         <f>IF(Autres!B55&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B55),".","_"),"=""", Autres!B55,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_READ_TEXT_TITLE="window.read.text.title";</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" t="str">
         <f>IF(Autres!B56&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B56),".","_"),"=""", Autres!B56,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_READ_SPECIFIC_TITLE="window.read.specific.title";</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Finalisation de la gestion de la liste des noms propres (WIP)
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\IdeaProjects\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71AA21D-9E10-4045-88AD-0A1A06518554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72CFBBC-2757-449B-95DC-D0EBB3604A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="25" activeTab="28" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="25" activeTab="30" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="1178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="1181">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -3590,6 +3590,16 @@
   </si>
   <si>
     <t>Reinicie el análisis y cierre</t>
+  </si>
+  <si>
+    <t>window.start.analysis.choose.type.proper.noun.treatment.optional.list.label</t>
+  </si>
+  <si>
+    <t>Choix du type de liste pour les noms propres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elección del tipo de lista para nombres propios
+</t>
   </si>
 </sst>
 </file>
@@ -28663,10 +28673,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757EF7E0-E814-48B2-A4AF-487C809E6C10}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29037,6 +29047,20 @@
       </c>
       <c r="D25" t="s">
         <v>1070</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>1180</v>
       </c>
     </row>
   </sheetData>
@@ -31480,7 +31504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDED278-398F-4C92-8A98-C2EDEC1D7320}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -31963,7 +31987,7 @@
   <dimension ref="A1:A903"/>
   <sheetViews>
     <sheetView showZeros="0" topLeftCell="A871" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A886" sqref="A1:A903"/>
+      <selection activeCell="A885" sqref="A1:A903"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35346,7 +35370,7 @@
     <row r="563" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A563" t="str">
         <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE('Commencer analyse'!B26,"=", 'Commencer analyse'!C26),IF('Commencer analyse'!C26&lt;&gt;"",'Commencer analyse'!C26,""))</f>
-        <v/>
+        <v>window.start.analysis.choose.type.proper.noun.treatment.optional.list.label=Choix du type de liste pour les noms propres</v>
       </c>
     </row>
     <row r="564" spans="1:1" x14ac:dyDescent="0.25">
@@ -37399,8 +37423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
   <dimension ref="A1:A883"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A854" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A873" sqref="A1:A883"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A854" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A874" sqref="A1:A883"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40759,7 +40783,8 @@
     <row r="559" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A559" t="str">
         <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE('Commencer analyse'!B26,"=", 'Commencer analyse'!D26),IF('Commencer analyse'!D26&lt;&gt;"",'Commencer analyse'!D26,""))</f>
-        <v/>
+        <v xml:space="preserve">window.start.analysis.choose.type.proper.noun.treatment.optional.list.label=Elección del tipo de lista para nombres propios
+</v>
       </c>
     </row>
     <row r="560" spans="1:1" x14ac:dyDescent="0.25">
@@ -42716,8 +42741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
   <dimension ref="A1:A905"/>
   <sheetViews>
-    <sheetView topLeftCell="A865" workbookViewId="0">
-      <selection activeCell="A891" sqref="A890:A891"/>
+    <sheetView topLeftCell="A541" workbookViewId="0">
+      <selection activeCell="A555" sqref="A555"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46052,7 +46077,7 @@
     <row r="555" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A555" t="str">
         <f>IF('Commencer analyse'!B26&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B26),".","_"),"=""", 'Commencer analyse'!B26,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_CHOOSE_TYPE_PROPER_NOUN_TREATMENT_OPTIONAL_LIST_LABEL="window.start.analysis.choose.type.proper.noun.treatment.optional.list.label";</v>
       </c>
     </row>
     <row r="556" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Ajout de plusieurs fonctionnalités sur l'analyse des tokens
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\IdeaProjects\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72CFBBC-2757-449B-95DC-D0EBB3604A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0845EE-FDEF-4F48-A7AA-AEA00A29CD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="25" activeTab="30" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="25" activeTab="29" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="1181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="1191">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -3164,12 +3164,6 @@
   </si>
   <si>
     <t>window.start.analysis.choose.analyse.option.panel.title</t>
-  </si>
-  <si>
-    <t>Options disponibles/nécessaires pour l'analyse</t>
-  </si>
-  <si>
-    <t>Opciones disponibles/requeridas para el análisis</t>
   </si>
   <si>
     <t>window.start.analysis.start.button.label</t>
@@ -3600,6 +3594,42 @@
   <si>
     <t xml:space="preserve">Elección del tipo de lista para nombres propios
 </t>
+  </si>
+  <si>
+    <t>Options nécessaires pour l'analyse</t>
+  </si>
+  <si>
+    <t>Opciones requeridas para el análisis</t>
+  </si>
+  <si>
+    <t>window.start.analysis.information.optionals.liste.message</t>
+  </si>
+  <si>
+    <t>window.result.token.action.show.detail.for.word.button.label</t>
+  </si>
+  <si>
+    <t>Consulter les documents contenant les mots sélectionnés</t>
+  </si>
+  <si>
+    <t>Consultar documentos que contienen las palabras seleccionadas</t>
+  </si>
+  <si>
+    <t>window.start.analysis.help.button.label</t>
+  </si>
+  <si>
+    <t>Ouvrir l'aide</t>
+  </si>
+  <si>
+    <t>Ayuda abierta</t>
+  </si>
+  <si>
+    <t>window.help.user.title</t>
+  </si>
+  <si>
+    <t>Aide utilisateur</t>
+  </si>
+  <si>
+    <t>Ayuda al usuario</t>
   </si>
 </sst>
 </file>
@@ -26316,13 +26346,13 @@
         <v>51</v>
       </c>
       <c r="B60" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="C60" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="D60" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
     </row>
   </sheetData>
@@ -27075,10 +27105,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B861A8A-1131-4099-83D4-ECA745EBF0ED}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27675,13 +27705,13 @@
         <v>36</v>
       </c>
       <c r="B54" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="C54" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D54" t="s">
         <v>1116</v>
-      </c>
-      <c r="D54" t="s">
-        <v>1118</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -27689,13 +27719,13 @@
         <v>37</v>
       </c>
       <c r="B55" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C55" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D55" t="s">
         <v>1117</v>
-      </c>
-      <c r="D55" t="s">
-        <v>1119</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -27703,13 +27733,27 @@
         <v>38</v>
       </c>
       <c r="B56" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D56" t="s">
         <v>1113</v>
       </c>
-      <c r="C56" t="s">
-        <v>1114</v>
-      </c>
-      <c r="D56" t="s">
-        <v>1115</v>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>39</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1190</v>
       </c>
     </row>
   </sheetData>
@@ -28673,10 +28717,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757EF7E0-E814-48B2-A4AF-487C809E6C10}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28889,10 +28933,10 @@
         <v>1035</v>
       </c>
       <c r="C14" t="s">
-        <v>1036</v>
+        <v>1179</v>
       </c>
       <c r="D14" t="s">
-        <v>1037</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -28900,13 +28944,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>1038</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>1039</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>1040</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -28914,13 +28958,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D16" t="s">
         <v>1041</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1042</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1043</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -28928,13 +28972,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D17" t="s">
         <v>1044</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1046</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -28942,13 +28986,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="C18" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="D18" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -28956,13 +29000,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="C19" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="D19" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -28970,13 +29014,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="C20" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="D20" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -28984,13 +29028,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="C21" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D21" t="s">
         <v>1061</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1063</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -28998,13 +29042,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="C22" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D22" t="s">
         <v>1062</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1064</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -29012,13 +29056,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D23" t="s">
         <v>1065</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1066</v>
-      </c>
-      <c r="D23" t="s">
-        <v>1067</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -29026,13 +29070,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C24" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D24" t="s">
         <v>1057</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -29040,13 +29084,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D25" t="s">
         <v>1068</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1069</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1070</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -29054,13 +29098,51 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>1178</v>
       </c>
-      <c r="C26" t="s">
-        <v>1179</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>1180</v>
+    </row>
+    <row r="27" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Pour lancer l'analyse vous devez sélectionner les listes à utiliser.&lt;BR/&gt;",
+"Ces listes sont utilisé pour prétraiter les données (exemple : supprimer les stopwords)&lt;BR/&gt;",
+"Pour cela 2 choix s'offre à vous&lt;BR/&gt;&lt;UL&gt;",
+"&lt;LI&gt;Créer une liste vierge à partir du menu Analyse - Gestion des listes et la compléter suite à l'analyse&lt;/LI&gt;",
+"&lt;LI&gt;Choisir une liste existante et la compléter au besoin suite à l'analyse&lt;/LI&gt;&lt;/UL&gt;&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Pour lancer l'analyse vous devez sélectionner les listes à utiliser.&lt;BR/&gt;Ces listes sont utilisé pour prétraiter les données (exemple : supprimer les stopwords)&lt;BR/&gt;Pour cela 2 choix s'offre à vous&lt;BR/&gt;&lt;UL&gt;&lt;LI&gt;Créer une liste vierge à partir du menu Analyse - Gestion des listes et la compléter suite à l'analyse&lt;/LI&gt;&lt;LI&gt;Choisir une liste existante et la compléter au besoin suite à l'analyse&lt;/LI&gt;&lt;/UL&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Para iniciar el análisis debe seleccionar las listas a utilizar.&lt;BR/&gt;",
+"Estas listas se utilizan para preprocesar datos (ejemplo: eliminar stopwords)&lt;BR/&gt;",
+"Para eso se le ofrecen 2 opciones &lt;BR/&gt;&lt;UL&gt;",
+"&lt;LI&gt;Cree una lista en blanco desde el menú Análisis - Gestión de listas y complétela después del análisis&lt;/LI&gt;",
+"&lt;LI&gt;Elija una lista existente y complétela si es necesario después del análisis &lt;/LI&gt;&lt;/UL&gt;&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Para iniciar el análisis debe seleccionar las listas a utilizar.&lt;BR/&gt;Estas listas se utilizan para preprocesar datos (ejemplo: eliminar stopwords)&lt;BR/&gt;Para eso se le ofrecen 2 opciones &lt;BR/&gt;&lt;UL&gt;&lt;LI&gt;Cree una lista en blanco desde el menú Análisis - Gestión de listas y complétela después del análisis&lt;/LI&gt;&lt;LI&gt;Elija una lista existente y complétela si es necesario después del análisis &lt;/LI&gt;&lt;/UL&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1187</v>
       </c>
     </row>
   </sheetData>
@@ -31001,8 +31083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CC416E-27E9-484D-A35C-2643F99323FB}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31031,13 +31113,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="C3" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="D3" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -31045,13 +31127,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -31059,13 +31141,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="C5" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="D5" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -31073,13 +31155,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -31087,13 +31169,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -31101,13 +31183,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="C8" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -31115,13 +31197,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -31129,13 +31211,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>1105</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>1107</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>1109</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -31143,18 +31225,28 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>1106</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>1108</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>1110</v>
-      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>1184</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31199,13 +31291,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="C3" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="D3" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -31213,13 +31305,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -31227,13 +31319,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="C5" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="D5" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -31241,13 +31333,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>1097</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>1099</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -31255,13 +31347,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="C7" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -31269,13 +31361,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>1102</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>1103</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>1104</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -31283,13 +31375,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>1149</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>1150</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>1151</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -31343,13 +31435,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="C3" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="D3" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -31357,7 +31449,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Dans cette étape vous pouvez gérer les noms propres à nettoyer&lt;BR/&gt;",
@@ -31377,13 +31469,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="C5" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="D5" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -31391,7 +31483,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Quelle est le nouveau nom propre à ajouter ?&lt;BR/&gt;",
@@ -31409,13 +31501,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -31423,13 +31515,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="C8" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="D8" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -31437,13 +31529,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="C9" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="D9" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -31451,13 +31543,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="C10" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="D10" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -31465,13 +31557,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="C11" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="D11" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -31479,7 +31571,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="C12" t="s">
         <v>981</v>
@@ -31534,13 +31626,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="C3" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="D3" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -31548,7 +31640,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Cette fenêtre vous permet d'ajouter facilement des noms propres à une liste&lt;BR/&gt;",
@@ -31570,13 +31662,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C5" t="s">
         <v>1152</v>
       </c>
-      <c r="C5" t="s">
-        <v>1154</v>
-      </c>
       <c r="D5" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -31584,7 +31676,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>895</v>
@@ -31598,13 +31690,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -31612,13 +31704,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="C8" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="D8" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -31626,13 +31718,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D9" t="s">
         <v>1162</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1163</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1164</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -31640,13 +31732,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>1168</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>1170</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -31654,13 +31746,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="C11" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="D11" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -31668,13 +31760,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C12" t="s">
         <v>1167</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>1169</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1171</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -31682,13 +31774,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>1172</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>1174</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -31696,13 +31788,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="C14" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="D14" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
   </sheetData>
@@ -31986,8 +32078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904B2FA-CBC2-495A-A197-D0CDD47EB1AE}">
   <dimension ref="A1:A903"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A871" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A885" sqref="A1:A903"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A880" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A900" sqref="A1:A903"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34398,7 +34490,7 @@
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" t="str">
         <f>IF(Autres!B57&lt;&gt;"",CONCATENATE(Autres!B57,"=", Autres!C57),IF(Autres!C57&lt;&gt;"",Autres!C57,""))</f>
-        <v/>
+        <v>window.help.user.title=Aide utilisateur</v>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
@@ -35298,7 +35390,7 @@
     <row r="551" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A551" t="str">
         <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE('Commencer analyse'!B14,"=", 'Commencer analyse'!C14),IF('Commencer analyse'!C14&lt;&gt;"",'Commencer analyse'!C14,""))</f>
-        <v>window.start.analysis.choose.analyse.option.panel.title=Options disponibles/nécessaires pour l'analyse</v>
+        <v>window.start.analysis.choose.analyse.option.panel.title=Options nécessaires pour l'analyse</v>
       </c>
     </row>
     <row r="552" spans="1:1" x14ac:dyDescent="0.25">
@@ -35376,13 +35468,13 @@
     <row r="564" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A564" t="str">
         <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE('Commencer analyse'!B27,"=", 'Commencer analyse'!C27),IF('Commencer analyse'!C27&lt;&gt;"",'Commencer analyse'!C27,""))</f>
-        <v/>
+        <v>window.start.analysis.information.optionals.liste.message=&lt;HTML&gt;&lt;P&gt;Pour lancer l'analyse vous devez sélectionner les listes à utiliser.&lt;BR/&gt;Ces listes sont utilisé pour prétraiter les données (exemple : supprimer les stopwords)&lt;BR/&gt;Pour cela 2 choix s'offre à vous&lt;BR/&gt;&lt;UL&gt;&lt;LI&gt;Créer une liste vierge à partir du menu Analyse - Gestion des listes et la compléter suite à l'analyse&lt;/LI&gt;&lt;LI&gt;Choisir une liste existante et la compléter au besoin suite à l'analyse&lt;/LI&gt;&lt;/UL&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="565" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A565" t="str">
         <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE('Commencer analyse'!B28,"=", 'Commencer analyse'!C28),IF('Commencer analyse'!C28&lt;&gt;"",'Commencer analyse'!C28,""))</f>
-        <v/>
+        <v>window.start.analysis.help.button.label=Ouvrir l'aide</v>
       </c>
     </row>
     <row r="566" spans="1:1" x14ac:dyDescent="0.25">
@@ -36744,7 +36836,7 @@
     <row r="792" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A792" t="str">
         <f>IF('Resultat Analyse'!B12&lt;&gt;"",CONCATENATE('Resultat Analyse'!B12,"=", 'Resultat Analyse'!C12),IF('Resultat Analyse'!C12&lt;&gt;"",'Resultat Analyse'!C12,""))</f>
-        <v/>
+        <v>window.result.token.action.show.detail.for.word.button.label=Consulter les documents contenant les mots sélectionnés</v>
       </c>
     </row>
     <row r="793" spans="1:1" x14ac:dyDescent="0.25">
@@ -37423,8 +37515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
   <dimension ref="A1:A883"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A854" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A874" sqref="A1:A883"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39817,7 +39909,7 @@
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" t="str">
         <f>IF(Autres!B57&lt;&gt;"",CONCATENATE(Autres!B57,"=", Autres!D57),IF(Autres!D57&lt;&gt;"",Autres!D57,""))</f>
-        <v/>
+        <v>window.help.user.title=Ayuda al usuario</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
@@ -40711,7 +40803,7 @@
     <row r="547" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A547" t="str">
         <f>IF('Commencer analyse'!B14&lt;&gt;"",CONCATENATE('Commencer analyse'!B14,"=", 'Commencer analyse'!D14),IF('Commencer analyse'!D14&lt;&gt;"",'Commencer analyse'!D14,""))</f>
-        <v>window.start.analysis.choose.analyse.option.panel.title=Opciones disponibles/requeridas para el análisis</v>
+        <v>window.start.analysis.choose.analyse.option.panel.title=Opciones requeridas para el análisis</v>
       </c>
     </row>
     <row r="548" spans="1:1" x14ac:dyDescent="0.25">
@@ -40790,13 +40882,13 @@
     <row r="560" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A560" t="str">
         <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE('Commencer analyse'!B27,"=", 'Commencer analyse'!D27),IF('Commencer analyse'!D27&lt;&gt;"",'Commencer analyse'!D27,""))</f>
-        <v/>
+        <v>window.start.analysis.information.optionals.liste.message=&lt;HTML&gt;&lt;P&gt;Para iniciar el análisis debe seleccionar las listas a utilizar.&lt;BR/&gt;Estas listas se utilizan para preprocesar datos (ejemplo: eliminar stopwords)&lt;BR/&gt;Para eso se le ofrecen 2 opciones &lt;BR/&gt;&lt;UL&gt;&lt;LI&gt;Cree una lista en blanco desde el menú Análisis - Gestión de listas y complétela después del análisis&lt;/LI&gt;&lt;LI&gt;Elija una lista existente y complétela si es necesario después del análisis &lt;/LI&gt;&lt;/UL&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
       </c>
     </row>
     <row r="561" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A561" t="str">
         <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE('Commencer analyse'!B28,"=", 'Commencer analyse'!D28),IF('Commencer analyse'!D28&lt;&gt;"",'Commencer analyse'!D28,""))</f>
-        <v/>
+        <v>window.start.analysis.help.button.label=Ayuda abierta</v>
       </c>
     </row>
     <row r="562" spans="1:1" x14ac:dyDescent="0.25">
@@ -42122,7 +42214,7 @@
     <row r="782" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A782" t="str">
         <f>IF('Resultat Analyse'!B12&lt;&gt;"",CONCATENATE('Resultat Analyse'!B12,"=", 'Resultat Analyse'!D12),IF('Resultat Analyse'!D12&lt;&gt;"",'Resultat Analyse'!D12,""))</f>
-        <v/>
+        <v>window.result.token.action.show.detail.for.word.button.label=Consultar documentos que contienen las palabras seleccionadas</v>
       </c>
     </row>
     <row r="783" spans="1:1" x14ac:dyDescent="0.25">
@@ -42741,8 +42833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
   <dimension ref="A1:A905"/>
   <sheetViews>
-    <sheetView topLeftCell="A541" workbookViewId="0">
-      <selection activeCell="A555" sqref="A555"/>
+    <sheetView topLeftCell="A385" workbookViewId="0">
+      <selection activeCell="A397" sqref="A397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45129,7 +45221,7 @@
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" t="str">
         <f>IF(Autres!B57&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER(Autres!B57),".","_"),"=""", Autres!B57,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_HELP_USER_TITLE="window.help.user.title";</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
@@ -46083,13 +46175,13 @@
     <row r="556" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A556" t="str">
         <f>IF('Commencer analyse'!B27&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B27),".","_"),"=""", 'Commencer analyse'!B27,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_INFORMATION_OPTIONALS_LISTE_MESSAGE="window.start.analysis.information.optionals.liste.message";</v>
       </c>
     </row>
     <row r="557" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A557" t="str">
         <f>IF('Commencer analyse'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Commencer analyse'!B28),".","_"),"=""", 'Commencer analyse'!B28,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_START_ANALYSIS_HELP_BUTTON_LABEL="window.start.analysis.help.button.label";</v>
       </c>
     </row>
     <row r="558" spans="1:1" x14ac:dyDescent="0.25">
@@ -47235,7 +47327,7 @@
     <row r="748" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A748" t="str">
         <f>IF('Resultat Analyse'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B12),".","_"),"=""", 'Resultat Analyse'!B12,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_RESULT_TOKEN_ACTION_SHOW_DETAIL_FOR_WORD_BUTTON_LABEL="window.result.token.action.show.detail.for.word.button.label";</v>
       </c>
     </row>
     <row r="749" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Ajout de la fonctionnalité de regroupements des résultats (reste à faire, le regroupement pour les champs spécifiques)
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\IdeaProjects\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0845EE-FDEF-4F48-A7AA-AEA00A29CD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817A2D24-F974-48FD-9F21-2BF8CA34A878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="25" activeTab="29" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="26" activeTab="31" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,10 @@
     <sheet name="Detail Resultat Analyse Token" sheetId="32" r:id="rId27"/>
     <sheet name="Nom propres" sheetId="33" r:id="rId28"/>
     <sheet name="Analyse ajout nom propres" sheetId="34" r:id="rId29"/>
-    <sheet name="FR_Properties" sheetId="14" r:id="rId30"/>
-    <sheet name="ES_Properties" sheetId="16" r:id="rId31"/>
-    <sheet name="Constants" sheetId="18" r:id="rId32"/>
+    <sheet name="Grouper resultat" sheetId="35" r:id="rId30"/>
+    <sheet name="FR_Properties" sheetId="14" r:id="rId31"/>
+    <sheet name="ES_Properties" sheetId="16" r:id="rId32"/>
+    <sheet name="Constants" sheetId="18" r:id="rId33"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="1191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="1207">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -3630,6 +3631,54 @@
   </si>
   <si>
     <t>Ayuda al usuario</t>
+  </si>
+  <si>
+    <t>window.result.token.global.label</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>window.analysis.result.group.panel.title</t>
+  </si>
+  <si>
+    <t>Regrouper les résultat</t>
+  </si>
+  <si>
+    <t>window.analysis.result.group.information.message</t>
+  </si>
+  <si>
+    <t>window.analysis.result.group.choose.field.panel</t>
+  </si>
+  <si>
+    <t>Elección de campos para analizar</t>
+  </si>
+  <si>
+    <t>Choix des champs</t>
+  </si>
+  <si>
+    <t>Elección de campos</t>
+  </si>
+  <si>
+    <t>window.analysis.result.group.button.label</t>
+  </si>
+  <si>
+    <t>Agrupa los resultados</t>
+  </si>
+  <si>
+    <t>window.result.token.action.show.group.result.button.label</t>
+  </si>
+  <si>
+    <t>Regrouper les résultats</t>
+  </si>
+  <si>
+    <t>Générer et fermer</t>
+  </si>
+  <si>
+    <t>Generar et fermer</t>
+  </si>
+  <si>
+    <t>window.result.token.group.result.information.panel.title</t>
   </si>
 </sst>
 </file>
@@ -25186,6 +25235,19 @@
 </table>
 </file>
 
+<file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{C57143BB-E3C2-41BD-81A5-C88BAA649133}" name="Tableau15212223293031" displayName="Tableau15212223293031" ref="A1:D15" totalsRowShown="0">
+  <autoFilter ref="A1:D15" xr:uid="{1C0F8CDE-76C5-4629-A51B-1F75FFD867D6}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{654B29B8-E5D1-4A5F-93FD-F0B7A7C5E48C}" name="Numero"/>
+    <tableColumn id="2" xr3:uid="{3F06810E-C043-4898-B2CD-E16C98C9ABAE}" name="Code"/>
+    <tableColumn id="3" xr3:uid="{BBA80C1F-D9AA-4C78-B133-5D68FA495C2D}" name="Français"/>
+    <tableColumn id="4" xr3:uid="{1ACED21F-7DD6-4D58-8262-78DA58D16E63}" name="Español"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5DEBEDFE-8B99-4A11-A730-60645233D5C1}" name="Tableau245" displayName="Tableau245" ref="A1:D25" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="A1:D25" xr:uid="{64900EF6-8A63-4911-AB00-264B2BB02147}"/>
@@ -28719,8 +28781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757EF7E0-E814-48B2-A4AF-487C809E6C10}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D10" sqref="C10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28876,7 +28938,7 @@
         <v>1028</v>
       </c>
       <c r="D10" t="s">
-        <v>1028</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -31081,10 +31143,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CC416E-27E9-484D-A35C-2643F99323FB}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31246,6 +31308,48 @@
       </c>
       <c r="D12" s="1" t="s">
         <v>1184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C15" t="s">
+        <v>981</v>
+      </c>
+      <c r="D15" t="s">
+        <v>982</v>
       </c>
     </row>
   </sheetData>
@@ -32075,11 +32179,125 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB84E775-5502-48B6-98AC-0814DC89D640}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="61.140625" customWidth="1"/>
+    <col min="3" max="3" width="77.85546875" customWidth="1"/>
+    <col min="4" max="4" width="88.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Cette fenêtre vous permet de regrouper les résultats&lt;BR/&gt;",
+"Pour cela vous devez cocher le ou les champs que vous souhaitez utiliser pour regrouper.&lt;BR/&gt;",
+"Un produit cartésien sera alors réalisé avec les valeurs des champs.&lt;BR/&gt;",
+"Pour générer les résultats cliquez ensuite sur générer.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Cette fenêtre vous permet de regrouper les résultats&lt;BR/&gt;Pour cela vous devez cocher le ou les champs que vous souhaitez utiliser pour regrouper.&lt;BR/&gt;Un produit cartésien sera alors réalisé avec les valeurs des champs.&lt;BR/&gt;Pour générer les résultats cliquez ensuite sur générer.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Esta ventana le permite agrupar los resultados&lt;BR/&gt;",
+"Para esto debes marcar el (los) campo (s) que quieres usar para agrupar.&lt;BR/&gt;",
+"Entonces se producirá un producto cartesiano con los valores de los campos.&lt;BR/&gt;",
+"Para generar los resultados, haga clic en generar.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Esta ventana le permite agrupar los resultados&lt;BR/&gt;Para esto debes marcar el (los) campo (s) que quieres usar para agrupar.&lt;BR/&gt;Entonces se producirá un producto cartesiano con los valores de los campos.&lt;BR/&gt;Para generar los resultados, haga clic en generar.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904B2FA-CBC2-495A-A197-D0CDD47EB1AE}">
-  <dimension ref="A1:A903"/>
+  <dimension ref="A1:A927"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A880" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A900" sqref="A1:A903"/>
+    <sheetView showZeros="0" topLeftCell="A897" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A915" sqref="A1:A927"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36842,19 +37060,19 @@
     <row r="793" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A793" t="str">
         <f>IF('Resultat Analyse'!B13&lt;&gt;"",CONCATENATE('Resultat Analyse'!B13,"=", 'Resultat Analyse'!C13),IF('Resultat Analyse'!C13&lt;&gt;"",'Resultat Analyse'!C13,""))</f>
-        <v/>
+        <v>window.result.token.global.label=Global</v>
       </c>
     </row>
     <row r="794" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A794" t="str">
         <f>IF('Resultat Analyse'!B14&lt;&gt;"",CONCATENATE('Resultat Analyse'!B14,"=", 'Resultat Analyse'!C14),IF('Resultat Analyse'!C14&lt;&gt;"",'Resultat Analyse'!C14,""))</f>
-        <v/>
+        <v>window.result.token.action.show.group.result.button.label=Regrouper les résultats</v>
       </c>
     </row>
     <row r="795" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A795" t="str">
         <f>IF('Resultat Analyse'!B15&lt;&gt;"",CONCATENATE('Resultat Analyse'!B15,"=", 'Resultat Analyse'!C15),IF('Resultat Analyse'!C15&lt;&gt;"",'Resultat Analyse'!C15,""))</f>
-        <v/>
+        <v>window.result.token.group.result.information.panel.title=Information</v>
       </c>
     </row>
     <row r="796" spans="1:1" x14ac:dyDescent="0.25">
@@ -37502,6 +37720,150 @@
     <row r="903" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A903" t="str">
         <f>IF('Analyse ajout nom propres'!B29&lt;&gt;"",CONCATENATE('Analyse ajout nom propres'!B29,"=", 'Analyse ajout nom propres'!C29),IF('Analyse ajout nom propres'!C29&lt;&gt;"",'Analyse ajout nom propres'!C29,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="904" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A904" t="str">
+        <f>IF('Grouper resultat'!B2&lt;&gt;"",CONCATENATE('Grouper resultat'!B2,"=", 'Grouper resultat'!C2),IF('Grouper resultat'!C2&lt;&gt;"",'Grouper resultat'!C2,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="905" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A905" t="str">
+        <f>IF('Grouper resultat'!B3&lt;&gt;"",CONCATENATE('Grouper resultat'!B3,"=", 'Grouper resultat'!C3),IF('Grouper resultat'!C3&lt;&gt;"",'Grouper resultat'!C3,""))</f>
+        <v>window.analysis.result.group.panel.title=Regrouper les résultat</v>
+      </c>
+    </row>
+    <row r="906" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A906" t="str">
+        <f>IF('Grouper resultat'!B4&lt;&gt;"",CONCATENATE('Grouper resultat'!B4,"=", 'Grouper resultat'!C4),IF('Grouper resultat'!C4&lt;&gt;"",'Grouper resultat'!C4,""))</f>
+        <v>window.analysis.result.group.information.message=&lt;HTML&gt;&lt;P&gt;Cette fenêtre vous permet de regrouper les résultats&lt;BR/&gt;Pour cela vous devez cocher le ou les champs que vous souhaitez utiliser pour regrouper.&lt;BR/&gt;Un produit cartésien sera alors réalisé avec les valeurs des champs.&lt;BR/&gt;Pour générer les résultats cliquez ensuite sur générer.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="907" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A907" t="str">
+        <f>IF('Grouper resultat'!B5&lt;&gt;"",CONCATENATE('Grouper resultat'!B5,"=", 'Grouper resultat'!C5),IF('Grouper resultat'!C5&lt;&gt;"",'Grouper resultat'!C5,""))</f>
+        <v>window.analysis.result.group.choose.field.panel=Choix des champs</v>
+      </c>
+    </row>
+    <row r="908" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A908" t="str">
+        <f>IF('Grouper resultat'!B6&lt;&gt;"",CONCATENATE('Grouper resultat'!B6,"=", 'Grouper resultat'!C6),IF('Grouper resultat'!C6&lt;&gt;"",'Grouper resultat'!C6,""))</f>
+        <v>window.analysis.result.group.button.label=Générer et fermer</v>
+      </c>
+    </row>
+    <row r="909" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A909" t="str">
+        <f>IF('Grouper resultat'!B7&lt;&gt;"",CONCATENATE('Grouper resultat'!B7,"=", 'Grouper resultat'!C7),IF('Grouper resultat'!C7&lt;&gt;"",'Grouper resultat'!C7,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="910" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A910" t="str">
+        <f>IF('Grouper resultat'!B8&lt;&gt;"",CONCATENATE('Grouper resultat'!B8,"=", 'Grouper resultat'!C8),IF('Grouper resultat'!C8&lt;&gt;"",'Grouper resultat'!C8,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="911" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A911" t="str">
+        <f>IF('Grouper resultat'!B9&lt;&gt;"",CONCATENATE('Grouper resultat'!B9,"=", 'Grouper resultat'!C9),IF('Grouper resultat'!C9&lt;&gt;"",'Grouper resultat'!C9,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="912" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A912" t="str">
+        <f>IF('Grouper resultat'!B10&lt;&gt;"",CONCATENATE('Grouper resultat'!B10,"=", 'Grouper resultat'!C10),IF('Grouper resultat'!C10&lt;&gt;"",'Grouper resultat'!C10,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="913" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A913" t="str">
+        <f>IF('Grouper resultat'!B11&lt;&gt;"",CONCATENATE('Grouper resultat'!B11,"=", 'Grouper resultat'!C11),IF('Grouper resultat'!C11&lt;&gt;"",'Grouper resultat'!C11,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="914" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A914" t="str">
+        <f>IF('Grouper resultat'!B12&lt;&gt;"",CONCATENATE('Grouper resultat'!B12,"=", 'Grouper resultat'!C12),IF('Grouper resultat'!C12&lt;&gt;"",'Grouper resultat'!C12,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="915" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A915" t="str">
+        <f>IF('Grouper resultat'!B13&lt;&gt;"",CONCATENATE('Grouper resultat'!B13,"=", 'Grouper resultat'!C13),IF('Grouper resultat'!C13&lt;&gt;"",'Grouper resultat'!C13,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="916" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A916" t="str">
+        <f>IF('Grouper resultat'!B14&lt;&gt;"",CONCATENATE('Grouper resultat'!B14,"=", 'Grouper resultat'!C14),IF('Grouper resultat'!C14&lt;&gt;"",'Grouper resultat'!C14,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="917" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A917" t="str">
+        <f>IF('Grouper resultat'!B15&lt;&gt;"",CONCATENATE('Grouper resultat'!B15,"=", 'Grouper resultat'!C15),IF('Grouper resultat'!C15&lt;&gt;"",'Grouper resultat'!C15,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="918" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A918" t="str">
+        <f>IF('Grouper resultat'!B16&lt;&gt;"",CONCATENATE('Grouper resultat'!B16,"=", 'Grouper resultat'!C16),IF('Grouper resultat'!C16&lt;&gt;"",'Grouper resultat'!C16,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="919" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A919" t="str">
+        <f>IF('Grouper resultat'!B17&lt;&gt;"",CONCATENATE('Grouper resultat'!B17,"=", 'Grouper resultat'!C17),IF('Grouper resultat'!C17&lt;&gt;"",'Grouper resultat'!C17,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="920" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A920" t="str">
+        <f>IF('Grouper resultat'!B18&lt;&gt;"",CONCATENATE('Grouper resultat'!B18,"=", 'Grouper resultat'!C18),IF('Grouper resultat'!C18&lt;&gt;"",'Grouper resultat'!C18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="921" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A921" t="str">
+        <f>IF('Grouper resultat'!B19&lt;&gt;"",CONCATENATE('Grouper resultat'!B19,"=", 'Grouper resultat'!C19),IF('Grouper resultat'!C19&lt;&gt;"",'Grouper resultat'!C19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="922" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A922" t="str">
+        <f>IF('Grouper resultat'!B20&lt;&gt;"",CONCATENATE('Grouper resultat'!B20,"=", 'Grouper resultat'!C20),IF('Grouper resultat'!C20&lt;&gt;"",'Grouper resultat'!C20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="923" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A923" t="str">
+        <f>IF('Grouper resultat'!B21&lt;&gt;"",CONCATENATE('Grouper resultat'!B21,"=", 'Grouper resultat'!C21),IF('Grouper resultat'!C21&lt;&gt;"",'Grouper resultat'!C21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="924" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A924" t="str">
+        <f>IF('Grouper resultat'!B22&lt;&gt;"",CONCATENATE('Grouper resultat'!B22,"=", 'Grouper resultat'!C22),IF('Grouper resultat'!C22&lt;&gt;"",'Grouper resultat'!C22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="925" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A925" t="str">
+        <f>IF('Grouper resultat'!B23&lt;&gt;"",CONCATENATE('Grouper resultat'!B23,"=", 'Grouper resultat'!C23),IF('Grouper resultat'!C23&lt;&gt;"",'Grouper resultat'!C23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="926" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A926" t="str">
+        <f>IF('Grouper resultat'!B24&lt;&gt;"",CONCATENATE('Grouper resultat'!B24,"=", 'Grouper resultat'!C24),IF('Grouper resultat'!C24&lt;&gt;"",'Grouper resultat'!C24,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="927" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A927" t="str">
+        <f>IF('Grouper resultat'!B25&lt;&gt;"",CONCATENATE('Grouper resultat'!B25,"=", 'Grouper resultat'!C25),IF('Grouper resultat'!C25&lt;&gt;"",'Grouper resultat'!C25,""))</f>
         <v/>
       </c>
     </row>
@@ -37511,12 +37873,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
-  <dimension ref="A1:A883"/>
+  <dimension ref="A1:A907"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A876" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A897" sqref="A1:A907"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40779,7 +41141,7 @@
     <row r="543" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A543" t="str">
         <f>IF('Commencer analyse'!B10&lt;&gt;"",CONCATENATE('Commencer analyse'!B10,"=", 'Commencer analyse'!D10),IF('Commencer analyse'!D10&lt;&gt;"",'Commencer analyse'!D10,""))</f>
-        <v>window.start.analysis.field.material.panel.title=Choix des champs à analyser</v>
+        <v>window.start.analysis.field.material.panel.title=Elección de campos para analizar</v>
       </c>
     </row>
     <row r="544" spans="1:1" x14ac:dyDescent="0.25">
@@ -42220,19 +42582,19 @@
     <row r="783" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A783" t="str">
         <f>IF('Resultat Analyse'!B13&lt;&gt;"",CONCATENATE('Resultat Analyse'!B13,"=", 'Resultat Analyse'!D13),IF('Resultat Analyse'!D13&lt;&gt;"",'Resultat Analyse'!D13,""))</f>
-        <v/>
+        <v>window.result.token.global.label=Global</v>
       </c>
     </row>
     <row r="784" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A784" t="str">
         <f>IF('Resultat Analyse'!B14&lt;&gt;"",CONCATENATE('Resultat Analyse'!B14,"=", 'Resultat Analyse'!D14),IF('Resultat Analyse'!D14&lt;&gt;"",'Resultat Analyse'!D14,""))</f>
-        <v/>
+        <v>window.result.token.action.show.group.result.button.label=Agrupa los resultados</v>
       </c>
     </row>
     <row r="785" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A785" t="str">
         <f>IF('Resultat Analyse'!B15&lt;&gt;"",CONCATENATE('Resultat Analyse'!B15,"=", 'Resultat Analyse'!D15),IF('Resultat Analyse'!D15&lt;&gt;"",'Resultat Analyse'!D15,""))</f>
-        <v/>
+        <v>window.result.token.group.result.information.panel.title=Información</v>
       </c>
     </row>
     <row r="786" spans="1:1" x14ac:dyDescent="0.25">
@@ -42820,6 +43182,150 @@
     <row r="883" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A883" t="str">
         <f>IF('Analyse ajout nom propres'!B24&lt;&gt;"",CONCATENATE('Analyse ajout nom propres'!B24,"=", 'Analyse ajout nom propres'!D24),IF('Analyse ajout nom propres'!D24&lt;&gt;"",'Analyse ajout nom propres'!D24,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="884" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A884" t="str">
+        <f>IF('Grouper resultat'!B2&lt;&gt;"",CONCATENATE('Grouper resultat'!B2,"=", 'Grouper resultat'!D2),IF('Grouper resultat'!D2&lt;&gt;"",'Grouper resultat'!D2,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="885" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A885" t="str">
+        <f>IF('Grouper resultat'!B3&lt;&gt;"",CONCATENATE('Grouper resultat'!B3,"=", 'Grouper resultat'!D3),IF('Grouper resultat'!D3&lt;&gt;"",'Grouper resultat'!D3,""))</f>
+        <v>window.analysis.result.group.panel.title=Agrupa los resultados</v>
+      </c>
+    </row>
+    <row r="886" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A886" t="str">
+        <f>IF('Grouper resultat'!B4&lt;&gt;"",CONCATENATE('Grouper resultat'!B4,"=", 'Grouper resultat'!D4),IF('Grouper resultat'!D4&lt;&gt;"",'Grouper resultat'!D4,""))</f>
+        <v>window.analysis.result.group.information.message=&lt;HTML&gt;&lt;P&gt;Esta ventana le permite agrupar los resultados&lt;BR/&gt;Para esto debes marcar el (los) campo (s) que quieres usar para agrupar.&lt;BR/&gt;Entonces se producirá un producto cartesiano con los valores de los campos.&lt;BR/&gt;Para generar los resultados, haga clic en generar.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="887" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A887" t="str">
+        <f>IF('Grouper resultat'!B5&lt;&gt;"",CONCATENATE('Grouper resultat'!B5,"=", 'Grouper resultat'!D5),IF('Grouper resultat'!D5&lt;&gt;"",'Grouper resultat'!D5,""))</f>
+        <v>window.analysis.result.group.choose.field.panel=Elección de campos</v>
+      </c>
+    </row>
+    <row r="888" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A888" t="str">
+        <f>IF('Grouper resultat'!B6&lt;&gt;"",CONCATENATE('Grouper resultat'!B6,"=", 'Grouper resultat'!D6),IF('Grouper resultat'!D6&lt;&gt;"",'Grouper resultat'!D6,""))</f>
+        <v>window.analysis.result.group.button.label=Generar et fermer</v>
+      </c>
+    </row>
+    <row r="889" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A889" t="str">
+        <f>IF('Grouper resultat'!B7&lt;&gt;"",CONCATENATE('Grouper resultat'!B7,"=", 'Grouper resultat'!D7),IF('Grouper resultat'!D7&lt;&gt;"",'Grouper resultat'!D7,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="890" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A890" t="str">
+        <f>IF('Grouper resultat'!B8&lt;&gt;"",CONCATENATE('Grouper resultat'!B8,"=", 'Grouper resultat'!D8),IF('Grouper resultat'!D8&lt;&gt;"",'Grouper resultat'!D8,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="891" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A891" t="str">
+        <f>IF('Grouper resultat'!B9&lt;&gt;"",CONCATENATE('Grouper resultat'!B9,"=", 'Grouper resultat'!D9),IF('Grouper resultat'!D9&lt;&gt;"",'Grouper resultat'!D9,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="892" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A892" t="str">
+        <f>IF('Grouper resultat'!B10&lt;&gt;"",CONCATENATE('Grouper resultat'!B10,"=", 'Grouper resultat'!D10),IF('Grouper resultat'!D10&lt;&gt;"",'Grouper resultat'!D10,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="893" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A893" t="str">
+        <f>IF('Grouper resultat'!B11&lt;&gt;"",CONCATENATE('Grouper resultat'!B11,"=", 'Grouper resultat'!D11),IF('Grouper resultat'!D11&lt;&gt;"",'Grouper resultat'!D11,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="894" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A894" t="str">
+        <f>IF('Grouper resultat'!B12&lt;&gt;"",CONCATENATE('Grouper resultat'!B12,"=", 'Grouper resultat'!D12),IF('Grouper resultat'!D12&lt;&gt;"",'Grouper resultat'!D12,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="895" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A895" t="str">
+        <f>IF('Grouper resultat'!B13&lt;&gt;"",CONCATENATE('Grouper resultat'!B13,"=", 'Grouper resultat'!D13),IF('Grouper resultat'!D13&lt;&gt;"",'Grouper resultat'!D13,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="896" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A896" t="str">
+        <f>IF('Grouper resultat'!B14&lt;&gt;"",CONCATENATE('Grouper resultat'!B14,"=", 'Grouper resultat'!D14),IF('Grouper resultat'!D14&lt;&gt;"",'Grouper resultat'!D14,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="897" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A897" t="str">
+        <f>IF('Grouper resultat'!B15&lt;&gt;"",CONCATENATE('Grouper resultat'!B15,"=", 'Grouper resultat'!D15),IF('Grouper resultat'!D15&lt;&gt;"",'Grouper resultat'!D15,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="898" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A898" t="str">
+        <f>IF('Grouper resultat'!B16&lt;&gt;"",CONCATENATE('Grouper resultat'!B16,"=", 'Grouper resultat'!D16),IF('Grouper resultat'!D16&lt;&gt;"",'Grouper resultat'!D16,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="899" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A899" t="str">
+        <f>IF('Grouper resultat'!B17&lt;&gt;"",CONCATENATE('Grouper resultat'!B17,"=", 'Grouper resultat'!D17),IF('Grouper resultat'!D17&lt;&gt;"",'Grouper resultat'!D17,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="900" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A900" t="str">
+        <f>IF('Grouper resultat'!B18&lt;&gt;"",CONCATENATE('Grouper resultat'!B18,"=", 'Grouper resultat'!D18),IF('Grouper resultat'!D18&lt;&gt;"",'Grouper resultat'!D18,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="901" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A901" t="str">
+        <f>IF('Grouper resultat'!B19&lt;&gt;"",CONCATENATE('Grouper resultat'!B19,"=", 'Grouper resultat'!D19),IF('Grouper resultat'!D19&lt;&gt;"",'Grouper resultat'!D19,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="902" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A902" t="str">
+        <f>IF('Grouper resultat'!B20&lt;&gt;"",CONCATENATE('Grouper resultat'!B20,"=", 'Grouper resultat'!D20),IF('Grouper resultat'!D20&lt;&gt;"",'Grouper resultat'!D20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="903" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A903" t="str">
+        <f>IF('Grouper resultat'!B21&lt;&gt;"",CONCATENATE('Grouper resultat'!B21,"=", 'Grouper resultat'!D21),IF('Grouper resultat'!D21&lt;&gt;"",'Grouper resultat'!D21,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="904" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A904" t="str">
+        <f>IF('Grouper resultat'!B22&lt;&gt;"",CONCATENATE('Grouper resultat'!B22,"=", 'Grouper resultat'!D22),IF('Grouper resultat'!D22&lt;&gt;"",'Grouper resultat'!D22,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="905" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A905" t="str">
+        <f>IF('Grouper resultat'!B23&lt;&gt;"",CONCATENATE('Grouper resultat'!B23,"=", 'Grouper resultat'!D23),IF('Grouper resultat'!D23&lt;&gt;"",'Grouper resultat'!D23,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="906" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A906" t="str">
+        <f>IF('Grouper resultat'!B24&lt;&gt;"",CONCATENATE('Grouper resultat'!B24,"=", 'Grouper resultat'!D24),IF('Grouper resultat'!D24&lt;&gt;"",'Grouper resultat'!D24,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="907" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A907" t="str">
+        <f>IF('Grouper resultat'!B25&lt;&gt;"",CONCATENATE('Grouper resultat'!B25,"=", 'Grouper resultat'!D25),IF('Grouper resultat'!D25&lt;&gt;"",'Grouper resultat'!D25,""))</f>
         <v/>
       </c>
     </row>
@@ -42829,12 +43335,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
-  <dimension ref="A1:A905"/>
+  <dimension ref="A1:A929"/>
   <sheetViews>
-    <sheetView topLeftCell="A385" workbookViewId="0">
-      <selection activeCell="A397" sqref="A397"/>
+    <sheetView topLeftCell="A738" workbookViewId="0">
+      <selection activeCell="A751" sqref="A751"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47333,19 +47839,19 @@
     <row r="749" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A749" t="str">
         <f>IF('Resultat Analyse'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B13),".","_"),"=""", 'Resultat Analyse'!B13,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_RESULT_TOKEN_GLOBAL_LABEL="window.result.token.global.label";</v>
       </c>
     </row>
     <row r="750" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A750" t="str">
         <f>IF('Resultat Analyse'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B14),".","_"),"=""", 'Resultat Analyse'!B14,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_RESULT_TOKEN_ACTION_SHOW_GROUP_RESULT_BUTTON_LABEL="window.result.token.action.show.group.result.button.label";</v>
       </c>
     </row>
     <row r="751" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A751" t="str">
         <f>IF('Resultat Analyse'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B15),".","_"),"=""", 'Resultat Analyse'!B15,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_RESULT_TOKEN_GROUP_RESULT_INFORMATION_PANEL_TITLE="window.result.token.group.result.information.panel.title";</v>
       </c>
     </row>
     <row r="752" spans="1:1" x14ac:dyDescent="0.25">
@@ -48269,6 +48775,150 @@
     <row r="905" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A905" t="str">
         <f>IF('Analyse ajout nom propres'!B28&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Analyse ajout nom propres'!B28),".","_"),"=""", 'Analyse ajout nom propres'!B28,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="906" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A906" t="str">
+        <f>IF('Grouper resultat'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B2),".","_"),"=""", 'Grouper resultat'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="907" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A907" t="str">
+        <f>IF('Grouper resultat'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B3),".","_"),"=""", 'Grouper resultat'!B3,""";"),"")</f>
+        <v>public static final String WINDOW_ANALYSIS_RESULT_GROUP_PANEL_TITLE="window.analysis.result.group.panel.title";</v>
+      </c>
+    </row>
+    <row r="908" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A908" t="str">
+        <f>IF('Grouper resultat'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B4),".","_"),"=""", 'Grouper resultat'!B4,""";"),"")</f>
+        <v>public static final String WINDOW_ANALYSIS_RESULT_GROUP_INFORMATION_MESSAGE="window.analysis.result.group.information.message";</v>
+      </c>
+    </row>
+    <row r="909" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A909" t="str">
+        <f>IF('Grouper resultat'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B5),".","_"),"=""", 'Grouper resultat'!B5,""";"),"")</f>
+        <v>public static final String WINDOW_ANALYSIS_RESULT_GROUP_CHOOSE_FIELD_PANEL="window.analysis.result.group.choose.field.panel";</v>
+      </c>
+    </row>
+    <row r="910" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A910" t="str">
+        <f>IF('Grouper resultat'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B6),".","_"),"=""", 'Grouper resultat'!B6,""";"),"")</f>
+        <v>public static final String WINDOW_ANALYSIS_RESULT_GROUP_BUTTON_LABEL="window.analysis.result.group.button.label";</v>
+      </c>
+    </row>
+    <row r="911" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A911" t="str">
+        <f>IF('Grouper resultat'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B7),".","_"),"=""", 'Grouper resultat'!B7,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="912" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A912" t="str">
+        <f>IF('Grouper resultat'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B8),".","_"),"=""", 'Grouper resultat'!B8,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="913" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A913" t="str">
+        <f>IF('Grouper resultat'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B9),".","_"),"=""", 'Grouper resultat'!B9,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="914" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A914" t="str">
+        <f>IF('Grouper resultat'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B10),".","_"),"=""", 'Grouper resultat'!B10,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="915" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A915" t="str">
+        <f>IF('Grouper resultat'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B11),".","_"),"=""", 'Grouper resultat'!B11,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="916" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A916" t="str">
+        <f>IF('Grouper resultat'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B12),".","_"),"=""", 'Grouper resultat'!B12,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="917" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A917" t="str">
+        <f>IF('Grouper resultat'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B13),".","_"),"=""", 'Grouper resultat'!B13,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="918" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A918" t="str">
+        <f>IF('Grouper resultat'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B14),".","_"),"=""", 'Grouper resultat'!B14,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="919" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A919" t="str">
+        <f>IF('Grouper resultat'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B15),".","_"),"=""", 'Grouper resultat'!B15,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="920" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A920" t="str">
+        <f>IF('Grouper resultat'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B16),".","_"),"=""", 'Grouper resultat'!B16,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="921" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A921" t="str">
+        <f>IF('Grouper resultat'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B17),".","_"),"=""", 'Grouper resultat'!B17,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="922" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A922" t="str">
+        <f>IF('Grouper resultat'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B18),".","_"),"=""", 'Grouper resultat'!B18,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="923" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A923" t="str">
+        <f>IF('Grouper resultat'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B19),".","_"),"=""", 'Grouper resultat'!B19,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="924" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A924" t="str">
+        <f>IF('Grouper resultat'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B20),".","_"),"=""", 'Grouper resultat'!B20,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="925" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A925" t="str">
+        <f>IF('Grouper resultat'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B21),".","_"),"=""", 'Grouper resultat'!B21,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="926" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A926" t="str">
+        <f>IF('Grouper resultat'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B22),".","_"),"=""", 'Grouper resultat'!B22,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="927" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A927" t="str">
+        <f>IF('Grouper resultat'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B23),".","_"),"=""", 'Grouper resultat'!B23,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="928" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A928" t="str">
+        <f>IF('Grouper resultat'!B24&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B24),".","_"),"=""", 'Grouper resultat'!B24,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="929" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A929" t="str">
+        <f>IF('Grouper resultat'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B25),".","_"),"=""", 'Grouper resultat'!B25,""";"),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
- Ajout de la fonctionnalité de l'export excel (WIP)
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\IdeaProjects\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817A2D24-F974-48FD-9F21-2BF8CA34A878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39FF679-569A-444A-A09E-C63B6BE55A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="26" activeTab="31" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="27" activeTab="30" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,10 @@
     <sheet name="Nom propres" sheetId="33" r:id="rId28"/>
     <sheet name="Analyse ajout nom propres" sheetId="34" r:id="rId29"/>
     <sheet name="Grouper resultat" sheetId="35" r:id="rId30"/>
-    <sheet name="FR_Properties" sheetId="14" r:id="rId31"/>
-    <sheet name="ES_Properties" sheetId="16" r:id="rId32"/>
-    <sheet name="Constants" sheetId="18" r:id="rId33"/>
+    <sheet name="Export Excel" sheetId="36" r:id="rId31"/>
+    <sheet name="FR_Properties" sheetId="14" r:id="rId32"/>
+    <sheet name="ES_Properties" sheetId="16" r:id="rId33"/>
+    <sheet name="Constants" sheetId="18" r:id="rId34"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="1207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="1217">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -3679,6 +3680,36 @@
   </si>
   <si>
     <t>window.result.token.group.result.information.panel.title</t>
+  </si>
+  <si>
+    <t>window.result.token.action.export.excel.button.label</t>
+  </si>
+  <si>
+    <t>Exporter dans Excel</t>
+  </si>
+  <si>
+    <t>Exportar a Excel</t>
+  </si>
+  <si>
+    <t>window.export.excel.panel.title</t>
+  </si>
+  <si>
+    <t>Export Excel</t>
+  </si>
+  <si>
+    <t>window.export.excel.information.message</t>
+  </si>
+  <si>
+    <t>window.export.excel.button.label</t>
+  </si>
+  <si>
+    <t>window.export.excel.file.picker.panel.label</t>
+  </si>
+  <si>
+    <t>window.export.excel.file.picker.panel.button</t>
+  </si>
+  <si>
+    <t>Exportar Excel</t>
   </si>
 </sst>
 </file>
@@ -25248,6 +25279,19 @@
 </table>
 </file>
 
+<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{AA0FCB44-B301-4BDF-99A5-97203C0D13EB}" name="Tableau1521222329303132" displayName="Tableau1521222329303132" ref="A1:D14" totalsRowShown="0">
+  <autoFilter ref="A1:D14" xr:uid="{1C0F8CDE-76C5-4629-A51B-1F75FFD867D6}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E3356A4C-DABF-425A-8BF9-D5E452A48590}" name="Numero"/>
+    <tableColumn id="2" xr3:uid="{A10CF7EA-05E4-4FCD-A5AF-9F5378B48E69}" name="Code"/>
+    <tableColumn id="3" xr3:uid="{7731F22A-F3D6-4071-B229-D584300A1187}" name="Français"/>
+    <tableColumn id="4" xr3:uid="{ACF829D2-F435-4746-A3C9-E91B331273A1}" name="Español"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5DEBEDFE-8B99-4A11-A730-60645233D5C1}" name="Tableau245" displayName="Tableau245" ref="A1:D25" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="A1:D25" xr:uid="{64900EF6-8A63-4911-AB00-264B2BB02147}"/>
@@ -26659,7 +26703,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A20" sqref="A20:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28097,7 +28141,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31143,10 +31187,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CC416E-27E9-484D-A35C-2643F99323FB}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31350,6 +31394,20 @@
       </c>
       <c r="D15" t="s">
         <v>982</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1209</v>
       </c>
     </row>
   </sheetData>
@@ -32293,11 +32351,133 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786FB214-BFC9-453E-80F9-B07C5F522F28}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="61.140625" customWidth="1"/>
+    <col min="3" max="3" width="77.85546875" customWidth="1"/>
+    <col min="4" max="4" width="88.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Cette fenêtre vous permet d'effectuer un export Excel&lt;BR/&gt;",
+"Pour cela choisisssez l'emplacement du fichier excel.&lt;BR/&gt;",
+"Et cliquer sur le bouton générer.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Cette fenêtre vous permet d'effectuer un export Excel&lt;BR/&gt;Pour cela choisisssez l'emplacement du fichier excel.&lt;BR/&gt;Et cliquer sur le bouton générer.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>CONCATENATE("&lt;HTML&gt;&lt;P&gt;Esta ventana le permite realizar una exportación a Excel&lt;BR/&gt;",
+"Para eso elija la ubicación del archivo de Excel.&lt;BR/&gt;",
+"Y haga clic en el botón generar.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;")</f>
+        <v>&lt;HTML&gt;&lt;P&gt;Esta ventana le permite realizar una exportación a Excel&lt;BR/&gt;Para eso elija la ubicación del archivo de Excel.&lt;BR/&gt;Y haga clic en el botón generar.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C7" t="s">
+        <v>835</v>
+      </c>
+      <c r="D7" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904B2FA-CBC2-495A-A197-D0CDD47EB1AE}">
   <dimension ref="A1:A927"/>
   <sheetViews>
     <sheetView showZeros="0" topLeftCell="A897" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A915" sqref="A1:A927"/>
+      <selection activeCell="A912" sqref="A1:A927"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37078,7 +37258,7 @@
     <row r="796" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A796" t="str">
         <f>IF('Resultat Analyse'!B16&lt;&gt;"",CONCATENATE('Resultat Analyse'!B16,"=", 'Resultat Analyse'!C16),IF('Resultat Analyse'!C16&lt;&gt;"",'Resultat Analyse'!C16,""))</f>
-        <v/>
+        <v>window.result.token.action.export.excel.button.label=Exporter dans Excel</v>
       </c>
     </row>
     <row r="797" spans="1:1" x14ac:dyDescent="0.25">
@@ -37873,12 +38053,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
   <dimension ref="A1:A907"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A876" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A897" sqref="A1:A907"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A1:A907"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42600,7 +42780,7 @@
     <row r="786" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A786" t="str">
         <f>IF('Resultat Analyse'!B16&lt;&gt;"",CONCATENATE('Resultat Analyse'!B16,"=", 'Resultat Analyse'!D16),IF('Resultat Analyse'!D16&lt;&gt;"",'Resultat Analyse'!D16,""))</f>
-        <v/>
+        <v>window.result.token.action.export.excel.button.label=Exportar a Excel</v>
       </c>
     </row>
     <row r="787" spans="1:1" x14ac:dyDescent="0.25">
@@ -43335,12 +43515,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
   <dimension ref="A1:A929"/>
   <sheetViews>
-    <sheetView topLeftCell="A738" workbookViewId="0">
-      <selection activeCell="A751" sqref="A751"/>
+    <sheetView topLeftCell="A747" workbookViewId="0">
+      <selection activeCell="A752" sqref="A752"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47857,7 +48037,7 @@
     <row r="752" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A752" t="str">
         <f>IF('Resultat Analyse'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Resultat Analyse'!B16),".","_"),"=""", 'Resultat Analyse'!B16,""";"),"")</f>
-        <v/>
+        <v>public static final String WINDOW_RESULT_TOKEN_ACTION_EXPORT_EXCEL_BUTTON_LABEL="window.result.token.action.export.excel.button.label";</v>
       </c>
     </row>
     <row r="753" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Ajout de la possibilité de scroll sur les onglets - Ajout de l'export des données brutes - Modification du chargement des onglets avec progression
</commit_message>
<xml_diff>
--- a/Interface_Traduction.xlsx
+++ b/Interface_Traduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\IdeaProjects\Caerus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A6E9C9-456C-401E-99C8-39CA20E2EDD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88460FC6-25C9-4E6B-B1EA-68E4DED91C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="27" activeTab="32" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="12" xr2:uid="{8ADA0D1E-DDEC-4467-9DB9-6BA0B7CD7108}"/>
   </bookViews>
   <sheets>
     <sheet name="Fenêtre principal" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="1227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="1233">
   <si>
     <t># Fenêtre principale</t>
   </si>
@@ -3740,6 +3740,24 @@
   </si>
   <si>
     <t>Numero del documento</t>
+  </si>
+  <si>
+    <t>window.export.excel.preference.panel.title</t>
+  </si>
+  <si>
+    <t>window.export.excel.preference.with.format.label</t>
+  </si>
+  <si>
+    <t>Préférences pour le fichier Excel</t>
+  </si>
+  <si>
+    <t>Inclure un format (tableau, couleur, etc)</t>
+  </si>
+  <si>
+    <t>Incluya un formato (tabla, color, etc.)</t>
+  </si>
+  <si>
+    <t>Preferencias para el archivo de Excel</t>
   </si>
 </sst>
 </file>
@@ -27243,7 +27261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B861A8A-1131-4099-83D4-ECA745EBF0ED}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
       <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
@@ -32443,8 +32461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786FB214-BFC9-453E-80F9-B07C5F522F28}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32544,9 +32562,33 @@
         <v>799</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1231</v>
+      </c>
+    </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>1232</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
@@ -32563,10 +32605,10 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904B2FA-CBC2-495A-A197-D0CDD47EB1AE}">
-  <dimension ref="A1:A934"/>
+  <dimension ref="A1:A950"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A124" sqref="A1:A934"/>
+    <sheetView showZeros="0" topLeftCell="A922" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A943" sqref="A1:A950"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38178,6 +38220,102 @@
         <v/>
       </c>
     </row>
+    <row r="935" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A935" t="str">
+        <f>IF('Export Excel'!B2&lt;&gt;"",CONCATENATE('Export Excel'!B2,"=", 'Export Excel'!C2),IF('Export Excel'!C2&lt;&gt;"",'Export Excel'!C2,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="936" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A936" t="str">
+        <f>IF('Export Excel'!B3&lt;&gt;"",CONCATENATE('Export Excel'!B3,"=", 'Export Excel'!C3),IF('Export Excel'!C3&lt;&gt;"",'Export Excel'!C3,""))</f>
+        <v>window.export.excel.panel.title=Export Excel</v>
+      </c>
+    </row>
+    <row r="937" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A937" t="str">
+        <f>IF('Export Excel'!B4&lt;&gt;"",CONCATENATE('Export Excel'!B4,"=", 'Export Excel'!C4),IF('Export Excel'!C4&lt;&gt;"",'Export Excel'!C4,""))</f>
+        <v>window.export.excel.information.message=&lt;HTML&gt;&lt;P&gt;Cette fenêtre vous permet d'effectuer un export Excel&lt;BR/&gt;Pour cela choisisssez l'emplacement du fichier excel.&lt;BR/&gt;Et cliquer sur le bouton générer.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="938" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A938" t="str">
+        <f>IF('Export Excel'!B5&lt;&gt;"",CONCATENATE('Export Excel'!B5,"=", 'Export Excel'!C5),IF('Export Excel'!C5&lt;&gt;"",'Export Excel'!C5,""))</f>
+        <v>window.export.excel.button.label=Générer et fermer</v>
+      </c>
+    </row>
+    <row r="939" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A939" t="str">
+        <f>IF('Export Excel'!B6&lt;&gt;"",CONCATENATE('Export Excel'!B6,"=", 'Export Excel'!C6),IF('Export Excel'!C6&lt;&gt;"",'Export Excel'!C6,""))</f>
+        <v>window.export.excel.file.picker.panel.label=Emplacement de l'enregistrement des Excel</v>
+      </c>
+    </row>
+    <row r="940" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A940" t="str">
+        <f>IF('Export Excel'!B7&lt;&gt;"",CONCATENATE('Export Excel'!B7,"=", 'Export Excel'!C7),IF('Export Excel'!C7&lt;&gt;"",'Export Excel'!C7,""))</f>
+        <v xml:space="preserve">window.export.excel.file.picker.panel.button=Parcourir... </v>
+      </c>
+    </row>
+    <row r="941" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A941" t="str">
+        <f>IF('Export Excel'!B8&lt;&gt;"",CONCATENATE('Export Excel'!B8,"=", 'Export Excel'!C8),IF('Export Excel'!C8&lt;&gt;"",'Export Excel'!C8,""))</f>
+        <v>window.export.excel.preference.with.format.label=Inclure un format (tableau, couleur, etc)</v>
+      </c>
+    </row>
+    <row r="942" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A942" t="str">
+        <f>IF('Export Excel'!B9&lt;&gt;"",CONCATENATE('Export Excel'!B9,"=", 'Export Excel'!C9),IF('Export Excel'!C9&lt;&gt;"",'Export Excel'!C9,""))</f>
+        <v>window.export.excel.preference.panel.title=Préférences pour le fichier Excel</v>
+      </c>
+    </row>
+    <row r="943" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A943" t="str">
+        <f>IF('Export Excel'!B10&lt;&gt;"",CONCATENATE('Export Excel'!B10,"=", 'Export Excel'!C10),IF('Export Excel'!C10&lt;&gt;"",'Export Excel'!C10,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="944" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A944" t="str">
+        <f>IF('Export Excel'!B11&lt;&gt;"",CONCATENATE('Export Excel'!B11,"=", 'Export Excel'!C11),IF('Export Excel'!C11&lt;&gt;"",'Export Excel'!C11,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="945" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A945" t="str">
+        <f>IF('Export Excel'!B12&lt;&gt;"",CONCATENATE('Export Excel'!B12,"=", 'Export Excel'!C12),IF('Export Excel'!C12&lt;&gt;"",'Export Excel'!C12,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="946" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A946" t="str">
+        <f>IF('Export Excel'!B13&lt;&gt;"",CONCATENATE('Export Excel'!B13,"=", 'Export Excel'!C13),IF('Export Excel'!C13&lt;&gt;"",'Export Excel'!C13,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="947" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A947" t="str">
+        <f>IF('Export Excel'!B14&lt;&gt;"",CONCATENATE('Export Excel'!B14,"=", 'Export Excel'!C14),IF('Export Excel'!C14&lt;&gt;"",'Export Excel'!C14,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="948" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A948" t="str">
+        <f>IF('Export Excel'!B15&lt;&gt;"",CONCATENATE('Export Excel'!B15,"=", 'Export Excel'!C15),IF('Export Excel'!C15&lt;&gt;"",'Export Excel'!C15,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="949" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A949" t="str">
+        <f>IF('Export Excel'!B16&lt;&gt;"",CONCATENATE('Export Excel'!B16,"=", 'Export Excel'!C16),IF('Export Excel'!C16&lt;&gt;"",'Export Excel'!C16,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="950" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A950" t="str">
+        <f>IF('Export Excel'!B17&lt;&gt;"",CONCATENATE('Export Excel'!B17,"=", 'Export Excel'!C17),IF('Export Excel'!C17&lt;&gt;"",'Export Excel'!C17,""))</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -38186,10 +38324,10 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD3DB96-F87F-4364-85D4-FC661FEC0D14}">
-  <dimension ref="A1:A914"/>
+  <dimension ref="A1:A929"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A1:A914"/>
+    <sheetView showZeros="0" topLeftCell="A907" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A918" sqref="A1:A929"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43682,6 +43820,96 @@
         <v/>
       </c>
     </row>
+    <row r="915" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A915" t="str">
+        <f>IF('Export Excel'!B2&lt;&gt;"",CONCATENATE('Export Excel'!B2,"=", 'Export Excel'!D2),IF('Export Excel'!D2&lt;&gt;"",'Export Excel'!D2,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="916" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A916" t="str">
+        <f>IF('Export Excel'!B3&lt;&gt;"",CONCATENATE('Export Excel'!B3,"=", 'Export Excel'!D3),IF('Export Excel'!D3&lt;&gt;"",'Export Excel'!D3,""))</f>
+        <v>window.export.excel.panel.title=Exportar Excel</v>
+      </c>
+    </row>
+    <row r="917" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A917" t="str">
+        <f>IF('Export Excel'!B4&lt;&gt;"",CONCATENATE('Export Excel'!B4,"=", 'Export Excel'!D4),IF('Export Excel'!D4&lt;&gt;"",'Export Excel'!D4,""))</f>
+        <v>window.export.excel.information.message=&lt;HTML&gt;&lt;P&gt;Esta ventana le permite realizar una exportación a Excel&lt;BR/&gt;Para eso elija la ubicación del archivo de Excel.&lt;BR/&gt;Y haga clic en el botón generar.&lt;BR/&gt;&lt;/P&gt;&lt;/HTML&gt;</v>
+      </c>
+    </row>
+    <row r="918" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A918" t="str">
+        <f>IF('Export Excel'!B5&lt;&gt;"",CONCATENATE('Export Excel'!B5,"=", 'Export Excel'!D5),IF('Export Excel'!D5&lt;&gt;"",'Export Excel'!D5,""))</f>
+        <v>window.export.excel.button.label=Generar et fermer</v>
+      </c>
+    </row>
+    <row r="919" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A919" t="str">
+        <f>IF('Export Excel'!B6&lt;&gt;"",CONCATENATE('Export Excel'!B6,"=", 'Export Excel'!D6),IF('Export Excel'!D6&lt;&gt;"",'Export Excel'!D6,""))</f>
+        <v>window.export.excel.file.picker.panel.label=Ubicación  para guardar los Excel</v>
+      </c>
+    </row>
+    <row r="920" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A920" t="str">
+        <f>IF('Export Excel'!B7&lt;&gt;"",CONCATENATE('Export Excel'!B7,"=", 'Export Excel'!D7),IF('Export Excel'!D7&lt;&gt;"",'Export Excel'!D7,""))</f>
+        <v xml:space="preserve">window.export.excel.file.picker.panel.button=Examinar... </v>
+      </c>
+    </row>
+    <row r="921" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A921" t="str">
+        <f>IF('Export Excel'!B8&lt;&gt;"",CONCATENATE('Export Excel'!B8,"=", 'Export Excel'!D8),IF('Export Excel'!D8&lt;&gt;"",'Export Excel'!D8,""))</f>
+        <v>window.export.excel.preference.with.format.label=Incluya un formato (tabla, color, etc.)</v>
+      </c>
+    </row>
+    <row r="922" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A922" t="str">
+        <f>IF('Export Excel'!B9&lt;&gt;"",CONCATENATE('Export Excel'!B9,"=", 'Export Excel'!D9),IF('Export Excel'!D9&lt;&gt;"",'Export Excel'!D9,""))</f>
+        <v>window.export.excel.preference.panel.title=Preferencias para el archivo de Excel</v>
+      </c>
+    </row>
+    <row r="923" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A923" t="str">
+        <f>IF('Export Excel'!B10&lt;&gt;"",CONCATENATE('Export Excel'!B10,"=", 'Export Excel'!D10),IF('Export Excel'!D10&lt;&gt;"",'Export Excel'!D10,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="924" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A924" t="str">
+        <f>IF('Export Excel'!B11&lt;&gt;"",CONCATENATE('Export Excel'!B11,"=", 'Export Excel'!D11),IF('Export Excel'!D11&lt;&gt;"",'Export Excel'!D11,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="925" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A925" t="str">
+        <f>IF('Export Excel'!B12&lt;&gt;"",CONCATENATE('Export Excel'!B12,"=", 'Export Excel'!D12),IF('Export Excel'!D12&lt;&gt;"",'Export Excel'!D12,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="926" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A926" t="str">
+        <f>IF('Export Excel'!B13&lt;&gt;"",CONCATENATE('Export Excel'!B13,"=", 'Export Excel'!D13),IF('Export Excel'!D13&lt;&gt;"",'Export Excel'!D13,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="927" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A927" t="str">
+        <f>IF('Export Excel'!B14&lt;&gt;"",CONCATENATE('Export Excel'!B14,"=", 'Export Excel'!D14),IF('Export Excel'!D14&lt;&gt;"",'Export Excel'!D14,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="928" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A928" t="str">
+        <f>IF('Export Excel'!B15&lt;&gt;"",CONCATENATE('Export Excel'!B15,"=", 'Export Excel'!D15),IF('Export Excel'!D15&lt;&gt;"",'Export Excel'!D15,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="929" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A929" t="str">
+        <f>IF('Export Excel'!B16&lt;&gt;"",CONCATENATE('Export Excel'!B16,"=", 'Export Excel'!D16),IF('Export Excel'!D16&lt;&gt;"",'Export Excel'!D16,""))</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -43690,10 +43918,10 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328A7A9-8E5F-4F10-88B1-0A63B886F3D8}">
-  <dimension ref="A1:A937"/>
+  <dimension ref="A1:A959"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125"/>
+    <sheetView topLeftCell="A928" workbookViewId="0">
+      <selection activeCell="A944" sqref="A944:A945"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49320,6 +49548,138 @@
     <row r="937" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A937" t="str">
         <f>IF('Grouper resultat'!B25&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Grouper resultat'!B25),".","_"),"=""", 'Grouper resultat'!B25,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="938" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A938" t="str">
+        <f>IF('Export Excel'!B2&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B2),".","_"),"=""", 'Export Excel'!B2,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="939" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A939" t="str">
+        <f>IF('Export Excel'!B3&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B3),".","_"),"=""", 'Export Excel'!B3,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_EXCEL_PANEL_TITLE="window.export.excel.panel.title";</v>
+      </c>
+    </row>
+    <row r="940" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A940" t="str">
+        <f>IF('Export Excel'!B4&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B4),".","_"),"=""", 'Export Excel'!B4,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_EXCEL_INFORMATION_MESSAGE="window.export.excel.information.message";</v>
+      </c>
+    </row>
+    <row r="941" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A941" t="str">
+        <f>IF('Export Excel'!B5&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B5),".","_"),"=""", 'Export Excel'!B5,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_EXCEL_BUTTON_LABEL="window.export.excel.button.label";</v>
+      </c>
+    </row>
+    <row r="942" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A942" t="str">
+        <f>IF('Export Excel'!B6&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B6),".","_"),"=""", 'Export Excel'!B6,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_EXCEL_FILE_PICKER_PANEL_LABEL="window.export.excel.file.picker.panel.label";</v>
+      </c>
+    </row>
+    <row r="943" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A943" t="str">
+        <f>IF('Export Excel'!B7&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B7),".","_"),"=""", 'Export Excel'!B7,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_EXCEL_FILE_PICKER_PANEL_BUTTON="window.export.excel.file.picker.panel.button";</v>
+      </c>
+    </row>
+    <row r="944" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A944" t="str">
+        <f>IF('Export Excel'!B8&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B8),".","_"),"=""", 'Export Excel'!B8,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_EXCEL_PREFERENCE_WITH_FORMAT_LABEL="window.export.excel.preference.with.format.label";</v>
+      </c>
+    </row>
+    <row r="945" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A945" t="str">
+        <f>IF('Export Excel'!B9&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B9),".","_"),"=""", 'Export Excel'!B9,""";"),"")</f>
+        <v>public static final String WINDOW_EXPORT_EXCEL_PREFERENCE_PANEL_TITLE="window.export.excel.preference.panel.title";</v>
+      </c>
+    </row>
+    <row r="946" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A946" t="str">
+        <f>IF('Export Excel'!B10&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B10),".","_"),"=""", 'Export Excel'!B10,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="947" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A947" t="str">
+        <f>IF('Export Excel'!B11&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B11),".","_"),"=""", 'Export Excel'!B11,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="948" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A948" t="str">
+        <f>IF('Export Excel'!B12&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B12),".","_"),"=""", 'Export Excel'!B12,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="949" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A949" t="str">
+        <f>IF('Export Excel'!B13&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B13),".","_"),"=""", 'Export Excel'!B13,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="950" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A950" t="str">
+        <f>IF('Export Excel'!B14&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B14),".","_"),"=""", 'Export Excel'!B14,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="951" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A951" t="str">
+        <f>IF('Export Excel'!B15&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B15),".","_"),"=""", 'Export Excel'!B15,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="952" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A952" t="str">
+        <f>IF('Export Excel'!B16&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B16),".","_"),"=""", 'Export Excel'!B16,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="953" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A953" t="str">
+        <f>IF('Export Excel'!B17&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B17),".","_"),"=""", 'Export Excel'!B17,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="954" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A954" t="str">
+        <f>IF('Export Excel'!B18&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B18),".","_"),"=""", 'Export Excel'!B18,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="955" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A955" t="str">
+        <f>IF('Export Excel'!B19&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B19),".","_"),"=""", 'Export Excel'!B19,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="956" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A956" t="str">
+        <f>IF('Export Excel'!B20&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B20),".","_"),"=""", 'Export Excel'!B20,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="957" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A957" t="str">
+        <f>IF('Export Excel'!B21&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B21),".","_"),"=""", 'Export Excel'!B21,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="958" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A958" t="str">
+        <f>IF('Export Excel'!B22&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B22),".","_"),"=""", 'Export Excel'!B22,""";"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="959" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A959" t="str">
+        <f>IF('Export Excel'!B23&lt;&gt;"",CONCATENATE("public static final String ",SUBSTITUTE(UPPER('Export Excel'!B23),".","_"),"=""", 'Export Excel'!B23,""";"),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>